<commit_message>
Altera ordem de exibicao das planilhas
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A70B199-0293-4343-BBCE-8CA9F34BD7BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1A4F1-02D2-4BA7-B987-E8B27B51FC44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CodeXP-Cronograma" sheetId="3" r:id="rId1"/>
-    <sheet name="Dailies" sheetId="2" r:id="rId2"/>
+    <sheet name="Dailies" sheetId="2" r:id="rId1"/>
+    <sheet name="CodeXP-Cronograma" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="149">
   <si>
     <t>S</t>
   </si>
@@ -2151,11 +2151,34 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2166,52 +2189,14 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2231,11 +2216,26 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2643,10 +2643,953 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:CT11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+    <col min="4" max="12" width="30.77734375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="20.77734375" style="1" customWidth="1"/>
+    <col min="15" max="17" width="15.77734375" style="1" customWidth="1"/>
+    <col min="18" max="32" width="15.77734375" customWidth="1"/>
+    <col min="33" max="47" width="5.6640625" customWidth="1"/>
+    <col min="48" max="48" width="3.6640625" style="2" customWidth="1"/>
+    <col min="49" max="49" width="3.6640625" style="3" customWidth="1"/>
+    <col min="50" max="71" width="5.6640625" customWidth="1"/>
+    <col min="72" max="72" width="3.6640625" style="3" customWidth="1"/>
+    <col min="73" max="74" width="5.6640625" customWidth="1"/>
+    <col min="75" max="75" width="3.6640625" style="3" customWidth="1"/>
+    <col min="76" max="97" width="5.6640625" customWidth="1"/>
+    <col min="98" max="98" width="3.6640625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:98" ht="13.2" customHeight="1">
+      <c r="A1" s="173"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="168" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="169">
+        <v>15</v>
+      </c>
+      <c r="E1" s="169">
+        <v>16</v>
+      </c>
+      <c r="F1" s="169">
+        <v>17</v>
+      </c>
+      <c r="G1" s="169">
+        <v>18</v>
+      </c>
+      <c r="H1" s="169">
+        <v>19</v>
+      </c>
+      <c r="I1" s="169">
+        <v>20</v>
+      </c>
+      <c r="J1" s="169">
+        <v>21</v>
+      </c>
+      <c r="K1" s="169">
+        <v>22</v>
+      </c>
+      <c r="L1" s="169">
+        <v>23</v>
+      </c>
+      <c r="M1" s="169">
+        <v>24</v>
+      </c>
+      <c r="N1" s="169">
+        <v>25</v>
+      </c>
+      <c r="O1" s="169">
+        <v>26</v>
+      </c>
+      <c r="P1" s="169">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="169">
+        <v>28</v>
+      </c>
+      <c r="R1" s="169">
+        <v>29</v>
+      </c>
+      <c r="S1" s="169">
+        <v>30</v>
+      </c>
+      <c r="T1" s="169">
+        <v>31</v>
+      </c>
+      <c r="U1" s="169">
+        <v>32</v>
+      </c>
+      <c r="V1" s="169">
+        <v>33</v>
+      </c>
+      <c r="W1" s="169">
+        <v>34</v>
+      </c>
+      <c r="X1" s="169">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="169">
+        <v>36</v>
+      </c>
+      <c r="Z1" s="169">
+        <v>37</v>
+      </c>
+      <c r="AA1" s="169">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="169">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="169">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="169">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="169">
+        <v>42</v>
+      </c>
+      <c r="AF1" s="169">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="169">
+        <v>44</v>
+      </c>
+      <c r="AH1" s="169">
+        <v>45</v>
+      </c>
+      <c r="AI1" s="169">
+        <v>46</v>
+      </c>
+      <c r="AJ1" s="169">
+        <v>47</v>
+      </c>
+      <c r="AK1" s="169">
+        <v>48</v>
+      </c>
+      <c r="AL1" s="169">
+        <v>49</v>
+      </c>
+      <c r="AM1" s="169">
+        <v>50</v>
+      </c>
+      <c r="AN1" s="169">
+        <v>51</v>
+      </c>
+      <c r="AO1" s="169">
+        <v>52</v>
+      </c>
+      <c r="AP1" s="169">
+        <v>53</v>
+      </c>
+      <c r="AQ1" s="169">
+        <v>54</v>
+      </c>
+      <c r="AR1" s="169">
+        <v>55</v>
+      </c>
+      <c r="AS1" s="169">
+        <v>56</v>
+      </c>
+      <c r="AT1" s="169">
+        <v>57</v>
+      </c>
+      <c r="AU1" s="169">
+        <v>58</v>
+      </c>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="169">
+        <v>59</v>
+      </c>
+      <c r="AY1" s="169">
+        <v>60</v>
+      </c>
+      <c r="AZ1" s="169">
+        <v>61</v>
+      </c>
+      <c r="BA1" s="169">
+        <v>62</v>
+      </c>
+      <c r="BB1" s="169">
+        <v>63</v>
+      </c>
+      <c r="BC1" s="169">
+        <v>64</v>
+      </c>
+      <c r="BD1" s="169">
+        <v>65</v>
+      </c>
+      <c r="BE1" s="169">
+        <v>66</v>
+      </c>
+      <c r="BF1" s="169">
+        <v>67</v>
+      </c>
+      <c r="BG1" s="169">
+        <v>68</v>
+      </c>
+      <c r="BH1" s="169">
+        <v>69</v>
+      </c>
+      <c r="BI1" s="169">
+        <v>70</v>
+      </c>
+      <c r="BJ1" s="171">
+        <v>71</v>
+      </c>
+      <c r="BK1" s="171">
+        <v>72</v>
+      </c>
+      <c r="BL1" s="171">
+        <v>73</v>
+      </c>
+      <c r="BM1" s="171">
+        <v>74</v>
+      </c>
+      <c r="BN1" s="171">
+        <v>75</v>
+      </c>
+      <c r="BO1" s="171">
+        <v>76</v>
+      </c>
+      <c r="BP1" s="171">
+        <v>77</v>
+      </c>
+      <c r="BQ1" s="171">
+        <v>78</v>
+      </c>
+      <c r="BR1" s="171">
+        <v>79</v>
+      </c>
+      <c r="BS1" s="171">
+        <v>80</v>
+      </c>
+      <c r="BT1" s="5"/>
+      <c r="BU1" s="169">
+        <v>81</v>
+      </c>
+      <c r="BV1" s="169">
+        <v>82</v>
+      </c>
+      <c r="BW1" s="5"/>
+      <c r="BX1" s="169">
+        <v>83</v>
+      </c>
+      <c r="BY1" s="169">
+        <v>84</v>
+      </c>
+      <c r="BZ1" s="169">
+        <v>85</v>
+      </c>
+      <c r="CA1" s="169">
+        <v>86</v>
+      </c>
+      <c r="CB1" s="169">
+        <v>87</v>
+      </c>
+      <c r="CC1" s="169">
+        <v>88</v>
+      </c>
+      <c r="CD1" s="169">
+        <v>89</v>
+      </c>
+      <c r="CE1" s="169">
+        <v>90</v>
+      </c>
+      <c r="CF1" s="169">
+        <v>91</v>
+      </c>
+      <c r="CG1" s="169">
+        <v>92</v>
+      </c>
+      <c r="CH1" s="169">
+        <v>93</v>
+      </c>
+      <c r="CI1" s="169">
+        <v>94</v>
+      </c>
+      <c r="CJ1" s="169">
+        <v>95</v>
+      </c>
+      <c r="CK1" s="169">
+        <v>96</v>
+      </c>
+      <c r="CL1" s="169">
+        <v>97</v>
+      </c>
+      <c r="CM1" s="169">
+        <v>98</v>
+      </c>
+      <c r="CN1" s="169">
+        <v>99</v>
+      </c>
+      <c r="CO1" s="169">
+        <v>100</v>
+      </c>
+      <c r="CP1" s="169">
+        <v>101</v>
+      </c>
+      <c r="CQ1" s="169">
+        <v>102</v>
+      </c>
+      <c r="CR1" s="169">
+        <v>103</v>
+      </c>
+      <c r="CS1" s="169">
+        <v>104</v>
+      </c>
+      <c r="CT1" s="6"/>
+    </row>
+    <row r="2" spans="1:98" ht="15" customHeight="1">
+      <c r="A2" s="173"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="168" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="195" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="195"/>
+      <c r="V2" s="195"/>
+      <c r="W2" s="195"/>
+      <c r="X2" s="195"/>
+      <c r="Y2" s="195"/>
+      <c r="Z2" s="195"/>
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="195"/>
+      <c r="AE2" s="195"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="195"/>
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="195"/>
+      <c r="AM2" s="195" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="195"/>
+      <c r="AQ2" s="195"/>
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="195"/>
+      <c r="AU2" s="195"/>
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="196"/>
+      <c r="AY2" s="196"/>
+      <c r="AZ2" s="196"/>
+      <c r="BA2" s="196"/>
+      <c r="BB2" s="196"/>
+      <c r="BC2" s="196"/>
+      <c r="BD2" s="196"/>
+      <c r="BE2" s="196"/>
+      <c r="BF2" s="196"/>
+      <c r="BG2" s="196"/>
+      <c r="BH2" s="196"/>
+      <c r="BI2" s="196"/>
+      <c r="BJ2" s="195" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK2" s="195"/>
+      <c r="BL2" s="195"/>
+      <c r="BM2" s="195"/>
+      <c r="BN2" s="195"/>
+      <c r="BO2" s="195"/>
+      <c r="BP2" s="195"/>
+      <c r="BQ2" s="195"/>
+      <c r="BR2" s="195"/>
+      <c r="BS2" s="195"/>
+      <c r="BT2" s="195"/>
+      <c r="BU2" s="195"/>
+      <c r="BV2" s="195"/>
+      <c r="BW2" s="195"/>
+      <c r="BX2" s="197"/>
+      <c r="BY2" s="197"/>
+      <c r="BZ2" s="197"/>
+      <c r="CA2" s="197"/>
+      <c r="CB2" s="197"/>
+      <c r="CC2" s="197"/>
+      <c r="CD2" s="197"/>
+      <c r="CE2" s="198" t="s">
+        <v>8</v>
+      </c>
+      <c r="CF2" s="199"/>
+      <c r="CG2" s="199"/>
+      <c r="CH2" s="199"/>
+      <c r="CI2" s="199"/>
+      <c r="CJ2" s="199"/>
+      <c r="CK2" s="199"/>
+      <c r="CL2" s="199"/>
+      <c r="CM2" s="199"/>
+      <c r="CN2" s="199"/>
+      <c r="CO2" s="199"/>
+      <c r="CP2" s="199"/>
+      <c r="CQ2" s="199"/>
+      <c r="CR2" s="199"/>
+      <c r="CS2" s="199"/>
+      <c r="CT2" s="172"/>
+    </row>
+    <row r="3" spans="1:98" ht="13.2" customHeight="1">
+      <c r="A3" s="173"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="175" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="169">
+        <v>13</v>
+      </c>
+      <c r="E3" s="169">
+        <v>14</v>
+      </c>
+      <c r="F3" s="169">
+        <v>15</v>
+      </c>
+      <c r="G3" s="176">
+        <v>16</v>
+      </c>
+      <c r="H3" s="176">
+        <v>19</v>
+      </c>
+      <c r="I3" s="169">
+        <v>20</v>
+      </c>
+      <c r="J3" s="169">
+        <v>21</v>
+      </c>
+      <c r="K3" s="169">
+        <v>22</v>
+      </c>
+      <c r="L3" s="176">
+        <v>23</v>
+      </c>
+      <c r="M3" s="176">
+        <v>26</v>
+      </c>
+      <c r="N3" s="169">
+        <v>27</v>
+      </c>
+      <c r="O3" s="169">
+        <v>28</v>
+      </c>
+      <c r="P3" s="169">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="169">
+        <v>30</v>
+      </c>
+      <c r="R3" s="169">
+        <v>2</v>
+      </c>
+      <c r="S3" s="169">
+        <v>3</v>
+      </c>
+      <c r="T3" s="169">
+        <v>4</v>
+      </c>
+      <c r="U3" s="169">
+        <v>5</v>
+      </c>
+      <c r="V3" s="169">
+        <v>6</v>
+      </c>
+      <c r="W3" s="169">
+        <v>9</v>
+      </c>
+      <c r="X3" s="169">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="169">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="169">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="169">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="169">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="169">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="169">
+        <v>18</v>
+      </c>
+      <c r="AE3" s="169">
+        <v>19</v>
+      </c>
+      <c r="AF3" s="169">
+        <v>20</v>
+      </c>
+      <c r="AG3" s="169">
+        <v>23</v>
+      </c>
+      <c r="AH3" s="169">
+        <v>24</v>
+      </c>
+      <c r="AI3" s="169">
+        <v>25</v>
+      </c>
+      <c r="AJ3" s="169">
+        <v>26</v>
+      </c>
+      <c r="AK3" s="169">
+        <v>27</v>
+      </c>
+      <c r="AL3" s="169">
+        <v>30</v>
+      </c>
+      <c r="AM3" s="170">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="170">
+        <v>2</v>
+      </c>
+      <c r="AO3" s="170">
+        <v>3</v>
+      </c>
+      <c r="AP3" s="170">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="170">
+        <v>7</v>
+      </c>
+      <c r="AR3" s="170">
+        <v>8</v>
+      </c>
+      <c r="AS3" s="170">
+        <v>9</v>
+      </c>
+      <c r="AT3" s="170">
+        <v>10</v>
+      </c>
+      <c r="AU3" s="170">
+        <v>11</v>
+      </c>
+      <c r="AV3" s="6">
+        <v>14</v>
+      </c>
+      <c r="AW3" s="6">
+        <v>15</v>
+      </c>
+      <c r="AX3" s="169">
+        <v>16</v>
+      </c>
+      <c r="AY3" s="169">
+        <v>17</v>
+      </c>
+      <c r="AZ3" s="169">
+        <v>18</v>
+      </c>
+      <c r="BA3" s="169">
+        <v>21</v>
+      </c>
+      <c r="BB3" s="169">
+        <v>22</v>
+      </c>
+      <c r="BC3" s="169">
+        <v>23</v>
+      </c>
+      <c r="BD3" s="169">
+        <v>24</v>
+      </c>
+      <c r="BE3" s="169">
+        <v>25</v>
+      </c>
+      <c r="BF3" s="169">
+        <v>28</v>
+      </c>
+      <c r="BG3" s="169">
+        <v>29</v>
+      </c>
+      <c r="BH3" s="169">
+        <v>30</v>
+      </c>
+      <c r="BI3" s="169">
+        <v>31</v>
+      </c>
+      <c r="BJ3" s="169">
+        <v>1</v>
+      </c>
+      <c r="BK3" s="169">
+        <v>4</v>
+      </c>
+      <c r="BL3" s="169">
+        <v>5</v>
+      </c>
+      <c r="BM3" s="169">
+        <v>6</v>
+      </c>
+      <c r="BN3" s="169">
+        <v>7</v>
+      </c>
+      <c r="BO3" s="169">
+        <v>8</v>
+      </c>
+      <c r="BP3" s="169">
+        <v>11</v>
+      </c>
+      <c r="BQ3" s="169">
+        <v>12</v>
+      </c>
+      <c r="BR3" s="169">
+        <v>13</v>
+      </c>
+      <c r="BS3" s="169">
+        <v>14</v>
+      </c>
+      <c r="BT3" s="6">
+        <v>15</v>
+      </c>
+      <c r="BU3" s="169">
+        <v>18</v>
+      </c>
+      <c r="BV3" s="169">
+        <v>19</v>
+      </c>
+      <c r="BW3" s="6">
+        <v>20</v>
+      </c>
+      <c r="BX3" s="169">
+        <v>21</v>
+      </c>
+      <c r="BY3" s="169">
+        <v>22</v>
+      </c>
+      <c r="BZ3" s="169">
+        <v>25</v>
+      </c>
+      <c r="CA3" s="169">
+        <v>26</v>
+      </c>
+      <c r="CB3" s="169">
+        <v>27</v>
+      </c>
+      <c r="CC3" s="169">
+        <v>28</v>
+      </c>
+      <c r="CD3" s="169">
+        <v>29</v>
+      </c>
+      <c r="CE3" s="169">
+        <v>2</v>
+      </c>
+      <c r="CF3" s="169">
+        <v>3</v>
+      </c>
+      <c r="CG3" s="169">
+        <v>4</v>
+      </c>
+      <c r="CH3" s="169">
+        <v>5</v>
+      </c>
+      <c r="CI3" s="169">
+        <v>6</v>
+      </c>
+      <c r="CJ3" s="169">
+        <v>9</v>
+      </c>
+      <c r="CK3" s="169">
+        <v>10</v>
+      </c>
+      <c r="CL3" s="169">
+        <v>11</v>
+      </c>
+      <c r="CM3" s="169">
+        <v>12</v>
+      </c>
+      <c r="CN3" s="169">
+        <v>13</v>
+      </c>
+      <c r="CO3" s="169">
+        <v>16</v>
+      </c>
+      <c r="CP3" s="169">
+        <v>17</v>
+      </c>
+      <c r="CQ3" s="169">
+        <v>18</v>
+      </c>
+      <c r="CR3" s="169">
+        <v>19</v>
+      </c>
+      <c r="CS3" s="169">
+        <v>20</v>
+      </c>
+      <c r="CT3" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
+      <c r="A4" s="204" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="205" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="205"/>
+      <c r="D4" s="206" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="200" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="200" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="200" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="203" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="203" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="203" t="s">
+        <v>148</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="AV4" s="194"/>
+      <c r="AW4" s="194"/>
+      <c r="BT4" s="194"/>
+      <c r="BW4" s="194"/>
+      <c r="CT4" s="194"/>
+    </row>
+    <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
+      <c r="A5" s="204"/>
+      <c r="B5" s="205" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="205"/>
+      <c r="D5" s="207"/>
+      <c r="E5" s="201"/>
+      <c r="F5" s="201"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="201"/>
+      <c r="I5" s="201"/>
+      <c r="J5" s="201"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="AV5" s="194"/>
+      <c r="AW5" s="194"/>
+      <c r="BT5" s="194"/>
+      <c r="BW5" s="194"/>
+      <c r="CT5" s="194"/>
+    </row>
+    <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
+      <c r="A6" s="204"/>
+      <c r="B6" s="205" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="205"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="201"/>
+      <c r="F6" s="201"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="201"/>
+      <c r="I6" s="201"/>
+      <c r="J6" s="201"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="AV6" s="194"/>
+      <c r="AW6" s="194"/>
+      <c r="BT6" s="194"/>
+      <c r="BW6" s="194"/>
+      <c r="CT6" s="194"/>
+    </row>
+    <row r="7" spans="1:98" ht="45" customHeight="1">
+      <c r="A7" s="204"/>
+      <c r="B7" s="205" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="205"/>
+      <c r="D7" s="207"/>
+      <c r="E7" s="201"/>
+      <c r="F7" s="201"/>
+      <c r="G7" s="202"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="V7" s="10"/>
+      <c r="AV7" s="194"/>
+      <c r="AW7" s="194"/>
+      <c r="BT7" s="194"/>
+      <c r="BW7" s="194"/>
+      <c r="CT7" s="194"/>
+    </row>
+    <row r="8" spans="1:98" ht="45" customHeight="1">
+      <c r="A8" s="204" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="205" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="205"/>
+      <c r="D8" s="207"/>
+      <c r="E8" s="201"/>
+      <c r="F8" s="201"/>
+      <c r="G8" s="202"/>
+      <c r="H8" s="201"/>
+      <c r="I8" s="201"/>
+      <c r="J8" s="201"/>
+      <c r="AV8" s="194"/>
+      <c r="AW8" s="194"/>
+      <c r="BT8" s="194"/>
+      <c r="BW8" s="194"/>
+      <c r="CT8" s="194"/>
+    </row>
+    <row r="9" spans="1:98" ht="45" customHeight="1">
+      <c r="A9" s="204"/>
+      <c r="B9" s="205" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="205"/>
+      <c r="D9" s="207"/>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="201"/>
+      <c r="AV9" s="194"/>
+      <c r="AW9" s="194"/>
+      <c r="BT9" s="194"/>
+      <c r="BW9" s="194"/>
+      <c r="CT9" s="194"/>
+    </row>
+    <row r="10" spans="1:98" ht="45" customHeight="1">
+      <c r="A10" s="204"/>
+      <c r="B10" s="205" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="205"/>
+      <c r="D10" s="207"/>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="202"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="201"/>
+      <c r="J10" s="201"/>
+      <c r="AV10" s="194"/>
+      <c r="AW10" s="194"/>
+      <c r="BT10" s="194"/>
+      <c r="BW10" s="194"/>
+      <c r="CT10" s="194"/>
+    </row>
+    <row r="11" spans="1:98" ht="45" customHeight="1">
+      <c r="A11" s="204"/>
+      <c r="B11" s="205" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="205"/>
+      <c r="D11" s="207"/>
+      <c r="E11" s="201"/>
+      <c r="F11" s="201"/>
+      <c r="G11" s="202"/>
+      <c r="H11" s="201"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="201"/>
+      <c r="AV11" s="194"/>
+      <c r="AW11" s="194"/>
+      <c r="BT11" s="194"/>
+      <c r="BW11" s="194"/>
+      <c r="CT11" s="194"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+  </mergeCells>
+  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -3307,13 +4250,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="188" t="s">
+      <c r="A4" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="190"/>
+      <c r="C4" s="182"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -3418,9 +4361,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="177"/>
-      <c r="B5" s="187"/>
-      <c r="C5" s="177"/>
+      <c r="A5" s="180"/>
+      <c r="B5" s="178"/>
+      <c r="C5" s="180"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -3525,11 +4468,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="177"/>
+      <c r="A6" s="180"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="177"/>
+      <c r="C6" s="180"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -3634,11 +4577,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="180"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="177"/>
+      <c r="C7" s="180"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -3743,11 +4686,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="177"/>
+      <c r="A8" s="180"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="177"/>
+      <c r="C8" s="180"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -3852,11 +4795,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="177"/>
+      <c r="A9" s="180"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="177"/>
+      <c r="C9" s="180"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -3961,11 +4904,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="177"/>
+      <c r="A10" s="180"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="177"/>
+      <c r="C10" s="180"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -4070,11 +5013,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="177"/>
+      <c r="A11" s="180"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="177"/>
+      <c r="C11" s="180"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -4179,9 +5122,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="177"/>
+      <c r="A12" s="180"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="178"/>
+      <c r="C12" s="183"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -4286,10 +5229,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="191" t="s">
+      <c r="A13" s="184" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="192" t="s">
+      <c r="B13" s="185" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -4398,8 +5341,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="177"/>
-      <c r="B14" s="183"/>
+      <c r="A14" s="180"/>
+      <c r="B14" s="186"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -4520,7 +5463,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="177"/>
+      <c r="A15" s="180"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -4630,7 +5573,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="177"/>
+      <c r="A16" s="180"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -4740,7 +5683,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="177"/>
+      <c r="A17" s="180"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -4852,7 +5795,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="177"/>
+      <c r="A18" s="180"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -4962,7 +5905,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="177"/>
+      <c r="A19" s="180"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -5072,7 +6015,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="177"/>
+      <c r="A20" s="180"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -5182,7 +6125,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="178"/>
+      <c r="A21" s="183"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -5293,7 +6236,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="186" t="s">
+      <c r="B22" s="177" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -5403,7 +6346,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="187"/>
+      <c r="B23" s="178"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -5510,13 +6453,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="179" t="s">
+      <c r="A24" s="188" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="181">
+      <c r="C24" s="190">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -5624,11 +6567,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="180"/>
+      <c r="A25" s="189"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="177"/>
+      <c r="C25" s="180"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -5734,11 +6677,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="180"/>
+      <c r="A26" s="189"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="177"/>
+      <c r="C26" s="180"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -5844,11 +6787,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="180"/>
+      <c r="A27" s="189"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="177"/>
+      <c r="C27" s="180"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -5954,11 +6897,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="180"/>
+      <c r="A28" s="189"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="177"/>
+      <c r="C28" s="180"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -6064,11 +7007,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="180"/>
+      <c r="A29" s="189"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="177"/>
+      <c r="C29" s="180"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -6174,11 +7117,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="180"/>
+      <c r="A30" s="189"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="177"/>
+      <c r="C30" s="180"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -6284,11 +7227,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="180"/>
+      <c r="A31" s="189"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="177"/>
+      <c r="C31" s="180"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -6394,11 +7337,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="180"/>
+      <c r="A32" s="189"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="177"/>
+      <c r="C32" s="180"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -6504,11 +7447,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="180"/>
+      <c r="A33" s="189"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="177"/>
+      <c r="C33" s="180"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -6614,11 +7557,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="180"/>
+      <c r="A34" s="189"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="177"/>
+      <c r="C34" s="180"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -6724,11 +7667,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="180"/>
+      <c r="A35" s="189"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="178"/>
+      <c r="C35" s="183"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -6834,11 +7777,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="180"/>
+      <c r="A36" s="189"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="181">
+      <c r="C36" s="190">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -6946,11 +7889,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="180"/>
+      <c r="A37" s="189"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="177"/>
+      <c r="C37" s="180"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -7056,11 +7999,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="180"/>
+      <c r="A38" s="189"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="177"/>
+      <c r="C38" s="180"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -7166,11 +8109,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="180"/>
+      <c r="A39" s="189"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="177"/>
+      <c r="C39" s="180"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -7276,11 +8219,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="180"/>
+      <c r="A40" s="189"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="177"/>
+      <c r="C40" s="180"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -7386,11 +8329,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="180"/>
+      <c r="A41" s="189"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="177"/>
+      <c r="C41" s="180"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -7496,11 +8439,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="180"/>
+      <c r="A42" s="189"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="177"/>
+      <c r="C42" s="180"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -7606,11 +8549,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="180"/>
+      <c r="A43" s="189"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="177"/>
+      <c r="C43" s="180"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -7716,11 +8659,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="180"/>
+      <c r="A44" s="189"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="177"/>
+      <c r="C44" s="180"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -7826,11 +8769,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="180"/>
+      <c r="A45" s="189"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="177"/>
+      <c r="C45" s="180"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -7936,11 +8879,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="180"/>
+      <c r="A46" s="189"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="177"/>
+      <c r="C46" s="180"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -8046,11 +8989,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="180"/>
+      <c r="A47" s="189"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="177"/>
+      <c r="C47" s="180"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -8164,11 +9107,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="180"/>
+      <c r="A48" s="189"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="177"/>
+      <c r="C48" s="180"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -8277,7 +9220,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="182" t="s">
+      <c r="B49" s="191" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -8387,7 +9330,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="183"/>
+      <c r="B50" s="186"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -11818,7 +12761,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="184" t="s">
+      <c r="A81" s="192" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -11930,7 +12873,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="177"/>
+      <c r="A82" s="180"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12040,7 +12983,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="177"/>
+      <c r="A83" s="180"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -12150,7 +13093,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="177"/>
+      <c r="A84" s="180"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -12260,7 +13203,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="177"/>
+      <c r="A85" s="180"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -12370,7 +13313,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="177"/>
+      <c r="A86" s="180"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -12480,7 +13423,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="177"/>
+      <c r="A87" s="180"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -12592,7 +13535,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="177"/>
+      <c r="A88" s="180"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -12702,7 +13645,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="177"/>
+      <c r="A89" s="180"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -12812,7 +13755,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="177"/>
+      <c r="A90" s="180"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -12922,11 +13865,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="177"/>
+      <c r="A91" s="180"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="185"/>
+      <c r="C91" s="193"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13032,11 +13975,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="177"/>
+      <c r="A92" s="180"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="177"/>
+      <c r="C92" s="180"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -13142,11 +14085,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="178"/>
+      <c r="A93" s="183"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="177"/>
+      <c r="C93" s="180"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -13370,7 +14313,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="176" t="s">
+      <c r="A95" s="187" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -13482,7 +14425,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="177"/>
+      <c r="A96" s="180"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -13592,7 +14535,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="177"/>
+      <c r="A97" s="180"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -13702,7 +14645,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="177"/>
+      <c r="A98" s="180"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -13812,7 +14755,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="177"/>
+      <c r="A99" s="180"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -13922,7 +14865,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="177"/>
+      <c r="A100" s="180"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14032,7 +14975,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="177"/>
+      <c r="A101" s="180"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -14142,7 +15085,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="177"/>
+      <c r="A102" s="180"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -14252,7 +15195,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="177"/>
+      <c r="A103" s="180"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -14364,7 +15307,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="177"/>
+      <c r="A104" s="180"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -14474,7 +15417,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="177"/>
+      <c r="A105" s="180"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -14592,7 +15535,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="177"/>
+      <c r="A106" s="180"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -14702,7 +15645,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="177"/>
+      <c r="A107" s="180"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -14812,7 +15755,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="177"/>
+      <c r="A108" s="180"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -14922,7 +15865,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="177"/>
+      <c r="A109" s="180"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15032,7 +15975,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="177"/>
+      <c r="A110" s="180"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -15142,7 +16085,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="177"/>
+      <c r="A111" s="180"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -15252,7 +16195,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="177"/>
+      <c r="A112" s="180"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -15362,7 +16305,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="177"/>
+      <c r="A113" s="180"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -15472,7 +16415,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="177"/>
+      <c r="A114" s="180"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -15582,7 +16525,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="177"/>
+      <c r="A115" s="180"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -15692,7 +16635,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="177"/>
+      <c r="A116" s="180"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -15818,7 +16761,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="177"/>
+      <c r="A117" s="180"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -15928,7 +16871,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="178"/>
+      <c r="A118" s="183"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -23299,12 +24242,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -23312,951 +24249,14 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:CT11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="13.21875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" customWidth="1"/>
-    <col min="4" max="12" width="30.77734375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="20.77734375" style="1" customWidth="1"/>
-    <col min="15" max="17" width="15.77734375" style="1" customWidth="1"/>
-    <col min="18" max="32" width="15.77734375" customWidth="1"/>
-    <col min="33" max="47" width="5.6640625" customWidth="1"/>
-    <col min="48" max="48" width="3.6640625" style="2" customWidth="1"/>
-    <col min="49" max="49" width="3.6640625" style="3" customWidth="1"/>
-    <col min="50" max="71" width="5.6640625" customWidth="1"/>
-    <col min="72" max="72" width="3.6640625" style="3" customWidth="1"/>
-    <col min="73" max="74" width="5.6640625" customWidth="1"/>
-    <col min="75" max="75" width="3.6640625" style="3" customWidth="1"/>
-    <col min="76" max="97" width="5.6640625" customWidth="1"/>
-    <col min="98" max="98" width="3.6640625" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:98" ht="13.2" customHeight="1">
-      <c r="A1" s="173"/>
-      <c r="B1" s="173"/>
-      <c r="C1" s="168" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="169">
-        <v>15</v>
-      </c>
-      <c r="E1" s="169">
-        <v>16</v>
-      </c>
-      <c r="F1" s="169">
-        <v>17</v>
-      </c>
-      <c r="G1" s="169">
-        <v>18</v>
-      </c>
-      <c r="H1" s="169">
-        <v>19</v>
-      </c>
-      <c r="I1" s="169">
-        <v>20</v>
-      </c>
-      <c r="J1" s="169">
-        <v>21</v>
-      </c>
-      <c r="K1" s="169">
-        <v>22</v>
-      </c>
-      <c r="L1" s="169">
-        <v>23</v>
-      </c>
-      <c r="M1" s="169">
-        <v>24</v>
-      </c>
-      <c r="N1" s="169">
-        <v>25</v>
-      </c>
-      <c r="O1" s="169">
-        <v>26</v>
-      </c>
-      <c r="P1" s="169">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="169">
-        <v>28</v>
-      </c>
-      <c r="R1" s="169">
-        <v>29</v>
-      </c>
-      <c r="S1" s="169">
-        <v>30</v>
-      </c>
-      <c r="T1" s="169">
-        <v>31</v>
-      </c>
-      <c r="U1" s="169">
-        <v>32</v>
-      </c>
-      <c r="V1" s="169">
-        <v>33</v>
-      </c>
-      <c r="W1" s="169">
-        <v>34</v>
-      </c>
-      <c r="X1" s="169">
-        <v>35</v>
-      </c>
-      <c r="Y1" s="169">
-        <v>36</v>
-      </c>
-      <c r="Z1" s="169">
-        <v>37</v>
-      </c>
-      <c r="AA1" s="169">
-        <v>38</v>
-      </c>
-      <c r="AB1" s="169">
-        <v>39</v>
-      </c>
-      <c r="AC1" s="169">
-        <v>40</v>
-      </c>
-      <c r="AD1" s="169">
-        <v>41</v>
-      </c>
-      <c r="AE1" s="169">
-        <v>42</v>
-      </c>
-      <c r="AF1" s="169">
-        <v>43</v>
-      </c>
-      <c r="AG1" s="169">
-        <v>44</v>
-      </c>
-      <c r="AH1" s="169">
-        <v>45</v>
-      </c>
-      <c r="AI1" s="169">
-        <v>46</v>
-      </c>
-      <c r="AJ1" s="169">
-        <v>47</v>
-      </c>
-      <c r="AK1" s="169">
-        <v>48</v>
-      </c>
-      <c r="AL1" s="169">
-        <v>49</v>
-      </c>
-      <c r="AM1" s="169">
-        <v>50</v>
-      </c>
-      <c r="AN1" s="169">
-        <v>51</v>
-      </c>
-      <c r="AO1" s="169">
-        <v>52</v>
-      </c>
-      <c r="AP1" s="169">
-        <v>53</v>
-      </c>
-      <c r="AQ1" s="169">
-        <v>54</v>
-      </c>
-      <c r="AR1" s="169">
-        <v>55</v>
-      </c>
-      <c r="AS1" s="169">
-        <v>56</v>
-      </c>
-      <c r="AT1" s="169">
-        <v>57</v>
-      </c>
-      <c r="AU1" s="169">
-        <v>58</v>
-      </c>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="169">
-        <v>59</v>
-      </c>
-      <c r="AY1" s="169">
-        <v>60</v>
-      </c>
-      <c r="AZ1" s="169">
-        <v>61</v>
-      </c>
-      <c r="BA1" s="169">
-        <v>62</v>
-      </c>
-      <c r="BB1" s="169">
-        <v>63</v>
-      </c>
-      <c r="BC1" s="169">
-        <v>64</v>
-      </c>
-      <c r="BD1" s="169">
-        <v>65</v>
-      </c>
-      <c r="BE1" s="169">
-        <v>66</v>
-      </c>
-      <c r="BF1" s="169">
-        <v>67</v>
-      </c>
-      <c r="BG1" s="169">
-        <v>68</v>
-      </c>
-      <c r="BH1" s="169">
-        <v>69</v>
-      </c>
-      <c r="BI1" s="169">
-        <v>70</v>
-      </c>
-      <c r="BJ1" s="171">
-        <v>71</v>
-      </c>
-      <c r="BK1" s="171">
-        <v>72</v>
-      </c>
-      <c r="BL1" s="171">
-        <v>73</v>
-      </c>
-      <c r="BM1" s="171">
-        <v>74</v>
-      </c>
-      <c r="BN1" s="171">
-        <v>75</v>
-      </c>
-      <c r="BO1" s="171">
-        <v>76</v>
-      </c>
-      <c r="BP1" s="171">
-        <v>77</v>
-      </c>
-      <c r="BQ1" s="171">
-        <v>78</v>
-      </c>
-      <c r="BR1" s="171">
-        <v>79</v>
-      </c>
-      <c r="BS1" s="171">
-        <v>80</v>
-      </c>
-      <c r="BT1" s="5"/>
-      <c r="BU1" s="169">
-        <v>81</v>
-      </c>
-      <c r="BV1" s="169">
-        <v>82</v>
-      </c>
-      <c r="BW1" s="5"/>
-      <c r="BX1" s="169">
-        <v>83</v>
-      </c>
-      <c r="BY1" s="169">
-        <v>84</v>
-      </c>
-      <c r="BZ1" s="169">
-        <v>85</v>
-      </c>
-      <c r="CA1" s="169">
-        <v>86</v>
-      </c>
-      <c r="CB1" s="169">
-        <v>87</v>
-      </c>
-      <c r="CC1" s="169">
-        <v>88</v>
-      </c>
-      <c r="CD1" s="169">
-        <v>89</v>
-      </c>
-      <c r="CE1" s="169">
-        <v>90</v>
-      </c>
-      <c r="CF1" s="169">
-        <v>91</v>
-      </c>
-      <c r="CG1" s="169">
-        <v>92</v>
-      </c>
-      <c r="CH1" s="169">
-        <v>93</v>
-      </c>
-      <c r="CI1" s="169">
-        <v>94</v>
-      </c>
-      <c r="CJ1" s="169">
-        <v>95</v>
-      </c>
-      <c r="CK1" s="169">
-        <v>96</v>
-      </c>
-      <c r="CL1" s="169">
-        <v>97</v>
-      </c>
-      <c r="CM1" s="169">
-        <v>98</v>
-      </c>
-      <c r="CN1" s="169">
-        <v>99</v>
-      </c>
-      <c r="CO1" s="169">
-        <v>100</v>
-      </c>
-      <c r="CP1" s="169">
-        <v>101</v>
-      </c>
-      <c r="CQ1" s="169">
-        <v>102</v>
-      </c>
-      <c r="CR1" s="169">
-        <v>103</v>
-      </c>
-      <c r="CS1" s="169">
-        <v>104</v>
-      </c>
-      <c r="CT1" s="6"/>
-    </row>
-    <row r="2" spans="1:98" ht="15" customHeight="1">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="168" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="200" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="200"/>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
-      <c r="M2" s="200"/>
-      <c r="N2" s="200"/>
-      <c r="O2" s="200"/>
-      <c r="P2" s="200"/>
-      <c r="Q2" s="200"/>
-      <c r="R2" s="200" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="200"/>
-      <c r="T2" s="200"/>
-      <c r="U2" s="200"/>
-      <c r="V2" s="200"/>
-      <c r="W2" s="200"/>
-      <c r="X2" s="200"/>
-      <c r="Y2" s="200"/>
-      <c r="Z2" s="200"/>
-      <c r="AA2" s="200"/>
-      <c r="AB2" s="200"/>
-      <c r="AC2" s="200"/>
-      <c r="AD2" s="200"/>
-      <c r="AE2" s="200"/>
-      <c r="AF2" s="200"/>
-      <c r="AG2" s="200"/>
-      <c r="AH2" s="200"/>
-      <c r="AI2" s="200"/>
-      <c r="AJ2" s="200"/>
-      <c r="AK2" s="200"/>
-      <c r="AL2" s="200"/>
-      <c r="AM2" s="200" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN2" s="200"/>
-      <c r="AO2" s="200"/>
-      <c r="AP2" s="200"/>
-      <c r="AQ2" s="200"/>
-      <c r="AR2" s="200"/>
-      <c r="AS2" s="200"/>
-      <c r="AT2" s="200"/>
-      <c r="AU2" s="200"/>
-      <c r="AV2" s="200"/>
-      <c r="AW2" s="200"/>
-      <c r="AX2" s="201"/>
-      <c r="AY2" s="201"/>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="201"/>
-      <c r="BB2" s="201"/>
-      <c r="BC2" s="201"/>
-      <c r="BD2" s="201"/>
-      <c r="BE2" s="201"/>
-      <c r="BF2" s="201"/>
-      <c r="BG2" s="201"/>
-      <c r="BH2" s="201"/>
-      <c r="BI2" s="201"/>
-      <c r="BJ2" s="200" t="s">
-        <v>7</v>
-      </c>
-      <c r="BK2" s="200"/>
-      <c r="BL2" s="200"/>
-      <c r="BM2" s="200"/>
-      <c r="BN2" s="200"/>
-      <c r="BO2" s="200"/>
-      <c r="BP2" s="200"/>
-      <c r="BQ2" s="200"/>
-      <c r="BR2" s="200"/>
-      <c r="BS2" s="200"/>
-      <c r="BT2" s="200"/>
-      <c r="BU2" s="200"/>
-      <c r="BV2" s="200"/>
-      <c r="BW2" s="200"/>
-      <c r="BX2" s="202"/>
-      <c r="BY2" s="202"/>
-      <c r="BZ2" s="202"/>
-      <c r="CA2" s="202"/>
-      <c r="CB2" s="202"/>
-      <c r="CC2" s="202"/>
-      <c r="CD2" s="202"/>
-      <c r="CE2" s="203" t="s">
-        <v>8</v>
-      </c>
-      <c r="CF2" s="204"/>
-      <c r="CG2" s="204"/>
-      <c r="CH2" s="204"/>
-      <c r="CI2" s="204"/>
-      <c r="CJ2" s="204"/>
-      <c r="CK2" s="204"/>
-      <c r="CL2" s="204"/>
-      <c r="CM2" s="204"/>
-      <c r="CN2" s="204"/>
-      <c r="CO2" s="204"/>
-      <c r="CP2" s="204"/>
-      <c r="CQ2" s="204"/>
-      <c r="CR2" s="204"/>
-      <c r="CS2" s="204"/>
-      <c r="CT2" s="172"/>
-    </row>
-    <row r="3" spans="1:98" ht="13.2" customHeight="1">
-      <c r="A3" s="173"/>
-      <c r="B3" s="174"/>
-      <c r="C3" s="175" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="169">
-        <v>13</v>
-      </c>
-      <c r="E3" s="169">
-        <v>14</v>
-      </c>
-      <c r="F3" s="169">
-        <v>15</v>
-      </c>
-      <c r="G3" s="207">
-        <v>16</v>
-      </c>
-      <c r="H3" s="207">
-        <v>19</v>
-      </c>
-      <c r="I3" s="169">
-        <v>20</v>
-      </c>
-      <c r="J3" s="169">
-        <v>21</v>
-      </c>
-      <c r="K3" s="169">
-        <v>22</v>
-      </c>
-      <c r="L3" s="207">
-        <v>23</v>
-      </c>
-      <c r="M3" s="207">
-        <v>26</v>
-      </c>
-      <c r="N3" s="169">
-        <v>27</v>
-      </c>
-      <c r="O3" s="169">
-        <v>28</v>
-      </c>
-      <c r="P3" s="169">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="169">
-        <v>30</v>
-      </c>
-      <c r="R3" s="169">
-        <v>2</v>
-      </c>
-      <c r="S3" s="169">
-        <v>3</v>
-      </c>
-      <c r="T3" s="169">
-        <v>4</v>
-      </c>
-      <c r="U3" s="169">
-        <v>5</v>
-      </c>
-      <c r="V3" s="169">
-        <v>6</v>
-      </c>
-      <c r="W3" s="169">
-        <v>9</v>
-      </c>
-      <c r="X3" s="169">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="169">
-        <v>11</v>
-      </c>
-      <c r="Z3" s="169">
-        <v>12</v>
-      </c>
-      <c r="AA3" s="169">
-        <v>13</v>
-      </c>
-      <c r="AB3" s="169">
-        <v>16</v>
-      </c>
-      <c r="AC3" s="169">
-        <v>17</v>
-      </c>
-      <c r="AD3" s="169">
-        <v>18</v>
-      </c>
-      <c r="AE3" s="169">
-        <v>19</v>
-      </c>
-      <c r="AF3" s="169">
-        <v>20</v>
-      </c>
-      <c r="AG3" s="169">
-        <v>23</v>
-      </c>
-      <c r="AH3" s="169">
-        <v>24</v>
-      </c>
-      <c r="AI3" s="169">
-        <v>25</v>
-      </c>
-      <c r="AJ3" s="169">
-        <v>26</v>
-      </c>
-      <c r="AK3" s="169">
-        <v>27</v>
-      </c>
-      <c r="AL3" s="169">
-        <v>30</v>
-      </c>
-      <c r="AM3" s="170">
-        <v>1</v>
-      </c>
-      <c r="AN3" s="170">
-        <v>2</v>
-      </c>
-      <c r="AO3" s="170">
-        <v>3</v>
-      </c>
-      <c r="AP3" s="170">
-        <v>4</v>
-      </c>
-      <c r="AQ3" s="170">
-        <v>7</v>
-      </c>
-      <c r="AR3" s="170">
-        <v>8</v>
-      </c>
-      <c r="AS3" s="170">
-        <v>9</v>
-      </c>
-      <c r="AT3" s="170">
-        <v>10</v>
-      </c>
-      <c r="AU3" s="170">
-        <v>11</v>
-      </c>
-      <c r="AV3" s="6">
-        <v>14</v>
-      </c>
-      <c r="AW3" s="6">
-        <v>15</v>
-      </c>
-      <c r="AX3" s="169">
-        <v>16</v>
-      </c>
-      <c r="AY3" s="169">
-        <v>17</v>
-      </c>
-      <c r="AZ3" s="169">
-        <v>18</v>
-      </c>
-      <c r="BA3" s="169">
-        <v>21</v>
-      </c>
-      <c r="BB3" s="169">
-        <v>22</v>
-      </c>
-      <c r="BC3" s="169">
-        <v>23</v>
-      </c>
-      <c r="BD3" s="169">
-        <v>24</v>
-      </c>
-      <c r="BE3" s="169">
-        <v>25</v>
-      </c>
-      <c r="BF3" s="169">
-        <v>28</v>
-      </c>
-      <c r="BG3" s="169">
-        <v>29</v>
-      </c>
-      <c r="BH3" s="169">
-        <v>30</v>
-      </c>
-      <c r="BI3" s="169">
-        <v>31</v>
-      </c>
-      <c r="BJ3" s="169">
-        <v>1</v>
-      </c>
-      <c r="BK3" s="169">
-        <v>4</v>
-      </c>
-      <c r="BL3" s="169">
-        <v>5</v>
-      </c>
-      <c r="BM3" s="169">
-        <v>6</v>
-      </c>
-      <c r="BN3" s="169">
-        <v>7</v>
-      </c>
-      <c r="BO3" s="169">
-        <v>8</v>
-      </c>
-      <c r="BP3" s="169">
-        <v>11</v>
-      </c>
-      <c r="BQ3" s="169">
-        <v>12</v>
-      </c>
-      <c r="BR3" s="169">
-        <v>13</v>
-      </c>
-      <c r="BS3" s="169">
-        <v>14</v>
-      </c>
-      <c r="BT3" s="6">
-        <v>15</v>
-      </c>
-      <c r="BU3" s="169">
-        <v>18</v>
-      </c>
-      <c r="BV3" s="169">
-        <v>19</v>
-      </c>
-      <c r="BW3" s="6">
-        <v>20</v>
-      </c>
-      <c r="BX3" s="169">
-        <v>21</v>
-      </c>
-      <c r="BY3" s="169">
-        <v>22</v>
-      </c>
-      <c r="BZ3" s="169">
-        <v>25</v>
-      </c>
-      <c r="CA3" s="169">
-        <v>26</v>
-      </c>
-      <c r="CB3" s="169">
-        <v>27</v>
-      </c>
-      <c r="CC3" s="169">
-        <v>28</v>
-      </c>
-      <c r="CD3" s="169">
-        <v>29</v>
-      </c>
-      <c r="CE3" s="169">
-        <v>2</v>
-      </c>
-      <c r="CF3" s="169">
-        <v>3</v>
-      </c>
-      <c r="CG3" s="169">
-        <v>4</v>
-      </c>
-      <c r="CH3" s="169">
-        <v>5</v>
-      </c>
-      <c r="CI3" s="169">
-        <v>6</v>
-      </c>
-      <c r="CJ3" s="169">
-        <v>9</v>
-      </c>
-      <c r="CK3" s="169">
-        <v>10</v>
-      </c>
-      <c r="CL3" s="169">
-        <v>11</v>
-      </c>
-      <c r="CM3" s="169">
-        <v>12</v>
-      </c>
-      <c r="CN3" s="169">
-        <v>13</v>
-      </c>
-      <c r="CO3" s="169">
-        <v>16</v>
-      </c>
-      <c r="CP3" s="169">
-        <v>17</v>
-      </c>
-      <c r="CQ3" s="169">
-        <v>18</v>
-      </c>
-      <c r="CR3" s="169">
-        <v>19</v>
-      </c>
-      <c r="CS3" s="169">
-        <v>20</v>
-      </c>
-      <c r="CT3" s="6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="193" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="195" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="195"/>
-      <c r="D4" s="196" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" s="205" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" s="205" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="205" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="198" t="s">
-        <v>146</v>
-      </c>
-      <c r="I4" s="198" t="s">
-        <v>147</v>
-      </c>
-      <c r="J4" s="198" t="s">
-        <v>148</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="AV4" s="194"/>
-      <c r="AW4" s="194"/>
-      <c r="BT4" s="194"/>
-      <c r="BW4" s="194"/>
-      <c r="CT4" s="194"/>
-    </row>
-    <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="193"/>
-      <c r="B5" s="195" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="195"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="199"/>
-      <c r="F5" s="199"/>
-      <c r="G5" s="206"/>
-      <c r="H5" s="199"/>
-      <c r="I5" s="199"/>
-      <c r="J5" s="199"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="AV5" s="194"/>
-      <c r="AW5" s="194"/>
-      <c r="BT5" s="194"/>
-      <c r="BW5" s="194"/>
-      <c r="CT5" s="194"/>
-    </row>
-    <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="193"/>
-      <c r="B6" s="195" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="195"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="199"/>
-      <c r="F6" s="199"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="199"/>
-      <c r="I6" s="199"/>
-      <c r="J6" s="199"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="BT6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="CT6" s="194"/>
-    </row>
-    <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="193"/>
-      <c r="B7" s="195" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="206"/>
-      <c r="H7" s="199"/>
-      <c r="I7" s="199"/>
-      <c r="J7" s="199"/>
-      <c r="V7" s="10"/>
-      <c r="AV7" s="194"/>
-      <c r="AW7" s="194"/>
-      <c r="BT7" s="194"/>
-      <c r="BW7" s="194"/>
-      <c r="CT7" s="194"/>
-    </row>
-    <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="193" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="195" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="195"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="199"/>
-      <c r="F8" s="199"/>
-      <c r="G8" s="206"/>
-      <c r="H8" s="199"/>
-      <c r="I8" s="199"/>
-      <c r="J8" s="199"/>
-      <c r="AV8" s="194"/>
-      <c r="AW8" s="194"/>
-      <c r="BT8" s="194"/>
-      <c r="BW8" s="194"/>
-      <c r="CT8" s="194"/>
-    </row>
-    <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="193"/>
-      <c r="B9" s="195" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="195"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="199"/>
-      <c r="F9" s="199"/>
-      <c r="G9" s="206"/>
-      <c r="H9" s="199"/>
-      <c r="I9" s="199"/>
-      <c r="J9" s="199"/>
-      <c r="AV9" s="194"/>
-      <c r="AW9" s="194"/>
-      <c r="BT9" s="194"/>
-      <c r="BW9" s="194"/>
-      <c r="CT9" s="194"/>
-    </row>
-    <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="193"/>
-      <c r="B10" s="195" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="195"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="199"/>
-      <c r="F10" s="199"/>
-      <c r="G10" s="206"/>
-      <c r="H10" s="199"/>
-      <c r="I10" s="199"/>
-      <c r="J10" s="199"/>
-      <c r="AV10" s="194"/>
-      <c r="AW10" s="194"/>
-      <c r="BT10" s="194"/>
-      <c r="BW10" s="194"/>
-      <c r="CT10" s="194"/>
-    </row>
-    <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="193"/>
-      <c r="B11" s="195" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="195"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="199"/>
-      <c r="G11" s="206"/>
-      <c r="H11" s="199"/>
-      <c r="I11" s="199"/>
-      <c r="J11" s="199"/>
-      <c r="AV11" s="194"/>
-      <c r="AW11" s="194"/>
-      <c r="BT11" s="194"/>
-      <c r="BW11" s="194"/>
-      <c r="CT11" s="194"/>
-    </row>
-  </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
-  </mergeCells>
-  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adiciona congelamento de paineis
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1A4F1-02D2-4BA7-B987-E8B27B51FC44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CA997C-FFEF-4619-B893-768531905F9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -2154,49 +2154,26 @@
     <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="13" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2216,25 +2193,48 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="13" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2646,8 +2646,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CT11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -2958,110 +2961,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="195" t="s">
+      <c r="D2" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="195"/>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="195" t="s">
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
+      <c r="L2" s="184"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="184"/>
+      <c r="O2" s="184"/>
+      <c r="P2" s="184"/>
+      <c r="Q2" s="184"/>
+      <c r="R2" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="195"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="195"/>
-      <c r="V2" s="195"/>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195"/>
-      <c r="Z2" s="195"/>
-      <c r="AA2" s="195"/>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="195"/>
-      <c r="AD2" s="195"/>
-      <c r="AE2" s="195"/>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="195"/>
-      <c r="AH2" s="195"/>
-      <c r="AI2" s="195"/>
-      <c r="AJ2" s="195"/>
-      <c r="AK2" s="195"/>
-      <c r="AL2" s="195"/>
-      <c r="AM2" s="195" t="s">
+      <c r="S2" s="184"/>
+      <c r="T2" s="184"/>
+      <c r="U2" s="184"/>
+      <c r="V2" s="184"/>
+      <c r="W2" s="184"/>
+      <c r="X2" s="184"/>
+      <c r="Y2" s="184"/>
+      <c r="Z2" s="184"/>
+      <c r="AA2" s="184"/>
+      <c r="AB2" s="184"/>
+      <c r="AC2" s="184"/>
+      <c r="AD2" s="184"/>
+      <c r="AE2" s="184"/>
+      <c r="AF2" s="184"/>
+      <c r="AG2" s="184"/>
+      <c r="AH2" s="184"/>
+      <c r="AI2" s="184"/>
+      <c r="AJ2" s="184"/>
+      <c r="AK2" s="184"/>
+      <c r="AL2" s="184"/>
+      <c r="AM2" s="184" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="195"/>
-      <c r="AO2" s="195"/>
-      <c r="AP2" s="195"/>
-      <c r="AQ2" s="195"/>
-      <c r="AR2" s="195"/>
-      <c r="AS2" s="195"/>
-      <c r="AT2" s="195"/>
-      <c r="AU2" s="195"/>
-      <c r="AV2" s="195"/>
-      <c r="AW2" s="195"/>
-      <c r="AX2" s="196"/>
-      <c r="AY2" s="196"/>
-      <c r="AZ2" s="196"/>
-      <c r="BA2" s="196"/>
-      <c r="BB2" s="196"/>
-      <c r="BC2" s="196"/>
-      <c r="BD2" s="196"/>
-      <c r="BE2" s="196"/>
-      <c r="BF2" s="196"/>
-      <c r="BG2" s="196"/>
-      <c r="BH2" s="196"/>
-      <c r="BI2" s="196"/>
-      <c r="BJ2" s="195" t="s">
+      <c r="AN2" s="184"/>
+      <c r="AO2" s="184"/>
+      <c r="AP2" s="184"/>
+      <c r="AQ2" s="184"/>
+      <c r="AR2" s="184"/>
+      <c r="AS2" s="184"/>
+      <c r="AT2" s="184"/>
+      <c r="AU2" s="184"/>
+      <c r="AV2" s="184"/>
+      <c r="AW2" s="184"/>
+      <c r="AX2" s="185"/>
+      <c r="AY2" s="185"/>
+      <c r="AZ2" s="185"/>
+      <c r="BA2" s="185"/>
+      <c r="BB2" s="185"/>
+      <c r="BC2" s="185"/>
+      <c r="BD2" s="185"/>
+      <c r="BE2" s="185"/>
+      <c r="BF2" s="185"/>
+      <c r="BG2" s="185"/>
+      <c r="BH2" s="185"/>
+      <c r="BI2" s="185"/>
+      <c r="BJ2" s="184" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="195"/>
-      <c r="BL2" s="195"/>
-      <c r="BM2" s="195"/>
-      <c r="BN2" s="195"/>
-      <c r="BO2" s="195"/>
-      <c r="BP2" s="195"/>
-      <c r="BQ2" s="195"/>
-      <c r="BR2" s="195"/>
-      <c r="BS2" s="195"/>
-      <c r="BT2" s="195"/>
-      <c r="BU2" s="195"/>
-      <c r="BV2" s="195"/>
-      <c r="BW2" s="195"/>
-      <c r="BX2" s="197"/>
-      <c r="BY2" s="197"/>
-      <c r="BZ2" s="197"/>
-      <c r="CA2" s="197"/>
-      <c r="CB2" s="197"/>
-      <c r="CC2" s="197"/>
-      <c r="CD2" s="197"/>
-      <c r="CE2" s="198" t="s">
+      <c r="BK2" s="184"/>
+      <c r="BL2" s="184"/>
+      <c r="BM2" s="184"/>
+      <c r="BN2" s="184"/>
+      <c r="BO2" s="184"/>
+      <c r="BP2" s="184"/>
+      <c r="BQ2" s="184"/>
+      <c r="BR2" s="184"/>
+      <c r="BS2" s="184"/>
+      <c r="BT2" s="184"/>
+      <c r="BU2" s="184"/>
+      <c r="BV2" s="184"/>
+      <c r="BW2" s="184"/>
+      <c r="BX2" s="186"/>
+      <c r="BY2" s="186"/>
+      <c r="BZ2" s="186"/>
+      <c r="CA2" s="186"/>
+      <c r="CB2" s="186"/>
+      <c r="CC2" s="186"/>
+      <c r="CD2" s="186"/>
+      <c r="CE2" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="199"/>
-      <c r="CG2" s="199"/>
-      <c r="CH2" s="199"/>
-      <c r="CI2" s="199"/>
-      <c r="CJ2" s="199"/>
-      <c r="CK2" s="199"/>
-      <c r="CL2" s="199"/>
-      <c r="CM2" s="199"/>
-      <c r="CN2" s="199"/>
-      <c r="CO2" s="199"/>
-      <c r="CP2" s="199"/>
-      <c r="CQ2" s="199"/>
-      <c r="CR2" s="199"/>
-      <c r="CS2" s="199"/>
+      <c r="CF2" s="188"/>
+      <c r="CG2" s="188"/>
+      <c r="CH2" s="188"/>
+      <c r="CI2" s="188"/>
+      <c r="CJ2" s="188"/>
+      <c r="CK2" s="188"/>
+      <c r="CL2" s="188"/>
+      <c r="CM2" s="188"/>
+      <c r="CN2" s="188"/>
+      <c r="CO2" s="188"/>
+      <c r="CP2" s="188"/>
+      <c r="CQ2" s="188"/>
+      <c r="CR2" s="188"/>
+      <c r="CS2" s="188"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3357,32 +3360,32 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="204" t="s">
+      <c r="A4" s="177" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="205" t="s">
+      <c r="B4" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="205"/>
-      <c r="D4" s="206" t="s">
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="200" t="s">
+      <c r="E4" s="189" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="200" t="s">
+      <c r="F4" s="189" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="200" t="s">
+      <c r="G4" s="189" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="203" t="s">
+      <c r="H4" s="182" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="203" t="s">
+      <c r="I4" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="203" t="s">
+      <c r="J4" s="182" t="s">
         <v>148</v>
       </c>
       <c r="K4" s="7"/>
@@ -3392,25 +3395,25 @@
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="194"/>
-      <c r="AW4" s="194"/>
-      <c r="BT4" s="194"/>
-      <c r="BW4" s="194"/>
-      <c r="CT4" s="194"/>
+      <c r="AV4" s="178"/>
+      <c r="AW4" s="178"/>
+      <c r="BT4" s="178"/>
+      <c r="BW4" s="178"/>
+      <c r="CT4" s="178"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="204"/>
-      <c r="B5" s="205" t="s">
+      <c r="A5" s="177"/>
+      <c r="B5" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="205"/>
-      <c r="D5" s="207"/>
-      <c r="E5" s="201"/>
-      <c r="F5" s="201"/>
-      <c r="G5" s="202"/>
-      <c r="H5" s="201"/>
-      <c r="I5" s="201"/>
-      <c r="J5" s="201"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -3418,25 +3421,25 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="194"/>
-      <c r="AW5" s="194"/>
-      <c r="BT5" s="194"/>
-      <c r="BW5" s="194"/>
-      <c r="CT5" s="194"/>
+      <c r="AV5" s="178"/>
+      <c r="AW5" s="178"/>
+      <c r="BT5" s="178"/>
+      <c r="BW5" s="178"/>
+      <c r="CT5" s="178"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="204"/>
-      <c r="B6" s="205" t="s">
+      <c r="A6" s="177"/>
+      <c r="B6" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="205"/>
-      <c r="D6" s="207"/>
-      <c r="E6" s="201"/>
-      <c r="F6" s="201"/>
-      <c r="G6" s="202"/>
-      <c r="H6" s="201"/>
-      <c r="I6" s="201"/>
-      <c r="J6" s="201"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="190"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="183"/>
+      <c r="J6" s="183"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -3444,112 +3447,123 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="BT6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="CT6" s="194"/>
+      <c r="AV6" s="178"/>
+      <c r="AW6" s="178"/>
+      <c r="BT6" s="178"/>
+      <c r="BW6" s="178"/>
+      <c r="CT6" s="178"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="204"/>
-      <c r="B7" s="205" t="s">
+      <c r="A7" s="177"/>
+      <c r="B7" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="205"/>
-      <c r="D7" s="207"/>
-      <c r="E7" s="201"/>
-      <c r="F7" s="201"/>
-      <c r="G7" s="202"/>
-      <c r="H7" s="201"/>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
+      <c r="C7" s="179"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="190"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="194"/>
-      <c r="AW7" s="194"/>
-      <c r="BT7" s="194"/>
-      <c r="BW7" s="194"/>
-      <c r="CT7" s="194"/>
+      <c r="AV7" s="178"/>
+      <c r="AW7" s="178"/>
+      <c r="BT7" s="178"/>
+      <c r="BW7" s="178"/>
+      <c r="CT7" s="178"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="204" t="s">
+      <c r="A8" s="177" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="205" t="s">
+      <c r="B8" s="179" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="205"/>
-      <c r="D8" s="207"/>
-      <c r="E8" s="201"/>
-      <c r="F8" s="201"/>
-      <c r="G8" s="202"/>
-      <c r="H8" s="201"/>
-      <c r="I8" s="201"/>
-      <c r="J8" s="201"/>
-      <c r="AV8" s="194"/>
-      <c r="AW8" s="194"/>
-      <c r="BT8" s="194"/>
-      <c r="BW8" s="194"/>
-      <c r="CT8" s="194"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="183"/>
+      <c r="G8" s="190"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="183"/>
+      <c r="AV8" s="178"/>
+      <c r="AW8" s="178"/>
+      <c r="BT8" s="178"/>
+      <c r="BW8" s="178"/>
+      <c r="CT8" s="178"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="204"/>
-      <c r="B9" s="205" t="s">
+      <c r="A9" s="177"/>
+      <c r="B9" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="205"/>
-      <c r="D9" s="207"/>
-      <c r="E9" s="201"/>
-      <c r="F9" s="201"/>
-      <c r="G9" s="202"/>
-      <c r="H9" s="201"/>
-      <c r="I9" s="201"/>
-      <c r="J9" s="201"/>
-      <c r="AV9" s="194"/>
-      <c r="AW9" s="194"/>
-      <c r="BT9" s="194"/>
-      <c r="BW9" s="194"/>
-      <c r="CT9" s="194"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="183"/>
+      <c r="F9" s="183"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="183"/>
+      <c r="I9" s="183"/>
+      <c r="J9" s="183"/>
+      <c r="AV9" s="178"/>
+      <c r="AW9" s="178"/>
+      <c r="BT9" s="178"/>
+      <c r="BW9" s="178"/>
+      <c r="CT9" s="178"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="204"/>
-      <c r="B10" s="205" t="s">
+      <c r="A10" s="177"/>
+      <c r="B10" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="205"/>
-      <c r="D10" s="207"/>
-      <c r="E10" s="201"/>
-      <c r="F10" s="201"/>
-      <c r="G10" s="202"/>
-      <c r="H10" s="201"/>
-      <c r="I10" s="201"/>
-      <c r="J10" s="201"/>
-      <c r="AV10" s="194"/>
-      <c r="AW10" s="194"/>
-      <c r="BT10" s="194"/>
-      <c r="BW10" s="194"/>
-      <c r="CT10" s="194"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="190"/>
+      <c r="H10" s="183"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="183"/>
+      <c r="AV10" s="178"/>
+      <c r="AW10" s="178"/>
+      <c r="BT10" s="178"/>
+      <c r="BW10" s="178"/>
+      <c r="CT10" s="178"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="204"/>
-      <c r="B11" s="205" t="s">
+      <c r="A11" s="177"/>
+      <c r="B11" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="205"/>
-      <c r="D11" s="207"/>
-      <c r="E11" s="201"/>
-      <c r="F11" s="201"/>
-      <c r="G11" s="202"/>
-      <c r="H11" s="201"/>
-      <c r="I11" s="201"/>
-      <c r="J11" s="201"/>
-      <c r="AV11" s="194"/>
-      <c r="AW11" s="194"/>
-      <c r="BT11" s="194"/>
-      <c r="BW11" s="194"/>
-      <c r="CT11" s="194"/>
+      <c r="C11" s="179"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="190"/>
+      <c r="H11" s="183"/>
+      <c r="I11" s="183"/>
+      <c r="J11" s="183"/>
+      <c r="AV11" s="178"/>
+      <c r="AW11" s="178"/>
+      <c r="BT11" s="178"/>
+      <c r="BW11" s="178"/>
+      <c r="CT11" s="178"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -3566,17 +3580,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3589,7 +3592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -4250,13 +4253,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="179" t="s">
+      <c r="A4" s="203" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="181" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="182"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -4361,9 +4364,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="180"/>
-      <c r="B5" s="178"/>
-      <c r="C5" s="180"/>
+      <c r="A5" s="192"/>
+      <c r="B5" s="202"/>
+      <c r="C5" s="192"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -4468,11 +4471,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="180"/>
+      <c r="A6" s="192"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="180"/>
+      <c r="C6" s="192"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -4577,11 +4580,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="180"/>
+      <c r="A7" s="192"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="180"/>
+      <c r="C7" s="192"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -4686,11 +4689,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="180"/>
+      <c r="A8" s="192"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="180"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -4795,11 +4798,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="180"/>
+      <c r="A9" s="192"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="180"/>
+      <c r="C9" s="192"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -4904,11 +4907,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="180"/>
+      <c r="A10" s="192"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="180"/>
+      <c r="C10" s="192"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5013,11 +5016,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="180"/>
+      <c r="A11" s="192"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="180"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5122,9 +5125,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="180"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="183"/>
+      <c r="C12" s="193"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -5229,10 +5232,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="184" t="s">
+      <c r="A13" s="206" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="185" t="s">
+      <c r="B13" s="207" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -5341,8 +5344,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="180"/>
-      <c r="B14" s="186"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="198"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -5463,7 +5466,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="180"/>
+      <c r="A15" s="192"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -5573,7 +5576,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="180"/>
+      <c r="A16" s="192"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -5683,7 +5686,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="180"/>
+      <c r="A17" s="192"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -5795,7 +5798,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="180"/>
+      <c r="A18" s="192"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -5905,7 +5908,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="180"/>
+      <c r="A19" s="192"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -6015,7 +6018,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="180"/>
+      <c r="A20" s="192"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -6125,7 +6128,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="183"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -6236,7 +6239,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="177" t="s">
+      <c r="B22" s="201" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -6346,7 +6349,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="178"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -6453,13 +6456,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="188" t="s">
+      <c r="A24" s="194" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="190">
+      <c r="C24" s="196">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -6567,11 +6570,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="189"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="180"/>
+      <c r="C25" s="192"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -6677,11 +6680,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="189"/>
+      <c r="A26" s="195"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="180"/>
+      <c r="C26" s="192"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -6787,11 +6790,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="189"/>
+      <c r="A27" s="195"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="180"/>
+      <c r="C27" s="192"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -6897,11 +6900,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="189"/>
+      <c r="A28" s="195"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="180"/>
+      <c r="C28" s="192"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -7007,11 +7010,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="189"/>
+      <c r="A29" s="195"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="180"/>
+      <c r="C29" s="192"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -7117,11 +7120,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="189"/>
+      <c r="A30" s="195"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="180"/>
+      <c r="C30" s="192"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -7227,11 +7230,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="189"/>
+      <c r="A31" s="195"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="180"/>
+      <c r="C31" s="192"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -7337,11 +7340,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="189"/>
+      <c r="A32" s="195"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="180"/>
+      <c r="C32" s="192"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -7447,11 +7450,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="189"/>
+      <c r="A33" s="195"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="180"/>
+      <c r="C33" s="192"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -7557,11 +7560,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="189"/>
+      <c r="A34" s="195"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="180"/>
+      <c r="C34" s="192"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -7667,11 +7670,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="189"/>
+      <c r="A35" s="195"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="183"/>
+      <c r="C35" s="193"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -7777,11 +7780,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="189"/>
+      <c r="A36" s="195"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="190">
+      <c r="C36" s="196">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -7889,11 +7892,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="189"/>
+      <c r="A37" s="195"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="180"/>
+      <c r="C37" s="192"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -7999,11 +8002,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="189"/>
+      <c r="A38" s="195"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="180"/>
+      <c r="C38" s="192"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -8109,11 +8112,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="189"/>
+      <c r="A39" s="195"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="180"/>
+      <c r="C39" s="192"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -8219,11 +8222,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="189"/>
+      <c r="A40" s="195"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="180"/>
+      <c r="C40" s="192"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -8329,11 +8332,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="189"/>
+      <c r="A41" s="195"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="180"/>
+      <c r="C41" s="192"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -8439,11 +8442,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="189"/>
+      <c r="A42" s="195"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="180"/>
+      <c r="C42" s="192"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -8549,11 +8552,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="189"/>
+      <c r="A43" s="195"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="180"/>
+      <c r="C43" s="192"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -8659,11 +8662,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="189"/>
+      <c r="A44" s="195"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="180"/>
+      <c r="C44" s="192"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -8769,11 +8772,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="189"/>
+      <c r="A45" s="195"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="180"/>
+      <c r="C45" s="192"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -8879,11 +8882,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="189"/>
+      <c r="A46" s="195"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="180"/>
+      <c r="C46" s="192"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -8989,11 +8992,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="189"/>
+      <c r="A47" s="195"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="180"/>
+      <c r="C47" s="192"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -9107,11 +9110,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="189"/>
+      <c r="A48" s="195"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="180"/>
+      <c r="C48" s="192"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -9220,7 +9223,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="191" t="s">
+      <c r="B49" s="197" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -9330,7 +9333,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="186"/>
+      <c r="B50" s="198"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -12761,7 +12764,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="192" t="s">
+      <c r="A81" s="199" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -12873,7 +12876,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="180"/>
+      <c r="A82" s="192"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12983,7 +12986,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="180"/>
+      <c r="A83" s="192"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -13093,7 +13096,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="180"/>
+      <c r="A84" s="192"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -13203,7 +13206,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="180"/>
+      <c r="A85" s="192"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -13313,7 +13316,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="180"/>
+      <c r="A86" s="192"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -13423,7 +13426,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="180"/>
+      <c r="A87" s="192"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -13535,7 +13538,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="180"/>
+      <c r="A88" s="192"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -13645,7 +13648,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="180"/>
+      <c r="A89" s="192"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -13755,7 +13758,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="180"/>
+      <c r="A90" s="192"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -13865,11 +13868,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="180"/>
+      <c r="A91" s="192"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="193"/>
+      <c r="C91" s="200"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13975,11 +13978,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="180"/>
+      <c r="A92" s="192"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="180"/>
+      <c r="C92" s="192"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -14085,11 +14088,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="183"/>
+      <c r="A93" s="193"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="180"/>
+      <c r="C93" s="192"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -14313,7 +14316,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="187" t="s">
+      <c r="A95" s="191" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -14425,7 +14428,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="180"/>
+      <c r="A96" s="192"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -14535,7 +14538,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="180"/>
+      <c r="A97" s="192"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -14645,7 +14648,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="180"/>
+      <c r="A98" s="192"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -14755,7 +14758,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="180"/>
+      <c r="A99" s="192"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -14865,7 +14868,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="180"/>
+      <c r="A100" s="192"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14975,7 +14978,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="180"/>
+      <c r="A101" s="192"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -15085,7 +15088,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="180"/>
+      <c r="A102" s="192"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -15195,7 +15198,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="180"/>
+      <c r="A103" s="192"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -15307,7 +15310,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="180"/>
+      <c r="A104" s="192"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -15417,7 +15420,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="180"/>
+      <c r="A105" s="192"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -15535,7 +15538,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="180"/>
+      <c r="A106" s="192"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -15645,7 +15648,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="180"/>
+      <c r="A107" s="192"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -15755,7 +15758,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="180"/>
+      <c r="A108" s="192"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -15865,7 +15868,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="180"/>
+      <c r="A109" s="192"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15975,7 +15978,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="180"/>
+      <c r="A110" s="192"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -16085,7 +16088,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="180"/>
+      <c r="A111" s="192"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -16195,7 +16198,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="180"/>
+      <c r="A112" s="192"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -16305,7 +16308,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="180"/>
+      <c r="A113" s="192"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -16415,7 +16418,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="180"/>
+      <c r="A114" s="192"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -16525,7 +16528,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="180"/>
+      <c r="A115" s="192"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -16635,7 +16638,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="180"/>
+      <c r="A116" s="192"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -16761,7 +16764,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="180"/>
+      <c r="A117" s="192"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -16871,7 +16874,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="183"/>
+      <c r="A118" s="193"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -24242,6 +24245,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -24249,12 +24258,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 21-08
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CA997C-FFEF-4619-B893-768531905F9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020137D-3404-401E-90B6-136636373288}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="150">
   <si>
     <t>S</t>
   </si>
@@ -639,8 +639,11 @@
 Início do layout de baixa fidelidade dos projetos de cada grupo</t>
   </si>
   <si>
-    <t xml:space="preserve">Criação do layout de alta fidelidade de algumas páginas do projeto Gufos usando o XD.
-</t>
+    <t>Criação do layout de alta fidelidade de algumas páginas do projeto Gufos usando o XD.
+Início do layout de alta fidelidade dos projetos de cada grupo</t>
+  </si>
+  <si>
+    <t>Continuação dos layouts de alta fidelidade (web e mobile) dos projetos de cada grupo para a empresa Linx</t>
   </si>
 </sst>
 </file>
@@ -2154,26 +2157,8 @@
     <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2193,14 +2178,52 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2211,30 +2234,10 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2647,10 +2650,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4:D11"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -2961,110 +2964,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="184"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="184"/>
-      <c r="O2" s="184"/>
-      <c r="P2" s="184"/>
-      <c r="Q2" s="184"/>
-      <c r="R2" s="184" t="s">
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
+      <c r="Q2" s="178"/>
+      <c r="R2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="184"/>
-      <c r="T2" s="184"/>
-      <c r="U2" s="184"/>
-      <c r="V2" s="184"/>
-      <c r="W2" s="184"/>
-      <c r="X2" s="184"/>
-      <c r="Y2" s="184"/>
-      <c r="Z2" s="184"/>
-      <c r="AA2" s="184"/>
-      <c r="AB2" s="184"/>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="184"/>
-      <c r="AG2" s="184"/>
-      <c r="AH2" s="184"/>
-      <c r="AI2" s="184"/>
-      <c r="AJ2" s="184"/>
-      <c r="AK2" s="184"/>
-      <c r="AL2" s="184"/>
-      <c r="AM2" s="184" t="s">
+      <c r="S2" s="178"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="178"/>
+      <c r="V2" s="178"/>
+      <c r="W2" s="178"/>
+      <c r="X2" s="178"/>
+      <c r="Y2" s="178"/>
+      <c r="Z2" s="178"/>
+      <c r="AA2" s="178"/>
+      <c r="AB2" s="178"/>
+      <c r="AC2" s="178"/>
+      <c r="AD2" s="178"/>
+      <c r="AE2" s="178"/>
+      <c r="AF2" s="178"/>
+      <c r="AG2" s="178"/>
+      <c r="AH2" s="178"/>
+      <c r="AI2" s="178"/>
+      <c r="AJ2" s="178"/>
+      <c r="AK2" s="178"/>
+      <c r="AL2" s="178"/>
+      <c r="AM2" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="184"/>
-      <c r="AO2" s="184"/>
-      <c r="AP2" s="184"/>
-      <c r="AQ2" s="184"/>
-      <c r="AR2" s="184"/>
-      <c r="AS2" s="184"/>
-      <c r="AT2" s="184"/>
-      <c r="AU2" s="184"/>
-      <c r="AV2" s="184"/>
-      <c r="AW2" s="184"/>
-      <c r="AX2" s="185"/>
-      <c r="AY2" s="185"/>
-      <c r="AZ2" s="185"/>
-      <c r="BA2" s="185"/>
-      <c r="BB2" s="185"/>
-      <c r="BC2" s="185"/>
-      <c r="BD2" s="185"/>
-      <c r="BE2" s="185"/>
-      <c r="BF2" s="185"/>
-      <c r="BG2" s="185"/>
-      <c r="BH2" s="185"/>
-      <c r="BI2" s="185"/>
-      <c r="BJ2" s="184" t="s">
+      <c r="AN2" s="178"/>
+      <c r="AO2" s="178"/>
+      <c r="AP2" s="178"/>
+      <c r="AQ2" s="178"/>
+      <c r="AR2" s="178"/>
+      <c r="AS2" s="178"/>
+      <c r="AT2" s="178"/>
+      <c r="AU2" s="178"/>
+      <c r="AV2" s="178"/>
+      <c r="AW2" s="178"/>
+      <c r="AX2" s="179"/>
+      <c r="AY2" s="179"/>
+      <c r="AZ2" s="179"/>
+      <c r="BA2" s="179"/>
+      <c r="BB2" s="179"/>
+      <c r="BC2" s="179"/>
+      <c r="BD2" s="179"/>
+      <c r="BE2" s="179"/>
+      <c r="BF2" s="179"/>
+      <c r="BG2" s="179"/>
+      <c r="BH2" s="179"/>
+      <c r="BI2" s="179"/>
+      <c r="BJ2" s="178" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="184"/>
-      <c r="BL2" s="184"/>
-      <c r="BM2" s="184"/>
-      <c r="BN2" s="184"/>
-      <c r="BO2" s="184"/>
-      <c r="BP2" s="184"/>
-      <c r="BQ2" s="184"/>
-      <c r="BR2" s="184"/>
-      <c r="BS2" s="184"/>
-      <c r="BT2" s="184"/>
-      <c r="BU2" s="184"/>
-      <c r="BV2" s="184"/>
-      <c r="BW2" s="184"/>
-      <c r="BX2" s="186"/>
-      <c r="BY2" s="186"/>
-      <c r="BZ2" s="186"/>
-      <c r="CA2" s="186"/>
-      <c r="CB2" s="186"/>
-      <c r="CC2" s="186"/>
-      <c r="CD2" s="186"/>
-      <c r="CE2" s="187" t="s">
+      <c r="BK2" s="178"/>
+      <c r="BL2" s="178"/>
+      <c r="BM2" s="178"/>
+      <c r="BN2" s="178"/>
+      <c r="BO2" s="178"/>
+      <c r="BP2" s="178"/>
+      <c r="BQ2" s="178"/>
+      <c r="BR2" s="178"/>
+      <c r="BS2" s="178"/>
+      <c r="BT2" s="178"/>
+      <c r="BU2" s="178"/>
+      <c r="BV2" s="178"/>
+      <c r="BW2" s="178"/>
+      <c r="BX2" s="180"/>
+      <c r="BY2" s="180"/>
+      <c r="BZ2" s="180"/>
+      <c r="CA2" s="180"/>
+      <c r="CB2" s="180"/>
+      <c r="CC2" s="180"/>
+      <c r="CD2" s="180"/>
+      <c r="CE2" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="188"/>
-      <c r="CG2" s="188"/>
-      <c r="CH2" s="188"/>
-      <c r="CI2" s="188"/>
-      <c r="CJ2" s="188"/>
-      <c r="CK2" s="188"/>
-      <c r="CL2" s="188"/>
-      <c r="CM2" s="188"/>
-      <c r="CN2" s="188"/>
-      <c r="CO2" s="188"/>
-      <c r="CP2" s="188"/>
-      <c r="CQ2" s="188"/>
-      <c r="CR2" s="188"/>
-      <c r="CS2" s="188"/>
+      <c r="CF2" s="182"/>
+      <c r="CG2" s="182"/>
+      <c r="CH2" s="182"/>
+      <c r="CI2" s="182"/>
+      <c r="CJ2" s="182"/>
+      <c r="CK2" s="182"/>
+      <c r="CL2" s="182"/>
+      <c r="CM2" s="182"/>
+      <c r="CN2" s="182"/>
+      <c r="CO2" s="182"/>
+      <c r="CP2" s="182"/>
+      <c r="CQ2" s="182"/>
+      <c r="CR2" s="182"/>
+      <c r="CS2" s="182"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3360,210 +3363,206 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="177" t="s">
+      <c r="A4" s="187" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
+      <c r="C4" s="188"/>
+      <c r="D4" s="189" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="189" t="s">
+      <c r="E4" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="189" t="s">
+      <c r="F4" s="183" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="189" t="s">
+      <c r="G4" s="183" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="182" t="s">
+      <c r="H4" s="186" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="182" t="s">
+      <c r="I4" s="186" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="182" t="s">
+      <c r="J4" s="186" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="186" t="s">
+        <v>149</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="178"/>
-      <c r="AW4" s="178"/>
-      <c r="BT4" s="178"/>
-      <c r="BW4" s="178"/>
-      <c r="CT4" s="178"/>
+      <c r="AV4" s="177"/>
+      <c r="AW4" s="177"/>
+      <c r="BT4" s="177"/>
+      <c r="BW4" s="177"/>
+      <c r="CT4" s="177"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="177"/>
-      <c r="B5" s="179" t="s">
+      <c r="A5" s="187"/>
+      <c r="B5" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="179"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="183"/>
-      <c r="F5" s="183"/>
-      <c r="G5" s="190"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183"/>
-      <c r="K5" s="7"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="185"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="184"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="178"/>
-      <c r="AW5" s="178"/>
-      <c r="BT5" s="178"/>
-      <c r="BW5" s="178"/>
-      <c r="CT5" s="178"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="BT5" s="177"/>
+      <c r="BW5" s="177"/>
+      <c r="CT5" s="177"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="177"/>
-      <c r="B6" s="179" t="s">
+      <c r="A6" s="187"/>
+      <c r="B6" s="188" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="183"/>
-      <c r="F6" s="183"/>
-      <c r="G6" s="190"/>
-      <c r="H6" s="183"/>
-      <c r="I6" s="183"/>
-      <c r="J6" s="183"/>
-      <c r="K6" s="7"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="184"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="178"/>
-      <c r="AW6" s="178"/>
-      <c r="BT6" s="178"/>
-      <c r="BW6" s="178"/>
-      <c r="CT6" s="178"/>
+      <c r="AV6" s="177"/>
+      <c r="AW6" s="177"/>
+      <c r="BT6" s="177"/>
+      <c r="BW6" s="177"/>
+      <c r="CT6" s="177"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="177"/>
-      <c r="B7" s="179" t="s">
+      <c r="A7" s="187"/>
+      <c r="B7" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="179"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="190"/>
-      <c r="H7" s="183"/>
-      <c r="I7" s="183"/>
-      <c r="J7" s="183"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="190"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="184"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="184"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="178"/>
-      <c r="AW7" s="178"/>
-      <c r="BT7" s="178"/>
-      <c r="BW7" s="178"/>
-      <c r="CT7" s="178"/>
+      <c r="AV7" s="177"/>
+      <c r="AW7" s="177"/>
+      <c r="BT7" s="177"/>
+      <c r="BW7" s="177"/>
+      <c r="CT7" s="177"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="177" t="s">
+      <c r="A8" s="187" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="179" t="s">
+      <c r="B8" s="188" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="179"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="183"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="190"/>
-      <c r="H8" s="183"/>
-      <c r="I8" s="183"/>
-      <c r="J8" s="183"/>
-      <c r="AV8" s="178"/>
-      <c r="AW8" s="178"/>
-      <c r="BT8" s="178"/>
-      <c r="BW8" s="178"/>
-      <c r="CT8" s="178"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="190"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="184"/>
+      <c r="AV8" s="177"/>
+      <c r="AW8" s="177"/>
+      <c r="BT8" s="177"/>
+      <c r="BW8" s="177"/>
+      <c r="CT8" s="177"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="177"/>
-      <c r="B9" s="179" t="s">
+      <c r="A9" s="187"/>
+      <c r="B9" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="179"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="183"/>
-      <c r="F9" s="183"/>
-      <c r="G9" s="190"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="183"/>
-      <c r="J9" s="183"/>
-      <c r="AV9" s="178"/>
-      <c r="AW9" s="178"/>
-      <c r="BT9" s="178"/>
-      <c r="BW9" s="178"/>
-      <c r="CT9" s="178"/>
+      <c r="C9" s="188"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="185"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="184"/>
+      <c r="AV9" s="177"/>
+      <c r="AW9" s="177"/>
+      <c r="BT9" s="177"/>
+      <c r="BW9" s="177"/>
+      <c r="CT9" s="177"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="177"/>
-      <c r="B10" s="179" t="s">
+      <c r="A10" s="187"/>
+      <c r="B10" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="179"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="190"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="183"/>
-      <c r="AV10" s="178"/>
-      <c r="AW10" s="178"/>
-      <c r="BT10" s="178"/>
-      <c r="BW10" s="178"/>
-      <c r="CT10" s="178"/>
+      <c r="C10" s="188"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="184"/>
+      <c r="AV10" s="177"/>
+      <c r="AW10" s="177"/>
+      <c r="BT10" s="177"/>
+      <c r="BW10" s="177"/>
+      <c r="CT10" s="177"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="177"/>
-      <c r="B11" s="179" t="s">
+      <c r="A11" s="187"/>
+      <c r="B11" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="179"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="183"/>
-      <c r="F11" s="183"/>
-      <c r="G11" s="190"/>
-      <c r="H11" s="183"/>
-      <c r="I11" s="183"/>
-      <c r="J11" s="183"/>
-      <c r="AV11" s="178"/>
-      <c r="AW11" s="178"/>
-      <c r="BT11" s="178"/>
-      <c r="BW11" s="178"/>
-      <c r="CT11" s="178"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="190"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="184"/>
+      <c r="AV11" s="177"/>
+      <c r="AW11" s="177"/>
+      <c r="BT11" s="177"/>
+      <c r="BW11" s="177"/>
+      <c r="CT11" s="177"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
+  <mergeCells count="28">
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -3580,6 +3579,18 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4253,13 +4264,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="193" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="196"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -4364,9 +4375,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="192"/>
-      <c r="B5" s="202"/>
-      <c r="C5" s="192"/>
+      <c r="A5" s="194"/>
+      <c r="B5" s="192"/>
+      <c r="C5" s="194"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -4471,11 +4482,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="192"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="192"/>
+      <c r="C6" s="194"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -4580,11 +4591,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="192"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="192"/>
+      <c r="C7" s="194"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -4689,11 +4700,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="192"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="192"/>
+      <c r="C8" s="194"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -4798,11 +4809,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="192"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="192"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -4907,11 +4918,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="192"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="192"/>
+      <c r="C10" s="194"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5016,11 +5027,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="192"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="192"/>
+      <c r="C11" s="194"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5125,9 +5136,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="192"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="193"/>
+      <c r="C12" s="197"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -5232,10 +5243,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="198" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="207" t="s">
+      <c r="B13" s="199" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -5344,8 +5355,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="192"/>
-      <c r="B14" s="198"/>
+      <c r="A14" s="194"/>
+      <c r="B14" s="200"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -5466,7 +5477,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="192"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -5576,7 +5587,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="192"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -5686,7 +5697,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="192"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -5798,7 +5809,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="192"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -5908,7 +5919,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="192"/>
+      <c r="A19" s="194"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -6018,7 +6029,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="192"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -6128,7 +6139,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="193"/>
+      <c r="A21" s="197"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -6239,7 +6250,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="201" t="s">
+      <c r="B22" s="191" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -6349,7 +6360,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="202"/>
+      <c r="B23" s="192"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -6456,13 +6467,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="194" t="s">
+      <c r="A24" s="202" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="196">
+      <c r="C24" s="204">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -6570,11 +6581,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="195"/>
+      <c r="A25" s="203"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="192"/>
+      <c r="C25" s="194"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -6680,11 +6691,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="195"/>
+      <c r="A26" s="203"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="192"/>
+      <c r="C26" s="194"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -6790,11 +6801,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="195"/>
+      <c r="A27" s="203"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="192"/>
+      <c r="C27" s="194"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -6900,11 +6911,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="195"/>
+      <c r="A28" s="203"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="192"/>
+      <c r="C28" s="194"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -7010,11 +7021,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="195"/>
+      <c r="A29" s="203"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="192"/>
+      <c r="C29" s="194"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -7120,11 +7131,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="195"/>
+      <c r="A30" s="203"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="192"/>
+      <c r="C30" s="194"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -7230,11 +7241,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="195"/>
+      <c r="A31" s="203"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="192"/>
+      <c r="C31" s="194"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -7340,11 +7351,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="195"/>
+      <c r="A32" s="203"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="192"/>
+      <c r="C32" s="194"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -7450,11 +7461,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="195"/>
+      <c r="A33" s="203"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="192"/>
+      <c r="C33" s="194"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -7560,11 +7571,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="195"/>
+      <c r="A34" s="203"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="192"/>
+      <c r="C34" s="194"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -7670,11 +7681,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="195"/>
+      <c r="A35" s="203"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="193"/>
+      <c r="C35" s="197"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -7780,11 +7791,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="195"/>
+      <c r="A36" s="203"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="196">
+      <c r="C36" s="204">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -7892,11 +7903,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="195"/>
+      <c r="A37" s="203"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="192"/>
+      <c r="C37" s="194"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -8002,11 +8013,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="195"/>
+      <c r="A38" s="203"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="192"/>
+      <c r="C38" s="194"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -8112,11 +8123,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="195"/>
+      <c r="A39" s="203"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="192"/>
+      <c r="C39" s="194"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -8222,11 +8233,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="195"/>
+      <c r="A40" s="203"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="192"/>
+      <c r="C40" s="194"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -8332,11 +8343,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="195"/>
+      <c r="A41" s="203"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="192"/>
+      <c r="C41" s="194"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -8442,11 +8453,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="195"/>
+      <c r="A42" s="203"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="192"/>
+      <c r="C42" s="194"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -8552,11 +8563,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="195"/>
+      <c r="A43" s="203"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="192"/>
+      <c r="C43" s="194"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -8662,11 +8673,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="195"/>
+      <c r="A44" s="203"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="192"/>
+      <c r="C44" s="194"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -8772,11 +8783,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="195"/>
+      <c r="A45" s="203"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="192"/>
+      <c r="C45" s="194"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -8882,11 +8893,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="195"/>
+      <c r="A46" s="203"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="192"/>
+      <c r="C46" s="194"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -8992,11 +9003,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="195"/>
+      <c r="A47" s="203"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="192"/>
+      <c r="C47" s="194"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -9110,11 +9121,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="195"/>
+      <c r="A48" s="203"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="192"/>
+      <c r="C48" s="194"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -9223,7 +9234,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="197" t="s">
+      <c r="B49" s="205" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -9333,7 +9344,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="198"/>
+      <c r="B50" s="200"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -12764,7 +12775,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="199" t="s">
+      <c r="A81" s="206" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -12876,7 +12887,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="192"/>
+      <c r="A82" s="194"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12986,7 +12997,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="192"/>
+      <c r="A83" s="194"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -13096,7 +13107,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="192"/>
+      <c r="A84" s="194"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -13206,7 +13217,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="192"/>
+      <c r="A85" s="194"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -13316,7 +13327,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="192"/>
+      <c r="A86" s="194"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -13426,7 +13437,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="192"/>
+      <c r="A87" s="194"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -13538,7 +13549,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="192"/>
+      <c r="A88" s="194"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -13648,7 +13659,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="192"/>
+      <c r="A89" s="194"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -13758,7 +13769,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="192"/>
+      <c r="A90" s="194"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -13868,11 +13879,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="192"/>
+      <c r="A91" s="194"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="200"/>
+      <c r="C91" s="207"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13978,11 +13989,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="192"/>
+      <c r="A92" s="194"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="192"/>
+      <c r="C92" s="194"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -14088,11 +14099,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="193"/>
+      <c r="A93" s="197"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="192"/>
+      <c r="C93" s="194"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -14316,7 +14327,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="191" t="s">
+      <c r="A95" s="201" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -14428,7 +14439,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="192"/>
+      <c r="A96" s="194"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -14538,7 +14549,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="192"/>
+      <c r="A97" s="194"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -14648,7 +14659,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="192"/>
+      <c r="A98" s="194"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -14758,7 +14769,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="192"/>
+      <c r="A99" s="194"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -14868,7 +14879,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="192"/>
+      <c r="A100" s="194"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14978,7 +14989,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="192"/>
+      <c r="A101" s="194"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -15088,7 +15099,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="192"/>
+      <c r="A102" s="194"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -15198,7 +15209,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="192"/>
+      <c r="A103" s="194"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -15310,7 +15321,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="192"/>
+      <c r="A104" s="194"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -15420,7 +15431,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="192"/>
+      <c r="A105" s="194"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -15538,7 +15549,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="192"/>
+      <c r="A106" s="194"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -15648,7 +15659,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="192"/>
+      <c r="A107" s="194"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -15758,7 +15769,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="192"/>
+      <c r="A108" s="194"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -15868,7 +15879,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="192"/>
+      <c r="A109" s="194"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15978,7 +15989,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="192"/>
+      <c r="A110" s="194"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -16088,7 +16099,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="192"/>
+      <c r="A111" s="194"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -16198,7 +16209,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="192"/>
+      <c r="A112" s="194"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -16308,7 +16319,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="192"/>
+      <c r="A113" s="194"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -16418,7 +16429,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="192"/>
+      <c r="A114" s="194"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -16528,7 +16539,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="192"/>
+      <c r="A115" s="194"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -16638,7 +16649,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="192"/>
+      <c r="A116" s="194"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -16764,7 +16775,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="192"/>
+      <c r="A117" s="194"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -16874,7 +16885,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="193"/>
+      <c r="A118" s="197"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -24245,12 +24256,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -24258,6 +24263,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 22 e 23-08
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2020137D-3404-401E-90B6-136636373288}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755B0D8C-C7DD-45C5-8658-04D5D439260A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="151">
   <si>
     <t>S</t>
   </si>
@@ -643,7 +643,12 @@
 Início do layout de alta fidelidade dos projetos de cada grupo</t>
   </si>
   <si>
-    <t>Continuação dos layouts de alta fidelidade (web e mobile) dos projetos de cada grupo para a empresa Linx</t>
+    <t>Continuação dos layouts de alta fidelidade (web e mobile) dos projetos de cada grupo para a empresa Linx.
+Encerramento da Sprint 2</t>
+  </si>
+  <si>
+    <t>Aula sobre Git e GitHub.
+Introdução ao HTML com uma atividade para entrega</t>
   </si>
 </sst>
 </file>
@@ -2157,8 +2162,26 @@
     <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2178,52 +2201,14 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2234,10 +2219,30 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2650,10 +2655,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -2964,110 +2969,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="178"/>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178"/>
-      <c r="N2" s="178"/>
-      <c r="O2" s="178"/>
-      <c r="P2" s="178"/>
-      <c r="Q2" s="178"/>
-      <c r="R2" s="178" t="s">
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
+      <c r="L2" s="184"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="184"/>
+      <c r="O2" s="184"/>
+      <c r="P2" s="184"/>
+      <c r="Q2" s="184"/>
+      <c r="R2" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="178"/>
-      <c r="T2" s="178"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="178"/>
-      <c r="W2" s="178"/>
-      <c r="X2" s="178"/>
-      <c r="Y2" s="178"/>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="178"/>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="178"/>
-      <c r="AG2" s="178"/>
-      <c r="AH2" s="178"/>
-      <c r="AI2" s="178"/>
-      <c r="AJ2" s="178"/>
-      <c r="AK2" s="178"/>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="178" t="s">
+      <c r="S2" s="184"/>
+      <c r="T2" s="184"/>
+      <c r="U2" s="184"/>
+      <c r="V2" s="184"/>
+      <c r="W2" s="184"/>
+      <c r="X2" s="184"/>
+      <c r="Y2" s="184"/>
+      <c r="Z2" s="184"/>
+      <c r="AA2" s="184"/>
+      <c r="AB2" s="184"/>
+      <c r="AC2" s="184"/>
+      <c r="AD2" s="184"/>
+      <c r="AE2" s="184"/>
+      <c r="AF2" s="184"/>
+      <c r="AG2" s="184"/>
+      <c r="AH2" s="184"/>
+      <c r="AI2" s="184"/>
+      <c r="AJ2" s="184"/>
+      <c r="AK2" s="184"/>
+      <c r="AL2" s="184"/>
+      <c r="AM2" s="184" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="178"/>
-      <c r="AP2" s="178"/>
-      <c r="AQ2" s="178"/>
-      <c r="AR2" s="178"/>
-      <c r="AS2" s="178"/>
-      <c r="AT2" s="178"/>
-      <c r="AU2" s="178"/>
-      <c r="AV2" s="178"/>
-      <c r="AW2" s="178"/>
-      <c r="AX2" s="179"/>
-      <c r="AY2" s="179"/>
-      <c r="AZ2" s="179"/>
-      <c r="BA2" s="179"/>
-      <c r="BB2" s="179"/>
-      <c r="BC2" s="179"/>
-      <c r="BD2" s="179"/>
-      <c r="BE2" s="179"/>
-      <c r="BF2" s="179"/>
-      <c r="BG2" s="179"/>
-      <c r="BH2" s="179"/>
-      <c r="BI2" s="179"/>
-      <c r="BJ2" s="178" t="s">
+      <c r="AN2" s="184"/>
+      <c r="AO2" s="184"/>
+      <c r="AP2" s="184"/>
+      <c r="AQ2" s="184"/>
+      <c r="AR2" s="184"/>
+      <c r="AS2" s="184"/>
+      <c r="AT2" s="184"/>
+      <c r="AU2" s="184"/>
+      <c r="AV2" s="184"/>
+      <c r="AW2" s="184"/>
+      <c r="AX2" s="185"/>
+      <c r="AY2" s="185"/>
+      <c r="AZ2" s="185"/>
+      <c r="BA2" s="185"/>
+      <c r="BB2" s="185"/>
+      <c r="BC2" s="185"/>
+      <c r="BD2" s="185"/>
+      <c r="BE2" s="185"/>
+      <c r="BF2" s="185"/>
+      <c r="BG2" s="185"/>
+      <c r="BH2" s="185"/>
+      <c r="BI2" s="185"/>
+      <c r="BJ2" s="184" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="178"/>
-      <c r="BL2" s="178"/>
-      <c r="BM2" s="178"/>
-      <c r="BN2" s="178"/>
-      <c r="BO2" s="178"/>
-      <c r="BP2" s="178"/>
-      <c r="BQ2" s="178"/>
-      <c r="BR2" s="178"/>
-      <c r="BS2" s="178"/>
-      <c r="BT2" s="178"/>
-      <c r="BU2" s="178"/>
-      <c r="BV2" s="178"/>
-      <c r="BW2" s="178"/>
-      <c r="BX2" s="180"/>
-      <c r="BY2" s="180"/>
-      <c r="BZ2" s="180"/>
-      <c r="CA2" s="180"/>
-      <c r="CB2" s="180"/>
-      <c r="CC2" s="180"/>
-      <c r="CD2" s="180"/>
-      <c r="CE2" s="181" t="s">
+      <c r="BK2" s="184"/>
+      <c r="BL2" s="184"/>
+      <c r="BM2" s="184"/>
+      <c r="BN2" s="184"/>
+      <c r="BO2" s="184"/>
+      <c r="BP2" s="184"/>
+      <c r="BQ2" s="184"/>
+      <c r="BR2" s="184"/>
+      <c r="BS2" s="184"/>
+      <c r="BT2" s="184"/>
+      <c r="BU2" s="184"/>
+      <c r="BV2" s="184"/>
+      <c r="BW2" s="184"/>
+      <c r="BX2" s="186"/>
+      <c r="BY2" s="186"/>
+      <c r="BZ2" s="186"/>
+      <c r="CA2" s="186"/>
+      <c r="CB2" s="186"/>
+      <c r="CC2" s="186"/>
+      <c r="CD2" s="186"/>
+      <c r="CE2" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="182"/>
-      <c r="CG2" s="182"/>
-      <c r="CH2" s="182"/>
-      <c r="CI2" s="182"/>
-      <c r="CJ2" s="182"/>
-      <c r="CK2" s="182"/>
-      <c r="CL2" s="182"/>
-      <c r="CM2" s="182"/>
-      <c r="CN2" s="182"/>
-      <c r="CO2" s="182"/>
-      <c r="CP2" s="182"/>
-      <c r="CQ2" s="182"/>
-      <c r="CR2" s="182"/>
-      <c r="CS2" s="182"/>
+      <c r="CF2" s="188"/>
+      <c r="CG2" s="188"/>
+      <c r="CH2" s="188"/>
+      <c r="CI2" s="188"/>
+      <c r="CJ2" s="188"/>
+      <c r="CK2" s="188"/>
+      <c r="CL2" s="188"/>
+      <c r="CM2" s="188"/>
+      <c r="CN2" s="188"/>
+      <c r="CO2" s="188"/>
+      <c r="CP2" s="188"/>
+      <c r="CQ2" s="188"/>
+      <c r="CR2" s="188"/>
+      <c r="CS2" s="188"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3363,206 +3368,226 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="177" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="188" t="s">
+      <c r="B4" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="189" t="s">
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="183" t="s">
+      <c r="E4" s="189" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="183" t="s">
+      <c r="F4" s="189" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="183" t="s">
+      <c r="G4" s="189" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="186" t="s">
+      <c r="H4" s="182" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="186" t="s">
+      <c r="I4" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="186" t="s">
+      <c r="J4" s="182" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="186" t="s">
+      <c r="K4" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="189" t="s">
+        <v>150</v>
+      </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="177"/>
-      <c r="AW4" s="177"/>
-      <c r="BT4" s="177"/>
-      <c r="BW4" s="177"/>
-      <c r="CT4" s="177"/>
+      <c r="AV4" s="178"/>
+      <c r="AW4" s="178"/>
+      <c r="BT4" s="178"/>
+      <c r="BW4" s="178"/>
+      <c r="CT4" s="178"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="187"/>
-      <c r="B5" s="188" t="s">
+      <c r="A5" s="177"/>
+      <c r="B5" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="188"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="185"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="7"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
+      <c r="K5" s="183"/>
+      <c r="L5" s="183"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="177"/>
-      <c r="AW5" s="177"/>
-      <c r="BT5" s="177"/>
-      <c r="BW5" s="177"/>
-      <c r="CT5" s="177"/>
+      <c r="AV5" s="178"/>
+      <c r="AW5" s="178"/>
+      <c r="BT5" s="178"/>
+      <c r="BW5" s="178"/>
+      <c r="CT5" s="178"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="187"/>
-      <c r="B6" s="188" t="s">
+      <c r="A6" s="177"/>
+      <c r="B6" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="188"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184"/>
-      <c r="J6" s="184"/>
-      <c r="K6" s="184"/>
-      <c r="L6" s="7"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="190"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="183"/>
+      <c r="J6" s="183"/>
+      <c r="K6" s="183"/>
+      <c r="L6" s="183"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="177"/>
-      <c r="AW6" s="177"/>
-      <c r="BT6" s="177"/>
-      <c r="BW6" s="177"/>
-      <c r="CT6" s="177"/>
+      <c r="AV6" s="178"/>
+      <c r="AW6" s="178"/>
+      <c r="BT6" s="178"/>
+      <c r="BW6" s="178"/>
+      <c r="CT6" s="178"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="187"/>
-      <c r="B7" s="188" t="s">
+      <c r="A7" s="177"/>
+      <c r="B7" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="188"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="185"/>
-      <c r="H7" s="184"/>
-      <c r="I7" s="184"/>
-      <c r="J7" s="184"/>
-      <c r="K7" s="184"/>
+      <c r="C7" s="179"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="190"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="183"/>
+      <c r="L7" s="183"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="177"/>
-      <c r="AW7" s="177"/>
-      <c r="BT7" s="177"/>
-      <c r="BW7" s="177"/>
-      <c r="CT7" s="177"/>
+      <c r="AV7" s="178"/>
+      <c r="AW7" s="178"/>
+      <c r="BT7" s="178"/>
+      <c r="BW7" s="178"/>
+      <c r="CT7" s="178"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="187" t="s">
+      <c r="A8" s="177" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="188" t="s">
+      <c r="B8" s="179" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="188"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="184"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="185"/>
-      <c r="H8" s="184"/>
-      <c r="I8" s="184"/>
-      <c r="J8" s="184"/>
-      <c r="K8" s="184"/>
-      <c r="AV8" s="177"/>
-      <c r="AW8" s="177"/>
-      <c r="BT8" s="177"/>
-      <c r="BW8" s="177"/>
-      <c r="CT8" s="177"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="183"/>
+      <c r="G8" s="190"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="183"/>
+      <c r="K8" s="183"/>
+      <c r="L8" s="183"/>
+      <c r="AV8" s="178"/>
+      <c r="AW8" s="178"/>
+      <c r="BT8" s="178"/>
+      <c r="BW8" s="178"/>
+      <c r="CT8" s="178"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="187"/>
-      <c r="B9" s="188" t="s">
+      <c r="A9" s="177"/>
+      <c r="B9" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="188"/>
-      <c r="D9" s="190"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="185"/>
-      <c r="H9" s="184"/>
-      <c r="I9" s="184"/>
-      <c r="J9" s="184"/>
-      <c r="K9" s="184"/>
-      <c r="AV9" s="177"/>
-      <c r="AW9" s="177"/>
-      <c r="BT9" s="177"/>
-      <c r="BW9" s="177"/>
-      <c r="CT9" s="177"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="183"/>
+      <c r="F9" s="183"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="183"/>
+      <c r="I9" s="183"/>
+      <c r="J9" s="183"/>
+      <c r="K9" s="183"/>
+      <c r="L9" s="183"/>
+      <c r="AV9" s="178"/>
+      <c r="AW9" s="178"/>
+      <c r="BT9" s="178"/>
+      <c r="BW9" s="178"/>
+      <c r="CT9" s="178"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="187"/>
-      <c r="B10" s="188" t="s">
+      <c r="A10" s="177"/>
+      <c r="B10" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="188"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="185"/>
-      <c r="H10" s="184"/>
-      <c r="I10" s="184"/>
-      <c r="J10" s="184"/>
-      <c r="K10" s="184"/>
-      <c r="AV10" s="177"/>
-      <c r="AW10" s="177"/>
-      <c r="BT10" s="177"/>
-      <c r="BW10" s="177"/>
-      <c r="CT10" s="177"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="190"/>
+      <c r="H10" s="183"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="183"/>
+      <c r="K10" s="183"/>
+      <c r="L10" s="183"/>
+      <c r="AV10" s="178"/>
+      <c r="AW10" s="178"/>
+      <c r="BT10" s="178"/>
+      <c r="BW10" s="178"/>
+      <c r="CT10" s="178"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="187"/>
-      <c r="B11" s="188" t="s">
+      <c r="A11" s="177"/>
+      <c r="B11" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="184"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="185"/>
-      <c r="H11" s="184"/>
-      <c r="I11" s="184"/>
-      <c r="J11" s="184"/>
-      <c r="K11" s="184"/>
-      <c r="AV11" s="177"/>
-      <c r="AW11" s="177"/>
-      <c r="BT11" s="177"/>
-      <c r="BW11" s="177"/>
-      <c r="CT11" s="177"/>
+      <c r="C11" s="179"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="190"/>
+      <c r="H11" s="183"/>
+      <c r="I11" s="183"/>
+      <c r="J11" s="183"/>
+      <c r="K11" s="183"/>
+      <c r="L11" s="183"/>
+      <c r="AV11" s="178"/>
+      <c r="AW11" s="178"/>
+      <c r="BT11" s="178"/>
+      <c r="BW11" s="178"/>
+      <c r="CT11" s="178"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -3579,18 +3604,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4264,13 +4277,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="203" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="196"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -4375,9 +4388,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="194"/>
-      <c r="B5" s="192"/>
-      <c r="C5" s="194"/>
+      <c r="A5" s="192"/>
+      <c r="B5" s="202"/>
+      <c r="C5" s="192"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -4482,11 +4495,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="194"/>
+      <c r="A6" s="192"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="194"/>
+      <c r="C6" s="192"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -4591,11 +4604,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="194"/>
+      <c r="A7" s="192"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="194"/>
+      <c r="C7" s="192"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -4700,11 +4713,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="194"/>
+      <c r="A8" s="192"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="194"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -4809,11 +4822,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="194"/>
+      <c r="A9" s="192"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="194"/>
+      <c r="C9" s="192"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -4918,11 +4931,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="194"/>
+      <c r="A10" s="192"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="194"/>
+      <c r="C10" s="192"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5027,11 +5040,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="194"/>
+      <c r="A11" s="192"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="194"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5136,9 +5149,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="194"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="197"/>
+      <c r="C12" s="193"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -5243,10 +5256,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="206" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="199" t="s">
+      <c r="B13" s="207" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -5355,8 +5368,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="194"/>
-      <c r="B14" s="200"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="198"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -5477,7 +5490,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="194"/>
+      <c r="A15" s="192"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -5587,7 +5600,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="194"/>
+      <c r="A16" s="192"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -5697,7 +5710,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="194"/>
+      <c r="A17" s="192"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -5809,7 +5822,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="194"/>
+      <c r="A18" s="192"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -5919,7 +5932,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="194"/>
+      <c r="A19" s="192"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -6029,7 +6042,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="194"/>
+      <c r="A20" s="192"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -6139,7 +6152,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="197"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -6250,7 +6263,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="191" t="s">
+      <c r="B22" s="201" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -6360,7 +6373,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="192"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -6467,13 +6480,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="202" t="s">
+      <c r="A24" s="194" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="204">
+      <c r="C24" s="196">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -6581,11 +6594,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="203"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="194"/>
+      <c r="C25" s="192"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -6691,11 +6704,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="203"/>
+      <c r="A26" s="195"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="194"/>
+      <c r="C26" s="192"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -6801,11 +6814,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="203"/>
+      <c r="A27" s="195"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="194"/>
+      <c r="C27" s="192"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -6911,11 +6924,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="203"/>
+      <c r="A28" s="195"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="194"/>
+      <c r="C28" s="192"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -7021,11 +7034,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="203"/>
+      <c r="A29" s="195"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="194"/>
+      <c r="C29" s="192"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -7131,11 +7144,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="203"/>
+      <c r="A30" s="195"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="194"/>
+      <c r="C30" s="192"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -7241,11 +7254,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="203"/>
+      <c r="A31" s="195"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="194"/>
+      <c r="C31" s="192"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -7351,11 +7364,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="203"/>
+      <c r="A32" s="195"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="194"/>
+      <c r="C32" s="192"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -7461,11 +7474,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="203"/>
+      <c r="A33" s="195"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="194"/>
+      <c r="C33" s="192"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -7571,11 +7584,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="203"/>
+      <c r="A34" s="195"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="194"/>
+      <c r="C34" s="192"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -7681,11 +7694,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="203"/>
+      <c r="A35" s="195"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="197"/>
+      <c r="C35" s="193"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -7791,11 +7804,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="203"/>
+      <c r="A36" s="195"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="204">
+      <c r="C36" s="196">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -7903,11 +7916,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="203"/>
+      <c r="A37" s="195"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="194"/>
+      <c r="C37" s="192"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -8013,11 +8026,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="203"/>
+      <c r="A38" s="195"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="194"/>
+      <c r="C38" s="192"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -8123,11 +8136,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="203"/>
+      <c r="A39" s="195"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="194"/>
+      <c r="C39" s="192"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -8233,11 +8246,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="203"/>
+      <c r="A40" s="195"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="194"/>
+      <c r="C40" s="192"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -8343,11 +8356,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="203"/>
+      <c r="A41" s="195"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="194"/>
+      <c r="C41" s="192"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -8453,11 +8466,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="203"/>
+      <c r="A42" s="195"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="194"/>
+      <c r="C42" s="192"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -8563,11 +8576,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="203"/>
+      <c r="A43" s="195"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="194"/>
+      <c r="C43" s="192"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -8673,11 +8686,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="203"/>
+      <c r="A44" s="195"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="194"/>
+      <c r="C44" s="192"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -8783,11 +8796,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="203"/>
+      <c r="A45" s="195"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="194"/>
+      <c r="C45" s="192"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -8893,11 +8906,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="203"/>
+      <c r="A46" s="195"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="194"/>
+      <c r="C46" s="192"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -9003,11 +9016,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="203"/>
+      <c r="A47" s="195"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="194"/>
+      <c r="C47" s="192"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -9121,11 +9134,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="203"/>
+      <c r="A48" s="195"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="194"/>
+      <c r="C48" s="192"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -9234,7 +9247,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="205" t="s">
+      <c r="B49" s="197" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -9344,7 +9357,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="200"/>
+      <c r="B50" s="198"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -12775,7 +12788,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="206" t="s">
+      <c r="A81" s="199" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -12887,7 +12900,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="194"/>
+      <c r="A82" s="192"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -12997,7 +13010,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="194"/>
+      <c r="A83" s="192"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -13107,7 +13120,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="194"/>
+      <c r="A84" s="192"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -13217,7 +13230,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="194"/>
+      <c r="A85" s="192"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -13327,7 +13340,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="194"/>
+      <c r="A86" s="192"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -13437,7 +13450,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="194"/>
+      <c r="A87" s="192"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -13549,7 +13562,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="194"/>
+      <c r="A88" s="192"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -13659,7 +13672,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="194"/>
+      <c r="A89" s="192"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -13769,7 +13782,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="194"/>
+      <c r="A90" s="192"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -13879,11 +13892,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="194"/>
+      <c r="A91" s="192"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="207"/>
+      <c r="C91" s="200"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -13989,11 +14002,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="194"/>
+      <c r="A92" s="192"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="194"/>
+      <c r="C92" s="192"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -14099,11 +14112,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="197"/>
+      <c r="A93" s="193"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="194"/>
+      <c r="C93" s="192"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -14327,7 +14340,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="201" t="s">
+      <c r="A95" s="191" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -14439,7 +14452,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="194"/>
+      <c r="A96" s="192"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -14549,7 +14562,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="194"/>
+      <c r="A97" s="192"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -14659,7 +14672,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="194"/>
+      <c r="A98" s="192"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -14769,7 +14782,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="194"/>
+      <c r="A99" s="192"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -14879,7 +14892,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="194"/>
+      <c r="A100" s="192"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -14989,7 +15002,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="194"/>
+      <c r="A101" s="192"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -15099,7 +15112,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="194"/>
+      <c r="A102" s="192"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -15209,7 +15222,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="194"/>
+      <c r="A103" s="192"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -15321,7 +15334,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="194"/>
+      <c r="A104" s="192"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -15431,7 +15444,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="194"/>
+      <c r="A105" s="192"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -15549,7 +15562,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="194"/>
+      <c r="A106" s="192"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -15659,7 +15672,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="194"/>
+      <c r="A107" s="192"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -15769,7 +15782,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="194"/>
+      <c r="A108" s="192"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -15879,7 +15892,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="194"/>
+      <c r="A109" s="192"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -15989,7 +16002,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="194"/>
+      <c r="A110" s="192"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -16099,7 +16112,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="194"/>
+      <c r="A111" s="192"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -16209,7 +16222,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="194"/>
+      <c r="A112" s="192"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -16319,7 +16332,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="194"/>
+      <c r="A113" s="192"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -16429,7 +16442,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="194"/>
+      <c r="A114" s="192"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -16539,7 +16552,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="194"/>
+      <c r="A115" s="192"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -16649,7 +16662,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="194"/>
+      <c r="A116" s="192"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -16775,7 +16788,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="194"/>
+      <c r="A117" s="192"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -16885,7 +16898,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="197"/>
+      <c r="A118" s="193"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -24256,6 +24269,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -24263,12 +24282,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 26-08
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755B0D8C-C7DD-45C5-8658-04D5D439260A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0C482B-EEF5-49D8-8C00-B52D0186B19E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="152">
   <si>
     <t>S</t>
   </si>
@@ -649,6 +649,9 @@
   <si>
     <t>Aula sobre Git e GitHub.
 Introdução ao HTML com uma atividade para entrega</t>
+  </si>
+  <si>
+    <t>Continuação com conteúdos HTML, apresentando tags como section, article, a, table, ul, ol e li</t>
   </si>
 </sst>
 </file>
@@ -2162,26 +2165,8 @@
     <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2201,14 +2186,52 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2219,30 +2242,10 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2655,10 +2658,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -2969,110 +2972,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="184"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="184"/>
-      <c r="O2" s="184"/>
-      <c r="P2" s="184"/>
-      <c r="Q2" s="184"/>
-      <c r="R2" s="184" t="s">
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
+      <c r="Q2" s="178"/>
+      <c r="R2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="184"/>
-      <c r="T2" s="184"/>
-      <c r="U2" s="184"/>
-      <c r="V2" s="184"/>
-      <c r="W2" s="184"/>
-      <c r="X2" s="184"/>
-      <c r="Y2" s="184"/>
-      <c r="Z2" s="184"/>
-      <c r="AA2" s="184"/>
-      <c r="AB2" s="184"/>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="184"/>
-      <c r="AG2" s="184"/>
-      <c r="AH2" s="184"/>
-      <c r="AI2" s="184"/>
-      <c r="AJ2" s="184"/>
-      <c r="AK2" s="184"/>
-      <c r="AL2" s="184"/>
-      <c r="AM2" s="184" t="s">
+      <c r="S2" s="178"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="178"/>
+      <c r="V2" s="178"/>
+      <c r="W2" s="178"/>
+      <c r="X2" s="178"/>
+      <c r="Y2" s="178"/>
+      <c r="Z2" s="178"/>
+      <c r="AA2" s="178"/>
+      <c r="AB2" s="178"/>
+      <c r="AC2" s="178"/>
+      <c r="AD2" s="178"/>
+      <c r="AE2" s="178"/>
+      <c r="AF2" s="178"/>
+      <c r="AG2" s="178"/>
+      <c r="AH2" s="178"/>
+      <c r="AI2" s="178"/>
+      <c r="AJ2" s="178"/>
+      <c r="AK2" s="178"/>
+      <c r="AL2" s="178"/>
+      <c r="AM2" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="184"/>
-      <c r="AO2" s="184"/>
-      <c r="AP2" s="184"/>
-      <c r="AQ2" s="184"/>
-      <c r="AR2" s="184"/>
-      <c r="AS2" s="184"/>
-      <c r="AT2" s="184"/>
-      <c r="AU2" s="184"/>
-      <c r="AV2" s="184"/>
-      <c r="AW2" s="184"/>
-      <c r="AX2" s="185"/>
-      <c r="AY2" s="185"/>
-      <c r="AZ2" s="185"/>
-      <c r="BA2" s="185"/>
-      <c r="BB2" s="185"/>
-      <c r="BC2" s="185"/>
-      <c r="BD2" s="185"/>
-      <c r="BE2" s="185"/>
-      <c r="BF2" s="185"/>
-      <c r="BG2" s="185"/>
-      <c r="BH2" s="185"/>
-      <c r="BI2" s="185"/>
-      <c r="BJ2" s="184" t="s">
+      <c r="AN2" s="178"/>
+      <c r="AO2" s="178"/>
+      <c r="AP2" s="178"/>
+      <c r="AQ2" s="178"/>
+      <c r="AR2" s="178"/>
+      <c r="AS2" s="178"/>
+      <c r="AT2" s="178"/>
+      <c r="AU2" s="178"/>
+      <c r="AV2" s="178"/>
+      <c r="AW2" s="178"/>
+      <c r="AX2" s="179"/>
+      <c r="AY2" s="179"/>
+      <c r="AZ2" s="179"/>
+      <c r="BA2" s="179"/>
+      <c r="BB2" s="179"/>
+      <c r="BC2" s="179"/>
+      <c r="BD2" s="179"/>
+      <c r="BE2" s="179"/>
+      <c r="BF2" s="179"/>
+      <c r="BG2" s="179"/>
+      <c r="BH2" s="179"/>
+      <c r="BI2" s="179"/>
+      <c r="BJ2" s="178" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="184"/>
-      <c r="BL2" s="184"/>
-      <c r="BM2" s="184"/>
-      <c r="BN2" s="184"/>
-      <c r="BO2" s="184"/>
-      <c r="BP2" s="184"/>
-      <c r="BQ2" s="184"/>
-      <c r="BR2" s="184"/>
-      <c r="BS2" s="184"/>
-      <c r="BT2" s="184"/>
-      <c r="BU2" s="184"/>
-      <c r="BV2" s="184"/>
-      <c r="BW2" s="184"/>
-      <c r="BX2" s="186"/>
-      <c r="BY2" s="186"/>
-      <c r="BZ2" s="186"/>
-      <c r="CA2" s="186"/>
-      <c r="CB2" s="186"/>
-      <c r="CC2" s="186"/>
-      <c r="CD2" s="186"/>
-      <c r="CE2" s="187" t="s">
+      <c r="BK2" s="178"/>
+      <c r="BL2" s="178"/>
+      <c r="BM2" s="178"/>
+      <c r="BN2" s="178"/>
+      <c r="BO2" s="178"/>
+      <c r="BP2" s="178"/>
+      <c r="BQ2" s="178"/>
+      <c r="BR2" s="178"/>
+      <c r="BS2" s="178"/>
+      <c r="BT2" s="178"/>
+      <c r="BU2" s="178"/>
+      <c r="BV2" s="178"/>
+      <c r="BW2" s="178"/>
+      <c r="BX2" s="180"/>
+      <c r="BY2" s="180"/>
+      <c r="BZ2" s="180"/>
+      <c r="CA2" s="180"/>
+      <c r="CB2" s="180"/>
+      <c r="CC2" s="180"/>
+      <c r="CD2" s="180"/>
+      <c r="CE2" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="188"/>
-      <c r="CG2" s="188"/>
-      <c r="CH2" s="188"/>
-      <c r="CI2" s="188"/>
-      <c r="CJ2" s="188"/>
-      <c r="CK2" s="188"/>
-      <c r="CL2" s="188"/>
-      <c r="CM2" s="188"/>
-      <c r="CN2" s="188"/>
-      <c r="CO2" s="188"/>
-      <c r="CP2" s="188"/>
-      <c r="CQ2" s="188"/>
-      <c r="CR2" s="188"/>
-      <c r="CS2" s="188"/>
+      <c r="CF2" s="182"/>
+      <c r="CG2" s="182"/>
+      <c r="CH2" s="182"/>
+      <c r="CI2" s="182"/>
+      <c r="CJ2" s="182"/>
+      <c r="CK2" s="182"/>
+      <c r="CL2" s="182"/>
+      <c r="CM2" s="182"/>
+      <c r="CN2" s="182"/>
+      <c r="CO2" s="182"/>
+      <c r="CP2" s="182"/>
+      <c r="CQ2" s="182"/>
+      <c r="CR2" s="182"/>
+      <c r="CS2" s="182"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3368,226 +3371,220 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="177" t="s">
+      <c r="A4" s="187" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
+      <c r="C4" s="188"/>
+      <c r="D4" s="189" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="189" t="s">
+      <c r="E4" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="189" t="s">
+      <c r="F4" s="183" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="189" t="s">
+      <c r="G4" s="183" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="182" t="s">
+      <c r="H4" s="186" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="182" t="s">
+      <c r="I4" s="186" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="182" t="s">
+      <c r="J4" s="186" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="182" t="s">
+      <c r="K4" s="186" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="189" t="s">
+      <c r="L4" s="183" t="s">
         <v>150</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="186" t="s">
+        <v>151</v>
+      </c>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="178"/>
-      <c r="AW4" s="178"/>
-      <c r="BT4" s="178"/>
-      <c r="BW4" s="178"/>
-      <c r="CT4" s="178"/>
+      <c r="AV4" s="177"/>
+      <c r="AW4" s="177"/>
+      <c r="BT4" s="177"/>
+      <c r="BW4" s="177"/>
+      <c r="CT4" s="177"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="177"/>
-      <c r="B5" s="179" t="s">
+      <c r="A5" s="187"/>
+      <c r="B5" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="179"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="183"/>
-      <c r="F5" s="183"/>
-      <c r="G5" s="190"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183"/>
-      <c r="K5" s="183"/>
-      <c r="L5" s="183"/>
-      <c r="M5" s="7"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="185"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="184"/>
+      <c r="L5" s="184"/>
+      <c r="M5" s="184"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="178"/>
-      <c r="AW5" s="178"/>
-      <c r="BT5" s="178"/>
-      <c r="BW5" s="178"/>
-      <c r="CT5" s="178"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="BT5" s="177"/>
+      <c r="BW5" s="177"/>
+      <c r="CT5" s="177"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="177"/>
-      <c r="B6" s="179" t="s">
+      <c r="A6" s="187"/>
+      <c r="B6" s="188" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="183"/>
-      <c r="F6" s="183"/>
-      <c r="G6" s="190"/>
-      <c r="H6" s="183"/>
-      <c r="I6" s="183"/>
-      <c r="J6" s="183"/>
-      <c r="K6" s="183"/>
-      <c r="L6" s="183"/>
-      <c r="M6" s="7"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="184"/>
+      <c r="L6" s="184"/>
+      <c r="M6" s="184"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="178"/>
-      <c r="AW6" s="178"/>
-      <c r="BT6" s="178"/>
-      <c r="BW6" s="178"/>
-      <c r="CT6" s="178"/>
+      <c r="AV6" s="177"/>
+      <c r="AW6" s="177"/>
+      <c r="BT6" s="177"/>
+      <c r="BW6" s="177"/>
+      <c r="CT6" s="177"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="177"/>
-      <c r="B7" s="179" t="s">
+      <c r="A7" s="187"/>
+      <c r="B7" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="179"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="190"/>
-      <c r="H7" s="183"/>
-      <c r="I7" s="183"/>
-      <c r="J7" s="183"/>
-      <c r="K7" s="183"/>
-      <c r="L7" s="183"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="190"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="184"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="184"/>
+      <c r="L7" s="184"/>
+      <c r="M7" s="184"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="178"/>
-      <c r="AW7" s="178"/>
-      <c r="BT7" s="178"/>
-      <c r="BW7" s="178"/>
-      <c r="CT7" s="178"/>
+      <c r="AV7" s="177"/>
+      <c r="AW7" s="177"/>
+      <c r="BT7" s="177"/>
+      <c r="BW7" s="177"/>
+      <c r="CT7" s="177"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="177" t="s">
+      <c r="A8" s="187" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="179" t="s">
+      <c r="B8" s="188" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="179"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="183"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="190"/>
-      <c r="H8" s="183"/>
-      <c r="I8" s="183"/>
-      <c r="J8" s="183"/>
-      <c r="K8" s="183"/>
-      <c r="L8" s="183"/>
-      <c r="AV8" s="178"/>
-      <c r="AW8" s="178"/>
-      <c r="BT8" s="178"/>
-      <c r="BW8" s="178"/>
-      <c r="CT8" s="178"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="190"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="184"/>
+      <c r="L8" s="184"/>
+      <c r="M8" s="184"/>
+      <c r="AV8" s="177"/>
+      <c r="AW8" s="177"/>
+      <c r="BT8" s="177"/>
+      <c r="BW8" s="177"/>
+      <c r="CT8" s="177"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="177"/>
-      <c r="B9" s="179" t="s">
+      <c r="A9" s="187"/>
+      <c r="B9" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="179"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="183"/>
-      <c r="F9" s="183"/>
-      <c r="G9" s="190"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="183"/>
-      <c r="J9" s="183"/>
-      <c r="K9" s="183"/>
-      <c r="L9" s="183"/>
-      <c r="AV9" s="178"/>
-      <c r="AW9" s="178"/>
-      <c r="BT9" s="178"/>
-      <c r="BW9" s="178"/>
-      <c r="CT9" s="178"/>
+      <c r="C9" s="188"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="185"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="184"/>
+      <c r="L9" s="184"/>
+      <c r="M9" s="184"/>
+      <c r="AV9" s="177"/>
+      <c r="AW9" s="177"/>
+      <c r="BT9" s="177"/>
+      <c r="BW9" s="177"/>
+      <c r="CT9" s="177"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="177"/>
-      <c r="B10" s="179" t="s">
+      <c r="A10" s="187"/>
+      <c r="B10" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="179"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="190"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="183"/>
-      <c r="K10" s="183"/>
-      <c r="L10" s="183"/>
-      <c r="AV10" s="178"/>
-      <c r="AW10" s="178"/>
-      <c r="BT10" s="178"/>
-      <c r="BW10" s="178"/>
-      <c r="CT10" s="178"/>
+      <c r="C10" s="188"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="184"/>
+      <c r="L10" s="184"/>
+      <c r="M10" s="184"/>
+      <c r="AV10" s="177"/>
+      <c r="AW10" s="177"/>
+      <c r="BT10" s="177"/>
+      <c r="BW10" s="177"/>
+      <c r="CT10" s="177"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="177"/>
-      <c r="B11" s="179" t="s">
+      <c r="A11" s="187"/>
+      <c r="B11" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="179"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="183"/>
-      <c r="F11" s="183"/>
-      <c r="G11" s="190"/>
-      <c r="H11" s="183"/>
-      <c r="I11" s="183"/>
-      <c r="J11" s="183"/>
-      <c r="K11" s="183"/>
-      <c r="L11" s="183"/>
-      <c r="AV11" s="178"/>
-      <c r="AW11" s="178"/>
-      <c r="BT11" s="178"/>
-      <c r="BW11" s="178"/>
-      <c r="CT11" s="178"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="190"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="184"/>
+      <c r="L11" s="184"/>
+      <c r="M11" s="184"/>
+      <c r="AV11" s="177"/>
+      <c r="AW11" s="177"/>
+      <c r="BT11" s="177"/>
+      <c r="BW11" s="177"/>
+      <c r="CT11" s="177"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
+  <mergeCells count="30">
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -3604,6 +3601,20 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4277,13 +4288,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="193" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="196"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -4388,9 +4399,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="192"/>
-      <c r="B5" s="202"/>
-      <c r="C5" s="192"/>
+      <c r="A5" s="194"/>
+      <c r="B5" s="192"/>
+      <c r="C5" s="194"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -4495,11 +4506,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="192"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="192"/>
+      <c r="C6" s="194"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -4604,11 +4615,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="192"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="192"/>
+      <c r="C7" s="194"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -4713,11 +4724,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="192"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="192"/>
+      <c r="C8" s="194"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -4822,11 +4833,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="192"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="192"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -4931,11 +4942,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="192"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="192"/>
+      <c r="C10" s="194"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5040,11 +5051,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="192"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="192"/>
+      <c r="C11" s="194"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5149,9 +5160,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="192"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="193"/>
+      <c r="C12" s="197"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -5256,10 +5267,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="198" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="207" t="s">
+      <c r="B13" s="199" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -5368,8 +5379,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="192"/>
-      <c r="B14" s="198"/>
+      <c r="A14" s="194"/>
+      <c r="B14" s="200"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -5490,7 +5501,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="192"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -5600,7 +5611,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="192"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -5710,7 +5721,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="192"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -5822,7 +5833,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="192"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -5932,7 +5943,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="192"/>
+      <c r="A19" s="194"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -6042,7 +6053,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="192"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -6152,7 +6163,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="193"/>
+      <c r="A21" s="197"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -6263,7 +6274,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="201" t="s">
+      <c r="B22" s="191" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -6373,7 +6384,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="202"/>
+      <c r="B23" s="192"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -6480,13 +6491,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="194" t="s">
+      <c r="A24" s="202" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="196">
+      <c r="C24" s="204">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -6594,11 +6605,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="195"/>
+      <c r="A25" s="203"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="192"/>
+      <c r="C25" s="194"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -6704,11 +6715,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="195"/>
+      <c r="A26" s="203"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="192"/>
+      <c r="C26" s="194"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -6814,11 +6825,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="195"/>
+      <c r="A27" s="203"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="192"/>
+      <c r="C27" s="194"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -6924,11 +6935,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="195"/>
+      <c r="A28" s="203"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="192"/>
+      <c r="C28" s="194"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -7034,11 +7045,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="195"/>
+      <c r="A29" s="203"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="192"/>
+      <c r="C29" s="194"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -7144,11 +7155,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="195"/>
+      <c r="A30" s="203"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="192"/>
+      <c r="C30" s="194"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -7254,11 +7265,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="195"/>
+      <c r="A31" s="203"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="192"/>
+      <c r="C31" s="194"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -7364,11 +7375,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="195"/>
+      <c r="A32" s="203"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="192"/>
+      <c r="C32" s="194"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -7474,11 +7485,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="195"/>
+      <c r="A33" s="203"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="192"/>
+      <c r="C33" s="194"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -7584,11 +7595,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="195"/>
+      <c r="A34" s="203"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="192"/>
+      <c r="C34" s="194"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -7694,11 +7705,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="195"/>
+      <c r="A35" s="203"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="193"/>
+      <c r="C35" s="197"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -7804,11 +7815,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="195"/>
+      <c r="A36" s="203"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="196">
+      <c r="C36" s="204">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -7916,11 +7927,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="195"/>
+      <c r="A37" s="203"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="192"/>
+      <c r="C37" s="194"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -8026,11 +8037,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="195"/>
+      <c r="A38" s="203"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="192"/>
+      <c r="C38" s="194"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -8136,11 +8147,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="195"/>
+      <c r="A39" s="203"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="192"/>
+      <c r="C39" s="194"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -8246,11 +8257,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="195"/>
+      <c r="A40" s="203"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="192"/>
+      <c r="C40" s="194"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -8356,11 +8367,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="195"/>
+      <c r="A41" s="203"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="192"/>
+      <c r="C41" s="194"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -8466,11 +8477,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="195"/>
+      <c r="A42" s="203"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="192"/>
+      <c r="C42" s="194"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -8576,11 +8587,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="195"/>
+      <c r="A43" s="203"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="192"/>
+      <c r="C43" s="194"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -8686,11 +8697,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="195"/>
+      <c r="A44" s="203"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="192"/>
+      <c r="C44" s="194"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -8796,11 +8807,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="195"/>
+      <c r="A45" s="203"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="192"/>
+      <c r="C45" s="194"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -8906,11 +8917,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="195"/>
+      <c r="A46" s="203"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="192"/>
+      <c r="C46" s="194"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -9016,11 +9027,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="195"/>
+      <c r="A47" s="203"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="192"/>
+      <c r="C47" s="194"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -9134,11 +9145,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="195"/>
+      <c r="A48" s="203"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="192"/>
+      <c r="C48" s="194"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -9247,7 +9258,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="197" t="s">
+      <c r="B49" s="205" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -9357,7 +9368,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="198"/>
+      <c r="B50" s="200"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -12788,7 +12799,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="199" t="s">
+      <c r="A81" s="206" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -12900,7 +12911,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="192"/>
+      <c r="A82" s="194"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -13010,7 +13021,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="192"/>
+      <c r="A83" s="194"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -13120,7 +13131,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="192"/>
+      <c r="A84" s="194"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -13230,7 +13241,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="192"/>
+      <c r="A85" s="194"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -13340,7 +13351,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="192"/>
+      <c r="A86" s="194"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -13450,7 +13461,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="192"/>
+      <c r="A87" s="194"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -13562,7 +13573,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="192"/>
+      <c r="A88" s="194"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -13672,7 +13683,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="192"/>
+      <c r="A89" s="194"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -13782,7 +13793,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="192"/>
+      <c r="A90" s="194"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -13892,11 +13903,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="192"/>
+      <c r="A91" s="194"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="200"/>
+      <c r="C91" s="207"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -14002,11 +14013,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="192"/>
+      <c r="A92" s="194"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="192"/>
+      <c r="C92" s="194"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -14112,11 +14123,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="193"/>
+      <c r="A93" s="197"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="192"/>
+      <c r="C93" s="194"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -14340,7 +14351,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="191" t="s">
+      <c r="A95" s="201" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -14452,7 +14463,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="192"/>
+      <c r="A96" s="194"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -14562,7 +14573,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="192"/>
+      <c r="A97" s="194"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -14672,7 +14683,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="192"/>
+      <c r="A98" s="194"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -14782,7 +14793,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="192"/>
+      <c r="A99" s="194"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -14892,7 +14903,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="192"/>
+      <c r="A100" s="194"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -15002,7 +15013,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="192"/>
+      <c r="A101" s="194"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -15112,7 +15123,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="192"/>
+      <c r="A102" s="194"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -15222,7 +15233,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="192"/>
+      <c r="A103" s="194"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -15334,7 +15345,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="192"/>
+      <c r="A104" s="194"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -15444,7 +15455,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="192"/>
+      <c r="A105" s="194"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -15562,7 +15573,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="192"/>
+      <c r="A106" s="194"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -15672,7 +15683,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="192"/>
+      <c r="A107" s="194"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -15782,7 +15793,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="192"/>
+      <c r="A108" s="194"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -15892,7 +15903,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="192"/>
+      <c r="A109" s="194"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -16002,7 +16013,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="192"/>
+      <c r="A110" s="194"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -16112,7 +16123,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="192"/>
+      <c r="A111" s="194"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -16222,7 +16233,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="192"/>
+      <c r="A112" s="194"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -16332,7 +16343,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="192"/>
+      <c r="A113" s="194"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -16442,7 +16453,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="192"/>
+      <c r="A114" s="194"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -16552,7 +16563,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="192"/>
+      <c r="A115" s="194"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -16662,7 +16673,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="192"/>
+      <c r="A116" s="194"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -16788,7 +16799,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="192"/>
+      <c r="A117" s="194"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -16898,7 +16909,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="193"/>
+      <c r="A118" s="197"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -24269,12 +24280,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -24282,6 +24287,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 27-08
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0C482B-EEF5-49D8-8C00-B52D0186B19E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A2717D-C318-4B97-8B5D-5FBDB4ED2DEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="154">
   <si>
     <t>S</t>
   </si>
@@ -647,11 +647,18 @@
 Encerramento da Sprint 2</t>
   </si>
   <si>
-    <t>Aula sobre Git e GitHub.
-Introdução ao HTML com uma atividade para entrega</t>
+    <t>Continuação com conteúdos HTML, apresentando tags como section, article, a, table, ul, ol e li</t>
   </si>
   <si>
-    <t>Continuação com conteúdos HTML, apresentando tags como section, article, a, table, ul, ol e li</t>
+    <t>Atividades para entrega aplicando os conceitos de HTML e CSS, reproduzindo o layout fornecido em um site</t>
+  </si>
+  <si>
+    <t>Aula sobre Git e GitHub.
+Introdução ao HTML e CSS com uma atividade para entrega</t>
+  </si>
+  <si>
+    <t>Revisão de propriedades CSS e exercícios de fixação Flexbox utilizando os sites Flexbox Froggy e Flexbox Defense.
+Reprodução do site de download do Spotify</t>
   </si>
 </sst>
 </file>
@@ -2165,8 +2172,26 @@
     <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2186,52 +2211,14 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2242,10 +2229,30 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2658,10 +2665,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4:M11"/>
+      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -2670,9 +2677,9 @@
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="12" width="30.77734375" style="1" customWidth="1"/>
-    <col min="13" max="14" width="20.77734375" style="1" customWidth="1"/>
-    <col min="15" max="17" width="15.77734375" style="1" customWidth="1"/>
-    <col min="18" max="32" width="15.77734375" customWidth="1"/>
+    <col min="13" max="17" width="20.77734375" style="1" customWidth="1"/>
+    <col min="18" max="20" width="20.77734375" customWidth="1"/>
+    <col min="21" max="32" width="15.77734375" customWidth="1"/>
     <col min="33" max="47" width="5.6640625" customWidth="1"/>
     <col min="48" max="48" width="3.6640625" style="2" customWidth="1"/>
     <col min="49" max="49" width="3.6640625" style="3" customWidth="1"/>
@@ -2972,110 +2979,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="178"/>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178"/>
-      <c r="N2" s="178"/>
-      <c r="O2" s="178"/>
-      <c r="P2" s="178"/>
-      <c r="Q2" s="178"/>
-      <c r="R2" s="178" t="s">
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
+      <c r="L2" s="184"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="184"/>
+      <c r="O2" s="184"/>
+      <c r="P2" s="184"/>
+      <c r="Q2" s="184"/>
+      <c r="R2" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="178"/>
-      <c r="T2" s="178"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="178"/>
-      <c r="W2" s="178"/>
-      <c r="X2" s="178"/>
-      <c r="Y2" s="178"/>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="178"/>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="178"/>
-      <c r="AG2" s="178"/>
-      <c r="AH2" s="178"/>
-      <c r="AI2" s="178"/>
-      <c r="AJ2" s="178"/>
-      <c r="AK2" s="178"/>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="178" t="s">
+      <c r="S2" s="184"/>
+      <c r="T2" s="184"/>
+      <c r="U2" s="184"/>
+      <c r="V2" s="184"/>
+      <c r="W2" s="184"/>
+      <c r="X2" s="184"/>
+      <c r="Y2" s="184"/>
+      <c r="Z2" s="184"/>
+      <c r="AA2" s="184"/>
+      <c r="AB2" s="184"/>
+      <c r="AC2" s="184"/>
+      <c r="AD2" s="184"/>
+      <c r="AE2" s="184"/>
+      <c r="AF2" s="184"/>
+      <c r="AG2" s="184"/>
+      <c r="AH2" s="184"/>
+      <c r="AI2" s="184"/>
+      <c r="AJ2" s="184"/>
+      <c r="AK2" s="184"/>
+      <c r="AL2" s="184"/>
+      <c r="AM2" s="184" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="178"/>
-      <c r="AP2" s="178"/>
-      <c r="AQ2" s="178"/>
-      <c r="AR2" s="178"/>
-      <c r="AS2" s="178"/>
-      <c r="AT2" s="178"/>
-      <c r="AU2" s="178"/>
-      <c r="AV2" s="178"/>
-      <c r="AW2" s="178"/>
-      <c r="AX2" s="179"/>
-      <c r="AY2" s="179"/>
-      <c r="AZ2" s="179"/>
-      <c r="BA2" s="179"/>
-      <c r="BB2" s="179"/>
-      <c r="BC2" s="179"/>
-      <c r="BD2" s="179"/>
-      <c r="BE2" s="179"/>
-      <c r="BF2" s="179"/>
-      <c r="BG2" s="179"/>
-      <c r="BH2" s="179"/>
-      <c r="BI2" s="179"/>
-      <c r="BJ2" s="178" t="s">
+      <c r="AN2" s="184"/>
+      <c r="AO2" s="184"/>
+      <c r="AP2" s="184"/>
+      <c r="AQ2" s="184"/>
+      <c r="AR2" s="184"/>
+      <c r="AS2" s="184"/>
+      <c r="AT2" s="184"/>
+      <c r="AU2" s="184"/>
+      <c r="AV2" s="184"/>
+      <c r="AW2" s="184"/>
+      <c r="AX2" s="185"/>
+      <c r="AY2" s="185"/>
+      <c r="AZ2" s="185"/>
+      <c r="BA2" s="185"/>
+      <c r="BB2" s="185"/>
+      <c r="BC2" s="185"/>
+      <c r="BD2" s="185"/>
+      <c r="BE2" s="185"/>
+      <c r="BF2" s="185"/>
+      <c r="BG2" s="185"/>
+      <c r="BH2" s="185"/>
+      <c r="BI2" s="185"/>
+      <c r="BJ2" s="184" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="178"/>
-      <c r="BL2" s="178"/>
-      <c r="BM2" s="178"/>
-      <c r="BN2" s="178"/>
-      <c r="BO2" s="178"/>
-      <c r="BP2" s="178"/>
-      <c r="BQ2" s="178"/>
-      <c r="BR2" s="178"/>
-      <c r="BS2" s="178"/>
-      <c r="BT2" s="178"/>
-      <c r="BU2" s="178"/>
-      <c r="BV2" s="178"/>
-      <c r="BW2" s="178"/>
-      <c r="BX2" s="180"/>
-      <c r="BY2" s="180"/>
-      <c r="BZ2" s="180"/>
-      <c r="CA2" s="180"/>
-      <c r="CB2" s="180"/>
-      <c r="CC2" s="180"/>
-      <c r="CD2" s="180"/>
-      <c r="CE2" s="181" t="s">
+      <c r="BK2" s="184"/>
+      <c r="BL2" s="184"/>
+      <c r="BM2" s="184"/>
+      <c r="BN2" s="184"/>
+      <c r="BO2" s="184"/>
+      <c r="BP2" s="184"/>
+      <c r="BQ2" s="184"/>
+      <c r="BR2" s="184"/>
+      <c r="BS2" s="184"/>
+      <c r="BT2" s="184"/>
+      <c r="BU2" s="184"/>
+      <c r="BV2" s="184"/>
+      <c r="BW2" s="184"/>
+      <c r="BX2" s="186"/>
+      <c r="BY2" s="186"/>
+      <c r="BZ2" s="186"/>
+      <c r="CA2" s="186"/>
+      <c r="CB2" s="186"/>
+      <c r="CC2" s="186"/>
+      <c r="CD2" s="186"/>
+      <c r="CE2" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="182"/>
-      <c r="CG2" s="182"/>
-      <c r="CH2" s="182"/>
-      <c r="CI2" s="182"/>
-      <c r="CJ2" s="182"/>
-      <c r="CK2" s="182"/>
-      <c r="CL2" s="182"/>
-      <c r="CM2" s="182"/>
-      <c r="CN2" s="182"/>
-      <c r="CO2" s="182"/>
-      <c r="CP2" s="182"/>
-      <c r="CQ2" s="182"/>
-      <c r="CR2" s="182"/>
-      <c r="CS2" s="182"/>
+      <c r="CF2" s="188"/>
+      <c r="CG2" s="188"/>
+      <c r="CH2" s="188"/>
+      <c r="CI2" s="188"/>
+      <c r="CJ2" s="188"/>
+      <c r="CK2" s="188"/>
+      <c r="CL2" s="188"/>
+      <c r="CM2" s="188"/>
+      <c r="CN2" s="188"/>
+      <c r="CO2" s="188"/>
+      <c r="CP2" s="188"/>
+      <c r="CQ2" s="188"/>
+      <c r="CR2" s="188"/>
+      <c r="CS2" s="188"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3371,220 +3378,250 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="177" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="188" t="s">
+      <c r="B4" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="189" t="s">
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="183" t="s">
+      <c r="E4" s="189" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="183" t="s">
+      <c r="F4" s="189" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="183" t="s">
+      <c r="G4" s="189" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="186" t="s">
+      <c r="H4" s="182" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="186" t="s">
+      <c r="I4" s="182" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="186" t="s">
+      <c r="J4" s="182" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="186" t="s">
+      <c r="K4" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="183" t="s">
+      <c r="L4" s="189" t="s">
+        <v>152</v>
+      </c>
+      <c r="M4" s="182" t="s">
         <v>150</v>
       </c>
-      <c r="M4" s="186" t="s">
+      <c r="N4" s="182" t="s">
         <v>151</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
+      <c r="O4" s="182" t="s">
+        <v>153</v>
+      </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="177"/>
-      <c r="AW4" s="177"/>
-      <c r="BT4" s="177"/>
-      <c r="BW4" s="177"/>
-      <c r="CT4" s="177"/>
+      <c r="AV4" s="178"/>
+      <c r="AW4" s="178"/>
+      <c r="BT4" s="178"/>
+      <c r="BW4" s="178"/>
+      <c r="CT4" s="178"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="187"/>
-      <c r="B5" s="188" t="s">
+      <c r="A5" s="177"/>
+      <c r="B5" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="188"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="185"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
+      <c r="K5" s="183"/>
+      <c r="L5" s="183"/>
+      <c r="M5" s="183"/>
+      <c r="N5" s="183"/>
+      <c r="O5" s="183"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="177"/>
-      <c r="AW5" s="177"/>
-      <c r="BT5" s="177"/>
-      <c r="BW5" s="177"/>
-      <c r="CT5" s="177"/>
+      <c r="AV5" s="178"/>
+      <c r="AW5" s="178"/>
+      <c r="BT5" s="178"/>
+      <c r="BW5" s="178"/>
+      <c r="CT5" s="178"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="187"/>
-      <c r="B6" s="188" t="s">
+      <c r="A6" s="177"/>
+      <c r="B6" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="188"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184"/>
-      <c r="J6" s="184"/>
-      <c r="K6" s="184"/>
-      <c r="L6" s="184"/>
-      <c r="M6" s="184"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="190"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="183"/>
+      <c r="J6" s="183"/>
+      <c r="K6" s="183"/>
+      <c r="L6" s="183"/>
+      <c r="M6" s="183"/>
+      <c r="N6" s="183"/>
+      <c r="O6" s="183"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="177"/>
-      <c r="AW6" s="177"/>
-      <c r="BT6" s="177"/>
-      <c r="BW6" s="177"/>
-      <c r="CT6" s="177"/>
+      <c r="AV6" s="178"/>
+      <c r="AW6" s="178"/>
+      <c r="BT6" s="178"/>
+      <c r="BW6" s="178"/>
+      <c r="CT6" s="178"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="187"/>
-      <c r="B7" s="188" t="s">
+      <c r="A7" s="177"/>
+      <c r="B7" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="188"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="185"/>
-      <c r="H7" s="184"/>
-      <c r="I7" s="184"/>
-      <c r="J7" s="184"/>
-      <c r="K7" s="184"/>
-      <c r="L7" s="184"/>
-      <c r="M7" s="184"/>
+      <c r="C7" s="179"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="190"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="183"/>
+      <c r="L7" s="183"/>
+      <c r="M7" s="183"/>
+      <c r="N7" s="183"/>
+      <c r="O7" s="183"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="177"/>
-      <c r="AW7" s="177"/>
-      <c r="BT7" s="177"/>
-      <c r="BW7" s="177"/>
-      <c r="CT7" s="177"/>
+      <c r="AV7" s="178"/>
+      <c r="AW7" s="178"/>
+      <c r="BT7" s="178"/>
+      <c r="BW7" s="178"/>
+      <c r="CT7" s="178"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="187" t="s">
+      <c r="A8" s="177" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="188" t="s">
+      <c r="B8" s="179" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="188"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="184"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="185"/>
-      <c r="H8" s="184"/>
-      <c r="I8" s="184"/>
-      <c r="J8" s="184"/>
-      <c r="K8" s="184"/>
-      <c r="L8" s="184"/>
-      <c r="M8" s="184"/>
-      <c r="AV8" s="177"/>
-      <c r="AW8" s="177"/>
-      <c r="BT8" s="177"/>
-      <c r="BW8" s="177"/>
-      <c r="CT8" s="177"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="183"/>
+      <c r="G8" s="190"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="183"/>
+      <c r="K8" s="183"/>
+      <c r="L8" s="183"/>
+      <c r="M8" s="183"/>
+      <c r="N8" s="183"/>
+      <c r="O8" s="183"/>
+      <c r="AV8" s="178"/>
+      <c r="AW8" s="178"/>
+      <c r="BT8" s="178"/>
+      <c r="BW8" s="178"/>
+      <c r="CT8" s="178"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="187"/>
-      <c r="B9" s="188" t="s">
+      <c r="A9" s="177"/>
+      <c r="B9" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="188"/>
-      <c r="D9" s="190"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="185"/>
-      <c r="H9" s="184"/>
-      <c r="I9" s="184"/>
-      <c r="J9" s="184"/>
-      <c r="K9" s="184"/>
-      <c r="L9" s="184"/>
-      <c r="M9" s="184"/>
-      <c r="AV9" s="177"/>
-      <c r="AW9" s="177"/>
-      <c r="BT9" s="177"/>
-      <c r="BW9" s="177"/>
-      <c r="CT9" s="177"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="183"/>
+      <c r="F9" s="183"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="183"/>
+      <c r="I9" s="183"/>
+      <c r="J9" s="183"/>
+      <c r="K9" s="183"/>
+      <c r="L9" s="183"/>
+      <c r="M9" s="183"/>
+      <c r="N9" s="183"/>
+      <c r="O9" s="183"/>
+      <c r="AV9" s="178"/>
+      <c r="AW9" s="178"/>
+      <c r="BT9" s="178"/>
+      <c r="BW9" s="178"/>
+      <c r="CT9" s="178"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="187"/>
-      <c r="B10" s="188" t="s">
+      <c r="A10" s="177"/>
+      <c r="B10" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="188"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="185"/>
-      <c r="H10" s="184"/>
-      <c r="I10" s="184"/>
-      <c r="J10" s="184"/>
-      <c r="K10" s="184"/>
-      <c r="L10" s="184"/>
-      <c r="M10" s="184"/>
-      <c r="AV10" s="177"/>
-      <c r="AW10" s="177"/>
-      <c r="BT10" s="177"/>
-      <c r="BW10" s="177"/>
-      <c r="CT10" s="177"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="190"/>
+      <c r="H10" s="183"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="183"/>
+      <c r="K10" s="183"/>
+      <c r="L10" s="183"/>
+      <c r="M10" s="183"/>
+      <c r="N10" s="183"/>
+      <c r="O10" s="183"/>
+      <c r="AV10" s="178"/>
+      <c r="AW10" s="178"/>
+      <c r="BT10" s="178"/>
+      <c r="BW10" s="178"/>
+      <c r="CT10" s="178"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="187"/>
-      <c r="B11" s="188" t="s">
+      <c r="A11" s="177"/>
+      <c r="B11" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="184"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="185"/>
-      <c r="H11" s="184"/>
-      <c r="I11" s="184"/>
-      <c r="J11" s="184"/>
-      <c r="K11" s="184"/>
-      <c r="L11" s="184"/>
-      <c r="M11" s="184"/>
-      <c r="AV11" s="177"/>
-      <c r="AW11" s="177"/>
-      <c r="BT11" s="177"/>
-      <c r="BW11" s="177"/>
-      <c r="CT11" s="177"/>
+      <c r="C11" s="179"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="190"/>
+      <c r="H11" s="183"/>
+      <c r="I11" s="183"/>
+      <c r="J11" s="183"/>
+      <c r="K11" s="183"/>
+      <c r="L11" s="183"/>
+      <c r="M11" s="183"/>
+      <c r="N11" s="183"/>
+      <c r="O11" s="183"/>
+      <c r="AV11" s="178"/>
+      <c r="AW11" s="178"/>
+      <c r="BT11" s="178"/>
+      <c r="BW11" s="178"/>
+      <c r="CT11" s="178"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -3601,20 +3638,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4288,13 +4311,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="203" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="196"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -4399,9 +4422,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="194"/>
-      <c r="B5" s="192"/>
-      <c r="C5" s="194"/>
+      <c r="A5" s="192"/>
+      <c r="B5" s="202"/>
+      <c r="C5" s="192"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -4506,11 +4529,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="194"/>
+      <c r="A6" s="192"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="194"/>
+      <c r="C6" s="192"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -4615,11 +4638,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="194"/>
+      <c r="A7" s="192"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="194"/>
+      <c r="C7" s="192"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -4724,11 +4747,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="194"/>
+      <c r="A8" s="192"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="194"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -4833,11 +4856,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="194"/>
+      <c r="A9" s="192"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="194"/>
+      <c r="C9" s="192"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -4942,11 +4965,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="194"/>
+      <c r="A10" s="192"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="194"/>
+      <c r="C10" s="192"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5051,11 +5074,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="194"/>
+      <c r="A11" s="192"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="194"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5160,9 +5183,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="194"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="197"/>
+      <c r="C12" s="193"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -5267,10 +5290,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="206" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="199" t="s">
+      <c r="B13" s="207" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -5379,8 +5402,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="194"/>
-      <c r="B14" s="200"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="198"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -5501,7 +5524,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="194"/>
+      <c r="A15" s="192"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -5611,7 +5634,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="194"/>
+      <c r="A16" s="192"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -5721,7 +5744,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="194"/>
+      <c r="A17" s="192"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -5833,7 +5856,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="194"/>
+      <c r="A18" s="192"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -5943,7 +5966,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="194"/>
+      <c r="A19" s="192"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -6053,7 +6076,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="194"/>
+      <c r="A20" s="192"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -6163,7 +6186,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="197"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -6274,7 +6297,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="191" t="s">
+      <c r="B22" s="201" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -6384,7 +6407,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="192"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -6491,13 +6514,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="202" t="s">
+      <c r="A24" s="194" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="204">
+      <c r="C24" s="196">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -6605,11 +6628,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="203"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="194"/>
+      <c r="C25" s="192"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -6715,11 +6738,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="203"/>
+      <c r="A26" s="195"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="194"/>
+      <c r="C26" s="192"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -6825,11 +6848,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="203"/>
+      <c r="A27" s="195"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="194"/>
+      <c r="C27" s="192"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -6935,11 +6958,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="203"/>
+      <c r="A28" s="195"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="194"/>
+      <c r="C28" s="192"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -7045,11 +7068,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="203"/>
+      <c r="A29" s="195"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="194"/>
+      <c r="C29" s="192"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -7155,11 +7178,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="203"/>
+      <c r="A30" s="195"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="194"/>
+      <c r="C30" s="192"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -7265,11 +7288,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="203"/>
+      <c r="A31" s="195"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="194"/>
+      <c r="C31" s="192"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -7375,11 +7398,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="203"/>
+      <c r="A32" s="195"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="194"/>
+      <c r="C32" s="192"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -7485,11 +7508,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="203"/>
+      <c r="A33" s="195"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="194"/>
+      <c r="C33" s="192"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -7595,11 +7618,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="203"/>
+      <c r="A34" s="195"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="194"/>
+      <c r="C34" s="192"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -7705,11 +7728,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="203"/>
+      <c r="A35" s="195"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="197"/>
+      <c r="C35" s="193"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -7815,11 +7838,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="203"/>
+      <c r="A36" s="195"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="204">
+      <c r="C36" s="196">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -7927,11 +7950,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="203"/>
+      <c r="A37" s="195"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="194"/>
+      <c r="C37" s="192"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -8037,11 +8060,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="203"/>
+      <c r="A38" s="195"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="194"/>
+      <c r="C38" s="192"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -8147,11 +8170,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="203"/>
+      <c r="A39" s="195"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="194"/>
+      <c r="C39" s="192"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -8257,11 +8280,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="203"/>
+      <c r="A40" s="195"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="194"/>
+      <c r="C40" s="192"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -8367,11 +8390,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="203"/>
+      <c r="A41" s="195"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="194"/>
+      <c r="C41" s="192"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -8477,11 +8500,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="203"/>
+      <c r="A42" s="195"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="194"/>
+      <c r="C42" s="192"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -8587,11 +8610,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="203"/>
+      <c r="A43" s="195"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="194"/>
+      <c r="C43" s="192"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -8697,11 +8720,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="203"/>
+      <c r="A44" s="195"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="194"/>
+      <c r="C44" s="192"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -8807,11 +8830,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="203"/>
+      <c r="A45" s="195"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="194"/>
+      <c r="C45" s="192"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -8917,11 +8940,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="203"/>
+      <c r="A46" s="195"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="194"/>
+      <c r="C46" s="192"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -9027,11 +9050,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="203"/>
+      <c r="A47" s="195"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="194"/>
+      <c r="C47" s="192"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -9145,11 +9168,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="203"/>
+      <c r="A48" s="195"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="194"/>
+      <c r="C48" s="192"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -9258,7 +9281,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="205" t="s">
+      <c r="B49" s="197" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -9368,7 +9391,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="200"/>
+      <c r="B50" s="198"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -12799,7 +12822,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="206" t="s">
+      <c r="A81" s="199" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -12911,7 +12934,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="194"/>
+      <c r="A82" s="192"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -13021,7 +13044,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="194"/>
+      <c r="A83" s="192"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -13131,7 +13154,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="194"/>
+      <c r="A84" s="192"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -13241,7 +13264,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="194"/>
+      <c r="A85" s="192"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -13351,7 +13374,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="194"/>
+      <c r="A86" s="192"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -13461,7 +13484,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="194"/>
+      <c r="A87" s="192"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -13573,7 +13596,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="194"/>
+      <c r="A88" s="192"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -13683,7 +13706,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="194"/>
+      <c r="A89" s="192"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -13793,7 +13816,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="194"/>
+      <c r="A90" s="192"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -13903,11 +13926,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="194"/>
+      <c r="A91" s="192"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="207"/>
+      <c r="C91" s="200"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -14013,11 +14036,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="194"/>
+      <c r="A92" s="192"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="194"/>
+      <c r="C92" s="192"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -14123,11 +14146,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="197"/>
+      <c r="A93" s="193"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="194"/>
+      <c r="C93" s="192"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -14351,7 +14374,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="201" t="s">
+      <c r="A95" s="191" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -14463,7 +14486,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="194"/>
+      <c r="A96" s="192"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -14573,7 +14596,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="194"/>
+      <c r="A97" s="192"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -14683,7 +14706,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="194"/>
+      <c r="A98" s="192"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -14793,7 +14816,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="194"/>
+      <c r="A99" s="192"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -14903,7 +14926,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="194"/>
+      <c r="A100" s="192"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -15013,7 +15036,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="194"/>
+      <c r="A101" s="192"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -15123,7 +15146,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="194"/>
+      <c r="A102" s="192"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -15233,7 +15256,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="194"/>
+      <c r="A103" s="192"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -15345,7 +15368,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="194"/>
+      <c r="A104" s="192"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -15455,7 +15478,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="194"/>
+      <c r="A105" s="192"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -15573,7 +15596,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="194"/>
+      <c r="A106" s="192"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -15683,7 +15706,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="194"/>
+      <c r="A107" s="192"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -15793,7 +15816,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="194"/>
+      <c r="A108" s="192"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -15903,7 +15926,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="194"/>
+      <c r="A109" s="192"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -16013,7 +16036,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="194"/>
+      <c r="A110" s="192"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -16123,7 +16146,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="194"/>
+      <c r="A111" s="192"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -16233,7 +16256,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="194"/>
+      <c r="A112" s="192"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -16343,7 +16366,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="194"/>
+      <c r="A113" s="192"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -16453,7 +16476,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="194"/>
+      <c r="A114" s="192"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -16563,7 +16586,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="194"/>
+      <c r="A115" s="192"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -16673,7 +16696,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="194"/>
+      <c r="A116" s="192"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -16799,7 +16822,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="194"/>
+      <c r="A117" s="192"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -16909,7 +16932,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="197"/>
+      <c r="A118" s="193"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -24280,6 +24303,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -24287,12 +24316,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Ajusta largura das colunas
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A2717D-C318-4B97-8B5D-5FBDB4ED2DEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -664,7 +663,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23">
     <font>
       <sz val="10"/>
@@ -2172,26 +2171,8 @@
     <xf numFmtId="0" fontId="17" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2211,14 +2192,52 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2229,36 +2248,16 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2661,14 +2660,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -2676,8 +2675,7 @@
     <col min="1" max="1" width="13.21875" style="8" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" customWidth="1"/>
-    <col min="4" max="12" width="30.77734375" style="1" customWidth="1"/>
-    <col min="13" max="17" width="20.77734375" style="1" customWidth="1"/>
+    <col min="4" max="17" width="20.77734375" style="1" customWidth="1"/>
     <col min="18" max="20" width="20.77734375" customWidth="1"/>
     <col min="21" max="32" width="15.77734375" customWidth="1"/>
     <col min="33" max="47" width="5.6640625" customWidth="1"/>
@@ -2979,110 +2977,110 @@
       <c r="C2" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="184"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="184"/>
-      <c r="O2" s="184"/>
-      <c r="P2" s="184"/>
-      <c r="Q2" s="184"/>
-      <c r="R2" s="184" t="s">
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="178"/>
+      <c r="Q2" s="178"/>
+      <c r="R2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="184"/>
-      <c r="T2" s="184"/>
-      <c r="U2" s="184"/>
-      <c r="V2" s="184"/>
-      <c r="W2" s="184"/>
-      <c r="X2" s="184"/>
-      <c r="Y2" s="184"/>
-      <c r="Z2" s="184"/>
-      <c r="AA2" s="184"/>
-      <c r="AB2" s="184"/>
-      <c r="AC2" s="184"/>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="184"/>
-      <c r="AG2" s="184"/>
-      <c r="AH2" s="184"/>
-      <c r="AI2" s="184"/>
-      <c r="AJ2" s="184"/>
-      <c r="AK2" s="184"/>
-      <c r="AL2" s="184"/>
-      <c r="AM2" s="184" t="s">
+      <c r="S2" s="178"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="178"/>
+      <c r="V2" s="178"/>
+      <c r="W2" s="178"/>
+      <c r="X2" s="178"/>
+      <c r="Y2" s="178"/>
+      <c r="Z2" s="178"/>
+      <c r="AA2" s="178"/>
+      <c r="AB2" s="178"/>
+      <c r="AC2" s="178"/>
+      <c r="AD2" s="178"/>
+      <c r="AE2" s="178"/>
+      <c r="AF2" s="178"/>
+      <c r="AG2" s="178"/>
+      <c r="AH2" s="178"/>
+      <c r="AI2" s="178"/>
+      <c r="AJ2" s="178"/>
+      <c r="AK2" s="178"/>
+      <c r="AL2" s="178"/>
+      <c r="AM2" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="184"/>
-      <c r="AO2" s="184"/>
-      <c r="AP2" s="184"/>
-      <c r="AQ2" s="184"/>
-      <c r="AR2" s="184"/>
-      <c r="AS2" s="184"/>
-      <c r="AT2" s="184"/>
-      <c r="AU2" s="184"/>
-      <c r="AV2" s="184"/>
-      <c r="AW2" s="184"/>
-      <c r="AX2" s="185"/>
-      <c r="AY2" s="185"/>
-      <c r="AZ2" s="185"/>
-      <c r="BA2" s="185"/>
-      <c r="BB2" s="185"/>
-      <c r="BC2" s="185"/>
-      <c r="BD2" s="185"/>
-      <c r="BE2" s="185"/>
-      <c r="BF2" s="185"/>
-      <c r="BG2" s="185"/>
-      <c r="BH2" s="185"/>
-      <c r="BI2" s="185"/>
-      <c r="BJ2" s="184" t="s">
+      <c r="AN2" s="178"/>
+      <c r="AO2" s="178"/>
+      <c r="AP2" s="178"/>
+      <c r="AQ2" s="178"/>
+      <c r="AR2" s="178"/>
+      <c r="AS2" s="178"/>
+      <c r="AT2" s="178"/>
+      <c r="AU2" s="178"/>
+      <c r="AV2" s="178"/>
+      <c r="AW2" s="178"/>
+      <c r="AX2" s="179"/>
+      <c r="AY2" s="179"/>
+      <c r="AZ2" s="179"/>
+      <c r="BA2" s="179"/>
+      <c r="BB2" s="179"/>
+      <c r="BC2" s="179"/>
+      <c r="BD2" s="179"/>
+      <c r="BE2" s="179"/>
+      <c r="BF2" s="179"/>
+      <c r="BG2" s="179"/>
+      <c r="BH2" s="179"/>
+      <c r="BI2" s="179"/>
+      <c r="BJ2" s="178" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="184"/>
-      <c r="BL2" s="184"/>
-      <c r="BM2" s="184"/>
-      <c r="BN2" s="184"/>
-      <c r="BO2" s="184"/>
-      <c r="BP2" s="184"/>
-      <c r="BQ2" s="184"/>
-      <c r="BR2" s="184"/>
-      <c r="BS2" s="184"/>
-      <c r="BT2" s="184"/>
-      <c r="BU2" s="184"/>
-      <c r="BV2" s="184"/>
-      <c r="BW2" s="184"/>
-      <c r="BX2" s="186"/>
-      <c r="BY2" s="186"/>
-      <c r="BZ2" s="186"/>
-      <c r="CA2" s="186"/>
-      <c r="CB2" s="186"/>
-      <c r="CC2" s="186"/>
-      <c r="CD2" s="186"/>
-      <c r="CE2" s="187" t="s">
+      <c r="BK2" s="178"/>
+      <c r="BL2" s="178"/>
+      <c r="BM2" s="178"/>
+      <c r="BN2" s="178"/>
+      <c r="BO2" s="178"/>
+      <c r="BP2" s="178"/>
+      <c r="BQ2" s="178"/>
+      <c r="BR2" s="178"/>
+      <c r="BS2" s="178"/>
+      <c r="BT2" s="178"/>
+      <c r="BU2" s="178"/>
+      <c r="BV2" s="178"/>
+      <c r="BW2" s="178"/>
+      <c r="BX2" s="180"/>
+      <c r="BY2" s="180"/>
+      <c r="BZ2" s="180"/>
+      <c r="CA2" s="180"/>
+      <c r="CB2" s="180"/>
+      <c r="CC2" s="180"/>
+      <c r="CD2" s="180"/>
+      <c r="CE2" s="181" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="188"/>
-      <c r="CG2" s="188"/>
-      <c r="CH2" s="188"/>
-      <c r="CI2" s="188"/>
-      <c r="CJ2" s="188"/>
-      <c r="CK2" s="188"/>
-      <c r="CL2" s="188"/>
-      <c r="CM2" s="188"/>
-      <c r="CN2" s="188"/>
-      <c r="CO2" s="188"/>
-      <c r="CP2" s="188"/>
-      <c r="CQ2" s="188"/>
-      <c r="CR2" s="188"/>
-      <c r="CS2" s="188"/>
+      <c r="CF2" s="182"/>
+      <c r="CG2" s="182"/>
+      <c r="CH2" s="182"/>
+      <c r="CI2" s="182"/>
+      <c r="CJ2" s="182"/>
+      <c r="CK2" s="182"/>
+      <c r="CL2" s="182"/>
+      <c r="CM2" s="182"/>
+      <c r="CN2" s="182"/>
+      <c r="CO2" s="182"/>
+      <c r="CP2" s="182"/>
+      <c r="CQ2" s="182"/>
+      <c r="CR2" s="182"/>
+      <c r="CS2" s="182"/>
       <c r="CT2" s="172"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3378,234 +3376,250 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="177" t="s">
+      <c r="A4" s="187" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
+      <c r="C4" s="188"/>
+      <c r="D4" s="189" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="189" t="s">
+      <c r="E4" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="189" t="s">
+      <c r="F4" s="183" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="189" t="s">
+      <c r="G4" s="183" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="182" t="s">
+      <c r="H4" s="186" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="182" t="s">
+      <c r="I4" s="186" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="182" t="s">
+      <c r="J4" s="186" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="182" t="s">
+      <c r="K4" s="186" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="189" t="s">
+      <c r="L4" s="183" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="182" t="s">
+      <c r="M4" s="186" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="182" t="s">
+      <c r="N4" s="186" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="182" t="s">
+      <c r="O4" s="186" t="s">
         <v>153</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="AV4" s="178"/>
-      <c r="AW4" s="178"/>
-      <c r="BT4" s="178"/>
-      <c r="BW4" s="178"/>
-      <c r="CT4" s="178"/>
+      <c r="AV4" s="177"/>
+      <c r="AW4" s="177"/>
+      <c r="BT4" s="177"/>
+      <c r="BW4" s="177"/>
+      <c r="CT4" s="177"/>
     </row>
     <row r="5" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="177"/>
-      <c r="B5" s="179" t="s">
+      <c r="A5" s="187"/>
+      <c r="B5" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="179"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="183"/>
-      <c r="F5" s="183"/>
-      <c r="G5" s="190"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183"/>
-      <c r="K5" s="183"/>
-      <c r="L5" s="183"/>
-      <c r="M5" s="183"/>
-      <c r="N5" s="183"/>
-      <c r="O5" s="183"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="185"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="184"/>
+      <c r="L5" s="184"/>
+      <c r="M5" s="184"/>
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="AV5" s="178"/>
-      <c r="AW5" s="178"/>
-      <c r="BT5" s="178"/>
-      <c r="BW5" s="178"/>
-      <c r="CT5" s="178"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="BT5" s="177"/>
+      <c r="BW5" s="177"/>
+      <c r="CT5" s="177"/>
     </row>
     <row r="6" spans="1:98" s="9" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="177"/>
-      <c r="B6" s="179" t="s">
+      <c r="A6" s="187"/>
+      <c r="B6" s="188" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="183"/>
-      <c r="F6" s="183"/>
-      <c r="G6" s="190"/>
-      <c r="H6" s="183"/>
-      <c r="I6" s="183"/>
-      <c r="J6" s="183"/>
-      <c r="K6" s="183"/>
-      <c r="L6" s="183"/>
-      <c r="M6" s="183"/>
-      <c r="N6" s="183"/>
-      <c r="O6" s="183"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="184"/>
+      <c r="L6" s="184"/>
+      <c r="M6" s="184"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="184"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="AV6" s="178"/>
-      <c r="AW6" s="178"/>
-      <c r="BT6" s="178"/>
-      <c r="BW6" s="178"/>
-      <c r="CT6" s="178"/>
+      <c r="AV6" s="177"/>
+      <c r="AW6" s="177"/>
+      <c r="BT6" s="177"/>
+      <c r="BW6" s="177"/>
+      <c r="CT6" s="177"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="177"/>
-      <c r="B7" s="179" t="s">
+      <c r="A7" s="187"/>
+      <c r="B7" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="179"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="190"/>
-      <c r="H7" s="183"/>
-      <c r="I7" s="183"/>
-      <c r="J7" s="183"/>
-      <c r="K7" s="183"/>
-      <c r="L7" s="183"/>
-      <c r="M7" s="183"/>
-      <c r="N7" s="183"/>
-      <c r="O7" s="183"/>
+      <c r="C7" s="188"/>
+      <c r="D7" s="190"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="184"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="184"/>
+      <c r="L7" s="184"/>
+      <c r="M7" s="184"/>
+      <c r="N7" s="184"/>
+      <c r="O7" s="184"/>
       <c r="V7" s="10"/>
-      <c r="AV7" s="178"/>
-      <c r="AW7" s="178"/>
-      <c r="BT7" s="178"/>
-      <c r="BW7" s="178"/>
-      <c r="CT7" s="178"/>
+      <c r="AV7" s="177"/>
+      <c r="AW7" s="177"/>
+      <c r="BT7" s="177"/>
+      <c r="BW7" s="177"/>
+      <c r="CT7" s="177"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="177" t="s">
+      <c r="A8" s="187" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="179" t="s">
+      <c r="B8" s="188" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="179"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="183"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="190"/>
-      <c r="H8" s="183"/>
-      <c r="I8" s="183"/>
-      <c r="J8" s="183"/>
-      <c r="K8" s="183"/>
-      <c r="L8" s="183"/>
-      <c r="M8" s="183"/>
-      <c r="N8" s="183"/>
-      <c r="O8" s="183"/>
-      <c r="AV8" s="178"/>
-      <c r="AW8" s="178"/>
-      <c r="BT8" s="178"/>
-      <c r="BW8" s="178"/>
-      <c r="CT8" s="178"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="190"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="184"/>
+      <c r="L8" s="184"/>
+      <c r="M8" s="184"/>
+      <c r="N8" s="184"/>
+      <c r="O8" s="184"/>
+      <c r="AV8" s="177"/>
+      <c r="AW8" s="177"/>
+      <c r="BT8" s="177"/>
+      <c r="BW8" s="177"/>
+      <c r="CT8" s="177"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="177"/>
-      <c r="B9" s="179" t="s">
+      <c r="A9" s="187"/>
+      <c r="B9" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="179"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="183"/>
-      <c r="F9" s="183"/>
-      <c r="G9" s="190"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="183"/>
-      <c r="J9" s="183"/>
-      <c r="K9" s="183"/>
-      <c r="L9" s="183"/>
-      <c r="M9" s="183"/>
-      <c r="N9" s="183"/>
-      <c r="O9" s="183"/>
-      <c r="AV9" s="178"/>
-      <c r="AW9" s="178"/>
-      <c r="BT9" s="178"/>
-      <c r="BW9" s="178"/>
-      <c r="CT9" s="178"/>
+      <c r="C9" s="188"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="185"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="184"/>
+      <c r="L9" s="184"/>
+      <c r="M9" s="184"/>
+      <c r="N9" s="184"/>
+      <c r="O9" s="184"/>
+      <c r="AV9" s="177"/>
+      <c r="AW9" s="177"/>
+      <c r="BT9" s="177"/>
+      <c r="BW9" s="177"/>
+      <c r="CT9" s="177"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="177"/>
-      <c r="B10" s="179" t="s">
+      <c r="A10" s="187"/>
+      <c r="B10" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="179"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="190"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="183"/>
-      <c r="K10" s="183"/>
-      <c r="L10" s="183"/>
-      <c r="M10" s="183"/>
-      <c r="N10" s="183"/>
-      <c r="O10" s="183"/>
-      <c r="AV10" s="178"/>
-      <c r="AW10" s="178"/>
-      <c r="BT10" s="178"/>
-      <c r="BW10" s="178"/>
-      <c r="CT10" s="178"/>
+      <c r="C10" s="188"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="184"/>
+      <c r="L10" s="184"/>
+      <c r="M10" s="184"/>
+      <c r="N10" s="184"/>
+      <c r="O10" s="184"/>
+      <c r="AV10" s="177"/>
+      <c r="AW10" s="177"/>
+      <c r="BT10" s="177"/>
+      <c r="BW10" s="177"/>
+      <c r="CT10" s="177"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="177"/>
-      <c r="B11" s="179" t="s">
+      <c r="A11" s="187"/>
+      <c r="B11" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="179"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="183"/>
-      <c r="F11" s="183"/>
-      <c r="G11" s="190"/>
-      <c r="H11" s="183"/>
-      <c r="I11" s="183"/>
-      <c r="J11" s="183"/>
-      <c r="K11" s="183"/>
-      <c r="L11" s="183"/>
-      <c r="M11" s="183"/>
-      <c r="N11" s="183"/>
-      <c r="O11" s="183"/>
-      <c r="AV11" s="178"/>
-      <c r="AW11" s="178"/>
-      <c r="BT11" s="178"/>
-      <c r="BW11" s="178"/>
-      <c r="CT11" s="178"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="190"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="184"/>
+      <c r="L11" s="184"/>
+      <c r="M11" s="184"/>
+      <c r="N11" s="184"/>
+      <c r="O11" s="184"/>
+      <c r="AV11" s="177"/>
+      <c r="AW11" s="177"/>
+      <c r="BT11" s="177"/>
+      <c r="BW11" s="177"/>
+      <c r="CT11" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -3622,22 +3636,6 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3647,7 +3645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4311,13 +4309,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="203" t="s">
+      <c r="A4" s="193" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="196"/>
       <c r="D4" s="59"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
@@ -4422,9 +4420,9 @@
       <c r="DA4" s="64"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="192"/>
-      <c r="B5" s="202"/>
-      <c r="C5" s="192"/>
+      <c r="A5" s="194"/>
+      <c r="B5" s="192"/>
+      <c r="C5" s="194"/>
       <c r="D5" s="65"/>
       <c r="E5" s="62"/>
       <c r="F5" s="62"/>
@@ -4529,11 +4527,11 @@
       <c r="DA5" s="66"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="192"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="192"/>
+      <c r="C6" s="194"/>
       <c r="D6" s="68"/>
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
@@ -4638,11 +4636,11 @@
       <c r="DA6" s="66"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="192"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="192"/>
+      <c r="C7" s="194"/>
       <c r="D7" s="68"/>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -4747,11 +4745,11 @@
       <c r="DA7" s="66"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="192"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="192"/>
+      <c r="C8" s="194"/>
       <c r="D8" s="68"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -4856,11 +4854,11 @@
       <c r="DA8" s="66"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="192"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="192"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="68"/>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -4965,11 +4963,11 @@
       <c r="DA9" s="66"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="192"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="192"/>
+      <c r="C10" s="194"/>
       <c r="D10" s="68"/>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5074,11 +5072,11 @@
       <c r="DA10" s="66"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="192"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="192"/>
+      <c r="C11" s="194"/>
       <c r="D11" s="68"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5183,9 +5181,9 @@
       <c r="DA11" s="66"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="192"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="73"/>
-      <c r="C12" s="193"/>
+      <c r="C12" s="197"/>
       <c r="D12" s="74"/>
       <c r="E12" s="75"/>
       <c r="F12" s="75"/>
@@ -5290,10 +5288,10 @@
       <c r="DA12" s="66"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="198" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="207" t="s">
+      <c r="B13" s="199" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="77"/>
@@ -5402,8 +5400,8 @@
       <c r="DB13" s="85"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="192"/>
-      <c r="B14" s="198"/>
+      <c r="A14" s="194"/>
+      <c r="B14" s="200"/>
       <c r="C14" s="86"/>
       <c r="D14" s="78"/>
       <c r="E14" s="79"/>
@@ -5524,7 +5522,7 @@
       <c r="DB14" s="85"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="192"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="89" t="s">
         <v>32</v>
       </c>
@@ -5634,7 +5632,7 @@
       <c r="DB15" s="85"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="192"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="90" t="s">
         <v>33</v>
       </c>
@@ -5744,7 +5742,7 @@
       <c r="DB16" s="85"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="192"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="90" t="s">
         <v>34</v>
       </c>
@@ -5856,7 +5854,7 @@
       <c r="DB17" s="85"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="192"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="90" t="s">
         <v>35</v>
       </c>
@@ -5966,7 +5964,7 @@
       <c r="DB18" s="85"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="192"/>
+      <c r="A19" s="194"/>
       <c r="B19" s="90" t="s">
         <v>36</v>
       </c>
@@ -6076,7 +6074,7 @@
       <c r="DB19" s="85"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="192"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="92" t="s">
         <v>37</v>
       </c>
@@ -6186,7 +6184,7 @@
       <c r="DB20" s="85"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="193"/>
+      <c r="A21" s="197"/>
       <c r="B21" s="93" t="s">
         <v>38</v>
       </c>
@@ -6297,7 +6295,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="95"/>
-      <c r="B22" s="201" t="s">
+      <c r="B22" s="191" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="96"/>
@@ -6407,7 +6405,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="95"/>
-      <c r="B23" s="202"/>
+      <c r="B23" s="192"/>
       <c r="C23" s="102"/>
       <c r="D23" s="97"/>
       <c r="E23" s="98"/>
@@ -6514,13 +6512,13 @@
       <c r="DB23" s="101"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="194" t="s">
+      <c r="A24" s="202" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="196">
+      <c r="C24" s="204">
         <v>0.1</v>
       </c>
       <c r="D24" s="97"/>
@@ -6628,11 +6626,11 @@
       <c r="DB24" s="101"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="195"/>
+      <c r="A25" s="203"/>
       <c r="B25" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="192"/>
+      <c r="C25" s="194"/>
       <c r="D25" s="106"/>
       <c r="E25" s="100"/>
       <c r="F25" s="100"/>
@@ -6738,11 +6736,11 @@
       <c r="DB25" s="101"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="195"/>
+      <c r="A26" s="203"/>
       <c r="B26" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="192"/>
+      <c r="C26" s="194"/>
       <c r="D26" s="106"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
@@ -6848,11 +6846,11 @@
       <c r="DB26" s="101"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="195"/>
+      <c r="A27" s="203"/>
       <c r="B27" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="192"/>
+      <c r="C27" s="194"/>
       <c r="D27" s="106"/>
       <c r="E27" s="100"/>
       <c r="F27" s="100"/>
@@ -6958,11 +6956,11 @@
       <c r="DB27" s="101"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="195"/>
+      <c r="A28" s="203"/>
       <c r="B28" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="192"/>
+      <c r="C28" s="194"/>
       <c r="D28" s="106"/>
       <c r="E28" s="100"/>
       <c r="F28" s="100"/>
@@ -7068,11 +7066,11 @@
       <c r="DB28" s="101"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="195"/>
+      <c r="A29" s="203"/>
       <c r="B29" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="192"/>
+      <c r="C29" s="194"/>
       <c r="D29" s="106"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
@@ -7178,11 +7176,11 @@
       <c r="DB29" s="101"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="195"/>
+      <c r="A30" s="203"/>
       <c r="B30" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="192"/>
+      <c r="C30" s="194"/>
       <c r="D30" s="106"/>
       <c r="E30" s="100"/>
       <c r="F30" s="100"/>
@@ -7288,11 +7286,11 @@
       <c r="DB30" s="101"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="195"/>
+      <c r="A31" s="203"/>
       <c r="B31" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="192"/>
+      <c r="C31" s="194"/>
       <c r="D31" s="106"/>
       <c r="E31" s="100"/>
       <c r="F31" s="100"/>
@@ -7398,11 +7396,11 @@
       <c r="DB31" s="101"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="195"/>
+      <c r="A32" s="203"/>
       <c r="B32" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="192"/>
+      <c r="C32" s="194"/>
       <c r="D32" s="106"/>
       <c r="E32" s="100"/>
       <c r="F32" s="100"/>
@@ -7508,11 +7506,11 @@
       <c r="DB32" s="101"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="195"/>
+      <c r="A33" s="203"/>
       <c r="B33" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="192"/>
+      <c r="C33" s="194"/>
       <c r="D33" s="106"/>
       <c r="E33" s="100"/>
       <c r="F33" s="100"/>
@@ -7618,11 +7616,11 @@
       <c r="DB33" s="101"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="195"/>
+      <c r="A34" s="203"/>
       <c r="B34" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="192"/>
+      <c r="C34" s="194"/>
       <c r="D34" s="106"/>
       <c r="E34" s="100"/>
       <c r="F34" s="100"/>
@@ -7728,11 +7726,11 @@
       <c r="DB34" s="101"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="195"/>
+      <c r="A35" s="203"/>
       <c r="B35" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="193"/>
+      <c r="C35" s="197"/>
       <c r="D35" s="106"/>
       <c r="E35" s="100"/>
       <c r="F35" s="100"/>
@@ -7838,11 +7836,11 @@
       <c r="DB35" s="101"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="195"/>
+      <c r="A36" s="203"/>
       <c r="B36" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="196">
+      <c r="C36" s="204">
         <v>0.1</v>
       </c>
       <c r="D36" s="106"/>
@@ -7950,11 +7948,11 @@
       <c r="DB36" s="101"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="195"/>
+      <c r="A37" s="203"/>
       <c r="B37" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="192"/>
+      <c r="C37" s="194"/>
       <c r="D37" s="106"/>
       <c r="E37" s="100"/>
       <c r="F37" s="100"/>
@@ -8060,11 +8058,11 @@
       <c r="DB37" s="101"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="195"/>
+      <c r="A38" s="203"/>
       <c r="B38" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="192"/>
+      <c r="C38" s="194"/>
       <c r="D38" s="106"/>
       <c r="E38" s="100"/>
       <c r="F38" s="100"/>
@@ -8170,11 +8168,11 @@
       <c r="DB38" s="101"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="195"/>
+      <c r="A39" s="203"/>
       <c r="B39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="192"/>
+      <c r="C39" s="194"/>
       <c r="D39" s="106"/>
       <c r="E39" s="100"/>
       <c r="F39" s="100"/>
@@ -8280,11 +8278,11 @@
       <c r="DB39" s="101"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="195"/>
+      <c r="A40" s="203"/>
       <c r="B40" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="192"/>
+      <c r="C40" s="194"/>
       <c r="D40" s="106"/>
       <c r="E40" s="100"/>
       <c r="F40" s="100"/>
@@ -8390,11 +8388,11 @@
       <c r="DB40" s="101"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="195"/>
+      <c r="A41" s="203"/>
       <c r="B41" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="192"/>
+      <c r="C41" s="194"/>
       <c r="D41" s="106"/>
       <c r="E41" s="100"/>
       <c r="F41" s="100"/>
@@ -8500,11 +8498,11 @@
       <c r="DB41" s="101"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="195"/>
+      <c r="A42" s="203"/>
       <c r="B42" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="192"/>
+      <c r="C42" s="194"/>
       <c r="D42" s="106"/>
       <c r="E42" s="100"/>
       <c r="F42" s="100"/>
@@ -8610,11 +8608,11 @@
       <c r="DB42" s="101"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="195"/>
+      <c r="A43" s="203"/>
       <c r="B43" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="192"/>
+      <c r="C43" s="194"/>
       <c r="D43" s="106"/>
       <c r="E43" s="100"/>
       <c r="F43" s="100"/>
@@ -8720,11 +8718,11 @@
       <c r="DB43" s="101"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="195"/>
+      <c r="A44" s="203"/>
       <c r="B44" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="192"/>
+      <c r="C44" s="194"/>
       <c r="D44" s="106"/>
       <c r="E44" s="100"/>
       <c r="F44" s="100"/>
@@ -8830,11 +8828,11 @@
       <c r="DB44" s="101"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="195"/>
+      <c r="A45" s="203"/>
       <c r="B45" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="192"/>
+      <c r="C45" s="194"/>
       <c r="D45" s="106"/>
       <c r="E45" s="100"/>
       <c r="F45" s="100"/>
@@ -8940,11 +8938,11 @@
       <c r="DB45" s="101"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="195"/>
+      <c r="A46" s="203"/>
       <c r="B46" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="192"/>
+      <c r="C46" s="194"/>
       <c r="D46" s="106"/>
       <c r="E46" s="100"/>
       <c r="F46" s="100"/>
@@ -9050,11 +9048,11 @@
       <c r="DB46" s="101"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="195"/>
+      <c r="A47" s="203"/>
       <c r="B47" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="192"/>
+      <c r="C47" s="194"/>
       <c r="D47" s="106"/>
       <c r="E47" s="100"/>
       <c r="F47" s="100"/>
@@ -9168,11 +9166,11 @@
       <c r="DB47" s="101"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="195"/>
+      <c r="A48" s="203"/>
       <c r="B48" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="192"/>
+      <c r="C48" s="194"/>
       <c r="D48" s="106"/>
       <c r="E48" s="100"/>
       <c r="F48" s="100"/>
@@ -9281,7 +9279,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="113"/>
-      <c r="B49" s="197" t="s">
+      <c r="B49" s="205" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="113"/>
@@ -9391,7 +9389,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="118"/>
-      <c r="B50" s="198"/>
+      <c r="B50" s="200"/>
       <c r="C50" s="118"/>
       <c r="D50" s="114"/>
       <c r="E50" s="115"/>
@@ -12822,7 +12820,7 @@
       <c r="DB80" s="117"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="199" t="s">
+      <c r="A81" s="206" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="124" t="s">
@@ -12934,7 +12932,7 @@
       <c r="DB81" s="131"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="192"/>
+      <c r="A82" s="194"/>
       <c r="B82" s="132" t="s">
         <v>100</v>
       </c>
@@ -13044,7 +13042,7 @@
       <c r="DB82" s="131"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="192"/>
+      <c r="A83" s="194"/>
       <c r="B83" s="132" t="s">
         <v>101</v>
       </c>
@@ -13154,7 +13152,7 @@
       <c r="DB83" s="131"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="192"/>
+      <c r="A84" s="194"/>
       <c r="B84" s="132" t="s">
         <v>102</v>
       </c>
@@ -13264,7 +13262,7 @@
       <c r="DB84" s="131"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="192"/>
+      <c r="A85" s="194"/>
       <c r="B85" s="132" t="s">
         <v>103</v>
       </c>
@@ -13374,7 +13372,7 @@
       <c r="DB85" s="131"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="192"/>
+      <c r="A86" s="194"/>
       <c r="B86" s="132" t="s">
         <v>104</v>
       </c>
@@ -13484,7 +13482,7 @@
       <c r="DB86" s="131"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="192"/>
+      <c r="A87" s="194"/>
       <c r="B87" s="132" t="s">
         <v>105</v>
       </c>
@@ -13596,7 +13594,7 @@
       <c r="DB87" s="131"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="192"/>
+      <c r="A88" s="194"/>
       <c r="B88" s="132" t="s">
         <v>106</v>
       </c>
@@ -13706,7 +13704,7 @@
       <c r="DB88" s="131"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="192"/>
+      <c r="A89" s="194"/>
       <c r="B89" s="132" t="s">
         <v>107</v>
       </c>
@@ -13816,7 +13814,7 @@
       <c r="DB89" s="131"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="192"/>
+      <c r="A90" s="194"/>
       <c r="B90" s="132" t="s">
         <v>108</v>
       </c>
@@ -13926,11 +13924,11 @@
       <c r="DB90" s="131"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="192"/>
+      <c r="A91" s="194"/>
       <c r="B91" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="200"/>
+      <c r="C91" s="207"/>
       <c r="D91" s="126"/>
       <c r="E91" s="127"/>
       <c r="F91" s="127"/>
@@ -14036,11 +14034,11 @@
       <c r="DB91" s="131"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="192"/>
+      <c r="A92" s="194"/>
       <c r="B92" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="192"/>
+      <c r="C92" s="194"/>
       <c r="D92" s="126"/>
       <c r="E92" s="127"/>
       <c r="F92" s="127"/>
@@ -14146,11 +14144,11 @@
       <c r="DB92" s="131"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="193"/>
+      <c r="A93" s="197"/>
       <c r="B93" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="192"/>
+      <c r="C93" s="194"/>
       <c r="D93" s="126"/>
       <c r="E93" s="127"/>
       <c r="F93" s="127"/>
@@ -14374,7 +14372,7 @@
       <c r="DB94" s="131"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="191" t="s">
+      <c r="A95" s="201" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="139" t="s">
@@ -14486,7 +14484,7 @@
       <c r="DB95" s="143"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="192"/>
+      <c r="A96" s="194"/>
       <c r="B96" s="144" t="s">
         <v>114</v>
       </c>
@@ -14596,7 +14594,7 @@
       <c r="DB96" s="143"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="192"/>
+      <c r="A97" s="194"/>
       <c r="B97" s="147" t="s">
         <v>115</v>
       </c>
@@ -14706,7 +14704,7 @@
       <c r="DB97" s="143"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="192"/>
+      <c r="A98" s="194"/>
       <c r="B98" s="147" t="s">
         <v>116</v>
       </c>
@@ -14816,7 +14814,7 @@
       <c r="DB98" s="143"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="192"/>
+      <c r="A99" s="194"/>
       <c r="B99" s="147" t="s">
         <v>117</v>
       </c>
@@ -14926,7 +14924,7 @@
       <c r="DB99" s="143"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="192"/>
+      <c r="A100" s="194"/>
       <c r="B100" s="147" t="s">
         <v>118</v>
       </c>
@@ -15036,7 +15034,7 @@
       <c r="DB100" s="143"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="192"/>
+      <c r="A101" s="194"/>
       <c r="B101" s="147" t="s">
         <v>119</v>
       </c>
@@ -15146,7 +15144,7 @@
       <c r="DB101" s="143"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="192"/>
+      <c r="A102" s="194"/>
       <c r="B102" s="147" t="s">
         <v>120</v>
       </c>
@@ -15256,7 +15254,7 @@
       <c r="DB102" s="143"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="192"/>
+      <c r="A103" s="194"/>
       <c r="B103" s="147" t="s">
         <v>121</v>
       </c>
@@ -15368,7 +15366,7 @@
       <c r="DB103" s="143"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="192"/>
+      <c r="A104" s="194"/>
       <c r="B104" s="147" t="s">
         <v>122</v>
       </c>
@@ -15478,7 +15476,7 @@
       <c r="DB104" s="143"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="192"/>
+      <c r="A105" s="194"/>
       <c r="B105" s="150" t="s">
         <v>123</v>
       </c>
@@ -15596,7 +15594,7 @@
       <c r="DB105" s="143"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="192"/>
+      <c r="A106" s="194"/>
       <c r="B106" s="151" t="s">
         <v>125</v>
       </c>
@@ -15706,7 +15704,7 @@
       <c r="DB106" s="143"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="192"/>
+      <c r="A107" s="194"/>
       <c r="B107" s="152" t="s">
         <v>126</v>
       </c>
@@ -15816,7 +15814,7 @@
       <c r="DB107" s="143"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="192"/>
+      <c r="A108" s="194"/>
       <c r="B108" s="147" t="s">
         <v>127</v>
       </c>
@@ -15926,7 +15924,7 @@
       <c r="DB108" s="143"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="192"/>
+      <c r="A109" s="194"/>
       <c r="B109" s="147" t="s">
         <v>128</v>
       </c>
@@ -16036,7 +16034,7 @@
       <c r="DB109" s="143"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="192"/>
+      <c r="A110" s="194"/>
       <c r="B110" s="147" t="s">
         <v>129</v>
       </c>
@@ -16146,7 +16144,7 @@
       <c r="DB110" s="143"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="192"/>
+      <c r="A111" s="194"/>
       <c r="B111" s="147" t="s">
         <v>130</v>
       </c>
@@ -16256,7 +16254,7 @@
       <c r="DB111" s="143"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="192"/>
+      <c r="A112" s="194"/>
       <c r="B112" s="147" t="s">
         <v>131</v>
       </c>
@@ -16366,7 +16364,7 @@
       <c r="DB112" s="143"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="192"/>
+      <c r="A113" s="194"/>
       <c r="B113" s="147" t="s">
         <v>132</v>
       </c>
@@ -16476,7 +16474,7 @@
       <c r="DB113" s="143"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="192"/>
+      <c r="A114" s="194"/>
       <c r="B114" s="147" t="s">
         <v>133</v>
       </c>
@@ -16586,7 +16584,7 @@
       <c r="DB114" s="143"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="192"/>
+      <c r="A115" s="194"/>
       <c r="B115" s="147" t="s">
         <v>134</v>
       </c>
@@ -16696,7 +16694,7 @@
       <c r="DB115" s="143"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="192"/>
+      <c r="A116" s="194"/>
       <c r="B116" s="153" t="s">
         <v>135</v>
       </c>
@@ -16822,7 +16820,7 @@
       <c r="DB116" s="143"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="192"/>
+      <c r="A117" s="194"/>
       <c r="B117" s="150" t="s">
         <v>136</v>
       </c>
@@ -16932,7 +16930,7 @@
       <c r="DB117" s="143"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="193"/>
+      <c r="A118" s="197"/>
       <c r="B118" s="156" t="s">
         <v>137</v>
       </c>
@@ -24303,12 +24301,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -24316,6 +24308,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 02-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725EC9E9-3FF4-45D7-8E38-D32AEF459D4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5393897D-8FE6-4533-B985-078F570484C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="157">
   <si>
     <t>S</t>
   </si>
@@ -668,6 +668,9 @@
   <si>
     <t>Posicionamento de elementos usando position absolute e relativo.
 Responsividade com media queries</t>
+  </si>
+  <si>
+    <t>Criação da página de cadastro de categorias do projeto Gufos</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2172,14 +2175,42 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2196,11 +2227,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2211,71 +2271,23 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2781,7 +2793,7 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="R4" sqref="R4:R11"/>
@@ -3093,110 +3105,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="178"/>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178"/>
-      <c r="N2" s="178"/>
-      <c r="O2" s="178"/>
-      <c r="P2" s="178"/>
-      <c r="Q2" s="178"/>
-      <c r="R2" s="178" t="s">
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="188"/>
+      <c r="K2" s="188"/>
+      <c r="L2" s="188"/>
+      <c r="M2" s="188"/>
+      <c r="N2" s="188"/>
+      <c r="O2" s="188"/>
+      <c r="P2" s="188"/>
+      <c r="Q2" s="188"/>
+      <c r="R2" s="188" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="178"/>
-      <c r="T2" s="178"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="178"/>
-      <c r="W2" s="178"/>
-      <c r="X2" s="178"/>
-      <c r="Y2" s="178"/>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="178"/>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="178"/>
-      <c r="AG2" s="178"/>
-      <c r="AH2" s="178"/>
-      <c r="AI2" s="178"/>
-      <c r="AJ2" s="178"/>
-      <c r="AK2" s="178"/>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="178" t="s">
+      <c r="S2" s="188"/>
+      <c r="T2" s="188"/>
+      <c r="U2" s="188"/>
+      <c r="V2" s="188"/>
+      <c r="W2" s="188"/>
+      <c r="X2" s="188"/>
+      <c r="Y2" s="188"/>
+      <c r="Z2" s="188"/>
+      <c r="AA2" s="188"/>
+      <c r="AB2" s="188"/>
+      <c r="AC2" s="188"/>
+      <c r="AD2" s="188"/>
+      <c r="AE2" s="188"/>
+      <c r="AF2" s="188"/>
+      <c r="AG2" s="188"/>
+      <c r="AH2" s="188"/>
+      <c r="AI2" s="188"/>
+      <c r="AJ2" s="188"/>
+      <c r="AK2" s="188"/>
+      <c r="AL2" s="188"/>
+      <c r="AM2" s="188" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="178"/>
-      <c r="AP2" s="178"/>
-      <c r="AQ2" s="178"/>
-      <c r="AR2" s="178"/>
-      <c r="AS2" s="178"/>
-      <c r="AT2" s="178"/>
-      <c r="AU2" s="178"/>
-      <c r="AV2" s="178"/>
-      <c r="AW2" s="178"/>
-      <c r="AX2" s="179"/>
-      <c r="AY2" s="179"/>
-      <c r="AZ2" s="179"/>
-      <c r="BA2" s="179"/>
-      <c r="BB2" s="179"/>
-      <c r="BC2" s="179"/>
-      <c r="BD2" s="179"/>
-      <c r="BE2" s="179"/>
-      <c r="BF2" s="179"/>
-      <c r="BG2" s="179"/>
-      <c r="BH2" s="179"/>
-      <c r="BI2" s="179"/>
-      <c r="BJ2" s="178" t="s">
+      <c r="AN2" s="188"/>
+      <c r="AO2" s="188"/>
+      <c r="AP2" s="188"/>
+      <c r="AQ2" s="188"/>
+      <c r="AR2" s="188"/>
+      <c r="AS2" s="188"/>
+      <c r="AT2" s="188"/>
+      <c r="AU2" s="188"/>
+      <c r="AV2" s="188"/>
+      <c r="AW2" s="188"/>
+      <c r="AX2" s="189"/>
+      <c r="AY2" s="189"/>
+      <c r="AZ2" s="189"/>
+      <c r="BA2" s="189"/>
+      <c r="BB2" s="189"/>
+      <c r="BC2" s="189"/>
+      <c r="BD2" s="189"/>
+      <c r="BE2" s="189"/>
+      <c r="BF2" s="189"/>
+      <c r="BG2" s="189"/>
+      <c r="BH2" s="189"/>
+      <c r="BI2" s="189"/>
+      <c r="BJ2" s="188" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="178"/>
-      <c r="BL2" s="178"/>
-      <c r="BM2" s="178"/>
-      <c r="BN2" s="178"/>
-      <c r="BO2" s="178"/>
-      <c r="BP2" s="178"/>
-      <c r="BQ2" s="178"/>
-      <c r="BR2" s="178"/>
-      <c r="BS2" s="178"/>
-      <c r="BT2" s="178"/>
-      <c r="BU2" s="178"/>
-      <c r="BV2" s="178"/>
-      <c r="BW2" s="178"/>
-      <c r="BX2" s="180"/>
-      <c r="BY2" s="180"/>
-      <c r="BZ2" s="180"/>
-      <c r="CA2" s="180"/>
-      <c r="CB2" s="180"/>
-      <c r="CC2" s="180"/>
-      <c r="CD2" s="180"/>
-      <c r="CE2" s="181" t="s">
+      <c r="BK2" s="188"/>
+      <c r="BL2" s="188"/>
+      <c r="BM2" s="188"/>
+      <c r="BN2" s="188"/>
+      <c r="BO2" s="188"/>
+      <c r="BP2" s="188"/>
+      <c r="BQ2" s="188"/>
+      <c r="BR2" s="188"/>
+      <c r="BS2" s="188"/>
+      <c r="BT2" s="188"/>
+      <c r="BU2" s="188"/>
+      <c r="BV2" s="188"/>
+      <c r="BW2" s="188"/>
+      <c r="BX2" s="190"/>
+      <c r="BY2" s="190"/>
+      <c r="BZ2" s="190"/>
+      <c r="CA2" s="190"/>
+      <c r="CB2" s="190"/>
+      <c r="CC2" s="190"/>
+      <c r="CD2" s="190"/>
+      <c r="CE2" s="191" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="182"/>
-      <c r="CG2" s="182"/>
-      <c r="CH2" s="182"/>
-      <c r="CI2" s="182"/>
-      <c r="CJ2" s="182"/>
-      <c r="CK2" s="182"/>
-      <c r="CL2" s="182"/>
-      <c r="CM2" s="182"/>
-      <c r="CN2" s="182"/>
-      <c r="CO2" s="182"/>
-      <c r="CP2" s="182"/>
-      <c r="CQ2" s="182"/>
-      <c r="CR2" s="182"/>
-      <c r="CS2" s="182"/>
+      <c r="CF2" s="192"/>
+      <c r="CG2" s="192"/>
+      <c r="CH2" s="192"/>
+      <c r="CI2" s="192"/>
+      <c r="CJ2" s="192"/>
+      <c r="CK2" s="192"/>
+      <c r="CL2" s="192"/>
+      <c r="CM2" s="192"/>
+      <c r="CN2" s="192"/>
+      <c r="CO2" s="192"/>
+      <c r="CP2" s="192"/>
+      <c r="CQ2" s="192"/>
+      <c r="CR2" s="192"/>
+      <c r="CS2" s="192"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3319,10 +3331,10 @@
       <c r="AO3" s="168">
         <v>3</v>
       </c>
-      <c r="AP3" s="213">
+      <c r="AP3" s="177">
         <v>4</v>
       </c>
-      <c r="AQ3" s="213">
+      <c r="AQ3" s="177">
         <v>7</v>
       </c>
       <c r="AR3" s="168">
@@ -3334,7 +3346,7 @@
       <c r="AT3" s="168">
         <v>10</v>
       </c>
-      <c r="AU3" s="213">
+      <c r="AU3" s="177">
         <v>11</v>
       </c>
       <c r="AV3" s="6">
@@ -3492,608 +3504,585 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="175" t="s">
+      <c r="A4" s="194" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="195" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="202" t="s">
+      <c r="C4" s="195"/>
+      <c r="D4" s="193" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="202" t="s">
+      <c r="E4" s="193" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="202" t="s">
+      <c r="F4" s="193" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="202" t="s">
+      <c r="G4" s="193" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="202" t="s">
+      <c r="H4" s="193" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="202" t="s">
+      <c r="I4" s="193" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="202" t="s">
+      <c r="J4" s="193" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="202" t="s">
+      <c r="K4" s="193" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="203" t="s">
+      <c r="L4" s="186" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="203" t="s">
+      <c r="M4" s="186" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="203" t="s">
+      <c r="N4" s="186" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="203" t="s">
+      <c r="O4" s="186" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="203" t="s">
+      <c r="P4" s="186" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="203" t="s">
+      <c r="Q4" s="186" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="204"/>
-      <c r="S4" s="204"/>
-      <c r="T4" s="204"/>
-      <c r="U4" s="204"/>
-      <c r="V4" s="204"/>
-      <c r="W4" s="206"/>
-      <c r="X4" s="206"/>
-      <c r="Y4" s="206"/>
-      <c r="Z4" s="206"/>
-      <c r="AA4" s="206"/>
-      <c r="AB4" s="208"/>
-      <c r="AC4" s="208"/>
-      <c r="AD4" s="208"/>
-      <c r="AE4" s="208"/>
-      <c r="AF4" s="208"/>
-      <c r="AG4" s="208"/>
-      <c r="AH4" s="208"/>
-      <c r="AI4" s="208"/>
-      <c r="AJ4" s="208"/>
-      <c r="AK4" s="208"/>
-      <c r="AL4" s="208"/>
-      <c r="AM4" s="208"/>
-      <c r="AN4" s="208"/>
-      <c r="AO4" s="208"/>
-      <c r="AP4" s="208"/>
-      <c r="AQ4" s="208"/>
-      <c r="AR4" s="208"/>
-      <c r="AS4" s="208"/>
-      <c r="AT4" s="208"/>
-      <c r="AU4" s="209"/>
-      <c r="AV4" s="176"/>
-      <c r="AW4" s="176"/>
-      <c r="AX4" s="205"/>
-      <c r="AY4" s="206"/>
-      <c r="AZ4" s="206"/>
-      <c r="BA4" s="206"/>
-      <c r="BB4" s="206"/>
-      <c r="BC4" s="206"/>
-      <c r="BD4" s="206"/>
-      <c r="BE4" s="206"/>
-      <c r="BF4" s="201"/>
-      <c r="BG4" s="201"/>
-      <c r="BT4" s="176"/>
-      <c r="BW4" s="176"/>
-      <c r="CT4" s="176"/>
+      <c r="R4" s="186" t="s">
+        <v>156</v>
+      </c>
+      <c r="S4" s="186"/>
+      <c r="T4" s="186"/>
+      <c r="U4" s="186"/>
+      <c r="V4" s="186"/>
+      <c r="W4" s="213"/>
+      <c r="X4" s="213"/>
+      <c r="Y4" s="213"/>
+      <c r="Z4" s="213"/>
+      <c r="AA4" s="213"/>
+      <c r="AB4" s="214"/>
+      <c r="AC4" s="214"/>
+      <c r="AD4" s="214"/>
+      <c r="AE4" s="214"/>
+      <c r="AF4" s="214"/>
+      <c r="AG4" s="214"/>
+      <c r="AH4" s="214"/>
+      <c r="AI4" s="214"/>
+      <c r="AJ4" s="214"/>
+      <c r="AK4" s="214"/>
+      <c r="AL4" s="214"/>
+      <c r="AM4" s="214"/>
+      <c r="AN4" s="214"/>
+      <c r="AO4" s="214"/>
+      <c r="AP4" s="214"/>
+      <c r="AQ4" s="214"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
+      <c r="AU4" s="175"/>
+      <c r="AV4" s="187"/>
+      <c r="AW4" s="187"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="187"/>
+      <c r="BW4" s="187"/>
+      <c r="CT4" s="187"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="175"/>
-      <c r="B5" s="177" t="s">
+      <c r="A5" s="194"/>
+      <c r="B5" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="177"/>
-      <c r="D5" s="202"/>
-      <c r="E5" s="202"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="202"/>
-      <c r="H5" s="202"/>
-      <c r="I5" s="202"/>
-      <c r="J5" s="202"/>
-      <c r="K5" s="202"/>
-      <c r="L5" s="203"/>
-      <c r="M5" s="203"/>
-      <c r="N5" s="203"/>
-      <c r="O5" s="203"/>
-      <c r="P5" s="203"/>
-      <c r="Q5" s="203"/>
-      <c r="R5" s="204"/>
-      <c r="S5" s="204"/>
-      <c r="T5" s="204"/>
-      <c r="U5" s="204"/>
-      <c r="V5" s="204"/>
-      <c r="W5" s="206"/>
-      <c r="X5" s="206"/>
-      <c r="Y5" s="206"/>
-      <c r="Z5" s="206"/>
-      <c r="AA5" s="206"/>
-      <c r="AB5" s="210"/>
-      <c r="AC5" s="210"/>
-      <c r="AD5" s="210"/>
-      <c r="AE5" s="210"/>
-      <c r="AF5" s="210"/>
-      <c r="AG5" s="210"/>
-      <c r="AH5" s="210"/>
-      <c r="AI5" s="210"/>
-      <c r="AJ5" s="210"/>
-      <c r="AK5" s="210"/>
-      <c r="AL5" s="210"/>
-      <c r="AM5" s="210"/>
-      <c r="AN5" s="210"/>
-      <c r="AO5" s="210"/>
-      <c r="AP5" s="210"/>
-      <c r="AQ5" s="210"/>
-      <c r="AR5" s="210"/>
-      <c r="AS5" s="210"/>
-      <c r="AT5" s="210"/>
-      <c r="AU5" s="209"/>
-      <c r="AV5" s="176"/>
-      <c r="AW5" s="176"/>
-      <c r="AX5" s="207"/>
-      <c r="AY5" s="206"/>
-      <c r="AZ5" s="206"/>
-      <c r="BA5" s="206"/>
-      <c r="BB5" s="206"/>
-      <c r="BC5" s="206"/>
-      <c r="BD5" s="206"/>
-      <c r="BE5" s="206"/>
-      <c r="BF5" s="200"/>
-      <c r="BG5" s="200"/>
-      <c r="BT5" s="176"/>
-      <c r="BW5" s="176"/>
-      <c r="CT5" s="176"/>
+      <c r="C5" s="195"/>
+      <c r="D5" s="193"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="193"/>
+      <c r="G5" s="193"/>
+      <c r="H5" s="193"/>
+      <c r="I5" s="193"/>
+      <c r="J5" s="193"/>
+      <c r="K5" s="193"/>
+      <c r="L5" s="186"/>
+      <c r="M5" s="186"/>
+      <c r="N5" s="186"/>
+      <c r="O5" s="186"/>
+      <c r="P5" s="186"/>
+      <c r="Q5" s="186"/>
+      <c r="R5" s="186"/>
+      <c r="S5" s="186"/>
+      <c r="T5" s="186"/>
+      <c r="U5" s="186"/>
+      <c r="V5" s="186"/>
+      <c r="W5" s="213"/>
+      <c r="X5" s="213"/>
+      <c r="Y5" s="213"/>
+      <c r="Z5" s="213"/>
+      <c r="AA5" s="213"/>
+      <c r="AB5" s="215"/>
+      <c r="AC5" s="215"/>
+      <c r="AD5" s="215"/>
+      <c r="AE5" s="215"/>
+      <c r="AF5" s="215"/>
+      <c r="AG5" s="215"/>
+      <c r="AH5" s="215"/>
+      <c r="AI5" s="215"/>
+      <c r="AJ5" s="215"/>
+      <c r="AK5" s="215"/>
+      <c r="AL5" s="215"/>
+      <c r="AM5" s="215"/>
+      <c r="AN5" s="215"/>
+      <c r="AO5" s="215"/>
+      <c r="AP5" s="215"/>
+      <c r="AQ5" s="215"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
+      <c r="AU5" s="175"/>
+      <c r="AV5" s="187"/>
+      <c r="AW5" s="187"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="187"/>
+      <c r="BW5" s="187"/>
+      <c r="CT5" s="187"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="175"/>
-      <c r="B6" s="177" t="s">
+      <c r="A6" s="194"/>
+      <c r="B6" s="195" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="177"/>
-      <c r="D6" s="202"/>
-      <c r="E6" s="202"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="202"/>
-      <c r="H6" s="202"/>
-      <c r="I6" s="202"/>
-      <c r="J6" s="202"/>
-      <c r="K6" s="202"/>
-      <c r="L6" s="203"/>
-      <c r="M6" s="203"/>
-      <c r="N6" s="203"/>
-      <c r="O6" s="203"/>
-      <c r="P6" s="203"/>
-      <c r="Q6" s="203"/>
-      <c r="R6" s="204"/>
-      <c r="S6" s="204"/>
-      <c r="T6" s="204"/>
-      <c r="U6" s="204"/>
-      <c r="V6" s="204"/>
-      <c r="W6" s="206"/>
-      <c r="X6" s="206"/>
-      <c r="Y6" s="206"/>
-      <c r="Z6" s="206"/>
-      <c r="AA6" s="206"/>
-      <c r="AB6" s="210"/>
-      <c r="AC6" s="210"/>
-      <c r="AD6" s="210"/>
-      <c r="AE6" s="210"/>
-      <c r="AF6" s="210"/>
-      <c r="AG6" s="210"/>
-      <c r="AH6" s="210"/>
-      <c r="AI6" s="210"/>
-      <c r="AJ6" s="210"/>
-      <c r="AK6" s="210"/>
-      <c r="AL6" s="210"/>
-      <c r="AM6" s="210"/>
-      <c r="AN6" s="210"/>
-      <c r="AO6" s="210"/>
-      <c r="AP6" s="210"/>
-      <c r="AQ6" s="210"/>
-      <c r="AR6" s="210"/>
-      <c r="AS6" s="210"/>
-      <c r="AT6" s="210"/>
-      <c r="AU6" s="209"/>
-      <c r="AV6" s="176"/>
-      <c r="AW6" s="176"/>
-      <c r="AX6" s="207"/>
-      <c r="AY6" s="206"/>
-      <c r="AZ6" s="206"/>
-      <c r="BA6" s="206"/>
-      <c r="BB6" s="206"/>
-      <c r="BC6" s="206"/>
-      <c r="BD6" s="206"/>
-      <c r="BE6" s="206"/>
-      <c r="BF6" s="200"/>
-      <c r="BG6" s="200"/>
-      <c r="BT6" s="176"/>
-      <c r="BW6" s="176"/>
-      <c r="CT6" s="176"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="193"/>
+      <c r="E6" s="193"/>
+      <c r="F6" s="193"/>
+      <c r="G6" s="193"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="193"/>
+      <c r="J6" s="193"/>
+      <c r="K6" s="193"/>
+      <c r="L6" s="186"/>
+      <c r="M6" s="186"/>
+      <c r="N6" s="186"/>
+      <c r="O6" s="186"/>
+      <c r="P6" s="186"/>
+      <c r="Q6" s="186"/>
+      <c r="R6" s="186"/>
+      <c r="S6" s="186"/>
+      <c r="T6" s="186"/>
+      <c r="U6" s="186"/>
+      <c r="V6" s="186"/>
+      <c r="W6" s="213"/>
+      <c r="X6" s="213"/>
+      <c r="Y6" s="213"/>
+      <c r="Z6" s="213"/>
+      <c r="AA6" s="213"/>
+      <c r="AB6" s="215"/>
+      <c r="AC6" s="215"/>
+      <c r="AD6" s="215"/>
+      <c r="AE6" s="215"/>
+      <c r="AF6" s="215"/>
+      <c r="AG6" s="215"/>
+      <c r="AH6" s="215"/>
+      <c r="AI6" s="215"/>
+      <c r="AJ6" s="215"/>
+      <c r="AK6" s="215"/>
+      <c r="AL6" s="215"/>
+      <c r="AM6" s="215"/>
+      <c r="AN6" s="215"/>
+      <c r="AO6" s="215"/>
+      <c r="AP6" s="215"/>
+      <c r="AQ6" s="215"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
+      <c r="AU6" s="175"/>
+      <c r="AV6" s="187"/>
+      <c r="AW6" s="187"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="187"/>
+      <c r="BW6" s="187"/>
+      <c r="CT6" s="187"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="175"/>
-      <c r="B7" s="177" t="s">
+      <c r="A7" s="194"/>
+      <c r="B7" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="177"/>
-      <c r="D7" s="202"/>
-      <c r="E7" s="202"/>
-      <c r="F7" s="202"/>
-      <c r="G7" s="202"/>
-      <c r="H7" s="202"/>
-      <c r="I7" s="202"/>
-      <c r="J7" s="202"/>
-      <c r="K7" s="202"/>
-      <c r="L7" s="203"/>
-      <c r="M7" s="203"/>
-      <c r="N7" s="203"/>
-      <c r="O7" s="203"/>
-      <c r="P7" s="203"/>
-      <c r="Q7" s="203"/>
-      <c r="R7" s="204"/>
-      <c r="S7" s="204"/>
-      <c r="T7" s="204"/>
-      <c r="U7" s="204"/>
-      <c r="V7" s="204"/>
-      <c r="W7" s="206"/>
-      <c r="X7" s="206"/>
-      <c r="Y7" s="206"/>
-      <c r="Z7" s="206"/>
-      <c r="AA7" s="206"/>
-      <c r="AB7" s="210"/>
-      <c r="AC7" s="210"/>
-      <c r="AD7" s="210"/>
-      <c r="AE7" s="210"/>
-      <c r="AF7" s="210"/>
-      <c r="AG7" s="210"/>
-      <c r="AH7" s="210"/>
-      <c r="AI7" s="210"/>
-      <c r="AJ7" s="210"/>
-      <c r="AK7" s="210"/>
-      <c r="AL7" s="210"/>
-      <c r="AM7" s="210"/>
-      <c r="AN7" s="210"/>
-      <c r="AO7" s="210"/>
-      <c r="AP7" s="210"/>
-      <c r="AQ7" s="210"/>
-      <c r="AR7" s="210"/>
-      <c r="AS7" s="210"/>
-      <c r="AT7" s="210"/>
-      <c r="AU7" s="211"/>
-      <c r="AV7" s="176"/>
-      <c r="AW7" s="176"/>
-      <c r="AX7" s="207"/>
-      <c r="AY7" s="206"/>
-      <c r="AZ7" s="206"/>
-      <c r="BA7" s="206"/>
-      <c r="BB7" s="206"/>
-      <c r="BC7" s="206"/>
-      <c r="BD7" s="206"/>
-      <c r="BE7" s="206"/>
-      <c r="BF7" s="200"/>
-      <c r="BG7" s="200"/>
-      <c r="BT7" s="176"/>
-      <c r="BW7" s="176"/>
-      <c r="CT7" s="176"/>
+      <c r="C7" s="195"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="193"/>
+      <c r="K7" s="193"/>
+      <c r="L7" s="186"/>
+      <c r="M7" s="186"/>
+      <c r="N7" s="186"/>
+      <c r="O7" s="186"/>
+      <c r="P7" s="186"/>
+      <c r="Q7" s="186"/>
+      <c r="R7" s="186"/>
+      <c r="S7" s="186"/>
+      <c r="T7" s="186"/>
+      <c r="U7" s="186"/>
+      <c r="V7" s="186"/>
+      <c r="W7" s="213"/>
+      <c r="X7" s="213"/>
+      <c r="Y7" s="213"/>
+      <c r="Z7" s="213"/>
+      <c r="AA7" s="213"/>
+      <c r="AB7" s="215"/>
+      <c r="AC7" s="215"/>
+      <c r="AD7" s="215"/>
+      <c r="AE7" s="215"/>
+      <c r="AF7" s="215"/>
+      <c r="AG7" s="215"/>
+      <c r="AH7" s="215"/>
+      <c r="AI7" s="215"/>
+      <c r="AJ7" s="215"/>
+      <c r="AK7" s="215"/>
+      <c r="AL7" s="215"/>
+      <c r="AM7" s="215"/>
+      <c r="AN7" s="215"/>
+      <c r="AO7" s="215"/>
+      <c r="AP7" s="215"/>
+      <c r="AQ7" s="215"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
+      <c r="AU7" s="176"/>
+      <c r="AV7" s="187"/>
+      <c r="AW7" s="187"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="187"/>
+      <c r="BW7" s="187"/>
+      <c r="CT7" s="187"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="175" t="s">
+      <c r="A8" s="194" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="177" t="s">
+      <c r="B8" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="177"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="202"/>
-      <c r="H8" s="202"/>
-      <c r="I8" s="202"/>
-      <c r="J8" s="202"/>
-      <c r="K8" s="202"/>
-      <c r="L8" s="203"/>
-      <c r="M8" s="203"/>
-      <c r="N8" s="203"/>
-      <c r="O8" s="203"/>
-      <c r="P8" s="203"/>
-      <c r="Q8" s="203"/>
-      <c r="R8" s="204"/>
-      <c r="S8" s="204"/>
-      <c r="T8" s="204"/>
-      <c r="U8" s="204"/>
-      <c r="V8" s="204"/>
-      <c r="W8" s="206"/>
-      <c r="X8" s="206"/>
-      <c r="Y8" s="206"/>
-      <c r="Z8" s="206"/>
-      <c r="AA8" s="206"/>
-      <c r="AB8" s="210"/>
-      <c r="AC8" s="210"/>
-      <c r="AD8" s="210"/>
-      <c r="AE8" s="210"/>
-      <c r="AF8" s="210"/>
-      <c r="AG8" s="210"/>
-      <c r="AH8" s="210"/>
-      <c r="AI8" s="210"/>
-      <c r="AJ8" s="210"/>
-      <c r="AK8" s="210"/>
-      <c r="AL8" s="210"/>
-      <c r="AM8" s="210"/>
-      <c r="AN8" s="210"/>
-      <c r="AO8" s="210"/>
-      <c r="AP8" s="210"/>
-      <c r="AQ8" s="210"/>
-      <c r="AR8" s="210"/>
-      <c r="AS8" s="210"/>
-      <c r="AT8" s="210"/>
-      <c r="AU8" s="211"/>
-      <c r="AV8" s="176"/>
-      <c r="AW8" s="176"/>
-      <c r="AX8" s="207"/>
-      <c r="AY8" s="206"/>
-      <c r="AZ8" s="206"/>
-      <c r="BA8" s="206"/>
-      <c r="BB8" s="206"/>
-      <c r="BC8" s="206"/>
-      <c r="BD8" s="206"/>
-      <c r="BE8" s="206"/>
-      <c r="BF8" s="200"/>
-      <c r="BG8" s="200"/>
-      <c r="BT8" s="176"/>
-      <c r="BW8" s="176"/>
-      <c r="CT8" s="176"/>
+      <c r="C8" s="195"/>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="193"/>
+      <c r="H8" s="193"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="193"/>
+      <c r="K8" s="193"/>
+      <c r="L8" s="186"/>
+      <c r="M8" s="186"/>
+      <c r="N8" s="186"/>
+      <c r="O8" s="186"/>
+      <c r="P8" s="186"/>
+      <c r="Q8" s="186"/>
+      <c r="R8" s="186"/>
+      <c r="S8" s="186"/>
+      <c r="T8" s="186"/>
+      <c r="U8" s="186"/>
+      <c r="V8" s="186"/>
+      <c r="W8" s="213"/>
+      <c r="X8" s="213"/>
+      <c r="Y8" s="213"/>
+      <c r="Z8" s="213"/>
+      <c r="AA8" s="213"/>
+      <c r="AB8" s="215"/>
+      <c r="AC8" s="215"/>
+      <c r="AD8" s="215"/>
+      <c r="AE8" s="215"/>
+      <c r="AF8" s="215"/>
+      <c r="AG8" s="215"/>
+      <c r="AH8" s="215"/>
+      <c r="AI8" s="215"/>
+      <c r="AJ8" s="215"/>
+      <c r="AK8" s="215"/>
+      <c r="AL8" s="215"/>
+      <c r="AM8" s="215"/>
+      <c r="AN8" s="215"/>
+      <c r="AO8" s="215"/>
+      <c r="AP8" s="215"/>
+      <c r="AQ8" s="215"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
+      <c r="AU8" s="176"/>
+      <c r="AV8" s="187"/>
+      <c r="AW8" s="187"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="187"/>
+      <c r="BW8" s="187"/>
+      <c r="CT8" s="187"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="175"/>
-      <c r="B9" s="177" t="s">
+      <c r="A9" s="194"/>
+      <c r="B9" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="177"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="202"/>
-      <c r="H9" s="202"/>
-      <c r="I9" s="202"/>
-      <c r="J9" s="202"/>
-      <c r="K9" s="202"/>
-      <c r="L9" s="203"/>
-      <c r="M9" s="203"/>
-      <c r="N9" s="203"/>
-      <c r="O9" s="203"/>
-      <c r="P9" s="203"/>
-      <c r="Q9" s="203"/>
-      <c r="R9" s="204"/>
-      <c r="S9" s="204"/>
-      <c r="T9" s="204"/>
-      <c r="U9" s="204"/>
-      <c r="V9" s="204"/>
-      <c r="W9" s="206"/>
-      <c r="X9" s="206"/>
-      <c r="Y9" s="206"/>
-      <c r="Z9" s="206"/>
-      <c r="AA9" s="206"/>
-      <c r="AB9" s="210"/>
-      <c r="AC9" s="210"/>
-      <c r="AD9" s="210"/>
-      <c r="AE9" s="210"/>
-      <c r="AF9" s="210"/>
-      <c r="AG9" s="210"/>
-      <c r="AH9" s="210"/>
-      <c r="AI9" s="210"/>
-      <c r="AJ9" s="210"/>
-      <c r="AK9" s="210"/>
-      <c r="AL9" s="210"/>
-      <c r="AM9" s="210"/>
-      <c r="AN9" s="210"/>
-      <c r="AO9" s="210"/>
-      <c r="AP9" s="210"/>
-      <c r="AQ9" s="210"/>
-      <c r="AR9" s="210"/>
-      <c r="AS9" s="210"/>
-      <c r="AT9" s="210"/>
-      <c r="AU9" s="211"/>
-      <c r="AV9" s="176"/>
-      <c r="AW9" s="176"/>
-      <c r="AX9" s="207"/>
-      <c r="AY9" s="206"/>
-      <c r="AZ9" s="206"/>
-      <c r="BA9" s="206"/>
-      <c r="BB9" s="206"/>
-      <c r="BC9" s="206"/>
-      <c r="BD9" s="206"/>
-      <c r="BE9" s="206"/>
-      <c r="BF9" s="200"/>
-      <c r="BG9" s="200"/>
-      <c r="BT9" s="176"/>
-      <c r="BW9" s="176"/>
-      <c r="CT9" s="176"/>
+      <c r="C9" s="195"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="193"/>
+      <c r="L9" s="186"/>
+      <c r="M9" s="186"/>
+      <c r="N9" s="186"/>
+      <c r="O9" s="186"/>
+      <c r="P9" s="186"/>
+      <c r="Q9" s="186"/>
+      <c r="R9" s="186"/>
+      <c r="S9" s="186"/>
+      <c r="T9" s="186"/>
+      <c r="U9" s="186"/>
+      <c r="V9" s="186"/>
+      <c r="W9" s="213"/>
+      <c r="X9" s="213"/>
+      <c r="Y9" s="213"/>
+      <c r="Z9" s="213"/>
+      <c r="AA9" s="213"/>
+      <c r="AB9" s="215"/>
+      <c r="AC9" s="215"/>
+      <c r="AD9" s="215"/>
+      <c r="AE9" s="215"/>
+      <c r="AF9" s="215"/>
+      <c r="AG9" s="215"/>
+      <c r="AH9" s="215"/>
+      <c r="AI9" s="215"/>
+      <c r="AJ9" s="215"/>
+      <c r="AK9" s="215"/>
+      <c r="AL9" s="215"/>
+      <c r="AM9" s="215"/>
+      <c r="AN9" s="215"/>
+      <c r="AO9" s="215"/>
+      <c r="AP9" s="215"/>
+      <c r="AQ9" s="215"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
+      <c r="AU9" s="176"/>
+      <c r="AV9" s="187"/>
+      <c r="AW9" s="187"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="187"/>
+      <c r="BW9" s="187"/>
+      <c r="CT9" s="187"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="175"/>
-      <c r="B10" s="177" t="s">
+      <c r="A10" s="194"/>
+      <c r="B10" s="195" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="177"/>
-      <c r="D10" s="202"/>
-      <c r="E10" s="202"/>
-      <c r="F10" s="202"/>
-      <c r="G10" s="202"/>
-      <c r="H10" s="202"/>
-      <c r="I10" s="202"/>
-      <c r="J10" s="202"/>
-      <c r="K10" s="202"/>
-      <c r="L10" s="203"/>
-      <c r="M10" s="203"/>
-      <c r="N10" s="203"/>
-      <c r="O10" s="203"/>
-      <c r="P10" s="203"/>
-      <c r="Q10" s="203"/>
-      <c r="R10" s="204"/>
-      <c r="S10" s="204"/>
-      <c r="T10" s="204"/>
-      <c r="U10" s="204"/>
-      <c r="V10" s="204"/>
-      <c r="W10" s="206"/>
-      <c r="X10" s="206"/>
-      <c r="Y10" s="206"/>
-      <c r="Z10" s="206"/>
-      <c r="AA10" s="206"/>
-      <c r="AB10" s="210"/>
-      <c r="AC10" s="210"/>
-      <c r="AD10" s="210"/>
-      <c r="AE10" s="210"/>
-      <c r="AF10" s="210"/>
-      <c r="AG10" s="210"/>
-      <c r="AH10" s="210"/>
-      <c r="AI10" s="210"/>
-      <c r="AJ10" s="210"/>
-      <c r="AK10" s="210"/>
-      <c r="AL10" s="210"/>
-      <c r="AM10" s="210"/>
-      <c r="AN10" s="210"/>
-      <c r="AO10" s="210"/>
-      <c r="AP10" s="210"/>
-      <c r="AQ10" s="210"/>
-      <c r="AR10" s="210"/>
-      <c r="AS10" s="210"/>
-      <c r="AT10" s="210"/>
-      <c r="AU10" s="211"/>
-      <c r="AV10" s="176"/>
-      <c r="AW10" s="176"/>
-      <c r="AX10" s="207"/>
-      <c r="AY10" s="206"/>
-      <c r="AZ10" s="206"/>
-      <c r="BA10" s="206"/>
-      <c r="BB10" s="206"/>
-      <c r="BC10" s="206"/>
-      <c r="BD10" s="206"/>
-      <c r="BE10" s="206"/>
-      <c r="BF10" s="200"/>
-      <c r="BG10" s="200"/>
-      <c r="BT10" s="176"/>
-      <c r="BW10" s="176"/>
-      <c r="CT10" s="176"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="193"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="193"/>
+      <c r="G10" s="193"/>
+      <c r="H10" s="193"/>
+      <c r="I10" s="193"/>
+      <c r="J10" s="193"/>
+      <c r="K10" s="193"/>
+      <c r="L10" s="186"/>
+      <c r="M10" s="186"/>
+      <c r="N10" s="186"/>
+      <c r="O10" s="186"/>
+      <c r="P10" s="186"/>
+      <c r="Q10" s="186"/>
+      <c r="R10" s="186"/>
+      <c r="S10" s="186"/>
+      <c r="T10" s="186"/>
+      <c r="U10" s="186"/>
+      <c r="V10" s="186"/>
+      <c r="W10" s="213"/>
+      <c r="X10" s="213"/>
+      <c r="Y10" s="213"/>
+      <c r="Z10" s="213"/>
+      <c r="AA10" s="213"/>
+      <c r="AB10" s="215"/>
+      <c r="AC10" s="215"/>
+      <c r="AD10" s="215"/>
+      <c r="AE10" s="215"/>
+      <c r="AF10" s="215"/>
+      <c r="AG10" s="215"/>
+      <c r="AH10" s="215"/>
+      <c r="AI10" s="215"/>
+      <c r="AJ10" s="215"/>
+      <c r="AK10" s="215"/>
+      <c r="AL10" s="215"/>
+      <c r="AM10" s="215"/>
+      <c r="AN10" s="215"/>
+      <c r="AO10" s="215"/>
+      <c r="AP10" s="215"/>
+      <c r="AQ10" s="215"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
+      <c r="AU10" s="176"/>
+      <c r="AV10" s="187"/>
+      <c r="AW10" s="187"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="187"/>
+      <c r="BW10" s="187"/>
+      <c r="CT10" s="187"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="175"/>
-      <c r="B11" s="177" t="s">
+      <c r="A11" s="194"/>
+      <c r="B11" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="177"/>
-      <c r="D11" s="202"/>
-      <c r="E11" s="202"/>
-      <c r="F11" s="202"/>
-      <c r="G11" s="202"/>
-      <c r="H11" s="202"/>
-      <c r="I11" s="202"/>
-      <c r="J11" s="202"/>
-      <c r="K11" s="202"/>
-      <c r="L11" s="203"/>
-      <c r="M11" s="203"/>
-      <c r="N11" s="203"/>
-      <c r="O11" s="203"/>
-      <c r="P11" s="203"/>
-      <c r="Q11" s="203"/>
-      <c r="R11" s="204"/>
-      <c r="S11" s="204"/>
-      <c r="T11" s="204"/>
-      <c r="U11" s="204"/>
-      <c r="V11" s="204"/>
-      <c r="W11" s="206"/>
-      <c r="X11" s="206"/>
-      <c r="Y11" s="206"/>
-      <c r="Z11" s="206"/>
-      <c r="AA11" s="206"/>
-      <c r="AB11" s="212"/>
-      <c r="AC11" s="212"/>
-      <c r="AD11" s="212"/>
-      <c r="AE11" s="212"/>
-      <c r="AF11" s="212"/>
-      <c r="AG11" s="212"/>
-      <c r="AH11" s="212"/>
-      <c r="AI11" s="212"/>
-      <c r="AJ11" s="212"/>
-      <c r="AK11" s="212"/>
-      <c r="AL11" s="212"/>
-      <c r="AM11" s="212"/>
-      <c r="AN11" s="212"/>
-      <c r="AO11" s="212"/>
-      <c r="AP11" s="212"/>
-      <c r="AQ11" s="212"/>
-      <c r="AR11" s="212"/>
-      <c r="AS11" s="212"/>
-      <c r="AT11" s="212"/>
-      <c r="AU11" s="211"/>
-      <c r="AV11" s="176"/>
-      <c r="AW11" s="176"/>
-      <c r="AX11" s="207"/>
-      <c r="AY11" s="206"/>
-      <c r="AZ11" s="206"/>
-      <c r="BA11" s="206"/>
-      <c r="BB11" s="206"/>
-      <c r="BC11" s="206"/>
-      <c r="BD11" s="206"/>
-      <c r="BE11" s="206"/>
-      <c r="BF11" s="200"/>
-      <c r="BG11" s="200"/>
-      <c r="BT11" s="176"/>
-      <c r="BW11" s="176"/>
-      <c r="CT11" s="176"/>
+      <c r="C11" s="195"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="193"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="193"/>
+      <c r="I11" s="193"/>
+      <c r="J11" s="193"/>
+      <c r="K11" s="193"/>
+      <c r="L11" s="186"/>
+      <c r="M11" s="186"/>
+      <c r="N11" s="186"/>
+      <c r="O11" s="186"/>
+      <c r="P11" s="186"/>
+      <c r="Q11" s="186"/>
+      <c r="R11" s="186"/>
+      <c r="S11" s="186"/>
+      <c r="T11" s="186"/>
+      <c r="U11" s="186"/>
+      <c r="V11" s="186"/>
+      <c r="W11" s="213"/>
+      <c r="X11" s="213"/>
+      <c r="Y11" s="213"/>
+      <c r="Z11" s="213"/>
+      <c r="AA11" s="213"/>
+      <c r="AB11" s="216"/>
+      <c r="AC11" s="216"/>
+      <c r="AD11" s="216"/>
+      <c r="AE11" s="216"/>
+      <c r="AF11" s="216"/>
+      <c r="AG11" s="216"/>
+      <c r="AH11" s="216"/>
+      <c r="AI11" s="216"/>
+      <c r="AJ11" s="216"/>
+      <c r="AK11" s="216"/>
+      <c r="AL11" s="216"/>
+      <c r="AM11" s="216"/>
+      <c r="AN11" s="216"/>
+      <c r="AO11" s="216"/>
+      <c r="AP11" s="216"/>
+      <c r="AQ11" s="216"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
+      <c r="AU11" s="176"/>
+      <c r="AV11" s="187"/>
+      <c r="AW11" s="187"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="187"/>
+      <c r="BW11" s="187"/>
+      <c r="CT11" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4110,22 +4099,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5647,13 +5661,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="195" t="s">
+      <c r="A4" s="198" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="197"/>
+      <c r="C4" s="201"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5758,9 +5772,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="184"/>
-      <c r="B5" s="194"/>
-      <c r="C5" s="184"/>
+      <c r="A5" s="199"/>
+      <c r="B5" s="197"/>
+      <c r="C5" s="199"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5865,11 +5879,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="184"/>
+      <c r="A6" s="199"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="184"/>
+      <c r="C6" s="199"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -5974,11 +5988,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="184"/>
+      <c r="A7" s="199"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="184"/>
+      <c r="C7" s="199"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6083,11 +6097,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="184"/>
+      <c r="A8" s="199"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="184"/>
+      <c r="C8" s="199"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6192,11 +6206,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="184"/>
+      <c r="A9" s="199"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="184"/>
+      <c r="C9" s="199"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6301,11 +6315,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="184"/>
+      <c r="A10" s="199"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="184"/>
+      <c r="C10" s="199"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6410,11 +6424,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="184"/>
+      <c r="A11" s="199"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="184"/>
+      <c r="C11" s="199"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6519,9 +6533,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="184"/>
+      <c r="A12" s="199"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="185"/>
+      <c r="C12" s="202"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6626,10 +6640,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="198" t="s">
+      <c r="A13" s="203" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="199" t="s">
+      <c r="B13" s="204" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6738,8 +6752,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="184"/>
-      <c r="B14" s="190"/>
+      <c r="A14" s="199"/>
+      <c r="B14" s="205"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6860,7 +6874,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="184"/>
+      <c r="A15" s="199"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -6970,7 +6984,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="184"/>
+      <c r="A16" s="199"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7080,7 +7094,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="184"/>
+      <c r="A17" s="199"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7192,7 +7206,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="184"/>
+      <c r="A18" s="199"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7302,7 +7316,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="184"/>
+      <c r="A19" s="199"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7412,7 +7426,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="184"/>
+      <c r="A20" s="199"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7522,7 +7536,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="185"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7633,7 +7647,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="93"/>
-      <c r="B22" s="193" t="s">
+      <c r="B22" s="196" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7743,7 +7757,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="93"/>
-      <c r="B23" s="194"/>
+      <c r="B23" s="197"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7850,13 +7864,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="186" t="s">
+      <c r="A24" s="207" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="188">
+      <c r="C24" s="209">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -7964,11 +7978,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="187"/>
+      <c r="A25" s="208"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="184"/>
+      <c r="C25" s="199"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8074,11 +8088,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="187"/>
+      <c r="A26" s="208"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="184"/>
+      <c r="C26" s="199"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8184,11 +8198,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="187"/>
+      <c r="A27" s="208"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="184"/>
+      <c r="C27" s="199"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8294,11 +8308,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="187"/>
+      <c r="A28" s="208"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="184"/>
+      <c r="C28" s="199"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8404,11 +8418,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="187"/>
+      <c r="A29" s="208"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="184"/>
+      <c r="C29" s="199"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8514,11 +8528,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="187"/>
+      <c r="A30" s="208"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="184"/>
+      <c r="C30" s="199"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8624,11 +8638,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="187"/>
+      <c r="A31" s="208"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="184"/>
+      <c r="C31" s="199"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8734,11 +8748,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="187"/>
+      <c r="A32" s="208"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="184"/>
+      <c r="C32" s="199"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8844,11 +8858,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="187"/>
+      <c r="A33" s="208"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="184"/>
+      <c r="C33" s="199"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -8954,11 +8968,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="187"/>
+      <c r="A34" s="208"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="184"/>
+      <c r="C34" s="199"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9064,11 +9078,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="187"/>
+      <c r="A35" s="208"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="185"/>
+      <c r="C35" s="202"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9174,11 +9188,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="187"/>
+      <c r="A36" s="208"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="188">
+      <c r="C36" s="209">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9286,11 +9300,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="187"/>
+      <c r="A37" s="208"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="184"/>
+      <c r="C37" s="199"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9396,11 +9410,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="187"/>
+      <c r="A38" s="208"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="184"/>
+      <c r="C38" s="199"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9506,11 +9520,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="187"/>
+      <c r="A39" s="208"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="184"/>
+      <c r="C39" s="199"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9616,11 +9630,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="187"/>
+      <c r="A40" s="208"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="184"/>
+      <c r="C40" s="199"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9726,11 +9740,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="187"/>
+      <c r="A41" s="208"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="184"/>
+      <c r="C41" s="199"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9836,11 +9850,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="187"/>
+      <c r="A42" s="208"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="184"/>
+      <c r="C42" s="199"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -9946,11 +9960,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="187"/>
+      <c r="A43" s="208"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="184"/>
+      <c r="C43" s="199"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10056,11 +10070,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="187"/>
+      <c r="A44" s="208"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="184"/>
+      <c r="C44" s="199"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10166,11 +10180,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="187"/>
+      <c r="A45" s="208"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="184"/>
+      <c r="C45" s="199"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10276,11 +10290,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="187"/>
+      <c r="A46" s="208"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="184"/>
+      <c r="C46" s="199"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10386,11 +10400,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="187"/>
+      <c r="A47" s="208"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="184"/>
+      <c r="C47" s="199"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10504,11 +10518,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="187"/>
+      <c r="A48" s="208"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="184"/>
+      <c r="C48" s="199"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10617,7 +10631,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="111"/>
-      <c r="B49" s="189" t="s">
+      <c r="B49" s="210" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10727,7 +10741,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="116"/>
-      <c r="B50" s="190"/>
+      <c r="B50" s="205"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14158,7 +14172,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="191" t="s">
+      <c r="A81" s="211" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14270,7 +14284,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="184"/>
+      <c r="A82" s="199"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14380,7 +14394,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="184"/>
+      <c r="A83" s="199"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14490,7 +14504,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="184"/>
+      <c r="A84" s="199"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14600,7 +14614,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="184"/>
+      <c r="A85" s="199"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14710,7 +14724,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="184"/>
+      <c r="A86" s="199"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14820,7 +14834,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="184"/>
+      <c r="A87" s="199"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -14932,7 +14946,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="184"/>
+      <c r="A88" s="199"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15042,7 +15056,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="184"/>
+      <c r="A89" s="199"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15152,7 +15166,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="184"/>
+      <c r="A90" s="199"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15262,11 +15276,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="184"/>
+      <c r="A91" s="199"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="192"/>
+      <c r="C91" s="212"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15372,11 +15386,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="184"/>
+      <c r="A92" s="199"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="184"/>
+      <c r="C92" s="199"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15482,11 +15496,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="185"/>
+      <c r="A93" s="202"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="184"/>
+      <c r="C93" s="199"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15710,7 +15724,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="183" t="s">
+      <c r="A95" s="206" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15822,7 +15836,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="184"/>
+      <c r="A96" s="199"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -15932,7 +15946,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="184"/>
+      <c r="A97" s="199"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16042,7 +16056,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="184"/>
+      <c r="A98" s="199"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16152,7 +16166,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="184"/>
+      <c r="A99" s="199"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16262,7 +16276,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="184"/>
+      <c r="A100" s="199"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16372,7 +16386,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="184"/>
+      <c r="A101" s="199"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16482,7 +16496,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="184"/>
+      <c r="A102" s="199"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16592,7 +16606,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="184"/>
+      <c r="A103" s="199"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16704,7 +16718,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="184"/>
+      <c r="A104" s="199"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16814,7 +16828,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="184"/>
+      <c r="A105" s="199"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -16932,7 +16946,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="184"/>
+      <c r="A106" s="199"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17042,7 +17056,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="184"/>
+      <c r="A107" s="199"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17152,7 +17166,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="184"/>
+      <c r="A108" s="199"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17262,7 +17276,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="184"/>
+      <c r="A109" s="199"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17372,7 +17386,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="184"/>
+      <c r="A110" s="199"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17482,7 +17496,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="184"/>
+      <c r="A111" s="199"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17592,7 +17606,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="184"/>
+      <c r="A112" s="199"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17702,7 +17716,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="184"/>
+      <c r="A113" s="199"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17812,7 +17826,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="184"/>
+      <c r="A114" s="199"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17922,7 +17936,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="184"/>
+      <c r="A115" s="199"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18032,7 +18046,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="184"/>
+      <c r="A116" s="199"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18158,7 +18172,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="184"/>
+      <c r="A117" s="199"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18268,7 +18282,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="185"/>
+      <c r="A118" s="202"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25639,12 +25653,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25652,6 +25660,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 03, 04 e 05-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5393897D-8FE6-4533-B985-078F570484C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C514EA69-CA2C-4FB4-B0FE-6BD553AFC3FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="160">
   <si>
     <t>S</t>
   </si>
@@ -671,6 +671,16 @@
   </si>
   <si>
     <t>Criação da página de cadastro de categorias do projeto Gufos</t>
+  </si>
+  <si>
+    <t>Criação da página de login do projeto Gufos</t>
+  </si>
+  <si>
+    <t>Criação da página home do projeto Gufos.
+Início da página home dos projetos para a empresa Linx</t>
+  </si>
+  <si>
+    <t>Criação de 3 telas para os projetos da empresa Linx</t>
   </si>
 </sst>
 </file>
@@ -2182,14 +2192,47 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2206,61 +2249,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2271,22 +2273,30 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2793,10 +2803,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R4" sqref="R4:R11"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -3105,110 +3115,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="188" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="188"/>
-      <c r="K2" s="188"/>
-      <c r="L2" s="188"/>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="188"/>
-      <c r="P2" s="188"/>
-      <c r="Q2" s="188"/>
-      <c r="R2" s="188" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="188"/>
-      <c r="T2" s="188"/>
-      <c r="U2" s="188"/>
-      <c r="V2" s="188"/>
-      <c r="W2" s="188"/>
-      <c r="X2" s="188"/>
-      <c r="Y2" s="188"/>
-      <c r="Z2" s="188"/>
-      <c r="AA2" s="188"/>
-      <c r="AB2" s="188"/>
-      <c r="AC2" s="188"/>
-      <c r="AD2" s="188"/>
-      <c r="AE2" s="188"/>
-      <c r="AF2" s="188"/>
-      <c r="AG2" s="188"/>
-      <c r="AH2" s="188"/>
-      <c r="AI2" s="188"/>
-      <c r="AJ2" s="188"/>
-      <c r="AK2" s="188"/>
-      <c r="AL2" s="188"/>
-      <c r="AM2" s="188" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="188"/>
-      <c r="AO2" s="188"/>
-      <c r="AP2" s="188"/>
-      <c r="AQ2" s="188"/>
-      <c r="AR2" s="188"/>
-      <c r="AS2" s="188"/>
-      <c r="AT2" s="188"/>
-      <c r="AU2" s="188"/>
-      <c r="AV2" s="188"/>
-      <c r="AW2" s="188"/>
-      <c r="AX2" s="189"/>
-      <c r="AY2" s="189"/>
-      <c r="AZ2" s="189"/>
-      <c r="BA2" s="189"/>
-      <c r="BB2" s="189"/>
-      <c r="BC2" s="189"/>
-      <c r="BD2" s="189"/>
-      <c r="BE2" s="189"/>
-      <c r="BF2" s="189"/>
-      <c r="BG2" s="189"/>
-      <c r="BH2" s="189"/>
-      <c r="BI2" s="189"/>
-      <c r="BJ2" s="188" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="188"/>
-      <c r="BL2" s="188"/>
-      <c r="BM2" s="188"/>
-      <c r="BN2" s="188"/>
-      <c r="BO2" s="188"/>
-      <c r="BP2" s="188"/>
-      <c r="BQ2" s="188"/>
-      <c r="BR2" s="188"/>
-      <c r="BS2" s="188"/>
-      <c r="BT2" s="188"/>
-      <c r="BU2" s="188"/>
-      <c r="BV2" s="188"/>
-      <c r="BW2" s="188"/>
-      <c r="BX2" s="190"/>
-      <c r="BY2" s="190"/>
-      <c r="BZ2" s="190"/>
-      <c r="CA2" s="190"/>
-      <c r="CB2" s="190"/>
-      <c r="CC2" s="190"/>
-      <c r="CD2" s="190"/>
-      <c r="CE2" s="191" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="192"/>
-      <c r="CG2" s="192"/>
-      <c r="CH2" s="192"/>
-      <c r="CI2" s="192"/>
-      <c r="CJ2" s="192"/>
-      <c r="CK2" s="192"/>
-      <c r="CL2" s="192"/>
-      <c r="CM2" s="192"/>
-      <c r="CN2" s="192"/>
-      <c r="CO2" s="192"/>
-      <c r="CP2" s="192"/>
-      <c r="CQ2" s="192"/>
-      <c r="CR2" s="192"/>
-      <c r="CS2" s="192"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3504,569 +3514,632 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="194" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="195"/>
-      <c r="D4" s="193" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="193" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="193" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="193" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="193" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="193" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="193" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="193" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="186" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="186" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="186" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="186" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="186" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="186" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="186" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="186"/>
-      <c r="T4" s="186"/>
-      <c r="U4" s="186"/>
-      <c r="V4" s="186"/>
-      <c r="W4" s="213"/>
-      <c r="X4" s="213"/>
-      <c r="Y4" s="213"/>
-      <c r="Z4" s="213"/>
-      <c r="AA4" s="213"/>
-      <c r="AB4" s="214"/>
-      <c r="AC4" s="214"/>
-      <c r="AD4" s="214"/>
-      <c r="AE4" s="214"/>
-      <c r="AF4" s="214"/>
-      <c r="AG4" s="214"/>
-      <c r="AH4" s="214"/>
-      <c r="AI4" s="214"/>
-      <c r="AJ4" s="214"/>
-      <c r="AK4" s="214"/>
-      <c r="AL4" s="214"/>
-      <c r="AM4" s="214"/>
-      <c r="AN4" s="214"/>
-      <c r="AO4" s="214"/>
-      <c r="AP4" s="214"/>
-      <c r="AQ4" s="214"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="S4" s="187" t="s">
+        <v>157</v>
+      </c>
+      <c r="T4" s="187" t="s">
+        <v>158</v>
+      </c>
+      <c r="U4" s="187" t="s">
+        <v>159</v>
+      </c>
+      <c r="V4" s="187"/>
+      <c r="W4" s="188"/>
+      <c r="X4" s="188"/>
+      <c r="Y4" s="188"/>
+      <c r="Z4" s="188"/>
+      <c r="AA4" s="188"/>
+      <c r="AB4" s="189"/>
+      <c r="AC4" s="189"/>
+      <c r="AD4" s="189"/>
+      <c r="AE4" s="189"/>
+      <c r="AF4" s="189"/>
+      <c r="AG4" s="189"/>
+      <c r="AH4" s="189"/>
+      <c r="AI4" s="189"/>
+      <c r="AJ4" s="189"/>
+      <c r="AK4" s="189"/>
+      <c r="AL4" s="189"/>
+      <c r="AM4" s="189"/>
+      <c r="AN4" s="189"/>
+      <c r="AO4" s="189"/>
+      <c r="AP4" s="189"/>
+      <c r="AQ4" s="189"/>
+      <c r="AR4" s="192"/>
+      <c r="AS4" s="192"/>
+      <c r="AT4" s="192"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="187"/>
-      <c r="AW4" s="187"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="187"/>
-      <c r="BW4" s="187"/>
-      <c r="CT4" s="187"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="195"/>
+      <c r="AY4" s="197"/>
+      <c r="AZ4" s="197"/>
+      <c r="BA4" s="197"/>
+      <c r="BB4" s="197"/>
+      <c r="BC4" s="197"/>
+      <c r="BD4" s="197"/>
+      <c r="BE4" s="197"/>
+      <c r="BF4" s="198"/>
+      <c r="BG4" s="198"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="194"/>
-      <c r="B5" s="195" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="195"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="193"/>
-      <c r="I5" s="193"/>
-      <c r="J5" s="193"/>
-      <c r="K5" s="193"/>
-      <c r="L5" s="186"/>
-      <c r="M5" s="186"/>
-      <c r="N5" s="186"/>
-      <c r="O5" s="186"/>
-      <c r="P5" s="186"/>
-      <c r="Q5" s="186"/>
-      <c r="R5" s="186"/>
-      <c r="S5" s="186"/>
-      <c r="T5" s="186"/>
-      <c r="U5" s="186"/>
-      <c r="V5" s="186"/>
-      <c r="W5" s="213"/>
-      <c r="X5" s="213"/>
-      <c r="Y5" s="213"/>
-      <c r="Z5" s="213"/>
-      <c r="AA5" s="213"/>
-      <c r="AB5" s="215"/>
-      <c r="AC5" s="215"/>
-      <c r="AD5" s="215"/>
-      <c r="AE5" s="215"/>
-      <c r="AF5" s="215"/>
-      <c r="AG5" s="215"/>
-      <c r="AH5" s="215"/>
-      <c r="AI5" s="215"/>
-      <c r="AJ5" s="215"/>
-      <c r="AK5" s="215"/>
-      <c r="AL5" s="215"/>
-      <c r="AM5" s="215"/>
-      <c r="AN5" s="215"/>
-      <c r="AO5" s="215"/>
-      <c r="AP5" s="215"/>
-      <c r="AQ5" s="215"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="190"/>
+      <c r="AC5" s="190"/>
+      <c r="AD5" s="190"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="190"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="190"/>
+      <c r="AK5" s="190"/>
+      <c r="AL5" s="190"/>
+      <c r="AM5" s="190"/>
+      <c r="AN5" s="190"/>
+      <c r="AO5" s="190"/>
+      <c r="AP5" s="190"/>
+      <c r="AQ5" s="190"/>
+      <c r="AR5" s="193"/>
+      <c r="AS5" s="193"/>
+      <c r="AT5" s="193"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="187"/>
-      <c r="AW5" s="187"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="187"/>
-      <c r="BW5" s="187"/>
-      <c r="CT5" s="187"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="196"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="197"/>
+      <c r="BA5" s="197"/>
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="199"/>
+      <c r="BG5" s="199"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="194"/>
-      <c r="B6" s="195" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="195"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="193"/>
-      <c r="J6" s="193"/>
-      <c r="K6" s="193"/>
-      <c r="L6" s="186"/>
-      <c r="M6" s="186"/>
-      <c r="N6" s="186"/>
-      <c r="O6" s="186"/>
-      <c r="P6" s="186"/>
-      <c r="Q6" s="186"/>
-      <c r="R6" s="186"/>
-      <c r="S6" s="186"/>
-      <c r="T6" s="186"/>
-      <c r="U6" s="186"/>
-      <c r="V6" s="186"/>
-      <c r="W6" s="213"/>
-      <c r="X6" s="213"/>
-      <c r="Y6" s="213"/>
-      <c r="Z6" s="213"/>
-      <c r="AA6" s="213"/>
-      <c r="AB6" s="215"/>
-      <c r="AC6" s="215"/>
-      <c r="AD6" s="215"/>
-      <c r="AE6" s="215"/>
-      <c r="AF6" s="215"/>
-      <c r="AG6" s="215"/>
-      <c r="AH6" s="215"/>
-      <c r="AI6" s="215"/>
-      <c r="AJ6" s="215"/>
-      <c r="AK6" s="215"/>
-      <c r="AL6" s="215"/>
-      <c r="AM6" s="215"/>
-      <c r="AN6" s="215"/>
-      <c r="AO6" s="215"/>
-      <c r="AP6" s="215"/>
-      <c r="AQ6" s="215"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
+      <c r="AB6" s="190"/>
+      <c r="AC6" s="190"/>
+      <c r="AD6" s="190"/>
+      <c r="AE6" s="190"/>
+      <c r="AF6" s="190"/>
+      <c r="AG6" s="190"/>
+      <c r="AH6" s="190"/>
+      <c r="AI6" s="190"/>
+      <c r="AJ6" s="190"/>
+      <c r="AK6" s="190"/>
+      <c r="AL6" s="190"/>
+      <c r="AM6" s="190"/>
+      <c r="AN6" s="190"/>
+      <c r="AO6" s="190"/>
+      <c r="AP6" s="190"/>
+      <c r="AQ6" s="190"/>
+      <c r="AR6" s="193"/>
+      <c r="AS6" s="193"/>
+      <c r="AT6" s="193"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="187"/>
-      <c r="AW6" s="187"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="187"/>
-      <c r="BW6" s="187"/>
-      <c r="CT6" s="187"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="199"/>
+      <c r="BG6" s="199"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="194"/>
-      <c r="B7" s="195" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="193"/>
-      <c r="E7" s="193"/>
-      <c r="F7" s="193"/>
-      <c r="G7" s="193"/>
-      <c r="H7" s="193"/>
-      <c r="I7" s="193"/>
-      <c r="J7" s="193"/>
-      <c r="K7" s="193"/>
-      <c r="L7" s="186"/>
-      <c r="M7" s="186"/>
-      <c r="N7" s="186"/>
-      <c r="O7" s="186"/>
-      <c r="P7" s="186"/>
-      <c r="Q7" s="186"/>
-      <c r="R7" s="186"/>
-      <c r="S7" s="186"/>
-      <c r="T7" s="186"/>
-      <c r="U7" s="186"/>
-      <c r="V7" s="186"/>
-      <c r="W7" s="213"/>
-      <c r="X7" s="213"/>
-      <c r="Y7" s="213"/>
-      <c r="Z7" s="213"/>
-      <c r="AA7" s="213"/>
-      <c r="AB7" s="215"/>
-      <c r="AC7" s="215"/>
-      <c r="AD7" s="215"/>
-      <c r="AE7" s="215"/>
-      <c r="AF7" s="215"/>
-      <c r="AG7" s="215"/>
-      <c r="AH7" s="215"/>
-      <c r="AI7" s="215"/>
-      <c r="AJ7" s="215"/>
-      <c r="AK7" s="215"/>
-      <c r="AL7" s="215"/>
-      <c r="AM7" s="215"/>
-      <c r="AN7" s="215"/>
-      <c r="AO7" s="215"/>
-      <c r="AP7" s="215"/>
-      <c r="AQ7" s="215"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
+      <c r="AB7" s="190"/>
+      <c r="AC7" s="190"/>
+      <c r="AD7" s="190"/>
+      <c r="AE7" s="190"/>
+      <c r="AF7" s="190"/>
+      <c r="AG7" s="190"/>
+      <c r="AH7" s="190"/>
+      <c r="AI7" s="190"/>
+      <c r="AJ7" s="190"/>
+      <c r="AK7" s="190"/>
+      <c r="AL7" s="190"/>
+      <c r="AM7" s="190"/>
+      <c r="AN7" s="190"/>
+      <c r="AO7" s="190"/>
+      <c r="AP7" s="190"/>
+      <c r="AQ7" s="190"/>
+      <c r="AR7" s="193"/>
+      <c r="AS7" s="193"/>
+      <c r="AT7" s="193"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="187"/>
-      <c r="AW7" s="187"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="187"/>
-      <c r="BW7" s="187"/>
-      <c r="CT7" s="187"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="196"/>
+      <c r="AY7" s="197"/>
+      <c r="AZ7" s="197"/>
+      <c r="BA7" s="197"/>
+      <c r="BB7" s="197"/>
+      <c r="BC7" s="197"/>
+      <c r="BD7" s="197"/>
+      <c r="BE7" s="197"/>
+      <c r="BF7" s="199"/>
+      <c r="BG7" s="199"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="194" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="195"/>
-      <c r="D8" s="193"/>
-      <c r="E8" s="193"/>
-      <c r="F8" s="193"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="193"/>
-      <c r="I8" s="193"/>
-      <c r="J8" s="193"/>
-      <c r="K8" s="193"/>
-      <c r="L8" s="186"/>
-      <c r="M8" s="186"/>
-      <c r="N8" s="186"/>
-      <c r="O8" s="186"/>
-      <c r="P8" s="186"/>
-      <c r="Q8" s="186"/>
-      <c r="R8" s="186"/>
-      <c r="S8" s="186"/>
-      <c r="T8" s="186"/>
-      <c r="U8" s="186"/>
-      <c r="V8" s="186"/>
-      <c r="W8" s="213"/>
-      <c r="X8" s="213"/>
-      <c r="Y8" s="213"/>
-      <c r="Z8" s="213"/>
-      <c r="AA8" s="213"/>
-      <c r="AB8" s="215"/>
-      <c r="AC8" s="215"/>
-      <c r="AD8" s="215"/>
-      <c r="AE8" s="215"/>
-      <c r="AF8" s="215"/>
-      <c r="AG8" s="215"/>
-      <c r="AH8" s="215"/>
-      <c r="AI8" s="215"/>
-      <c r="AJ8" s="215"/>
-      <c r="AK8" s="215"/>
-      <c r="AL8" s="215"/>
-      <c r="AM8" s="215"/>
-      <c r="AN8" s="215"/>
-      <c r="AO8" s="215"/>
-      <c r="AP8" s="215"/>
-      <c r="AQ8" s="215"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
+      <c r="AB8" s="190"/>
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="190"/>
+      <c r="AG8" s="190"/>
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="190"/>
+      <c r="AL8" s="190"/>
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="190"/>
+      <c r="AQ8" s="190"/>
+      <c r="AR8" s="193"/>
+      <c r="AS8" s="193"/>
+      <c r="AT8" s="193"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="187"/>
-      <c r="AW8" s="187"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="187"/>
-      <c r="BW8" s="187"/>
-      <c r="CT8" s="187"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="196"/>
+      <c r="AY8" s="197"/>
+      <c r="AZ8" s="197"/>
+      <c r="BA8" s="197"/>
+      <c r="BB8" s="197"/>
+      <c r="BC8" s="197"/>
+      <c r="BD8" s="197"/>
+      <c r="BE8" s="197"/>
+      <c r="BF8" s="199"/>
+      <c r="BG8" s="199"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="194"/>
-      <c r="B9" s="195" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="195"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="193"/>
-      <c r="K9" s="193"/>
-      <c r="L9" s="186"/>
-      <c r="M9" s="186"/>
-      <c r="N9" s="186"/>
-      <c r="O9" s="186"/>
-      <c r="P9" s="186"/>
-      <c r="Q9" s="186"/>
-      <c r="R9" s="186"/>
-      <c r="S9" s="186"/>
-      <c r="T9" s="186"/>
-      <c r="U9" s="186"/>
-      <c r="V9" s="186"/>
-      <c r="W9" s="213"/>
-      <c r="X9" s="213"/>
-      <c r="Y9" s="213"/>
-      <c r="Z9" s="213"/>
-      <c r="AA9" s="213"/>
-      <c r="AB9" s="215"/>
-      <c r="AC9" s="215"/>
-      <c r="AD9" s="215"/>
-      <c r="AE9" s="215"/>
-      <c r="AF9" s="215"/>
-      <c r="AG9" s="215"/>
-      <c r="AH9" s="215"/>
-      <c r="AI9" s="215"/>
-      <c r="AJ9" s="215"/>
-      <c r="AK9" s="215"/>
-      <c r="AL9" s="215"/>
-      <c r="AM9" s="215"/>
-      <c r="AN9" s="215"/>
-      <c r="AO9" s="215"/>
-      <c r="AP9" s="215"/>
-      <c r="AQ9" s="215"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="190"/>
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="190"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="190"/>
+      <c r="AL9" s="190"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="190"/>
+      <c r="AR9" s="193"/>
+      <c r="AS9" s="193"/>
+      <c r="AT9" s="193"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="187"/>
-      <c r="AW9" s="187"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="187"/>
-      <c r="BW9" s="187"/>
-      <c r="CT9" s="187"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="196"/>
+      <c r="AY9" s="197"/>
+      <c r="AZ9" s="197"/>
+      <c r="BA9" s="197"/>
+      <c r="BB9" s="197"/>
+      <c r="BC9" s="197"/>
+      <c r="BD9" s="197"/>
+      <c r="BE9" s="197"/>
+      <c r="BF9" s="199"/>
+      <c r="BG9" s="199"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="194"/>
-      <c r="B10" s="195" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="195"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="193"/>
-      <c r="J10" s="193"/>
-      <c r="K10" s="193"/>
-      <c r="L10" s="186"/>
-      <c r="M10" s="186"/>
-      <c r="N10" s="186"/>
-      <c r="O10" s="186"/>
-      <c r="P10" s="186"/>
-      <c r="Q10" s="186"/>
-      <c r="R10" s="186"/>
-      <c r="S10" s="186"/>
-      <c r="T10" s="186"/>
-      <c r="U10" s="186"/>
-      <c r="V10" s="186"/>
-      <c r="W10" s="213"/>
-      <c r="X10" s="213"/>
-      <c r="Y10" s="213"/>
-      <c r="Z10" s="213"/>
-      <c r="AA10" s="213"/>
-      <c r="AB10" s="215"/>
-      <c r="AC10" s="215"/>
-      <c r="AD10" s="215"/>
-      <c r="AE10" s="215"/>
-      <c r="AF10" s="215"/>
-      <c r="AG10" s="215"/>
-      <c r="AH10" s="215"/>
-      <c r="AI10" s="215"/>
-      <c r="AJ10" s="215"/>
-      <c r="AK10" s="215"/>
-      <c r="AL10" s="215"/>
-      <c r="AM10" s="215"/>
-      <c r="AN10" s="215"/>
-      <c r="AO10" s="215"/>
-      <c r="AP10" s="215"/>
-      <c r="AQ10" s="215"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
+      <c r="AB10" s="190"/>
+      <c r="AC10" s="190"/>
+      <c r="AD10" s="190"/>
+      <c r="AE10" s="190"/>
+      <c r="AF10" s="190"/>
+      <c r="AG10" s="190"/>
+      <c r="AH10" s="190"/>
+      <c r="AI10" s="190"/>
+      <c r="AJ10" s="190"/>
+      <c r="AK10" s="190"/>
+      <c r="AL10" s="190"/>
+      <c r="AM10" s="190"/>
+      <c r="AN10" s="190"/>
+      <c r="AO10" s="190"/>
+      <c r="AP10" s="190"/>
+      <c r="AQ10" s="190"/>
+      <c r="AR10" s="193"/>
+      <c r="AS10" s="193"/>
+      <c r="AT10" s="193"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="187"/>
-      <c r="AW10" s="187"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="187"/>
-      <c r="BW10" s="187"/>
-      <c r="CT10" s="187"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="196"/>
+      <c r="AY10" s="197"/>
+      <c r="AZ10" s="197"/>
+      <c r="BA10" s="197"/>
+      <c r="BB10" s="197"/>
+      <c r="BC10" s="197"/>
+      <c r="BD10" s="197"/>
+      <c r="BE10" s="197"/>
+      <c r="BF10" s="199"/>
+      <c r="BG10" s="199"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="194"/>
-      <c r="B11" s="195" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="195"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="193"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="193"/>
-      <c r="K11" s="193"/>
-      <c r="L11" s="186"/>
-      <c r="M11" s="186"/>
-      <c r="N11" s="186"/>
-      <c r="O11" s="186"/>
-      <c r="P11" s="186"/>
-      <c r="Q11" s="186"/>
-      <c r="R11" s="186"/>
-      <c r="S11" s="186"/>
-      <c r="T11" s="186"/>
-      <c r="U11" s="186"/>
-      <c r="V11" s="186"/>
-      <c r="W11" s="213"/>
-      <c r="X11" s="213"/>
-      <c r="Y11" s="213"/>
-      <c r="Z11" s="213"/>
-      <c r="AA11" s="213"/>
-      <c r="AB11" s="216"/>
-      <c r="AC11" s="216"/>
-      <c r="AD11" s="216"/>
-      <c r="AE11" s="216"/>
-      <c r="AF11" s="216"/>
-      <c r="AG11" s="216"/>
-      <c r="AH11" s="216"/>
-      <c r="AI11" s="216"/>
-      <c r="AJ11" s="216"/>
-      <c r="AK11" s="216"/>
-      <c r="AL11" s="216"/>
-      <c r="AM11" s="216"/>
-      <c r="AN11" s="216"/>
-      <c r="AO11" s="216"/>
-      <c r="AP11" s="216"/>
-      <c r="AQ11" s="216"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
+      <c r="AB11" s="191"/>
+      <c r="AC11" s="191"/>
+      <c r="AD11" s="191"/>
+      <c r="AE11" s="191"/>
+      <c r="AF11" s="191"/>
+      <c r="AG11" s="191"/>
+      <c r="AH11" s="191"/>
+      <c r="AI11" s="191"/>
+      <c r="AJ11" s="191"/>
+      <c r="AK11" s="191"/>
+      <c r="AL11" s="191"/>
+      <c r="AM11" s="191"/>
+      <c r="AN11" s="191"/>
+      <c r="AO11" s="191"/>
+      <c r="AP11" s="191"/>
+      <c r="AQ11" s="191"/>
+      <c r="AR11" s="194"/>
+      <c r="AS11" s="194"/>
+      <c r="AT11" s="194"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="187"/>
-      <c r="AW11" s="187"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="187"/>
-      <c r="BW11" s="187"/>
-      <c r="CT11" s="187"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="196"/>
+      <c r="AY11" s="197"/>
+      <c r="AZ11" s="197"/>
+      <c r="BA11" s="197"/>
+      <c r="BB11" s="197"/>
+      <c r="BC11" s="197"/>
+      <c r="BD11" s="197"/>
+      <c r="BE11" s="197"/>
+      <c r="BF11" s="199"/>
+      <c r="BG11" s="199"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4083,63 +4156,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4153,7 +4169,7 @@
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -5001,7 +5017,7 @@
   <dimension ref="A1:DB1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AA25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C4" sqref="C4:C12"/>
@@ -5661,13 +5677,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="200" t="s">
+      <c r="B4" s="213" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="201"/>
+      <c r="C4" s="214"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5772,9 +5788,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="199"/>
-      <c r="B5" s="197"/>
-      <c r="C5" s="199"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="211"/>
+      <c r="C5" s="201"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5879,11 +5895,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="199"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="199"/>
+      <c r="C6" s="201"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -5988,11 +6004,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="199"/>
+      <c r="A7" s="201"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="199"/>
+      <c r="C7" s="201"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6097,11 +6113,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="199"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="199"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6206,11 +6222,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="199"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="199"/>
+      <c r="C9" s="201"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6315,11 +6331,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="199"/>
+      <c r="A10" s="201"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="199"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6424,11 +6440,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="199"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="199"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6533,7 +6549,7 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="199"/>
+      <c r="A12" s="201"/>
       <c r="B12" s="71"/>
       <c r="C12" s="202"/>
       <c r="D12" s="72"/>
@@ -6640,10 +6656,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="203" t="s">
+      <c r="A13" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="204" t="s">
+      <c r="B13" s="216" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6752,8 +6768,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="199"/>
-      <c r="B14" s="205"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="207"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6874,7 +6890,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="199"/>
+      <c r="A15" s="201"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -6984,7 +7000,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="199"/>
+      <c r="A16" s="201"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7094,7 +7110,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="199"/>
+      <c r="A17" s="201"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7206,7 +7222,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="199"/>
+      <c r="A18" s="201"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7316,7 +7332,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="199"/>
+      <c r="A19" s="201"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7426,7 +7442,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="199"/>
+      <c r="A20" s="201"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7647,7 +7663,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="93"/>
-      <c r="B22" s="196" t="s">
+      <c r="B22" s="210" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7757,7 +7773,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="93"/>
-      <c r="B23" s="197"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7864,13 +7880,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="207" t="s">
+      <c r="A24" s="203" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="209">
+      <c r="C24" s="205">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -7978,11 +7994,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="208"/>
+      <c r="A25" s="204"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="199"/>
+      <c r="C25" s="201"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8088,11 +8104,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="208"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="199"/>
+      <c r="C26" s="201"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8198,11 +8214,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="208"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="199"/>
+      <c r="C27" s="201"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8308,11 +8324,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="208"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="199"/>
+      <c r="C28" s="201"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8418,11 +8434,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="208"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="199"/>
+      <c r="C29" s="201"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8528,11 +8544,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="208"/>
+      <c r="A30" s="204"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="199"/>
+      <c r="C30" s="201"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8638,11 +8654,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="208"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="199"/>
+      <c r="C31" s="201"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8748,11 +8764,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="208"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="199"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8858,11 +8874,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="208"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="199"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -8968,11 +8984,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="208"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="199"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9078,7 +9094,7 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="208"/>
+      <c r="A35" s="204"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
@@ -9188,11 +9204,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="208"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="209">
+      <c r="C36" s="205">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9300,11 +9316,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="208"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="199"/>
+      <c r="C37" s="201"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9410,11 +9426,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="208"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="199"/>
+      <c r="C38" s="201"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9520,11 +9536,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="208"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="199"/>
+      <c r="C39" s="201"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9630,11 +9646,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="208"/>
+      <c r="A40" s="204"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="199"/>
+      <c r="C40" s="201"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9740,11 +9756,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="208"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="199"/>
+      <c r="C41" s="201"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9850,11 +9866,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="208"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="199"/>
+      <c r="C42" s="201"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -9960,11 +9976,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="208"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="199"/>
+      <c r="C43" s="201"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10070,11 +10086,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="208"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="199"/>
+      <c r="C44" s="201"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10180,11 +10196,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="208"/>
+      <c r="A45" s="204"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="199"/>
+      <c r="C45" s="201"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10290,11 +10306,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="208"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="199"/>
+      <c r="C46" s="201"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10400,11 +10416,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="208"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="199"/>
+      <c r="C47" s="201"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10518,11 +10534,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="208"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="199"/>
+      <c r="C48" s="201"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10631,7 +10647,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="111"/>
-      <c r="B49" s="210" t="s">
+      <c r="B49" s="206" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10741,7 +10757,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="116"/>
-      <c r="B50" s="205"/>
+      <c r="B50" s="207"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14172,7 +14188,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="211" t="s">
+      <c r="A81" s="208" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14284,7 +14300,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="199"/>
+      <c r="A82" s="201"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14394,7 +14410,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="199"/>
+      <c r="A83" s="201"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14504,7 +14520,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="199"/>
+      <c r="A84" s="201"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14614,7 +14630,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="199"/>
+      <c r="A85" s="201"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14724,7 +14740,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="199"/>
+      <c r="A86" s="201"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14834,7 +14850,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="199"/>
+      <c r="A87" s="201"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -14946,7 +14962,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="199"/>
+      <c r="A88" s="201"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15056,7 +15072,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="199"/>
+      <c r="A89" s="201"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15166,7 +15182,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="199"/>
+      <c r="A90" s="201"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15276,11 +15292,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="199"/>
+      <c r="A91" s="201"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="212"/>
+      <c r="C91" s="209"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15386,11 +15402,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="199"/>
+      <c r="A92" s="201"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="199"/>
+      <c r="C92" s="201"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15500,7 +15516,7 @@
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="199"/>
+      <c r="C93" s="201"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15724,7 +15740,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="206" t="s">
+      <c r="A95" s="200" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15836,7 +15852,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="199"/>
+      <c r="A96" s="201"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -15946,7 +15962,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="199"/>
+      <c r="A97" s="201"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16056,7 +16072,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="199"/>
+      <c r="A98" s="201"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16166,7 +16182,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="199"/>
+      <c r="A99" s="201"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16276,7 +16292,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="199"/>
+      <c r="A100" s="201"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16386,7 +16402,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="199"/>
+      <c r="A101" s="201"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16496,7 +16512,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="199"/>
+      <c r="A102" s="201"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16606,7 +16622,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="199"/>
+      <c r="A103" s="201"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16718,7 +16734,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="199"/>
+      <c r="A104" s="201"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16828,7 +16844,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="199"/>
+      <c r="A105" s="201"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -16946,7 +16962,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="199"/>
+      <c r="A106" s="201"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17056,7 +17072,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="199"/>
+      <c r="A107" s="201"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17166,7 +17182,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="199"/>
+      <c r="A108" s="201"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17276,7 +17292,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="199"/>
+      <c r="A109" s="201"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17386,7 +17402,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="199"/>
+      <c r="A110" s="201"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17496,7 +17512,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="199"/>
+      <c r="A111" s="201"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17606,7 +17622,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="199"/>
+      <c r="A112" s="201"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17716,7 +17732,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="199"/>
+      <c r="A113" s="201"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17826,7 +17842,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="199"/>
+      <c r="A114" s="201"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17936,7 +17952,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="199"/>
+      <c r="A115" s="201"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18046,7 +18062,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="199"/>
+      <c r="A116" s="201"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18172,7 +18188,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="199"/>
+      <c r="A117" s="201"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -25653,6 +25669,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25660,12 +25682,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 06-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C514EA69-CA2C-4FB4-B0FE-6BD553AFC3FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD97DEBF-A6F8-412D-B20F-BE0C24B83FC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="161">
   <si>
     <t>S</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>Criação de 3 telas para os projetos da empresa Linx</t>
+  </si>
+  <si>
+    <t>Continuação das telas para os projetos da empresa Linx</t>
   </si>
 </sst>
 </file>
@@ -2192,17 +2195,47 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2219,50 +2252,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2273,30 +2296,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2806,7 +2809,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4:V11"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -3115,110 +3118,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="192"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
+      <c r="AF2" s="192"/>
+      <c r="AG2" s="192"/>
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="192"/>
+      <c r="AJ2" s="192"/>
+      <c r="AK2" s="192"/>
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="192"/>
+      <c r="AQ2" s="192"/>
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="192"/>
+      <c r="AV2" s="192"/>
+      <c r="AW2" s="192"/>
+      <c r="AX2" s="193"/>
+      <c r="AY2" s="193"/>
+      <c r="AZ2" s="193"/>
+      <c r="BA2" s="193"/>
+      <c r="BB2" s="193"/>
+      <c r="BC2" s="193"/>
+      <c r="BD2" s="193"/>
+      <c r="BE2" s="193"/>
+      <c r="BF2" s="193"/>
+      <c r="BG2" s="193"/>
+      <c r="BH2" s="193"/>
+      <c r="BI2" s="193"/>
+      <c r="BJ2" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="192"/>
+      <c r="BL2" s="192"/>
+      <c r="BM2" s="192"/>
+      <c r="BN2" s="192"/>
+      <c r="BO2" s="192"/>
+      <c r="BP2" s="192"/>
+      <c r="BQ2" s="192"/>
+      <c r="BR2" s="192"/>
+      <c r="BS2" s="192"/>
+      <c r="BT2" s="192"/>
+      <c r="BU2" s="192"/>
+      <c r="BV2" s="192"/>
+      <c r="BW2" s="192"/>
+      <c r="BX2" s="194"/>
+      <c r="BY2" s="194"/>
+      <c r="BZ2" s="194"/>
+      <c r="CA2" s="194"/>
+      <c r="CB2" s="194"/>
+      <c r="CC2" s="194"/>
+      <c r="CD2" s="194"/>
+      <c r="CE2" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="196"/>
+      <c r="CG2" s="196"/>
+      <c r="CH2" s="196"/>
+      <c r="CI2" s="196"/>
+      <c r="CJ2" s="196"/>
+      <c r="CK2" s="196"/>
+      <c r="CL2" s="196"/>
+      <c r="CM2" s="196"/>
+      <c r="CN2" s="196"/>
+      <c r="CO2" s="196"/>
+      <c r="CP2" s="196"/>
+      <c r="CQ2" s="196"/>
+      <c r="CR2" s="196"/>
+      <c r="CS2" s="196"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3514,616 +3517,593 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="199"/>
+      <c r="D4" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="197" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="197" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="197" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="197" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="197" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="197" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="190" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="190" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="190" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="190" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="190" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="190" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187"/>
-      <c r="W4" s="188"/>
-      <c r="X4" s="188"/>
-      <c r="Y4" s="188"/>
-      <c r="Z4" s="188"/>
-      <c r="AA4" s="188"/>
-      <c r="AB4" s="189"/>
-      <c r="AC4" s="189"/>
-      <c r="AD4" s="189"/>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="189"/>
-      <c r="AG4" s="189"/>
-      <c r="AH4" s="189"/>
-      <c r="AI4" s="189"/>
-      <c r="AJ4" s="189"/>
-      <c r="AK4" s="189"/>
-      <c r="AL4" s="189"/>
-      <c r="AM4" s="189"/>
-      <c r="AN4" s="189"/>
-      <c r="AO4" s="189"/>
-      <c r="AP4" s="189"/>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
+      <c r="V4" s="190" t="s">
+        <v>160</v>
+      </c>
+      <c r="W4" s="189"/>
+      <c r="X4" s="189"/>
+      <c r="Y4" s="189"/>
+      <c r="Z4" s="189"/>
+      <c r="AA4" s="189"/>
+      <c r="AB4" s="186"/>
+      <c r="AC4" s="186"/>
+      <c r="AD4" s="186"/>
+      <c r="AE4" s="186"/>
+      <c r="AF4" s="186"/>
+      <c r="AG4" s="186"/>
+      <c r="AH4" s="186"/>
+      <c r="AI4" s="186"/>
+      <c r="AJ4" s="186"/>
+      <c r="AK4" s="186"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="195"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="198"/>
-      <c r="BG4" s="198"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="191"/>
+      <c r="AW4" s="191"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="191"/>
+      <c r="BW4" s="191"/>
+      <c r="CT4" s="191"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="198"/>
+      <c r="B5" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="190"/>
-      <c r="AC5" s="190"/>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="190"/>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="190"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="190"/>
-      <c r="AP5" s="190"/>
-      <c r="AQ5" s="190"/>
-      <c r="AR5" s="193"/>
-      <c r="AS5" s="193"/>
-      <c r="AT5" s="193"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="197"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="197"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="190"/>
+      <c r="P5" s="190"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="190"/>
+      <c r="S5" s="190"/>
+      <c r="T5" s="190"/>
+      <c r="U5" s="190"/>
+      <c r="V5" s="190"/>
+      <c r="W5" s="189"/>
+      <c r="X5" s="189"/>
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="189"/>
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="187"/>
+      <c r="AC5" s="187"/>
+      <c r="AD5" s="187"/>
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="187"/>
+      <c r="AG5" s="187"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="196"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="197"/>
-      <c r="BA5" s="197"/>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="199"/>
-      <c r="BG5" s="199"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="191"/>
+      <c r="AW5" s="191"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="191"/>
+      <c r="BW5" s="191"/>
+      <c r="CT5" s="191"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="198"/>
+      <c r="B6" s="199" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="190"/>
-      <c r="AC6" s="190"/>
-      <c r="AD6" s="190"/>
-      <c r="AE6" s="190"/>
-      <c r="AF6" s="190"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="190"/>
-      <c r="AI6" s="190"/>
-      <c r="AJ6" s="190"/>
-      <c r="AK6" s="190"/>
-      <c r="AL6" s="190"/>
-      <c r="AM6" s="190"/>
-      <c r="AN6" s="190"/>
-      <c r="AO6" s="190"/>
-      <c r="AP6" s="190"/>
-      <c r="AQ6" s="190"/>
-      <c r="AR6" s="193"/>
-      <c r="AS6" s="193"/>
-      <c r="AT6" s="193"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="N6" s="190"/>
+      <c r="O6" s="190"/>
+      <c r="P6" s="190"/>
+      <c r="Q6" s="190"/>
+      <c r="R6" s="190"/>
+      <c r="S6" s="190"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="190"/>
+      <c r="V6" s="190"/>
+      <c r="W6" s="189"/>
+      <c r="X6" s="189"/>
+      <c r="Y6" s="189"/>
+      <c r="Z6" s="189"/>
+      <c r="AA6" s="189"/>
+      <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
+      <c r="AD6" s="187"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="187"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="197"/>
-      <c r="AZ6" s="197"/>
-      <c r="BA6" s="197"/>
-      <c r="BB6" s="197"/>
-      <c r="BC6" s="197"/>
-      <c r="BD6" s="197"/>
-      <c r="BE6" s="197"/>
-      <c r="BF6" s="199"/>
-      <c r="BG6" s="199"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="191"/>
+      <c r="AW6" s="191"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="191"/>
+      <c r="BW6" s="191"/>
+      <c r="CT6" s="191"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="198"/>
+      <c r="B7" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="190"/>
-      <c r="AC7" s="190"/>
-      <c r="AD7" s="190"/>
-      <c r="AE7" s="190"/>
-      <c r="AF7" s="190"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="190"/>
-      <c r="AI7" s="190"/>
-      <c r="AJ7" s="190"/>
-      <c r="AK7" s="190"/>
-      <c r="AL7" s="190"/>
-      <c r="AM7" s="190"/>
-      <c r="AN7" s="190"/>
-      <c r="AO7" s="190"/>
-      <c r="AP7" s="190"/>
-      <c r="AQ7" s="190"/>
-      <c r="AR7" s="193"/>
-      <c r="AS7" s="193"/>
-      <c r="AT7" s="193"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="197"/>
+      <c r="F7" s="197"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
+      <c r="Q7" s="190"/>
+      <c r="R7" s="190"/>
+      <c r="S7" s="190"/>
+      <c r="T7" s="190"/>
+      <c r="U7" s="190"/>
+      <c r="V7" s="190"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="189"/>
+      <c r="Y7" s="189"/>
+      <c r="Z7" s="189"/>
+      <c r="AA7" s="189"/>
+      <c r="AB7" s="187"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="196"/>
-      <c r="AY7" s="197"/>
-      <c r="AZ7" s="197"/>
-      <c r="BA7" s="197"/>
-      <c r="BB7" s="197"/>
-      <c r="BC7" s="197"/>
-      <c r="BD7" s="197"/>
-      <c r="BE7" s="197"/>
-      <c r="BF7" s="199"/>
-      <c r="BG7" s="199"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="191"/>
+      <c r="AW7" s="191"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="191"/>
+      <c r="BW7" s="191"/>
+      <c r="CT7" s="191"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="190"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="193"/>
-      <c r="AS8" s="193"/>
-      <c r="AT8" s="193"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="197"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="190"/>
+      <c r="R8" s="190"/>
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="190"/>
+      <c r="W8" s="189"/>
+      <c r="X8" s="189"/>
+      <c r="Y8" s="189"/>
+      <c r="Z8" s="189"/>
+      <c r="AA8" s="189"/>
+      <c r="AB8" s="187"/>
+      <c r="AC8" s="187"/>
+      <c r="AD8" s="187"/>
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="187"/>
+      <c r="AG8" s="187"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="196"/>
-      <c r="AY8" s="197"/>
-      <c r="AZ8" s="197"/>
-      <c r="BA8" s="197"/>
-      <c r="BB8" s="197"/>
-      <c r="BC8" s="197"/>
-      <c r="BD8" s="197"/>
-      <c r="BE8" s="197"/>
-      <c r="BF8" s="199"/>
-      <c r="BG8" s="199"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="191"/>
+      <c r="AW8" s="191"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="191"/>
+      <c r="BW8" s="191"/>
+      <c r="CT8" s="191"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="198"/>
+      <c r="B9" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
-      <c r="AB9" s="190"/>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="190"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="190"/>
-      <c r="AL9" s="190"/>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="190"/>
-      <c r="AQ9" s="190"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="197"/>
+      <c r="I9" s="197"/>
+      <c r="J9" s="197"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="190"/>
+      <c r="W9" s="189"/>
+      <c r="X9" s="189"/>
+      <c r="Y9" s="189"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="189"/>
+      <c r="AB9" s="187"/>
+      <c r="AC9" s="187"/>
+      <c r="AD9" s="187"/>
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="187"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="196"/>
-      <c r="AY9" s="197"/>
-      <c r="AZ9" s="197"/>
-      <c r="BA9" s="197"/>
-      <c r="BB9" s="197"/>
-      <c r="BC9" s="197"/>
-      <c r="BD9" s="197"/>
-      <c r="BE9" s="197"/>
-      <c r="BF9" s="199"/>
-      <c r="BG9" s="199"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="191"/>
+      <c r="AW9" s="191"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="191"/>
+      <c r="BW9" s="191"/>
+      <c r="CT9" s="191"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="198"/>
+      <c r="B10" s="199" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="190"/>
-      <c r="AC10" s="190"/>
-      <c r="AD10" s="190"/>
-      <c r="AE10" s="190"/>
-      <c r="AF10" s="190"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="190"/>
-      <c r="AI10" s="190"/>
-      <c r="AJ10" s="190"/>
-      <c r="AK10" s="190"/>
-      <c r="AL10" s="190"/>
-      <c r="AM10" s="190"/>
-      <c r="AN10" s="190"/>
-      <c r="AO10" s="190"/>
-      <c r="AP10" s="190"/>
-      <c r="AQ10" s="190"/>
-      <c r="AR10" s="193"/>
-      <c r="AS10" s="193"/>
-      <c r="AT10" s="193"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="197"/>
+      <c r="K10" s="197"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="190"/>
+      <c r="O10" s="190"/>
+      <c r="P10" s="190"/>
+      <c r="Q10" s="190"/>
+      <c r="R10" s="190"/>
+      <c r="S10" s="190"/>
+      <c r="T10" s="190"/>
+      <c r="U10" s="190"/>
+      <c r="V10" s="190"/>
+      <c r="W10" s="189"/>
+      <c r="X10" s="189"/>
+      <c r="Y10" s="189"/>
+      <c r="Z10" s="189"/>
+      <c r="AA10" s="189"/>
+      <c r="AB10" s="187"/>
+      <c r="AC10" s="187"/>
+      <c r="AD10" s="187"/>
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="187"/>
+      <c r="AG10" s="187"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="196"/>
-      <c r="AY10" s="197"/>
-      <c r="AZ10" s="197"/>
-      <c r="BA10" s="197"/>
-      <c r="BB10" s="197"/>
-      <c r="BC10" s="197"/>
-      <c r="BD10" s="197"/>
-      <c r="BE10" s="197"/>
-      <c r="BF10" s="199"/>
-      <c r="BG10" s="199"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="191"/>
+      <c r="AW10" s="191"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="191"/>
+      <c r="BW10" s="191"/>
+      <c r="CT10" s="191"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="198"/>
+      <c r="B11" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="191"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="191"/>
-      <c r="AE11" s="191"/>
-      <c r="AF11" s="191"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="191"/>
-      <c r="AI11" s="191"/>
-      <c r="AJ11" s="191"/>
-      <c r="AK11" s="191"/>
-      <c r="AL11" s="191"/>
-      <c r="AM11" s="191"/>
-      <c r="AN11" s="191"/>
-      <c r="AO11" s="191"/>
-      <c r="AP11" s="191"/>
-      <c r="AQ11" s="191"/>
-      <c r="AR11" s="194"/>
-      <c r="AS11" s="194"/>
-      <c r="AT11" s="194"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
+      <c r="N11" s="190"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="190"/>
+      <c r="Q11" s="190"/>
+      <c r="R11" s="190"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="190"/>
+      <c r="U11" s="190"/>
+      <c r="V11" s="190"/>
+      <c r="W11" s="189"/>
+      <c r="X11" s="189"/>
+      <c r="Y11" s="189"/>
+      <c r="Z11" s="189"/>
+      <c r="AA11" s="189"/>
+      <c r="AB11" s="188"/>
+      <c r="AC11" s="188"/>
+      <c r="AD11" s="188"/>
+      <c r="AE11" s="188"/>
+      <c r="AF11" s="188"/>
+      <c r="AG11" s="188"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="196"/>
-      <c r="AY11" s="197"/>
-      <c r="AZ11" s="197"/>
-      <c r="BA11" s="197"/>
-      <c r="BB11" s="197"/>
-      <c r="BC11" s="197"/>
-      <c r="BD11" s="197"/>
-      <c r="BE11" s="197"/>
-      <c r="BF11" s="199"/>
-      <c r="BG11" s="199"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="191"/>
+      <c r="AW11" s="191"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="191"/>
+      <c r="BW11" s="191"/>
+      <c r="CT11" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4140,22 +4120,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5677,13 +5682,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="212" t="s">
+      <c r="A4" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="214"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5788,9 +5793,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="201"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="201"/>
+      <c r="A5" s="203"/>
+      <c r="B5" s="201"/>
+      <c r="C5" s="203"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5895,11 +5900,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="201"/>
+      <c r="A6" s="203"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="201"/>
+      <c r="C6" s="203"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6004,11 +6009,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="201"/>
+      <c r="A7" s="203"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="201"/>
+      <c r="C7" s="203"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6113,11 +6118,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="201"/>
+      <c r="A8" s="203"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="201"/>
+      <c r="C8" s="203"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6222,11 +6227,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="201"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="201"/>
+      <c r="C9" s="203"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6331,11 +6336,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="201"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="203"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6440,11 +6445,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="201"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="203"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6549,9 +6554,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="201"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="202"/>
+      <c r="C12" s="206"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6656,10 +6661,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="208" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6768,8 +6773,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="201"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6890,7 +6895,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="201"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7000,7 +7005,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="201"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7110,7 +7115,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="201"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7222,7 +7227,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="201"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7332,7 +7337,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="201"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7442,7 +7447,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="201"/>
+      <c r="A20" s="203"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7552,7 +7557,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="202"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7663,7 +7668,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="93"/>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="200" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7773,7 +7778,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="93"/>
-      <c r="B23" s="211"/>
+      <c r="B23" s="201"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7880,13 +7885,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="203" t="s">
+      <c r="A24" s="211" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="205">
+      <c r="C24" s="213">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -7994,11 +7999,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="204"/>
+      <c r="A25" s="212"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="201"/>
+      <c r="C25" s="203"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8104,11 +8109,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="204"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="203"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8214,11 +8219,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="204"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="201"/>
+      <c r="C27" s="203"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8324,11 +8329,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="204"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="201"/>
+      <c r="C28" s="203"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8434,11 +8439,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="204"/>
+      <c r="A29" s="212"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="201"/>
+      <c r="C29" s="203"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8544,11 +8549,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="204"/>
+      <c r="A30" s="212"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="201"/>
+      <c r="C30" s="203"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8654,11 +8659,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="204"/>
+      <c r="A31" s="212"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="201"/>
+      <c r="C31" s="203"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8764,11 +8769,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="204"/>
+      <c r="A32" s="212"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="201"/>
+      <c r="C32" s="203"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8874,11 +8879,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="204"/>
+      <c r="A33" s="212"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="201"/>
+      <c r="C33" s="203"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -8984,11 +8989,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="204"/>
+      <c r="A34" s="212"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="201"/>
+      <c r="C34" s="203"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9094,11 +9099,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="204"/>
+      <c r="A35" s="212"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="202"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9204,11 +9209,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="204"/>
+      <c r="A36" s="212"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="205">
+      <c r="C36" s="213">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9316,11 +9321,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="204"/>
+      <c r="A37" s="212"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="201"/>
+      <c r="C37" s="203"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9426,11 +9431,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="204"/>
+      <c r="A38" s="212"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="201"/>
+      <c r="C38" s="203"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9536,11 +9541,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="204"/>
+      <c r="A39" s="212"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="201"/>
+      <c r="C39" s="203"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9646,11 +9651,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="204"/>
+      <c r="A40" s="212"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="201"/>
+      <c r="C40" s="203"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9756,11 +9761,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="204"/>
+      <c r="A41" s="212"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="201"/>
+      <c r="C41" s="203"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9866,11 +9871,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="204"/>
+      <c r="A42" s="212"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="201"/>
+      <c r="C42" s="203"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -9976,11 +9981,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="204"/>
+      <c r="A43" s="212"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="201"/>
+      <c r="C43" s="203"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10086,11 +10091,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="204"/>
+      <c r="A44" s="212"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="201"/>
+      <c r="C44" s="203"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10196,11 +10201,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="204"/>
+      <c r="A45" s="212"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10306,11 +10311,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="204"/>
+      <c r="A46" s="212"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="201"/>
+      <c r="C46" s="203"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10416,11 +10421,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="204"/>
+      <c r="A47" s="212"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="201"/>
+      <c r="C47" s="203"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10534,11 +10539,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="204"/>
+      <c r="A48" s="212"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="201"/>
+      <c r="C48" s="203"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10647,7 +10652,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="111"/>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="214" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10757,7 +10762,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="116"/>
-      <c r="B50" s="207"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14188,7 +14193,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="208" t="s">
+      <c r="A81" s="215" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14300,7 +14305,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="201"/>
+      <c r="A82" s="203"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14410,7 +14415,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="201"/>
+      <c r="A83" s="203"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14520,7 +14525,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="201"/>
+      <c r="A84" s="203"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14630,7 +14635,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="201"/>
+      <c r="A85" s="203"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14740,7 +14745,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="201"/>
+      <c r="A86" s="203"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14850,7 +14855,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="201"/>
+      <c r="A87" s="203"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -14962,7 +14967,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="201"/>
+      <c r="A88" s="203"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15072,7 +15077,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="201"/>
+      <c r="A89" s="203"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15182,7 +15187,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="201"/>
+      <c r="A90" s="203"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15292,11 +15297,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="201"/>
+      <c r="A91" s="203"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="209"/>
+      <c r="C91" s="216"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15402,11 +15407,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="201"/>
+      <c r="A92" s="203"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="203"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15512,11 +15517,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="202"/>
+      <c r="A93" s="206"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="201"/>
+      <c r="C93" s="203"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15740,7 +15745,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="200" t="s">
+      <c r="A95" s="210" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15852,7 +15857,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="201"/>
+      <c r="A96" s="203"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -15962,7 +15967,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="201"/>
+      <c r="A97" s="203"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16072,7 +16077,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="201"/>
+      <c r="A98" s="203"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16182,7 +16187,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="201"/>
+      <c r="A99" s="203"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16292,7 +16297,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="201"/>
+      <c r="A100" s="203"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16402,7 +16407,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="201"/>
+      <c r="A101" s="203"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16512,7 +16517,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="201"/>
+      <c r="A102" s="203"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16622,7 +16627,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="201"/>
+      <c r="A103" s="203"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16734,7 +16739,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="201"/>
+      <c r="A104" s="203"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16844,7 +16849,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="201"/>
+      <c r="A105" s="203"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -16962,7 +16967,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="201"/>
+      <c r="A106" s="203"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17072,7 +17077,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="201"/>
+      <c r="A107" s="203"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17182,7 +17187,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="201"/>
+      <c r="A108" s="203"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17292,7 +17297,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="201"/>
+      <c r="A109" s="203"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17402,7 +17407,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="201"/>
+      <c r="A110" s="203"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17512,7 +17517,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="201"/>
+      <c r="A111" s="203"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17622,7 +17627,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="201"/>
+      <c r="A112" s="203"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17732,7 +17737,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="201"/>
+      <c r="A113" s="203"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17842,7 +17847,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="201"/>
+      <c r="A114" s="203"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17952,7 +17957,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="201"/>
+      <c r="A115" s="203"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18062,7 +18067,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="201"/>
+      <c r="A116" s="203"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18188,7 +18193,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="201"/>
+      <c r="A117" s="203"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18298,7 +18303,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="202"/>
+      <c r="A118" s="206"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25669,12 +25674,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25682,6 +25681,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 09-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD97DEBF-A6F8-412D-B20F-BE0C24B83FC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0E8FD6-BABD-44E1-B18E-514D2ECC5AE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="162">
   <si>
     <t>S</t>
   </si>
@@ -684,6 +684,12 @@
   </si>
   <si>
     <t>Continuação das telas para os projetos da empresa Linx</t>
+  </si>
+  <si>
+    <t>Palestra de boas práticas em apresentação pela ThoughtWorks.
+Finalização de integração e navegação das páginas construídas.
+Reunião com os Scrum Masters e POs para alinhamento da sinergia dos grupos.
+Montagem da apresentação do andamento dos projetos para a coordenação</t>
   </si>
 </sst>
 </file>
@@ -2195,14 +2201,47 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2219,73 +2258,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2296,10 +2282,30 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2809,7 +2815,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W4" sqref="W4:W11"/>
+      <selection pane="bottomRight" activeCell="X4" sqref="X4:X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -3118,110 +3124,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="192" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="192"/>
-      <c r="I2" s="192"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="192" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="192"/>
-      <c r="T2" s="192"/>
-      <c r="U2" s="192"/>
-      <c r="V2" s="192"/>
-      <c r="W2" s="192"/>
-      <c r="X2" s="192"/>
-      <c r="Y2" s="192"/>
-      <c r="Z2" s="192"/>
-      <c r="AA2" s="192"/>
-      <c r="AB2" s="192"/>
-      <c r="AC2" s="192"/>
-      <c r="AD2" s="192"/>
-      <c r="AE2" s="192"/>
-      <c r="AF2" s="192"/>
-      <c r="AG2" s="192"/>
-      <c r="AH2" s="192"/>
-      <c r="AI2" s="192"/>
-      <c r="AJ2" s="192"/>
-      <c r="AK2" s="192"/>
-      <c r="AL2" s="192"/>
-      <c r="AM2" s="192" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="192"/>
-      <c r="AO2" s="192"/>
-      <c r="AP2" s="192"/>
-      <c r="AQ2" s="192"/>
-      <c r="AR2" s="192"/>
-      <c r="AS2" s="192"/>
-      <c r="AT2" s="192"/>
-      <c r="AU2" s="192"/>
-      <c r="AV2" s="192"/>
-      <c r="AW2" s="192"/>
-      <c r="AX2" s="193"/>
-      <c r="AY2" s="193"/>
-      <c r="AZ2" s="193"/>
-      <c r="BA2" s="193"/>
-      <c r="BB2" s="193"/>
-      <c r="BC2" s="193"/>
-      <c r="BD2" s="193"/>
-      <c r="BE2" s="193"/>
-      <c r="BF2" s="193"/>
-      <c r="BG2" s="193"/>
-      <c r="BH2" s="193"/>
-      <c r="BI2" s="193"/>
-      <c r="BJ2" s="192" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="192"/>
-      <c r="BL2" s="192"/>
-      <c r="BM2" s="192"/>
-      <c r="BN2" s="192"/>
-      <c r="BO2" s="192"/>
-      <c r="BP2" s="192"/>
-      <c r="BQ2" s="192"/>
-      <c r="BR2" s="192"/>
-      <c r="BS2" s="192"/>
-      <c r="BT2" s="192"/>
-      <c r="BU2" s="192"/>
-      <c r="BV2" s="192"/>
-      <c r="BW2" s="192"/>
-      <c r="BX2" s="194"/>
-      <c r="BY2" s="194"/>
-      <c r="BZ2" s="194"/>
-      <c r="CA2" s="194"/>
-      <c r="CB2" s="194"/>
-      <c r="CC2" s="194"/>
-      <c r="CD2" s="194"/>
-      <c r="CE2" s="195" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="196"/>
-      <c r="CG2" s="196"/>
-      <c r="CH2" s="196"/>
-      <c r="CI2" s="196"/>
-      <c r="CJ2" s="196"/>
-      <c r="CK2" s="196"/>
-      <c r="CL2" s="196"/>
-      <c r="CM2" s="196"/>
-      <c r="CN2" s="196"/>
-      <c r="CO2" s="196"/>
-      <c r="CP2" s="196"/>
-      <c r="CQ2" s="196"/>
-      <c r="CR2" s="196"/>
-      <c r="CS2" s="196"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3517,577 +3523,636 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="199"/>
-      <c r="D4" s="197" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="197" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="197" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="197" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="197" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="197" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="197" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="190" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="190" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="190" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="190" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="190" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="190" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="190" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="190" t="s">
+      <c r="S4" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="190" t="s">
+      <c r="T4" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="190" t="s">
+      <c r="U4" s="187" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="190" t="s">
+      <c r="V4" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="189"/>
-      <c r="X4" s="189"/>
-      <c r="Y4" s="189"/>
-      <c r="Z4" s="189"/>
-      <c r="AA4" s="189"/>
-      <c r="AB4" s="186"/>
-      <c r="AC4" s="186"/>
-      <c r="AD4" s="186"/>
-      <c r="AE4" s="186"/>
-      <c r="AF4" s="186"/>
-      <c r="AG4" s="186"/>
-      <c r="AH4" s="186"/>
-      <c r="AI4" s="186"/>
-      <c r="AJ4" s="186"/>
-      <c r="AK4" s="186"/>
-      <c r="AL4" s="186"/>
-      <c r="AM4" s="186"/>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="W4" s="188" t="s">
+        <v>161</v>
+      </c>
+      <c r="X4" s="188"/>
+      <c r="Y4" s="188"/>
+      <c r="Z4" s="188"/>
+      <c r="AA4" s="188"/>
+      <c r="AB4" s="189"/>
+      <c r="AC4" s="189"/>
+      <c r="AD4" s="189"/>
+      <c r="AE4" s="189"/>
+      <c r="AF4" s="189"/>
+      <c r="AG4" s="189"/>
+      <c r="AH4" s="189"/>
+      <c r="AI4" s="189"/>
+      <c r="AJ4" s="189"/>
+      <c r="AK4" s="189"/>
+      <c r="AL4" s="189"/>
+      <c r="AM4" s="189"/>
+      <c r="AN4" s="189"/>
+      <c r="AO4" s="189"/>
+      <c r="AP4" s="189"/>
+      <c r="AQ4" s="189"/>
+      <c r="AR4" s="192"/>
+      <c r="AS4" s="192"/>
+      <c r="AT4" s="192"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="191"/>
-      <c r="AW4" s="191"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="191"/>
-      <c r="BW4" s="191"/>
-      <c r="CT4" s="191"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="195"/>
+      <c r="AY4" s="197"/>
+      <c r="AZ4" s="197"/>
+      <c r="BA4" s="197"/>
+      <c r="BB4" s="197"/>
+      <c r="BC4" s="197"/>
+      <c r="BD4" s="197"/>
+      <c r="BE4" s="197"/>
+      <c r="BF4" s="198"/>
+      <c r="BG4" s="198"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="198"/>
-      <c r="B5" s="199" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="197"/>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197"/>
-      <c r="I5" s="197"/>
-      <c r="J5" s="197"/>
-      <c r="K5" s="197"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
-      <c r="N5" s="190"/>
-      <c r="O5" s="190"/>
-      <c r="P5" s="190"/>
-      <c r="Q5" s="190"/>
-      <c r="R5" s="190"/>
-      <c r="S5" s="190"/>
-      <c r="T5" s="190"/>
-      <c r="U5" s="190"/>
-      <c r="V5" s="190"/>
-      <c r="W5" s="189"/>
-      <c r="X5" s="189"/>
-      <c r="Y5" s="189"/>
-      <c r="Z5" s="189"/>
-      <c r="AA5" s="189"/>
-      <c r="AB5" s="187"/>
-      <c r="AC5" s="187"/>
-      <c r="AD5" s="187"/>
-      <c r="AE5" s="187"/>
-      <c r="AF5" s="187"/>
-      <c r="AG5" s="187"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="190"/>
+      <c r="AC5" s="190"/>
+      <c r="AD5" s="190"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="190"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="190"/>
+      <c r="AK5" s="190"/>
+      <c r="AL5" s="190"/>
+      <c r="AM5" s="190"/>
+      <c r="AN5" s="190"/>
+      <c r="AO5" s="190"/>
+      <c r="AP5" s="190"/>
+      <c r="AQ5" s="190"/>
+      <c r="AR5" s="193"/>
+      <c r="AS5" s="193"/>
+      <c r="AT5" s="193"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="191"/>
-      <c r="AW5" s="191"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="191"/>
-      <c r="BW5" s="191"/>
-      <c r="CT5" s="191"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="196"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="197"/>
+      <c r="BA5" s="197"/>
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="199"/>
+      <c r="BG5" s="199"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="199"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="197"/>
-      <c r="H6" s="197"/>
-      <c r="I6" s="197"/>
-      <c r="J6" s="197"/>
-      <c r="K6" s="197"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
-      <c r="N6" s="190"/>
-      <c r="O6" s="190"/>
-      <c r="P6" s="190"/>
-      <c r="Q6" s="190"/>
-      <c r="R6" s="190"/>
-      <c r="S6" s="190"/>
-      <c r="T6" s="190"/>
-      <c r="U6" s="190"/>
-      <c r="V6" s="190"/>
-      <c r="W6" s="189"/>
-      <c r="X6" s="189"/>
-      <c r="Y6" s="189"/>
-      <c r="Z6" s="189"/>
-      <c r="AA6" s="189"/>
-      <c r="AB6" s="187"/>
-      <c r="AC6" s="187"/>
-      <c r="AD6" s="187"/>
-      <c r="AE6" s="187"/>
-      <c r="AF6" s="187"/>
-      <c r="AG6" s="187"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
+      <c r="AB6" s="190"/>
+      <c r="AC6" s="190"/>
+      <c r="AD6" s="190"/>
+      <c r="AE6" s="190"/>
+      <c r="AF6" s="190"/>
+      <c r="AG6" s="190"/>
+      <c r="AH6" s="190"/>
+      <c r="AI6" s="190"/>
+      <c r="AJ6" s="190"/>
+      <c r="AK6" s="190"/>
+      <c r="AL6" s="190"/>
+      <c r="AM6" s="190"/>
+      <c r="AN6" s="190"/>
+      <c r="AO6" s="190"/>
+      <c r="AP6" s="190"/>
+      <c r="AQ6" s="190"/>
+      <c r="AR6" s="193"/>
+      <c r="AS6" s="193"/>
+      <c r="AT6" s="193"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="191"/>
-      <c r="AW6" s="191"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="191"/>
-      <c r="BW6" s="191"/>
-      <c r="CT6" s="191"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="199"/>
+      <c r="BG6" s="199"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="198"/>
-      <c r="B7" s="199" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="197"/>
-      <c r="F7" s="197"/>
-      <c r="G7" s="197"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="197"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="197"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="190"/>
-      <c r="N7" s="190"/>
-      <c r="O7" s="190"/>
-      <c r="P7" s="190"/>
-      <c r="Q7" s="190"/>
-      <c r="R7" s="190"/>
-      <c r="S7" s="190"/>
-      <c r="T7" s="190"/>
-      <c r="U7" s="190"/>
-      <c r="V7" s="190"/>
-      <c r="W7" s="189"/>
-      <c r="X7" s="189"/>
-      <c r="Y7" s="189"/>
-      <c r="Z7" s="189"/>
-      <c r="AA7" s="189"/>
-      <c r="AB7" s="187"/>
-      <c r="AC7" s="187"/>
-      <c r="AD7" s="187"/>
-      <c r="AE7" s="187"/>
-      <c r="AF7" s="187"/>
-      <c r="AG7" s="187"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
+      <c r="AB7" s="190"/>
+      <c r="AC7" s="190"/>
+      <c r="AD7" s="190"/>
+      <c r="AE7" s="190"/>
+      <c r="AF7" s="190"/>
+      <c r="AG7" s="190"/>
+      <c r="AH7" s="190"/>
+      <c r="AI7" s="190"/>
+      <c r="AJ7" s="190"/>
+      <c r="AK7" s="190"/>
+      <c r="AL7" s="190"/>
+      <c r="AM7" s="190"/>
+      <c r="AN7" s="190"/>
+      <c r="AO7" s="190"/>
+      <c r="AP7" s="190"/>
+      <c r="AQ7" s="190"/>
+      <c r="AR7" s="193"/>
+      <c r="AS7" s="193"/>
+      <c r="AT7" s="193"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="191"/>
-      <c r="AW7" s="191"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="191"/>
-      <c r="BW7" s="191"/>
-      <c r="CT7" s="191"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="196"/>
+      <c r="AY7" s="197"/>
+      <c r="AZ7" s="197"/>
+      <c r="BA7" s="197"/>
+      <c r="BB7" s="197"/>
+      <c r="BC7" s="197"/>
+      <c r="BD7" s="197"/>
+      <c r="BE7" s="197"/>
+      <c r="BF7" s="199"/>
+      <c r="BG7" s="199"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="198" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="199" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="199"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="197"/>
-      <c r="K8" s="197"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="190"/>
-      <c r="N8" s="190"/>
-      <c r="O8" s="190"/>
-      <c r="P8" s="190"/>
-      <c r="Q8" s="190"/>
-      <c r="R8" s="190"/>
-      <c r="S8" s="190"/>
-      <c r="T8" s="190"/>
-      <c r="U8" s="190"/>
-      <c r="V8" s="190"/>
-      <c r="W8" s="189"/>
-      <c r="X8" s="189"/>
-      <c r="Y8" s="189"/>
-      <c r="Z8" s="189"/>
-      <c r="AA8" s="189"/>
-      <c r="AB8" s="187"/>
-      <c r="AC8" s="187"/>
-      <c r="AD8" s="187"/>
-      <c r="AE8" s="187"/>
-      <c r="AF8" s="187"/>
-      <c r="AG8" s="187"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
+      <c r="AB8" s="190"/>
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="190"/>
+      <c r="AG8" s="190"/>
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="190"/>
+      <c r="AL8" s="190"/>
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="190"/>
+      <c r="AQ8" s="190"/>
+      <c r="AR8" s="193"/>
+      <c r="AS8" s="193"/>
+      <c r="AT8" s="193"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="191"/>
-      <c r="AW8" s="191"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="191"/>
-      <c r="BW8" s="191"/>
-      <c r="CT8" s="191"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="196"/>
+      <c r="AY8" s="197"/>
+      <c r="AZ8" s="197"/>
+      <c r="BA8" s="197"/>
+      <c r="BB8" s="197"/>
+      <c r="BC8" s="197"/>
+      <c r="BD8" s="197"/>
+      <c r="BE8" s="197"/>
+      <c r="BF8" s="199"/>
+      <c r="BG8" s="199"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="198"/>
-      <c r="B9" s="199" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="199"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="190"/>
-      <c r="M9" s="190"/>
-      <c r="N9" s="190"/>
-      <c r="O9" s="190"/>
-      <c r="P9" s="190"/>
-      <c r="Q9" s="190"/>
-      <c r="R9" s="190"/>
-      <c r="S9" s="190"/>
-      <c r="T9" s="190"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="190"/>
-      <c r="W9" s="189"/>
-      <c r="X9" s="189"/>
-      <c r="Y9" s="189"/>
-      <c r="Z9" s="189"/>
-      <c r="AA9" s="189"/>
-      <c r="AB9" s="187"/>
-      <c r="AC9" s="187"/>
-      <c r="AD9" s="187"/>
-      <c r="AE9" s="187"/>
-      <c r="AF9" s="187"/>
-      <c r="AG9" s="187"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="190"/>
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="190"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="190"/>
+      <c r="AL9" s="190"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="190"/>
+      <c r="AR9" s="193"/>
+      <c r="AS9" s="193"/>
+      <c r="AT9" s="193"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="191"/>
-      <c r="AW9" s="191"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="191"/>
-      <c r="BW9" s="191"/>
-      <c r="CT9" s="191"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="196"/>
+      <c r="AY9" s="197"/>
+      <c r="AZ9" s="197"/>
+      <c r="BA9" s="197"/>
+      <c r="BB9" s="197"/>
+      <c r="BC9" s="197"/>
+      <c r="BD9" s="197"/>
+      <c r="BE9" s="197"/>
+      <c r="BF9" s="199"/>
+      <c r="BG9" s="199"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="199"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
-      <c r="J10" s="197"/>
-      <c r="K10" s="197"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="190"/>
-      <c r="N10" s="190"/>
-      <c r="O10" s="190"/>
-      <c r="P10" s="190"/>
-      <c r="Q10" s="190"/>
-      <c r="R10" s="190"/>
-      <c r="S10" s="190"/>
-      <c r="T10" s="190"/>
-      <c r="U10" s="190"/>
-      <c r="V10" s="190"/>
-      <c r="W10" s="189"/>
-      <c r="X10" s="189"/>
-      <c r="Y10" s="189"/>
-      <c r="Z10" s="189"/>
-      <c r="AA10" s="189"/>
-      <c r="AB10" s="187"/>
-      <c r="AC10" s="187"/>
-      <c r="AD10" s="187"/>
-      <c r="AE10" s="187"/>
-      <c r="AF10" s="187"/>
-      <c r="AG10" s="187"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
+      <c r="AB10" s="190"/>
+      <c r="AC10" s="190"/>
+      <c r="AD10" s="190"/>
+      <c r="AE10" s="190"/>
+      <c r="AF10" s="190"/>
+      <c r="AG10" s="190"/>
+      <c r="AH10" s="190"/>
+      <c r="AI10" s="190"/>
+      <c r="AJ10" s="190"/>
+      <c r="AK10" s="190"/>
+      <c r="AL10" s="190"/>
+      <c r="AM10" s="190"/>
+      <c r="AN10" s="190"/>
+      <c r="AO10" s="190"/>
+      <c r="AP10" s="190"/>
+      <c r="AQ10" s="190"/>
+      <c r="AR10" s="193"/>
+      <c r="AS10" s="193"/>
+      <c r="AT10" s="193"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="191"/>
-      <c r="AW10" s="191"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="191"/>
-      <c r="BW10" s="191"/>
-      <c r="CT10" s="191"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="196"/>
+      <c r="AY10" s="197"/>
+      <c r="AZ10" s="197"/>
+      <c r="BA10" s="197"/>
+      <c r="BB10" s="197"/>
+      <c r="BC10" s="197"/>
+      <c r="BD10" s="197"/>
+      <c r="BE10" s="197"/>
+      <c r="BF10" s="199"/>
+      <c r="BG10" s="199"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="198"/>
-      <c r="B11" s="199" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="197"/>
-      <c r="J11" s="197"/>
-      <c r="K11" s="197"/>
-      <c r="L11" s="190"/>
-      <c r="M11" s="190"/>
-      <c r="N11" s="190"/>
-      <c r="O11" s="190"/>
-      <c r="P11" s="190"/>
-      <c r="Q11" s="190"/>
-      <c r="R11" s="190"/>
-      <c r="S11" s="190"/>
-      <c r="T11" s="190"/>
-      <c r="U11" s="190"/>
-      <c r="V11" s="190"/>
-      <c r="W11" s="189"/>
-      <c r="X11" s="189"/>
-      <c r="Y11" s="189"/>
-      <c r="Z11" s="189"/>
-      <c r="AA11" s="189"/>
-      <c r="AB11" s="188"/>
-      <c r="AC11" s="188"/>
-      <c r="AD11" s="188"/>
-      <c r="AE11" s="188"/>
-      <c r="AF11" s="188"/>
-      <c r="AG11" s="188"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
+      <c r="AB11" s="191"/>
+      <c r="AC11" s="191"/>
+      <c r="AD11" s="191"/>
+      <c r="AE11" s="191"/>
+      <c r="AF11" s="191"/>
+      <c r="AG11" s="191"/>
+      <c r="AH11" s="191"/>
+      <c r="AI11" s="191"/>
+      <c r="AJ11" s="191"/>
+      <c r="AK11" s="191"/>
+      <c r="AL11" s="191"/>
+      <c r="AM11" s="191"/>
+      <c r="AN11" s="191"/>
+      <c r="AO11" s="191"/>
+      <c r="AP11" s="191"/>
+      <c r="AQ11" s="191"/>
+      <c r="AR11" s="194"/>
+      <c r="AS11" s="194"/>
+      <c r="AT11" s="194"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="191"/>
-      <c r="AW11" s="191"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="191"/>
-      <c r="BW11" s="191"/>
-      <c r="CT11" s="191"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="196"/>
+      <c r="AY11" s="197"/>
+      <c r="AZ11" s="197"/>
+      <c r="BA11" s="197"/>
+      <c r="BB11" s="197"/>
+      <c r="BC11" s="197"/>
+      <c r="BD11" s="197"/>
+      <c r="BE11" s="197"/>
+      <c r="BF11" s="199"/>
+      <c r="BG11" s="199"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4104,63 +4169,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5682,13 +5690,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="213" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="214"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5793,9 +5801,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="203"/>
-      <c r="B5" s="201"/>
-      <c r="C5" s="203"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="211"/>
+      <c r="C5" s="201"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5900,11 +5908,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="203"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="203"/>
+      <c r="C6" s="201"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6009,11 +6017,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="203"/>
+      <c r="A7" s="201"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="203"/>
+      <c r="C7" s="201"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6118,11 +6126,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="203"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="203"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6227,11 +6235,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="203"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="203"/>
+      <c r="C9" s="201"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6336,11 +6344,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="203"/>
+      <c r="A10" s="201"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="203"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6445,11 +6453,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="203"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="203"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6554,9 +6562,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="203"/>
+      <c r="A12" s="201"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="206"/>
+      <c r="C12" s="202"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6661,10 +6669,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="207" t="s">
+      <c r="A13" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="208" t="s">
+      <c r="B13" s="216" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6773,8 +6781,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="203"/>
-      <c r="B14" s="209"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="207"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6895,7 +6903,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="203"/>
+      <c r="A15" s="201"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7005,7 +7013,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="203"/>
+      <c r="A16" s="201"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7115,7 +7123,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="203"/>
+      <c r="A17" s="201"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7227,7 +7235,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="203"/>
+      <c r="A18" s="201"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7337,7 +7345,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="203"/>
+      <c r="A19" s="201"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7447,7 +7455,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="203"/>
+      <c r="A20" s="201"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7557,7 +7565,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="206"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7668,7 +7676,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="93"/>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="210" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7778,7 +7786,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="93"/>
-      <c r="B23" s="201"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7885,13 +7893,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="203" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="213">
+      <c r="C24" s="205">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -7999,11 +8007,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="212"/>
+      <c r="A25" s="204"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="203"/>
+      <c r="C25" s="201"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8109,11 +8117,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="212"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="203"/>
+      <c r="C26" s="201"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8219,11 +8227,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="212"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="203"/>
+      <c r="C27" s="201"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8329,11 +8337,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="212"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="203"/>
+      <c r="C28" s="201"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8439,11 +8447,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="212"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="203"/>
+      <c r="C29" s="201"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8549,11 +8557,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="212"/>
+      <c r="A30" s="204"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="203"/>
+      <c r="C30" s="201"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8659,11 +8667,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="212"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="203"/>
+      <c r="C31" s="201"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8769,11 +8777,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="212"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="203"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8879,11 +8887,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="212"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="203"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -8989,11 +8997,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="212"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="203"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9099,11 +9107,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="212"/>
+      <c r="A35" s="204"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="206"/>
+      <c r="C35" s="202"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9209,11 +9217,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="212"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="213">
+      <c r="C36" s="205">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9321,11 +9329,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="212"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="203"/>
+      <c r="C37" s="201"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9431,11 +9439,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="212"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="203"/>
+      <c r="C38" s="201"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9541,11 +9549,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="212"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="203"/>
+      <c r="C39" s="201"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9651,11 +9659,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="212"/>
+      <c r="A40" s="204"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="203"/>
+      <c r="C40" s="201"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9761,11 +9769,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="212"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="203"/>
+      <c r="C41" s="201"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9871,11 +9879,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="212"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="203"/>
+      <c r="C42" s="201"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -9981,11 +9989,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="212"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="203"/>
+      <c r="C43" s="201"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10091,11 +10099,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="212"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="203"/>
+      <c r="C44" s="201"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10201,11 +10209,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="212"/>
+      <c r="A45" s="204"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="203"/>
+      <c r="C45" s="201"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10311,11 +10319,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="212"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="203"/>
+      <c r="C46" s="201"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10421,11 +10429,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="212"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="203"/>
+      <c r="C47" s="201"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10539,11 +10547,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="212"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="203"/>
+      <c r="C48" s="201"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10652,7 +10660,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="111"/>
-      <c r="B49" s="214" t="s">
+      <c r="B49" s="206" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10762,7 +10770,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="116"/>
-      <c r="B50" s="209"/>
+      <c r="B50" s="207"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14193,7 +14201,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="215" t="s">
+      <c r="A81" s="208" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14305,7 +14313,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="203"/>
+      <c r="A82" s="201"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14415,7 +14423,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="203"/>
+      <c r="A83" s="201"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14525,7 +14533,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="203"/>
+      <c r="A84" s="201"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14635,7 +14643,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="203"/>
+      <c r="A85" s="201"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14745,7 +14753,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="203"/>
+      <c r="A86" s="201"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14855,7 +14863,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="203"/>
+      <c r="A87" s="201"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -14967,7 +14975,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="203"/>
+      <c r="A88" s="201"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15077,7 +15085,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="203"/>
+      <c r="A89" s="201"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15187,7 +15195,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="203"/>
+      <c r="A90" s="201"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15297,11 +15305,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="203"/>
+      <c r="A91" s="201"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="216"/>
+      <c r="C91" s="209"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15407,11 +15415,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="203"/>
+      <c r="A92" s="201"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="203"/>
+      <c r="C92" s="201"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15517,11 +15525,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="206"/>
+      <c r="A93" s="202"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="203"/>
+      <c r="C93" s="201"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15745,7 +15753,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="210" t="s">
+      <c r="A95" s="200" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15857,7 +15865,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="203"/>
+      <c r="A96" s="201"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -15967,7 +15975,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="203"/>
+      <c r="A97" s="201"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16077,7 +16085,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="203"/>
+      <c r="A98" s="201"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16187,7 +16195,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="203"/>
+      <c r="A99" s="201"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16297,7 +16305,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="203"/>
+      <c r="A100" s="201"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16407,7 +16415,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="203"/>
+      <c r="A101" s="201"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16517,7 +16525,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="203"/>
+      <c r="A102" s="201"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16627,7 +16635,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="203"/>
+      <c r="A103" s="201"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16739,7 +16747,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="203"/>
+      <c r="A104" s="201"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16849,7 +16857,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="203"/>
+      <c r="A105" s="201"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -16967,7 +16975,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="203"/>
+      <c r="A106" s="201"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17077,7 +17085,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="203"/>
+      <c r="A107" s="201"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17187,7 +17195,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="203"/>
+      <c r="A108" s="201"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17297,7 +17305,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="203"/>
+      <c r="A109" s="201"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17407,7 +17415,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="203"/>
+      <c r="A110" s="201"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17517,7 +17525,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="203"/>
+      <c r="A111" s="201"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17627,7 +17635,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="203"/>
+      <c r="A112" s="201"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17737,7 +17745,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="203"/>
+      <c r="A113" s="201"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17847,7 +17855,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="203"/>
+      <c r="A114" s="201"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17957,7 +17965,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="203"/>
+      <c r="A115" s="201"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18067,7 +18075,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="203"/>
+      <c r="A116" s="201"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18193,7 +18201,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="203"/>
+      <c r="A117" s="201"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18303,7 +18311,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="206"/>
+      <c r="A118" s="202"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25674,6 +25682,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25681,12 +25695,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 10-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0E8FD6-BABD-44E1-B18E-514D2ECC5AE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA1DA02-5744-4401-A142-CADA969DB65F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="163">
   <si>
     <t>S</t>
   </si>
@@ -689,7 +689,10 @@
     <t>Palestra de boas práticas em apresentação pela ThoughtWorks.
 Finalização de integração e navegação das páginas construídas.
 Reunião com os Scrum Masters e POs para alinhamento da sinergia dos grupos.
-Montagem da apresentação do andamento dos projetos para a coordenação</t>
+Montagem da apresentação do andamento dos projetos para a coordenação e direção</t>
+  </si>
+  <si>
+    <t>Montagem da apresentação do andamento dos projetos para a coordenação e direção</t>
   </si>
 </sst>
 </file>
@@ -2201,17 +2204,47 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2228,50 +2261,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2282,30 +2305,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2812,10 +2815,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X4" sqref="X4:X11"/>
+      <selection pane="bottomRight" activeCell="Y4" sqref="Y4:Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -3124,110 +3127,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="192"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
+      <c r="AF2" s="192"/>
+      <c r="AG2" s="192"/>
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="192"/>
+      <c r="AJ2" s="192"/>
+      <c r="AK2" s="192"/>
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="192"/>
+      <c r="AQ2" s="192"/>
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="192"/>
+      <c r="AV2" s="192"/>
+      <c r="AW2" s="192"/>
+      <c r="AX2" s="193"/>
+      <c r="AY2" s="193"/>
+      <c r="AZ2" s="193"/>
+      <c r="BA2" s="193"/>
+      <c r="BB2" s="193"/>
+      <c r="BC2" s="193"/>
+      <c r="BD2" s="193"/>
+      <c r="BE2" s="193"/>
+      <c r="BF2" s="193"/>
+      <c r="BG2" s="193"/>
+      <c r="BH2" s="193"/>
+      <c r="BI2" s="193"/>
+      <c r="BJ2" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="192"/>
+      <c r="BL2" s="192"/>
+      <c r="BM2" s="192"/>
+      <c r="BN2" s="192"/>
+      <c r="BO2" s="192"/>
+      <c r="BP2" s="192"/>
+      <c r="BQ2" s="192"/>
+      <c r="BR2" s="192"/>
+      <c r="BS2" s="192"/>
+      <c r="BT2" s="192"/>
+      <c r="BU2" s="192"/>
+      <c r="BV2" s="192"/>
+      <c r="BW2" s="192"/>
+      <c r="BX2" s="194"/>
+      <c r="BY2" s="194"/>
+      <c r="BZ2" s="194"/>
+      <c r="CA2" s="194"/>
+      <c r="CB2" s="194"/>
+      <c r="CC2" s="194"/>
+      <c r="CD2" s="194"/>
+      <c r="CE2" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="196"/>
+      <c r="CG2" s="196"/>
+      <c r="CH2" s="196"/>
+      <c r="CI2" s="196"/>
+      <c r="CJ2" s="196"/>
+      <c r="CK2" s="196"/>
+      <c r="CL2" s="196"/>
+      <c r="CM2" s="196"/>
+      <c r="CN2" s="196"/>
+      <c r="CO2" s="196"/>
+      <c r="CP2" s="196"/>
+      <c r="CQ2" s="196"/>
+      <c r="CR2" s="196"/>
+      <c r="CS2" s="196"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1">
@@ -3523,620 +3526,597 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="199"/>
+      <c r="D4" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="197" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="197" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="197" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="197" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="197" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="197" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="190" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="190" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="190" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="190" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="190" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="190" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="190" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188"/>
-      <c r="Y4" s="188"/>
-      <c r="Z4" s="188"/>
-      <c r="AA4" s="188"/>
-      <c r="AB4" s="189"/>
-      <c r="AC4" s="189"/>
-      <c r="AD4" s="189"/>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="189"/>
-      <c r="AG4" s="189"/>
-      <c r="AH4" s="189"/>
-      <c r="AI4" s="189"/>
-      <c r="AJ4" s="189"/>
-      <c r="AK4" s="189"/>
-      <c r="AL4" s="189"/>
-      <c r="AM4" s="189"/>
-      <c r="AN4" s="189"/>
-      <c r="AO4" s="189"/>
-      <c r="AP4" s="189"/>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
+      <c r="X4" s="189" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y4" s="189"/>
+      <c r="Z4" s="189"/>
+      <c r="AA4" s="189"/>
+      <c r="AB4" s="186"/>
+      <c r="AC4" s="186"/>
+      <c r="AD4" s="186"/>
+      <c r="AE4" s="186"/>
+      <c r="AF4" s="186"/>
+      <c r="AG4" s="186"/>
+      <c r="AH4" s="186"/>
+      <c r="AI4" s="186"/>
+      <c r="AJ4" s="186"/>
+      <c r="AK4" s="186"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="195"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="198"/>
-      <c r="BG4" s="198"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="191"/>
+      <c r="AW4" s="191"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="191"/>
+      <c r="BW4" s="191"/>
+      <c r="CT4" s="191"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="198"/>
+      <c r="B5" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="190"/>
-      <c r="AC5" s="190"/>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="190"/>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="190"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="190"/>
-      <c r="AP5" s="190"/>
-      <c r="AQ5" s="190"/>
-      <c r="AR5" s="193"/>
-      <c r="AS5" s="193"/>
-      <c r="AT5" s="193"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="197"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="197"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="190"/>
+      <c r="P5" s="190"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="190"/>
+      <c r="S5" s="190"/>
+      <c r="T5" s="190"/>
+      <c r="U5" s="190"/>
+      <c r="V5" s="190"/>
+      <c r="W5" s="189"/>
+      <c r="X5" s="189"/>
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="189"/>
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="187"/>
+      <c r="AC5" s="187"/>
+      <c r="AD5" s="187"/>
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="187"/>
+      <c r="AG5" s="187"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="196"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="197"/>
-      <c r="BA5" s="197"/>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="199"/>
-      <c r="BG5" s="199"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="191"/>
+      <c r="AW5" s="191"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="191"/>
+      <c r="BW5" s="191"/>
+      <c r="CT5" s="191"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="198"/>
+      <c r="B6" s="199" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="190"/>
-      <c r="AC6" s="190"/>
-      <c r="AD6" s="190"/>
-      <c r="AE6" s="190"/>
-      <c r="AF6" s="190"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="190"/>
-      <c r="AI6" s="190"/>
-      <c r="AJ6" s="190"/>
-      <c r="AK6" s="190"/>
-      <c r="AL6" s="190"/>
-      <c r="AM6" s="190"/>
-      <c r="AN6" s="190"/>
-      <c r="AO6" s="190"/>
-      <c r="AP6" s="190"/>
-      <c r="AQ6" s="190"/>
-      <c r="AR6" s="193"/>
-      <c r="AS6" s="193"/>
-      <c r="AT6" s="193"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="N6" s="190"/>
+      <c r="O6" s="190"/>
+      <c r="P6" s="190"/>
+      <c r="Q6" s="190"/>
+      <c r="R6" s="190"/>
+      <c r="S6" s="190"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="190"/>
+      <c r="V6" s="190"/>
+      <c r="W6" s="189"/>
+      <c r="X6" s="189"/>
+      <c r="Y6" s="189"/>
+      <c r="Z6" s="189"/>
+      <c r="AA6" s="189"/>
+      <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
+      <c r="AD6" s="187"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="187"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="197"/>
-      <c r="AZ6" s="197"/>
-      <c r="BA6" s="197"/>
-      <c r="BB6" s="197"/>
-      <c r="BC6" s="197"/>
-      <c r="BD6" s="197"/>
-      <c r="BE6" s="197"/>
-      <c r="BF6" s="199"/>
-      <c r="BG6" s="199"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="191"/>
+      <c r="AW6" s="191"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="191"/>
+      <c r="BW6" s="191"/>
+      <c r="CT6" s="191"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="198"/>
+      <c r="B7" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="190"/>
-      <c r="AC7" s="190"/>
-      <c r="AD7" s="190"/>
-      <c r="AE7" s="190"/>
-      <c r="AF7" s="190"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="190"/>
-      <c r="AI7" s="190"/>
-      <c r="AJ7" s="190"/>
-      <c r="AK7" s="190"/>
-      <c r="AL7" s="190"/>
-      <c r="AM7" s="190"/>
-      <c r="AN7" s="190"/>
-      <c r="AO7" s="190"/>
-      <c r="AP7" s="190"/>
-      <c r="AQ7" s="190"/>
-      <c r="AR7" s="193"/>
-      <c r="AS7" s="193"/>
-      <c r="AT7" s="193"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="197"/>
+      <c r="F7" s="197"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
+      <c r="Q7" s="190"/>
+      <c r="R7" s="190"/>
+      <c r="S7" s="190"/>
+      <c r="T7" s="190"/>
+      <c r="U7" s="190"/>
+      <c r="V7" s="190"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="189"/>
+      <c r="Y7" s="189"/>
+      <c r="Z7" s="189"/>
+      <c r="AA7" s="189"/>
+      <c r="AB7" s="187"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="196"/>
-      <c r="AY7" s="197"/>
-      <c r="AZ7" s="197"/>
-      <c r="BA7" s="197"/>
-      <c r="BB7" s="197"/>
-      <c r="BC7" s="197"/>
-      <c r="BD7" s="197"/>
-      <c r="BE7" s="197"/>
-      <c r="BF7" s="199"/>
-      <c r="BG7" s="199"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="191"/>
+      <c r="AW7" s="191"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="191"/>
+      <c r="BW7" s="191"/>
+      <c r="CT7" s="191"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="190"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="193"/>
-      <c r="AS8" s="193"/>
-      <c r="AT8" s="193"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="197"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="190"/>
+      <c r="R8" s="190"/>
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="190"/>
+      <c r="W8" s="189"/>
+      <c r="X8" s="189"/>
+      <c r="Y8" s="189"/>
+      <c r="Z8" s="189"/>
+      <c r="AA8" s="189"/>
+      <c r="AB8" s="187"/>
+      <c r="AC8" s="187"/>
+      <c r="AD8" s="187"/>
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="187"/>
+      <c r="AG8" s="187"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="196"/>
-      <c r="AY8" s="197"/>
-      <c r="AZ8" s="197"/>
-      <c r="BA8" s="197"/>
-      <c r="BB8" s="197"/>
-      <c r="BC8" s="197"/>
-      <c r="BD8" s="197"/>
-      <c r="BE8" s="197"/>
-      <c r="BF8" s="199"/>
-      <c r="BG8" s="199"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="191"/>
+      <c r="AW8" s="191"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="191"/>
+      <c r="BW8" s="191"/>
+      <c r="CT8" s="191"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="198"/>
+      <c r="B9" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
-      <c r="AB9" s="190"/>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="190"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="190"/>
-      <c r="AL9" s="190"/>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="190"/>
-      <c r="AQ9" s="190"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="197"/>
+      <c r="I9" s="197"/>
+      <c r="J9" s="197"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="190"/>
+      <c r="W9" s="189"/>
+      <c r="X9" s="189"/>
+      <c r="Y9" s="189"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="189"/>
+      <c r="AB9" s="187"/>
+      <c r="AC9" s="187"/>
+      <c r="AD9" s="187"/>
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="187"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="196"/>
-      <c r="AY9" s="197"/>
-      <c r="AZ9" s="197"/>
-      <c r="BA9" s="197"/>
-      <c r="BB9" s="197"/>
-      <c r="BC9" s="197"/>
-      <c r="BD9" s="197"/>
-      <c r="BE9" s="197"/>
-      <c r="BF9" s="199"/>
-      <c r="BG9" s="199"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="191"/>
+      <c r="AW9" s="191"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="191"/>
+      <c r="BW9" s="191"/>
+      <c r="CT9" s="191"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="198"/>
+      <c r="B10" s="199" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="190"/>
-      <c r="AC10" s="190"/>
-      <c r="AD10" s="190"/>
-      <c r="AE10" s="190"/>
-      <c r="AF10" s="190"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="190"/>
-      <c r="AI10" s="190"/>
-      <c r="AJ10" s="190"/>
-      <c r="AK10" s="190"/>
-      <c r="AL10" s="190"/>
-      <c r="AM10" s="190"/>
-      <c r="AN10" s="190"/>
-      <c r="AO10" s="190"/>
-      <c r="AP10" s="190"/>
-      <c r="AQ10" s="190"/>
-      <c r="AR10" s="193"/>
-      <c r="AS10" s="193"/>
-      <c r="AT10" s="193"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="197"/>
+      <c r="K10" s="197"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="190"/>
+      <c r="O10" s="190"/>
+      <c r="P10" s="190"/>
+      <c r="Q10" s="190"/>
+      <c r="R10" s="190"/>
+      <c r="S10" s="190"/>
+      <c r="T10" s="190"/>
+      <c r="U10" s="190"/>
+      <c r="V10" s="190"/>
+      <c r="W10" s="189"/>
+      <c r="X10" s="189"/>
+      <c r="Y10" s="189"/>
+      <c r="Z10" s="189"/>
+      <c r="AA10" s="189"/>
+      <c r="AB10" s="187"/>
+      <c r="AC10" s="187"/>
+      <c r="AD10" s="187"/>
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="187"/>
+      <c r="AG10" s="187"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="196"/>
-      <c r="AY10" s="197"/>
-      <c r="AZ10" s="197"/>
-      <c r="BA10" s="197"/>
-      <c r="BB10" s="197"/>
-      <c r="BC10" s="197"/>
-      <c r="BD10" s="197"/>
-      <c r="BE10" s="197"/>
-      <c r="BF10" s="199"/>
-      <c r="BG10" s="199"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="191"/>
+      <c r="AW10" s="191"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="191"/>
+      <c r="BW10" s="191"/>
+      <c r="CT10" s="191"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="198"/>
+      <c r="B11" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="191"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="191"/>
-      <c r="AE11" s="191"/>
-      <c r="AF11" s="191"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="191"/>
-      <c r="AI11" s="191"/>
-      <c r="AJ11" s="191"/>
-      <c r="AK11" s="191"/>
-      <c r="AL11" s="191"/>
-      <c r="AM11" s="191"/>
-      <c r="AN11" s="191"/>
-      <c r="AO11" s="191"/>
-      <c r="AP11" s="191"/>
-      <c r="AQ11" s="191"/>
-      <c r="AR11" s="194"/>
-      <c r="AS11" s="194"/>
-      <c r="AT11" s="194"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
+      <c r="N11" s="190"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="190"/>
+      <c r="Q11" s="190"/>
+      <c r="R11" s="190"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="190"/>
+      <c r="U11" s="190"/>
+      <c r="V11" s="190"/>
+      <c r="W11" s="189"/>
+      <c r="X11" s="189"/>
+      <c r="Y11" s="189"/>
+      <c r="Z11" s="189"/>
+      <c r="AA11" s="189"/>
+      <c r="AB11" s="188"/>
+      <c r="AC11" s="188"/>
+      <c r="AD11" s="188"/>
+      <c r="AE11" s="188"/>
+      <c r="AF11" s="188"/>
+      <c r="AG11" s="188"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="196"/>
-      <c r="AY11" s="197"/>
-      <c r="AZ11" s="197"/>
-      <c r="BA11" s="197"/>
-      <c r="BB11" s="197"/>
-      <c r="BC11" s="197"/>
-      <c r="BD11" s="197"/>
-      <c r="BE11" s="197"/>
-      <c r="BF11" s="199"/>
-      <c r="BG11" s="199"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="191"/>
+      <c r="AW11" s="191"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="191"/>
+      <c r="BW11" s="191"/>
+      <c r="CT11" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4153,22 +4133,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5690,13 +5695,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1">
-      <c r="A4" s="212" t="s">
+      <c r="A4" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="214"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5801,9 +5806,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="201"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="201"/>
+      <c r="A5" s="203"/>
+      <c r="B5" s="201"/>
+      <c r="C5" s="203"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5908,11 +5913,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A6" s="201"/>
+      <c r="A6" s="203"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="201"/>
+      <c r="C6" s="203"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6017,11 +6022,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A7" s="201"/>
+      <c r="A7" s="203"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="201"/>
+      <c r="C7" s="203"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6126,11 +6131,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A8" s="201"/>
+      <c r="A8" s="203"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="201"/>
+      <c r="C8" s="203"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6235,11 +6240,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A9" s="201"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="201"/>
+      <c r="C9" s="203"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6344,11 +6349,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A10" s="201"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="203"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6453,11 +6458,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A11" s="201"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="203"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6562,9 +6567,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A12" s="201"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="202"/>
+      <c r="C12" s="206"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6669,10 +6674,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="208" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6781,8 +6786,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1">
-      <c r="A14" s="201"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6903,7 +6908,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A15" s="201"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7013,7 +7018,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A16" s="201"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7123,7 +7128,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A17" s="201"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7235,7 +7240,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A18" s="201"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7345,7 +7350,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A19" s="201"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7455,7 +7460,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A20" s="201"/>
+      <c r="A20" s="203"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7565,7 +7570,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A21" s="202"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7676,7 +7681,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1">
       <c r="A22" s="93"/>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="200" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7786,7 +7791,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
       <c r="A23" s="93"/>
-      <c r="B23" s="211"/>
+      <c r="B23" s="201"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7893,13 +7898,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A24" s="203" t="s">
+      <c r="A24" s="211" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="205">
+      <c r="C24" s="213">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8007,11 +8012,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A25" s="204"/>
+      <c r="A25" s="212"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="201"/>
+      <c r="C25" s="203"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8117,11 +8122,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A26" s="204"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="203"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8227,11 +8232,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A27" s="204"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="201"/>
+      <c r="C27" s="203"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8337,11 +8342,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A28" s="204"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="201"/>
+      <c r="C28" s="203"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8447,11 +8452,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A29" s="204"/>
+      <c r="A29" s="212"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="201"/>
+      <c r="C29" s="203"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8557,11 +8562,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A30" s="204"/>
+      <c r="A30" s="212"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="201"/>
+      <c r="C30" s="203"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8667,11 +8672,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A31" s="204"/>
+      <c r="A31" s="212"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="201"/>
+      <c r="C31" s="203"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8777,11 +8782,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A32" s="204"/>
+      <c r="A32" s="212"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="201"/>
+      <c r="C32" s="203"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8887,11 +8892,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A33" s="204"/>
+      <c r="A33" s="212"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="201"/>
+      <c r="C33" s="203"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -8997,11 +9002,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="204"/>
+      <c r="A34" s="212"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="201"/>
+      <c r="C34" s="203"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9107,11 +9112,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A35" s="204"/>
+      <c r="A35" s="212"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="202"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9217,11 +9222,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A36" s="204"/>
+      <c r="A36" s="212"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="205">
+      <c r="C36" s="213">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9329,11 +9334,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A37" s="204"/>
+      <c r="A37" s="212"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="201"/>
+      <c r="C37" s="203"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9439,11 +9444,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A38" s="204"/>
+      <c r="A38" s="212"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="201"/>
+      <c r="C38" s="203"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9549,11 +9554,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A39" s="204"/>
+      <c r="A39" s="212"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="201"/>
+      <c r="C39" s="203"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9659,11 +9664,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A40" s="204"/>
+      <c r="A40" s="212"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="201"/>
+      <c r="C40" s="203"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9769,11 +9774,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A41" s="204"/>
+      <c r="A41" s="212"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="201"/>
+      <c r="C41" s="203"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9879,11 +9884,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A42" s="204"/>
+      <c r="A42" s="212"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="201"/>
+      <c r="C42" s="203"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -9989,11 +9994,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A43" s="204"/>
+      <c r="A43" s="212"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="201"/>
+      <c r="C43" s="203"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10099,11 +10104,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A44" s="204"/>
+      <c r="A44" s="212"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="201"/>
+      <c r="C44" s="203"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10209,11 +10214,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1">
-      <c r="A45" s="204"/>
+      <c r="A45" s="212"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10319,11 +10324,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="204"/>
+      <c r="A46" s="212"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="201"/>
+      <c r="C46" s="203"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10429,11 +10434,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="204"/>
+      <c r="A47" s="212"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="201"/>
+      <c r="C47" s="203"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10547,11 +10552,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A48" s="204"/>
+      <c r="A48" s="212"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="201"/>
+      <c r="C48" s="203"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10660,7 +10665,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1">
       <c r="A49" s="111"/>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="214" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10770,7 +10775,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1">
       <c r="A50" s="116"/>
-      <c r="B50" s="207"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14201,7 +14206,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A81" s="208" t="s">
+      <c r="A81" s="215" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14313,7 +14318,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A82" s="201"/>
+      <c r="A82" s="203"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14423,7 +14428,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A83" s="201"/>
+      <c r="A83" s="203"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14533,7 +14538,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A84" s="201"/>
+      <c r="A84" s="203"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14643,7 +14648,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A85" s="201"/>
+      <c r="A85" s="203"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14753,7 +14758,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A86" s="201"/>
+      <c r="A86" s="203"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14863,7 +14868,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A87" s="201"/>
+      <c r="A87" s="203"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -14975,7 +14980,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A88" s="201"/>
+      <c r="A88" s="203"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15085,7 +15090,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A89" s="201"/>
+      <c r="A89" s="203"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15195,7 +15200,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1">
-      <c r="A90" s="201"/>
+      <c r="A90" s="203"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15305,11 +15310,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1">
-      <c r="A91" s="201"/>
+      <c r="A91" s="203"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="209"/>
+      <c r="C91" s="216"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15415,11 +15420,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A92" s="201"/>
+      <c r="A92" s="203"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="203"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15525,11 +15530,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A93" s="202"/>
+      <c r="A93" s="206"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="201"/>
+      <c r="C93" s="203"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15753,7 +15758,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1">
-      <c r="A95" s="200" t="s">
+      <c r="A95" s="210" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15865,7 +15870,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A96" s="201"/>
+      <c r="A96" s="203"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -15975,7 +15980,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1">
-      <c r="A97" s="201"/>
+      <c r="A97" s="203"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16085,7 +16090,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1">
-      <c r="A98" s="201"/>
+      <c r="A98" s="203"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16195,7 +16200,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1">
-      <c r="A99" s="201"/>
+      <c r="A99" s="203"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16305,7 +16310,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1">
-      <c r="A100" s="201"/>
+      <c r="A100" s="203"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16415,7 +16420,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1">
-      <c r="A101" s="201"/>
+      <c r="A101" s="203"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16525,7 +16530,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1">
-      <c r="A102" s="201"/>
+      <c r="A102" s="203"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16635,7 +16640,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1">
-      <c r="A103" s="201"/>
+      <c r="A103" s="203"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16747,7 +16752,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1">
-      <c r="A104" s="201"/>
+      <c r="A104" s="203"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16857,7 +16862,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A105" s="201"/>
+      <c r="A105" s="203"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -16975,7 +16980,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A106" s="201"/>
+      <c r="A106" s="203"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17085,7 +17090,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1">
-      <c r="A107" s="201"/>
+      <c r="A107" s="203"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17195,7 +17200,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1">
-      <c r="A108" s="201"/>
+      <c r="A108" s="203"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17305,7 +17310,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1">
-      <c r="A109" s="201"/>
+      <c r="A109" s="203"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17415,7 +17420,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1">
-      <c r="A110" s="201"/>
+      <c r="A110" s="203"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17525,7 +17530,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1">
-      <c r="A111" s="201"/>
+      <c r="A111" s="203"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17635,7 +17640,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1">
-      <c r="A112" s="201"/>
+      <c r="A112" s="203"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17745,7 +17750,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1">
-      <c r="A113" s="201"/>
+      <c r="A113" s="203"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17855,7 +17860,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1">
-      <c r="A114" s="201"/>
+      <c r="A114" s="203"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17965,7 +17970,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A115" s="201"/>
+      <c r="A115" s="203"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18075,7 +18080,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A116" s="201"/>
+      <c r="A116" s="203"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18201,7 +18206,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1">
-      <c r="A117" s="201"/>
+      <c r="A117" s="203"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18311,7 +18316,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A118" s="202"/>
+      <c r="A118" s="206"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25682,12 +25687,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25695,6 +25694,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 12-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD74A2E1-7D73-4382-9792-800BBE75B7FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE27D4-B38C-4320-B914-C8F71C5F0932}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
   <si>
     <t>S</t>
   </si>
@@ -696,6 +696,10 @@
   </si>
   <si>
     <t>Apresentação do andamento dos projetos para a coordenação</t>
+  </si>
+  <si>
+    <t>Sprint Review
+Lógica de leitura e escrita em console</t>
   </si>
 </sst>
 </file>
@@ -1874,7 +1878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2221,17 +2225,47 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2248,50 +2282,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2302,30 +2326,13 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2835,7 +2842,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4:Z11"/>
+      <selection pane="bottomRight" activeCell="AA4" sqref="AA4:AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3144,110 +3151,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="192"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
+      <c r="AF2" s="192"/>
+      <c r="AG2" s="192"/>
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="192"/>
+      <c r="AJ2" s="192"/>
+      <c r="AK2" s="192"/>
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="192"/>
+      <c r="AQ2" s="192"/>
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="192"/>
+      <c r="AV2" s="192"/>
+      <c r="AW2" s="192"/>
+      <c r="AX2" s="193"/>
+      <c r="AY2" s="193"/>
+      <c r="AZ2" s="193"/>
+      <c r="BA2" s="193"/>
+      <c r="BB2" s="193"/>
+      <c r="BC2" s="193"/>
+      <c r="BD2" s="193"/>
+      <c r="BE2" s="193"/>
+      <c r="BF2" s="193"/>
+      <c r="BG2" s="193"/>
+      <c r="BH2" s="193"/>
+      <c r="BI2" s="193"/>
+      <c r="BJ2" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="192"/>
+      <c r="BL2" s="192"/>
+      <c r="BM2" s="192"/>
+      <c r="BN2" s="192"/>
+      <c r="BO2" s="192"/>
+      <c r="BP2" s="192"/>
+      <c r="BQ2" s="192"/>
+      <c r="BR2" s="192"/>
+      <c r="BS2" s="192"/>
+      <c r="BT2" s="192"/>
+      <c r="BU2" s="192"/>
+      <c r="BV2" s="192"/>
+      <c r="BW2" s="192"/>
+      <c r="BX2" s="194"/>
+      <c r="BY2" s="194"/>
+      <c r="BZ2" s="194"/>
+      <c r="CA2" s="194"/>
+      <c r="CB2" s="194"/>
+      <c r="CC2" s="194"/>
+      <c r="CD2" s="194"/>
+      <c r="CE2" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="196"/>
+      <c r="CG2" s="196"/>
+      <c r="CH2" s="196"/>
+      <c r="CI2" s="196"/>
+      <c r="CJ2" s="196"/>
+      <c r="CK2" s="196"/>
+      <c r="CL2" s="196"/>
+      <c r="CM2" s="196"/>
+      <c r="CN2" s="196"/>
+      <c r="CO2" s="196"/>
+      <c r="CP2" s="196"/>
+      <c r="CQ2" s="196"/>
+      <c r="CR2" s="196"/>
+      <c r="CS2" s="196"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3543,624 +3550,601 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="199"/>
+      <c r="D4" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="197" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="197" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="197" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="197" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="197" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="197" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="190" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="190" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="190" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="190" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="190" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="190" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="190" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="217" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188" t="s">
+      <c r="X4" s="217" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="188" t="s">
+      <c r="Y4" s="217" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="188"/>
-      <c r="AA4" s="188"/>
-      <c r="AB4" s="189"/>
-      <c r="AC4" s="189"/>
-      <c r="AD4" s="189"/>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="189"/>
-      <c r="AG4" s="189"/>
-      <c r="AH4" s="189"/>
-      <c r="AI4" s="189"/>
-      <c r="AJ4" s="189"/>
-      <c r="AK4" s="189"/>
-      <c r="AL4" s="189"/>
-      <c r="AM4" s="189"/>
-      <c r="AN4" s="189"/>
-      <c r="AO4" s="189"/>
-      <c r="AP4" s="189"/>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
+      <c r="Z4" s="217" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA4" s="189"/>
+      <c r="AB4" s="186"/>
+      <c r="AC4" s="186"/>
+      <c r="AD4" s="186"/>
+      <c r="AE4" s="186"/>
+      <c r="AF4" s="186"/>
+      <c r="AG4" s="186"/>
+      <c r="AH4" s="186"/>
+      <c r="AI4" s="186"/>
+      <c r="AJ4" s="186"/>
+      <c r="AK4" s="186"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="195"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="198"/>
-      <c r="BG4" s="198"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="191"/>
+      <c r="AW4" s="191"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="191"/>
+      <c r="BW4" s="191"/>
+      <c r="CT4" s="191"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="198"/>
+      <c r="B5" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="190"/>
-      <c r="AC5" s="190"/>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="190"/>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="190"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="190"/>
-      <c r="AP5" s="190"/>
-      <c r="AQ5" s="190"/>
-      <c r="AR5" s="193"/>
-      <c r="AS5" s="193"/>
-      <c r="AT5" s="193"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="197"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="197"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="190"/>
+      <c r="P5" s="190"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="190"/>
+      <c r="S5" s="190"/>
+      <c r="T5" s="190"/>
+      <c r="U5" s="190"/>
+      <c r="V5" s="190"/>
+      <c r="W5" s="217"/>
+      <c r="X5" s="217"/>
+      <c r="Y5" s="217"/>
+      <c r="Z5" s="217"/>
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="187"/>
+      <c r="AC5" s="187"/>
+      <c r="AD5" s="187"/>
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="187"/>
+      <c r="AG5" s="187"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="196"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="197"/>
-      <c r="BA5" s="197"/>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="199"/>
-      <c r="BG5" s="199"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="191"/>
+      <c r="AW5" s="191"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="191"/>
+      <c r="BW5" s="191"/>
+      <c r="CT5" s="191"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="198"/>
+      <c r="B6" s="199" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="190"/>
-      <c r="AC6" s="190"/>
-      <c r="AD6" s="190"/>
-      <c r="AE6" s="190"/>
-      <c r="AF6" s="190"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="190"/>
-      <c r="AI6" s="190"/>
-      <c r="AJ6" s="190"/>
-      <c r="AK6" s="190"/>
-      <c r="AL6" s="190"/>
-      <c r="AM6" s="190"/>
-      <c r="AN6" s="190"/>
-      <c r="AO6" s="190"/>
-      <c r="AP6" s="190"/>
-      <c r="AQ6" s="190"/>
-      <c r="AR6" s="193"/>
-      <c r="AS6" s="193"/>
-      <c r="AT6" s="193"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="N6" s="190"/>
+      <c r="O6" s="190"/>
+      <c r="P6" s="190"/>
+      <c r="Q6" s="190"/>
+      <c r="R6" s="190"/>
+      <c r="S6" s="190"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="190"/>
+      <c r="V6" s="190"/>
+      <c r="W6" s="217"/>
+      <c r="X6" s="217"/>
+      <c r="Y6" s="217"/>
+      <c r="Z6" s="217"/>
+      <c r="AA6" s="189"/>
+      <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
+      <c r="AD6" s="187"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="187"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="197"/>
-      <c r="AZ6" s="197"/>
-      <c r="BA6" s="197"/>
-      <c r="BB6" s="197"/>
-      <c r="BC6" s="197"/>
-      <c r="BD6" s="197"/>
-      <c r="BE6" s="197"/>
-      <c r="BF6" s="199"/>
-      <c r="BG6" s="199"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="191"/>
+      <c r="AW6" s="191"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="191"/>
+      <c r="BW6" s="191"/>
+      <c r="CT6" s="191"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="198"/>
+      <c r="B7" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="190"/>
-      <c r="AC7" s="190"/>
-      <c r="AD7" s="190"/>
-      <c r="AE7" s="190"/>
-      <c r="AF7" s="190"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="190"/>
-      <c r="AI7" s="190"/>
-      <c r="AJ7" s="190"/>
-      <c r="AK7" s="190"/>
-      <c r="AL7" s="190"/>
-      <c r="AM7" s="190"/>
-      <c r="AN7" s="190"/>
-      <c r="AO7" s="190"/>
-      <c r="AP7" s="190"/>
-      <c r="AQ7" s="190"/>
-      <c r="AR7" s="193"/>
-      <c r="AS7" s="193"/>
-      <c r="AT7" s="193"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="197"/>
+      <c r="F7" s="197"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
+      <c r="Q7" s="190"/>
+      <c r="R7" s="190"/>
+      <c r="S7" s="190"/>
+      <c r="T7" s="190"/>
+      <c r="U7" s="190"/>
+      <c r="V7" s="190"/>
+      <c r="W7" s="217"/>
+      <c r="X7" s="217"/>
+      <c r="Y7" s="217"/>
+      <c r="Z7" s="217"/>
+      <c r="AA7" s="189"/>
+      <c r="AB7" s="187"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="196"/>
-      <c r="AY7" s="197"/>
-      <c r="AZ7" s="197"/>
-      <c r="BA7" s="197"/>
-      <c r="BB7" s="197"/>
-      <c r="BC7" s="197"/>
-      <c r="BD7" s="197"/>
-      <c r="BE7" s="197"/>
-      <c r="BF7" s="199"/>
-      <c r="BG7" s="199"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="191"/>
+      <c r="AW7" s="191"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="191"/>
+      <c r="BW7" s="191"/>
+      <c r="CT7" s="191"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="190"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="193"/>
-      <c r="AS8" s="193"/>
-      <c r="AT8" s="193"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="197"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="190"/>
+      <c r="R8" s="190"/>
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="190"/>
+      <c r="W8" s="217"/>
+      <c r="X8" s="217"/>
+      <c r="Y8" s="217"/>
+      <c r="Z8" s="217"/>
+      <c r="AA8" s="189"/>
+      <c r="AB8" s="187"/>
+      <c r="AC8" s="187"/>
+      <c r="AD8" s="187"/>
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="187"/>
+      <c r="AG8" s="187"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="196"/>
-      <c r="AY8" s="197"/>
-      <c r="AZ8" s="197"/>
-      <c r="BA8" s="197"/>
-      <c r="BB8" s="197"/>
-      <c r="BC8" s="197"/>
-      <c r="BD8" s="197"/>
-      <c r="BE8" s="197"/>
-      <c r="BF8" s="199"/>
-      <c r="BG8" s="199"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="191"/>
+      <c r="AW8" s="191"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="191"/>
+      <c r="BW8" s="191"/>
+      <c r="CT8" s="191"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="198"/>
+      <c r="B9" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
-      <c r="AB9" s="190"/>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="190"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="190"/>
-      <c r="AL9" s="190"/>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="190"/>
-      <c r="AQ9" s="190"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="197"/>
+      <c r="I9" s="197"/>
+      <c r="J9" s="197"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="190"/>
+      <c r="W9" s="217"/>
+      <c r="X9" s="217"/>
+      <c r="Y9" s="217"/>
+      <c r="Z9" s="217"/>
+      <c r="AA9" s="189"/>
+      <c r="AB9" s="187"/>
+      <c r="AC9" s="187"/>
+      <c r="AD9" s="187"/>
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="187"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="196"/>
-      <c r="AY9" s="197"/>
-      <c r="AZ9" s="197"/>
-      <c r="BA9" s="197"/>
-      <c r="BB9" s="197"/>
-      <c r="BC9" s="197"/>
-      <c r="BD9" s="197"/>
-      <c r="BE9" s="197"/>
-      <c r="BF9" s="199"/>
-      <c r="BG9" s="199"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="191"/>
+      <c r="AW9" s="191"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="191"/>
+      <c r="BW9" s="191"/>
+      <c r="CT9" s="191"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="198"/>
+      <c r="B10" s="199" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="190"/>
-      <c r="AC10" s="190"/>
-      <c r="AD10" s="190"/>
-      <c r="AE10" s="190"/>
-      <c r="AF10" s="190"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="190"/>
-      <c r="AI10" s="190"/>
-      <c r="AJ10" s="190"/>
-      <c r="AK10" s="190"/>
-      <c r="AL10" s="190"/>
-      <c r="AM10" s="190"/>
-      <c r="AN10" s="190"/>
-      <c r="AO10" s="190"/>
-      <c r="AP10" s="190"/>
-      <c r="AQ10" s="190"/>
-      <c r="AR10" s="193"/>
-      <c r="AS10" s="193"/>
-      <c r="AT10" s="193"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="197"/>
+      <c r="K10" s="197"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="190"/>
+      <c r="O10" s="190"/>
+      <c r="P10" s="190"/>
+      <c r="Q10" s="190"/>
+      <c r="R10" s="190"/>
+      <c r="S10" s="190"/>
+      <c r="T10" s="190"/>
+      <c r="U10" s="190"/>
+      <c r="V10" s="190"/>
+      <c r="W10" s="217"/>
+      <c r="X10" s="217"/>
+      <c r="Y10" s="217"/>
+      <c r="Z10" s="217"/>
+      <c r="AA10" s="189"/>
+      <c r="AB10" s="187"/>
+      <c r="AC10" s="187"/>
+      <c r="AD10" s="187"/>
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="187"/>
+      <c r="AG10" s="187"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="196"/>
-      <c r="AY10" s="197"/>
-      <c r="AZ10" s="197"/>
-      <c r="BA10" s="197"/>
-      <c r="BB10" s="197"/>
-      <c r="BC10" s="197"/>
-      <c r="BD10" s="197"/>
-      <c r="BE10" s="197"/>
-      <c r="BF10" s="199"/>
-      <c r="BG10" s="199"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="191"/>
+      <c r="AW10" s="191"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="191"/>
+      <c r="BW10" s="191"/>
+      <c r="CT10" s="191"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="198"/>
+      <c r="B11" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="191"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="191"/>
-      <c r="AE11" s="191"/>
-      <c r="AF11" s="191"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="191"/>
-      <c r="AI11" s="191"/>
-      <c r="AJ11" s="191"/>
-      <c r="AK11" s="191"/>
-      <c r="AL11" s="191"/>
-      <c r="AM11" s="191"/>
-      <c r="AN11" s="191"/>
-      <c r="AO11" s="191"/>
-      <c r="AP11" s="191"/>
-      <c r="AQ11" s="191"/>
-      <c r="AR11" s="194"/>
-      <c r="AS11" s="194"/>
-      <c r="AT11" s="194"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
+      <c r="N11" s="190"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="190"/>
+      <c r="Q11" s="190"/>
+      <c r="R11" s="190"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="190"/>
+      <c r="U11" s="190"/>
+      <c r="V11" s="190"/>
+      <c r="W11" s="217"/>
+      <c r="X11" s="217"/>
+      <c r="Y11" s="217"/>
+      <c r="Z11" s="217"/>
+      <c r="AA11" s="189"/>
+      <c r="AB11" s="188"/>
+      <c r="AC11" s="188"/>
+      <c r="AD11" s="188"/>
+      <c r="AE11" s="188"/>
+      <c r="AF11" s="188"/>
+      <c r="AG11" s="188"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="196"/>
-      <c r="AY11" s="197"/>
-      <c r="AZ11" s="197"/>
-      <c r="BA11" s="197"/>
-      <c r="BB11" s="197"/>
-      <c r="BC11" s="197"/>
-      <c r="BD11" s="197"/>
-      <c r="BE11" s="197"/>
-      <c r="BF11" s="199"/>
-      <c r="BG11" s="199"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="191"/>
+      <c r="AW11" s="191"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="191"/>
+      <c r="BW11" s="191"/>
+      <c r="CT11" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4177,22 +4161,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5714,13 +5723,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="212" t="s">
+      <c r="A4" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="214"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5825,9 +5834,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="201"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="201"/>
+      <c r="A5" s="203"/>
+      <c r="B5" s="201"/>
+      <c r="C5" s="203"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5932,11 +5941,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="201"/>
+      <c r="A6" s="203"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="201"/>
+      <c r="C6" s="203"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6041,11 +6050,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="201"/>
+      <c r="A7" s="203"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="201"/>
+      <c r="C7" s="203"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6150,11 +6159,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201"/>
+      <c r="A8" s="203"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="201"/>
+      <c r="C8" s="203"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6259,11 +6268,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="201"/>
+      <c r="C9" s="203"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6368,11 +6377,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="203"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6477,11 +6486,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="203"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6586,9 +6595,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="201"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="202"/>
+      <c r="C12" s="206"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6693,10 +6702,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="208" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6805,8 +6814,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="201"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6927,7 +6936,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="201"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7037,7 +7046,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7147,7 +7156,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7259,7 +7268,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7369,7 +7378,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7479,7 +7488,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="201"/>
+      <c r="A20" s="203"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7589,7 +7598,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="202"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7700,7 +7709,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="200" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7810,7 +7819,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="211"/>
+      <c r="B23" s="201"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7917,13 +7926,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="203" t="s">
+      <c r="A24" s="211" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="205">
+      <c r="C24" s="213">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8031,11 +8040,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="204"/>
+      <c r="A25" s="212"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="201"/>
+      <c r="C25" s="203"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8141,11 +8150,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="204"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="203"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8251,11 +8260,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="204"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="201"/>
+      <c r="C27" s="203"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8361,11 +8370,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="204"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="201"/>
+      <c r="C28" s="203"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8471,11 +8480,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="204"/>
+      <c r="A29" s="212"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="201"/>
+      <c r="C29" s="203"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8581,11 +8590,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="204"/>
+      <c r="A30" s="212"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="201"/>
+      <c r="C30" s="203"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8691,11 +8700,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="204"/>
+      <c r="A31" s="212"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="201"/>
+      <c r="C31" s="203"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8801,11 +8810,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="204"/>
+      <c r="A32" s="212"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="201"/>
+      <c r="C32" s="203"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8911,11 +8920,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="204"/>
+      <c r="A33" s="212"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="201"/>
+      <c r="C33" s="203"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9021,11 +9030,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="204"/>
+      <c r="A34" s="212"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="201"/>
+      <c r="C34" s="203"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9131,11 +9140,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="204"/>
+      <c r="A35" s="212"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="202"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9241,11 +9250,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="204"/>
+      <c r="A36" s="212"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="205">
+      <c r="C36" s="213">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9353,11 +9362,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="204"/>
+      <c r="A37" s="212"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="201"/>
+      <c r="C37" s="203"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9463,11 +9472,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="204"/>
+      <c r="A38" s="212"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="201"/>
+      <c r="C38" s="203"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9573,11 +9582,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="204"/>
+      <c r="A39" s="212"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="201"/>
+      <c r="C39" s="203"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9683,11 +9692,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="204"/>
+      <c r="A40" s="212"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="201"/>
+      <c r="C40" s="203"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9793,11 +9802,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="204"/>
+      <c r="A41" s="212"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="201"/>
+      <c r="C41" s="203"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9903,11 +9912,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="204"/>
+      <c r="A42" s="212"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="201"/>
+      <c r="C42" s="203"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10013,11 +10022,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="204"/>
+      <c r="A43" s="212"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="201"/>
+      <c r="C43" s="203"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10123,11 +10132,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="204"/>
+      <c r="A44" s="212"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="201"/>
+      <c r="C44" s="203"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10233,11 +10242,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="204"/>
+      <c r="A45" s="212"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10343,11 +10352,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="204"/>
+      <c r="A46" s="212"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="201"/>
+      <c r="C46" s="203"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10453,11 +10462,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="204"/>
+      <c r="A47" s="212"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="201"/>
+      <c r="C47" s="203"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10571,11 +10580,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="204"/>
+      <c r="A48" s="212"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="201"/>
+      <c r="C48" s="203"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10684,7 +10693,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="214" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10794,7 +10803,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="207"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14225,7 +14234,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="208" t="s">
+      <c r="A81" s="215" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14337,7 +14346,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="201"/>
+      <c r="A82" s="203"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14447,7 +14456,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="201"/>
+      <c r="A83" s="203"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14557,7 +14566,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="201"/>
+      <c r="A84" s="203"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14667,7 +14676,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="201"/>
+      <c r="A85" s="203"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14777,7 +14786,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="201"/>
+      <c r="A86" s="203"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14887,7 +14896,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="201"/>
+      <c r="A87" s="203"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -14999,7 +15008,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="201"/>
+      <c r="A88" s="203"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15109,7 +15118,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="201"/>
+      <c r="A89" s="203"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15219,7 +15228,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="201"/>
+      <c r="A90" s="203"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15329,11 +15338,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="201"/>
+      <c r="A91" s="203"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="209"/>
+      <c r="C91" s="216"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15439,11 +15448,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="201"/>
+      <c r="A92" s="203"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="203"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15549,11 +15558,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="202"/>
+      <c r="A93" s="206"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="201"/>
+      <c r="C93" s="203"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15777,7 +15786,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="200" t="s">
+      <c r="A95" s="210" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15889,7 +15898,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="201"/>
+      <c r="A96" s="203"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -15999,7 +16008,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="201"/>
+      <c r="A97" s="203"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16109,7 +16118,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="201"/>
+      <c r="A98" s="203"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16219,7 +16228,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="201"/>
+      <c r="A99" s="203"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16329,7 +16338,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="201"/>
+      <c r="A100" s="203"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16439,7 +16448,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="201"/>
+      <c r="A101" s="203"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16549,7 +16558,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="201"/>
+      <c r="A102" s="203"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16659,7 +16668,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="201"/>
+      <c r="A103" s="203"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16771,7 +16780,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="201"/>
+      <c r="A104" s="203"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16881,7 +16890,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="201"/>
+      <c r="A105" s="203"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -16999,7 +17008,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="201"/>
+      <c r="A106" s="203"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17109,7 +17118,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="201"/>
+      <c r="A107" s="203"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17219,7 +17228,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="201"/>
+      <c r="A108" s="203"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17329,7 +17338,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="201"/>
+      <c r="A109" s="203"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17439,7 +17448,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="201"/>
+      <c r="A110" s="203"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17549,7 +17558,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="201"/>
+      <c r="A111" s="203"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17659,7 +17668,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="201"/>
+      <c r="A112" s="203"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17769,7 +17778,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="201"/>
+      <c r="A113" s="203"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17879,7 +17888,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="201"/>
+      <c r="A114" s="203"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17989,7 +17998,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="201"/>
+      <c r="A115" s="203"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18099,7 +18108,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="201"/>
+      <c r="A116" s="203"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18225,7 +18234,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="201"/>
+      <c r="A117" s="203"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18335,7 +18344,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="202"/>
+      <c r="A118" s="206"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25706,12 +25715,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25719,6 +25722,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 13, 16 e 17-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE27D4-B38C-4320-B914-C8F71C5F0932}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4FD77C-3E60-42F6-82A0-26DD2E6C1A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="168">
   <si>
     <t>S</t>
   </si>
@@ -700,6 +700,16 @@
   <si>
     <t>Sprint Review
 Lógica de leitura e escrita em console</t>
+  </si>
+  <si>
+    <t>Não foi realizado acompanhamento pois presenciamos as Sprints Reviews com os grupos do técnico</t>
+  </si>
+  <si>
+    <t>Correção de exercícios de lógica estrutural propostos no dia 13/09.
+Conceitos sobre lógica condicional (if / else )</t>
+  </si>
+  <si>
+    <t>Conceitos e exercícios sobre lógica condicional ( switch / case )</t>
   </si>
 </sst>
 </file>
@@ -1878,7 +1888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2225,14 +2235,47 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2249,73 +2292,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2326,13 +2316,39 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2839,10 +2855,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA4" sqref="AA4:AA11"/>
+      <selection pane="bottomRight" activeCell="AD4" sqref="AD4:AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3151,110 +3167,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="192" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="192"/>
-      <c r="I2" s="192"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="192" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="192"/>
-      <c r="T2" s="192"/>
-      <c r="U2" s="192"/>
-      <c r="V2" s="192"/>
-      <c r="W2" s="192"/>
-      <c r="X2" s="192"/>
-      <c r="Y2" s="192"/>
-      <c r="Z2" s="192"/>
-      <c r="AA2" s="192"/>
-      <c r="AB2" s="192"/>
-      <c r="AC2" s="192"/>
-      <c r="AD2" s="192"/>
-      <c r="AE2" s="192"/>
-      <c r="AF2" s="192"/>
-      <c r="AG2" s="192"/>
-      <c r="AH2" s="192"/>
-      <c r="AI2" s="192"/>
-      <c r="AJ2" s="192"/>
-      <c r="AK2" s="192"/>
-      <c r="AL2" s="192"/>
-      <c r="AM2" s="192" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="192"/>
-      <c r="AO2" s="192"/>
-      <c r="AP2" s="192"/>
-      <c r="AQ2" s="192"/>
-      <c r="AR2" s="192"/>
-      <c r="AS2" s="192"/>
-      <c r="AT2" s="192"/>
-      <c r="AU2" s="192"/>
-      <c r="AV2" s="192"/>
-      <c r="AW2" s="192"/>
-      <c r="AX2" s="193"/>
-      <c r="AY2" s="193"/>
-      <c r="AZ2" s="193"/>
-      <c r="BA2" s="193"/>
-      <c r="BB2" s="193"/>
-      <c r="BC2" s="193"/>
-      <c r="BD2" s="193"/>
-      <c r="BE2" s="193"/>
-      <c r="BF2" s="193"/>
-      <c r="BG2" s="193"/>
-      <c r="BH2" s="193"/>
-      <c r="BI2" s="193"/>
-      <c r="BJ2" s="192" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="192"/>
-      <c r="BL2" s="192"/>
-      <c r="BM2" s="192"/>
-      <c r="BN2" s="192"/>
-      <c r="BO2" s="192"/>
-      <c r="BP2" s="192"/>
-      <c r="BQ2" s="192"/>
-      <c r="BR2" s="192"/>
-      <c r="BS2" s="192"/>
-      <c r="BT2" s="192"/>
-      <c r="BU2" s="192"/>
-      <c r="BV2" s="192"/>
-      <c r="BW2" s="192"/>
-      <c r="BX2" s="194"/>
-      <c r="BY2" s="194"/>
-      <c r="BZ2" s="194"/>
-      <c r="CA2" s="194"/>
-      <c r="CB2" s="194"/>
-      <c r="CC2" s="194"/>
-      <c r="CD2" s="194"/>
-      <c r="CE2" s="195" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="196"/>
-      <c r="CG2" s="196"/>
-      <c r="CH2" s="196"/>
-      <c r="CI2" s="196"/>
-      <c r="CJ2" s="196"/>
-      <c r="CK2" s="196"/>
-      <c r="CL2" s="196"/>
-      <c r="CM2" s="196"/>
-      <c r="CN2" s="196"/>
-      <c r="CO2" s="196"/>
-      <c r="CP2" s="196"/>
-      <c r="CQ2" s="196"/>
-      <c r="CR2" s="196"/>
-      <c r="CS2" s="196"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3550,585 +3566,648 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="199"/>
-      <c r="D4" s="197" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="197" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="197" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="197" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="197" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="197" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="197" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="190" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="190" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="190" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="190" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="190" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="190" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="190" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="190" t="s">
+      <c r="S4" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="190" t="s">
+      <c r="T4" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="190" t="s">
+      <c r="U4" s="187" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="190" t="s">
+      <c r="V4" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="217" t="s">
+      <c r="W4" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="217" t="s">
+      <c r="X4" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="217" t="s">
+      <c r="Y4" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="217" t="s">
+      <c r="Z4" s="188" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="189"/>
-      <c r="AB4" s="186"/>
-      <c r="AC4" s="186"/>
-      <c r="AD4" s="186"/>
-      <c r="AE4" s="186"/>
-      <c r="AF4" s="186"/>
-      <c r="AG4" s="186"/>
-      <c r="AH4" s="186"/>
-      <c r="AI4" s="186"/>
-      <c r="AJ4" s="186"/>
-      <c r="AK4" s="186"/>
-      <c r="AL4" s="186"/>
-      <c r="AM4" s="186"/>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="AA4" s="188" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB4" s="217" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC4" s="217" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD4" s="217"/>
+      <c r="AE4" s="217"/>
+      <c r="AF4" s="217"/>
+      <c r="AG4" s="189"/>
+      <c r="AH4" s="189"/>
+      <c r="AI4" s="189"/>
+      <c r="AJ4" s="189"/>
+      <c r="AK4" s="189"/>
+      <c r="AL4" s="189"/>
+      <c r="AM4" s="189"/>
+      <c r="AN4" s="189"/>
+      <c r="AO4" s="189"/>
+      <c r="AP4" s="189"/>
+      <c r="AQ4" s="189"/>
+      <c r="AR4" s="192"/>
+      <c r="AS4" s="192"/>
+      <c r="AT4" s="192"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="191"/>
-      <c r="AW4" s="191"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="191"/>
-      <c r="BW4" s="191"/>
-      <c r="CT4" s="191"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="195"/>
+      <c r="AY4" s="197"/>
+      <c r="AZ4" s="197"/>
+      <c r="BA4" s="197"/>
+      <c r="BB4" s="197"/>
+      <c r="BC4" s="197"/>
+      <c r="BD4" s="197"/>
+      <c r="BE4" s="197"/>
+      <c r="BF4" s="198"/>
+      <c r="BG4" s="198"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="198"/>
-      <c r="B5" s="199" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="197"/>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197"/>
-      <c r="I5" s="197"/>
-      <c r="J5" s="197"/>
-      <c r="K5" s="197"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
-      <c r="N5" s="190"/>
-      <c r="O5" s="190"/>
-      <c r="P5" s="190"/>
-      <c r="Q5" s="190"/>
-      <c r="R5" s="190"/>
-      <c r="S5" s="190"/>
-      <c r="T5" s="190"/>
-      <c r="U5" s="190"/>
-      <c r="V5" s="190"/>
-      <c r="W5" s="217"/>
-      <c r="X5" s="217"/>
-      <c r="Y5" s="217"/>
-      <c r="Z5" s="217"/>
-      <c r="AA5" s="189"/>
-      <c r="AB5" s="187"/>
-      <c r="AC5" s="187"/>
-      <c r="AD5" s="187"/>
-      <c r="AE5" s="187"/>
-      <c r="AF5" s="187"/>
-      <c r="AG5" s="187"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="218"/>
+      <c r="AC5" s="218"/>
+      <c r="AD5" s="218"/>
+      <c r="AE5" s="218"/>
+      <c r="AF5" s="218"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="190"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="190"/>
+      <c r="AK5" s="190"/>
+      <c r="AL5" s="190"/>
+      <c r="AM5" s="190"/>
+      <c r="AN5" s="190"/>
+      <c r="AO5" s="190"/>
+      <c r="AP5" s="190"/>
+      <c r="AQ5" s="190"/>
+      <c r="AR5" s="193"/>
+      <c r="AS5" s="193"/>
+      <c r="AT5" s="193"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="191"/>
-      <c r="AW5" s="191"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="191"/>
-      <c r="BW5" s="191"/>
-      <c r="CT5" s="191"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="196"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="197"/>
+      <c r="BA5" s="197"/>
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="199"/>
+      <c r="BG5" s="199"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="199"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="197"/>
-      <c r="H6" s="197"/>
-      <c r="I6" s="197"/>
-      <c r="J6" s="197"/>
-      <c r="K6" s="197"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
-      <c r="N6" s="190"/>
-      <c r="O6" s="190"/>
-      <c r="P6" s="190"/>
-      <c r="Q6" s="190"/>
-      <c r="R6" s="190"/>
-      <c r="S6" s="190"/>
-      <c r="T6" s="190"/>
-      <c r="U6" s="190"/>
-      <c r="V6" s="190"/>
-      <c r="W6" s="217"/>
-      <c r="X6" s="217"/>
-      <c r="Y6" s="217"/>
-      <c r="Z6" s="217"/>
-      <c r="AA6" s="189"/>
-      <c r="AB6" s="187"/>
-      <c r="AC6" s="187"/>
-      <c r="AD6" s="187"/>
-      <c r="AE6" s="187"/>
-      <c r="AF6" s="187"/>
-      <c r="AG6" s="187"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
+      <c r="AB6" s="218"/>
+      <c r="AC6" s="218"/>
+      <c r="AD6" s="218"/>
+      <c r="AE6" s="218"/>
+      <c r="AF6" s="218"/>
+      <c r="AG6" s="190"/>
+      <c r="AH6" s="190"/>
+      <c r="AI6" s="190"/>
+      <c r="AJ6" s="190"/>
+      <c r="AK6" s="190"/>
+      <c r="AL6" s="190"/>
+      <c r="AM6" s="190"/>
+      <c r="AN6" s="190"/>
+      <c r="AO6" s="190"/>
+      <c r="AP6" s="190"/>
+      <c r="AQ6" s="190"/>
+      <c r="AR6" s="193"/>
+      <c r="AS6" s="193"/>
+      <c r="AT6" s="193"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="191"/>
-      <c r="AW6" s="191"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="191"/>
-      <c r="BW6" s="191"/>
-      <c r="CT6" s="191"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="199"/>
+      <c r="BG6" s="199"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="198"/>
-      <c r="B7" s="199" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="197"/>
-      <c r="F7" s="197"/>
-      <c r="G7" s="197"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="197"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="197"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="190"/>
-      <c r="N7" s="190"/>
-      <c r="O7" s="190"/>
-      <c r="P7" s="190"/>
-      <c r="Q7" s="190"/>
-      <c r="R7" s="190"/>
-      <c r="S7" s="190"/>
-      <c r="T7" s="190"/>
-      <c r="U7" s="190"/>
-      <c r="V7" s="190"/>
-      <c r="W7" s="217"/>
-      <c r="X7" s="217"/>
-      <c r="Y7" s="217"/>
-      <c r="Z7" s="217"/>
-      <c r="AA7" s="189"/>
-      <c r="AB7" s="187"/>
-      <c r="AC7" s="187"/>
-      <c r="AD7" s="187"/>
-      <c r="AE7" s="187"/>
-      <c r="AF7" s="187"/>
-      <c r="AG7" s="187"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
+      <c r="AB7" s="218"/>
+      <c r="AC7" s="218"/>
+      <c r="AD7" s="218"/>
+      <c r="AE7" s="218"/>
+      <c r="AF7" s="218"/>
+      <c r="AG7" s="190"/>
+      <c r="AH7" s="190"/>
+      <c r="AI7" s="190"/>
+      <c r="AJ7" s="190"/>
+      <c r="AK7" s="190"/>
+      <c r="AL7" s="190"/>
+      <c r="AM7" s="190"/>
+      <c r="AN7" s="190"/>
+      <c r="AO7" s="190"/>
+      <c r="AP7" s="190"/>
+      <c r="AQ7" s="190"/>
+      <c r="AR7" s="193"/>
+      <c r="AS7" s="193"/>
+      <c r="AT7" s="193"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="191"/>
-      <c r="AW7" s="191"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="191"/>
-      <c r="BW7" s="191"/>
-      <c r="CT7" s="191"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="196"/>
+      <c r="AY7" s="197"/>
+      <c r="AZ7" s="197"/>
+      <c r="BA7" s="197"/>
+      <c r="BB7" s="197"/>
+      <c r="BC7" s="197"/>
+      <c r="BD7" s="197"/>
+      <c r="BE7" s="197"/>
+      <c r="BF7" s="199"/>
+      <c r="BG7" s="199"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="198" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="199" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="199"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="197"/>
-      <c r="K8" s="197"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="190"/>
-      <c r="N8" s="190"/>
-      <c r="O8" s="190"/>
-      <c r="P8" s="190"/>
-      <c r="Q8" s="190"/>
-      <c r="R8" s="190"/>
-      <c r="S8" s="190"/>
-      <c r="T8" s="190"/>
-      <c r="U8" s="190"/>
-      <c r="V8" s="190"/>
-      <c r="W8" s="217"/>
-      <c r="X8" s="217"/>
-      <c r="Y8" s="217"/>
-      <c r="Z8" s="217"/>
-      <c r="AA8" s="189"/>
-      <c r="AB8" s="187"/>
-      <c r="AC8" s="187"/>
-      <c r="AD8" s="187"/>
-      <c r="AE8" s="187"/>
-      <c r="AF8" s="187"/>
-      <c r="AG8" s="187"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
+      <c r="AB8" s="218"/>
+      <c r="AC8" s="218"/>
+      <c r="AD8" s="218"/>
+      <c r="AE8" s="218"/>
+      <c r="AF8" s="218"/>
+      <c r="AG8" s="190"/>
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="190"/>
+      <c r="AL8" s="190"/>
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="190"/>
+      <c r="AQ8" s="190"/>
+      <c r="AR8" s="193"/>
+      <c r="AS8" s="193"/>
+      <c r="AT8" s="193"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="191"/>
-      <c r="AW8" s="191"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="191"/>
-      <c r="BW8" s="191"/>
-      <c r="CT8" s="191"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="196"/>
+      <c r="AY8" s="197"/>
+      <c r="AZ8" s="197"/>
+      <c r="BA8" s="197"/>
+      <c r="BB8" s="197"/>
+      <c r="BC8" s="197"/>
+      <c r="BD8" s="197"/>
+      <c r="BE8" s="197"/>
+      <c r="BF8" s="199"/>
+      <c r="BG8" s="199"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="198"/>
-      <c r="B9" s="199" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="199"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="190"/>
-      <c r="M9" s="190"/>
-      <c r="N9" s="190"/>
-      <c r="O9" s="190"/>
-      <c r="P9" s="190"/>
-      <c r="Q9" s="190"/>
-      <c r="R9" s="190"/>
-      <c r="S9" s="190"/>
-      <c r="T9" s="190"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="190"/>
-      <c r="W9" s="217"/>
-      <c r="X9" s="217"/>
-      <c r="Y9" s="217"/>
-      <c r="Z9" s="217"/>
-      <c r="AA9" s="189"/>
-      <c r="AB9" s="187"/>
-      <c r="AC9" s="187"/>
-      <c r="AD9" s="187"/>
-      <c r="AE9" s="187"/>
-      <c r="AF9" s="187"/>
-      <c r="AG9" s="187"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="218"/>
+      <c r="AC9" s="218"/>
+      <c r="AD9" s="218"/>
+      <c r="AE9" s="218"/>
+      <c r="AF9" s="218"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="190"/>
+      <c r="AL9" s="190"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="190"/>
+      <c r="AR9" s="193"/>
+      <c r="AS9" s="193"/>
+      <c r="AT9" s="193"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="191"/>
-      <c r="AW9" s="191"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="191"/>
-      <c r="BW9" s="191"/>
-      <c r="CT9" s="191"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="196"/>
+      <c r="AY9" s="197"/>
+      <c r="AZ9" s="197"/>
+      <c r="BA9" s="197"/>
+      <c r="BB9" s="197"/>
+      <c r="BC9" s="197"/>
+      <c r="BD9" s="197"/>
+      <c r="BE9" s="197"/>
+      <c r="BF9" s="199"/>
+      <c r="BG9" s="199"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="199"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
-      <c r="J10" s="197"/>
-      <c r="K10" s="197"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="190"/>
-      <c r="N10" s="190"/>
-      <c r="O10" s="190"/>
-      <c r="P10" s="190"/>
-      <c r="Q10" s="190"/>
-      <c r="R10" s="190"/>
-      <c r="S10" s="190"/>
-      <c r="T10" s="190"/>
-      <c r="U10" s="190"/>
-      <c r="V10" s="190"/>
-      <c r="W10" s="217"/>
-      <c r="X10" s="217"/>
-      <c r="Y10" s="217"/>
-      <c r="Z10" s="217"/>
-      <c r="AA10" s="189"/>
-      <c r="AB10" s="187"/>
-      <c r="AC10" s="187"/>
-      <c r="AD10" s="187"/>
-      <c r="AE10" s="187"/>
-      <c r="AF10" s="187"/>
-      <c r="AG10" s="187"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
+      <c r="AB10" s="218"/>
+      <c r="AC10" s="218"/>
+      <c r="AD10" s="218"/>
+      <c r="AE10" s="218"/>
+      <c r="AF10" s="218"/>
+      <c r="AG10" s="190"/>
+      <c r="AH10" s="190"/>
+      <c r="AI10" s="190"/>
+      <c r="AJ10" s="190"/>
+      <c r="AK10" s="190"/>
+      <c r="AL10" s="190"/>
+      <c r="AM10" s="190"/>
+      <c r="AN10" s="190"/>
+      <c r="AO10" s="190"/>
+      <c r="AP10" s="190"/>
+      <c r="AQ10" s="190"/>
+      <c r="AR10" s="193"/>
+      <c r="AS10" s="193"/>
+      <c r="AT10" s="193"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="191"/>
-      <c r="AW10" s="191"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="191"/>
-      <c r="BW10" s="191"/>
-      <c r="CT10" s="191"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="196"/>
+      <c r="AY10" s="197"/>
+      <c r="AZ10" s="197"/>
+      <c r="BA10" s="197"/>
+      <c r="BB10" s="197"/>
+      <c r="BC10" s="197"/>
+      <c r="BD10" s="197"/>
+      <c r="BE10" s="197"/>
+      <c r="BF10" s="199"/>
+      <c r="BG10" s="199"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="198"/>
-      <c r="B11" s="199" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="197"/>
-      <c r="J11" s="197"/>
-      <c r="K11" s="197"/>
-      <c r="L11" s="190"/>
-      <c r="M11" s="190"/>
-      <c r="N11" s="190"/>
-      <c r="O11" s="190"/>
-      <c r="P11" s="190"/>
-      <c r="Q11" s="190"/>
-      <c r="R11" s="190"/>
-      <c r="S11" s="190"/>
-      <c r="T11" s="190"/>
-      <c r="U11" s="190"/>
-      <c r="V11" s="190"/>
-      <c r="W11" s="217"/>
-      <c r="X11" s="217"/>
-      <c r="Y11" s="217"/>
-      <c r="Z11" s="217"/>
-      <c r="AA11" s="189"/>
-      <c r="AB11" s="188"/>
-      <c r="AC11" s="188"/>
-      <c r="AD11" s="188"/>
-      <c r="AE11" s="188"/>
-      <c r="AF11" s="188"/>
-      <c r="AG11" s="188"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
+      <c r="AB11" s="219"/>
+      <c r="AC11" s="219"/>
+      <c r="AD11" s="219"/>
+      <c r="AE11" s="219"/>
+      <c r="AF11" s="219"/>
+      <c r="AG11" s="191"/>
+      <c r="AH11" s="191"/>
+      <c r="AI11" s="191"/>
+      <c r="AJ11" s="191"/>
+      <c r="AK11" s="191"/>
+      <c r="AL11" s="191"/>
+      <c r="AM11" s="191"/>
+      <c r="AN11" s="191"/>
+      <c r="AO11" s="191"/>
+      <c r="AP11" s="191"/>
+      <c r="AQ11" s="191"/>
+      <c r="AR11" s="194"/>
+      <c r="AS11" s="194"/>
+      <c r="AT11" s="194"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="191"/>
-      <c r="AW11" s="191"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="191"/>
-      <c r="BW11" s="191"/>
-      <c r="CT11" s="191"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="196"/>
+      <c r="AY11" s="197"/>
+      <c r="AZ11" s="197"/>
+      <c r="BA11" s="197"/>
+      <c r="BB11" s="197"/>
+      <c r="BC11" s="197"/>
+      <c r="BD11" s="197"/>
+      <c r="BE11" s="197"/>
+      <c r="BF11" s="199"/>
+      <c r="BG11" s="199"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4145,63 +4224,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5723,13 +5745,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="213" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="214"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5834,9 +5856,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="203"/>
-      <c r="B5" s="201"/>
-      <c r="C5" s="203"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="211"/>
+      <c r="C5" s="201"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5941,11 +5963,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="203"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="203"/>
+      <c r="C6" s="201"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6050,11 +6072,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="203"/>
+      <c r="A7" s="201"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="203"/>
+      <c r="C7" s="201"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6159,11 +6181,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="203"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="203"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6268,11 +6290,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="203"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="203"/>
+      <c r="C9" s="201"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6377,11 +6399,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="203"/>
+      <c r="A10" s="201"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="203"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6486,11 +6508,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="203"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="203"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6595,9 +6617,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="203"/>
+      <c r="A12" s="201"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="206"/>
+      <c r="C12" s="202"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6702,10 +6724,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="207" t="s">
+      <c r="A13" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="208" t="s">
+      <c r="B13" s="216" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6814,8 +6836,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="203"/>
-      <c r="B14" s="209"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="207"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6936,7 +6958,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="203"/>
+      <c r="A15" s="201"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7046,7 +7068,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="203"/>
+      <c r="A16" s="201"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7156,7 +7178,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="203"/>
+      <c r="A17" s="201"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7268,7 +7290,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203"/>
+      <c r="A18" s="201"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7378,7 +7400,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203"/>
+      <c r="A19" s="201"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7488,7 +7510,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="203"/>
+      <c r="A20" s="201"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7598,7 +7620,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="206"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7709,7 +7731,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="210" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7819,7 +7841,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="201"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7926,13 +7948,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="203" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="213">
+      <c r="C24" s="205">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8040,11 +8062,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="212"/>
+      <c r="A25" s="204"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="203"/>
+      <c r="C25" s="201"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8150,11 +8172,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="212"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="203"/>
+      <c r="C26" s="201"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8260,11 +8282,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="212"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="203"/>
+      <c r="C27" s="201"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8370,11 +8392,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="212"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="203"/>
+      <c r="C28" s="201"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8480,11 +8502,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="212"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="203"/>
+      <c r="C29" s="201"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8590,11 +8612,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="212"/>
+      <c r="A30" s="204"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="203"/>
+      <c r="C30" s="201"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8700,11 +8722,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="212"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="203"/>
+      <c r="C31" s="201"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8810,11 +8832,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="212"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="203"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8920,11 +8942,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="212"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="203"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9030,11 +9052,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="212"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="203"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9140,11 +9162,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="212"/>
+      <c r="A35" s="204"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="206"/>
+      <c r="C35" s="202"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9250,11 +9272,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="212"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="213">
+      <c r="C36" s="205">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9362,11 +9384,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="212"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="203"/>
+      <c r="C37" s="201"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9472,11 +9494,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="212"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="203"/>
+      <c r="C38" s="201"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9582,11 +9604,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="212"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="203"/>
+      <c r="C39" s="201"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9692,11 +9714,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="212"/>
+      <c r="A40" s="204"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="203"/>
+      <c r="C40" s="201"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9802,11 +9824,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="212"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="203"/>
+      <c r="C41" s="201"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9912,11 +9934,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="212"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="203"/>
+      <c r="C42" s="201"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10022,11 +10044,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="212"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="203"/>
+      <c r="C43" s="201"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10132,11 +10154,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="212"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="203"/>
+      <c r="C44" s="201"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10242,11 +10264,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="212"/>
+      <c r="A45" s="204"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="203"/>
+      <c r="C45" s="201"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10352,11 +10374,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="212"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="203"/>
+      <c r="C46" s="201"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10462,11 +10484,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="212"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="203"/>
+      <c r="C47" s="201"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10580,11 +10602,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="212"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="203"/>
+      <c r="C48" s="201"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10693,7 +10715,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="214" t="s">
+      <c r="B49" s="206" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10803,7 +10825,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="209"/>
+      <c r="B50" s="207"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14234,7 +14256,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="215" t="s">
+      <c r="A81" s="208" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14346,7 +14368,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="203"/>
+      <c r="A82" s="201"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14456,7 +14478,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="203"/>
+      <c r="A83" s="201"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14566,7 +14588,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="203"/>
+      <c r="A84" s="201"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14676,7 +14698,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="203"/>
+      <c r="A85" s="201"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14786,7 +14808,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="203"/>
+      <c r="A86" s="201"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14896,7 +14918,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="203"/>
+      <c r="A87" s="201"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15008,7 +15030,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="203"/>
+      <c r="A88" s="201"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15118,7 +15140,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="203"/>
+      <c r="A89" s="201"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15228,7 +15250,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="203"/>
+      <c r="A90" s="201"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15338,11 +15360,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="203"/>
+      <c r="A91" s="201"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="216"/>
+      <c r="C91" s="209"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15448,11 +15470,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="203"/>
+      <c r="A92" s="201"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="203"/>
+      <c r="C92" s="201"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15558,11 +15580,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="206"/>
+      <c r="A93" s="202"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="203"/>
+      <c r="C93" s="201"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15786,7 +15808,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="210" t="s">
+      <c r="A95" s="200" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15898,7 +15920,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="203"/>
+      <c r="A96" s="201"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16008,7 +16030,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="203"/>
+      <c r="A97" s="201"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16118,7 +16140,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="203"/>
+      <c r="A98" s="201"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16228,7 +16250,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="203"/>
+      <c r="A99" s="201"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16338,7 +16360,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="203"/>
+      <c r="A100" s="201"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16448,7 +16470,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="203"/>
+      <c r="A101" s="201"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16558,7 +16580,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="203"/>
+      <c r="A102" s="201"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16668,7 +16690,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="203"/>
+      <c r="A103" s="201"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16780,7 +16802,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="203"/>
+      <c r="A104" s="201"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16890,7 +16912,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="203"/>
+      <c r="A105" s="201"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17008,7 +17030,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="203"/>
+      <c r="A106" s="201"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17118,7 +17140,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="203"/>
+      <c r="A107" s="201"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17228,7 +17250,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="203"/>
+      <c r="A108" s="201"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17338,7 +17360,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="203"/>
+      <c r="A109" s="201"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17448,7 +17470,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="203"/>
+      <c r="A110" s="201"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17558,7 +17580,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="203"/>
+      <c r="A111" s="201"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17668,7 +17690,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="203"/>
+      <c r="A112" s="201"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17778,7 +17800,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="203"/>
+      <c r="A113" s="201"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17888,7 +17910,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="203"/>
+      <c r="A114" s="201"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -17998,7 +18020,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="203"/>
+      <c r="A115" s="201"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18108,7 +18130,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="203"/>
+      <c r="A116" s="201"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18234,7 +18256,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="203"/>
+      <c r="A117" s="201"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18344,7 +18366,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="206"/>
+      <c r="A118" s="202"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25715,6 +25737,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25722,12 +25750,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 18-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4FD77C-3E60-42F6-82A0-26DD2E6C1A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F944F-86F7-42ED-B7C8-D4232185A487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="169">
   <si>
     <t>S</t>
   </si>
@@ -710,6 +710,9 @@
   </si>
   <si>
     <t>Conceitos e exercícios sobre lógica condicional ( switch / case )</t>
+  </si>
+  <si>
+    <t>Conceitos e exercícios sobre lógica de repetição ( condicional / contada )</t>
   </si>
 </sst>
 </file>
@@ -2235,17 +2238,56 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2262,50 +2304,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2316,39 +2348,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2858,7 +2861,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD4" sqref="AD4:AD11"/>
+      <selection pane="bottomRight" activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3167,110 +3170,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="195" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="195"/>
+      <c r="V2" s="195"/>
+      <c r="W2" s="195"/>
+      <c r="X2" s="195"/>
+      <c r="Y2" s="195"/>
+      <c r="Z2" s="195"/>
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="195"/>
+      <c r="AE2" s="195"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="195"/>
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="195"/>
+      <c r="AM2" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="195"/>
+      <c r="AQ2" s="195"/>
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="195"/>
+      <c r="AU2" s="195"/>
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="196"/>
+      <c r="AY2" s="196"/>
+      <c r="AZ2" s="196"/>
+      <c r="BA2" s="196"/>
+      <c r="BB2" s="196"/>
+      <c r="BC2" s="196"/>
+      <c r="BD2" s="196"/>
+      <c r="BE2" s="196"/>
+      <c r="BF2" s="196"/>
+      <c r="BG2" s="196"/>
+      <c r="BH2" s="196"/>
+      <c r="BI2" s="196"/>
+      <c r="BJ2" s="195" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="195"/>
+      <c r="BL2" s="195"/>
+      <c r="BM2" s="195"/>
+      <c r="BN2" s="195"/>
+      <c r="BO2" s="195"/>
+      <c r="BP2" s="195"/>
+      <c r="BQ2" s="195"/>
+      <c r="BR2" s="195"/>
+      <c r="BS2" s="195"/>
+      <c r="BT2" s="195"/>
+      <c r="BU2" s="195"/>
+      <c r="BV2" s="195"/>
+      <c r="BW2" s="195"/>
+      <c r="BX2" s="197"/>
+      <c r="BY2" s="197"/>
+      <c r="BZ2" s="197"/>
+      <c r="CA2" s="197"/>
+      <c r="CB2" s="197"/>
+      <c r="CC2" s="197"/>
+      <c r="CD2" s="197"/>
+      <c r="CE2" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="199"/>
+      <c r="CG2" s="199"/>
+      <c r="CH2" s="199"/>
+      <c r="CI2" s="199"/>
+      <c r="CJ2" s="199"/>
+      <c r="CK2" s="199"/>
+      <c r="CL2" s="199"/>
+      <c r="CM2" s="199"/>
+      <c r="CN2" s="199"/>
+      <c r="CO2" s="199"/>
+      <c r="CP2" s="199"/>
+      <c r="CQ2" s="199"/>
+      <c r="CR2" s="199"/>
+      <c r="CS2" s="199"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3566,632 +3569,609 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="201" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="202"/>
+      <c r="D4" s="200" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="200" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="200" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="200" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="200" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="200" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="200" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="200" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="193" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="193" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="193" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="193" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="193" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="193" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="193" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="193" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="193" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="193" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="193" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="192" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188" t="s">
+      <c r="X4" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="188" t="s">
+      <c r="Y4" s="192" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="188" t="s">
+      <c r="Z4" s="192" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="188" t="s">
+      <c r="AA4" s="192" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="217" t="s">
+      <c r="AB4" s="189" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="217" t="s">
+      <c r="AC4" s="189" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="217"/>
-      <c r="AE4" s="217"/>
-      <c r="AF4" s="217"/>
-      <c r="AG4" s="189"/>
-      <c r="AH4" s="189"/>
-      <c r="AI4" s="189"/>
-      <c r="AJ4" s="189"/>
-      <c r="AK4" s="189"/>
-      <c r="AL4" s="189"/>
-      <c r="AM4" s="189"/>
-      <c r="AN4" s="189"/>
-      <c r="AO4" s="189"/>
-      <c r="AP4" s="189"/>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
+      <c r="AD4" s="189" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE4" s="189"/>
+      <c r="AF4" s="189"/>
+      <c r="AG4" s="186"/>
+      <c r="AH4" s="186"/>
+      <c r="AI4" s="186"/>
+      <c r="AJ4" s="186"/>
+      <c r="AK4" s="186"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="195"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="198"/>
-      <c r="BG4" s="198"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="194"/>
+      <c r="AW4" s="194"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="194"/>
+      <c r="BW4" s="194"/>
+      <c r="CT4" s="194"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="201"/>
+      <c r="B5" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="218"/>
-      <c r="AC5" s="218"/>
-      <c r="AD5" s="218"/>
-      <c r="AE5" s="218"/>
-      <c r="AF5" s="218"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="190"/>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="190"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="190"/>
-      <c r="AP5" s="190"/>
-      <c r="AQ5" s="190"/>
-      <c r="AR5" s="193"/>
-      <c r="AS5" s="193"/>
-      <c r="AT5" s="193"/>
+      <c r="C5" s="202"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="193"/>
+      <c r="M5" s="193"/>
+      <c r="N5" s="193"/>
+      <c r="O5" s="193"/>
+      <c r="P5" s="193"/>
+      <c r="Q5" s="193"/>
+      <c r="R5" s="193"/>
+      <c r="S5" s="193"/>
+      <c r="T5" s="193"/>
+      <c r="U5" s="193"/>
+      <c r="V5" s="193"/>
+      <c r="W5" s="192"/>
+      <c r="X5" s="192"/>
+      <c r="Y5" s="192"/>
+      <c r="Z5" s="192"/>
+      <c r="AA5" s="192"/>
+      <c r="AB5" s="190"/>
+      <c r="AC5" s="190"/>
+      <c r="AD5" s="190"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="187"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="196"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="197"/>
-      <c r="BA5" s="197"/>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="199"/>
-      <c r="BG5" s="199"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="194"/>
+      <c r="AW5" s="194"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="194"/>
+      <c r="BW5" s="194"/>
+      <c r="CT5" s="194"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="201"/>
+      <c r="B6" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="218"/>
-      <c r="AC6" s="218"/>
-      <c r="AD6" s="218"/>
-      <c r="AE6" s="218"/>
-      <c r="AF6" s="218"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="190"/>
-      <c r="AI6" s="190"/>
-      <c r="AJ6" s="190"/>
-      <c r="AK6" s="190"/>
-      <c r="AL6" s="190"/>
-      <c r="AM6" s="190"/>
-      <c r="AN6" s="190"/>
-      <c r="AO6" s="190"/>
-      <c r="AP6" s="190"/>
-      <c r="AQ6" s="190"/>
-      <c r="AR6" s="193"/>
-      <c r="AS6" s="193"/>
-      <c r="AT6" s="193"/>
+      <c r="C6" s="202"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="H6" s="200"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="200"/>
+      <c r="K6" s="200"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
+      <c r="P6" s="193"/>
+      <c r="Q6" s="193"/>
+      <c r="R6" s="193"/>
+      <c r="S6" s="193"/>
+      <c r="T6" s="193"/>
+      <c r="U6" s="193"/>
+      <c r="V6" s="193"/>
+      <c r="W6" s="192"/>
+      <c r="X6" s="192"/>
+      <c r="Y6" s="192"/>
+      <c r="Z6" s="192"/>
+      <c r="AA6" s="192"/>
+      <c r="AB6" s="190"/>
+      <c r="AC6" s="190"/>
+      <c r="AD6" s="190"/>
+      <c r="AE6" s="190"/>
+      <c r="AF6" s="190"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="197"/>
-      <c r="AZ6" s="197"/>
-      <c r="BA6" s="197"/>
-      <c r="BB6" s="197"/>
-      <c r="BC6" s="197"/>
-      <c r="BD6" s="197"/>
-      <c r="BE6" s="197"/>
-      <c r="BF6" s="199"/>
-      <c r="BG6" s="199"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="194"/>
+      <c r="AW6" s="194"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="194"/>
+      <c r="BW6" s="194"/>
+      <c r="CT6" s="194"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="201"/>
+      <c r="B7" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="218"/>
-      <c r="AC7" s="218"/>
-      <c r="AD7" s="218"/>
-      <c r="AE7" s="218"/>
-      <c r="AF7" s="218"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="190"/>
-      <c r="AI7" s="190"/>
-      <c r="AJ7" s="190"/>
-      <c r="AK7" s="190"/>
-      <c r="AL7" s="190"/>
-      <c r="AM7" s="190"/>
-      <c r="AN7" s="190"/>
-      <c r="AO7" s="190"/>
-      <c r="AP7" s="190"/>
-      <c r="AQ7" s="190"/>
-      <c r="AR7" s="193"/>
-      <c r="AS7" s="193"/>
-      <c r="AT7" s="193"/>
+      <c r="C7" s="202"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="200"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="200"/>
+      <c r="J7" s="200"/>
+      <c r="K7" s="200"/>
+      <c r="L7" s="193"/>
+      <c r="M7" s="193"/>
+      <c r="N7" s="193"/>
+      <c r="O7" s="193"/>
+      <c r="P7" s="193"/>
+      <c r="Q7" s="193"/>
+      <c r="R7" s="193"/>
+      <c r="S7" s="193"/>
+      <c r="T7" s="193"/>
+      <c r="U7" s="193"/>
+      <c r="V7" s="193"/>
+      <c r="W7" s="192"/>
+      <c r="X7" s="192"/>
+      <c r="Y7" s="192"/>
+      <c r="Z7" s="192"/>
+      <c r="AA7" s="192"/>
+      <c r="AB7" s="190"/>
+      <c r="AC7" s="190"/>
+      <c r="AD7" s="190"/>
+      <c r="AE7" s="190"/>
+      <c r="AF7" s="190"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="196"/>
-      <c r="AY7" s="197"/>
-      <c r="AZ7" s="197"/>
-      <c r="BA7" s="197"/>
-      <c r="BB7" s="197"/>
-      <c r="BC7" s="197"/>
-      <c r="BD7" s="197"/>
-      <c r="BE7" s="197"/>
-      <c r="BF7" s="199"/>
-      <c r="BG7" s="199"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="194"/>
+      <c r="AW7" s="194"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="194"/>
+      <c r="BW7" s="194"/>
+      <c r="CT7" s="194"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="201" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
-      <c r="AB8" s="218"/>
-      <c r="AC8" s="218"/>
-      <c r="AD8" s="218"/>
-      <c r="AE8" s="218"/>
-      <c r="AF8" s="218"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="193"/>
-      <c r="AS8" s="193"/>
-      <c r="AT8" s="193"/>
+      <c r="C8" s="202"/>
+      <c r="D8" s="200"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="200"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="200"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="193"/>
+      <c r="N8" s="193"/>
+      <c r="O8" s="193"/>
+      <c r="P8" s="193"/>
+      <c r="Q8" s="193"/>
+      <c r="R8" s="193"/>
+      <c r="S8" s="193"/>
+      <c r="T8" s="193"/>
+      <c r="U8" s="193"/>
+      <c r="V8" s="193"/>
+      <c r="W8" s="192"/>
+      <c r="X8" s="192"/>
+      <c r="Y8" s="192"/>
+      <c r="Z8" s="192"/>
+      <c r="AA8" s="192"/>
+      <c r="AB8" s="190"/>
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="190"/>
+      <c r="AG8" s="187"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="196"/>
-      <c r="AY8" s="197"/>
-      <c r="AZ8" s="197"/>
-      <c r="BA8" s="197"/>
-      <c r="BB8" s="197"/>
-      <c r="BC8" s="197"/>
-      <c r="BD8" s="197"/>
-      <c r="BE8" s="197"/>
-      <c r="BF8" s="199"/>
-      <c r="BG8" s="199"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="194"/>
+      <c r="AW8" s="194"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="194"/>
+      <c r="BW8" s="194"/>
+      <c r="CT8" s="194"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="201"/>
+      <c r="B9" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
-      <c r="AB9" s="218"/>
-      <c r="AC9" s="218"/>
-      <c r="AD9" s="218"/>
-      <c r="AE9" s="218"/>
-      <c r="AF9" s="218"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="190"/>
-      <c r="AL9" s="190"/>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="190"/>
-      <c r="AQ9" s="190"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="200"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="193"/>
+      <c r="N9" s="193"/>
+      <c r="O9" s="193"/>
+      <c r="P9" s="193"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="193"/>
+      <c r="S9" s="193"/>
+      <c r="T9" s="193"/>
+      <c r="U9" s="193"/>
+      <c r="V9" s="193"/>
+      <c r="W9" s="192"/>
+      <c r="X9" s="192"/>
+      <c r="Y9" s="192"/>
+      <c r="Z9" s="192"/>
+      <c r="AA9" s="192"/>
+      <c r="AB9" s="190"/>
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="190"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="196"/>
-      <c r="AY9" s="197"/>
-      <c r="AZ9" s="197"/>
-      <c r="BA9" s="197"/>
-      <c r="BB9" s="197"/>
-      <c r="BC9" s="197"/>
-      <c r="BD9" s="197"/>
-      <c r="BE9" s="197"/>
-      <c r="BF9" s="199"/>
-      <c r="BG9" s="199"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="194"/>
+      <c r="AW9" s="194"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="194"/>
+      <c r="BW9" s="194"/>
+      <c r="CT9" s="194"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="201"/>
+      <c r="B10" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="218"/>
-      <c r="AC10" s="218"/>
-      <c r="AD10" s="218"/>
-      <c r="AE10" s="218"/>
-      <c r="AF10" s="218"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="190"/>
-      <c r="AI10" s="190"/>
-      <c r="AJ10" s="190"/>
-      <c r="AK10" s="190"/>
-      <c r="AL10" s="190"/>
-      <c r="AM10" s="190"/>
-      <c r="AN10" s="190"/>
-      <c r="AO10" s="190"/>
-      <c r="AP10" s="190"/>
-      <c r="AQ10" s="190"/>
-      <c r="AR10" s="193"/>
-      <c r="AS10" s="193"/>
-      <c r="AT10" s="193"/>
+      <c r="C10" s="202"/>
+      <c r="D10" s="200"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="200"/>
+      <c r="K10" s="200"/>
+      <c r="L10" s="193"/>
+      <c r="M10" s="193"/>
+      <c r="N10" s="193"/>
+      <c r="O10" s="193"/>
+      <c r="P10" s="193"/>
+      <c r="Q10" s="193"/>
+      <c r="R10" s="193"/>
+      <c r="S10" s="193"/>
+      <c r="T10" s="193"/>
+      <c r="U10" s="193"/>
+      <c r="V10" s="193"/>
+      <c r="W10" s="192"/>
+      <c r="X10" s="192"/>
+      <c r="Y10" s="192"/>
+      <c r="Z10" s="192"/>
+      <c r="AA10" s="192"/>
+      <c r="AB10" s="190"/>
+      <c r="AC10" s="190"/>
+      <c r="AD10" s="190"/>
+      <c r="AE10" s="190"/>
+      <c r="AF10" s="190"/>
+      <c r="AG10" s="187"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="196"/>
-      <c r="AY10" s="197"/>
-      <c r="AZ10" s="197"/>
-      <c r="BA10" s="197"/>
-      <c r="BB10" s="197"/>
-      <c r="BC10" s="197"/>
-      <c r="BD10" s="197"/>
-      <c r="BE10" s="197"/>
-      <c r="BF10" s="199"/>
-      <c r="BG10" s="199"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="194"/>
+      <c r="AW10" s="194"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="194"/>
+      <c r="BW10" s="194"/>
+      <c r="CT10" s="194"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="201"/>
+      <c r="B11" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="219"/>
-      <c r="AC11" s="219"/>
-      <c r="AD11" s="219"/>
-      <c r="AE11" s="219"/>
-      <c r="AF11" s="219"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="191"/>
-      <c r="AI11" s="191"/>
-      <c r="AJ11" s="191"/>
-      <c r="AK11" s="191"/>
-      <c r="AL11" s="191"/>
-      <c r="AM11" s="191"/>
-      <c r="AN11" s="191"/>
-      <c r="AO11" s="191"/>
-      <c r="AP11" s="191"/>
-      <c r="AQ11" s="191"/>
-      <c r="AR11" s="194"/>
-      <c r="AS11" s="194"/>
-      <c r="AT11" s="194"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="200"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="193"/>
+      <c r="M11" s="193"/>
+      <c r="N11" s="193"/>
+      <c r="O11" s="193"/>
+      <c r="P11" s="193"/>
+      <c r="Q11" s="193"/>
+      <c r="R11" s="193"/>
+      <c r="S11" s="193"/>
+      <c r="T11" s="193"/>
+      <c r="U11" s="193"/>
+      <c r="V11" s="193"/>
+      <c r="W11" s="192"/>
+      <c r="X11" s="192"/>
+      <c r="Y11" s="192"/>
+      <c r="Z11" s="192"/>
+      <c r="AA11" s="192"/>
+      <c r="AB11" s="191"/>
+      <c r="AC11" s="191"/>
+      <c r="AD11" s="191"/>
+      <c r="AE11" s="191"/>
+      <c r="AF11" s="191"/>
+      <c r="AG11" s="188"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="196"/>
-      <c r="AY11" s="197"/>
-      <c r="AZ11" s="197"/>
-      <c r="BA11" s="197"/>
-      <c r="BB11" s="197"/>
-      <c r="BC11" s="197"/>
-      <c r="BD11" s="197"/>
-      <c r="BE11" s="197"/>
-      <c r="BF11" s="199"/>
-      <c r="BG11" s="199"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="194"/>
+      <c r="AW11" s="194"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="194"/>
+      <c r="BW11" s="194"/>
+      <c r="CT11" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4208,22 +4188,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5745,13 +5750,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="212" t="s">
+      <c r="A4" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="214"/>
+      <c r="C4" s="208"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5856,9 +5861,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="201"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="201"/>
+      <c r="A5" s="206"/>
+      <c r="B5" s="204"/>
+      <c r="C5" s="206"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5963,11 +5968,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="201"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="201"/>
+      <c r="C6" s="206"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6072,11 +6077,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="201"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="201"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6181,11 +6186,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201"/>
+      <c r="A8" s="206"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="201"/>
+      <c r="C8" s="206"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6290,11 +6295,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+      <c r="A9" s="206"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="201"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6399,11 +6404,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+      <c r="A10" s="206"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6508,11 +6513,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
+      <c r="A11" s="206"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="206"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6617,9 +6622,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="201"/>
+      <c r="A12" s="206"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="202"/>
+      <c r="C12" s="209"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6724,10 +6729,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="210" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="211" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6836,8 +6841,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="201"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="206"/>
+      <c r="B14" s="212"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6958,7 +6963,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="201"/>
+      <c r="A15" s="206"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7068,7 +7073,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="206"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7178,7 +7183,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7290,7 +7295,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
+      <c r="A18" s="206"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7400,7 +7405,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
+      <c r="A19" s="206"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7510,7 +7515,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="201"/>
+      <c r="A20" s="206"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7620,7 +7625,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="202"/>
+      <c r="A21" s="209"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7731,7 +7736,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="203" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7841,7 +7846,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="211"/>
+      <c r="B23" s="204"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7948,13 +7953,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="203" t="s">
+      <c r="A24" s="214" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="205">
+      <c r="C24" s="216">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8062,11 +8067,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="204"/>
+      <c r="A25" s="215"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="201"/>
+      <c r="C25" s="206"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8172,11 +8177,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="204"/>
+      <c r="A26" s="215"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="206"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8282,11 +8287,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="204"/>
+      <c r="A27" s="215"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="201"/>
+      <c r="C27" s="206"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8392,11 +8397,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="204"/>
+      <c r="A28" s="215"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="201"/>
+      <c r="C28" s="206"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8502,11 +8507,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="204"/>
+      <c r="A29" s="215"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="201"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8612,11 +8617,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="204"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="201"/>
+      <c r="C30" s="206"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8722,11 +8727,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="204"/>
+      <c r="A31" s="215"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="201"/>
+      <c r="C31" s="206"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8832,11 +8837,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="204"/>
+      <c r="A32" s="215"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="201"/>
+      <c r="C32" s="206"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8942,11 +8947,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="204"/>
+      <c r="A33" s="215"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="201"/>
+      <c r="C33" s="206"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9052,11 +9057,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="204"/>
+      <c r="A34" s="215"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="201"/>
+      <c r="C34" s="206"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9162,11 +9167,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="204"/>
+      <c r="A35" s="215"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="202"/>
+      <c r="C35" s="209"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9272,11 +9277,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="204"/>
+      <c r="A36" s="215"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="205">
+      <c r="C36" s="216">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9384,11 +9389,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="204"/>
+      <c r="A37" s="215"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="201"/>
+      <c r="C37" s="206"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9494,11 +9499,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="204"/>
+      <c r="A38" s="215"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="201"/>
+      <c r="C38" s="206"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9604,11 +9609,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="204"/>
+      <c r="A39" s="215"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="201"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9714,11 +9719,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="204"/>
+      <c r="A40" s="215"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="201"/>
+      <c r="C40" s="206"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9824,11 +9829,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="204"/>
+      <c r="A41" s="215"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="201"/>
+      <c r="C41" s="206"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9934,11 +9939,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="204"/>
+      <c r="A42" s="215"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="201"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10044,11 +10049,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="204"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="201"/>
+      <c r="C43" s="206"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10154,11 +10159,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="204"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="201"/>
+      <c r="C44" s="206"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10264,11 +10269,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="204"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="206"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10374,11 +10379,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="204"/>
+      <c r="A46" s="215"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="201"/>
+      <c r="C46" s="206"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10484,11 +10489,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="204"/>
+      <c r="A47" s="215"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="201"/>
+      <c r="C47" s="206"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10602,11 +10607,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="204"/>
+      <c r="A48" s="215"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="201"/>
+      <c r="C48" s="206"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10715,7 +10720,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="217" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10825,7 +10830,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="207"/>
+      <c r="B50" s="212"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14256,7 +14261,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="208" t="s">
+      <c r="A81" s="218" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14368,7 +14373,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="201"/>
+      <c r="A82" s="206"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14478,7 +14483,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="201"/>
+      <c r="A83" s="206"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14588,7 +14593,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="201"/>
+      <c r="A84" s="206"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14698,7 +14703,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="201"/>
+      <c r="A85" s="206"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14808,7 +14813,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="201"/>
+      <c r="A86" s="206"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14918,7 +14923,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="201"/>
+      <c r="A87" s="206"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15030,7 +15035,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="201"/>
+      <c r="A88" s="206"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15140,7 +15145,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="201"/>
+      <c r="A89" s="206"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15250,7 +15255,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="201"/>
+      <c r="A90" s="206"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15360,11 +15365,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="201"/>
+      <c r="A91" s="206"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="209"/>
+      <c r="C91" s="219"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15470,11 +15475,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="201"/>
+      <c r="A92" s="206"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="206"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15580,11 +15585,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="202"/>
+      <c r="A93" s="209"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="201"/>
+      <c r="C93" s="206"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15808,7 +15813,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="200" t="s">
+      <c r="A95" s="213" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15920,7 +15925,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="201"/>
+      <c r="A96" s="206"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16030,7 +16035,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="201"/>
+      <c r="A97" s="206"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16140,7 +16145,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="201"/>
+      <c r="A98" s="206"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16250,7 +16255,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="201"/>
+      <c r="A99" s="206"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16360,7 +16365,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="201"/>
+      <c r="A100" s="206"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16470,7 +16475,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="201"/>
+      <c r="A101" s="206"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16580,7 +16585,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="201"/>
+      <c r="A102" s="206"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16690,7 +16695,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="201"/>
+      <c r="A103" s="206"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16802,7 +16807,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="201"/>
+      <c r="A104" s="206"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16912,7 +16917,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="201"/>
+      <c r="A105" s="206"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17030,7 +17035,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="201"/>
+      <c r="A106" s="206"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17140,7 +17145,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="201"/>
+      <c r="A107" s="206"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17250,7 +17255,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="201"/>
+      <c r="A108" s="206"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17360,7 +17365,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="201"/>
+      <c r="A109" s="206"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17470,7 +17475,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="201"/>
+      <c r="A110" s="206"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17580,7 +17585,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="201"/>
+      <c r="A111" s="206"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17690,7 +17695,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="201"/>
+      <c r="A112" s="206"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17800,7 +17805,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="201"/>
+      <c r="A113" s="206"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17910,7 +17915,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="201"/>
+      <c r="A114" s="206"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18020,7 +18025,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="201"/>
+      <c r="A115" s="206"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18130,7 +18135,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="201"/>
+      <c r="A116" s="206"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18256,7 +18261,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="201"/>
+      <c r="A117" s="206"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18366,7 +18371,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="202"/>
+      <c r="A118" s="209"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25737,12 +25742,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25750,6 +25749,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 19 e 20-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898F944F-86F7-42ED-B7C8-D4232185A487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD1986-1BD3-4ACF-97A0-2A61C9D88BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="171">
   <si>
     <t>S</t>
   </si>
@@ -713,6 +713,13 @@
   </si>
   <si>
     <t>Conceitos e exercícios sobre lógica de repetição ( condicional / contada )</t>
+  </si>
+  <si>
+    <t>Conceitos e exercícios sobre lógica de repetição ( condicional / contada ) usando C#</t>
+  </si>
+  <si>
+    <t>Correção de exercícios.
+Conceitos e exercícios sobre Vetor</t>
   </si>
 </sst>
 </file>
@@ -2238,14 +2245,56 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2262,82 +2311,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2348,10 +2335,30 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2858,10 +2865,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD12" sqref="AD12"/>
+      <selection pane="bottomRight" activeCell="AG4" sqref="AG4:AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3170,110 +3177,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="195" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="195"/>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="195" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="195"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="195"/>
-      <c r="V2" s="195"/>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195"/>
-      <c r="Z2" s="195"/>
-      <c r="AA2" s="195"/>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="195"/>
-      <c r="AD2" s="195"/>
-      <c r="AE2" s="195"/>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="195"/>
-      <c r="AH2" s="195"/>
-      <c r="AI2" s="195"/>
-      <c r="AJ2" s="195"/>
-      <c r="AK2" s="195"/>
-      <c r="AL2" s="195"/>
-      <c r="AM2" s="195" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="195"/>
-      <c r="AO2" s="195"/>
-      <c r="AP2" s="195"/>
-      <c r="AQ2" s="195"/>
-      <c r="AR2" s="195"/>
-      <c r="AS2" s="195"/>
-      <c r="AT2" s="195"/>
-      <c r="AU2" s="195"/>
-      <c r="AV2" s="195"/>
-      <c r="AW2" s="195"/>
-      <c r="AX2" s="196"/>
-      <c r="AY2" s="196"/>
-      <c r="AZ2" s="196"/>
-      <c r="BA2" s="196"/>
-      <c r="BB2" s="196"/>
-      <c r="BC2" s="196"/>
-      <c r="BD2" s="196"/>
-      <c r="BE2" s="196"/>
-      <c r="BF2" s="196"/>
-      <c r="BG2" s="196"/>
-      <c r="BH2" s="196"/>
-      <c r="BI2" s="196"/>
-      <c r="BJ2" s="195" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="195"/>
-      <c r="BL2" s="195"/>
-      <c r="BM2" s="195"/>
-      <c r="BN2" s="195"/>
-      <c r="BO2" s="195"/>
-      <c r="BP2" s="195"/>
-      <c r="BQ2" s="195"/>
-      <c r="BR2" s="195"/>
-      <c r="BS2" s="195"/>
-      <c r="BT2" s="195"/>
-      <c r="BU2" s="195"/>
-      <c r="BV2" s="195"/>
-      <c r="BW2" s="195"/>
-      <c r="BX2" s="197"/>
-      <c r="BY2" s="197"/>
-      <c r="BZ2" s="197"/>
-      <c r="CA2" s="197"/>
-      <c r="CB2" s="197"/>
-      <c r="CC2" s="197"/>
-      <c r="CD2" s="197"/>
-      <c r="CE2" s="198" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="199"/>
-      <c r="CG2" s="199"/>
-      <c r="CH2" s="199"/>
-      <c r="CI2" s="199"/>
-      <c r="CJ2" s="199"/>
-      <c r="CK2" s="199"/>
-      <c r="CL2" s="199"/>
-      <c r="CM2" s="199"/>
-      <c r="CN2" s="199"/>
-      <c r="CO2" s="199"/>
-      <c r="CP2" s="199"/>
-      <c r="CQ2" s="199"/>
-      <c r="CR2" s="199"/>
-      <c r="CS2" s="199"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3569,83 +3576,83 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="202" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="202"/>
-      <c r="D4" s="200" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="200" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="200" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="200" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="200" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="200" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="200" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="200" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="193" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="193" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="193" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="193" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="193" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="193" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="193" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="193" t="s">
+      <c r="S4" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="193" t="s">
+      <c r="T4" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="193" t="s">
+      <c r="U4" s="187" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="193" t="s">
+      <c r="V4" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="192" t="s">
+      <c r="W4" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="192" t="s">
+      <c r="X4" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="192" t="s">
+      <c r="Y4" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="192" t="s">
+      <c r="Z4" s="188" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="192" t="s">
+      <c r="AA4" s="188" t="s">
         <v>165</v>
       </c>
       <c r="AB4" s="189" t="s">
@@ -3657,505 +3664,566 @@
       <c r="AD4" s="189" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="189"/>
-      <c r="AG4" s="186"/>
-      <c r="AH4" s="186"/>
-      <c r="AI4" s="186"/>
-      <c r="AJ4" s="186"/>
-      <c r="AK4" s="186"/>
-      <c r="AL4" s="186"/>
-      <c r="AM4" s="186"/>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="AE4" s="189" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF4" s="189" t="s">
+        <v>170</v>
+      </c>
+      <c r="AG4" s="192"/>
+      <c r="AH4" s="192"/>
+      <c r="AI4" s="192"/>
+      <c r="AJ4" s="192"/>
+      <c r="AK4" s="192"/>
+      <c r="AL4" s="192"/>
+      <c r="AM4" s="192"/>
+      <c r="AN4" s="192"/>
+      <c r="AO4" s="192"/>
+      <c r="AP4" s="192"/>
+      <c r="AQ4" s="192"/>
+      <c r="AR4" s="195"/>
+      <c r="AS4" s="195"/>
+      <c r="AT4" s="195"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="194"/>
-      <c r="AW4" s="194"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="194"/>
-      <c r="BW4" s="194"/>
-      <c r="CT4" s="194"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="198"/>
+      <c r="AY4" s="200"/>
+      <c r="AZ4" s="200"/>
+      <c r="BA4" s="200"/>
+      <c r="BB4" s="200"/>
+      <c r="BC4" s="200"/>
+      <c r="BD4" s="200"/>
+      <c r="BE4" s="200"/>
+      <c r="BF4" s="201"/>
+      <c r="BG4" s="201"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="201"/>
-      <c r="B5" s="202" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="202"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200"/>
-      <c r="I5" s="200"/>
-      <c r="J5" s="200"/>
-      <c r="K5" s="200"/>
-      <c r="L5" s="193"/>
-      <c r="M5" s="193"/>
-      <c r="N5" s="193"/>
-      <c r="O5" s="193"/>
-      <c r="P5" s="193"/>
-      <c r="Q5" s="193"/>
-      <c r="R5" s="193"/>
-      <c r="S5" s="193"/>
-      <c r="T5" s="193"/>
-      <c r="U5" s="193"/>
-      <c r="V5" s="193"/>
-      <c r="W5" s="192"/>
-      <c r="X5" s="192"/>
-      <c r="Y5" s="192"/>
-      <c r="Z5" s="192"/>
-      <c r="AA5" s="192"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
       <c r="AB5" s="190"/>
       <c r="AC5" s="190"/>
       <c r="AD5" s="190"/>
       <c r="AE5" s="190"/>
       <c r="AF5" s="190"/>
-      <c r="AG5" s="187"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="AG5" s="193"/>
+      <c r="AH5" s="193"/>
+      <c r="AI5" s="193"/>
+      <c r="AJ5" s="193"/>
+      <c r="AK5" s="193"/>
+      <c r="AL5" s="193"/>
+      <c r="AM5" s="193"/>
+      <c r="AN5" s="193"/>
+      <c r="AO5" s="193"/>
+      <c r="AP5" s="193"/>
+      <c r="AQ5" s="193"/>
+      <c r="AR5" s="196"/>
+      <c r="AS5" s="196"/>
+      <c r="AT5" s="196"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="194"/>
-      <c r="AW5" s="194"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="194"/>
-      <c r="BW5" s="194"/>
-      <c r="CT5" s="194"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="199"/>
+      <c r="AY5" s="200"/>
+      <c r="AZ5" s="200"/>
+      <c r="BA5" s="200"/>
+      <c r="BB5" s="200"/>
+      <c r="BC5" s="200"/>
+      <c r="BD5" s="200"/>
+      <c r="BE5" s="200"/>
+      <c r="BF5" s="202"/>
+      <c r="BG5" s="202"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="201"/>
-      <c r="B6" s="202" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="202"/>
-      <c r="D6" s="200"/>
-      <c r="E6" s="200"/>
-      <c r="F6" s="200"/>
-      <c r="G6" s="200"/>
-      <c r="H6" s="200"/>
-      <c r="I6" s="200"/>
-      <c r="J6" s="200"/>
-      <c r="K6" s="200"/>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
-      <c r="O6" s="193"/>
-      <c r="P6" s="193"/>
-      <c r="Q6" s="193"/>
-      <c r="R6" s="193"/>
-      <c r="S6" s="193"/>
-      <c r="T6" s="193"/>
-      <c r="U6" s="193"/>
-      <c r="V6" s="193"/>
-      <c r="W6" s="192"/>
-      <c r="X6" s="192"/>
-      <c r="Y6" s="192"/>
-      <c r="Z6" s="192"/>
-      <c r="AA6" s="192"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
       <c r="AB6" s="190"/>
       <c r="AC6" s="190"/>
       <c r="AD6" s="190"/>
       <c r="AE6" s="190"/>
       <c r="AF6" s="190"/>
-      <c r="AG6" s="187"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="AG6" s="193"/>
+      <c r="AH6" s="193"/>
+      <c r="AI6" s="193"/>
+      <c r="AJ6" s="193"/>
+      <c r="AK6" s="193"/>
+      <c r="AL6" s="193"/>
+      <c r="AM6" s="193"/>
+      <c r="AN6" s="193"/>
+      <c r="AO6" s="193"/>
+      <c r="AP6" s="193"/>
+      <c r="AQ6" s="193"/>
+      <c r="AR6" s="196"/>
+      <c r="AS6" s="196"/>
+      <c r="AT6" s="196"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="CT6" s="194"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="199"/>
+      <c r="AY6" s="200"/>
+      <c r="AZ6" s="200"/>
+      <c r="BA6" s="200"/>
+      <c r="BB6" s="200"/>
+      <c r="BC6" s="200"/>
+      <c r="BD6" s="200"/>
+      <c r="BE6" s="200"/>
+      <c r="BF6" s="202"/>
+      <c r="BG6" s="202"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="201"/>
-      <c r="B7" s="202" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="202"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="200"/>
-      <c r="H7" s="200"/>
-      <c r="I7" s="200"/>
-      <c r="J7" s="200"/>
-      <c r="K7" s="200"/>
-      <c r="L7" s="193"/>
-      <c r="M7" s="193"/>
-      <c r="N7" s="193"/>
-      <c r="O7" s="193"/>
-      <c r="P7" s="193"/>
-      <c r="Q7" s="193"/>
-      <c r="R7" s="193"/>
-      <c r="S7" s="193"/>
-      <c r="T7" s="193"/>
-      <c r="U7" s="193"/>
-      <c r="V7" s="193"/>
-      <c r="W7" s="192"/>
-      <c r="X7" s="192"/>
-      <c r="Y7" s="192"/>
-      <c r="Z7" s="192"/>
-      <c r="AA7" s="192"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
       <c r="AB7" s="190"/>
       <c r="AC7" s="190"/>
       <c r="AD7" s="190"/>
       <c r="AE7" s="190"/>
       <c r="AF7" s="190"/>
-      <c r="AG7" s="187"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="AG7" s="193"/>
+      <c r="AH7" s="193"/>
+      <c r="AI7" s="193"/>
+      <c r="AJ7" s="193"/>
+      <c r="AK7" s="193"/>
+      <c r="AL7" s="193"/>
+      <c r="AM7" s="193"/>
+      <c r="AN7" s="193"/>
+      <c r="AO7" s="193"/>
+      <c r="AP7" s="193"/>
+      <c r="AQ7" s="193"/>
+      <c r="AR7" s="196"/>
+      <c r="AS7" s="196"/>
+      <c r="AT7" s="196"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="194"/>
-      <c r="AW7" s="194"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="194"/>
-      <c r="BW7" s="194"/>
-      <c r="CT7" s="194"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="199"/>
+      <c r="AY7" s="200"/>
+      <c r="AZ7" s="200"/>
+      <c r="BA7" s="200"/>
+      <c r="BB7" s="200"/>
+      <c r="BC7" s="200"/>
+      <c r="BD7" s="200"/>
+      <c r="BE7" s="200"/>
+      <c r="BF7" s="202"/>
+      <c r="BG7" s="202"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="201" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="202" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="202"/>
-      <c r="D8" s="200"/>
-      <c r="E8" s="200"/>
-      <c r="F8" s="200"/>
-      <c r="G8" s="200"/>
-      <c r="H8" s="200"/>
-      <c r="I8" s="200"/>
-      <c r="J8" s="200"/>
-      <c r="K8" s="200"/>
-      <c r="L8" s="193"/>
-      <c r="M8" s="193"/>
-      <c r="N8" s="193"/>
-      <c r="O8" s="193"/>
-      <c r="P8" s="193"/>
-      <c r="Q8" s="193"/>
-      <c r="R8" s="193"/>
-      <c r="S8" s="193"/>
-      <c r="T8" s="193"/>
-      <c r="U8" s="193"/>
-      <c r="V8" s="193"/>
-      <c r="W8" s="192"/>
-      <c r="X8" s="192"/>
-      <c r="Y8" s="192"/>
-      <c r="Z8" s="192"/>
-      <c r="AA8" s="192"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
       <c r="AB8" s="190"/>
       <c r="AC8" s="190"/>
       <c r="AD8" s="190"/>
       <c r="AE8" s="190"/>
       <c r="AF8" s="190"/>
-      <c r="AG8" s="187"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="AG8" s="193"/>
+      <c r="AH8" s="193"/>
+      <c r="AI8" s="193"/>
+      <c r="AJ8" s="193"/>
+      <c r="AK8" s="193"/>
+      <c r="AL8" s="193"/>
+      <c r="AM8" s="193"/>
+      <c r="AN8" s="193"/>
+      <c r="AO8" s="193"/>
+      <c r="AP8" s="193"/>
+      <c r="AQ8" s="193"/>
+      <c r="AR8" s="196"/>
+      <c r="AS8" s="196"/>
+      <c r="AT8" s="196"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="194"/>
-      <c r="AW8" s="194"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="194"/>
-      <c r="BW8" s="194"/>
-      <c r="CT8" s="194"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="199"/>
+      <c r="AY8" s="200"/>
+      <c r="AZ8" s="200"/>
+      <c r="BA8" s="200"/>
+      <c r="BB8" s="200"/>
+      <c r="BC8" s="200"/>
+      <c r="BD8" s="200"/>
+      <c r="BE8" s="200"/>
+      <c r="BF8" s="202"/>
+      <c r="BG8" s="202"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="201"/>
-      <c r="B9" s="202" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="202"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="200"/>
-      <c r="I9" s="200"/>
-      <c r="J9" s="200"/>
-      <c r="K9" s="200"/>
-      <c r="L9" s="193"/>
-      <c r="M9" s="193"/>
-      <c r="N9" s="193"/>
-      <c r="O9" s="193"/>
-      <c r="P9" s="193"/>
-      <c r="Q9" s="193"/>
-      <c r="R9" s="193"/>
-      <c r="S9" s="193"/>
-      <c r="T9" s="193"/>
-      <c r="U9" s="193"/>
-      <c r="V9" s="193"/>
-      <c r="W9" s="192"/>
-      <c r="X9" s="192"/>
-      <c r="Y9" s="192"/>
-      <c r="Z9" s="192"/>
-      <c r="AA9" s="192"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
       <c r="AB9" s="190"/>
       <c r="AC9" s="190"/>
       <c r="AD9" s="190"/>
       <c r="AE9" s="190"/>
       <c r="AF9" s="190"/>
-      <c r="AG9" s="187"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="AG9" s="193"/>
+      <c r="AH9" s="193"/>
+      <c r="AI9" s="193"/>
+      <c r="AJ9" s="193"/>
+      <c r="AK9" s="193"/>
+      <c r="AL9" s="193"/>
+      <c r="AM9" s="193"/>
+      <c r="AN9" s="193"/>
+      <c r="AO9" s="193"/>
+      <c r="AP9" s="193"/>
+      <c r="AQ9" s="193"/>
+      <c r="AR9" s="196"/>
+      <c r="AS9" s="196"/>
+      <c r="AT9" s="196"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="194"/>
-      <c r="AW9" s="194"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="194"/>
-      <c r="BW9" s="194"/>
-      <c r="CT9" s="194"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="199"/>
+      <c r="AY9" s="200"/>
+      <c r="AZ9" s="200"/>
+      <c r="BA9" s="200"/>
+      <c r="BB9" s="200"/>
+      <c r="BC9" s="200"/>
+      <c r="BD9" s="200"/>
+      <c r="BE9" s="200"/>
+      <c r="BF9" s="202"/>
+      <c r="BG9" s="202"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="200"/>
-      <c r="E10" s="200"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="200"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200"/>
-      <c r="K10" s="200"/>
-      <c r="L10" s="193"/>
-      <c r="M10" s="193"/>
-      <c r="N10" s="193"/>
-      <c r="O10" s="193"/>
-      <c r="P10" s="193"/>
-      <c r="Q10" s="193"/>
-      <c r="R10" s="193"/>
-      <c r="S10" s="193"/>
-      <c r="T10" s="193"/>
-      <c r="U10" s="193"/>
-      <c r="V10" s="193"/>
-      <c r="W10" s="192"/>
-      <c r="X10" s="192"/>
-      <c r="Y10" s="192"/>
-      <c r="Z10" s="192"/>
-      <c r="AA10" s="192"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
       <c r="AB10" s="190"/>
       <c r="AC10" s="190"/>
       <c r="AD10" s="190"/>
       <c r="AE10" s="190"/>
       <c r="AF10" s="190"/>
-      <c r="AG10" s="187"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="AG10" s="193"/>
+      <c r="AH10" s="193"/>
+      <c r="AI10" s="193"/>
+      <c r="AJ10" s="193"/>
+      <c r="AK10" s="193"/>
+      <c r="AL10" s="193"/>
+      <c r="AM10" s="193"/>
+      <c r="AN10" s="193"/>
+      <c r="AO10" s="193"/>
+      <c r="AP10" s="193"/>
+      <c r="AQ10" s="193"/>
+      <c r="AR10" s="196"/>
+      <c r="AS10" s="196"/>
+      <c r="AT10" s="196"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="194"/>
-      <c r="AW10" s="194"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="194"/>
-      <c r="BW10" s="194"/>
-      <c r="CT10" s="194"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="199"/>
+      <c r="AY10" s="200"/>
+      <c r="AZ10" s="200"/>
+      <c r="BA10" s="200"/>
+      <c r="BB10" s="200"/>
+      <c r="BC10" s="200"/>
+      <c r="BD10" s="200"/>
+      <c r="BE10" s="200"/>
+      <c r="BF10" s="202"/>
+      <c r="BG10" s="202"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="201"/>
-      <c r="B11" s="202" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="202"/>
-      <c r="D11" s="200"/>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="200"/>
-      <c r="H11" s="200"/>
-      <c r="I11" s="200"/>
-      <c r="J11" s="200"/>
-      <c r="K11" s="200"/>
-      <c r="L11" s="193"/>
-      <c r="M11" s="193"/>
-      <c r="N11" s="193"/>
-      <c r="O11" s="193"/>
-      <c r="P11" s="193"/>
-      <c r="Q11" s="193"/>
-      <c r="R11" s="193"/>
-      <c r="S11" s="193"/>
-      <c r="T11" s="193"/>
-      <c r="U11" s="193"/>
-      <c r="V11" s="193"/>
-      <c r="W11" s="192"/>
-      <c r="X11" s="192"/>
-      <c r="Y11" s="192"/>
-      <c r="Z11" s="192"/>
-      <c r="AA11" s="192"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
       <c r="AB11" s="191"/>
       <c r="AC11" s="191"/>
       <c r="AD11" s="191"/>
       <c r="AE11" s="191"/>
       <c r="AF11" s="191"/>
-      <c r="AG11" s="188"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="AG11" s="194"/>
+      <c r="AH11" s="194"/>
+      <c r="AI11" s="194"/>
+      <c r="AJ11" s="194"/>
+      <c r="AK11" s="194"/>
+      <c r="AL11" s="194"/>
+      <c r="AM11" s="194"/>
+      <c r="AN11" s="194"/>
+      <c r="AO11" s="194"/>
+      <c r="AP11" s="194"/>
+      <c r="AQ11" s="194"/>
+      <c r="AR11" s="197"/>
+      <c r="AS11" s="197"/>
+      <c r="AT11" s="197"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="194"/>
-      <c r="AW11" s="194"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="194"/>
-      <c r="BW11" s="194"/>
-      <c r="CT11" s="194"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="199"/>
+      <c r="AY11" s="200"/>
+      <c r="AZ11" s="200"/>
+      <c r="BA11" s="200"/>
+      <c r="BB11" s="200"/>
+      <c r="BC11" s="200"/>
+      <c r="BD11" s="200"/>
+      <c r="BE11" s="200"/>
+      <c r="BF11" s="202"/>
+      <c r="BG11" s="202"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4172,63 +4240,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5750,13 +5761,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="205" t="s">
+      <c r="A4" s="215" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="207" t="s">
+      <c r="B4" s="216" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="208"/>
+      <c r="C4" s="217"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5861,9 +5872,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="206"/>
-      <c r="B5" s="204"/>
-      <c r="C5" s="206"/>
+      <c r="A5" s="204"/>
+      <c r="B5" s="214"/>
+      <c r="C5" s="204"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5968,11 +5979,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="206"/>
+      <c r="A6" s="204"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="206"/>
+      <c r="C6" s="204"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6077,11 +6088,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="206"/>
+      <c r="A7" s="204"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="206"/>
+      <c r="C7" s="204"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6186,11 +6197,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="206"/>
+      <c r="A8" s="204"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="206"/>
+      <c r="C8" s="204"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6295,11 +6306,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="206"/>
+      <c r="A9" s="204"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="206"/>
+      <c r="C9" s="204"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6404,11 +6415,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="206"/>
+      <c r="A10" s="204"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="206"/>
+      <c r="C10" s="204"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6513,11 +6524,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="206"/>
+      <c r="A11" s="204"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="206"/>
+      <c r="C11" s="204"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6622,9 +6633,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="206"/>
+      <c r="A12" s="204"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="209"/>
+      <c r="C12" s="205"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6729,10 +6740,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="210" t="s">
+      <c r="A13" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="211" t="s">
+      <c r="B13" s="219" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6841,8 +6852,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="206"/>
-      <c r="B14" s="212"/>
+      <c r="A14" s="204"/>
+      <c r="B14" s="210"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6963,7 +6974,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="206"/>
+      <c r="A15" s="204"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7073,7 +7084,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="206"/>
+      <c r="A16" s="204"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7183,7 +7194,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="206"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7295,7 +7306,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="206"/>
+      <c r="A18" s="204"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7405,7 +7416,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="206"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7515,7 +7526,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="206"/>
+      <c r="A20" s="204"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7625,7 +7636,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="209"/>
+      <c r="A21" s="205"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7736,7 +7747,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="213" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7846,7 +7857,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="204"/>
+      <c r="B23" s="214"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7953,13 +7964,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="214" t="s">
+      <c r="A24" s="206" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="216">
+      <c r="C24" s="208">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8067,11 +8078,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="215"/>
+      <c r="A25" s="207"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="206"/>
+      <c r="C25" s="204"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8177,11 +8188,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="215"/>
+      <c r="A26" s="207"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="206"/>
+      <c r="C26" s="204"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8287,11 +8298,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="215"/>
+      <c r="A27" s="207"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="206"/>
+      <c r="C27" s="204"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8397,11 +8408,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="215"/>
+      <c r="A28" s="207"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="206"/>
+      <c r="C28" s="204"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8507,11 +8518,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="215"/>
+      <c r="A29" s="207"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="206"/>
+      <c r="C29" s="204"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8617,11 +8628,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="215"/>
+      <c r="A30" s="207"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="206"/>
+      <c r="C30" s="204"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8727,11 +8738,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="215"/>
+      <c r="A31" s="207"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="206"/>
+      <c r="C31" s="204"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8837,11 +8848,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="215"/>
+      <c r="A32" s="207"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="206"/>
+      <c r="C32" s="204"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8947,11 +8958,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="215"/>
+      <c r="A33" s="207"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="206"/>
+      <c r="C33" s="204"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9057,11 +9068,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="215"/>
+      <c r="A34" s="207"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="206"/>
+      <c r="C34" s="204"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9167,11 +9178,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="215"/>
+      <c r="A35" s="207"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="209"/>
+      <c r="C35" s="205"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9277,11 +9288,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="215"/>
+      <c r="A36" s="207"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="216">
+      <c r="C36" s="208">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9389,11 +9400,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="215"/>
+      <c r="A37" s="207"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="206"/>
+      <c r="C37" s="204"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9499,11 +9510,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="215"/>
+      <c r="A38" s="207"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="206"/>
+      <c r="C38" s="204"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9609,11 +9620,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="215"/>
+      <c r="A39" s="207"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="206"/>
+      <c r="C39" s="204"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9719,11 +9730,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="215"/>
+      <c r="A40" s="207"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="206"/>
+      <c r="C40" s="204"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9829,11 +9840,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="215"/>
+      <c r="A41" s="207"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="206"/>
+      <c r="C41" s="204"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9939,11 +9950,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="215"/>
+      <c r="A42" s="207"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="206"/>
+      <c r="C42" s="204"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10049,11 +10060,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="215"/>
+      <c r="A43" s="207"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="206"/>
+      <c r="C43" s="204"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10159,11 +10170,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="215"/>
+      <c r="A44" s="207"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="206"/>
+      <c r="C44" s="204"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10269,11 +10280,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="215"/>
+      <c r="A45" s="207"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="206"/>
+      <c r="C45" s="204"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10379,11 +10390,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="215"/>
+      <c r="A46" s="207"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="206"/>
+      <c r="C46" s="204"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10489,11 +10500,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="215"/>
+      <c r="A47" s="207"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="206"/>
+      <c r="C47" s="204"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10607,11 +10618,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="215"/>
+      <c r="A48" s="207"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="206"/>
+      <c r="C48" s="204"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10720,7 +10731,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="217" t="s">
+      <c r="B49" s="209" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10830,7 +10841,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="212"/>
+      <c r="B50" s="210"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14261,7 +14272,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="218" t="s">
+      <c r="A81" s="211" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14373,7 +14384,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="206"/>
+      <c r="A82" s="204"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14483,7 +14494,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="206"/>
+      <c r="A83" s="204"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14593,7 +14604,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="206"/>
+      <c r="A84" s="204"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14703,7 +14714,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="206"/>
+      <c r="A85" s="204"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14813,7 +14824,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="206"/>
+      <c r="A86" s="204"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14923,7 +14934,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="206"/>
+      <c r="A87" s="204"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15035,7 +15046,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="206"/>
+      <c r="A88" s="204"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15145,7 +15156,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="206"/>
+      <c r="A89" s="204"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15255,7 +15266,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="206"/>
+      <c r="A90" s="204"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15365,11 +15376,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="206"/>
+      <c r="A91" s="204"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="219"/>
+      <c r="C91" s="212"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15475,11 +15486,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="206"/>
+      <c r="A92" s="204"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="206"/>
+      <c r="C92" s="204"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15585,11 +15596,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="209"/>
+      <c r="A93" s="205"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="206"/>
+      <c r="C93" s="204"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15813,7 +15824,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="213" t="s">
+      <c r="A95" s="203" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15925,7 +15936,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="206"/>
+      <c r="A96" s="204"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16035,7 +16046,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="206"/>
+      <c r="A97" s="204"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16145,7 +16156,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="206"/>
+      <c r="A98" s="204"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16255,7 +16266,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="206"/>
+      <c r="A99" s="204"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16365,7 +16376,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="206"/>
+      <c r="A100" s="204"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16475,7 +16486,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="206"/>
+      <c r="A101" s="204"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16585,7 +16596,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="206"/>
+      <c r="A102" s="204"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16695,7 +16706,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="206"/>
+      <c r="A103" s="204"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16807,7 +16818,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="206"/>
+      <c r="A104" s="204"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16917,7 +16928,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="206"/>
+      <c r="A105" s="204"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17035,7 +17046,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="206"/>
+      <c r="A106" s="204"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17145,7 +17156,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="206"/>
+      <c r="A107" s="204"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17255,7 +17266,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="206"/>
+      <c r="A108" s="204"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17365,7 +17376,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="206"/>
+      <c r="A109" s="204"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17475,7 +17486,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="206"/>
+      <c r="A110" s="204"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17585,7 +17596,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="206"/>
+      <c r="A111" s="204"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17695,7 +17706,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="206"/>
+      <c r="A112" s="204"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17805,7 +17816,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="206"/>
+      <c r="A113" s="204"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17915,7 +17926,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="206"/>
+      <c r="A114" s="204"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18025,7 +18036,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="206"/>
+      <c r="A115" s="204"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18135,7 +18146,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="206"/>
+      <c r="A116" s="204"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18261,7 +18272,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="206"/>
+      <c r="A117" s="204"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18371,7 +18382,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="209"/>
+      <c r="A118" s="205"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25742,6 +25753,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25749,12 +25766,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 23-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD1986-1BD3-4ACF-97A0-2A61C9D88BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083CACA2-B5F2-4710-BF5E-99FDEE52EA60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="172">
   <si>
     <t>S</t>
   </si>
@@ -720,6 +720,9 @@
   <si>
     <t>Correção de exercícios.
 Conceitos e exercícios sobre Vetor</t>
+  </si>
+  <si>
+    <t>Correção de exercícios sobre Vetor</t>
   </si>
 </sst>
 </file>
@@ -2245,17 +2248,56 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2272,59 +2314,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2335,30 +2358,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2868,7 +2871,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG4" sqref="AG4:AG11"/>
+      <selection pane="bottomRight" activeCell="AE4" sqref="AE4:AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3177,110 +3180,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="195" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="195"/>
+      <c r="V2" s="195"/>
+      <c r="W2" s="195"/>
+      <c r="X2" s="195"/>
+      <c r="Y2" s="195"/>
+      <c r="Z2" s="195"/>
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="195"/>
+      <c r="AE2" s="195"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="195"/>
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="195"/>
+      <c r="AM2" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="195"/>
+      <c r="AQ2" s="195"/>
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="195"/>
+      <c r="AU2" s="195"/>
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="196"/>
+      <c r="AY2" s="196"/>
+      <c r="AZ2" s="196"/>
+      <c r="BA2" s="196"/>
+      <c r="BB2" s="196"/>
+      <c r="BC2" s="196"/>
+      <c r="BD2" s="196"/>
+      <c r="BE2" s="196"/>
+      <c r="BF2" s="196"/>
+      <c r="BG2" s="196"/>
+      <c r="BH2" s="196"/>
+      <c r="BI2" s="196"/>
+      <c r="BJ2" s="195" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="195"/>
+      <c r="BL2" s="195"/>
+      <c r="BM2" s="195"/>
+      <c r="BN2" s="195"/>
+      <c r="BO2" s="195"/>
+      <c r="BP2" s="195"/>
+      <c r="BQ2" s="195"/>
+      <c r="BR2" s="195"/>
+      <c r="BS2" s="195"/>
+      <c r="BT2" s="195"/>
+      <c r="BU2" s="195"/>
+      <c r="BV2" s="195"/>
+      <c r="BW2" s="195"/>
+      <c r="BX2" s="197"/>
+      <c r="BY2" s="197"/>
+      <c r="BZ2" s="197"/>
+      <c r="CA2" s="197"/>
+      <c r="CB2" s="197"/>
+      <c r="CC2" s="197"/>
+      <c r="CD2" s="197"/>
+      <c r="CE2" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="199"/>
+      <c r="CG2" s="199"/>
+      <c r="CH2" s="199"/>
+      <c r="CI2" s="199"/>
+      <c r="CJ2" s="199"/>
+      <c r="CK2" s="199"/>
+      <c r="CL2" s="199"/>
+      <c r="CM2" s="199"/>
+      <c r="CN2" s="199"/>
+      <c r="CO2" s="199"/>
+      <c r="CP2" s="199"/>
+      <c r="CQ2" s="199"/>
+      <c r="CR2" s="199"/>
+      <c r="CS2" s="199"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3576,83 +3579,83 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="201" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="202"/>
+      <c r="D4" s="200" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="200" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="200" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="200" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="200" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="200" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="200" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="200" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="193" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="193" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="193" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="193" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="193" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="193" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="193" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="193" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="193" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="193" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="193" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="192" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188" t="s">
+      <c r="X4" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="188" t="s">
+      <c r="Y4" s="192" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="188" t="s">
+      <c r="Z4" s="192" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="188" t="s">
+      <c r="AA4" s="192" t="s">
         <v>165</v>
       </c>
       <c r="AB4" s="189" t="s">
@@ -3670,544 +3673,521 @@
       <c r="AF4" s="189" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="192"/>
-      <c r="AH4" s="192"/>
-      <c r="AI4" s="192"/>
-      <c r="AJ4" s="192"/>
-      <c r="AK4" s="192"/>
-      <c r="AL4" s="192"/>
-      <c r="AM4" s="192"/>
-      <c r="AN4" s="192"/>
-      <c r="AO4" s="192"/>
-      <c r="AP4" s="192"/>
-      <c r="AQ4" s="192"/>
-      <c r="AR4" s="195"/>
-      <c r="AS4" s="195"/>
-      <c r="AT4" s="195"/>
+      <c r="AG4" s="189" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH4" s="186"/>
+      <c r="AI4" s="186"/>
+      <c r="AJ4" s="186"/>
+      <c r="AK4" s="186"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="198"/>
-      <c r="AY4" s="200"/>
-      <c r="AZ4" s="200"/>
-      <c r="BA4" s="200"/>
-      <c r="BB4" s="200"/>
-      <c r="BC4" s="200"/>
-      <c r="BD4" s="200"/>
-      <c r="BE4" s="200"/>
-      <c r="BF4" s="201"/>
-      <c r="BG4" s="201"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="194"/>
+      <c r="AW4" s="194"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="194"/>
+      <c r="BW4" s="194"/>
+      <c r="CT4" s="194"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="201"/>
+      <c r="B5" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
+      <c r="C5" s="202"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="193"/>
+      <c r="M5" s="193"/>
+      <c r="N5" s="193"/>
+      <c r="O5" s="193"/>
+      <c r="P5" s="193"/>
+      <c r="Q5" s="193"/>
+      <c r="R5" s="193"/>
+      <c r="S5" s="193"/>
+      <c r="T5" s="193"/>
+      <c r="U5" s="193"/>
+      <c r="V5" s="193"/>
+      <c r="W5" s="192"/>
+      <c r="X5" s="192"/>
+      <c r="Y5" s="192"/>
+      <c r="Z5" s="192"/>
+      <c r="AA5" s="192"/>
       <c r="AB5" s="190"/>
       <c r="AC5" s="190"/>
       <c r="AD5" s="190"/>
       <c r="AE5" s="190"/>
       <c r="AF5" s="190"/>
-      <c r="AG5" s="193"/>
-      <c r="AH5" s="193"/>
-      <c r="AI5" s="193"/>
-      <c r="AJ5" s="193"/>
-      <c r="AK5" s="193"/>
-      <c r="AL5" s="193"/>
-      <c r="AM5" s="193"/>
-      <c r="AN5" s="193"/>
-      <c r="AO5" s="193"/>
-      <c r="AP5" s="193"/>
-      <c r="AQ5" s="193"/>
-      <c r="AR5" s="196"/>
-      <c r="AS5" s="196"/>
-      <c r="AT5" s="196"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="199"/>
-      <c r="AY5" s="200"/>
-      <c r="AZ5" s="200"/>
-      <c r="BA5" s="200"/>
-      <c r="BB5" s="200"/>
-      <c r="BC5" s="200"/>
-      <c r="BD5" s="200"/>
-      <c r="BE5" s="200"/>
-      <c r="BF5" s="202"/>
-      <c r="BG5" s="202"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="194"/>
+      <c r="AW5" s="194"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="194"/>
+      <c r="BW5" s="194"/>
+      <c r="CT5" s="194"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="201"/>
+      <c r="B6" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
+      <c r="C6" s="202"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="H6" s="200"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="200"/>
+      <c r="K6" s="200"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
+      <c r="P6" s="193"/>
+      <c r="Q6" s="193"/>
+      <c r="R6" s="193"/>
+      <c r="S6" s="193"/>
+      <c r="T6" s="193"/>
+      <c r="U6" s="193"/>
+      <c r="V6" s="193"/>
+      <c r="W6" s="192"/>
+      <c r="X6" s="192"/>
+      <c r="Y6" s="192"/>
+      <c r="Z6" s="192"/>
+      <c r="AA6" s="192"/>
       <c r="AB6" s="190"/>
       <c r="AC6" s="190"/>
       <c r="AD6" s="190"/>
       <c r="AE6" s="190"/>
       <c r="AF6" s="190"/>
-      <c r="AG6" s="193"/>
-      <c r="AH6" s="193"/>
-      <c r="AI6" s="193"/>
-      <c r="AJ6" s="193"/>
-      <c r="AK6" s="193"/>
-      <c r="AL6" s="193"/>
-      <c r="AM6" s="193"/>
-      <c r="AN6" s="193"/>
-      <c r="AO6" s="193"/>
-      <c r="AP6" s="193"/>
-      <c r="AQ6" s="193"/>
-      <c r="AR6" s="196"/>
-      <c r="AS6" s="196"/>
-      <c r="AT6" s="196"/>
+      <c r="AG6" s="190"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="199"/>
-      <c r="AY6" s="200"/>
-      <c r="AZ6" s="200"/>
-      <c r="BA6" s="200"/>
-      <c r="BB6" s="200"/>
-      <c r="BC6" s="200"/>
-      <c r="BD6" s="200"/>
-      <c r="BE6" s="200"/>
-      <c r="BF6" s="202"/>
-      <c r="BG6" s="202"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="194"/>
+      <c r="AW6" s="194"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="194"/>
+      <c r="BW6" s="194"/>
+      <c r="CT6" s="194"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="201"/>
+      <c r="B7" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
+      <c r="C7" s="202"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="200"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="200"/>
+      <c r="J7" s="200"/>
+      <c r="K7" s="200"/>
+      <c r="L7" s="193"/>
+      <c r="M7" s="193"/>
+      <c r="N7" s="193"/>
+      <c r="O7" s="193"/>
+      <c r="P7" s="193"/>
+      <c r="Q7" s="193"/>
+      <c r="R7" s="193"/>
+      <c r="S7" s="193"/>
+      <c r="T7" s="193"/>
+      <c r="U7" s="193"/>
+      <c r="V7" s="193"/>
+      <c r="W7" s="192"/>
+      <c r="X7" s="192"/>
+      <c r="Y7" s="192"/>
+      <c r="Z7" s="192"/>
+      <c r="AA7" s="192"/>
       <c r="AB7" s="190"/>
       <c r="AC7" s="190"/>
       <c r="AD7" s="190"/>
       <c r="AE7" s="190"/>
       <c r="AF7" s="190"/>
-      <c r="AG7" s="193"/>
-      <c r="AH7" s="193"/>
-      <c r="AI7" s="193"/>
-      <c r="AJ7" s="193"/>
-      <c r="AK7" s="193"/>
-      <c r="AL7" s="193"/>
-      <c r="AM7" s="193"/>
-      <c r="AN7" s="193"/>
-      <c r="AO7" s="193"/>
-      <c r="AP7" s="193"/>
-      <c r="AQ7" s="193"/>
-      <c r="AR7" s="196"/>
-      <c r="AS7" s="196"/>
-      <c r="AT7" s="196"/>
+      <c r="AG7" s="190"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="199"/>
-      <c r="AY7" s="200"/>
-      <c r="AZ7" s="200"/>
-      <c r="BA7" s="200"/>
-      <c r="BB7" s="200"/>
-      <c r="BC7" s="200"/>
-      <c r="BD7" s="200"/>
-      <c r="BE7" s="200"/>
-      <c r="BF7" s="202"/>
-      <c r="BG7" s="202"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="194"/>
+      <c r="AW7" s="194"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="194"/>
+      <c r="BW7" s="194"/>
+      <c r="CT7" s="194"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="201" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
+      <c r="C8" s="202"/>
+      <c r="D8" s="200"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="200"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="200"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="193"/>
+      <c r="N8" s="193"/>
+      <c r="O8" s="193"/>
+      <c r="P8" s="193"/>
+      <c r="Q8" s="193"/>
+      <c r="R8" s="193"/>
+      <c r="S8" s="193"/>
+      <c r="T8" s="193"/>
+      <c r="U8" s="193"/>
+      <c r="V8" s="193"/>
+      <c r="W8" s="192"/>
+      <c r="X8" s="192"/>
+      <c r="Y8" s="192"/>
+      <c r="Z8" s="192"/>
+      <c r="AA8" s="192"/>
       <c r="AB8" s="190"/>
       <c r="AC8" s="190"/>
       <c r="AD8" s="190"/>
       <c r="AE8" s="190"/>
       <c r="AF8" s="190"/>
-      <c r="AG8" s="193"/>
-      <c r="AH8" s="193"/>
-      <c r="AI8" s="193"/>
-      <c r="AJ8" s="193"/>
-      <c r="AK8" s="193"/>
-      <c r="AL8" s="193"/>
-      <c r="AM8" s="193"/>
-      <c r="AN8" s="193"/>
-      <c r="AO8" s="193"/>
-      <c r="AP8" s="193"/>
-      <c r="AQ8" s="193"/>
-      <c r="AR8" s="196"/>
-      <c r="AS8" s="196"/>
-      <c r="AT8" s="196"/>
+      <c r="AG8" s="190"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="199"/>
-      <c r="AY8" s="200"/>
-      <c r="AZ8" s="200"/>
-      <c r="BA8" s="200"/>
-      <c r="BB8" s="200"/>
-      <c r="BC8" s="200"/>
-      <c r="BD8" s="200"/>
-      <c r="BE8" s="200"/>
-      <c r="BF8" s="202"/>
-      <c r="BG8" s="202"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="194"/>
+      <c r="AW8" s="194"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="194"/>
+      <c r="BW8" s="194"/>
+      <c r="CT8" s="194"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="201"/>
+      <c r="B9" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="200"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="193"/>
+      <c r="N9" s="193"/>
+      <c r="O9" s="193"/>
+      <c r="P9" s="193"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="193"/>
+      <c r="S9" s="193"/>
+      <c r="T9" s="193"/>
+      <c r="U9" s="193"/>
+      <c r="V9" s="193"/>
+      <c r="W9" s="192"/>
+      <c r="X9" s="192"/>
+      <c r="Y9" s="192"/>
+      <c r="Z9" s="192"/>
+      <c r="AA9" s="192"/>
       <c r="AB9" s="190"/>
       <c r="AC9" s="190"/>
       <c r="AD9" s="190"/>
       <c r="AE9" s="190"/>
       <c r="AF9" s="190"/>
-      <c r="AG9" s="193"/>
-      <c r="AH9" s="193"/>
-      <c r="AI9" s="193"/>
-      <c r="AJ9" s="193"/>
-      <c r="AK9" s="193"/>
-      <c r="AL9" s="193"/>
-      <c r="AM9" s="193"/>
-      <c r="AN9" s="193"/>
-      <c r="AO9" s="193"/>
-      <c r="AP9" s="193"/>
-      <c r="AQ9" s="193"/>
-      <c r="AR9" s="196"/>
-      <c r="AS9" s="196"/>
-      <c r="AT9" s="196"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="199"/>
-      <c r="AY9" s="200"/>
-      <c r="AZ9" s="200"/>
-      <c r="BA9" s="200"/>
-      <c r="BB9" s="200"/>
-      <c r="BC9" s="200"/>
-      <c r="BD9" s="200"/>
-      <c r="BE9" s="200"/>
-      <c r="BF9" s="202"/>
-      <c r="BG9" s="202"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="194"/>
+      <c r="AW9" s="194"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="194"/>
+      <c r="BW9" s="194"/>
+      <c r="CT9" s="194"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="201"/>
+      <c r="B10" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
+      <c r="C10" s="202"/>
+      <c r="D10" s="200"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="200"/>
+      <c r="K10" s="200"/>
+      <c r="L10" s="193"/>
+      <c r="M10" s="193"/>
+      <c r="N10" s="193"/>
+      <c r="O10" s="193"/>
+      <c r="P10" s="193"/>
+      <c r="Q10" s="193"/>
+      <c r="R10" s="193"/>
+      <c r="S10" s="193"/>
+      <c r="T10" s="193"/>
+      <c r="U10" s="193"/>
+      <c r="V10" s="193"/>
+      <c r="W10" s="192"/>
+      <c r="X10" s="192"/>
+      <c r="Y10" s="192"/>
+      <c r="Z10" s="192"/>
+      <c r="AA10" s="192"/>
       <c r="AB10" s="190"/>
       <c r="AC10" s="190"/>
       <c r="AD10" s="190"/>
       <c r="AE10" s="190"/>
       <c r="AF10" s="190"/>
-      <c r="AG10" s="193"/>
-      <c r="AH10" s="193"/>
-      <c r="AI10" s="193"/>
-      <c r="AJ10" s="193"/>
-      <c r="AK10" s="193"/>
-      <c r="AL10" s="193"/>
-      <c r="AM10" s="193"/>
-      <c r="AN10" s="193"/>
-      <c r="AO10" s="193"/>
-      <c r="AP10" s="193"/>
-      <c r="AQ10" s="193"/>
-      <c r="AR10" s="196"/>
-      <c r="AS10" s="196"/>
-      <c r="AT10" s="196"/>
+      <c r="AG10" s="190"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="199"/>
-      <c r="AY10" s="200"/>
-      <c r="AZ10" s="200"/>
-      <c r="BA10" s="200"/>
-      <c r="BB10" s="200"/>
-      <c r="BC10" s="200"/>
-      <c r="BD10" s="200"/>
-      <c r="BE10" s="200"/>
-      <c r="BF10" s="202"/>
-      <c r="BG10" s="202"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="194"/>
+      <c r="AW10" s="194"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="194"/>
+      <c r="BW10" s="194"/>
+      <c r="CT10" s="194"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="201"/>
+      <c r="B11" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="200"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="193"/>
+      <c r="M11" s="193"/>
+      <c r="N11" s="193"/>
+      <c r="O11" s="193"/>
+      <c r="P11" s="193"/>
+      <c r="Q11" s="193"/>
+      <c r="R11" s="193"/>
+      <c r="S11" s="193"/>
+      <c r="T11" s="193"/>
+      <c r="U11" s="193"/>
+      <c r="V11" s="193"/>
+      <c r="W11" s="192"/>
+      <c r="X11" s="192"/>
+      <c r="Y11" s="192"/>
+      <c r="Z11" s="192"/>
+      <c r="AA11" s="192"/>
       <c r="AB11" s="191"/>
       <c r="AC11" s="191"/>
       <c r="AD11" s="191"/>
       <c r="AE11" s="191"/>
       <c r="AF11" s="191"/>
-      <c r="AG11" s="194"/>
-      <c r="AH11" s="194"/>
-      <c r="AI11" s="194"/>
-      <c r="AJ11" s="194"/>
-      <c r="AK11" s="194"/>
-      <c r="AL11" s="194"/>
-      <c r="AM11" s="194"/>
-      <c r="AN11" s="194"/>
-      <c r="AO11" s="194"/>
-      <c r="AP11" s="194"/>
-      <c r="AQ11" s="194"/>
-      <c r="AR11" s="197"/>
-      <c r="AS11" s="197"/>
-      <c r="AT11" s="197"/>
+      <c r="AG11" s="191"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="199"/>
-      <c r="AY11" s="200"/>
-      <c r="AZ11" s="200"/>
-      <c r="BA11" s="200"/>
-      <c r="BB11" s="200"/>
-      <c r="BC11" s="200"/>
-      <c r="BD11" s="200"/>
-      <c r="BE11" s="200"/>
-      <c r="BF11" s="202"/>
-      <c r="BG11" s="202"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="194"/>
+      <c r="AW11" s="194"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="194"/>
+      <c r="BW11" s="194"/>
+      <c r="CT11" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4224,22 +4204,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5761,13 +5766,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="215" t="s">
+      <c r="A4" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="217"/>
+      <c r="C4" s="208"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5872,9 +5877,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="204"/>
-      <c r="B5" s="214"/>
-      <c r="C5" s="204"/>
+      <c r="A5" s="206"/>
+      <c r="B5" s="204"/>
+      <c r="C5" s="206"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5979,11 +5984,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="204"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="204"/>
+      <c r="C6" s="206"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6088,11 +6093,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="204"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="204"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6197,11 +6202,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="204"/>
+      <c r="A8" s="206"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="204"/>
+      <c r="C8" s="206"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6306,11 +6311,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="204"/>
+      <c r="A9" s="206"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="204"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6415,11 +6420,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="204"/>
+      <c r="A10" s="206"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="204"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6524,11 +6529,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="204"/>
+      <c r="A11" s="206"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="204"/>
+      <c r="C11" s="206"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6633,9 +6638,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="204"/>
+      <c r="A12" s="206"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="205"/>
+      <c r="C12" s="209"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6740,10 +6745,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="218" t="s">
+      <c r="A13" s="210" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="219" t="s">
+      <c r="B13" s="211" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6852,8 +6857,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="204"/>
-      <c r="B14" s="210"/>
+      <c r="A14" s="206"/>
+      <c r="B14" s="212"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6974,7 +6979,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="204"/>
+      <c r="A15" s="206"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7084,7 +7089,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="204"/>
+      <c r="A16" s="206"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7194,7 +7199,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="204"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7306,7 +7311,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="204"/>
+      <c r="A18" s="206"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7416,7 +7421,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="204"/>
+      <c r="A19" s="206"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7526,7 +7531,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="204"/>
+      <c r="A20" s="206"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7636,7 +7641,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="205"/>
+      <c r="A21" s="209"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7747,7 +7752,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="203" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7857,7 +7862,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="214"/>
+      <c r="B23" s="204"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7964,13 +7969,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="206" t="s">
+      <c r="A24" s="214" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="208">
+      <c r="C24" s="216">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8078,11 +8083,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="207"/>
+      <c r="A25" s="215"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="204"/>
+      <c r="C25" s="206"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8188,11 +8193,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="207"/>
+      <c r="A26" s="215"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="204"/>
+      <c r="C26" s="206"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8298,11 +8303,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="207"/>
+      <c r="A27" s="215"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="204"/>
+      <c r="C27" s="206"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8408,11 +8413,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="207"/>
+      <c r="A28" s="215"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="204"/>
+      <c r="C28" s="206"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8518,11 +8523,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="207"/>
+      <c r="A29" s="215"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="204"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8628,11 +8633,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="207"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="204"/>
+      <c r="C30" s="206"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8738,11 +8743,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="207"/>
+      <c r="A31" s="215"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="204"/>
+      <c r="C31" s="206"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8848,11 +8853,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="207"/>
+      <c r="A32" s="215"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="204"/>
+      <c r="C32" s="206"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8958,11 +8963,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="207"/>
+      <c r="A33" s="215"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="204"/>
+      <c r="C33" s="206"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9068,11 +9073,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="207"/>
+      <c r="A34" s="215"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="204"/>
+      <c r="C34" s="206"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9178,11 +9183,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="207"/>
+      <c r="A35" s="215"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="205"/>
+      <c r="C35" s="209"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9288,11 +9293,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="207"/>
+      <c r="A36" s="215"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="208">
+      <c r="C36" s="216">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9400,11 +9405,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="207"/>
+      <c r="A37" s="215"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="204"/>
+      <c r="C37" s="206"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9510,11 +9515,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="207"/>
+      <c r="A38" s="215"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="204"/>
+      <c r="C38" s="206"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9620,11 +9625,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="207"/>
+      <c r="A39" s="215"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="204"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9730,11 +9735,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="207"/>
+      <c r="A40" s="215"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="204"/>
+      <c r="C40" s="206"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9840,11 +9845,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="207"/>
+      <c r="A41" s="215"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="204"/>
+      <c r="C41" s="206"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9950,11 +9955,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="207"/>
+      <c r="A42" s="215"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="204"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10060,11 +10065,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="207"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="204"/>
+      <c r="C43" s="206"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10170,11 +10175,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="207"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="204"/>
+      <c r="C44" s="206"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10280,11 +10285,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="207"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="204"/>
+      <c r="C45" s="206"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10390,11 +10395,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="207"/>
+      <c r="A46" s="215"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="204"/>
+      <c r="C46" s="206"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10500,11 +10505,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="207"/>
+      <c r="A47" s="215"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="204"/>
+      <c r="C47" s="206"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10618,11 +10623,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="207"/>
+      <c r="A48" s="215"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="204"/>
+      <c r="C48" s="206"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10731,7 +10736,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="209" t="s">
+      <c r="B49" s="217" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10841,7 +10846,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="210"/>
+      <c r="B50" s="212"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14272,7 +14277,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="211" t="s">
+      <c r="A81" s="218" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14384,7 +14389,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="204"/>
+      <c r="A82" s="206"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14494,7 +14499,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="204"/>
+      <c r="A83" s="206"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14604,7 +14609,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="204"/>
+      <c r="A84" s="206"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14714,7 +14719,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="204"/>
+      <c r="A85" s="206"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14824,7 +14829,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="204"/>
+      <c r="A86" s="206"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14934,7 +14939,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="204"/>
+      <c r="A87" s="206"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15046,7 +15051,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="204"/>
+      <c r="A88" s="206"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15156,7 +15161,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="204"/>
+      <c r="A89" s="206"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15266,7 +15271,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="204"/>
+      <c r="A90" s="206"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15376,11 +15381,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="204"/>
+      <c r="A91" s="206"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="212"/>
+      <c r="C91" s="219"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15486,11 +15491,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="204"/>
+      <c r="A92" s="206"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="204"/>
+      <c r="C92" s="206"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15596,11 +15601,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="205"/>
+      <c r="A93" s="209"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="204"/>
+      <c r="C93" s="206"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15824,7 +15829,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="203" t="s">
+      <c r="A95" s="213" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15936,7 +15941,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="204"/>
+      <c r="A96" s="206"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16046,7 +16051,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="204"/>
+      <c r="A97" s="206"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16156,7 +16161,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="204"/>
+      <c r="A98" s="206"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16266,7 +16271,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="204"/>
+      <c r="A99" s="206"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16376,7 +16381,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="204"/>
+      <c r="A100" s="206"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16486,7 +16491,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="204"/>
+      <c r="A101" s="206"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16596,7 +16601,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="204"/>
+      <c r="A102" s="206"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16706,7 +16711,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="204"/>
+      <c r="A103" s="206"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16818,7 +16823,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="204"/>
+      <c r="A104" s="206"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16928,7 +16933,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="204"/>
+      <c r="A105" s="206"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17046,7 +17051,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="204"/>
+      <c r="A106" s="206"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17156,7 +17161,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="204"/>
+      <c r="A107" s="206"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17266,7 +17271,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="204"/>
+      <c r="A108" s="206"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17376,7 +17381,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="204"/>
+      <c r="A109" s="206"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17486,7 +17491,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="204"/>
+      <c r="A110" s="206"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17596,7 +17601,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="204"/>
+      <c r="A111" s="206"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17706,7 +17711,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="204"/>
+      <c r="A112" s="206"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17816,7 +17821,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="204"/>
+      <c r="A113" s="206"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17926,7 +17931,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="204"/>
+      <c r="A114" s="206"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18036,7 +18041,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="204"/>
+      <c r="A115" s="206"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18146,7 +18151,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="204"/>
+      <c r="A116" s="206"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18272,7 +18277,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="204"/>
+      <c r="A117" s="206"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18382,7 +18387,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="205"/>
+      <c r="A118" s="209"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25753,12 +25758,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25766,6 +25765,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 24-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083CACA2-B5F2-4710-BF5E-99FDEE52EA60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E928BD8C-0612-48C8-9CB3-C28C3C135447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="173">
   <si>
     <t>S</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>Correção de exercícios sobre Vetor</t>
+  </si>
+  <si>
+    <t>Planejamento dos conteúdos de Front-End II</t>
   </si>
 </sst>
 </file>
@@ -2248,14 +2251,56 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2272,82 +2317,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2358,10 +2341,30 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2871,7 +2874,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AE4" sqref="AE4:AE11"/>
+      <selection pane="bottomRight" activeCell="AH4" sqref="AH4:AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3180,110 +3183,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="195" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="195"/>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="195" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="195"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="195"/>
-      <c r="V2" s="195"/>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195"/>
-      <c r="Z2" s="195"/>
-      <c r="AA2" s="195"/>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="195"/>
-      <c r="AD2" s="195"/>
-      <c r="AE2" s="195"/>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="195"/>
-      <c r="AH2" s="195"/>
-      <c r="AI2" s="195"/>
-      <c r="AJ2" s="195"/>
-      <c r="AK2" s="195"/>
-      <c r="AL2" s="195"/>
-      <c r="AM2" s="195" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="195"/>
-      <c r="AO2" s="195"/>
-      <c r="AP2" s="195"/>
-      <c r="AQ2" s="195"/>
-      <c r="AR2" s="195"/>
-      <c r="AS2" s="195"/>
-      <c r="AT2" s="195"/>
-      <c r="AU2" s="195"/>
-      <c r="AV2" s="195"/>
-      <c r="AW2" s="195"/>
-      <c r="AX2" s="196"/>
-      <c r="AY2" s="196"/>
-      <c r="AZ2" s="196"/>
-      <c r="BA2" s="196"/>
-      <c r="BB2" s="196"/>
-      <c r="BC2" s="196"/>
-      <c r="BD2" s="196"/>
-      <c r="BE2" s="196"/>
-      <c r="BF2" s="196"/>
-      <c r="BG2" s="196"/>
-      <c r="BH2" s="196"/>
-      <c r="BI2" s="196"/>
-      <c r="BJ2" s="195" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="195"/>
-      <c r="BL2" s="195"/>
-      <c r="BM2" s="195"/>
-      <c r="BN2" s="195"/>
-      <c r="BO2" s="195"/>
-      <c r="BP2" s="195"/>
-      <c r="BQ2" s="195"/>
-      <c r="BR2" s="195"/>
-      <c r="BS2" s="195"/>
-      <c r="BT2" s="195"/>
-      <c r="BU2" s="195"/>
-      <c r="BV2" s="195"/>
-      <c r="BW2" s="195"/>
-      <c r="BX2" s="197"/>
-      <c r="BY2" s="197"/>
-      <c r="BZ2" s="197"/>
-      <c r="CA2" s="197"/>
-      <c r="CB2" s="197"/>
-      <c r="CC2" s="197"/>
-      <c r="CD2" s="197"/>
-      <c r="CE2" s="198" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="199"/>
-      <c r="CG2" s="199"/>
-      <c r="CH2" s="199"/>
-      <c r="CI2" s="199"/>
-      <c r="CJ2" s="199"/>
-      <c r="CK2" s="199"/>
-      <c r="CL2" s="199"/>
-      <c r="CM2" s="199"/>
-      <c r="CN2" s="199"/>
-      <c r="CO2" s="199"/>
-      <c r="CP2" s="199"/>
-      <c r="CQ2" s="199"/>
-      <c r="CR2" s="199"/>
-      <c r="CS2" s="199"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3579,83 +3582,83 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="202" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="202"/>
-      <c r="D4" s="200" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="200" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="200" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="200" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="200" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="200" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="200" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="200" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="193" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="193" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="193" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="193" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="193" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="193" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="193" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="193" t="s">
+      <c r="S4" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="193" t="s">
+      <c r="T4" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="193" t="s">
+      <c r="U4" s="187" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="193" t="s">
+      <c r="V4" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="192" t="s">
+      <c r="W4" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="192" t="s">
+      <c r="X4" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="192" t="s">
+      <c r="Y4" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="192" t="s">
+      <c r="Z4" s="188" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="192" t="s">
+      <c r="AA4" s="188" t="s">
         <v>165</v>
       </c>
       <c r="AB4" s="189" t="s">
@@ -3676,502 +3679,561 @@
       <c r="AG4" s="189" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="186"/>
-      <c r="AI4" s="186"/>
-      <c r="AJ4" s="186"/>
-      <c r="AK4" s="186"/>
-      <c r="AL4" s="186"/>
-      <c r="AM4" s="186"/>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="AH4" s="192" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI4" s="192"/>
+      <c r="AJ4" s="192"/>
+      <c r="AK4" s="192"/>
+      <c r="AL4" s="192"/>
+      <c r="AM4" s="192"/>
+      <c r="AN4" s="192"/>
+      <c r="AO4" s="192"/>
+      <c r="AP4" s="192"/>
+      <c r="AQ4" s="192"/>
+      <c r="AR4" s="195"/>
+      <c r="AS4" s="195"/>
+      <c r="AT4" s="195"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="194"/>
-      <c r="AW4" s="194"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="194"/>
-      <c r="BW4" s="194"/>
-      <c r="CT4" s="194"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="198"/>
+      <c r="AY4" s="200"/>
+      <c r="AZ4" s="200"/>
+      <c r="BA4" s="200"/>
+      <c r="BB4" s="200"/>
+      <c r="BC4" s="200"/>
+      <c r="BD4" s="200"/>
+      <c r="BE4" s="200"/>
+      <c r="BF4" s="201"/>
+      <c r="BG4" s="201"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="201"/>
-      <c r="B5" s="202" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="202"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200"/>
-      <c r="I5" s="200"/>
-      <c r="J5" s="200"/>
-      <c r="K5" s="200"/>
-      <c r="L5" s="193"/>
-      <c r="M5" s="193"/>
-      <c r="N5" s="193"/>
-      <c r="O5" s="193"/>
-      <c r="P5" s="193"/>
-      <c r="Q5" s="193"/>
-      <c r="R5" s="193"/>
-      <c r="S5" s="193"/>
-      <c r="T5" s="193"/>
-      <c r="U5" s="193"/>
-      <c r="V5" s="193"/>
-      <c r="W5" s="192"/>
-      <c r="X5" s="192"/>
-      <c r="Y5" s="192"/>
-      <c r="Z5" s="192"/>
-      <c r="AA5" s="192"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
       <c r="AB5" s="190"/>
       <c r="AC5" s="190"/>
       <c r="AD5" s="190"/>
       <c r="AE5" s="190"/>
       <c r="AF5" s="190"/>
       <c r="AG5" s="190"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="AH5" s="193"/>
+      <c r="AI5" s="193"/>
+      <c r="AJ5" s="193"/>
+      <c r="AK5" s="193"/>
+      <c r="AL5" s="193"/>
+      <c r="AM5" s="193"/>
+      <c r="AN5" s="193"/>
+      <c r="AO5" s="193"/>
+      <c r="AP5" s="193"/>
+      <c r="AQ5" s="193"/>
+      <c r="AR5" s="196"/>
+      <c r="AS5" s="196"/>
+      <c r="AT5" s="196"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="194"/>
-      <c r="AW5" s="194"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="194"/>
-      <c r="BW5" s="194"/>
-      <c r="CT5" s="194"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="199"/>
+      <c r="AY5" s="200"/>
+      <c r="AZ5" s="200"/>
+      <c r="BA5" s="200"/>
+      <c r="BB5" s="200"/>
+      <c r="BC5" s="200"/>
+      <c r="BD5" s="200"/>
+      <c r="BE5" s="200"/>
+      <c r="BF5" s="202"/>
+      <c r="BG5" s="202"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="201"/>
-      <c r="B6" s="202" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="202"/>
-      <c r="D6" s="200"/>
-      <c r="E6" s="200"/>
-      <c r="F6" s="200"/>
-      <c r="G6" s="200"/>
-      <c r="H6" s="200"/>
-      <c r="I6" s="200"/>
-      <c r="J6" s="200"/>
-      <c r="K6" s="200"/>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
-      <c r="O6" s="193"/>
-      <c r="P6" s="193"/>
-      <c r="Q6" s="193"/>
-      <c r="R6" s="193"/>
-      <c r="S6" s="193"/>
-      <c r="T6" s="193"/>
-      <c r="U6" s="193"/>
-      <c r="V6" s="193"/>
-      <c r="W6" s="192"/>
-      <c r="X6" s="192"/>
-      <c r="Y6" s="192"/>
-      <c r="Z6" s="192"/>
-      <c r="AA6" s="192"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
       <c r="AB6" s="190"/>
       <c r="AC6" s="190"/>
       <c r="AD6" s="190"/>
       <c r="AE6" s="190"/>
       <c r="AF6" s="190"/>
       <c r="AG6" s="190"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="AH6" s="193"/>
+      <c r="AI6" s="193"/>
+      <c r="AJ6" s="193"/>
+      <c r="AK6" s="193"/>
+      <c r="AL6" s="193"/>
+      <c r="AM6" s="193"/>
+      <c r="AN6" s="193"/>
+      <c r="AO6" s="193"/>
+      <c r="AP6" s="193"/>
+      <c r="AQ6" s="193"/>
+      <c r="AR6" s="196"/>
+      <c r="AS6" s="196"/>
+      <c r="AT6" s="196"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="CT6" s="194"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="199"/>
+      <c r="AY6" s="200"/>
+      <c r="AZ6" s="200"/>
+      <c r="BA6" s="200"/>
+      <c r="BB6" s="200"/>
+      <c r="BC6" s="200"/>
+      <c r="BD6" s="200"/>
+      <c r="BE6" s="200"/>
+      <c r="BF6" s="202"/>
+      <c r="BG6" s="202"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="201"/>
-      <c r="B7" s="202" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="202"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="200"/>
-      <c r="H7" s="200"/>
-      <c r="I7" s="200"/>
-      <c r="J7" s="200"/>
-      <c r="K7" s="200"/>
-      <c r="L7" s="193"/>
-      <c r="M7" s="193"/>
-      <c r="N7" s="193"/>
-      <c r="O7" s="193"/>
-      <c r="P7" s="193"/>
-      <c r="Q7" s="193"/>
-      <c r="R7" s="193"/>
-      <c r="S7" s="193"/>
-      <c r="T7" s="193"/>
-      <c r="U7" s="193"/>
-      <c r="V7" s="193"/>
-      <c r="W7" s="192"/>
-      <c r="X7" s="192"/>
-      <c r="Y7" s="192"/>
-      <c r="Z7" s="192"/>
-      <c r="AA7" s="192"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
       <c r="AB7" s="190"/>
       <c r="AC7" s="190"/>
       <c r="AD7" s="190"/>
       <c r="AE7" s="190"/>
       <c r="AF7" s="190"/>
       <c r="AG7" s="190"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="AH7" s="193"/>
+      <c r="AI7" s="193"/>
+      <c r="AJ7" s="193"/>
+      <c r="AK7" s="193"/>
+      <c r="AL7" s="193"/>
+      <c r="AM7" s="193"/>
+      <c r="AN7" s="193"/>
+      <c r="AO7" s="193"/>
+      <c r="AP7" s="193"/>
+      <c r="AQ7" s="193"/>
+      <c r="AR7" s="196"/>
+      <c r="AS7" s="196"/>
+      <c r="AT7" s="196"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="194"/>
-      <c r="AW7" s="194"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="194"/>
-      <c r="BW7" s="194"/>
-      <c r="CT7" s="194"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="199"/>
+      <c r="AY7" s="200"/>
+      <c r="AZ7" s="200"/>
+      <c r="BA7" s="200"/>
+      <c r="BB7" s="200"/>
+      <c r="BC7" s="200"/>
+      <c r="BD7" s="200"/>
+      <c r="BE7" s="200"/>
+      <c r="BF7" s="202"/>
+      <c r="BG7" s="202"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="201" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="202" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="202"/>
-      <c r="D8" s="200"/>
-      <c r="E8" s="200"/>
-      <c r="F8" s="200"/>
-      <c r="G8" s="200"/>
-      <c r="H8" s="200"/>
-      <c r="I8" s="200"/>
-      <c r="J8" s="200"/>
-      <c r="K8" s="200"/>
-      <c r="L8" s="193"/>
-      <c r="M8" s="193"/>
-      <c r="N8" s="193"/>
-      <c r="O8" s="193"/>
-      <c r="P8" s="193"/>
-      <c r="Q8" s="193"/>
-      <c r="R8" s="193"/>
-      <c r="S8" s="193"/>
-      <c r="T8" s="193"/>
-      <c r="U8" s="193"/>
-      <c r="V8" s="193"/>
-      <c r="W8" s="192"/>
-      <c r="X8" s="192"/>
-      <c r="Y8" s="192"/>
-      <c r="Z8" s="192"/>
-      <c r="AA8" s="192"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
       <c r="AB8" s="190"/>
       <c r="AC8" s="190"/>
       <c r="AD8" s="190"/>
       <c r="AE8" s="190"/>
       <c r="AF8" s="190"/>
       <c r="AG8" s="190"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="AH8" s="193"/>
+      <c r="AI8" s="193"/>
+      <c r="AJ8" s="193"/>
+      <c r="AK8" s="193"/>
+      <c r="AL8" s="193"/>
+      <c r="AM8" s="193"/>
+      <c r="AN8" s="193"/>
+      <c r="AO8" s="193"/>
+      <c r="AP8" s="193"/>
+      <c r="AQ8" s="193"/>
+      <c r="AR8" s="196"/>
+      <c r="AS8" s="196"/>
+      <c r="AT8" s="196"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="194"/>
-      <c r="AW8" s="194"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="194"/>
-      <c r="BW8" s="194"/>
-      <c r="CT8" s="194"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="199"/>
+      <c r="AY8" s="200"/>
+      <c r="AZ8" s="200"/>
+      <c r="BA8" s="200"/>
+      <c r="BB8" s="200"/>
+      <c r="BC8" s="200"/>
+      <c r="BD8" s="200"/>
+      <c r="BE8" s="200"/>
+      <c r="BF8" s="202"/>
+      <c r="BG8" s="202"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="201"/>
-      <c r="B9" s="202" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="202"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="200"/>
-      <c r="I9" s="200"/>
-      <c r="J9" s="200"/>
-      <c r="K9" s="200"/>
-      <c r="L9" s="193"/>
-      <c r="M9" s="193"/>
-      <c r="N9" s="193"/>
-      <c r="O9" s="193"/>
-      <c r="P9" s="193"/>
-      <c r="Q9" s="193"/>
-      <c r="R9" s="193"/>
-      <c r="S9" s="193"/>
-      <c r="T9" s="193"/>
-      <c r="U9" s="193"/>
-      <c r="V9" s="193"/>
-      <c r="W9" s="192"/>
-      <c r="X9" s="192"/>
-      <c r="Y9" s="192"/>
-      <c r="Z9" s="192"/>
-      <c r="AA9" s="192"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
       <c r="AB9" s="190"/>
       <c r="AC9" s="190"/>
       <c r="AD9" s="190"/>
       <c r="AE9" s="190"/>
       <c r="AF9" s="190"/>
       <c r="AG9" s="190"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="AH9" s="193"/>
+      <c r="AI9" s="193"/>
+      <c r="AJ9" s="193"/>
+      <c r="AK9" s="193"/>
+      <c r="AL9" s="193"/>
+      <c r="AM9" s="193"/>
+      <c r="AN9" s="193"/>
+      <c r="AO9" s="193"/>
+      <c r="AP9" s="193"/>
+      <c r="AQ9" s="193"/>
+      <c r="AR9" s="196"/>
+      <c r="AS9" s="196"/>
+      <c r="AT9" s="196"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="194"/>
-      <c r="AW9" s="194"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="194"/>
-      <c r="BW9" s="194"/>
-      <c r="CT9" s="194"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="199"/>
+      <c r="AY9" s="200"/>
+      <c r="AZ9" s="200"/>
+      <c r="BA9" s="200"/>
+      <c r="BB9" s="200"/>
+      <c r="BC9" s="200"/>
+      <c r="BD9" s="200"/>
+      <c r="BE9" s="200"/>
+      <c r="BF9" s="202"/>
+      <c r="BG9" s="202"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="200"/>
-      <c r="E10" s="200"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="200"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200"/>
-      <c r="K10" s="200"/>
-      <c r="L10" s="193"/>
-      <c r="M10" s="193"/>
-      <c r="N10" s="193"/>
-      <c r="O10" s="193"/>
-      <c r="P10" s="193"/>
-      <c r="Q10" s="193"/>
-      <c r="R10" s="193"/>
-      <c r="S10" s="193"/>
-      <c r="T10" s="193"/>
-      <c r="U10" s="193"/>
-      <c r="V10" s="193"/>
-      <c r="W10" s="192"/>
-      <c r="X10" s="192"/>
-      <c r="Y10" s="192"/>
-      <c r="Z10" s="192"/>
-      <c r="AA10" s="192"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
       <c r="AB10" s="190"/>
       <c r="AC10" s="190"/>
       <c r="AD10" s="190"/>
       <c r="AE10" s="190"/>
       <c r="AF10" s="190"/>
       <c r="AG10" s="190"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="AH10" s="193"/>
+      <c r="AI10" s="193"/>
+      <c r="AJ10" s="193"/>
+      <c r="AK10" s="193"/>
+      <c r="AL10" s="193"/>
+      <c r="AM10" s="193"/>
+      <c r="AN10" s="193"/>
+      <c r="AO10" s="193"/>
+      <c r="AP10" s="193"/>
+      <c r="AQ10" s="193"/>
+      <c r="AR10" s="196"/>
+      <c r="AS10" s="196"/>
+      <c r="AT10" s="196"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="194"/>
-      <c r="AW10" s="194"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="194"/>
-      <c r="BW10" s="194"/>
-      <c r="CT10" s="194"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="199"/>
+      <c r="AY10" s="200"/>
+      <c r="AZ10" s="200"/>
+      <c r="BA10" s="200"/>
+      <c r="BB10" s="200"/>
+      <c r="BC10" s="200"/>
+      <c r="BD10" s="200"/>
+      <c r="BE10" s="200"/>
+      <c r="BF10" s="202"/>
+      <c r="BG10" s="202"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="201"/>
-      <c r="B11" s="202" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="202"/>
-      <c r="D11" s="200"/>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="200"/>
-      <c r="H11" s="200"/>
-      <c r="I11" s="200"/>
-      <c r="J11" s="200"/>
-      <c r="K11" s="200"/>
-      <c r="L11" s="193"/>
-      <c r="M11" s="193"/>
-      <c r="N11" s="193"/>
-      <c r="O11" s="193"/>
-      <c r="P11" s="193"/>
-      <c r="Q11" s="193"/>
-      <c r="R11" s="193"/>
-      <c r="S11" s="193"/>
-      <c r="T11" s="193"/>
-      <c r="U11" s="193"/>
-      <c r="V11" s="193"/>
-      <c r="W11" s="192"/>
-      <c r="X11" s="192"/>
-      <c r="Y11" s="192"/>
-      <c r="Z11" s="192"/>
-      <c r="AA11" s="192"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
       <c r="AB11" s="191"/>
       <c r="AC11" s="191"/>
       <c r="AD11" s="191"/>
       <c r="AE11" s="191"/>
       <c r="AF11" s="191"/>
       <c r="AG11" s="191"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="AH11" s="194"/>
+      <c r="AI11" s="194"/>
+      <c r="AJ11" s="194"/>
+      <c r="AK11" s="194"/>
+      <c r="AL11" s="194"/>
+      <c r="AM11" s="194"/>
+      <c r="AN11" s="194"/>
+      <c r="AO11" s="194"/>
+      <c r="AP11" s="194"/>
+      <c r="AQ11" s="194"/>
+      <c r="AR11" s="197"/>
+      <c r="AS11" s="197"/>
+      <c r="AT11" s="197"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="194"/>
-      <c r="AW11" s="194"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="194"/>
-      <c r="BW11" s="194"/>
-      <c r="CT11" s="194"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="199"/>
+      <c r="AY11" s="200"/>
+      <c r="AZ11" s="200"/>
+      <c r="BA11" s="200"/>
+      <c r="BB11" s="200"/>
+      <c r="BC11" s="200"/>
+      <c r="BD11" s="200"/>
+      <c r="BE11" s="200"/>
+      <c r="BF11" s="202"/>
+      <c r="BG11" s="202"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4188,63 +4250,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5766,13 +5771,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="205" t="s">
+      <c r="A4" s="215" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="207" t="s">
+      <c r="B4" s="216" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="208"/>
+      <c r="C4" s="217"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5877,9 +5882,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="206"/>
-      <c r="B5" s="204"/>
-      <c r="C5" s="206"/>
+      <c r="A5" s="204"/>
+      <c r="B5" s="214"/>
+      <c r="C5" s="204"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5984,11 +5989,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="206"/>
+      <c r="A6" s="204"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="206"/>
+      <c r="C6" s="204"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6093,11 +6098,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="206"/>
+      <c r="A7" s="204"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="206"/>
+      <c r="C7" s="204"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6202,11 +6207,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="206"/>
+      <c r="A8" s="204"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="206"/>
+      <c r="C8" s="204"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6311,11 +6316,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="206"/>
+      <c r="A9" s="204"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="206"/>
+      <c r="C9" s="204"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6420,11 +6425,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="206"/>
+      <c r="A10" s="204"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="206"/>
+      <c r="C10" s="204"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6529,11 +6534,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="206"/>
+      <c r="A11" s="204"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="206"/>
+      <c r="C11" s="204"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6638,9 +6643,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="206"/>
+      <c r="A12" s="204"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="209"/>
+      <c r="C12" s="205"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6745,10 +6750,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="210" t="s">
+      <c r="A13" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="211" t="s">
+      <c r="B13" s="219" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6857,8 +6862,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="206"/>
-      <c r="B14" s="212"/>
+      <c r="A14" s="204"/>
+      <c r="B14" s="210"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6979,7 +6984,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="206"/>
+      <c r="A15" s="204"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7089,7 +7094,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="206"/>
+      <c r="A16" s="204"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7199,7 +7204,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="206"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7311,7 +7316,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="206"/>
+      <c r="A18" s="204"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7421,7 +7426,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="206"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7531,7 +7536,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="206"/>
+      <c r="A20" s="204"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7641,7 +7646,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="209"/>
+      <c r="A21" s="205"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7752,7 +7757,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="213" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7862,7 +7867,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="204"/>
+      <c r="B23" s="214"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7969,13 +7974,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="214" t="s">
+      <c r="A24" s="206" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="216">
+      <c r="C24" s="208">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8083,11 +8088,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="215"/>
+      <c r="A25" s="207"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="206"/>
+      <c r="C25" s="204"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8193,11 +8198,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="215"/>
+      <c r="A26" s="207"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="206"/>
+      <c r="C26" s="204"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8303,11 +8308,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="215"/>
+      <c r="A27" s="207"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="206"/>
+      <c r="C27" s="204"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8413,11 +8418,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="215"/>
+      <c r="A28" s="207"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="206"/>
+      <c r="C28" s="204"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8523,11 +8528,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="215"/>
+      <c r="A29" s="207"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="206"/>
+      <c r="C29" s="204"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8633,11 +8638,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="215"/>
+      <c r="A30" s="207"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="206"/>
+      <c r="C30" s="204"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8743,11 +8748,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="215"/>
+      <c r="A31" s="207"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="206"/>
+      <c r="C31" s="204"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8853,11 +8858,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="215"/>
+      <c r="A32" s="207"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="206"/>
+      <c r="C32" s="204"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8963,11 +8968,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="215"/>
+      <c r="A33" s="207"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="206"/>
+      <c r="C33" s="204"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9073,11 +9078,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="215"/>
+      <c r="A34" s="207"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="206"/>
+      <c r="C34" s="204"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9183,11 +9188,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="215"/>
+      <c r="A35" s="207"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="209"/>
+      <c r="C35" s="205"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9293,11 +9298,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="215"/>
+      <c r="A36" s="207"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="216">
+      <c r="C36" s="208">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9405,11 +9410,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="215"/>
+      <c r="A37" s="207"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="206"/>
+      <c r="C37" s="204"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9515,11 +9520,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="215"/>
+      <c r="A38" s="207"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="206"/>
+      <c r="C38" s="204"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9625,11 +9630,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="215"/>
+      <c r="A39" s="207"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="206"/>
+      <c r="C39" s="204"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9735,11 +9740,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="215"/>
+      <c r="A40" s="207"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="206"/>
+      <c r="C40" s="204"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9845,11 +9850,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="215"/>
+      <c r="A41" s="207"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="206"/>
+      <c r="C41" s="204"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9955,11 +9960,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="215"/>
+      <c r="A42" s="207"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="206"/>
+      <c r="C42" s="204"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10065,11 +10070,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="215"/>
+      <c r="A43" s="207"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="206"/>
+      <c r="C43" s="204"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10175,11 +10180,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="215"/>
+      <c r="A44" s="207"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="206"/>
+      <c r="C44" s="204"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10285,11 +10290,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="215"/>
+      <c r="A45" s="207"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="206"/>
+      <c r="C45" s="204"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10395,11 +10400,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="215"/>
+      <c r="A46" s="207"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="206"/>
+      <c r="C46" s="204"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10505,11 +10510,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="215"/>
+      <c r="A47" s="207"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="206"/>
+      <c r="C47" s="204"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10623,11 +10628,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="215"/>
+      <c r="A48" s="207"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="206"/>
+      <c r="C48" s="204"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10736,7 +10741,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="217" t="s">
+      <c r="B49" s="209" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10846,7 +10851,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="212"/>
+      <c r="B50" s="210"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14277,7 +14282,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="218" t="s">
+      <c r="A81" s="211" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14389,7 +14394,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="206"/>
+      <c r="A82" s="204"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14499,7 +14504,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="206"/>
+      <c r="A83" s="204"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14609,7 +14614,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="206"/>
+      <c r="A84" s="204"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14719,7 +14724,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="206"/>
+      <c r="A85" s="204"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14829,7 +14834,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="206"/>
+      <c r="A86" s="204"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14939,7 +14944,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="206"/>
+      <c r="A87" s="204"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15051,7 +15056,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="206"/>
+      <c r="A88" s="204"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15161,7 +15166,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="206"/>
+      <c r="A89" s="204"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15271,7 +15276,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="206"/>
+      <c r="A90" s="204"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15381,11 +15386,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="206"/>
+      <c r="A91" s="204"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="219"/>
+      <c r="C91" s="212"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15491,11 +15496,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="206"/>
+      <c r="A92" s="204"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="206"/>
+      <c r="C92" s="204"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15601,11 +15606,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="209"/>
+      <c r="A93" s="205"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="206"/>
+      <c r="C93" s="204"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15829,7 +15834,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="213" t="s">
+      <c r="A95" s="203" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15941,7 +15946,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="206"/>
+      <c r="A96" s="204"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16051,7 +16056,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="206"/>
+      <c r="A97" s="204"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16161,7 +16166,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="206"/>
+      <c r="A98" s="204"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16271,7 +16276,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="206"/>
+      <c r="A99" s="204"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16381,7 +16386,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="206"/>
+      <c r="A100" s="204"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16491,7 +16496,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="206"/>
+      <c r="A101" s="204"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16601,7 +16606,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="206"/>
+      <c r="A102" s="204"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16711,7 +16716,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="206"/>
+      <c r="A103" s="204"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16823,7 +16828,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="206"/>
+      <c r="A104" s="204"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16933,7 +16938,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="206"/>
+      <c r="A105" s="204"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17051,7 +17056,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="206"/>
+      <c r="A106" s="204"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17161,7 +17166,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="206"/>
+      <c r="A107" s="204"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17271,7 +17276,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="206"/>
+      <c r="A108" s="204"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17381,7 +17386,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="206"/>
+      <c r="A109" s="204"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17491,7 +17496,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="206"/>
+      <c r="A110" s="204"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17601,7 +17606,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="206"/>
+      <c r="A111" s="204"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17711,7 +17716,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="206"/>
+      <c r="A112" s="204"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17821,7 +17826,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="206"/>
+      <c r="A113" s="204"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17931,7 +17936,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="206"/>
+      <c r="A114" s="204"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18041,7 +18046,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="206"/>
+      <c r="A115" s="204"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18151,7 +18156,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="206"/>
+      <c r="A116" s="204"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18277,7 +18282,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="206"/>
+      <c r="A117" s="204"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18387,7 +18392,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="209"/>
+      <c r="A118" s="205"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25758,6 +25763,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25765,12 +25776,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 25 e 26-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E928BD8C-0612-48C8-9CB3-C28C3C135447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB7FA35-E48E-4497-9C16-F9002CC7E48A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="175">
   <si>
     <t>S</t>
   </si>
@@ -726,6 +726,13 @@
   </si>
   <si>
     <t>Planejamento dos conteúdos de Front-End II</t>
+  </si>
+  <si>
+    <t>Laço Foreach
+Introdução padrão MVC</t>
+  </si>
+  <si>
+    <t>Aula sobre manipulação de arquivos Word dada pelo monitor</t>
   </si>
 </sst>
 </file>
@@ -2251,17 +2258,56 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2278,59 +2324,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2341,30 +2368,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2871,10 +2878,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AH4" sqref="AH4:AH11"/>
+      <selection pane="bottomRight" activeCell="AK4" sqref="AK4:AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3183,110 +3190,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="195" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="195"/>
+      <c r="V2" s="195"/>
+      <c r="W2" s="195"/>
+      <c r="X2" s="195"/>
+      <c r="Y2" s="195"/>
+      <c r="Z2" s="195"/>
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="195"/>
+      <c r="AE2" s="195"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="195"/>
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="195"/>
+      <c r="AM2" s="195" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="195"/>
+      <c r="AQ2" s="195"/>
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="195"/>
+      <c r="AU2" s="195"/>
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="196"/>
+      <c r="AY2" s="196"/>
+      <c r="AZ2" s="196"/>
+      <c r="BA2" s="196"/>
+      <c r="BB2" s="196"/>
+      <c r="BC2" s="196"/>
+      <c r="BD2" s="196"/>
+      <c r="BE2" s="196"/>
+      <c r="BF2" s="196"/>
+      <c r="BG2" s="196"/>
+      <c r="BH2" s="196"/>
+      <c r="BI2" s="196"/>
+      <c r="BJ2" s="195" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="195"/>
+      <c r="BL2" s="195"/>
+      <c r="BM2" s="195"/>
+      <c r="BN2" s="195"/>
+      <c r="BO2" s="195"/>
+      <c r="BP2" s="195"/>
+      <c r="BQ2" s="195"/>
+      <c r="BR2" s="195"/>
+      <c r="BS2" s="195"/>
+      <c r="BT2" s="195"/>
+      <c r="BU2" s="195"/>
+      <c r="BV2" s="195"/>
+      <c r="BW2" s="195"/>
+      <c r="BX2" s="197"/>
+      <c r="BY2" s="197"/>
+      <c r="BZ2" s="197"/>
+      <c r="CA2" s="197"/>
+      <c r="CB2" s="197"/>
+      <c r="CC2" s="197"/>
+      <c r="CD2" s="197"/>
+      <c r="CE2" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="199"/>
+      <c r="CG2" s="199"/>
+      <c r="CH2" s="199"/>
+      <c r="CI2" s="199"/>
+      <c r="CJ2" s="199"/>
+      <c r="CK2" s="199"/>
+      <c r="CL2" s="199"/>
+      <c r="CM2" s="199"/>
+      <c r="CN2" s="199"/>
+      <c r="CO2" s="199"/>
+      <c r="CP2" s="199"/>
+      <c r="CQ2" s="199"/>
+      <c r="CR2" s="199"/>
+      <c r="CS2" s="199"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3582,83 +3589,83 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="201" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="202"/>
+      <c r="D4" s="200" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="200" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="200" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="200" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="200" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="200" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="200" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="200" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="193" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="193" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="193" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="193" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="193" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="193" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="193" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="193" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="193" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="193" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="193" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="192" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188" t="s">
+      <c r="X4" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="188" t="s">
+      <c r="Y4" s="192" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="188" t="s">
+      <c r="Z4" s="192" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="188" t="s">
+      <c r="AA4" s="192" t="s">
         <v>165</v>
       </c>
       <c r="AB4" s="189" t="s">
@@ -3679,545 +3686,524 @@
       <c r="AG4" s="189" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="192" t="s">
+      <c r="AH4" s="186" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="192"/>
-      <c r="AJ4" s="192"/>
-      <c r="AK4" s="192"/>
-      <c r="AL4" s="192"/>
-      <c r="AM4" s="192"/>
-      <c r="AN4" s="192"/>
-      <c r="AO4" s="192"/>
-      <c r="AP4" s="192"/>
-      <c r="AQ4" s="192"/>
-      <c r="AR4" s="195"/>
-      <c r="AS4" s="195"/>
-      <c r="AT4" s="195"/>
+      <c r="AI4" s="186" t="s">
+        <v>174</v>
+      </c>
+      <c r="AJ4" s="186" t="s">
+        <v>173</v>
+      </c>
+      <c r="AK4" s="186"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="175"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="198"/>
-      <c r="AY4" s="200"/>
-      <c r="AZ4" s="200"/>
-      <c r="BA4" s="200"/>
-      <c r="BB4" s="200"/>
-      <c r="BC4" s="200"/>
-      <c r="BD4" s="200"/>
-      <c r="BE4" s="200"/>
-      <c r="BF4" s="201"/>
-      <c r="BG4" s="201"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="194"/>
+      <c r="AW4" s="194"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="194"/>
+      <c r="BW4" s="194"/>
+      <c r="CT4" s="194"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="201"/>
+      <c r="B5" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
+      <c r="C5" s="202"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="193"/>
+      <c r="M5" s="193"/>
+      <c r="N5" s="193"/>
+      <c r="O5" s="193"/>
+      <c r="P5" s="193"/>
+      <c r="Q5" s="193"/>
+      <c r="R5" s="193"/>
+      <c r="S5" s="193"/>
+      <c r="T5" s="193"/>
+      <c r="U5" s="193"/>
+      <c r="V5" s="193"/>
+      <c r="W5" s="192"/>
+      <c r="X5" s="192"/>
+      <c r="Y5" s="192"/>
+      <c r="Z5" s="192"/>
+      <c r="AA5" s="192"/>
       <c r="AB5" s="190"/>
       <c r="AC5" s="190"/>
       <c r="AD5" s="190"/>
       <c r="AE5" s="190"/>
       <c r="AF5" s="190"/>
       <c r="AG5" s="190"/>
-      <c r="AH5" s="193"/>
-      <c r="AI5" s="193"/>
-      <c r="AJ5" s="193"/>
-      <c r="AK5" s="193"/>
-      <c r="AL5" s="193"/>
-      <c r="AM5" s="193"/>
-      <c r="AN5" s="193"/>
-      <c r="AO5" s="193"/>
-      <c r="AP5" s="193"/>
-      <c r="AQ5" s="193"/>
-      <c r="AR5" s="196"/>
-      <c r="AS5" s="196"/>
-      <c r="AT5" s="196"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="175"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="199"/>
-      <c r="AY5" s="200"/>
-      <c r="AZ5" s="200"/>
-      <c r="BA5" s="200"/>
-      <c r="BB5" s="200"/>
-      <c r="BC5" s="200"/>
-      <c r="BD5" s="200"/>
-      <c r="BE5" s="200"/>
-      <c r="BF5" s="202"/>
-      <c r="BG5" s="202"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="194"/>
+      <c r="AW5" s="194"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="194"/>
+      <c r="BW5" s="194"/>
+      <c r="CT5" s="194"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="201"/>
+      <c r="B6" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
+      <c r="C6" s="202"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="H6" s="200"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="200"/>
+      <c r="K6" s="200"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
+      <c r="P6" s="193"/>
+      <c r="Q6" s="193"/>
+      <c r="R6" s="193"/>
+      <c r="S6" s="193"/>
+      <c r="T6" s="193"/>
+      <c r="U6" s="193"/>
+      <c r="V6" s="193"/>
+      <c r="W6" s="192"/>
+      <c r="X6" s="192"/>
+      <c r="Y6" s="192"/>
+      <c r="Z6" s="192"/>
+      <c r="AA6" s="192"/>
       <c r="AB6" s="190"/>
       <c r="AC6" s="190"/>
       <c r="AD6" s="190"/>
       <c r="AE6" s="190"/>
       <c r="AF6" s="190"/>
       <c r="AG6" s="190"/>
-      <c r="AH6" s="193"/>
-      <c r="AI6" s="193"/>
-      <c r="AJ6" s="193"/>
-      <c r="AK6" s="193"/>
-      <c r="AL6" s="193"/>
-      <c r="AM6" s="193"/>
-      <c r="AN6" s="193"/>
-      <c r="AO6" s="193"/>
-      <c r="AP6" s="193"/>
-      <c r="AQ6" s="193"/>
-      <c r="AR6" s="196"/>
-      <c r="AS6" s="196"/>
-      <c r="AT6" s="196"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="175"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="199"/>
-      <c r="AY6" s="200"/>
-      <c r="AZ6" s="200"/>
-      <c r="BA6" s="200"/>
-      <c r="BB6" s="200"/>
-      <c r="BC6" s="200"/>
-      <c r="BD6" s="200"/>
-      <c r="BE6" s="200"/>
-      <c r="BF6" s="202"/>
-      <c r="BG6" s="202"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="194"/>
+      <c r="AW6" s="194"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="194"/>
+      <c r="BW6" s="194"/>
+      <c r="CT6" s="194"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="201"/>
+      <c r="B7" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
+      <c r="C7" s="202"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="200"/>
+      <c r="G7" s="200"/>
+      <c r="H7" s="200"/>
+      <c r="I7" s="200"/>
+      <c r="J7" s="200"/>
+      <c r="K7" s="200"/>
+      <c r="L7" s="193"/>
+      <c r="M7" s="193"/>
+      <c r="N7" s="193"/>
+      <c r="O7" s="193"/>
+      <c r="P7" s="193"/>
+      <c r="Q7" s="193"/>
+      <c r="R7" s="193"/>
+      <c r="S7" s="193"/>
+      <c r="T7" s="193"/>
+      <c r="U7" s="193"/>
+      <c r="V7" s="193"/>
+      <c r="W7" s="192"/>
+      <c r="X7" s="192"/>
+      <c r="Y7" s="192"/>
+      <c r="Z7" s="192"/>
+      <c r="AA7" s="192"/>
       <c r="AB7" s="190"/>
       <c r="AC7" s="190"/>
       <c r="AD7" s="190"/>
       <c r="AE7" s="190"/>
       <c r="AF7" s="190"/>
       <c r="AG7" s="190"/>
-      <c r="AH7" s="193"/>
-      <c r="AI7" s="193"/>
-      <c r="AJ7" s="193"/>
-      <c r="AK7" s="193"/>
-      <c r="AL7" s="193"/>
-      <c r="AM7" s="193"/>
-      <c r="AN7" s="193"/>
-      <c r="AO7" s="193"/>
-      <c r="AP7" s="193"/>
-      <c r="AQ7" s="193"/>
-      <c r="AR7" s="196"/>
-      <c r="AS7" s="196"/>
-      <c r="AT7" s="196"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="176"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="199"/>
-      <c r="AY7" s="200"/>
-      <c r="AZ7" s="200"/>
-      <c r="BA7" s="200"/>
-      <c r="BB7" s="200"/>
-      <c r="BC7" s="200"/>
-      <c r="BD7" s="200"/>
-      <c r="BE7" s="200"/>
-      <c r="BF7" s="202"/>
-      <c r="BG7" s="202"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="194"/>
+      <c r="AW7" s="194"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="194"/>
+      <c r="BW7" s="194"/>
+      <c r="CT7" s="194"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="201" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
+      <c r="C8" s="202"/>
+      <c r="D8" s="200"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="200"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="200"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="193"/>
+      <c r="N8" s="193"/>
+      <c r="O8" s="193"/>
+      <c r="P8" s="193"/>
+      <c r="Q8" s="193"/>
+      <c r="R8" s="193"/>
+      <c r="S8" s="193"/>
+      <c r="T8" s="193"/>
+      <c r="U8" s="193"/>
+      <c r="V8" s="193"/>
+      <c r="W8" s="192"/>
+      <c r="X8" s="192"/>
+      <c r="Y8" s="192"/>
+      <c r="Z8" s="192"/>
+      <c r="AA8" s="192"/>
       <c r="AB8" s="190"/>
       <c r="AC8" s="190"/>
       <c r="AD8" s="190"/>
       <c r="AE8" s="190"/>
       <c r="AF8" s="190"/>
       <c r="AG8" s="190"/>
-      <c r="AH8" s="193"/>
-      <c r="AI8" s="193"/>
-      <c r="AJ8" s="193"/>
-      <c r="AK8" s="193"/>
-      <c r="AL8" s="193"/>
-      <c r="AM8" s="193"/>
-      <c r="AN8" s="193"/>
-      <c r="AO8" s="193"/>
-      <c r="AP8" s="193"/>
-      <c r="AQ8" s="193"/>
-      <c r="AR8" s="196"/>
-      <c r="AS8" s="196"/>
-      <c r="AT8" s="196"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="176"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="199"/>
-      <c r="AY8" s="200"/>
-      <c r="AZ8" s="200"/>
-      <c r="BA8" s="200"/>
-      <c r="BB8" s="200"/>
-      <c r="BC8" s="200"/>
-      <c r="BD8" s="200"/>
-      <c r="BE8" s="200"/>
-      <c r="BF8" s="202"/>
-      <c r="BG8" s="202"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="194"/>
+      <c r="AW8" s="194"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="194"/>
+      <c r="BW8" s="194"/>
+      <c r="CT8" s="194"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="201"/>
+      <c r="B9" s="202" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="200"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="193"/>
+      <c r="N9" s="193"/>
+      <c r="O9" s="193"/>
+      <c r="P9" s="193"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="193"/>
+      <c r="S9" s="193"/>
+      <c r="T9" s="193"/>
+      <c r="U9" s="193"/>
+      <c r="V9" s="193"/>
+      <c r="W9" s="192"/>
+      <c r="X9" s="192"/>
+      <c r="Y9" s="192"/>
+      <c r="Z9" s="192"/>
+      <c r="AA9" s="192"/>
       <c r="AB9" s="190"/>
       <c r="AC9" s="190"/>
       <c r="AD9" s="190"/>
       <c r="AE9" s="190"/>
       <c r="AF9" s="190"/>
       <c r="AG9" s="190"/>
-      <c r="AH9" s="193"/>
-      <c r="AI9" s="193"/>
-      <c r="AJ9" s="193"/>
-      <c r="AK9" s="193"/>
-      <c r="AL9" s="193"/>
-      <c r="AM9" s="193"/>
-      <c r="AN9" s="193"/>
-      <c r="AO9" s="193"/>
-      <c r="AP9" s="193"/>
-      <c r="AQ9" s="193"/>
-      <c r="AR9" s="196"/>
-      <c r="AS9" s="196"/>
-      <c r="AT9" s="196"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="176"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="199"/>
-      <c r="AY9" s="200"/>
-      <c r="AZ9" s="200"/>
-      <c r="BA9" s="200"/>
-      <c r="BB9" s="200"/>
-      <c r="BC9" s="200"/>
-      <c r="BD9" s="200"/>
-      <c r="BE9" s="200"/>
-      <c r="BF9" s="202"/>
-      <c r="BG9" s="202"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="194"/>
+      <c r="AW9" s="194"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="194"/>
+      <c r="BW9" s="194"/>
+      <c r="CT9" s="194"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="201"/>
+      <c r="B10" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
+      <c r="C10" s="202"/>
+      <c r="D10" s="200"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="200"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="200"/>
+      <c r="K10" s="200"/>
+      <c r="L10" s="193"/>
+      <c r="M10" s="193"/>
+      <c r="N10" s="193"/>
+      <c r="O10" s="193"/>
+      <c r="P10" s="193"/>
+      <c r="Q10" s="193"/>
+      <c r="R10" s="193"/>
+      <c r="S10" s="193"/>
+      <c r="T10" s="193"/>
+      <c r="U10" s="193"/>
+      <c r="V10" s="193"/>
+      <c r="W10" s="192"/>
+      <c r="X10" s="192"/>
+      <c r="Y10" s="192"/>
+      <c r="Z10" s="192"/>
+      <c r="AA10" s="192"/>
       <c r="AB10" s="190"/>
       <c r="AC10" s="190"/>
       <c r="AD10" s="190"/>
       <c r="AE10" s="190"/>
       <c r="AF10" s="190"/>
       <c r="AG10" s="190"/>
-      <c r="AH10" s="193"/>
-      <c r="AI10" s="193"/>
-      <c r="AJ10" s="193"/>
-      <c r="AK10" s="193"/>
-      <c r="AL10" s="193"/>
-      <c r="AM10" s="193"/>
-      <c r="AN10" s="193"/>
-      <c r="AO10" s="193"/>
-      <c r="AP10" s="193"/>
-      <c r="AQ10" s="193"/>
-      <c r="AR10" s="196"/>
-      <c r="AS10" s="196"/>
-      <c r="AT10" s="196"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="176"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="199"/>
-      <c r="AY10" s="200"/>
-      <c r="AZ10" s="200"/>
-      <c r="BA10" s="200"/>
-      <c r="BB10" s="200"/>
-      <c r="BC10" s="200"/>
-      <c r="BD10" s="200"/>
-      <c r="BE10" s="200"/>
-      <c r="BF10" s="202"/>
-      <c r="BG10" s="202"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="194"/>
+      <c r="AW10" s="194"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="194"/>
+      <c r="BW10" s="194"/>
+      <c r="CT10" s="194"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="201"/>
+      <c r="B11" s="202" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="200"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="193"/>
+      <c r="M11" s="193"/>
+      <c r="N11" s="193"/>
+      <c r="O11" s="193"/>
+      <c r="P11" s="193"/>
+      <c r="Q11" s="193"/>
+      <c r="R11" s="193"/>
+      <c r="S11" s="193"/>
+      <c r="T11" s="193"/>
+      <c r="U11" s="193"/>
+      <c r="V11" s="193"/>
+      <c r="W11" s="192"/>
+      <c r="X11" s="192"/>
+      <c r="Y11" s="192"/>
+      <c r="Z11" s="192"/>
+      <c r="AA11" s="192"/>
       <c r="AB11" s="191"/>
       <c r="AC11" s="191"/>
       <c r="AD11" s="191"/>
       <c r="AE11" s="191"/>
       <c r="AF11" s="191"/>
       <c r="AG11" s="191"/>
-      <c r="AH11" s="194"/>
-      <c r="AI11" s="194"/>
-      <c r="AJ11" s="194"/>
-      <c r="AK11" s="194"/>
-      <c r="AL11" s="194"/>
-      <c r="AM11" s="194"/>
-      <c r="AN11" s="194"/>
-      <c r="AO11" s="194"/>
-      <c r="AP11" s="194"/>
-      <c r="AQ11" s="194"/>
-      <c r="AR11" s="197"/>
-      <c r="AS11" s="197"/>
-      <c r="AT11" s="197"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="176"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="199"/>
-      <c r="AY11" s="200"/>
-      <c r="AZ11" s="200"/>
-      <c r="BA11" s="200"/>
-      <c r="BB11" s="200"/>
-      <c r="BC11" s="200"/>
-      <c r="BD11" s="200"/>
-      <c r="BE11" s="200"/>
-      <c r="BF11" s="202"/>
-      <c r="BG11" s="202"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="194"/>
+      <c r="AW11" s="194"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="194"/>
+      <c r="BW11" s="194"/>
+      <c r="CT11" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4234,22 +4220,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5771,13 +5782,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="215" t="s">
+      <c r="A4" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="216" t="s">
+      <c r="B4" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="217"/>
+      <c r="C4" s="208"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5882,9 +5893,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="204"/>
-      <c r="B5" s="214"/>
-      <c r="C5" s="204"/>
+      <c r="A5" s="206"/>
+      <c r="B5" s="204"/>
+      <c r="C5" s="206"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -5989,11 +6000,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="204"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="204"/>
+      <c r="C6" s="206"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6098,11 +6109,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="204"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="204"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6207,11 +6218,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="204"/>
+      <c r="A8" s="206"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="204"/>
+      <c r="C8" s="206"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6316,11 +6327,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="204"/>
+      <c r="A9" s="206"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="204"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6425,11 +6436,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="204"/>
+      <c r="A10" s="206"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="204"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6534,11 +6545,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="204"/>
+      <c r="A11" s="206"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="204"/>
+      <c r="C11" s="206"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6643,9 +6654,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="204"/>
+      <c r="A12" s="206"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="205"/>
+      <c r="C12" s="209"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6750,10 +6761,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="218" t="s">
+      <c r="A13" s="210" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="219" t="s">
+      <c r="B13" s="211" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6862,8 +6873,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="204"/>
-      <c r="B14" s="210"/>
+      <c r="A14" s="206"/>
+      <c r="B14" s="212"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6984,7 +6995,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="204"/>
+      <c r="A15" s="206"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7094,7 +7105,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="204"/>
+      <c r="A16" s="206"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7204,7 +7215,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="204"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7316,7 +7327,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="204"/>
+      <c r="A18" s="206"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7426,7 +7437,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="204"/>
+      <c r="A19" s="206"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7536,7 +7547,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="204"/>
+      <c r="A20" s="206"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7646,7 +7657,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="205"/>
+      <c r="A21" s="209"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7757,7 +7768,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="203" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7867,7 +7878,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="214"/>
+      <c r="B23" s="204"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7974,13 +7985,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="206" t="s">
+      <c r="A24" s="214" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="208">
+      <c r="C24" s="216">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8088,11 +8099,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="207"/>
+      <c r="A25" s="215"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="204"/>
+      <c r="C25" s="206"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8198,11 +8209,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="207"/>
+      <c r="A26" s="215"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="204"/>
+      <c r="C26" s="206"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8308,11 +8319,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="207"/>
+      <c r="A27" s="215"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="204"/>
+      <c r="C27" s="206"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8418,11 +8429,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="207"/>
+      <c r="A28" s="215"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="204"/>
+      <c r="C28" s="206"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8528,11 +8539,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="207"/>
+      <c r="A29" s="215"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="204"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8638,11 +8649,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="207"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="204"/>
+      <c r="C30" s="206"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8748,11 +8759,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="207"/>
+      <c r="A31" s="215"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="204"/>
+      <c r="C31" s="206"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8858,11 +8869,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="207"/>
+      <c r="A32" s="215"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="204"/>
+      <c r="C32" s="206"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8968,11 +8979,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="207"/>
+      <c r="A33" s="215"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="204"/>
+      <c r="C33" s="206"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9078,11 +9089,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="207"/>
+      <c r="A34" s="215"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="204"/>
+      <c r="C34" s="206"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9188,11 +9199,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="207"/>
+      <c r="A35" s="215"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="205"/>
+      <c r="C35" s="209"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9298,11 +9309,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="207"/>
+      <c r="A36" s="215"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="208">
+      <c r="C36" s="216">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9410,11 +9421,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="207"/>
+      <c r="A37" s="215"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="204"/>
+      <c r="C37" s="206"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9520,11 +9531,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="207"/>
+      <c r="A38" s="215"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="204"/>
+      <c r="C38" s="206"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9630,11 +9641,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="207"/>
+      <c r="A39" s="215"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="204"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9740,11 +9751,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="207"/>
+      <c r="A40" s="215"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="204"/>
+      <c r="C40" s="206"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9850,11 +9861,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="207"/>
+      <c r="A41" s="215"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="204"/>
+      <c r="C41" s="206"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9960,11 +9971,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="207"/>
+      <c r="A42" s="215"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="204"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10070,11 +10081,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="207"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="204"/>
+      <c r="C43" s="206"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10180,11 +10191,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="207"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="204"/>
+      <c r="C44" s="206"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10290,11 +10301,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="207"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="204"/>
+      <c r="C45" s="206"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10400,11 +10411,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="207"/>
+      <c r="A46" s="215"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="204"/>
+      <c r="C46" s="206"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10510,11 +10521,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="207"/>
+      <c r="A47" s="215"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="204"/>
+      <c r="C47" s="206"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10628,11 +10639,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="207"/>
+      <c r="A48" s="215"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="204"/>
+      <c r="C48" s="206"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10741,7 +10752,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="209" t="s">
+      <c r="B49" s="217" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10851,7 +10862,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="210"/>
+      <c r="B50" s="212"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14282,7 +14293,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="211" t="s">
+      <c r="A81" s="218" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14394,7 +14405,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="204"/>
+      <c r="A82" s="206"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14504,7 +14515,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="204"/>
+      <c r="A83" s="206"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14614,7 +14625,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="204"/>
+      <c r="A84" s="206"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14724,7 +14735,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="204"/>
+      <c r="A85" s="206"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14834,7 +14845,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="204"/>
+      <c r="A86" s="206"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14944,7 +14955,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="204"/>
+      <c r="A87" s="206"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15056,7 +15067,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="204"/>
+      <c r="A88" s="206"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15166,7 +15177,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="204"/>
+      <c r="A89" s="206"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15276,7 +15287,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="204"/>
+      <c r="A90" s="206"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15386,11 +15397,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="204"/>
+      <c r="A91" s="206"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="212"/>
+      <c r="C91" s="219"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15496,11 +15507,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="204"/>
+      <c r="A92" s="206"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="204"/>
+      <c r="C92" s="206"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15606,11 +15617,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="205"/>
+      <c r="A93" s="209"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="204"/>
+      <c r="C93" s="206"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15834,7 +15845,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="203" t="s">
+      <c r="A95" s="213" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15946,7 +15957,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="204"/>
+      <c r="A96" s="206"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16056,7 +16067,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="204"/>
+      <c r="A97" s="206"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16166,7 +16177,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="204"/>
+      <c r="A98" s="206"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16276,7 +16287,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="204"/>
+      <c r="A99" s="206"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16386,7 +16397,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="204"/>
+      <c r="A100" s="206"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16496,7 +16507,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="204"/>
+      <c r="A101" s="206"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16606,7 +16617,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="204"/>
+      <c r="A102" s="206"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16716,7 +16727,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="204"/>
+      <c r="A103" s="206"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16828,7 +16839,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="204"/>
+      <c r="A104" s="206"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16938,7 +16949,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="204"/>
+      <c r="A105" s="206"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17056,7 +17067,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="204"/>
+      <c r="A106" s="206"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17166,7 +17177,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="204"/>
+      <c r="A107" s="206"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17276,7 +17287,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="204"/>
+      <c r="A108" s="206"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17386,7 +17397,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="204"/>
+      <c r="A109" s="206"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17496,7 +17507,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="204"/>
+      <c r="A110" s="206"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17606,7 +17617,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="204"/>
+      <c r="A111" s="206"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17716,7 +17727,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="204"/>
+      <c r="A112" s="206"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17826,7 +17837,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="204"/>
+      <c r="A113" s="206"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17936,7 +17947,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="204"/>
+      <c r="A114" s="206"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18046,7 +18057,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="204"/>
+      <c r="A115" s="206"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18156,7 +18167,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="204"/>
+      <c r="A116" s="206"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18282,7 +18293,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="204"/>
+      <c r="A117" s="206"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18392,7 +18403,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="205"/>
+      <c r="A118" s="209"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25763,12 +25774,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25776,6 +25781,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 27 e 30-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB7FA35-E48E-4497-9C16-F9002CC7E48A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -27,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="177">
   <si>
     <t>S</t>
   </si>
@@ -734,12 +733,18 @@
   <si>
     <t>Aula sobre manipulação de arquivos Word dada pelo monitor</t>
   </si>
+  <si>
+    <t>Exercícios função</t>
+  </si>
+  <si>
+    <t>Não houve acompanhamento pois foi realizada apresentação dos projetos da turma do técnico para a coordenação</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -876,6 +881,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1911,7 +1922,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2251,63 +2262,17 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2324,40 +2289,26 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2368,16 +2319,67 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2874,14 +2876,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AK4" sqref="AK4:AK11"/>
+      <selection pane="bottomRight" activeCell="AM4" sqref="AM4:AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3190,110 +3192,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="195" t="s">
+      <c r="D2" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="195"/>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="195" t="s">
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="179"/>
+      <c r="K2" s="179"/>
+      <c r="L2" s="179"/>
+      <c r="M2" s="179"/>
+      <c r="N2" s="179"/>
+      <c r="O2" s="179"/>
+      <c r="P2" s="179"/>
+      <c r="Q2" s="179"/>
+      <c r="R2" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="195"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="195"/>
-      <c r="V2" s="195"/>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195"/>
-      <c r="Z2" s="195"/>
-      <c r="AA2" s="195"/>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="195"/>
-      <c r="AD2" s="195"/>
-      <c r="AE2" s="195"/>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="195"/>
-      <c r="AH2" s="195"/>
-      <c r="AI2" s="195"/>
-      <c r="AJ2" s="195"/>
-      <c r="AK2" s="195"/>
-      <c r="AL2" s="195"/>
-      <c r="AM2" s="195" t="s">
+      <c r="S2" s="179"/>
+      <c r="T2" s="179"/>
+      <c r="U2" s="179"/>
+      <c r="V2" s="179"/>
+      <c r="W2" s="179"/>
+      <c r="X2" s="179"/>
+      <c r="Y2" s="179"/>
+      <c r="Z2" s="179"/>
+      <c r="AA2" s="179"/>
+      <c r="AB2" s="179"/>
+      <c r="AC2" s="179"/>
+      <c r="AD2" s="179"/>
+      <c r="AE2" s="179"/>
+      <c r="AF2" s="179"/>
+      <c r="AG2" s="179"/>
+      <c r="AH2" s="179"/>
+      <c r="AI2" s="179"/>
+      <c r="AJ2" s="179"/>
+      <c r="AK2" s="179"/>
+      <c r="AL2" s="179"/>
+      <c r="AM2" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="195"/>
-      <c r="AO2" s="195"/>
-      <c r="AP2" s="195"/>
-      <c r="AQ2" s="195"/>
-      <c r="AR2" s="195"/>
-      <c r="AS2" s="195"/>
-      <c r="AT2" s="195"/>
-      <c r="AU2" s="195"/>
-      <c r="AV2" s="195"/>
-      <c r="AW2" s="195"/>
-      <c r="AX2" s="196"/>
-      <c r="AY2" s="196"/>
-      <c r="AZ2" s="196"/>
-      <c r="BA2" s="196"/>
-      <c r="BB2" s="196"/>
-      <c r="BC2" s="196"/>
-      <c r="BD2" s="196"/>
-      <c r="BE2" s="196"/>
-      <c r="BF2" s="196"/>
-      <c r="BG2" s="196"/>
-      <c r="BH2" s="196"/>
-      <c r="BI2" s="196"/>
-      <c r="BJ2" s="195" t="s">
+      <c r="AN2" s="179"/>
+      <c r="AO2" s="179"/>
+      <c r="AP2" s="179"/>
+      <c r="AQ2" s="179"/>
+      <c r="AR2" s="179"/>
+      <c r="AS2" s="179"/>
+      <c r="AT2" s="179"/>
+      <c r="AU2" s="179"/>
+      <c r="AV2" s="179"/>
+      <c r="AW2" s="179"/>
+      <c r="AX2" s="180"/>
+      <c r="AY2" s="180"/>
+      <c r="AZ2" s="180"/>
+      <c r="BA2" s="180"/>
+      <c r="BB2" s="180"/>
+      <c r="BC2" s="180"/>
+      <c r="BD2" s="180"/>
+      <c r="BE2" s="180"/>
+      <c r="BF2" s="180"/>
+      <c r="BG2" s="180"/>
+      <c r="BH2" s="180"/>
+      <c r="BI2" s="180"/>
+      <c r="BJ2" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="195"/>
-      <c r="BL2" s="195"/>
-      <c r="BM2" s="195"/>
-      <c r="BN2" s="195"/>
-      <c r="BO2" s="195"/>
-      <c r="BP2" s="195"/>
-      <c r="BQ2" s="195"/>
-      <c r="BR2" s="195"/>
-      <c r="BS2" s="195"/>
-      <c r="BT2" s="195"/>
-      <c r="BU2" s="195"/>
-      <c r="BV2" s="195"/>
-      <c r="BW2" s="195"/>
-      <c r="BX2" s="197"/>
-      <c r="BY2" s="197"/>
-      <c r="BZ2" s="197"/>
-      <c r="CA2" s="197"/>
-      <c r="CB2" s="197"/>
-      <c r="CC2" s="197"/>
-      <c r="CD2" s="197"/>
-      <c r="CE2" s="198" t="s">
+      <c r="BK2" s="179"/>
+      <c r="BL2" s="179"/>
+      <c r="BM2" s="179"/>
+      <c r="BN2" s="179"/>
+      <c r="BO2" s="179"/>
+      <c r="BP2" s="179"/>
+      <c r="BQ2" s="179"/>
+      <c r="BR2" s="179"/>
+      <c r="BS2" s="179"/>
+      <c r="BT2" s="179"/>
+      <c r="BU2" s="179"/>
+      <c r="BV2" s="179"/>
+      <c r="BW2" s="179"/>
+      <c r="BX2" s="181"/>
+      <c r="BY2" s="181"/>
+      <c r="BZ2" s="181"/>
+      <c r="CA2" s="181"/>
+      <c r="CB2" s="181"/>
+      <c r="CC2" s="181"/>
+      <c r="CD2" s="181"/>
+      <c r="CE2" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="199"/>
-      <c r="CG2" s="199"/>
-      <c r="CH2" s="199"/>
-      <c r="CI2" s="199"/>
-      <c r="CJ2" s="199"/>
-      <c r="CK2" s="199"/>
-      <c r="CL2" s="199"/>
-      <c r="CM2" s="199"/>
-      <c r="CN2" s="199"/>
-      <c r="CO2" s="199"/>
-      <c r="CP2" s="199"/>
-      <c r="CQ2" s="199"/>
-      <c r="CR2" s="199"/>
-      <c r="CS2" s="199"/>
+      <c r="CF2" s="183"/>
+      <c r="CG2" s="183"/>
+      <c r="CH2" s="183"/>
+      <c r="CI2" s="183"/>
+      <c r="CJ2" s="183"/>
+      <c r="CK2" s="183"/>
+      <c r="CL2" s="183"/>
+      <c r="CM2" s="183"/>
+      <c r="CN2" s="183"/>
+      <c r="CO2" s="183"/>
+      <c r="CP2" s="183"/>
+      <c r="CQ2" s="183"/>
+      <c r="CR2" s="183"/>
+      <c r="CS2" s="183"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3416,10 +3418,10 @@
       <c r="AO3" s="168">
         <v>3</v>
       </c>
-      <c r="AP3" s="177">
+      <c r="AP3" s="175">
         <v>4</v>
       </c>
-      <c r="AQ3" s="177">
+      <c r="AQ3" s="175">
         <v>7</v>
       </c>
       <c r="AR3" s="168">
@@ -3431,7 +3433,7 @@
       <c r="AT3" s="168">
         <v>10</v>
       </c>
-      <c r="AU3" s="177">
+      <c r="AU3" s="175">
         <v>11</v>
       </c>
       <c r="AV3" s="6">
@@ -3588,606 +3590,667 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+    <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="176" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="202" t="s">
+      <c r="B4" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="202"/>
-      <c r="D4" s="200" t="s">
+      <c r="C4" s="178"/>
+      <c r="D4" s="206" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="200" t="s">
+      <c r="E4" s="206" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="200" t="s">
+      <c r="F4" s="206" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="200" t="s">
+      <c r="G4" s="206" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="200" t="s">
+      <c r="H4" s="206" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="200" t="s">
+      <c r="I4" s="206" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="200" t="s">
+      <c r="J4" s="206" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="200" t="s">
+      <c r="K4" s="206" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="193" t="s">
+      <c r="L4" s="207" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="193" t="s">
+      <c r="M4" s="207" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="193" t="s">
+      <c r="N4" s="207" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="193" t="s">
+      <c r="O4" s="207" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="193" t="s">
+      <c r="P4" s="207" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="193" t="s">
+      <c r="Q4" s="207" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="193" t="s">
+      <c r="R4" s="207" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="193" t="s">
+      <c r="S4" s="207" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="193" t="s">
+      <c r="T4" s="207" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="193" t="s">
+      <c r="U4" s="207" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="193" t="s">
+      <c r="V4" s="207" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="192" t="s">
+      <c r="W4" s="208" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="192" t="s">
+      <c r="X4" s="208" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="192" t="s">
+      <c r="Y4" s="208" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="192" t="s">
+      <c r="Z4" s="208" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="192" t="s">
+      <c r="AA4" s="208" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="189" t="s">
+      <c r="AB4" s="209" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="189" t="s">
+      <c r="AC4" s="209" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="189" t="s">
+      <c r="AD4" s="209" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="189" t="s">
+      <c r="AE4" s="209" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="189" t="s">
+      <c r="AF4" s="209" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="189" t="s">
+      <c r="AG4" s="209" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="186" t="s">
+      <c r="AH4" s="209" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="186" t="s">
+      <c r="AI4" s="209" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="186" t="s">
+      <c r="AJ4" s="209" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="186"/>
-      <c r="AL4" s="186"/>
-      <c r="AM4" s="186"/>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
-      <c r="AU4" s="175"/>
-      <c r="AV4" s="194"/>
-      <c r="AW4" s="194"/>
+      <c r="AK4" s="209" t="s">
+        <v>175</v>
+      </c>
+      <c r="AL4" s="209" t="s">
+        <v>176</v>
+      </c>
+      <c r="AM4" s="209"/>
+      <c r="AN4" s="209"/>
+      <c r="AO4" s="209"/>
+      <c r="AP4" s="209"/>
+      <c r="AQ4" s="209"/>
+      <c r="AR4" s="210"/>
+      <c r="AS4" s="210"/>
+      <c r="AT4" s="210"/>
+      <c r="AU4" s="211"/>
+      <c r="AV4" s="177"/>
+      <c r="AW4" s="177"/>
       <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="194"/>
-      <c r="BW4" s="194"/>
-      <c r="CT4" s="194"/>
-    </row>
-    <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="201"/>
-      <c r="B5" s="202" t="s">
+      <c r="AY4" s="186"/>
+      <c r="AZ4" s="186"/>
+      <c r="BA4" s="186"/>
+      <c r="BB4" s="186"/>
+      <c r="BC4" s="186"/>
+      <c r="BD4" s="186"/>
+      <c r="BE4" s="186"/>
+      <c r="BF4" s="187"/>
+      <c r="BG4" s="187"/>
+      <c r="BT4" s="177"/>
+      <c r="BW4" s="177"/>
+      <c r="CT4" s="177"/>
+    </row>
+    <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="176"/>
+      <c r="B5" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="202"/>
-      <c r="D5" s="200"/>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200"/>
-      <c r="I5" s="200"/>
-      <c r="J5" s="200"/>
-      <c r="K5" s="200"/>
-      <c r="L5" s="193"/>
-      <c r="M5" s="193"/>
-      <c r="N5" s="193"/>
-      <c r="O5" s="193"/>
-      <c r="P5" s="193"/>
-      <c r="Q5" s="193"/>
-      <c r="R5" s="193"/>
-      <c r="S5" s="193"/>
-      <c r="T5" s="193"/>
-      <c r="U5" s="193"/>
-      <c r="V5" s="193"/>
-      <c r="W5" s="192"/>
-      <c r="X5" s="192"/>
-      <c r="Y5" s="192"/>
-      <c r="Z5" s="192"/>
-      <c r="AA5" s="192"/>
-      <c r="AB5" s="190"/>
-      <c r="AC5" s="190"/>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
-      <c r="AU5" s="175"/>
-      <c r="AV5" s="194"/>
-      <c r="AW5" s="194"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="206"/>
+      <c r="F5" s="206"/>
+      <c r="G5" s="206"/>
+      <c r="H5" s="206"/>
+      <c r="I5" s="206"/>
+      <c r="J5" s="206"/>
+      <c r="K5" s="206"/>
+      <c r="L5" s="207"/>
+      <c r="M5" s="207"/>
+      <c r="N5" s="207"/>
+      <c r="O5" s="207"/>
+      <c r="P5" s="207"/>
+      <c r="Q5" s="207"/>
+      <c r="R5" s="207"/>
+      <c r="S5" s="207"/>
+      <c r="T5" s="207"/>
+      <c r="U5" s="207"/>
+      <c r="V5" s="207"/>
+      <c r="W5" s="208"/>
+      <c r="X5" s="208"/>
+      <c r="Y5" s="208"/>
+      <c r="Z5" s="208"/>
+      <c r="AA5" s="208"/>
+      <c r="AB5" s="212"/>
+      <c r="AC5" s="212"/>
+      <c r="AD5" s="212"/>
+      <c r="AE5" s="212"/>
+      <c r="AF5" s="212"/>
+      <c r="AG5" s="212"/>
+      <c r="AH5" s="212"/>
+      <c r="AI5" s="212"/>
+      <c r="AJ5" s="212"/>
+      <c r="AK5" s="212"/>
+      <c r="AL5" s="212"/>
+      <c r="AM5" s="212"/>
+      <c r="AN5" s="212"/>
+      <c r="AO5" s="212"/>
+      <c r="AP5" s="212"/>
+      <c r="AQ5" s="212"/>
+      <c r="AR5" s="213"/>
+      <c r="AS5" s="213"/>
+      <c r="AT5" s="213"/>
+      <c r="AU5" s="211"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
       <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="194"/>
-      <c r="BW5" s="194"/>
-      <c r="CT5" s="194"/>
-    </row>
-    <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="201"/>
-      <c r="B6" s="202" t="s">
+      <c r="AY5" s="186"/>
+      <c r="AZ5" s="186"/>
+      <c r="BA5" s="186"/>
+      <c r="BB5" s="186"/>
+      <c r="BC5" s="186"/>
+      <c r="BD5" s="186"/>
+      <c r="BE5" s="186"/>
+      <c r="BF5" s="188"/>
+      <c r="BG5" s="188"/>
+      <c r="BT5" s="177"/>
+      <c r="BW5" s="177"/>
+      <c r="CT5" s="177"/>
+    </row>
+    <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="176"/>
+      <c r="B6" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="202"/>
-      <c r="D6" s="200"/>
-      <c r="E6" s="200"/>
-      <c r="F6" s="200"/>
-      <c r="G6" s="200"/>
-      <c r="H6" s="200"/>
-      <c r="I6" s="200"/>
-      <c r="J6" s="200"/>
-      <c r="K6" s="200"/>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
-      <c r="O6" s="193"/>
-      <c r="P6" s="193"/>
-      <c r="Q6" s="193"/>
-      <c r="R6" s="193"/>
-      <c r="S6" s="193"/>
-      <c r="T6" s="193"/>
-      <c r="U6" s="193"/>
-      <c r="V6" s="193"/>
-      <c r="W6" s="192"/>
-      <c r="X6" s="192"/>
-      <c r="Y6" s="192"/>
-      <c r="Z6" s="192"/>
-      <c r="AA6" s="192"/>
-      <c r="AB6" s="190"/>
-      <c r="AC6" s="190"/>
-      <c r="AD6" s="190"/>
-      <c r="AE6" s="190"/>
-      <c r="AF6" s="190"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
-      <c r="AU6" s="175"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="206"/>
+      <c r="E6" s="206"/>
+      <c r="F6" s="206"/>
+      <c r="G6" s="206"/>
+      <c r="H6" s="206"/>
+      <c r="I6" s="206"/>
+      <c r="J6" s="206"/>
+      <c r="K6" s="206"/>
+      <c r="L6" s="207"/>
+      <c r="M6" s="207"/>
+      <c r="N6" s="207"/>
+      <c r="O6" s="207"/>
+      <c r="P6" s="207"/>
+      <c r="Q6" s="207"/>
+      <c r="R6" s="207"/>
+      <c r="S6" s="207"/>
+      <c r="T6" s="207"/>
+      <c r="U6" s="207"/>
+      <c r="V6" s="207"/>
+      <c r="W6" s="208"/>
+      <c r="X6" s="208"/>
+      <c r="Y6" s="208"/>
+      <c r="Z6" s="208"/>
+      <c r="AA6" s="208"/>
+      <c r="AB6" s="212"/>
+      <c r="AC6" s="212"/>
+      <c r="AD6" s="212"/>
+      <c r="AE6" s="212"/>
+      <c r="AF6" s="212"/>
+      <c r="AG6" s="212"/>
+      <c r="AH6" s="212"/>
+      <c r="AI6" s="212"/>
+      <c r="AJ6" s="212"/>
+      <c r="AK6" s="212"/>
+      <c r="AL6" s="212"/>
+      <c r="AM6" s="212"/>
+      <c r="AN6" s="212"/>
+      <c r="AO6" s="212"/>
+      <c r="AP6" s="212"/>
+      <c r="AQ6" s="212"/>
+      <c r="AR6" s="213"/>
+      <c r="AS6" s="213"/>
+      <c r="AT6" s="213"/>
+      <c r="AU6" s="211"/>
+      <c r="AV6" s="177"/>
+      <c r="AW6" s="177"/>
       <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="CT6" s="194"/>
-    </row>
-    <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="201"/>
-      <c r="B7" s="202" t="s">
+      <c r="AY6" s="186"/>
+      <c r="AZ6" s="186"/>
+      <c r="BA6" s="186"/>
+      <c r="BB6" s="186"/>
+      <c r="BC6" s="186"/>
+      <c r="BD6" s="186"/>
+      <c r="BE6" s="186"/>
+      <c r="BF6" s="188"/>
+      <c r="BG6" s="188"/>
+      <c r="BT6" s="177"/>
+      <c r="BW6" s="177"/>
+      <c r="CT6" s="177"/>
+    </row>
+    <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="176"/>
+      <c r="B7" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="202"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="200"/>
-      <c r="H7" s="200"/>
-      <c r="I7" s="200"/>
-      <c r="J7" s="200"/>
-      <c r="K7" s="200"/>
-      <c r="L7" s="193"/>
-      <c r="M7" s="193"/>
-      <c r="N7" s="193"/>
-      <c r="O7" s="193"/>
-      <c r="P7" s="193"/>
-      <c r="Q7" s="193"/>
-      <c r="R7" s="193"/>
-      <c r="S7" s="193"/>
-      <c r="T7" s="193"/>
-      <c r="U7" s="193"/>
-      <c r="V7" s="193"/>
-      <c r="W7" s="192"/>
-      <c r="X7" s="192"/>
-      <c r="Y7" s="192"/>
-      <c r="Z7" s="192"/>
-      <c r="AA7" s="192"/>
-      <c r="AB7" s="190"/>
-      <c r="AC7" s="190"/>
-      <c r="AD7" s="190"/>
-      <c r="AE7" s="190"/>
-      <c r="AF7" s="190"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
-      <c r="AU7" s="176"/>
-      <c r="AV7" s="194"/>
-      <c r="AW7" s="194"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="206"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="206"/>
+      <c r="H7" s="206"/>
+      <c r="I7" s="206"/>
+      <c r="J7" s="206"/>
+      <c r="K7" s="206"/>
+      <c r="L7" s="207"/>
+      <c r="M7" s="207"/>
+      <c r="N7" s="207"/>
+      <c r="O7" s="207"/>
+      <c r="P7" s="207"/>
+      <c r="Q7" s="207"/>
+      <c r="R7" s="207"/>
+      <c r="S7" s="207"/>
+      <c r="T7" s="207"/>
+      <c r="U7" s="207"/>
+      <c r="V7" s="207"/>
+      <c r="W7" s="208"/>
+      <c r="X7" s="208"/>
+      <c r="Y7" s="208"/>
+      <c r="Z7" s="208"/>
+      <c r="AA7" s="208"/>
+      <c r="AB7" s="212"/>
+      <c r="AC7" s="212"/>
+      <c r="AD7" s="212"/>
+      <c r="AE7" s="212"/>
+      <c r="AF7" s="212"/>
+      <c r="AG7" s="212"/>
+      <c r="AH7" s="212"/>
+      <c r="AI7" s="212"/>
+      <c r="AJ7" s="212"/>
+      <c r="AK7" s="212"/>
+      <c r="AL7" s="212"/>
+      <c r="AM7" s="212"/>
+      <c r="AN7" s="212"/>
+      <c r="AO7" s="212"/>
+      <c r="AP7" s="212"/>
+      <c r="AQ7" s="212"/>
+      <c r="AR7" s="213"/>
+      <c r="AS7" s="213"/>
+      <c r="AT7" s="213"/>
+      <c r="AU7" s="214"/>
+      <c r="AV7" s="177"/>
+      <c r="AW7" s="177"/>
       <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="194"/>
-      <c r="BW7" s="194"/>
-      <c r="CT7" s="194"/>
-    </row>
-    <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="201" t="s">
+      <c r="AY7" s="186"/>
+      <c r="AZ7" s="186"/>
+      <c r="BA7" s="186"/>
+      <c r="BB7" s="186"/>
+      <c r="BC7" s="186"/>
+      <c r="BD7" s="186"/>
+      <c r="BE7" s="186"/>
+      <c r="BF7" s="188"/>
+      <c r="BG7" s="188"/>
+      <c r="BT7" s="177"/>
+      <c r="BW7" s="177"/>
+      <c r="CT7" s="177"/>
+    </row>
+    <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="176" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="202" t="s">
+      <c r="B8" s="178" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="202"/>
-      <c r="D8" s="200"/>
-      <c r="E8" s="200"/>
-      <c r="F8" s="200"/>
-      <c r="G8" s="200"/>
-      <c r="H8" s="200"/>
-      <c r="I8" s="200"/>
-      <c r="J8" s="200"/>
-      <c r="K8" s="200"/>
-      <c r="L8" s="193"/>
-      <c r="M8" s="193"/>
-      <c r="N8" s="193"/>
-      <c r="O8" s="193"/>
-      <c r="P8" s="193"/>
-      <c r="Q8" s="193"/>
-      <c r="R8" s="193"/>
-      <c r="S8" s="193"/>
-      <c r="T8" s="193"/>
-      <c r="U8" s="193"/>
-      <c r="V8" s="193"/>
-      <c r="W8" s="192"/>
-      <c r="X8" s="192"/>
-      <c r="Y8" s="192"/>
-      <c r="Z8" s="192"/>
-      <c r="AA8" s="192"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="190"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
-      <c r="AU8" s="176"/>
-      <c r="AV8" s="194"/>
-      <c r="AW8" s="194"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="206"/>
+      <c r="E8" s="206"/>
+      <c r="F8" s="206"/>
+      <c r="G8" s="206"/>
+      <c r="H8" s="206"/>
+      <c r="I8" s="206"/>
+      <c r="J8" s="206"/>
+      <c r="K8" s="206"/>
+      <c r="L8" s="207"/>
+      <c r="M8" s="207"/>
+      <c r="N8" s="207"/>
+      <c r="O8" s="207"/>
+      <c r="P8" s="207"/>
+      <c r="Q8" s="207"/>
+      <c r="R8" s="207"/>
+      <c r="S8" s="207"/>
+      <c r="T8" s="207"/>
+      <c r="U8" s="207"/>
+      <c r="V8" s="207"/>
+      <c r="W8" s="208"/>
+      <c r="X8" s="208"/>
+      <c r="Y8" s="208"/>
+      <c r="Z8" s="208"/>
+      <c r="AA8" s="208"/>
+      <c r="AB8" s="212"/>
+      <c r="AC8" s="212"/>
+      <c r="AD8" s="212"/>
+      <c r="AE8" s="212"/>
+      <c r="AF8" s="212"/>
+      <c r="AG8" s="212"/>
+      <c r="AH8" s="212"/>
+      <c r="AI8" s="212"/>
+      <c r="AJ8" s="212"/>
+      <c r="AK8" s="212"/>
+      <c r="AL8" s="212"/>
+      <c r="AM8" s="212"/>
+      <c r="AN8" s="212"/>
+      <c r="AO8" s="212"/>
+      <c r="AP8" s="212"/>
+      <c r="AQ8" s="212"/>
+      <c r="AR8" s="213"/>
+      <c r="AS8" s="213"/>
+      <c r="AT8" s="213"/>
+      <c r="AU8" s="214"/>
+      <c r="AV8" s="177"/>
+      <c r="AW8" s="177"/>
       <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="194"/>
-      <c r="BW8" s="194"/>
-      <c r="CT8" s="194"/>
-    </row>
-    <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="201"/>
-      <c r="B9" s="202" t="s">
+      <c r="AY8" s="186"/>
+      <c r="AZ8" s="186"/>
+      <c r="BA8" s="186"/>
+      <c r="BB8" s="186"/>
+      <c r="BC8" s="186"/>
+      <c r="BD8" s="186"/>
+      <c r="BE8" s="186"/>
+      <c r="BF8" s="188"/>
+      <c r="BG8" s="188"/>
+      <c r="BT8" s="177"/>
+      <c r="BW8" s="177"/>
+      <c r="CT8" s="177"/>
+    </row>
+    <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="176"/>
+      <c r="B9" s="178" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="202"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="200"/>
-      <c r="I9" s="200"/>
-      <c r="J9" s="200"/>
-      <c r="K9" s="200"/>
-      <c r="L9" s="193"/>
-      <c r="M9" s="193"/>
-      <c r="N9" s="193"/>
-      <c r="O9" s="193"/>
-      <c r="P9" s="193"/>
-      <c r="Q9" s="193"/>
-      <c r="R9" s="193"/>
-      <c r="S9" s="193"/>
-      <c r="T9" s="193"/>
-      <c r="U9" s="193"/>
-      <c r="V9" s="193"/>
-      <c r="W9" s="192"/>
-      <c r="X9" s="192"/>
-      <c r="Y9" s="192"/>
-      <c r="Z9" s="192"/>
-      <c r="AA9" s="192"/>
-      <c r="AB9" s="190"/>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="190"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
-      <c r="AU9" s="176"/>
-      <c r="AV9" s="194"/>
-      <c r="AW9" s="194"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="206"/>
+      <c r="E9" s="206"/>
+      <c r="F9" s="206"/>
+      <c r="G9" s="206"/>
+      <c r="H9" s="206"/>
+      <c r="I9" s="206"/>
+      <c r="J9" s="206"/>
+      <c r="K9" s="206"/>
+      <c r="L9" s="207"/>
+      <c r="M9" s="207"/>
+      <c r="N9" s="207"/>
+      <c r="O9" s="207"/>
+      <c r="P9" s="207"/>
+      <c r="Q9" s="207"/>
+      <c r="R9" s="207"/>
+      <c r="S9" s="207"/>
+      <c r="T9" s="207"/>
+      <c r="U9" s="207"/>
+      <c r="V9" s="207"/>
+      <c r="W9" s="208"/>
+      <c r="X9" s="208"/>
+      <c r="Y9" s="208"/>
+      <c r="Z9" s="208"/>
+      <c r="AA9" s="208"/>
+      <c r="AB9" s="212"/>
+      <c r="AC9" s="212"/>
+      <c r="AD9" s="212"/>
+      <c r="AE9" s="212"/>
+      <c r="AF9" s="212"/>
+      <c r="AG9" s="212"/>
+      <c r="AH9" s="212"/>
+      <c r="AI9" s="212"/>
+      <c r="AJ9" s="212"/>
+      <c r="AK9" s="212"/>
+      <c r="AL9" s="212"/>
+      <c r="AM9" s="212"/>
+      <c r="AN9" s="212"/>
+      <c r="AO9" s="212"/>
+      <c r="AP9" s="212"/>
+      <c r="AQ9" s="212"/>
+      <c r="AR9" s="213"/>
+      <c r="AS9" s="213"/>
+      <c r="AT9" s="213"/>
+      <c r="AU9" s="214"/>
+      <c r="AV9" s="177"/>
+      <c r="AW9" s="177"/>
       <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="194"/>
-      <c r="BW9" s="194"/>
-      <c r="CT9" s="194"/>
-    </row>
-    <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202" t="s">
+      <c r="AY9" s="186"/>
+      <c r="AZ9" s="186"/>
+      <c r="BA9" s="186"/>
+      <c r="BB9" s="186"/>
+      <c r="BC9" s="186"/>
+      <c r="BD9" s="186"/>
+      <c r="BE9" s="186"/>
+      <c r="BF9" s="188"/>
+      <c r="BG9" s="188"/>
+      <c r="BT9" s="177"/>
+      <c r="BW9" s="177"/>
+      <c r="CT9" s="177"/>
+    </row>
+    <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="176"/>
+      <c r="B10" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="202"/>
-      <c r="D10" s="200"/>
-      <c r="E10" s="200"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="200"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200"/>
-      <c r="K10" s="200"/>
-      <c r="L10" s="193"/>
-      <c r="M10" s="193"/>
-      <c r="N10" s="193"/>
-      <c r="O10" s="193"/>
-      <c r="P10" s="193"/>
-      <c r="Q10" s="193"/>
-      <c r="R10" s="193"/>
-      <c r="S10" s="193"/>
-      <c r="T10" s="193"/>
-      <c r="U10" s="193"/>
-      <c r="V10" s="193"/>
-      <c r="W10" s="192"/>
-      <c r="X10" s="192"/>
-      <c r="Y10" s="192"/>
-      <c r="Z10" s="192"/>
-      <c r="AA10" s="192"/>
-      <c r="AB10" s="190"/>
-      <c r="AC10" s="190"/>
-      <c r="AD10" s="190"/>
-      <c r="AE10" s="190"/>
-      <c r="AF10" s="190"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
-      <c r="AU10" s="176"/>
-      <c r="AV10" s="194"/>
-      <c r="AW10" s="194"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="206"/>
+      <c r="E10" s="206"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="206"/>
+      <c r="H10" s="206"/>
+      <c r="I10" s="206"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="206"/>
+      <c r="L10" s="207"/>
+      <c r="M10" s="207"/>
+      <c r="N10" s="207"/>
+      <c r="O10" s="207"/>
+      <c r="P10" s="207"/>
+      <c r="Q10" s="207"/>
+      <c r="R10" s="207"/>
+      <c r="S10" s="207"/>
+      <c r="T10" s="207"/>
+      <c r="U10" s="207"/>
+      <c r="V10" s="207"/>
+      <c r="W10" s="208"/>
+      <c r="X10" s="208"/>
+      <c r="Y10" s="208"/>
+      <c r="Z10" s="208"/>
+      <c r="AA10" s="208"/>
+      <c r="AB10" s="212"/>
+      <c r="AC10" s="212"/>
+      <c r="AD10" s="212"/>
+      <c r="AE10" s="212"/>
+      <c r="AF10" s="212"/>
+      <c r="AG10" s="212"/>
+      <c r="AH10" s="212"/>
+      <c r="AI10" s="212"/>
+      <c r="AJ10" s="212"/>
+      <c r="AK10" s="212"/>
+      <c r="AL10" s="212"/>
+      <c r="AM10" s="212"/>
+      <c r="AN10" s="212"/>
+      <c r="AO10" s="212"/>
+      <c r="AP10" s="212"/>
+      <c r="AQ10" s="212"/>
+      <c r="AR10" s="213"/>
+      <c r="AS10" s="213"/>
+      <c r="AT10" s="213"/>
+      <c r="AU10" s="214"/>
+      <c r="AV10" s="177"/>
+      <c r="AW10" s="177"/>
       <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="194"/>
-      <c r="BW10" s="194"/>
-      <c r="CT10" s="194"/>
-    </row>
-    <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="201"/>
-      <c r="B11" s="202" t="s">
+      <c r="AY10" s="186"/>
+      <c r="AZ10" s="186"/>
+      <c r="BA10" s="186"/>
+      <c r="BB10" s="186"/>
+      <c r="BC10" s="186"/>
+      <c r="BD10" s="186"/>
+      <c r="BE10" s="186"/>
+      <c r="BF10" s="188"/>
+      <c r="BG10" s="188"/>
+      <c r="BT10" s="177"/>
+      <c r="BW10" s="177"/>
+      <c r="CT10" s="177"/>
+    </row>
+    <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="176"/>
+      <c r="B11" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="202"/>
-      <c r="D11" s="200"/>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="200"/>
-      <c r="H11" s="200"/>
-      <c r="I11" s="200"/>
-      <c r="J11" s="200"/>
-      <c r="K11" s="200"/>
-      <c r="L11" s="193"/>
-      <c r="M11" s="193"/>
-      <c r="N11" s="193"/>
-      <c r="O11" s="193"/>
-      <c r="P11" s="193"/>
-      <c r="Q11" s="193"/>
-      <c r="R11" s="193"/>
-      <c r="S11" s="193"/>
-      <c r="T11" s="193"/>
-      <c r="U11" s="193"/>
-      <c r="V11" s="193"/>
-      <c r="W11" s="192"/>
-      <c r="X11" s="192"/>
-      <c r="Y11" s="192"/>
-      <c r="Z11" s="192"/>
-      <c r="AA11" s="192"/>
-      <c r="AB11" s="191"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="191"/>
-      <c r="AE11" s="191"/>
-      <c r="AF11" s="191"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
-      <c r="AU11" s="176"/>
-      <c r="AV11" s="194"/>
-      <c r="AW11" s="194"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="206"/>
+      <c r="E11" s="206"/>
+      <c r="F11" s="206"/>
+      <c r="G11" s="206"/>
+      <c r="H11" s="206"/>
+      <c r="I11" s="206"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="206"/>
+      <c r="L11" s="207"/>
+      <c r="M11" s="207"/>
+      <c r="N11" s="207"/>
+      <c r="O11" s="207"/>
+      <c r="P11" s="207"/>
+      <c r="Q11" s="207"/>
+      <c r="R11" s="207"/>
+      <c r="S11" s="207"/>
+      <c r="T11" s="207"/>
+      <c r="U11" s="207"/>
+      <c r="V11" s="207"/>
+      <c r="W11" s="208"/>
+      <c r="X11" s="208"/>
+      <c r="Y11" s="208"/>
+      <c r="Z11" s="208"/>
+      <c r="AA11" s="208"/>
+      <c r="AB11" s="215"/>
+      <c r="AC11" s="215"/>
+      <c r="AD11" s="215"/>
+      <c r="AE11" s="215"/>
+      <c r="AF11" s="215"/>
+      <c r="AG11" s="215"/>
+      <c r="AH11" s="215"/>
+      <c r="AI11" s="215"/>
+      <c r="AJ11" s="215"/>
+      <c r="AK11" s="215"/>
+      <c r="AL11" s="215"/>
+      <c r="AM11" s="215"/>
+      <c r="AN11" s="215"/>
+      <c r="AO11" s="215"/>
+      <c r="AP11" s="215"/>
+      <c r="AQ11" s="215"/>
+      <c r="AR11" s="216"/>
+      <c r="AS11" s="216"/>
+      <c r="AT11" s="216"/>
+      <c r="AU11" s="214"/>
+      <c r="AV11" s="177"/>
+      <c r="AW11" s="177"/>
       <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="194"/>
-      <c r="BW11" s="194"/>
-      <c r="CT11" s="194"/>
+      <c r="AY11" s="186"/>
+      <c r="AZ11" s="186"/>
+      <c r="BA11" s="186"/>
+      <c r="BB11" s="186"/>
+      <c r="BC11" s="186"/>
+      <c r="BD11" s="186"/>
+      <c r="BE11" s="186"/>
+      <c r="BF11" s="188"/>
+      <c r="BG11" s="188"/>
+      <c r="BT11" s="177"/>
+      <c r="BW11" s="177"/>
+      <c r="CT11" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4204,63 +4267,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4270,7 +4276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17334876-DDC9-42EB-8687-1B5E40BF9E51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -5118,7 +5124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5782,13 +5788,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="205" t="s">
+      <c r="A4" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="207" t="s">
+      <c r="B4" s="202" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="208"/>
+      <c r="C4" s="203"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5893,9 +5899,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="206"/>
-      <c r="B5" s="204"/>
-      <c r="C5" s="206"/>
+      <c r="A5" s="190"/>
+      <c r="B5" s="200"/>
+      <c r="C5" s="190"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -6000,11 +6006,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="206"/>
+      <c r="A6" s="190"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="206"/>
+      <c r="C6" s="190"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6109,11 +6115,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="206"/>
+      <c r="A7" s="190"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="206"/>
+      <c r="C7" s="190"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6218,11 +6224,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="206"/>
+      <c r="A8" s="190"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="206"/>
+      <c r="C8" s="190"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6327,11 +6333,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="206"/>
+      <c r="A9" s="190"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="206"/>
+      <c r="C9" s="190"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6436,11 +6442,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="206"/>
+      <c r="A10" s="190"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="206"/>
+      <c r="C10" s="190"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6545,11 +6551,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="206"/>
+      <c r="A11" s="190"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="206"/>
+      <c r="C11" s="190"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6654,9 +6660,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="206"/>
+      <c r="A12" s="190"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="209"/>
+      <c r="C12" s="191"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6761,10 +6767,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="210" t="s">
+      <c r="A13" s="204" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="211" t="s">
+      <c r="B13" s="205" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6873,8 +6879,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="206"/>
-      <c r="B14" s="212"/>
+      <c r="A14" s="190"/>
+      <c r="B14" s="196"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -6995,7 +7001,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="206"/>
+      <c r="A15" s="190"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7105,7 +7111,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="206"/>
+      <c r="A16" s="190"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7215,7 +7221,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="206"/>
+      <c r="A17" s="190"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7327,7 +7333,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="206"/>
+      <c r="A18" s="190"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7437,7 +7443,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="206"/>
+      <c r="A19" s="190"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7547,7 +7553,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="206"/>
+      <c r="A20" s="190"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7657,7 +7663,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="209"/>
+      <c r="A21" s="191"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7768,7 +7774,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="203" t="s">
+      <c r="B22" s="199" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7878,7 +7884,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="204"/>
+      <c r="B23" s="200"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7985,13 +7991,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="214" t="s">
+      <c r="A24" s="192" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="216">
+      <c r="C24" s="194">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8099,11 +8105,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="215"/>
+      <c r="A25" s="193"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="206"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8209,11 +8215,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="215"/>
+      <c r="A26" s="193"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="206"/>
+      <c r="C26" s="190"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8319,11 +8325,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="215"/>
+      <c r="A27" s="193"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="206"/>
+      <c r="C27" s="190"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8429,11 +8435,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="215"/>
+      <c r="A28" s="193"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="206"/>
+      <c r="C28" s="190"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8539,11 +8545,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="215"/>
+      <c r="A29" s="193"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="206"/>
+      <c r="C29" s="190"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8649,11 +8655,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="215"/>
+      <c r="A30" s="193"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="206"/>
+      <c r="C30" s="190"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8759,11 +8765,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="215"/>
+      <c r="A31" s="193"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="206"/>
+      <c r="C31" s="190"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8869,11 +8875,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="215"/>
+      <c r="A32" s="193"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="206"/>
+      <c r="C32" s="190"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8979,11 +8985,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="215"/>
+      <c r="A33" s="193"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="206"/>
+      <c r="C33" s="190"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9089,11 +9095,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="215"/>
+      <c r="A34" s="193"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="206"/>
+      <c r="C34" s="190"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9199,11 +9205,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="215"/>
+      <c r="A35" s="193"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="209"/>
+      <c r="C35" s="191"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9309,11 +9315,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="215"/>
+      <c r="A36" s="193"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="216">
+      <c r="C36" s="194">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9421,11 +9427,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="215"/>
+      <c r="A37" s="193"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="206"/>
+      <c r="C37" s="190"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9531,11 +9537,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="215"/>
+      <c r="A38" s="193"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="206"/>
+      <c r="C38" s="190"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9641,11 +9647,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="215"/>
+      <c r="A39" s="193"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="206"/>
+      <c r="C39" s="190"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9751,11 +9757,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="215"/>
+      <c r="A40" s="193"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="206"/>
+      <c r="C40" s="190"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9861,11 +9867,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="215"/>
+      <c r="A41" s="193"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="206"/>
+      <c r="C41" s="190"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9971,11 +9977,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="215"/>
+      <c r="A42" s="193"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="206"/>
+      <c r="C42" s="190"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10081,11 +10087,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="215"/>
+      <c r="A43" s="193"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="206"/>
+      <c r="C43" s="190"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10191,11 +10197,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="215"/>
+      <c r="A44" s="193"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="206"/>
+      <c r="C44" s="190"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10301,11 +10307,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="215"/>
+      <c r="A45" s="193"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="206"/>
+      <c r="C45" s="190"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10411,11 +10417,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="215"/>
+      <c r="A46" s="193"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="206"/>
+      <c r="C46" s="190"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10521,11 +10527,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="215"/>
+      <c r="A47" s="193"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="206"/>
+      <c r="C47" s="190"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10639,11 +10645,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="215"/>
+      <c r="A48" s="193"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="206"/>
+      <c r="C48" s="190"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10752,7 +10758,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="217" t="s">
+      <c r="B49" s="195" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10862,7 +10868,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="212"/>
+      <c r="B50" s="196"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14293,7 +14299,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="218" t="s">
+      <c r="A81" s="197" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14405,7 +14411,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="206"/>
+      <c r="A82" s="190"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14515,7 +14521,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="206"/>
+      <c r="A83" s="190"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14625,7 +14631,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="206"/>
+      <c r="A84" s="190"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14735,7 +14741,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="206"/>
+      <c r="A85" s="190"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14845,7 +14851,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="206"/>
+      <c r="A86" s="190"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14955,7 +14961,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="206"/>
+      <c r="A87" s="190"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15067,7 +15073,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="206"/>
+      <c r="A88" s="190"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15177,7 +15183,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="206"/>
+      <c r="A89" s="190"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15287,7 +15293,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="206"/>
+      <c r="A90" s="190"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15397,11 +15403,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="206"/>
+      <c r="A91" s="190"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="219"/>
+      <c r="C91" s="198"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15507,11 +15513,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="206"/>
+      <c r="A92" s="190"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="206"/>
+      <c r="C92" s="190"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15617,11 +15623,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="209"/>
+      <c r="A93" s="191"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="206"/>
+      <c r="C93" s="190"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15845,7 +15851,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="213" t="s">
+      <c r="A95" s="189" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15957,7 +15963,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="206"/>
+      <c r="A96" s="190"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16067,7 +16073,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="206"/>
+      <c r="A97" s="190"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16177,7 +16183,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="206"/>
+      <c r="A98" s="190"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16287,7 +16293,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="206"/>
+      <c r="A99" s="190"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16397,7 +16403,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="206"/>
+      <c r="A100" s="190"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16507,7 +16513,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="206"/>
+      <c r="A101" s="190"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16617,7 +16623,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="206"/>
+      <c r="A102" s="190"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16727,7 +16733,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="206"/>
+      <c r="A103" s="190"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16839,7 +16845,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="206"/>
+      <c r="A104" s="190"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16949,7 +16955,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="206"/>
+      <c r="A105" s="190"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17067,7 +17073,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="206"/>
+      <c r="A106" s="190"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17177,7 +17183,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="206"/>
+      <c r="A107" s="190"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17287,7 +17293,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="206"/>
+      <c r="A108" s="190"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17397,7 +17403,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="206"/>
+      <c r="A109" s="190"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17507,7 +17513,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="206"/>
+      <c r="A110" s="190"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17617,7 +17623,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="206"/>
+      <c r="A111" s="190"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17727,7 +17733,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="206"/>
+      <c r="A112" s="190"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17837,7 +17843,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="206"/>
+      <c r="A113" s="190"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17947,7 +17953,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="206"/>
+      <c r="A114" s="190"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18057,7 +18063,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="206"/>
+      <c r="A115" s="190"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18167,7 +18173,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="206"/>
+      <c r="A116" s="190"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18293,7 +18299,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="206"/>
+      <c r="A117" s="190"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18403,7 +18409,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="209"/>
+      <c r="A118" s="191"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25774,6 +25780,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25781,12 +25793,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 01-10
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AB610F-A5AD-4DB9-8C5F-F6AA54E03E7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="178">
   <si>
     <t>S</t>
   </si>
@@ -739,11 +740,14 @@
   <si>
     <t>Não houve acompanhamento pois foi realizada apresentação dos projetos da turma do técnico para a coordenação</t>
   </si>
+  <si>
+    <t>Exercícios de programação orientada a objetos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2265,14 +2269,51 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2289,26 +2330,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2319,67 +2374,16 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2876,14 +2880,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AM4" sqref="AM4:AM11"/>
+      <selection pane="bottomRight" activeCell="AN4" sqref="AN4:AN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3192,110 +3196,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="179" t="s">
+      <c r="D2" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="179"/>
-      <c r="F2" s="179"/>
-      <c r="G2" s="179"/>
-      <c r="H2" s="179"/>
-      <c r="I2" s="179"/>
-      <c r="J2" s="179"/>
-      <c r="K2" s="179"/>
-      <c r="L2" s="179"/>
-      <c r="M2" s="179"/>
-      <c r="N2" s="179"/>
-      <c r="O2" s="179"/>
-      <c r="P2" s="179"/>
-      <c r="Q2" s="179"/>
-      <c r="R2" s="179" t="s">
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="192"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="179"/>
-      <c r="T2" s="179"/>
-      <c r="U2" s="179"/>
-      <c r="V2" s="179"/>
-      <c r="W2" s="179"/>
-      <c r="X2" s="179"/>
-      <c r="Y2" s="179"/>
-      <c r="Z2" s="179"/>
-      <c r="AA2" s="179"/>
-      <c r="AB2" s="179"/>
-      <c r="AC2" s="179"/>
-      <c r="AD2" s="179"/>
-      <c r="AE2" s="179"/>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="179"/>
-      <c r="AH2" s="179"/>
-      <c r="AI2" s="179"/>
-      <c r="AJ2" s="179"/>
-      <c r="AK2" s="179"/>
-      <c r="AL2" s="179"/>
-      <c r="AM2" s="179" t="s">
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
+      <c r="AF2" s="192"/>
+      <c r="AG2" s="192"/>
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="192"/>
+      <c r="AJ2" s="192"/>
+      <c r="AK2" s="192"/>
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="179"/>
-      <c r="AO2" s="179"/>
-      <c r="AP2" s="179"/>
-      <c r="AQ2" s="179"/>
-      <c r="AR2" s="179"/>
-      <c r="AS2" s="179"/>
-      <c r="AT2" s="179"/>
-      <c r="AU2" s="179"/>
-      <c r="AV2" s="179"/>
-      <c r="AW2" s="179"/>
-      <c r="AX2" s="180"/>
-      <c r="AY2" s="180"/>
-      <c r="AZ2" s="180"/>
-      <c r="BA2" s="180"/>
-      <c r="BB2" s="180"/>
-      <c r="BC2" s="180"/>
-      <c r="BD2" s="180"/>
-      <c r="BE2" s="180"/>
-      <c r="BF2" s="180"/>
-      <c r="BG2" s="180"/>
-      <c r="BH2" s="180"/>
-      <c r="BI2" s="180"/>
-      <c r="BJ2" s="179" t="s">
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="192"/>
+      <c r="AQ2" s="192"/>
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="192"/>
+      <c r="AV2" s="192"/>
+      <c r="AW2" s="192"/>
+      <c r="AX2" s="193"/>
+      <c r="AY2" s="193"/>
+      <c r="AZ2" s="193"/>
+      <c r="BA2" s="193"/>
+      <c r="BB2" s="193"/>
+      <c r="BC2" s="193"/>
+      <c r="BD2" s="193"/>
+      <c r="BE2" s="193"/>
+      <c r="BF2" s="193"/>
+      <c r="BG2" s="193"/>
+      <c r="BH2" s="193"/>
+      <c r="BI2" s="193"/>
+      <c r="BJ2" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="179"/>
-      <c r="BL2" s="179"/>
-      <c r="BM2" s="179"/>
-      <c r="BN2" s="179"/>
-      <c r="BO2" s="179"/>
-      <c r="BP2" s="179"/>
-      <c r="BQ2" s="179"/>
-      <c r="BR2" s="179"/>
-      <c r="BS2" s="179"/>
-      <c r="BT2" s="179"/>
-      <c r="BU2" s="179"/>
-      <c r="BV2" s="179"/>
-      <c r="BW2" s="179"/>
-      <c r="BX2" s="181"/>
-      <c r="BY2" s="181"/>
-      <c r="BZ2" s="181"/>
-      <c r="CA2" s="181"/>
-      <c r="CB2" s="181"/>
-      <c r="CC2" s="181"/>
-      <c r="CD2" s="181"/>
-      <c r="CE2" s="182" t="s">
+      <c r="BK2" s="192"/>
+      <c r="BL2" s="192"/>
+      <c r="BM2" s="192"/>
+      <c r="BN2" s="192"/>
+      <c r="BO2" s="192"/>
+      <c r="BP2" s="192"/>
+      <c r="BQ2" s="192"/>
+      <c r="BR2" s="192"/>
+      <c r="BS2" s="192"/>
+      <c r="BT2" s="192"/>
+      <c r="BU2" s="192"/>
+      <c r="BV2" s="192"/>
+      <c r="BW2" s="192"/>
+      <c r="BX2" s="194"/>
+      <c r="BY2" s="194"/>
+      <c r="BZ2" s="194"/>
+      <c r="CA2" s="194"/>
+      <c r="CB2" s="194"/>
+      <c r="CC2" s="194"/>
+      <c r="CD2" s="194"/>
+      <c r="CE2" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="183"/>
-      <c r="CG2" s="183"/>
-      <c r="CH2" s="183"/>
-      <c r="CI2" s="183"/>
-      <c r="CJ2" s="183"/>
-      <c r="CK2" s="183"/>
-      <c r="CL2" s="183"/>
-      <c r="CM2" s="183"/>
-      <c r="CN2" s="183"/>
-      <c r="CO2" s="183"/>
-      <c r="CP2" s="183"/>
-      <c r="CQ2" s="183"/>
-      <c r="CR2" s="183"/>
-      <c r="CS2" s="183"/>
+      <c r="CF2" s="196"/>
+      <c r="CG2" s="196"/>
+      <c r="CH2" s="196"/>
+      <c r="CI2" s="196"/>
+      <c r="CJ2" s="196"/>
+      <c r="CK2" s="196"/>
+      <c r="CL2" s="196"/>
+      <c r="CM2" s="196"/>
+      <c r="CN2" s="196"/>
+      <c r="CO2" s="196"/>
+      <c r="CP2" s="196"/>
+      <c r="CQ2" s="196"/>
+      <c r="CR2" s="196"/>
+      <c r="CS2" s="196"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3591,650 +3595,627 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="D4" s="206" t="s">
+      <c r="C4" s="199"/>
+      <c r="D4" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="206" t="s">
+      <c r="E4" s="197" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="206" t="s">
+      <c r="F4" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="206" t="s">
+      <c r="G4" s="197" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="206" t="s">
+      <c r="H4" s="197" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="206" t="s">
+      <c r="I4" s="197" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="206" t="s">
+      <c r="J4" s="197" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="206" t="s">
+      <c r="K4" s="197" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="207" t="s">
+      <c r="L4" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="207" t="s">
+      <c r="M4" s="190" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="207" t="s">
+      <c r="N4" s="190" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="207" t="s">
+      <c r="O4" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="207" t="s">
+      <c r="P4" s="190" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="207" t="s">
+      <c r="Q4" s="190" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="207" t="s">
+      <c r="R4" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="207" t="s">
+      <c r="S4" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="207" t="s">
+      <c r="T4" s="190" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="207" t="s">
+      <c r="U4" s="190" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="207" t="s">
+      <c r="V4" s="190" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="208" t="s">
+      <c r="W4" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="208" t="s">
+      <c r="X4" s="189" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="208" t="s">
+      <c r="Y4" s="189" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="208" t="s">
+      <c r="Z4" s="189" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="208" t="s">
+      <c r="AA4" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="209" t="s">
+      <c r="AB4" s="186" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="209" t="s">
+      <c r="AC4" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="209" t="s">
+      <c r="AD4" s="186" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="209" t="s">
+      <c r="AE4" s="186" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="209" t="s">
+      <c r="AF4" s="186" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="209" t="s">
+      <c r="AG4" s="186" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="209" t="s">
+      <c r="AH4" s="186" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="209" t="s">
+      <c r="AI4" s="186" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="209" t="s">
+      <c r="AJ4" s="186" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="209" t="s">
+      <c r="AK4" s="186" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" s="209" t="s">
+      <c r="AL4" s="186" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" s="209"/>
-      <c r="AN4" s="209"/>
-      <c r="AO4" s="209"/>
-      <c r="AP4" s="209"/>
-      <c r="AQ4" s="209"/>
-      <c r="AR4" s="210"/>
-      <c r="AS4" s="210"/>
-      <c r="AT4" s="210"/>
-      <c r="AU4" s="211"/>
-      <c r="AV4" s="177"/>
-      <c r="AW4" s="177"/>
+      <c r="AM4" s="186" t="s">
+        <v>177</v>
+      </c>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="186"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
+      <c r="AU4" s="176"/>
+      <c r="AV4" s="191"/>
+      <c r="AW4" s="191"/>
       <c r="AX4" s="184"/>
-      <c r="AY4" s="186"/>
-      <c r="AZ4" s="186"/>
-      <c r="BA4" s="186"/>
-      <c r="BB4" s="186"/>
-      <c r="BC4" s="186"/>
-      <c r="BD4" s="186"/>
-      <c r="BE4" s="186"/>
-      <c r="BF4" s="187"/>
-      <c r="BG4" s="187"/>
-      <c r="BT4" s="177"/>
-      <c r="BW4" s="177"/>
-      <c r="CT4" s="177"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="191"/>
+      <c r="BW4" s="191"/>
+      <c r="CT4" s="191"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="176"/>
-      <c r="B5" s="178" t="s">
+      <c r="A5" s="198"/>
+      <c r="B5" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="178"/>
-      <c r="D5" s="206"/>
-      <c r="E5" s="206"/>
-      <c r="F5" s="206"/>
-      <c r="G5" s="206"/>
-      <c r="H5" s="206"/>
-      <c r="I5" s="206"/>
-      <c r="J5" s="206"/>
-      <c r="K5" s="206"/>
-      <c r="L5" s="207"/>
-      <c r="M5" s="207"/>
-      <c r="N5" s="207"/>
-      <c r="O5" s="207"/>
-      <c r="P5" s="207"/>
-      <c r="Q5" s="207"/>
-      <c r="R5" s="207"/>
-      <c r="S5" s="207"/>
-      <c r="T5" s="207"/>
-      <c r="U5" s="207"/>
-      <c r="V5" s="207"/>
-      <c r="W5" s="208"/>
-      <c r="X5" s="208"/>
-      <c r="Y5" s="208"/>
-      <c r="Z5" s="208"/>
-      <c r="AA5" s="208"/>
-      <c r="AB5" s="212"/>
-      <c r="AC5" s="212"/>
-      <c r="AD5" s="212"/>
-      <c r="AE5" s="212"/>
-      <c r="AF5" s="212"/>
-      <c r="AG5" s="212"/>
-      <c r="AH5" s="212"/>
-      <c r="AI5" s="212"/>
-      <c r="AJ5" s="212"/>
-      <c r="AK5" s="212"/>
-      <c r="AL5" s="212"/>
-      <c r="AM5" s="212"/>
-      <c r="AN5" s="212"/>
-      <c r="AO5" s="212"/>
-      <c r="AP5" s="212"/>
-      <c r="AQ5" s="212"/>
-      <c r="AR5" s="213"/>
-      <c r="AS5" s="213"/>
-      <c r="AT5" s="213"/>
-      <c r="AU5" s="211"/>
-      <c r="AV5" s="177"/>
-      <c r="AW5" s="177"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="197"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="197"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="190"/>
+      <c r="P5" s="190"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="190"/>
+      <c r="S5" s="190"/>
+      <c r="T5" s="190"/>
+      <c r="U5" s="190"/>
+      <c r="V5" s="190"/>
+      <c r="W5" s="189"/>
+      <c r="X5" s="189"/>
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="189"/>
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="187"/>
+      <c r="AC5" s="187"/>
+      <c r="AD5" s="187"/>
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="187"/>
+      <c r="AG5" s="187"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
+      <c r="AU5" s="176"/>
+      <c r="AV5" s="191"/>
+      <c r="AW5" s="191"/>
       <c r="AX5" s="185"/>
-      <c r="AY5" s="186"/>
-      <c r="AZ5" s="186"/>
-      <c r="BA5" s="186"/>
-      <c r="BB5" s="186"/>
-      <c r="BC5" s="186"/>
-      <c r="BD5" s="186"/>
-      <c r="BE5" s="186"/>
-      <c r="BF5" s="188"/>
-      <c r="BG5" s="188"/>
-      <c r="BT5" s="177"/>
-      <c r="BW5" s="177"/>
-      <c r="CT5" s="177"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="191"/>
+      <c r="BW5" s="191"/>
+      <c r="CT5" s="191"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="176"/>
-      <c r="B6" s="178" t="s">
+      <c r="A6" s="198"/>
+      <c r="B6" s="199" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="206"/>
-      <c r="E6" s="206"/>
-      <c r="F6" s="206"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="206"/>
-      <c r="I6" s="206"/>
-      <c r="J6" s="206"/>
-      <c r="K6" s="206"/>
-      <c r="L6" s="207"/>
-      <c r="M6" s="207"/>
-      <c r="N6" s="207"/>
-      <c r="O6" s="207"/>
-      <c r="P6" s="207"/>
-      <c r="Q6" s="207"/>
-      <c r="R6" s="207"/>
-      <c r="S6" s="207"/>
-      <c r="T6" s="207"/>
-      <c r="U6" s="207"/>
-      <c r="V6" s="207"/>
-      <c r="W6" s="208"/>
-      <c r="X6" s="208"/>
-      <c r="Y6" s="208"/>
-      <c r="Z6" s="208"/>
-      <c r="AA6" s="208"/>
-      <c r="AB6" s="212"/>
-      <c r="AC6" s="212"/>
-      <c r="AD6" s="212"/>
-      <c r="AE6" s="212"/>
-      <c r="AF6" s="212"/>
-      <c r="AG6" s="212"/>
-      <c r="AH6" s="212"/>
-      <c r="AI6" s="212"/>
-      <c r="AJ6" s="212"/>
-      <c r="AK6" s="212"/>
-      <c r="AL6" s="212"/>
-      <c r="AM6" s="212"/>
-      <c r="AN6" s="212"/>
-      <c r="AO6" s="212"/>
-      <c r="AP6" s="212"/>
-      <c r="AQ6" s="212"/>
-      <c r="AR6" s="213"/>
-      <c r="AS6" s="213"/>
-      <c r="AT6" s="213"/>
-      <c r="AU6" s="211"/>
-      <c r="AV6" s="177"/>
-      <c r="AW6" s="177"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="N6" s="190"/>
+      <c r="O6" s="190"/>
+      <c r="P6" s="190"/>
+      <c r="Q6" s="190"/>
+      <c r="R6" s="190"/>
+      <c r="S6" s="190"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="190"/>
+      <c r="V6" s="190"/>
+      <c r="W6" s="189"/>
+      <c r="X6" s="189"/>
+      <c r="Y6" s="189"/>
+      <c r="Z6" s="189"/>
+      <c r="AA6" s="189"/>
+      <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
+      <c r="AD6" s="187"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="187"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
+      <c r="AU6" s="176"/>
+      <c r="AV6" s="191"/>
+      <c r="AW6" s="191"/>
       <c r="AX6" s="185"/>
-      <c r="AY6" s="186"/>
-      <c r="AZ6" s="186"/>
-      <c r="BA6" s="186"/>
-      <c r="BB6" s="186"/>
-      <c r="BC6" s="186"/>
-      <c r="BD6" s="186"/>
-      <c r="BE6" s="186"/>
-      <c r="BF6" s="188"/>
-      <c r="BG6" s="188"/>
-      <c r="BT6" s="177"/>
-      <c r="BW6" s="177"/>
-      <c r="CT6" s="177"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="191"/>
+      <c r="BW6" s="191"/>
+      <c r="CT6" s="191"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="176"/>
-      <c r="B7" s="178" t="s">
+      <c r="A7" s="198"/>
+      <c r="B7" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="206"/>
-      <c r="E7" s="206"/>
-      <c r="F7" s="206"/>
-      <c r="G7" s="206"/>
-      <c r="H7" s="206"/>
-      <c r="I7" s="206"/>
-      <c r="J7" s="206"/>
-      <c r="K7" s="206"/>
-      <c r="L7" s="207"/>
-      <c r="M7" s="207"/>
-      <c r="N7" s="207"/>
-      <c r="O7" s="207"/>
-      <c r="P7" s="207"/>
-      <c r="Q7" s="207"/>
-      <c r="R7" s="207"/>
-      <c r="S7" s="207"/>
-      <c r="T7" s="207"/>
-      <c r="U7" s="207"/>
-      <c r="V7" s="207"/>
-      <c r="W7" s="208"/>
-      <c r="X7" s="208"/>
-      <c r="Y7" s="208"/>
-      <c r="Z7" s="208"/>
-      <c r="AA7" s="208"/>
-      <c r="AB7" s="212"/>
-      <c r="AC7" s="212"/>
-      <c r="AD7" s="212"/>
-      <c r="AE7" s="212"/>
-      <c r="AF7" s="212"/>
-      <c r="AG7" s="212"/>
-      <c r="AH7" s="212"/>
-      <c r="AI7" s="212"/>
-      <c r="AJ7" s="212"/>
-      <c r="AK7" s="212"/>
-      <c r="AL7" s="212"/>
-      <c r="AM7" s="212"/>
-      <c r="AN7" s="212"/>
-      <c r="AO7" s="212"/>
-      <c r="AP7" s="212"/>
-      <c r="AQ7" s="212"/>
-      <c r="AR7" s="213"/>
-      <c r="AS7" s="213"/>
-      <c r="AT7" s="213"/>
-      <c r="AU7" s="214"/>
-      <c r="AV7" s="177"/>
-      <c r="AW7" s="177"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="197"/>
+      <c r="F7" s="197"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
+      <c r="Q7" s="190"/>
+      <c r="R7" s="190"/>
+      <c r="S7" s="190"/>
+      <c r="T7" s="190"/>
+      <c r="U7" s="190"/>
+      <c r="V7" s="190"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="189"/>
+      <c r="Y7" s="189"/>
+      <c r="Z7" s="189"/>
+      <c r="AA7" s="189"/>
+      <c r="AB7" s="187"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
+      <c r="AU7" s="177"/>
+      <c r="AV7" s="191"/>
+      <c r="AW7" s="191"/>
       <c r="AX7" s="185"/>
-      <c r="AY7" s="186"/>
-      <c r="AZ7" s="186"/>
-      <c r="BA7" s="186"/>
-      <c r="BB7" s="186"/>
-      <c r="BC7" s="186"/>
-      <c r="BD7" s="186"/>
-      <c r="BE7" s="186"/>
-      <c r="BF7" s="188"/>
-      <c r="BG7" s="188"/>
-      <c r="BT7" s="177"/>
-      <c r="BW7" s="177"/>
-      <c r="CT7" s="177"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="191"/>
+      <c r="BW7" s="191"/>
+      <c r="CT7" s="191"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="178" t="s">
+      <c r="B8" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="178"/>
-      <c r="D8" s="206"/>
-      <c r="E8" s="206"/>
-      <c r="F8" s="206"/>
-      <c r="G8" s="206"/>
-      <c r="H8" s="206"/>
-      <c r="I8" s="206"/>
-      <c r="J8" s="206"/>
-      <c r="K8" s="206"/>
-      <c r="L8" s="207"/>
-      <c r="M8" s="207"/>
-      <c r="N8" s="207"/>
-      <c r="O8" s="207"/>
-      <c r="P8" s="207"/>
-      <c r="Q8" s="207"/>
-      <c r="R8" s="207"/>
-      <c r="S8" s="207"/>
-      <c r="T8" s="207"/>
-      <c r="U8" s="207"/>
-      <c r="V8" s="207"/>
-      <c r="W8" s="208"/>
-      <c r="X8" s="208"/>
-      <c r="Y8" s="208"/>
-      <c r="Z8" s="208"/>
-      <c r="AA8" s="208"/>
-      <c r="AB8" s="212"/>
-      <c r="AC8" s="212"/>
-      <c r="AD8" s="212"/>
-      <c r="AE8" s="212"/>
-      <c r="AF8" s="212"/>
-      <c r="AG8" s="212"/>
-      <c r="AH8" s="212"/>
-      <c r="AI8" s="212"/>
-      <c r="AJ8" s="212"/>
-      <c r="AK8" s="212"/>
-      <c r="AL8" s="212"/>
-      <c r="AM8" s="212"/>
-      <c r="AN8" s="212"/>
-      <c r="AO8" s="212"/>
-      <c r="AP8" s="212"/>
-      <c r="AQ8" s="212"/>
-      <c r="AR8" s="213"/>
-      <c r="AS8" s="213"/>
-      <c r="AT8" s="213"/>
-      <c r="AU8" s="214"/>
-      <c r="AV8" s="177"/>
-      <c r="AW8" s="177"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="197"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="190"/>
+      <c r="R8" s="190"/>
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="190"/>
+      <c r="W8" s="189"/>
+      <c r="X8" s="189"/>
+      <c r="Y8" s="189"/>
+      <c r="Z8" s="189"/>
+      <c r="AA8" s="189"/>
+      <c r="AB8" s="187"/>
+      <c r="AC8" s="187"/>
+      <c r="AD8" s="187"/>
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="187"/>
+      <c r="AG8" s="187"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
+      <c r="AU8" s="177"/>
+      <c r="AV8" s="191"/>
+      <c r="AW8" s="191"/>
       <c r="AX8" s="185"/>
-      <c r="AY8" s="186"/>
-      <c r="AZ8" s="186"/>
-      <c r="BA8" s="186"/>
-      <c r="BB8" s="186"/>
-      <c r="BC8" s="186"/>
-      <c r="BD8" s="186"/>
-      <c r="BE8" s="186"/>
-      <c r="BF8" s="188"/>
-      <c r="BG8" s="188"/>
-      <c r="BT8" s="177"/>
-      <c r="BW8" s="177"/>
-      <c r="CT8" s="177"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="191"/>
+      <c r="BW8" s="191"/>
+      <c r="CT8" s="191"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="176"/>
-      <c r="B9" s="178" t="s">
+      <c r="A9" s="198"/>
+      <c r="B9" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="178"/>
-      <c r="D9" s="206"/>
-      <c r="E9" s="206"/>
-      <c r="F9" s="206"/>
-      <c r="G9" s="206"/>
-      <c r="H9" s="206"/>
-      <c r="I9" s="206"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="207"/>
-      <c r="M9" s="207"/>
-      <c r="N9" s="207"/>
-      <c r="O9" s="207"/>
-      <c r="P9" s="207"/>
-      <c r="Q9" s="207"/>
-      <c r="R9" s="207"/>
-      <c r="S9" s="207"/>
-      <c r="T9" s="207"/>
-      <c r="U9" s="207"/>
-      <c r="V9" s="207"/>
-      <c r="W9" s="208"/>
-      <c r="X9" s="208"/>
-      <c r="Y9" s="208"/>
-      <c r="Z9" s="208"/>
-      <c r="AA9" s="208"/>
-      <c r="AB9" s="212"/>
-      <c r="AC9" s="212"/>
-      <c r="AD9" s="212"/>
-      <c r="AE9" s="212"/>
-      <c r="AF9" s="212"/>
-      <c r="AG9" s="212"/>
-      <c r="AH9" s="212"/>
-      <c r="AI9" s="212"/>
-      <c r="AJ9" s="212"/>
-      <c r="AK9" s="212"/>
-      <c r="AL9" s="212"/>
-      <c r="AM9" s="212"/>
-      <c r="AN9" s="212"/>
-      <c r="AO9" s="212"/>
-      <c r="AP9" s="212"/>
-      <c r="AQ9" s="212"/>
-      <c r="AR9" s="213"/>
-      <c r="AS9" s="213"/>
-      <c r="AT9" s="213"/>
-      <c r="AU9" s="214"/>
-      <c r="AV9" s="177"/>
-      <c r="AW9" s="177"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="197"/>
+      <c r="I9" s="197"/>
+      <c r="J9" s="197"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="190"/>
+      <c r="W9" s="189"/>
+      <c r="X9" s="189"/>
+      <c r="Y9" s="189"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="189"/>
+      <c r="AB9" s="187"/>
+      <c r="AC9" s="187"/>
+      <c r="AD9" s="187"/>
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="187"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
+      <c r="AU9" s="177"/>
+      <c r="AV9" s="191"/>
+      <c r="AW9" s="191"/>
       <c r="AX9" s="185"/>
-      <c r="AY9" s="186"/>
-      <c r="AZ9" s="186"/>
-      <c r="BA9" s="186"/>
-      <c r="BB9" s="186"/>
-      <c r="BC9" s="186"/>
-      <c r="BD9" s="186"/>
-      <c r="BE9" s="186"/>
-      <c r="BF9" s="188"/>
-      <c r="BG9" s="188"/>
-      <c r="BT9" s="177"/>
-      <c r="BW9" s="177"/>
-      <c r="CT9" s="177"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="191"/>
+      <c r="BW9" s="191"/>
+      <c r="CT9" s="191"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="176"/>
-      <c r="B10" s="178" t="s">
+      <c r="A10" s="198"/>
+      <c r="B10" s="199" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="178"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="206"/>
-      <c r="H10" s="206"/>
-      <c r="I10" s="206"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="206"/>
-      <c r="L10" s="207"/>
-      <c r="M10" s="207"/>
-      <c r="N10" s="207"/>
-      <c r="O10" s="207"/>
-      <c r="P10" s="207"/>
-      <c r="Q10" s="207"/>
-      <c r="R10" s="207"/>
-      <c r="S10" s="207"/>
-      <c r="T10" s="207"/>
-      <c r="U10" s="207"/>
-      <c r="V10" s="207"/>
-      <c r="W10" s="208"/>
-      <c r="X10" s="208"/>
-      <c r="Y10" s="208"/>
-      <c r="Z10" s="208"/>
-      <c r="AA10" s="208"/>
-      <c r="AB10" s="212"/>
-      <c r="AC10" s="212"/>
-      <c r="AD10" s="212"/>
-      <c r="AE10" s="212"/>
-      <c r="AF10" s="212"/>
-      <c r="AG10" s="212"/>
-      <c r="AH10" s="212"/>
-      <c r="AI10" s="212"/>
-      <c r="AJ10" s="212"/>
-      <c r="AK10" s="212"/>
-      <c r="AL10" s="212"/>
-      <c r="AM10" s="212"/>
-      <c r="AN10" s="212"/>
-      <c r="AO10" s="212"/>
-      <c r="AP10" s="212"/>
-      <c r="AQ10" s="212"/>
-      <c r="AR10" s="213"/>
-      <c r="AS10" s="213"/>
-      <c r="AT10" s="213"/>
-      <c r="AU10" s="214"/>
-      <c r="AV10" s="177"/>
-      <c r="AW10" s="177"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="197"/>
+      <c r="K10" s="197"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="190"/>
+      <c r="O10" s="190"/>
+      <c r="P10" s="190"/>
+      <c r="Q10" s="190"/>
+      <c r="R10" s="190"/>
+      <c r="S10" s="190"/>
+      <c r="T10" s="190"/>
+      <c r="U10" s="190"/>
+      <c r="V10" s="190"/>
+      <c r="W10" s="189"/>
+      <c r="X10" s="189"/>
+      <c r="Y10" s="189"/>
+      <c r="Z10" s="189"/>
+      <c r="AA10" s="189"/>
+      <c r="AB10" s="187"/>
+      <c r="AC10" s="187"/>
+      <c r="AD10" s="187"/>
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="187"/>
+      <c r="AG10" s="187"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
+      <c r="AU10" s="177"/>
+      <c r="AV10" s="191"/>
+      <c r="AW10" s="191"/>
       <c r="AX10" s="185"/>
-      <c r="AY10" s="186"/>
-      <c r="AZ10" s="186"/>
-      <c r="BA10" s="186"/>
-      <c r="BB10" s="186"/>
-      <c r="BC10" s="186"/>
-      <c r="BD10" s="186"/>
-      <c r="BE10" s="186"/>
-      <c r="BF10" s="188"/>
-      <c r="BG10" s="188"/>
-      <c r="BT10" s="177"/>
-      <c r="BW10" s="177"/>
-      <c r="CT10" s="177"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="191"/>
+      <c r="BW10" s="191"/>
+      <c r="CT10" s="191"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="176"/>
-      <c r="B11" s="178" t="s">
+      <c r="A11" s="198"/>
+      <c r="B11" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="206"/>
-      <c r="E11" s="206"/>
-      <c r="F11" s="206"/>
-      <c r="G11" s="206"/>
-      <c r="H11" s="206"/>
-      <c r="I11" s="206"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="206"/>
-      <c r="L11" s="207"/>
-      <c r="M11" s="207"/>
-      <c r="N11" s="207"/>
-      <c r="O11" s="207"/>
-      <c r="P11" s="207"/>
-      <c r="Q11" s="207"/>
-      <c r="R11" s="207"/>
-      <c r="S11" s="207"/>
-      <c r="T11" s="207"/>
-      <c r="U11" s="207"/>
-      <c r="V11" s="207"/>
-      <c r="W11" s="208"/>
-      <c r="X11" s="208"/>
-      <c r="Y11" s="208"/>
-      <c r="Z11" s="208"/>
-      <c r="AA11" s="208"/>
-      <c r="AB11" s="215"/>
-      <c r="AC11" s="215"/>
-      <c r="AD11" s="215"/>
-      <c r="AE11" s="215"/>
-      <c r="AF11" s="215"/>
-      <c r="AG11" s="215"/>
-      <c r="AH11" s="215"/>
-      <c r="AI11" s="215"/>
-      <c r="AJ11" s="215"/>
-      <c r="AK11" s="215"/>
-      <c r="AL11" s="215"/>
-      <c r="AM11" s="215"/>
-      <c r="AN11" s="215"/>
-      <c r="AO11" s="215"/>
-      <c r="AP11" s="215"/>
-      <c r="AQ11" s="215"/>
-      <c r="AR11" s="216"/>
-      <c r="AS11" s="216"/>
-      <c r="AT11" s="216"/>
-      <c r="AU11" s="214"/>
-      <c r="AV11" s="177"/>
-      <c r="AW11" s="177"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
+      <c r="N11" s="190"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="190"/>
+      <c r="Q11" s="190"/>
+      <c r="R11" s="190"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="190"/>
+      <c r="U11" s="190"/>
+      <c r="V11" s="190"/>
+      <c r="W11" s="189"/>
+      <c r="X11" s="189"/>
+      <c r="Y11" s="189"/>
+      <c r="Z11" s="189"/>
+      <c r="AA11" s="189"/>
+      <c r="AB11" s="188"/>
+      <c r="AC11" s="188"/>
+      <c r="AD11" s="188"/>
+      <c r="AE11" s="188"/>
+      <c r="AF11" s="188"/>
+      <c r="AG11" s="188"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
+      <c r="AU11" s="177"/>
+      <c r="AV11" s="191"/>
+      <c r="AW11" s="191"/>
       <c r="AX11" s="185"/>
-      <c r="AY11" s="186"/>
-      <c r="AZ11" s="186"/>
-      <c r="BA11" s="186"/>
-      <c r="BB11" s="186"/>
-      <c r="BC11" s="186"/>
-      <c r="BD11" s="186"/>
-      <c r="BE11" s="186"/>
-      <c r="BF11" s="188"/>
-      <c r="BG11" s="188"/>
-      <c r="BT11" s="177"/>
-      <c r="BW11" s="177"/>
-      <c r="CT11" s="177"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="191"/>
+      <c r="BW11" s="191"/>
+      <c r="CT11" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4251,22 +4232,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4276,7 +4282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -5124,7 +5130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5788,13 +5794,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="202" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="203"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5899,9 +5905,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="190"/>
-      <c r="B5" s="200"/>
-      <c r="C5" s="190"/>
+      <c r="A5" s="203"/>
+      <c r="B5" s="201"/>
+      <c r="C5" s="203"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -6006,11 +6012,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="190"/>
+      <c r="A6" s="203"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="190"/>
+      <c r="C6" s="203"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6115,11 +6121,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="190"/>
+      <c r="A7" s="203"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="190"/>
+      <c r="C7" s="203"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6224,11 +6230,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="190"/>
+      <c r="A8" s="203"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="190"/>
+      <c r="C8" s="203"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6333,11 +6339,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="190"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="190"/>
+      <c r="C9" s="203"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6442,11 +6448,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="190"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="190"/>
+      <c r="C10" s="203"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6551,11 +6557,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="190"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="190"/>
+      <c r="C11" s="203"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6660,9 +6666,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="190"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="191"/>
+      <c r="C12" s="206"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6767,10 +6773,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="204" t="s">
+      <c r="A13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="205" t="s">
+      <c r="B13" s="208" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6879,8 +6885,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="190"/>
-      <c r="B14" s="196"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -7001,7 +7007,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="190"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7111,7 +7117,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="190"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7221,7 +7227,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="190"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7333,7 +7339,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="190"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7443,7 +7449,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="190"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7553,7 +7559,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="190"/>
+      <c r="A20" s="203"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7663,7 +7669,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="191"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7774,7 +7780,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="199" t="s">
+      <c r="B22" s="200" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7884,7 +7890,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="200"/>
+      <c r="B23" s="201"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7991,13 +7997,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="192" t="s">
+      <c r="A24" s="211" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="194">
+      <c r="C24" s="213">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8105,11 +8111,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="193"/>
+      <c r="A25" s="212"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="190"/>
+      <c r="C25" s="203"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8215,11 +8221,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="193"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="190"/>
+      <c r="C26" s="203"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8325,11 +8331,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="193"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="190"/>
+      <c r="C27" s="203"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8435,11 +8441,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="193"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="190"/>
+      <c r="C28" s="203"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8545,11 +8551,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="193"/>
+      <c r="A29" s="212"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="190"/>
+      <c r="C29" s="203"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8655,11 +8661,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="193"/>
+      <c r="A30" s="212"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="190"/>
+      <c r="C30" s="203"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8765,11 +8771,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="193"/>
+      <c r="A31" s="212"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="190"/>
+      <c r="C31" s="203"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8875,11 +8881,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="193"/>
+      <c r="A32" s="212"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="190"/>
+      <c r="C32" s="203"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8985,11 +8991,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="193"/>
+      <c r="A33" s="212"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="190"/>
+      <c r="C33" s="203"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9095,11 +9101,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="193"/>
+      <c r="A34" s="212"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="190"/>
+      <c r="C34" s="203"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9205,11 +9211,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="193"/>
+      <c r="A35" s="212"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="191"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9315,11 +9321,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="193"/>
+      <c r="A36" s="212"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="194">
+      <c r="C36" s="213">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9427,11 +9433,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="193"/>
+      <c r="A37" s="212"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="190"/>
+      <c r="C37" s="203"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9537,11 +9543,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="193"/>
+      <c r="A38" s="212"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="190"/>
+      <c r="C38" s="203"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9647,11 +9653,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="193"/>
+      <c r="A39" s="212"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="190"/>
+      <c r="C39" s="203"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9757,11 +9763,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="193"/>
+      <c r="A40" s="212"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="190"/>
+      <c r="C40" s="203"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9867,11 +9873,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="193"/>
+      <c r="A41" s="212"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="190"/>
+      <c r="C41" s="203"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9977,11 +9983,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="193"/>
+      <c r="A42" s="212"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="190"/>
+      <c r="C42" s="203"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10087,11 +10093,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="193"/>
+      <c r="A43" s="212"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="190"/>
+      <c r="C43" s="203"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10197,11 +10203,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="193"/>
+      <c r="A44" s="212"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="190"/>
+      <c r="C44" s="203"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10307,11 +10313,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="193"/>
+      <c r="A45" s="212"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="190"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10417,11 +10423,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="193"/>
+      <c r="A46" s="212"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="190"/>
+      <c r="C46" s="203"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10527,11 +10533,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="193"/>
+      <c r="A47" s="212"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="190"/>
+      <c r="C47" s="203"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10645,11 +10651,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="193"/>
+      <c r="A48" s="212"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="190"/>
+      <c r="C48" s="203"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10758,7 +10764,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="195" t="s">
+      <c r="B49" s="214" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10868,7 +10874,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="196"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14299,7 +14305,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="197" t="s">
+      <c r="A81" s="215" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14411,7 +14417,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="190"/>
+      <c r="A82" s="203"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14521,7 +14527,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="190"/>
+      <c r="A83" s="203"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14631,7 +14637,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="190"/>
+      <c r="A84" s="203"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14741,7 +14747,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="190"/>
+      <c r="A85" s="203"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14851,7 +14857,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="190"/>
+      <c r="A86" s="203"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14961,7 +14967,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="190"/>
+      <c r="A87" s="203"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15073,7 +15079,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="190"/>
+      <c r="A88" s="203"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15183,7 +15189,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="190"/>
+      <c r="A89" s="203"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15293,7 +15299,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="190"/>
+      <c r="A90" s="203"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15403,11 +15409,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="190"/>
+      <c r="A91" s="203"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="198"/>
+      <c r="C91" s="216"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15513,11 +15519,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="190"/>
+      <c r="A92" s="203"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="190"/>
+      <c r="C92" s="203"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15623,11 +15629,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="191"/>
+      <c r="A93" s="206"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="190"/>
+      <c r="C93" s="203"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15851,7 +15857,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="189" t="s">
+      <c r="A95" s="210" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15963,7 +15969,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="190"/>
+      <c r="A96" s="203"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16073,7 +16079,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="190"/>
+      <c r="A97" s="203"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16183,7 +16189,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="190"/>
+      <c r="A98" s="203"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16293,7 +16299,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="190"/>
+      <c r="A99" s="203"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16403,7 +16409,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="190"/>
+      <c r="A100" s="203"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16513,7 +16519,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="190"/>
+      <c r="A101" s="203"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16623,7 +16629,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="190"/>
+      <c r="A102" s="203"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16733,7 +16739,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="190"/>
+      <c r="A103" s="203"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16845,7 +16851,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="190"/>
+      <c r="A104" s="203"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16955,7 +16961,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="190"/>
+      <c r="A105" s="203"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17073,7 +17079,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="190"/>
+      <c r="A106" s="203"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17183,7 +17189,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="190"/>
+      <c r="A107" s="203"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17293,7 +17299,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="190"/>
+      <c r="A108" s="203"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17403,7 +17409,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="190"/>
+      <c r="A109" s="203"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17513,7 +17519,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="190"/>
+      <c r="A110" s="203"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17623,7 +17629,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="190"/>
+      <c r="A111" s="203"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17733,7 +17739,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="190"/>
+      <c r="A112" s="203"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17843,7 +17849,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="190"/>
+      <c r="A113" s="203"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17953,7 +17959,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="190"/>
+      <c r="A114" s="203"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18063,7 +18069,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="190"/>
+      <c r="A115" s="203"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18173,7 +18179,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="190"/>
+      <c r="A116" s="203"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18299,7 +18305,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="190"/>
+      <c r="A117" s="203"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18409,7 +18415,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="191"/>
+      <c r="A118" s="206"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25780,12 +25786,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25793,6 +25793,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento realizado em 02-10
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AB610F-A5AD-4DB9-8C5F-F6AA54E03E7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C049A4F-14B8-4D14-BF16-2CFD508E857D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="179">
   <si>
     <t>S</t>
   </si>
@@ -742,6 +742,9 @@
   </si>
   <si>
     <t>Exercícios de programação orientada a objetos</t>
+  </si>
+  <si>
+    <t>Construtor e Lista</t>
   </si>
 </sst>
 </file>
@@ -2273,14 +2276,47 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2297,73 +2333,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2374,10 +2357,30 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2884,7 +2887,7 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AN4" sqref="AN4:AN11"/>
@@ -3196,110 +3199,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="192" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="192"/>
-      <c r="I2" s="192"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="192" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="192"/>
-      <c r="T2" s="192"/>
-      <c r="U2" s="192"/>
-      <c r="V2" s="192"/>
-      <c r="W2" s="192"/>
-      <c r="X2" s="192"/>
-      <c r="Y2" s="192"/>
-      <c r="Z2" s="192"/>
-      <c r="AA2" s="192"/>
-      <c r="AB2" s="192"/>
-      <c r="AC2" s="192"/>
-      <c r="AD2" s="192"/>
-      <c r="AE2" s="192"/>
-      <c r="AF2" s="192"/>
-      <c r="AG2" s="192"/>
-      <c r="AH2" s="192"/>
-      <c r="AI2" s="192"/>
-      <c r="AJ2" s="192"/>
-      <c r="AK2" s="192"/>
-      <c r="AL2" s="192"/>
-      <c r="AM2" s="192" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="192"/>
-      <c r="AO2" s="192"/>
-      <c r="AP2" s="192"/>
-      <c r="AQ2" s="192"/>
-      <c r="AR2" s="192"/>
-      <c r="AS2" s="192"/>
-      <c r="AT2" s="192"/>
-      <c r="AU2" s="192"/>
-      <c r="AV2" s="192"/>
-      <c r="AW2" s="192"/>
-      <c r="AX2" s="193"/>
-      <c r="AY2" s="193"/>
-      <c r="AZ2" s="193"/>
-      <c r="BA2" s="193"/>
-      <c r="BB2" s="193"/>
-      <c r="BC2" s="193"/>
-      <c r="BD2" s="193"/>
-      <c r="BE2" s="193"/>
-      <c r="BF2" s="193"/>
-      <c r="BG2" s="193"/>
-      <c r="BH2" s="193"/>
-      <c r="BI2" s="193"/>
-      <c r="BJ2" s="192" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="192"/>
-      <c r="BL2" s="192"/>
-      <c r="BM2" s="192"/>
-      <c r="BN2" s="192"/>
-      <c r="BO2" s="192"/>
-      <c r="BP2" s="192"/>
-      <c r="BQ2" s="192"/>
-      <c r="BR2" s="192"/>
-      <c r="BS2" s="192"/>
-      <c r="BT2" s="192"/>
-      <c r="BU2" s="192"/>
-      <c r="BV2" s="192"/>
-      <c r="BW2" s="192"/>
-      <c r="BX2" s="194"/>
-      <c r="BY2" s="194"/>
-      <c r="BZ2" s="194"/>
-      <c r="CA2" s="194"/>
-      <c r="CB2" s="194"/>
-      <c r="CC2" s="194"/>
-      <c r="CD2" s="194"/>
-      <c r="CE2" s="195" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="196"/>
-      <c r="CG2" s="196"/>
-      <c r="CH2" s="196"/>
-      <c r="CI2" s="196"/>
-      <c r="CJ2" s="196"/>
-      <c r="CK2" s="196"/>
-      <c r="CL2" s="196"/>
-      <c r="CM2" s="196"/>
-      <c r="CN2" s="196"/>
-      <c r="CO2" s="196"/>
-      <c r="CP2" s="196"/>
-      <c r="CQ2" s="196"/>
-      <c r="CR2" s="196"/>
-      <c r="CS2" s="196"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3595,611 +3598,670 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="199"/>
-      <c r="D4" s="197" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="197" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="197" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="197" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="197" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="197" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="197" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="190" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="190" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="190" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="190" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="190" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="190" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="190" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="190" t="s">
+      <c r="S4" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="190" t="s">
+      <c r="T4" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="190" t="s">
+      <c r="U4" s="187" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="190" t="s">
+      <c r="V4" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="189" t="s">
+      <c r="W4" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="189" t="s">
+      <c r="X4" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="189" t="s">
+      <c r="Y4" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="189" t="s">
+      <c r="Z4" s="188" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="189" t="s">
+      <c r="AA4" s="188" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="186" t="s">
+      <c r="AB4" s="189" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="186" t="s">
+      <c r="AC4" s="189" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="186" t="s">
+      <c r="AD4" s="189" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="186" t="s">
+      <c r="AE4" s="189" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="186" t="s">
+      <c r="AF4" s="189" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="186" t="s">
+      <c r="AG4" s="189" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="186" t="s">
+      <c r="AH4" s="189" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="186" t="s">
+      <c r="AI4" s="189" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="186" t="s">
+      <c r="AJ4" s="189" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="186" t="s">
+      <c r="AK4" s="189" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" s="186" t="s">
+      <c r="AL4" s="189" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" s="186" t="s">
+      <c r="AM4" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="186"/>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="AN4" s="189" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO4" s="189"/>
+      <c r="AP4" s="189"/>
+      <c r="AQ4" s="189"/>
+      <c r="AR4" s="192"/>
+      <c r="AS4" s="192"/>
+      <c r="AT4" s="192"/>
       <c r="AU4" s="176"/>
-      <c r="AV4" s="191"/>
-      <c r="AW4" s="191"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="191"/>
-      <c r="BW4" s="191"/>
-      <c r="CT4" s="191"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="195"/>
+      <c r="AY4" s="197"/>
+      <c r="AZ4" s="197"/>
+      <c r="BA4" s="197"/>
+      <c r="BB4" s="197"/>
+      <c r="BC4" s="197"/>
+      <c r="BD4" s="197"/>
+      <c r="BE4" s="197"/>
+      <c r="BF4" s="198"/>
+      <c r="BG4" s="198"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="198"/>
-      <c r="B5" s="199" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="197"/>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197"/>
-      <c r="I5" s="197"/>
-      <c r="J5" s="197"/>
-      <c r="K5" s="197"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
-      <c r="N5" s="190"/>
-      <c r="O5" s="190"/>
-      <c r="P5" s="190"/>
-      <c r="Q5" s="190"/>
-      <c r="R5" s="190"/>
-      <c r="S5" s="190"/>
-      <c r="T5" s="190"/>
-      <c r="U5" s="190"/>
-      <c r="V5" s="190"/>
-      <c r="W5" s="189"/>
-      <c r="X5" s="189"/>
-      <c r="Y5" s="189"/>
-      <c r="Z5" s="189"/>
-      <c r="AA5" s="189"/>
-      <c r="AB5" s="187"/>
-      <c r="AC5" s="187"/>
-      <c r="AD5" s="187"/>
-      <c r="AE5" s="187"/>
-      <c r="AF5" s="187"/>
-      <c r="AG5" s="187"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="190"/>
+      <c r="AC5" s="190"/>
+      <c r="AD5" s="190"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="190"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="190"/>
+      <c r="AK5" s="190"/>
+      <c r="AL5" s="190"/>
+      <c r="AM5" s="190"/>
+      <c r="AN5" s="190"/>
+      <c r="AO5" s="190"/>
+      <c r="AP5" s="190"/>
+      <c r="AQ5" s="190"/>
+      <c r="AR5" s="193"/>
+      <c r="AS5" s="193"/>
+      <c r="AT5" s="193"/>
       <c r="AU5" s="176"/>
-      <c r="AV5" s="191"/>
-      <c r="AW5" s="191"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="191"/>
-      <c r="BW5" s="191"/>
-      <c r="CT5" s="191"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="196"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="197"/>
+      <c r="BA5" s="197"/>
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="199"/>
+      <c r="BG5" s="199"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="199"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="197"/>
-      <c r="H6" s="197"/>
-      <c r="I6" s="197"/>
-      <c r="J6" s="197"/>
-      <c r="K6" s="197"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
-      <c r="N6" s="190"/>
-      <c r="O6" s="190"/>
-      <c r="P6" s="190"/>
-      <c r="Q6" s="190"/>
-      <c r="R6" s="190"/>
-      <c r="S6" s="190"/>
-      <c r="T6" s="190"/>
-      <c r="U6" s="190"/>
-      <c r="V6" s="190"/>
-      <c r="W6" s="189"/>
-      <c r="X6" s="189"/>
-      <c r="Y6" s="189"/>
-      <c r="Z6" s="189"/>
-      <c r="AA6" s="189"/>
-      <c r="AB6" s="187"/>
-      <c r="AC6" s="187"/>
-      <c r="AD6" s="187"/>
-      <c r="AE6" s="187"/>
-      <c r="AF6" s="187"/>
-      <c r="AG6" s="187"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
+      <c r="AB6" s="190"/>
+      <c r="AC6" s="190"/>
+      <c r="AD6" s="190"/>
+      <c r="AE6" s="190"/>
+      <c r="AF6" s="190"/>
+      <c r="AG6" s="190"/>
+      <c r="AH6" s="190"/>
+      <c r="AI6" s="190"/>
+      <c r="AJ6" s="190"/>
+      <c r="AK6" s="190"/>
+      <c r="AL6" s="190"/>
+      <c r="AM6" s="190"/>
+      <c r="AN6" s="190"/>
+      <c r="AO6" s="190"/>
+      <c r="AP6" s="190"/>
+      <c r="AQ6" s="190"/>
+      <c r="AR6" s="193"/>
+      <c r="AS6" s="193"/>
+      <c r="AT6" s="193"/>
       <c r="AU6" s="176"/>
-      <c r="AV6" s="191"/>
-      <c r="AW6" s="191"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="191"/>
-      <c r="BW6" s="191"/>
-      <c r="CT6" s="191"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="199"/>
+      <c r="BG6" s="199"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="198"/>
-      <c r="B7" s="199" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="197"/>
-      <c r="F7" s="197"/>
-      <c r="G7" s="197"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="197"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="197"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="190"/>
-      <c r="N7" s="190"/>
-      <c r="O7" s="190"/>
-      <c r="P7" s="190"/>
-      <c r="Q7" s="190"/>
-      <c r="R7" s="190"/>
-      <c r="S7" s="190"/>
-      <c r="T7" s="190"/>
-      <c r="U7" s="190"/>
-      <c r="V7" s="190"/>
-      <c r="W7" s="189"/>
-      <c r="X7" s="189"/>
-      <c r="Y7" s="189"/>
-      <c r="Z7" s="189"/>
-      <c r="AA7" s="189"/>
-      <c r="AB7" s="187"/>
-      <c r="AC7" s="187"/>
-      <c r="AD7" s="187"/>
-      <c r="AE7" s="187"/>
-      <c r="AF7" s="187"/>
-      <c r="AG7" s="187"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
+      <c r="AB7" s="190"/>
+      <c r="AC7" s="190"/>
+      <c r="AD7" s="190"/>
+      <c r="AE7" s="190"/>
+      <c r="AF7" s="190"/>
+      <c r="AG7" s="190"/>
+      <c r="AH7" s="190"/>
+      <c r="AI7" s="190"/>
+      <c r="AJ7" s="190"/>
+      <c r="AK7" s="190"/>
+      <c r="AL7" s="190"/>
+      <c r="AM7" s="190"/>
+      <c r="AN7" s="190"/>
+      <c r="AO7" s="190"/>
+      <c r="AP7" s="190"/>
+      <c r="AQ7" s="190"/>
+      <c r="AR7" s="193"/>
+      <c r="AS7" s="193"/>
+      <c r="AT7" s="193"/>
       <c r="AU7" s="177"/>
-      <c r="AV7" s="191"/>
-      <c r="AW7" s="191"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="191"/>
-      <c r="BW7" s="191"/>
-      <c r="CT7" s="191"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="196"/>
+      <c r="AY7" s="197"/>
+      <c r="AZ7" s="197"/>
+      <c r="BA7" s="197"/>
+      <c r="BB7" s="197"/>
+      <c r="BC7" s="197"/>
+      <c r="BD7" s="197"/>
+      <c r="BE7" s="197"/>
+      <c r="BF7" s="199"/>
+      <c r="BG7" s="199"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="198" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="199" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="199"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="197"/>
-      <c r="K8" s="197"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="190"/>
-      <c r="N8" s="190"/>
-      <c r="O8" s="190"/>
-      <c r="P8" s="190"/>
-      <c r="Q8" s="190"/>
-      <c r="R8" s="190"/>
-      <c r="S8" s="190"/>
-      <c r="T8" s="190"/>
-      <c r="U8" s="190"/>
-      <c r="V8" s="190"/>
-      <c r="W8" s="189"/>
-      <c r="X8" s="189"/>
-      <c r="Y8" s="189"/>
-      <c r="Z8" s="189"/>
-      <c r="AA8" s="189"/>
-      <c r="AB8" s="187"/>
-      <c r="AC8" s="187"/>
-      <c r="AD8" s="187"/>
-      <c r="AE8" s="187"/>
-      <c r="AF8" s="187"/>
-      <c r="AG8" s="187"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
+      <c r="AB8" s="190"/>
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="190"/>
+      <c r="AG8" s="190"/>
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="190"/>
+      <c r="AL8" s="190"/>
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="190"/>
+      <c r="AQ8" s="190"/>
+      <c r="AR8" s="193"/>
+      <c r="AS8" s="193"/>
+      <c r="AT8" s="193"/>
       <c r="AU8" s="177"/>
-      <c r="AV8" s="191"/>
-      <c r="AW8" s="191"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="191"/>
-      <c r="BW8" s="191"/>
-      <c r="CT8" s="191"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="196"/>
+      <c r="AY8" s="197"/>
+      <c r="AZ8" s="197"/>
+      <c r="BA8" s="197"/>
+      <c r="BB8" s="197"/>
+      <c r="BC8" s="197"/>
+      <c r="BD8" s="197"/>
+      <c r="BE8" s="197"/>
+      <c r="BF8" s="199"/>
+      <c r="BG8" s="199"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="198"/>
-      <c r="B9" s="199" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="199"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="190"/>
-      <c r="M9" s="190"/>
-      <c r="N9" s="190"/>
-      <c r="O9" s="190"/>
-      <c r="P9" s="190"/>
-      <c r="Q9" s="190"/>
-      <c r="R9" s="190"/>
-      <c r="S9" s="190"/>
-      <c r="T9" s="190"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="190"/>
-      <c r="W9" s="189"/>
-      <c r="X9" s="189"/>
-      <c r="Y9" s="189"/>
-      <c r="Z9" s="189"/>
-      <c r="AA9" s="189"/>
-      <c r="AB9" s="187"/>
-      <c r="AC9" s="187"/>
-      <c r="AD9" s="187"/>
-      <c r="AE9" s="187"/>
-      <c r="AF9" s="187"/>
-      <c r="AG9" s="187"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="190"/>
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="190"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="190"/>
+      <c r="AL9" s="190"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="190"/>
+      <c r="AR9" s="193"/>
+      <c r="AS9" s="193"/>
+      <c r="AT9" s="193"/>
       <c r="AU9" s="177"/>
-      <c r="AV9" s="191"/>
-      <c r="AW9" s="191"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="191"/>
-      <c r="BW9" s="191"/>
-      <c r="CT9" s="191"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="196"/>
+      <c r="AY9" s="197"/>
+      <c r="AZ9" s="197"/>
+      <c r="BA9" s="197"/>
+      <c r="BB9" s="197"/>
+      <c r="BC9" s="197"/>
+      <c r="BD9" s="197"/>
+      <c r="BE9" s="197"/>
+      <c r="BF9" s="199"/>
+      <c r="BG9" s="199"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="199"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
-      <c r="J10" s="197"/>
-      <c r="K10" s="197"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="190"/>
-      <c r="N10" s="190"/>
-      <c r="O10" s="190"/>
-      <c r="P10" s="190"/>
-      <c r="Q10" s="190"/>
-      <c r="R10" s="190"/>
-      <c r="S10" s="190"/>
-      <c r="T10" s="190"/>
-      <c r="U10" s="190"/>
-      <c r="V10" s="190"/>
-      <c r="W10" s="189"/>
-      <c r="X10" s="189"/>
-      <c r="Y10" s="189"/>
-      <c r="Z10" s="189"/>
-      <c r="AA10" s="189"/>
-      <c r="AB10" s="187"/>
-      <c r="AC10" s="187"/>
-      <c r="AD10" s="187"/>
-      <c r="AE10" s="187"/>
-      <c r="AF10" s="187"/>
-      <c r="AG10" s="187"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
+      <c r="AB10" s="190"/>
+      <c r="AC10" s="190"/>
+      <c r="AD10" s="190"/>
+      <c r="AE10" s="190"/>
+      <c r="AF10" s="190"/>
+      <c r="AG10" s="190"/>
+      <c r="AH10" s="190"/>
+      <c r="AI10" s="190"/>
+      <c r="AJ10" s="190"/>
+      <c r="AK10" s="190"/>
+      <c r="AL10" s="190"/>
+      <c r="AM10" s="190"/>
+      <c r="AN10" s="190"/>
+      <c r="AO10" s="190"/>
+      <c r="AP10" s="190"/>
+      <c r="AQ10" s="190"/>
+      <c r="AR10" s="193"/>
+      <c r="AS10" s="193"/>
+      <c r="AT10" s="193"/>
       <c r="AU10" s="177"/>
-      <c r="AV10" s="191"/>
-      <c r="AW10" s="191"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="191"/>
-      <c r="BW10" s="191"/>
-      <c r="CT10" s="191"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="196"/>
+      <c r="AY10" s="197"/>
+      <c r="AZ10" s="197"/>
+      <c r="BA10" s="197"/>
+      <c r="BB10" s="197"/>
+      <c r="BC10" s="197"/>
+      <c r="BD10" s="197"/>
+      <c r="BE10" s="197"/>
+      <c r="BF10" s="199"/>
+      <c r="BG10" s="199"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="198"/>
-      <c r="B11" s="199" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="197"/>
-      <c r="J11" s="197"/>
-      <c r="K11" s="197"/>
-      <c r="L11" s="190"/>
-      <c r="M11" s="190"/>
-      <c r="N11" s="190"/>
-      <c r="O11" s="190"/>
-      <c r="P11" s="190"/>
-      <c r="Q11" s="190"/>
-      <c r="R11" s="190"/>
-      <c r="S11" s="190"/>
-      <c r="T11" s="190"/>
-      <c r="U11" s="190"/>
-      <c r="V11" s="190"/>
-      <c r="W11" s="189"/>
-      <c r="X11" s="189"/>
-      <c r="Y11" s="189"/>
-      <c r="Z11" s="189"/>
-      <c r="AA11" s="189"/>
-      <c r="AB11" s="188"/>
-      <c r="AC11" s="188"/>
-      <c r="AD11" s="188"/>
-      <c r="AE11" s="188"/>
-      <c r="AF11" s="188"/>
-      <c r="AG11" s="188"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
+      <c r="AB11" s="191"/>
+      <c r="AC11" s="191"/>
+      <c r="AD11" s="191"/>
+      <c r="AE11" s="191"/>
+      <c r="AF11" s="191"/>
+      <c r="AG11" s="191"/>
+      <c r="AH11" s="191"/>
+      <c r="AI11" s="191"/>
+      <c r="AJ11" s="191"/>
+      <c r="AK11" s="191"/>
+      <c r="AL11" s="191"/>
+      <c r="AM11" s="191"/>
+      <c r="AN11" s="191"/>
+      <c r="AO11" s="191"/>
+      <c r="AP11" s="191"/>
+      <c r="AQ11" s="191"/>
+      <c r="AR11" s="194"/>
+      <c r="AS11" s="194"/>
+      <c r="AT11" s="194"/>
       <c r="AU11" s="177"/>
-      <c r="AV11" s="191"/>
-      <c r="AW11" s="191"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="191"/>
-      <c r="BW11" s="191"/>
-      <c r="CT11" s="191"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="196"/>
+      <c r="AY11" s="197"/>
+      <c r="AZ11" s="197"/>
+      <c r="BA11" s="197"/>
+      <c r="BB11" s="197"/>
+      <c r="BC11" s="197"/>
+      <c r="BD11" s="197"/>
+      <c r="BE11" s="197"/>
+      <c r="BF11" s="199"/>
+      <c r="BG11" s="199"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4216,63 +4278,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5794,13 +5799,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="213" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="214"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5905,9 +5910,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="203"/>
-      <c r="B5" s="201"/>
-      <c r="C5" s="203"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="211"/>
+      <c r="C5" s="201"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -6012,11 +6017,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="203"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="203"/>
+      <c r="C6" s="201"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6121,11 +6126,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="203"/>
+      <c r="A7" s="201"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="203"/>
+      <c r="C7" s="201"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6230,11 +6235,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="203"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="203"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6339,11 +6344,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="203"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="203"/>
+      <c r="C9" s="201"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6448,11 +6453,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="203"/>
+      <c r="A10" s="201"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="203"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6557,11 +6562,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="203"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="203"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6666,9 +6671,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="203"/>
+      <c r="A12" s="201"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="206"/>
+      <c r="C12" s="202"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6773,10 +6778,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="207" t="s">
+      <c r="A13" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="208" t="s">
+      <c r="B13" s="216" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6885,8 +6890,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="203"/>
-      <c r="B14" s="209"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="207"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -7007,7 +7012,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="203"/>
+      <c r="A15" s="201"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7117,7 +7122,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="203"/>
+      <c r="A16" s="201"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7227,7 +7232,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="203"/>
+      <c r="A17" s="201"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7339,7 +7344,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203"/>
+      <c r="A18" s="201"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7449,7 +7454,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203"/>
+      <c r="A19" s="201"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7559,7 +7564,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="203"/>
+      <c r="A20" s="201"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7669,7 +7674,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="206"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7780,7 +7785,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="210" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7890,7 +7895,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="201"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -7997,13 +8002,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="203" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="213">
+      <c r="C24" s="205">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8111,11 +8116,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="212"/>
+      <c r="A25" s="204"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="203"/>
+      <c r="C25" s="201"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8221,11 +8226,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="212"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="203"/>
+      <c r="C26" s="201"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8331,11 +8336,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="212"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="203"/>
+      <c r="C27" s="201"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8441,11 +8446,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="212"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="203"/>
+      <c r="C28" s="201"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8551,11 +8556,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="212"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="203"/>
+      <c r="C29" s="201"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8661,11 +8666,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="212"/>
+      <c r="A30" s="204"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="203"/>
+      <c r="C30" s="201"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8771,11 +8776,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="212"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="203"/>
+      <c r="C31" s="201"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8881,11 +8886,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="212"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="203"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8991,11 +8996,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="212"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="203"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9101,11 +9106,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="212"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="203"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9211,11 +9216,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="212"/>
+      <c r="A35" s="204"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="206"/>
+      <c r="C35" s="202"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9321,11 +9326,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="212"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="213">
+      <c r="C36" s="205">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9433,11 +9438,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="212"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="203"/>
+      <c r="C37" s="201"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9543,11 +9548,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="212"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="203"/>
+      <c r="C38" s="201"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9653,11 +9658,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="212"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="203"/>
+      <c r="C39" s="201"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9763,11 +9768,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="212"/>
+      <c r="A40" s="204"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="203"/>
+      <c r="C40" s="201"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9873,11 +9878,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="212"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="203"/>
+      <c r="C41" s="201"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9983,11 +9988,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="212"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="203"/>
+      <c r="C42" s="201"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10093,11 +10098,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="212"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="203"/>
+      <c r="C43" s="201"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10203,11 +10208,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="212"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="203"/>
+      <c r="C44" s="201"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10313,11 +10318,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="212"/>
+      <c r="A45" s="204"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="203"/>
+      <c r="C45" s="201"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10423,11 +10428,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="212"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="203"/>
+      <c r="C46" s="201"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10533,11 +10538,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="212"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="203"/>
+      <c r="C47" s="201"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10651,11 +10656,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="212"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="203"/>
+      <c r="C48" s="201"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10764,7 +10769,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="214" t="s">
+      <c r="B49" s="206" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10874,7 +10879,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="209"/>
+      <c r="B50" s="207"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14305,7 +14310,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="215" t="s">
+      <c r="A81" s="208" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14417,7 +14422,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="203"/>
+      <c r="A82" s="201"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14527,7 +14532,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="203"/>
+      <c r="A83" s="201"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14637,7 +14642,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="203"/>
+      <c r="A84" s="201"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14747,7 +14752,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="203"/>
+      <c r="A85" s="201"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14857,7 +14862,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="203"/>
+      <c r="A86" s="201"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14967,7 +14972,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="203"/>
+      <c r="A87" s="201"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15079,7 +15084,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="203"/>
+      <c r="A88" s="201"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15189,7 +15194,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="203"/>
+      <c r="A89" s="201"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15299,7 +15304,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="203"/>
+      <c r="A90" s="201"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15409,11 +15414,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="203"/>
+      <c r="A91" s="201"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="216"/>
+      <c r="C91" s="209"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15519,11 +15524,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="203"/>
+      <c r="A92" s="201"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="203"/>
+      <c r="C92" s="201"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15629,11 +15634,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="206"/>
+      <c r="A93" s="202"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="203"/>
+      <c r="C93" s="201"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15857,7 +15862,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="210" t="s">
+      <c r="A95" s="200" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15969,7 +15974,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="203"/>
+      <c r="A96" s="201"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16079,7 +16084,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="203"/>
+      <c r="A97" s="201"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16189,7 +16194,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="203"/>
+      <c r="A98" s="201"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16299,7 +16304,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="203"/>
+      <c r="A99" s="201"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16409,7 +16414,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="203"/>
+      <c r="A100" s="201"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16519,7 +16524,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="203"/>
+      <c r="A101" s="201"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16629,7 +16634,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="203"/>
+      <c r="A102" s="201"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16739,7 +16744,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="203"/>
+      <c r="A103" s="201"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16851,7 +16856,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="203"/>
+      <c r="A104" s="201"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16961,7 +16966,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="203"/>
+      <c r="A105" s="201"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17079,7 +17084,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="203"/>
+      <c r="A106" s="201"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17189,7 +17194,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="203"/>
+      <c r="A107" s="201"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17299,7 +17304,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="203"/>
+      <c r="A108" s="201"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17409,7 +17414,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="203"/>
+      <c r="A109" s="201"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17519,7 +17524,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="203"/>
+      <c r="A110" s="201"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17629,7 +17634,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="203"/>
+      <c r="A111" s="201"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17739,7 +17744,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="203"/>
+      <c r="A112" s="201"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17849,7 +17854,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="203"/>
+      <c r="A113" s="201"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17959,7 +17964,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="203"/>
+      <c r="A114" s="201"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18069,7 +18074,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="203"/>
+      <c r="A115" s="201"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18179,7 +18184,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="203"/>
+      <c r="A116" s="201"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18305,7 +18310,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="203"/>
+      <c r="A117" s="201"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18415,7 +18420,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="206"/>
+      <c r="A118" s="202"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25786,6 +25791,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25793,12 +25804,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 03-10
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C049A4F-14B8-4D14-BF16-2CFD508E857D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FA92A5-6973-4A37-A6D7-8D0BBE22FFDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="180">
   <si>
     <t>S</t>
   </si>
@@ -745,6 +745,10 @@
   </si>
   <si>
     <t>Construtor e Lista</t>
+  </si>
+  <si>
+    <t>Correção do exercício Vingadores.
+Ajustes nas páginas para apresentação à Linx.</t>
   </si>
 </sst>
 </file>
@@ -2276,17 +2280,47 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2303,50 +2337,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2357,30 +2381,10 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2890,7 +2894,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AN4" sqref="AN4:AN11"/>
+      <selection pane="bottomRight" activeCell="AP4" sqref="AP4:AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3199,110 +3203,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="192"/>
+      <c r="I2" s="192"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
+      <c r="AF2" s="192"/>
+      <c r="AG2" s="192"/>
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="192"/>
+      <c r="AJ2" s="192"/>
+      <c r="AK2" s="192"/>
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="192"/>
+      <c r="AQ2" s="192"/>
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="192"/>
+      <c r="AT2" s="192"/>
+      <c r="AU2" s="192"/>
+      <c r="AV2" s="192"/>
+      <c r="AW2" s="192"/>
+      <c r="AX2" s="193"/>
+      <c r="AY2" s="193"/>
+      <c r="AZ2" s="193"/>
+      <c r="BA2" s="193"/>
+      <c r="BB2" s="193"/>
+      <c r="BC2" s="193"/>
+      <c r="BD2" s="193"/>
+      <c r="BE2" s="193"/>
+      <c r="BF2" s="193"/>
+      <c r="BG2" s="193"/>
+      <c r="BH2" s="193"/>
+      <c r="BI2" s="193"/>
+      <c r="BJ2" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="192"/>
+      <c r="BL2" s="192"/>
+      <c r="BM2" s="192"/>
+      <c r="BN2" s="192"/>
+      <c r="BO2" s="192"/>
+      <c r="BP2" s="192"/>
+      <c r="BQ2" s="192"/>
+      <c r="BR2" s="192"/>
+      <c r="BS2" s="192"/>
+      <c r="BT2" s="192"/>
+      <c r="BU2" s="192"/>
+      <c r="BV2" s="192"/>
+      <c r="BW2" s="192"/>
+      <c r="BX2" s="194"/>
+      <c r="BY2" s="194"/>
+      <c r="BZ2" s="194"/>
+      <c r="CA2" s="194"/>
+      <c r="CB2" s="194"/>
+      <c r="CC2" s="194"/>
+      <c r="CD2" s="194"/>
+      <c r="CE2" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="196"/>
+      <c r="CG2" s="196"/>
+      <c r="CH2" s="196"/>
+      <c r="CI2" s="196"/>
+      <c r="CJ2" s="196"/>
+      <c r="CK2" s="196"/>
+      <c r="CL2" s="196"/>
+      <c r="CM2" s="196"/>
+      <c r="CN2" s="196"/>
+      <c r="CO2" s="196"/>
+      <c r="CP2" s="196"/>
+      <c r="CQ2" s="196"/>
+      <c r="CR2" s="196"/>
+      <c r="CS2" s="196"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3598,654 +3602,631 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="198" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="199"/>
+      <c r="D4" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="197" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="197" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="197" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="197" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="197" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="197" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="197" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="190" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="190" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="190" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="190" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="190" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="190" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="190" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="190" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188" t="s">
+      <c r="X4" s="189" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="188" t="s">
+      <c r="Y4" s="189" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="188" t="s">
+      <c r="Z4" s="189" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="188" t="s">
+      <c r="AA4" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="189" t="s">
+      <c r="AB4" s="186" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="189" t="s">
+      <c r="AC4" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="189" t="s">
+      <c r="AD4" s="186" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="189" t="s">
+      <c r="AE4" s="186" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="189" t="s">
+      <c r="AF4" s="186" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="189" t="s">
+      <c r="AG4" s="186" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="189" t="s">
+      <c r="AH4" s="186" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="189" t="s">
+      <c r="AI4" s="186" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="189" t="s">
+      <c r="AJ4" s="186" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="189" t="s">
+      <c r="AK4" s="186" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" s="189" t="s">
+      <c r="AL4" s="186" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" s="189" t="s">
+      <c r="AM4" s="186" t="s">
         <v>177</v>
       </c>
-      <c r="AN4" s="189" t="s">
+      <c r="AN4" s="186" t="s">
         <v>178</v>
       </c>
-      <c r="AO4" s="189"/>
-      <c r="AP4" s="189"/>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
+      <c r="AO4" s="186" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="181"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="181"/>
       <c r="AU4" s="176"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="195"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="198"/>
-      <c r="BG4" s="198"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
+      <c r="AV4" s="191"/>
+      <c r="AW4" s="191"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="180"/>
+      <c r="BA4" s="180"/>
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="178"/>
+      <c r="BT4" s="191"/>
+      <c r="BW4" s="191"/>
+      <c r="CT4" s="191"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="A5" s="198"/>
+      <c r="B5" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="190"/>
-      <c r="AC5" s="190"/>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="190"/>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="190"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="190"/>
-      <c r="AP5" s="190"/>
-      <c r="AQ5" s="190"/>
-      <c r="AR5" s="193"/>
-      <c r="AS5" s="193"/>
-      <c r="AT5" s="193"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="197"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="197"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="190"/>
+      <c r="P5" s="190"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="190"/>
+      <c r="S5" s="190"/>
+      <c r="T5" s="190"/>
+      <c r="U5" s="190"/>
+      <c r="V5" s="190"/>
+      <c r="W5" s="189"/>
+      <c r="X5" s="189"/>
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="189"/>
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="187"/>
+      <c r="AC5" s="187"/>
+      <c r="AD5" s="187"/>
+      <c r="AE5" s="187"/>
+      <c r="AF5" s="187"/>
+      <c r="AG5" s="187"/>
+      <c r="AH5" s="187"/>
+      <c r="AI5" s="187"/>
+      <c r="AJ5" s="187"/>
+      <c r="AK5" s="187"/>
+      <c r="AL5" s="187"/>
+      <c r="AM5" s="187"/>
+      <c r="AN5" s="187"/>
+      <c r="AO5" s="187"/>
+      <c r="AP5" s="187"/>
+      <c r="AQ5" s="187"/>
+      <c r="AR5" s="182"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="182"/>
       <c r="AU5" s="176"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="196"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="197"/>
-      <c r="BA5" s="197"/>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="199"/>
-      <c r="BG5" s="199"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
+      <c r="AV5" s="191"/>
+      <c r="AW5" s="191"/>
+      <c r="AX5" s="185"/>
+      <c r="AY5" s="180"/>
+      <c r="AZ5" s="180"/>
+      <c r="BA5" s="180"/>
+      <c r="BB5" s="180"/>
+      <c r="BC5" s="180"/>
+      <c r="BD5" s="180"/>
+      <c r="BE5" s="180"/>
+      <c r="BF5" s="179"/>
+      <c r="BG5" s="179"/>
+      <c r="BT5" s="191"/>
+      <c r="BW5" s="191"/>
+      <c r="CT5" s="191"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="A6" s="198"/>
+      <c r="B6" s="199" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="190"/>
-      <c r="AC6" s="190"/>
-      <c r="AD6" s="190"/>
-      <c r="AE6" s="190"/>
-      <c r="AF6" s="190"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="190"/>
-      <c r="AI6" s="190"/>
-      <c r="AJ6" s="190"/>
-      <c r="AK6" s="190"/>
-      <c r="AL6" s="190"/>
-      <c r="AM6" s="190"/>
-      <c r="AN6" s="190"/>
-      <c r="AO6" s="190"/>
-      <c r="AP6" s="190"/>
-      <c r="AQ6" s="190"/>
-      <c r="AR6" s="193"/>
-      <c r="AS6" s="193"/>
-      <c r="AT6" s="193"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="N6" s="190"/>
+      <c r="O6" s="190"/>
+      <c r="P6" s="190"/>
+      <c r="Q6" s="190"/>
+      <c r="R6" s="190"/>
+      <c r="S6" s="190"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="190"/>
+      <c r="V6" s="190"/>
+      <c r="W6" s="189"/>
+      <c r="X6" s="189"/>
+      <c r="Y6" s="189"/>
+      <c r="Z6" s="189"/>
+      <c r="AA6" s="189"/>
+      <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
+      <c r="AD6" s="187"/>
+      <c r="AE6" s="187"/>
+      <c r="AF6" s="187"/>
+      <c r="AG6" s="187"/>
+      <c r="AH6" s="187"/>
+      <c r="AI6" s="187"/>
+      <c r="AJ6" s="187"/>
+      <c r="AK6" s="187"/>
+      <c r="AL6" s="187"/>
+      <c r="AM6" s="187"/>
+      <c r="AN6" s="187"/>
+      <c r="AO6" s="187"/>
+      <c r="AP6" s="187"/>
+      <c r="AQ6" s="187"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="182"/>
       <c r="AU6" s="176"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="197"/>
-      <c r="AZ6" s="197"/>
-      <c r="BA6" s="197"/>
-      <c r="BB6" s="197"/>
-      <c r="BC6" s="197"/>
-      <c r="BD6" s="197"/>
-      <c r="BE6" s="197"/>
-      <c r="BF6" s="199"/>
-      <c r="BG6" s="199"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
+      <c r="AV6" s="191"/>
+      <c r="AW6" s="191"/>
+      <c r="AX6" s="185"/>
+      <c r="AY6" s="180"/>
+      <c r="AZ6" s="180"/>
+      <c r="BA6" s="180"/>
+      <c r="BB6" s="180"/>
+      <c r="BC6" s="180"/>
+      <c r="BD6" s="180"/>
+      <c r="BE6" s="180"/>
+      <c r="BF6" s="179"/>
+      <c r="BG6" s="179"/>
+      <c r="BT6" s="191"/>
+      <c r="BW6" s="191"/>
+      <c r="CT6" s="191"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="A7" s="198"/>
+      <c r="B7" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="190"/>
-      <c r="AC7" s="190"/>
-      <c r="AD7" s="190"/>
-      <c r="AE7" s="190"/>
-      <c r="AF7" s="190"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="190"/>
-      <c r="AI7" s="190"/>
-      <c r="AJ7" s="190"/>
-      <c r="AK7" s="190"/>
-      <c r="AL7" s="190"/>
-      <c r="AM7" s="190"/>
-      <c r="AN7" s="190"/>
-      <c r="AO7" s="190"/>
-      <c r="AP7" s="190"/>
-      <c r="AQ7" s="190"/>
-      <c r="AR7" s="193"/>
-      <c r="AS7" s="193"/>
-      <c r="AT7" s="193"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="197"/>
+      <c r="F7" s="197"/>
+      <c r="G7" s="197"/>
+      <c r="H7" s="197"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="197"/>
+      <c r="K7" s="197"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
+      <c r="Q7" s="190"/>
+      <c r="R7" s="190"/>
+      <c r="S7" s="190"/>
+      <c r="T7" s="190"/>
+      <c r="U7" s="190"/>
+      <c r="V7" s="190"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="189"/>
+      <c r="Y7" s="189"/>
+      <c r="Z7" s="189"/>
+      <c r="AA7" s="189"/>
+      <c r="AB7" s="187"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="187"/>
+      <c r="AP7" s="187"/>
+      <c r="AQ7" s="187"/>
+      <c r="AR7" s="182"/>
+      <c r="AS7" s="182"/>
+      <c r="AT7" s="182"/>
       <c r="AU7" s="177"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="196"/>
-      <c r="AY7" s="197"/>
-      <c r="AZ7" s="197"/>
-      <c r="BA7" s="197"/>
-      <c r="BB7" s="197"/>
-      <c r="BC7" s="197"/>
-      <c r="BD7" s="197"/>
-      <c r="BE7" s="197"/>
-      <c r="BF7" s="199"/>
-      <c r="BG7" s="199"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
+      <c r="AV7" s="191"/>
+      <c r="AW7" s="191"/>
+      <c r="AX7" s="185"/>
+      <c r="AY7" s="180"/>
+      <c r="AZ7" s="180"/>
+      <c r="BA7" s="180"/>
+      <c r="BB7" s="180"/>
+      <c r="BC7" s="180"/>
+      <c r="BD7" s="180"/>
+      <c r="BE7" s="180"/>
+      <c r="BF7" s="179"/>
+      <c r="BG7" s="179"/>
+      <c r="BT7" s="191"/>
+      <c r="BW7" s="191"/>
+      <c r="CT7" s="191"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="190"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="193"/>
-      <c r="AS8" s="193"/>
-      <c r="AT8" s="193"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="197"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="190"/>
+      <c r="R8" s="190"/>
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="190"/>
+      <c r="W8" s="189"/>
+      <c r="X8" s="189"/>
+      <c r="Y8" s="189"/>
+      <c r="Z8" s="189"/>
+      <c r="AA8" s="189"/>
+      <c r="AB8" s="187"/>
+      <c r="AC8" s="187"/>
+      <c r="AD8" s="187"/>
+      <c r="AE8" s="187"/>
+      <c r="AF8" s="187"/>
+      <c r="AG8" s="187"/>
+      <c r="AH8" s="187"/>
+      <c r="AI8" s="187"/>
+      <c r="AJ8" s="187"/>
+      <c r="AK8" s="187"/>
+      <c r="AL8" s="187"/>
+      <c r="AM8" s="187"/>
+      <c r="AN8" s="187"/>
+      <c r="AO8" s="187"/>
+      <c r="AP8" s="187"/>
+      <c r="AQ8" s="187"/>
+      <c r="AR8" s="182"/>
+      <c r="AS8" s="182"/>
+      <c r="AT8" s="182"/>
       <c r="AU8" s="177"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="196"/>
-      <c r="AY8" s="197"/>
-      <c r="AZ8" s="197"/>
-      <c r="BA8" s="197"/>
-      <c r="BB8" s="197"/>
-      <c r="BC8" s="197"/>
-      <c r="BD8" s="197"/>
-      <c r="BE8" s="197"/>
-      <c r="BF8" s="199"/>
-      <c r="BG8" s="199"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
+      <c r="AV8" s="191"/>
+      <c r="AW8" s="191"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="180"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="179"/>
+      <c r="BG8" s="179"/>
+      <c r="BT8" s="191"/>
+      <c r="BW8" s="191"/>
+      <c r="CT8" s="191"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="198"/>
+      <c r="B9" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
-      <c r="AB9" s="190"/>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="190"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="190"/>
-      <c r="AL9" s="190"/>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="190"/>
-      <c r="AQ9" s="190"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="197"/>
+      <c r="I9" s="197"/>
+      <c r="J9" s="197"/>
+      <c r="K9" s="197"/>
+      <c r="L9" s="190"/>
+      <c r="M9" s="190"/>
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="190"/>
+      <c r="R9" s="190"/>
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="190"/>
+      <c r="W9" s="189"/>
+      <c r="X9" s="189"/>
+      <c r="Y9" s="189"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="189"/>
+      <c r="AB9" s="187"/>
+      <c r="AC9" s="187"/>
+      <c r="AD9" s="187"/>
+      <c r="AE9" s="187"/>
+      <c r="AF9" s="187"/>
+      <c r="AG9" s="187"/>
+      <c r="AH9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="187"/>
+      <c r="AM9" s="187"/>
+      <c r="AN9" s="187"/>
+      <c r="AO9" s="187"/>
+      <c r="AP9" s="187"/>
+      <c r="AQ9" s="187"/>
+      <c r="AR9" s="182"/>
+      <c r="AS9" s="182"/>
+      <c r="AT9" s="182"/>
       <c r="AU9" s="177"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="196"/>
-      <c r="AY9" s="197"/>
-      <c r="AZ9" s="197"/>
-      <c r="BA9" s="197"/>
-      <c r="BB9" s="197"/>
-      <c r="BC9" s="197"/>
-      <c r="BD9" s="197"/>
-      <c r="BE9" s="197"/>
-      <c r="BF9" s="199"/>
-      <c r="BG9" s="199"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
+      <c r="AV9" s="191"/>
+      <c r="AW9" s="191"/>
+      <c r="AX9" s="185"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="180"/>
+      <c r="BB9" s="180"/>
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="179"/>
+      <c r="BG9" s="179"/>
+      <c r="BT9" s="191"/>
+      <c r="BW9" s="191"/>
+      <c r="CT9" s="191"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="A10" s="198"/>
+      <c r="B10" s="199" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="190"/>
-      <c r="AC10" s="190"/>
-      <c r="AD10" s="190"/>
-      <c r="AE10" s="190"/>
-      <c r="AF10" s="190"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="190"/>
-      <c r="AI10" s="190"/>
-      <c r="AJ10" s="190"/>
-      <c r="AK10" s="190"/>
-      <c r="AL10" s="190"/>
-      <c r="AM10" s="190"/>
-      <c r="AN10" s="190"/>
-      <c r="AO10" s="190"/>
-      <c r="AP10" s="190"/>
-      <c r="AQ10" s="190"/>
-      <c r="AR10" s="193"/>
-      <c r="AS10" s="193"/>
-      <c r="AT10" s="193"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="197"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="197"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="197"/>
+      <c r="K10" s="197"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="190"/>
+      <c r="O10" s="190"/>
+      <c r="P10" s="190"/>
+      <c r="Q10" s="190"/>
+      <c r="R10" s="190"/>
+      <c r="S10" s="190"/>
+      <c r="T10" s="190"/>
+      <c r="U10" s="190"/>
+      <c r="V10" s="190"/>
+      <c r="W10" s="189"/>
+      <c r="X10" s="189"/>
+      <c r="Y10" s="189"/>
+      <c r="Z10" s="189"/>
+      <c r="AA10" s="189"/>
+      <c r="AB10" s="187"/>
+      <c r="AC10" s="187"/>
+      <c r="AD10" s="187"/>
+      <c r="AE10" s="187"/>
+      <c r="AF10" s="187"/>
+      <c r="AG10" s="187"/>
+      <c r="AH10" s="187"/>
+      <c r="AI10" s="187"/>
+      <c r="AJ10" s="187"/>
+      <c r="AK10" s="187"/>
+      <c r="AL10" s="187"/>
+      <c r="AM10" s="187"/>
+      <c r="AN10" s="187"/>
+      <c r="AO10" s="187"/>
+      <c r="AP10" s="187"/>
+      <c r="AQ10" s="187"/>
+      <c r="AR10" s="182"/>
+      <c r="AS10" s="182"/>
+      <c r="AT10" s="182"/>
       <c r="AU10" s="177"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="196"/>
-      <c r="AY10" s="197"/>
-      <c r="AZ10" s="197"/>
-      <c r="BA10" s="197"/>
-      <c r="BB10" s="197"/>
-      <c r="BC10" s="197"/>
-      <c r="BD10" s="197"/>
-      <c r="BE10" s="197"/>
-      <c r="BF10" s="199"/>
-      <c r="BG10" s="199"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
+      <c r="AV10" s="191"/>
+      <c r="AW10" s="191"/>
+      <c r="AX10" s="185"/>
+      <c r="AY10" s="180"/>
+      <c r="AZ10" s="180"/>
+      <c r="BA10" s="180"/>
+      <c r="BB10" s="180"/>
+      <c r="BC10" s="180"/>
+      <c r="BD10" s="180"/>
+      <c r="BE10" s="180"/>
+      <c r="BF10" s="179"/>
+      <c r="BG10" s="179"/>
+      <c r="BT10" s="191"/>
+      <c r="BW10" s="191"/>
+      <c r="CT10" s="191"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="A11" s="198"/>
+      <c r="B11" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="191"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="191"/>
-      <c r="AE11" s="191"/>
-      <c r="AF11" s="191"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="191"/>
-      <c r="AI11" s="191"/>
-      <c r="AJ11" s="191"/>
-      <c r="AK11" s="191"/>
-      <c r="AL11" s="191"/>
-      <c r="AM11" s="191"/>
-      <c r="AN11" s="191"/>
-      <c r="AO11" s="191"/>
-      <c r="AP11" s="191"/>
-      <c r="AQ11" s="191"/>
-      <c r="AR11" s="194"/>
-      <c r="AS11" s="194"/>
-      <c r="AT11" s="194"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="197"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
+      <c r="N11" s="190"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="190"/>
+      <c r="Q11" s="190"/>
+      <c r="R11" s="190"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="190"/>
+      <c r="U11" s="190"/>
+      <c r="V11" s="190"/>
+      <c r="W11" s="189"/>
+      <c r="X11" s="189"/>
+      <c r="Y11" s="189"/>
+      <c r="Z11" s="189"/>
+      <c r="AA11" s="189"/>
+      <c r="AB11" s="188"/>
+      <c r="AC11" s="188"/>
+      <c r="AD11" s="188"/>
+      <c r="AE11" s="188"/>
+      <c r="AF11" s="188"/>
+      <c r="AG11" s="188"/>
+      <c r="AH11" s="188"/>
+      <c r="AI11" s="188"/>
+      <c r="AJ11" s="188"/>
+      <c r="AK11" s="188"/>
+      <c r="AL11" s="188"/>
+      <c r="AM11" s="188"/>
+      <c r="AN11" s="188"/>
+      <c r="AO11" s="188"/>
+      <c r="AP11" s="188"/>
+      <c r="AQ11" s="188"/>
+      <c r="AR11" s="183"/>
+      <c r="AS11" s="183"/>
+      <c r="AT11" s="183"/>
       <c r="AU11" s="177"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="196"/>
-      <c r="AY11" s="197"/>
-      <c r="AZ11" s="197"/>
-      <c r="BA11" s="197"/>
-      <c r="BB11" s="197"/>
-      <c r="BC11" s="197"/>
-      <c r="BD11" s="197"/>
-      <c r="BE11" s="197"/>
-      <c r="BF11" s="199"/>
-      <c r="BG11" s="199"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="AV11" s="191"/>
+      <c r="AW11" s="191"/>
+      <c r="AX11" s="185"/>
+      <c r="AY11" s="180"/>
+      <c r="AZ11" s="180"/>
+      <c r="BA11" s="180"/>
+      <c r="BB11" s="180"/>
+      <c r="BC11" s="180"/>
+      <c r="BD11" s="180"/>
+      <c r="BE11" s="180"/>
+      <c r="BF11" s="179"/>
+      <c r="BG11" s="179"/>
+      <c r="BT11" s="191"/>
+      <c r="BW11" s="191"/>
+      <c r="CT11" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4262,22 +4243,47 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5799,13 +5805,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="212" t="s">
+      <c r="A4" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="214"/>
+      <c r="C4" s="205"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5910,9 +5916,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="201"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="201"/>
+      <c r="A5" s="203"/>
+      <c r="B5" s="201"/>
+      <c r="C5" s="203"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -6017,11 +6023,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="201"/>
+      <c r="A6" s="203"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="201"/>
+      <c r="C6" s="203"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6126,11 +6132,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="201"/>
+      <c r="A7" s="203"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="201"/>
+      <c r="C7" s="203"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6235,11 +6241,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201"/>
+      <c r="A8" s="203"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="201"/>
+      <c r="C8" s="203"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6344,11 +6350,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="201"/>
+      <c r="C9" s="203"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6453,11 +6459,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="203"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6562,11 +6568,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="203"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6671,9 +6677,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="201"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="202"/>
+      <c r="C12" s="206"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6778,10 +6784,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="207" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="208" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6890,8 +6896,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="201"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="203"/>
+      <c r="B14" s="209"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -7012,7 +7018,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="201"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7122,7 +7128,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7232,7 +7238,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7344,7 +7350,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7454,7 +7460,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7564,7 +7570,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="201"/>
+      <c r="A20" s="203"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7674,7 +7680,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="202"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7785,7 +7791,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="200" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7895,7 +7901,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="211"/>
+      <c r="B23" s="201"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -8002,13 +8008,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="203" t="s">
+      <c r="A24" s="211" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="205">
+      <c r="C24" s="213">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8116,11 +8122,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="204"/>
+      <c r="A25" s="212"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="201"/>
+      <c r="C25" s="203"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8226,11 +8232,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="204"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="203"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8336,11 +8342,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="204"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="201"/>
+      <c r="C27" s="203"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8446,11 +8452,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="204"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="201"/>
+      <c r="C28" s="203"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8556,11 +8562,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="204"/>
+      <c r="A29" s="212"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="201"/>
+      <c r="C29" s="203"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8666,11 +8672,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="204"/>
+      <c r="A30" s="212"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="201"/>
+      <c r="C30" s="203"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8776,11 +8782,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="204"/>
+      <c r="A31" s="212"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="201"/>
+      <c r="C31" s="203"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8886,11 +8892,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="204"/>
+      <c r="A32" s="212"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="201"/>
+      <c r="C32" s="203"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -8996,11 +9002,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="204"/>
+      <c r="A33" s="212"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="201"/>
+      <c r="C33" s="203"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9106,11 +9112,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="204"/>
+      <c r="A34" s="212"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="201"/>
+      <c r="C34" s="203"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9216,11 +9222,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="204"/>
+      <c r="A35" s="212"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="202"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9326,11 +9332,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="204"/>
+      <c r="A36" s="212"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="205">
+      <c r="C36" s="213">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9438,11 +9444,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="204"/>
+      <c r="A37" s="212"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="201"/>
+      <c r="C37" s="203"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9548,11 +9554,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="204"/>
+      <c r="A38" s="212"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="201"/>
+      <c r="C38" s="203"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9658,11 +9664,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="204"/>
+      <c r="A39" s="212"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="201"/>
+      <c r="C39" s="203"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9768,11 +9774,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="204"/>
+      <c r="A40" s="212"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="201"/>
+      <c r="C40" s="203"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9878,11 +9884,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="204"/>
+      <c r="A41" s="212"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="201"/>
+      <c r="C41" s="203"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9988,11 +9994,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="204"/>
+      <c r="A42" s="212"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="201"/>
+      <c r="C42" s="203"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10098,11 +10104,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="204"/>
+      <c r="A43" s="212"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="201"/>
+      <c r="C43" s="203"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10208,11 +10214,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="204"/>
+      <c r="A44" s="212"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="201"/>
+      <c r="C44" s="203"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10318,11 +10324,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="204"/>
+      <c r="A45" s="212"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10428,11 +10434,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="204"/>
+      <c r="A46" s="212"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="201"/>
+      <c r="C46" s="203"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10538,11 +10544,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="204"/>
+      <c r="A47" s="212"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="201"/>
+      <c r="C47" s="203"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10656,11 +10662,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="204"/>
+      <c r="A48" s="212"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="201"/>
+      <c r="C48" s="203"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10769,7 +10775,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="214" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10879,7 +10885,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="207"/>
+      <c r="B50" s="209"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14310,7 +14316,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="208" t="s">
+      <c r="A81" s="215" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14422,7 +14428,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="201"/>
+      <c r="A82" s="203"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14532,7 +14538,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="201"/>
+      <c r="A83" s="203"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14642,7 +14648,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="201"/>
+      <c r="A84" s="203"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14752,7 +14758,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="201"/>
+      <c r="A85" s="203"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14862,7 +14868,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="201"/>
+      <c r="A86" s="203"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14972,7 +14978,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="201"/>
+      <c r="A87" s="203"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15084,7 +15090,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="201"/>
+      <c r="A88" s="203"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15194,7 +15200,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="201"/>
+      <c r="A89" s="203"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15304,7 +15310,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="201"/>
+      <c r="A90" s="203"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15414,11 +15420,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="201"/>
+      <c r="A91" s="203"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="209"/>
+      <c r="C91" s="216"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15524,11 +15530,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="201"/>
+      <c r="A92" s="203"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="203"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15634,11 +15640,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="202"/>
+      <c r="A93" s="206"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="201"/>
+      <c r="C93" s="203"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15862,7 +15868,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="200" t="s">
+      <c r="A95" s="210" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15974,7 +15980,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="201"/>
+      <c r="A96" s="203"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16084,7 +16090,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="201"/>
+      <c r="A97" s="203"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16194,7 +16200,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="201"/>
+      <c r="A98" s="203"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16304,7 +16310,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="201"/>
+      <c r="A99" s="203"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16414,7 +16420,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="201"/>
+      <c r="A100" s="203"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16524,7 +16530,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="201"/>
+      <c r="A101" s="203"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16634,7 +16640,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="201"/>
+      <c r="A102" s="203"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16744,7 +16750,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="201"/>
+      <c r="A103" s="203"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16856,7 +16862,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="201"/>
+      <c r="A104" s="203"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16966,7 +16972,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="201"/>
+      <c r="A105" s="203"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17084,7 +17090,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="201"/>
+      <c r="A106" s="203"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17194,7 +17200,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="201"/>
+      <c r="A107" s="203"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17304,7 +17310,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="201"/>
+      <c r="A108" s="203"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17414,7 +17420,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="201"/>
+      <c r="A109" s="203"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17524,7 +17530,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="201"/>
+      <c r="A110" s="203"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17634,7 +17640,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="201"/>
+      <c r="A111" s="203"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17744,7 +17750,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="201"/>
+      <c r="A112" s="203"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17854,7 +17860,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="201"/>
+      <c r="A113" s="203"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17964,7 +17970,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="201"/>
+      <c r="A114" s="203"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18074,7 +18080,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="201"/>
+      <c r="A115" s="203"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18184,7 +18190,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="201"/>
+      <c r="A116" s="203"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18310,7 +18316,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="201"/>
+      <c r="A117" s="203"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18420,7 +18426,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="202"/>
+      <c r="A118" s="206"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25791,12 +25797,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25804,6 +25804,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento realizado em 04-10
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FA92A5-6973-4A37-A6D7-8D0BBE22FFDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0404403F-A70B-4DF1-9E0B-00A2CF2D5404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="181">
   <si>
     <t>S</t>
   </si>
@@ -749,6 +749,9 @@
   <si>
     <t>Correção do exercício Vingadores.
 Ajustes nas páginas para apresentação à Linx.</t>
+  </si>
+  <si>
+    <t>Ajustes nos sites e reunião com a Linx</t>
   </si>
 </sst>
 </file>
@@ -2280,14 +2283,47 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2304,73 +2340,20 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2381,10 +2364,30 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2894,7 +2897,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP4" sqref="AP4:AP11"/>
+      <selection pane="bottomRight" activeCell="AQ4" sqref="AQ4:AQ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3203,110 +3206,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="192" t="s">
+      <c r="D2" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="192"/>
-      <c r="I2" s="192"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="192"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="192" t="s">
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="192"/>
-      <c r="T2" s="192"/>
-      <c r="U2" s="192"/>
-      <c r="V2" s="192"/>
-      <c r="W2" s="192"/>
-      <c r="X2" s="192"/>
-      <c r="Y2" s="192"/>
-      <c r="Z2" s="192"/>
-      <c r="AA2" s="192"/>
-      <c r="AB2" s="192"/>
-      <c r="AC2" s="192"/>
-      <c r="AD2" s="192"/>
-      <c r="AE2" s="192"/>
-      <c r="AF2" s="192"/>
-      <c r="AG2" s="192"/>
-      <c r="AH2" s="192"/>
-      <c r="AI2" s="192"/>
-      <c r="AJ2" s="192"/>
-      <c r="AK2" s="192"/>
-      <c r="AL2" s="192"/>
-      <c r="AM2" s="192" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182"/>
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182"/>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="182"/>
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="182"/>
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="182"/>
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="182"/>
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="192"/>
-      <c r="AO2" s="192"/>
-      <c r="AP2" s="192"/>
-      <c r="AQ2" s="192"/>
-      <c r="AR2" s="192"/>
-      <c r="AS2" s="192"/>
-      <c r="AT2" s="192"/>
-      <c r="AU2" s="192"/>
-      <c r="AV2" s="192"/>
-      <c r="AW2" s="192"/>
-      <c r="AX2" s="193"/>
-      <c r="AY2" s="193"/>
-      <c r="AZ2" s="193"/>
-      <c r="BA2" s="193"/>
-      <c r="BB2" s="193"/>
-      <c r="BC2" s="193"/>
-      <c r="BD2" s="193"/>
-      <c r="BE2" s="193"/>
-      <c r="BF2" s="193"/>
-      <c r="BG2" s="193"/>
-      <c r="BH2" s="193"/>
-      <c r="BI2" s="193"/>
-      <c r="BJ2" s="192" t="s">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="182"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="182"/>
+      <c r="AR2" s="182"/>
+      <c r="AS2" s="182"/>
+      <c r="AT2" s="182"/>
+      <c r="AU2" s="182"/>
+      <c r="AV2" s="182"/>
+      <c r="AW2" s="182"/>
+      <c r="AX2" s="183"/>
+      <c r="AY2" s="183"/>
+      <c r="AZ2" s="183"/>
+      <c r="BA2" s="183"/>
+      <c r="BB2" s="183"/>
+      <c r="BC2" s="183"/>
+      <c r="BD2" s="183"/>
+      <c r="BE2" s="183"/>
+      <c r="BF2" s="183"/>
+      <c r="BG2" s="183"/>
+      <c r="BH2" s="183"/>
+      <c r="BI2" s="183"/>
+      <c r="BJ2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="192"/>
-      <c r="BL2" s="192"/>
-      <c r="BM2" s="192"/>
-      <c r="BN2" s="192"/>
-      <c r="BO2" s="192"/>
-      <c r="BP2" s="192"/>
-      <c r="BQ2" s="192"/>
-      <c r="BR2" s="192"/>
-      <c r="BS2" s="192"/>
-      <c r="BT2" s="192"/>
-      <c r="BU2" s="192"/>
-      <c r="BV2" s="192"/>
-      <c r="BW2" s="192"/>
-      <c r="BX2" s="194"/>
-      <c r="BY2" s="194"/>
-      <c r="BZ2" s="194"/>
-      <c r="CA2" s="194"/>
-      <c r="CB2" s="194"/>
-      <c r="CC2" s="194"/>
-      <c r="CD2" s="194"/>
-      <c r="CE2" s="195" t="s">
+      <c r="BK2" s="182"/>
+      <c r="BL2" s="182"/>
+      <c r="BM2" s="182"/>
+      <c r="BN2" s="182"/>
+      <c r="BO2" s="182"/>
+      <c r="BP2" s="182"/>
+      <c r="BQ2" s="182"/>
+      <c r="BR2" s="182"/>
+      <c r="BS2" s="182"/>
+      <c r="BT2" s="182"/>
+      <c r="BU2" s="182"/>
+      <c r="BV2" s="182"/>
+      <c r="BW2" s="182"/>
+      <c r="BX2" s="184"/>
+      <c r="BY2" s="184"/>
+      <c r="BZ2" s="184"/>
+      <c r="CA2" s="184"/>
+      <c r="CB2" s="184"/>
+      <c r="CC2" s="184"/>
+      <c r="CD2" s="184"/>
+      <c r="CE2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="196"/>
-      <c r="CG2" s="196"/>
-      <c r="CH2" s="196"/>
-      <c r="CI2" s="196"/>
-      <c r="CJ2" s="196"/>
-      <c r="CK2" s="196"/>
-      <c r="CL2" s="196"/>
-      <c r="CM2" s="196"/>
-      <c r="CN2" s="196"/>
-      <c r="CO2" s="196"/>
-      <c r="CP2" s="196"/>
-      <c r="CQ2" s="196"/>
-      <c r="CR2" s="196"/>
-      <c r="CS2" s="196"/>
+      <c r="CF2" s="186"/>
+      <c r="CG2" s="186"/>
+      <c r="CH2" s="186"/>
+      <c r="CI2" s="186"/>
+      <c r="CJ2" s="186"/>
+      <c r="CK2" s="186"/>
+      <c r="CL2" s="186"/>
+      <c r="CM2" s="186"/>
+      <c r="CN2" s="186"/>
+      <c r="CO2" s="186"/>
+      <c r="CP2" s="186"/>
+      <c r="CQ2" s="186"/>
+      <c r="CR2" s="186"/>
+      <c r="CS2" s="186"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3602,615 +3605,674 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="198" t="s">
+      <c r="A4" s="178" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="199"/>
-      <c r="D4" s="197" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="181" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="197" t="s">
+      <c r="F4" s="181" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="197" t="s">
+      <c r="G4" s="181" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="197" t="s">
+      <c r="H4" s="181" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="197" t="s">
+      <c r="I4" s="181" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="197" t="s">
+      <c r="J4" s="181" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="197" t="s">
+      <c r="K4" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="190" t="s">
+      <c r="L4" s="187" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="190" t="s">
+      <c r="M4" s="187" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="190" t="s">
+      <c r="N4" s="187" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="190" t="s">
+      <c r="O4" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="190" t="s">
+      <c r="P4" s="187" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="190" t="s">
+      <c r="Q4" s="187" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="190" t="s">
+      <c r="R4" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="190" t="s">
+      <c r="S4" s="187" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="190" t="s">
+      <c r="T4" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="190" t="s">
+      <c r="U4" s="187" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="190" t="s">
+      <c r="V4" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="189" t="s">
+      <c r="W4" s="188" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="189" t="s">
+      <c r="X4" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="189" t="s">
+      <c r="Y4" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="189" t="s">
+      <c r="Z4" s="188" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="189" t="s">
+      <c r="AA4" s="188" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="186" t="s">
+      <c r="AB4" s="189" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="186" t="s">
+      <c r="AC4" s="189" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="186" t="s">
+      <c r="AD4" s="189" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="186" t="s">
+      <c r="AE4" s="189" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="186" t="s">
+      <c r="AF4" s="189" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="186" t="s">
+      <c r="AG4" s="189" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="186" t="s">
+      <c r="AH4" s="189" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="186" t="s">
+      <c r="AI4" s="189" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="186" t="s">
+      <c r="AJ4" s="189" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="186" t="s">
+      <c r="AK4" s="189" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" s="186" t="s">
+      <c r="AL4" s="189" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" s="186" t="s">
+      <c r="AM4" s="189" t="s">
         <v>177</v>
       </c>
-      <c r="AN4" s="186" t="s">
+      <c r="AN4" s="189" t="s">
         <v>178</v>
       </c>
-      <c r="AO4" s="186" t="s">
+      <c r="AO4" s="189" t="s">
         <v>179</v>
       </c>
-      <c r="AP4" s="186"/>
-      <c r="AQ4" s="186"/>
-      <c r="AR4" s="181"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="181"/>
+      <c r="AP4" s="189" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ4" s="189"/>
+      <c r="AR4" s="192"/>
+      <c r="AS4" s="192"/>
+      <c r="AT4" s="192"/>
       <c r="AU4" s="176"/>
-      <c r="AV4" s="191"/>
-      <c r="AW4" s="191"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="180"/>
-      <c r="BA4" s="180"/>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="178"/>
-      <c r="BT4" s="191"/>
-      <c r="BW4" s="191"/>
-      <c r="CT4" s="191"/>
+      <c r="AV4" s="179"/>
+      <c r="AW4" s="179"/>
+      <c r="AX4" s="195"/>
+      <c r="AY4" s="197"/>
+      <c r="AZ4" s="197"/>
+      <c r="BA4" s="197"/>
+      <c r="BB4" s="197"/>
+      <c r="BC4" s="197"/>
+      <c r="BD4" s="197"/>
+      <c r="BE4" s="197"/>
+      <c r="BF4" s="198"/>
+      <c r="BG4" s="198"/>
+      <c r="BT4" s="179"/>
+      <c r="BW4" s="179"/>
+      <c r="CT4" s="179"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="198"/>
-      <c r="B5" s="199" t="s">
+      <c r="A5" s="178"/>
+      <c r="B5" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="197"/>
-      <c r="G5" s="197"/>
-      <c r="H5" s="197"/>
-      <c r="I5" s="197"/>
-      <c r="J5" s="197"/>
-      <c r="K5" s="197"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
-      <c r="N5" s="190"/>
-      <c r="O5" s="190"/>
-      <c r="P5" s="190"/>
-      <c r="Q5" s="190"/>
-      <c r="R5" s="190"/>
-      <c r="S5" s="190"/>
-      <c r="T5" s="190"/>
-      <c r="U5" s="190"/>
-      <c r="V5" s="190"/>
-      <c r="W5" s="189"/>
-      <c r="X5" s="189"/>
-      <c r="Y5" s="189"/>
-      <c r="Z5" s="189"/>
-      <c r="AA5" s="189"/>
-      <c r="AB5" s="187"/>
-      <c r="AC5" s="187"/>
-      <c r="AD5" s="187"/>
-      <c r="AE5" s="187"/>
-      <c r="AF5" s="187"/>
-      <c r="AG5" s="187"/>
-      <c r="AH5" s="187"/>
-      <c r="AI5" s="187"/>
-      <c r="AJ5" s="187"/>
-      <c r="AK5" s="187"/>
-      <c r="AL5" s="187"/>
-      <c r="AM5" s="187"/>
-      <c r="AN5" s="187"/>
-      <c r="AO5" s="187"/>
-      <c r="AP5" s="187"/>
-      <c r="AQ5" s="187"/>
-      <c r="AR5" s="182"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="182"/>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="188"/>
+      <c r="X5" s="188"/>
+      <c r="Y5" s="188"/>
+      <c r="Z5" s="188"/>
+      <c r="AA5" s="188"/>
+      <c r="AB5" s="190"/>
+      <c r="AC5" s="190"/>
+      <c r="AD5" s="190"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="190"/>
+      <c r="AH5" s="190"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="190"/>
+      <c r="AK5" s="190"/>
+      <c r="AL5" s="190"/>
+      <c r="AM5" s="190"/>
+      <c r="AN5" s="190"/>
+      <c r="AO5" s="190"/>
+      <c r="AP5" s="190"/>
+      <c r="AQ5" s="190"/>
+      <c r="AR5" s="193"/>
+      <c r="AS5" s="193"/>
+      <c r="AT5" s="193"/>
       <c r="AU5" s="176"/>
-      <c r="AV5" s="191"/>
-      <c r="AW5" s="191"/>
-      <c r="AX5" s="185"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="180"/>
-      <c r="BA5" s="180"/>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="179"/>
-      <c r="BG5" s="179"/>
-      <c r="BT5" s="191"/>
-      <c r="BW5" s="191"/>
-      <c r="CT5" s="191"/>
+      <c r="AV5" s="179"/>
+      <c r="AW5" s="179"/>
+      <c r="AX5" s="196"/>
+      <c r="AY5" s="197"/>
+      <c r="AZ5" s="197"/>
+      <c r="BA5" s="197"/>
+      <c r="BB5" s="197"/>
+      <c r="BC5" s="197"/>
+      <c r="BD5" s="197"/>
+      <c r="BE5" s="197"/>
+      <c r="BF5" s="199"/>
+      <c r="BG5" s="199"/>
+      <c r="BT5" s="179"/>
+      <c r="BW5" s="179"/>
+      <c r="CT5" s="179"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199" t="s">
+      <c r="A6" s="178"/>
+      <c r="B6" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="199"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="197"/>
-      <c r="H6" s="197"/>
-      <c r="I6" s="197"/>
-      <c r="J6" s="197"/>
-      <c r="K6" s="197"/>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
-      <c r="N6" s="190"/>
-      <c r="O6" s="190"/>
-      <c r="P6" s="190"/>
-      <c r="Q6" s="190"/>
-      <c r="R6" s="190"/>
-      <c r="S6" s="190"/>
-      <c r="T6" s="190"/>
-      <c r="U6" s="190"/>
-      <c r="V6" s="190"/>
-      <c r="W6" s="189"/>
-      <c r="X6" s="189"/>
-      <c r="Y6" s="189"/>
-      <c r="Z6" s="189"/>
-      <c r="AA6" s="189"/>
-      <c r="AB6" s="187"/>
-      <c r="AC6" s="187"/>
-      <c r="AD6" s="187"/>
-      <c r="AE6" s="187"/>
-      <c r="AF6" s="187"/>
-      <c r="AG6" s="187"/>
-      <c r="AH6" s="187"/>
-      <c r="AI6" s="187"/>
-      <c r="AJ6" s="187"/>
-      <c r="AK6" s="187"/>
-      <c r="AL6" s="187"/>
-      <c r="AM6" s="187"/>
-      <c r="AN6" s="187"/>
-      <c r="AO6" s="187"/>
-      <c r="AP6" s="187"/>
-      <c r="AQ6" s="187"/>
-      <c r="AR6" s="182"/>
-      <c r="AS6" s="182"/>
-      <c r="AT6" s="182"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="181"/>
+      <c r="G6" s="181"/>
+      <c r="H6" s="181"/>
+      <c r="I6" s="181"/>
+      <c r="J6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="188"/>
+      <c r="X6" s="188"/>
+      <c r="Y6" s="188"/>
+      <c r="Z6" s="188"/>
+      <c r="AA6" s="188"/>
+      <c r="AB6" s="190"/>
+      <c r="AC6" s="190"/>
+      <c r="AD6" s="190"/>
+      <c r="AE6" s="190"/>
+      <c r="AF6" s="190"/>
+      <c r="AG6" s="190"/>
+      <c r="AH6" s="190"/>
+      <c r="AI6" s="190"/>
+      <c r="AJ6" s="190"/>
+      <c r="AK6" s="190"/>
+      <c r="AL6" s="190"/>
+      <c r="AM6" s="190"/>
+      <c r="AN6" s="190"/>
+      <c r="AO6" s="190"/>
+      <c r="AP6" s="190"/>
+      <c r="AQ6" s="190"/>
+      <c r="AR6" s="193"/>
+      <c r="AS6" s="193"/>
+      <c r="AT6" s="193"/>
       <c r="AU6" s="176"/>
-      <c r="AV6" s="191"/>
-      <c r="AW6" s="191"/>
-      <c r="AX6" s="185"/>
-      <c r="AY6" s="180"/>
-      <c r="AZ6" s="180"/>
-      <c r="BA6" s="180"/>
-      <c r="BB6" s="180"/>
-      <c r="BC6" s="180"/>
-      <c r="BD6" s="180"/>
-      <c r="BE6" s="180"/>
-      <c r="BF6" s="179"/>
-      <c r="BG6" s="179"/>
-      <c r="BT6" s="191"/>
-      <c r="BW6" s="191"/>
-      <c r="CT6" s="191"/>
+      <c r="AV6" s="179"/>
+      <c r="AW6" s="179"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="199"/>
+      <c r="BG6" s="199"/>
+      <c r="BT6" s="179"/>
+      <c r="BW6" s="179"/>
+      <c r="CT6" s="179"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="198"/>
-      <c r="B7" s="199" t="s">
+      <c r="A7" s="178"/>
+      <c r="B7" s="180" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="197"/>
-      <c r="F7" s="197"/>
-      <c r="G7" s="197"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="197"/>
-      <c r="J7" s="197"/>
-      <c r="K7" s="197"/>
-      <c r="L7" s="190"/>
-      <c r="M7" s="190"/>
-      <c r="N7" s="190"/>
-      <c r="O7" s="190"/>
-      <c r="P7" s="190"/>
-      <c r="Q7" s="190"/>
-      <c r="R7" s="190"/>
-      <c r="S7" s="190"/>
-      <c r="T7" s="190"/>
-      <c r="U7" s="190"/>
-      <c r="V7" s="190"/>
-      <c r="W7" s="189"/>
-      <c r="X7" s="189"/>
-      <c r="Y7" s="189"/>
-      <c r="Z7" s="189"/>
-      <c r="AA7" s="189"/>
-      <c r="AB7" s="187"/>
-      <c r="AC7" s="187"/>
-      <c r="AD7" s="187"/>
-      <c r="AE7" s="187"/>
-      <c r="AF7" s="187"/>
-      <c r="AG7" s="187"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="182"/>
-      <c r="AS7" s="182"/>
-      <c r="AT7" s="182"/>
+      <c r="C7" s="180"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="181"/>
+      <c r="H7" s="181"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="181"/>
+      <c r="K7" s="181"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="188"/>
+      <c r="X7" s="188"/>
+      <c r="Y7" s="188"/>
+      <c r="Z7" s="188"/>
+      <c r="AA7" s="188"/>
+      <c r="AB7" s="190"/>
+      <c r="AC7" s="190"/>
+      <c r="AD7" s="190"/>
+      <c r="AE7" s="190"/>
+      <c r="AF7" s="190"/>
+      <c r="AG7" s="190"/>
+      <c r="AH7" s="190"/>
+      <c r="AI7" s="190"/>
+      <c r="AJ7" s="190"/>
+      <c r="AK7" s="190"/>
+      <c r="AL7" s="190"/>
+      <c r="AM7" s="190"/>
+      <c r="AN7" s="190"/>
+      <c r="AO7" s="190"/>
+      <c r="AP7" s="190"/>
+      <c r="AQ7" s="190"/>
+      <c r="AR7" s="193"/>
+      <c r="AS7" s="193"/>
+      <c r="AT7" s="193"/>
       <c r="AU7" s="177"/>
-      <c r="AV7" s="191"/>
-      <c r="AW7" s="191"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="180"/>
-      <c r="AZ7" s="180"/>
-      <c r="BA7" s="180"/>
-      <c r="BB7" s="180"/>
-      <c r="BC7" s="180"/>
-      <c r="BD7" s="180"/>
-      <c r="BE7" s="180"/>
-      <c r="BF7" s="179"/>
-      <c r="BG7" s="179"/>
-      <c r="BT7" s="191"/>
-      <c r="BW7" s="191"/>
-      <c r="CT7" s="191"/>
+      <c r="AV7" s="179"/>
+      <c r="AW7" s="179"/>
+      <c r="AX7" s="196"/>
+      <c r="AY7" s="197"/>
+      <c r="AZ7" s="197"/>
+      <c r="BA7" s="197"/>
+      <c r="BB7" s="197"/>
+      <c r="BC7" s="197"/>
+      <c r="BD7" s="197"/>
+      <c r="BE7" s="197"/>
+      <c r="BF7" s="199"/>
+      <c r="BG7" s="199"/>
+      <c r="BT7" s="179"/>
+      <c r="BW7" s="179"/>
+      <c r="CT7" s="179"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="198" t="s">
+      <c r="A8" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="199" t="s">
+      <c r="B8" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="199"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="197"/>
-      <c r="K8" s="197"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="190"/>
-      <c r="N8" s="190"/>
-      <c r="O8" s="190"/>
-      <c r="P8" s="190"/>
-      <c r="Q8" s="190"/>
-      <c r="R8" s="190"/>
-      <c r="S8" s="190"/>
-      <c r="T8" s="190"/>
-      <c r="U8" s="190"/>
-      <c r="V8" s="190"/>
-      <c r="W8" s="189"/>
-      <c r="X8" s="189"/>
-      <c r="Y8" s="189"/>
-      <c r="Z8" s="189"/>
-      <c r="AA8" s="189"/>
-      <c r="AB8" s="187"/>
-      <c r="AC8" s="187"/>
-      <c r="AD8" s="187"/>
-      <c r="AE8" s="187"/>
-      <c r="AF8" s="187"/>
-      <c r="AG8" s="187"/>
-      <c r="AH8" s="187"/>
-      <c r="AI8" s="187"/>
-      <c r="AJ8" s="187"/>
-      <c r="AK8" s="187"/>
-      <c r="AL8" s="187"/>
-      <c r="AM8" s="187"/>
-      <c r="AN8" s="187"/>
-      <c r="AO8" s="187"/>
-      <c r="AP8" s="187"/>
-      <c r="AQ8" s="187"/>
-      <c r="AR8" s="182"/>
-      <c r="AS8" s="182"/>
-      <c r="AT8" s="182"/>
+      <c r="C8" s="180"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="181"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181"/>
+      <c r="L8" s="187"/>
+      <c r="M8" s="187"/>
+      <c r="N8" s="187"/>
+      <c r="O8" s="187"/>
+      <c r="P8" s="187"/>
+      <c r="Q8" s="187"/>
+      <c r="R8" s="187"/>
+      <c r="S8" s="187"/>
+      <c r="T8" s="187"/>
+      <c r="U8" s="187"/>
+      <c r="V8" s="187"/>
+      <c r="W8" s="188"/>
+      <c r="X8" s="188"/>
+      <c r="Y8" s="188"/>
+      <c r="Z8" s="188"/>
+      <c r="AA8" s="188"/>
+      <c r="AB8" s="190"/>
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="190"/>
+      <c r="AG8" s="190"/>
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="190"/>
+      <c r="AL8" s="190"/>
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="190"/>
+      <c r="AQ8" s="190"/>
+      <c r="AR8" s="193"/>
+      <c r="AS8" s="193"/>
+      <c r="AT8" s="193"/>
       <c r="AU8" s="177"/>
-      <c r="AV8" s="191"/>
-      <c r="AW8" s="191"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="180"/>
-      <c r="AZ8" s="180"/>
-      <c r="BA8" s="180"/>
-      <c r="BB8" s="180"/>
-      <c r="BC8" s="180"/>
-      <c r="BD8" s="180"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="179"/>
-      <c r="BG8" s="179"/>
-      <c r="BT8" s="191"/>
-      <c r="BW8" s="191"/>
-      <c r="CT8" s="191"/>
+      <c r="AV8" s="179"/>
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="196"/>
+      <c r="AY8" s="197"/>
+      <c r="AZ8" s="197"/>
+      <c r="BA8" s="197"/>
+      <c r="BB8" s="197"/>
+      <c r="BC8" s="197"/>
+      <c r="BD8" s="197"/>
+      <c r="BE8" s="197"/>
+      <c r="BF8" s="199"/>
+      <c r="BG8" s="199"/>
+      <c r="BT8" s="179"/>
+      <c r="BW8" s="179"/>
+      <c r="CT8" s="179"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="198"/>
-      <c r="B9" s="199" t="s">
+      <c r="A9" s="178"/>
+      <c r="B9" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="199"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="197"/>
-      <c r="J9" s="197"/>
-      <c r="K9" s="197"/>
-      <c r="L9" s="190"/>
-      <c r="M9" s="190"/>
-      <c r="N9" s="190"/>
-      <c r="O9" s="190"/>
-      <c r="P9" s="190"/>
-      <c r="Q9" s="190"/>
-      <c r="R9" s="190"/>
-      <c r="S9" s="190"/>
-      <c r="T9" s="190"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="190"/>
-      <c r="W9" s="189"/>
-      <c r="X9" s="189"/>
-      <c r="Y9" s="189"/>
-      <c r="Z9" s="189"/>
-      <c r="AA9" s="189"/>
-      <c r="AB9" s="187"/>
-      <c r="AC9" s="187"/>
-      <c r="AD9" s="187"/>
-      <c r="AE9" s="187"/>
-      <c r="AF9" s="187"/>
-      <c r="AG9" s="187"/>
-      <c r="AH9" s="187"/>
-      <c r="AI9" s="187"/>
-      <c r="AJ9" s="187"/>
-      <c r="AK9" s="187"/>
-      <c r="AL9" s="187"/>
-      <c r="AM9" s="187"/>
-      <c r="AN9" s="187"/>
-      <c r="AO9" s="187"/>
-      <c r="AP9" s="187"/>
-      <c r="AQ9" s="187"/>
-      <c r="AR9" s="182"/>
-      <c r="AS9" s="182"/>
-      <c r="AT9" s="182"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="187"/>
+      <c r="M9" s="187"/>
+      <c r="N9" s="187"/>
+      <c r="O9" s="187"/>
+      <c r="P9" s="187"/>
+      <c r="Q9" s="187"/>
+      <c r="R9" s="187"/>
+      <c r="S9" s="187"/>
+      <c r="T9" s="187"/>
+      <c r="U9" s="187"/>
+      <c r="V9" s="187"/>
+      <c r="W9" s="188"/>
+      <c r="X9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="190"/>
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="190"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="190"/>
+      <c r="AL9" s="190"/>
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="190"/>
+      <c r="AR9" s="193"/>
+      <c r="AS9" s="193"/>
+      <c r="AT9" s="193"/>
       <c r="AU9" s="177"/>
-      <c r="AV9" s="191"/>
-      <c r="AW9" s="191"/>
-      <c r="AX9" s="185"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="180"/>
-      <c r="BB9" s="180"/>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="179"/>
-      <c r="BG9" s="179"/>
-      <c r="BT9" s="191"/>
-      <c r="BW9" s="191"/>
-      <c r="CT9" s="191"/>
+      <c r="AV9" s="179"/>
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="196"/>
+      <c r="AY9" s="197"/>
+      <c r="AZ9" s="197"/>
+      <c r="BA9" s="197"/>
+      <c r="BB9" s="197"/>
+      <c r="BC9" s="197"/>
+      <c r="BD9" s="197"/>
+      <c r="BE9" s="197"/>
+      <c r="BF9" s="199"/>
+      <c r="BG9" s="199"/>
+      <c r="BT9" s="179"/>
+      <c r="BW9" s="179"/>
+      <c r="CT9" s="179"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199" t="s">
+      <c r="A10" s="178"/>
+      <c r="B10" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="199"/>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="197"/>
-      <c r="J10" s="197"/>
-      <c r="K10" s="197"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="190"/>
-      <c r="N10" s="190"/>
-      <c r="O10" s="190"/>
-      <c r="P10" s="190"/>
-      <c r="Q10" s="190"/>
-      <c r="R10" s="190"/>
-      <c r="S10" s="190"/>
-      <c r="T10" s="190"/>
-      <c r="U10" s="190"/>
-      <c r="V10" s="190"/>
-      <c r="W10" s="189"/>
-      <c r="X10" s="189"/>
-      <c r="Y10" s="189"/>
-      <c r="Z10" s="189"/>
-      <c r="AA10" s="189"/>
-      <c r="AB10" s="187"/>
-      <c r="AC10" s="187"/>
-      <c r="AD10" s="187"/>
-      <c r="AE10" s="187"/>
-      <c r="AF10" s="187"/>
-      <c r="AG10" s="187"/>
-      <c r="AH10" s="187"/>
-      <c r="AI10" s="187"/>
-      <c r="AJ10" s="187"/>
-      <c r="AK10" s="187"/>
-      <c r="AL10" s="187"/>
-      <c r="AM10" s="187"/>
-      <c r="AN10" s="187"/>
-      <c r="AO10" s="187"/>
-      <c r="AP10" s="187"/>
-      <c r="AQ10" s="187"/>
-      <c r="AR10" s="182"/>
-      <c r="AS10" s="182"/>
-      <c r="AT10" s="182"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="N10" s="187"/>
+      <c r="O10" s="187"/>
+      <c r="P10" s="187"/>
+      <c r="Q10" s="187"/>
+      <c r="R10" s="187"/>
+      <c r="S10" s="187"/>
+      <c r="T10" s="187"/>
+      <c r="U10" s="187"/>
+      <c r="V10" s="187"/>
+      <c r="W10" s="188"/>
+      <c r="X10" s="188"/>
+      <c r="Y10" s="188"/>
+      <c r="Z10" s="188"/>
+      <c r="AA10" s="188"/>
+      <c r="AB10" s="190"/>
+      <c r="AC10" s="190"/>
+      <c r="AD10" s="190"/>
+      <c r="AE10" s="190"/>
+      <c r="AF10" s="190"/>
+      <c r="AG10" s="190"/>
+      <c r="AH10" s="190"/>
+      <c r="AI10" s="190"/>
+      <c r="AJ10" s="190"/>
+      <c r="AK10" s="190"/>
+      <c r="AL10" s="190"/>
+      <c r="AM10" s="190"/>
+      <c r="AN10" s="190"/>
+      <c r="AO10" s="190"/>
+      <c r="AP10" s="190"/>
+      <c r="AQ10" s="190"/>
+      <c r="AR10" s="193"/>
+      <c r="AS10" s="193"/>
+      <c r="AT10" s="193"/>
       <c r="AU10" s="177"/>
-      <c r="AV10" s="191"/>
-      <c r="AW10" s="191"/>
-      <c r="AX10" s="185"/>
-      <c r="AY10" s="180"/>
-      <c r="AZ10" s="180"/>
-      <c r="BA10" s="180"/>
-      <c r="BB10" s="180"/>
-      <c r="BC10" s="180"/>
-      <c r="BD10" s="180"/>
-      <c r="BE10" s="180"/>
-      <c r="BF10" s="179"/>
-      <c r="BG10" s="179"/>
-      <c r="BT10" s="191"/>
-      <c r="BW10" s="191"/>
-      <c r="CT10" s="191"/>
+      <c r="AV10" s="179"/>
+      <c r="AW10" s="179"/>
+      <c r="AX10" s="196"/>
+      <c r="AY10" s="197"/>
+      <c r="AZ10" s="197"/>
+      <c r="BA10" s="197"/>
+      <c r="BB10" s="197"/>
+      <c r="BC10" s="197"/>
+      <c r="BD10" s="197"/>
+      <c r="BE10" s="197"/>
+      <c r="BF10" s="199"/>
+      <c r="BG10" s="199"/>
+      <c r="BT10" s="179"/>
+      <c r="BW10" s="179"/>
+      <c r="CT10" s="179"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="198"/>
-      <c r="B11" s="199" t="s">
+      <c r="A11" s="178"/>
+      <c r="B11" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="197"/>
-      <c r="J11" s="197"/>
-      <c r="K11" s="197"/>
-      <c r="L11" s="190"/>
-      <c r="M11" s="190"/>
-      <c r="N11" s="190"/>
-      <c r="O11" s="190"/>
-      <c r="P11" s="190"/>
-      <c r="Q11" s="190"/>
-      <c r="R11" s="190"/>
-      <c r="S11" s="190"/>
-      <c r="T11" s="190"/>
-      <c r="U11" s="190"/>
-      <c r="V11" s="190"/>
-      <c r="W11" s="189"/>
-      <c r="X11" s="189"/>
-      <c r="Y11" s="189"/>
-      <c r="Z11" s="189"/>
-      <c r="AA11" s="189"/>
-      <c r="AB11" s="188"/>
-      <c r="AC11" s="188"/>
-      <c r="AD11" s="188"/>
-      <c r="AE11" s="188"/>
-      <c r="AF11" s="188"/>
-      <c r="AG11" s="188"/>
-      <c r="AH11" s="188"/>
-      <c r="AI11" s="188"/>
-      <c r="AJ11" s="188"/>
-      <c r="AK11" s="188"/>
-      <c r="AL11" s="188"/>
-      <c r="AM11" s="188"/>
-      <c r="AN11" s="188"/>
-      <c r="AO11" s="188"/>
-      <c r="AP11" s="188"/>
-      <c r="AQ11" s="188"/>
-      <c r="AR11" s="183"/>
-      <c r="AS11" s="183"/>
-      <c r="AT11" s="183"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="188"/>
+      <c r="X11" s="188"/>
+      <c r="Y11" s="188"/>
+      <c r="Z11" s="188"/>
+      <c r="AA11" s="188"/>
+      <c r="AB11" s="191"/>
+      <c r="AC11" s="191"/>
+      <c r="AD11" s="191"/>
+      <c r="AE11" s="191"/>
+      <c r="AF11" s="191"/>
+      <c r="AG11" s="191"/>
+      <c r="AH11" s="191"/>
+      <c r="AI11" s="191"/>
+      <c r="AJ11" s="191"/>
+      <c r="AK11" s="191"/>
+      <c r="AL11" s="191"/>
+      <c r="AM11" s="191"/>
+      <c r="AN11" s="191"/>
+      <c r="AO11" s="191"/>
+      <c r="AP11" s="191"/>
+      <c r="AQ11" s="191"/>
+      <c r="AR11" s="194"/>
+      <c r="AS11" s="194"/>
+      <c r="AT11" s="194"/>
       <c r="AU11" s="177"/>
-      <c r="AV11" s="191"/>
-      <c r="AW11" s="191"/>
-      <c r="AX11" s="185"/>
-      <c r="AY11" s="180"/>
-      <c r="AZ11" s="180"/>
-      <c r="BA11" s="180"/>
-      <c r="BB11" s="180"/>
-      <c r="BC11" s="180"/>
-      <c r="BD11" s="180"/>
-      <c r="BE11" s="180"/>
-      <c r="BF11" s="179"/>
-      <c r="BG11" s="179"/>
-      <c r="BT11" s="191"/>
-      <c r="BW11" s="191"/>
-      <c r="CT11" s="191"/>
+      <c r="AV11" s="179"/>
+      <c r="AW11" s="179"/>
+      <c r="AX11" s="196"/>
+      <c r="AY11" s="197"/>
+      <c r="AZ11" s="197"/>
+      <c r="BA11" s="197"/>
+      <c r="BB11" s="197"/>
+      <c r="BC11" s="197"/>
+      <c r="BD11" s="197"/>
+      <c r="BE11" s="197"/>
+      <c r="BF11" s="199"/>
+      <c r="BG11" s="199"/>
+      <c r="BT11" s="179"/>
+      <c r="BW11" s="179"/>
+      <c r="CT11" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="CT4:CT11"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+    <mergeCell ref="AM2:BI2"/>
+    <mergeCell ref="BJ2:CD2"/>
+    <mergeCell ref="BW4:BW11"/>
+    <mergeCell ref="CE2:CS2"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="K4:K11"/>
+    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="M4:M11"/>
+    <mergeCell ref="N4:N11"/>
+    <mergeCell ref="O4:O11"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="AV4:AV11"/>
@@ -4227,63 +4289,6 @@
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="I4:I11"/>
     <mergeCell ref="J4:J11"/>
-    <mergeCell ref="CT4:CT11"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="R2:AL2"/>
-    <mergeCell ref="AM2:BI2"/>
-    <mergeCell ref="BJ2:CD2"/>
-    <mergeCell ref="BW4:BW11"/>
-    <mergeCell ref="CE2:CS2"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="K4:K11"/>
-    <mergeCell ref="L4:L11"/>
-    <mergeCell ref="M4:M11"/>
-    <mergeCell ref="N4:N11"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5805,13 +5810,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="213" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="214"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5916,9 +5921,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="203"/>
-      <c r="B5" s="201"/>
-      <c r="C5" s="203"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="211"/>
+      <c r="C5" s="201"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -6023,11 +6028,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="203"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="203"/>
+      <c r="C6" s="201"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6132,11 +6137,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="203"/>
+      <c r="A7" s="201"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="203"/>
+      <c r="C7" s="201"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6241,11 +6246,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="203"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="203"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6350,11 +6355,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="203"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="203"/>
+      <c r="C9" s="201"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6459,11 +6464,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="203"/>
+      <c r="A10" s="201"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="203"/>
+      <c r="C10" s="201"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6568,11 +6573,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="203"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="203"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6677,9 +6682,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="203"/>
+      <c r="A12" s="201"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="206"/>
+      <c r="C12" s="202"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6784,10 +6789,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="207" t="s">
+      <c r="A13" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="208" t="s">
+      <c r="B13" s="216" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6896,8 +6901,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="203"/>
-      <c r="B14" s="209"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="207"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -7018,7 +7023,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="203"/>
+      <c r="A15" s="201"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7128,7 +7133,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="203"/>
+      <c r="A16" s="201"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7238,7 +7243,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="203"/>
+      <c r="A17" s="201"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7350,7 +7355,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203"/>
+      <c r="A18" s="201"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7460,7 +7465,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203"/>
+      <c r="A19" s="201"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7570,7 +7575,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="203"/>
+      <c r="A20" s="201"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7680,7 +7685,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="206"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7791,7 +7796,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="200" t="s">
+      <c r="B22" s="210" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7901,7 +7906,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="201"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -8008,13 +8013,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="203" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="213">
+      <c r="C24" s="205">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8122,11 +8127,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="212"/>
+      <c r="A25" s="204"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="203"/>
+      <c r="C25" s="201"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8232,11 +8237,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="212"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="203"/>
+      <c r="C26" s="201"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8342,11 +8347,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="212"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="203"/>
+      <c r="C27" s="201"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8452,11 +8457,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="212"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="203"/>
+      <c r="C28" s="201"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8562,11 +8567,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="212"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="203"/>
+      <c r="C29" s="201"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8672,11 +8677,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="212"/>
+      <c r="A30" s="204"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="203"/>
+      <c r="C30" s="201"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8782,11 +8787,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="212"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="203"/>
+      <c r="C31" s="201"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8892,11 +8897,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="212"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="203"/>
+      <c r="C32" s="201"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -9002,11 +9007,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="212"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="203"/>
+      <c r="C33" s="201"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9112,11 +9117,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="212"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="203"/>
+      <c r="C34" s="201"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9222,11 +9227,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="212"/>
+      <c r="A35" s="204"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="206"/>
+      <c r="C35" s="202"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9332,11 +9337,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="212"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="213">
+      <c r="C36" s="205">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9444,11 +9449,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="212"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="203"/>
+      <c r="C37" s="201"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9554,11 +9559,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="212"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="203"/>
+      <c r="C38" s="201"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9664,11 +9669,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="212"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="203"/>
+      <c r="C39" s="201"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9774,11 +9779,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="212"/>
+      <c r="A40" s="204"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="203"/>
+      <c r="C40" s="201"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9884,11 +9889,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="212"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="203"/>
+      <c r="C41" s="201"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9994,11 +9999,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="212"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="203"/>
+      <c r="C42" s="201"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10104,11 +10109,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="212"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="203"/>
+      <c r="C43" s="201"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10214,11 +10219,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="212"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="203"/>
+      <c r="C44" s="201"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10324,11 +10329,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="212"/>
+      <c r="A45" s="204"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="203"/>
+      <c r="C45" s="201"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10434,11 +10439,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="212"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="203"/>
+      <c r="C46" s="201"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10544,11 +10549,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="212"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="203"/>
+      <c r="C47" s="201"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10662,11 +10667,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="212"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="203"/>
+      <c r="C48" s="201"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10775,7 +10780,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="214" t="s">
+      <c r="B49" s="206" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10885,7 +10890,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="209"/>
+      <c r="B50" s="207"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14316,7 +14321,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="215" t="s">
+      <c r="A81" s="208" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14428,7 +14433,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="203"/>
+      <c r="A82" s="201"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14538,7 +14543,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="203"/>
+      <c r="A83" s="201"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14648,7 +14653,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="203"/>
+      <c r="A84" s="201"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14758,7 +14763,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="203"/>
+      <c r="A85" s="201"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14868,7 +14873,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="203"/>
+      <c r="A86" s="201"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14978,7 +14983,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="203"/>
+      <c r="A87" s="201"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15090,7 +15095,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="203"/>
+      <c r="A88" s="201"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15200,7 +15205,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="203"/>
+      <c r="A89" s="201"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15310,7 +15315,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="203"/>
+      <c r="A90" s="201"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15420,11 +15425,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="203"/>
+      <c r="A91" s="201"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="216"/>
+      <c r="C91" s="209"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15530,11 +15535,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="203"/>
+      <c r="A92" s="201"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="203"/>
+      <c r="C92" s="201"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15640,11 +15645,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="206"/>
+      <c r="A93" s="202"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="203"/>
+      <c r="C93" s="201"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15868,7 +15873,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="210" t="s">
+      <c r="A95" s="200" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15980,7 +15985,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="203"/>
+      <c r="A96" s="201"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16090,7 +16095,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="203"/>
+      <c r="A97" s="201"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16200,7 +16205,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="203"/>
+      <c r="A98" s="201"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16310,7 +16315,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="203"/>
+      <c r="A99" s="201"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16420,7 +16425,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="203"/>
+      <c r="A100" s="201"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16530,7 +16535,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="203"/>
+      <c r="A101" s="201"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16640,7 +16645,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="203"/>
+      <c r="A102" s="201"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16750,7 +16755,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="203"/>
+      <c r="A103" s="201"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16862,7 +16867,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="203"/>
+      <c r="A104" s="201"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16972,7 +16977,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="203"/>
+      <c r="A105" s="201"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17090,7 +17095,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="203"/>
+      <c r="A106" s="201"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17200,7 +17205,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="203"/>
+      <c r="A107" s="201"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17310,7 +17315,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="203"/>
+      <c r="A108" s="201"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17420,7 +17425,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="203"/>
+      <c r="A109" s="201"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17530,7 +17535,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="203"/>
+      <c r="A110" s="201"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17640,7 +17645,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="203"/>
+      <c r="A111" s="201"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17750,7 +17755,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="203"/>
+      <c r="A112" s="201"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17860,7 +17865,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="203"/>
+      <c r="A113" s="201"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17970,7 +17975,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="203"/>
+      <c r="A114" s="201"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18080,7 +18085,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="203"/>
+      <c r="A115" s="201"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18190,7 +18195,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="203"/>
+      <c r="A116" s="201"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18316,7 +18321,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="203"/>
+      <c r="A117" s="201"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18426,7 +18431,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="206"/>
+      <c r="A118" s="202"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25797,6 +25802,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25804,12 +25815,6 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias de 07 a 11-10
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0404403F-A70B-4DF1-9E0B-00A2CF2D5404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7A2D30-9BDF-470C-B3CD-0E4ABFF8A4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="185">
   <si>
     <t>S</t>
   </si>
@@ -753,6 +753,18 @@
   <si>
     <t>Ajustes nos sites e reunião com a Linx</t>
   </si>
+  <si>
+    <t>Exercícios modelagem BD</t>
+  </si>
+  <si>
+    <t>Modelagem e criação do banco de dados do projeto Gufos</t>
+  </si>
+  <si>
+    <t>Não foi possível realizar acompanhamento devido às atividades do SAEP</t>
+  </si>
+  <si>
+    <t>Nossa Sra Aparecida</t>
+  </si>
 </sst>
 </file>
 
@@ -1068,7 +1080,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="70">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -1931,12 +1943,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2279,10 +2311,6 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2325,15 +2353,6 @@
     <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2342,6 +2361,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2894,10 +2919,10 @@
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AM4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ4" sqref="AQ4:AQ11"/>
+      <selection pane="bottomRight" activeCell="AY4" sqref="AY4:AY11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3206,110 +3231,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="180" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182" t="s">
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
+      <c r="N2" s="180"/>
+      <c r="O2" s="180"/>
+      <c r="P2" s="180"/>
+      <c r="Q2" s="180"/>
+      <c r="R2" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="182"/>
-      <c r="AA2" s="182"/>
-      <c r="AB2" s="182"/>
-      <c r="AC2" s="182"/>
-      <c r="AD2" s="182"/>
-      <c r="AE2" s="182"/>
-      <c r="AF2" s="182"/>
-      <c r="AG2" s="182"/>
-      <c r="AH2" s="182"/>
-      <c r="AI2" s="182"/>
-      <c r="AJ2" s="182"/>
-      <c r="AK2" s="182"/>
-      <c r="AL2" s="182"/>
-      <c r="AM2" s="182" t="s">
+      <c r="S2" s="180"/>
+      <c r="T2" s="180"/>
+      <c r="U2" s="180"/>
+      <c r="V2" s="180"/>
+      <c r="W2" s="180"/>
+      <c r="X2" s="180"/>
+      <c r="Y2" s="180"/>
+      <c r="Z2" s="180"/>
+      <c r="AA2" s="180"/>
+      <c r="AB2" s="180"/>
+      <c r="AC2" s="180"/>
+      <c r="AD2" s="180"/>
+      <c r="AE2" s="180"/>
+      <c r="AF2" s="180"/>
+      <c r="AG2" s="180"/>
+      <c r="AH2" s="180"/>
+      <c r="AI2" s="180"/>
+      <c r="AJ2" s="180"/>
+      <c r="AK2" s="180"/>
+      <c r="AL2" s="180"/>
+      <c r="AM2" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="182"/>
-      <c r="AO2" s="182"/>
-      <c r="AP2" s="182"/>
-      <c r="AQ2" s="182"/>
-      <c r="AR2" s="182"/>
-      <c r="AS2" s="182"/>
-      <c r="AT2" s="182"/>
-      <c r="AU2" s="182"/>
-      <c r="AV2" s="182"/>
-      <c r="AW2" s="182"/>
-      <c r="AX2" s="183"/>
-      <c r="AY2" s="183"/>
-      <c r="AZ2" s="183"/>
-      <c r="BA2" s="183"/>
-      <c r="BB2" s="183"/>
-      <c r="BC2" s="183"/>
-      <c r="BD2" s="183"/>
-      <c r="BE2" s="183"/>
-      <c r="BF2" s="183"/>
-      <c r="BG2" s="183"/>
-      <c r="BH2" s="183"/>
-      <c r="BI2" s="183"/>
-      <c r="BJ2" s="182" t="s">
+      <c r="AN2" s="180"/>
+      <c r="AO2" s="180"/>
+      <c r="AP2" s="180"/>
+      <c r="AQ2" s="180"/>
+      <c r="AR2" s="180"/>
+      <c r="AS2" s="180"/>
+      <c r="AT2" s="180"/>
+      <c r="AU2" s="180"/>
+      <c r="AV2" s="180"/>
+      <c r="AW2" s="180"/>
+      <c r="AX2" s="181"/>
+      <c r="AY2" s="181"/>
+      <c r="AZ2" s="181"/>
+      <c r="BA2" s="181"/>
+      <c r="BB2" s="181"/>
+      <c r="BC2" s="181"/>
+      <c r="BD2" s="181"/>
+      <c r="BE2" s="181"/>
+      <c r="BF2" s="181"/>
+      <c r="BG2" s="181"/>
+      <c r="BH2" s="181"/>
+      <c r="BI2" s="181"/>
+      <c r="BJ2" s="180" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="182"/>
-      <c r="BL2" s="182"/>
-      <c r="BM2" s="182"/>
-      <c r="BN2" s="182"/>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="182"/>
-      <c r="BT2" s="182"/>
-      <c r="BU2" s="182"/>
-      <c r="BV2" s="182"/>
-      <c r="BW2" s="182"/>
-      <c r="BX2" s="184"/>
-      <c r="BY2" s="184"/>
-      <c r="BZ2" s="184"/>
-      <c r="CA2" s="184"/>
-      <c r="CB2" s="184"/>
-      <c r="CC2" s="184"/>
-      <c r="CD2" s="184"/>
-      <c r="CE2" s="185" t="s">
+      <c r="BK2" s="180"/>
+      <c r="BL2" s="180"/>
+      <c r="BM2" s="180"/>
+      <c r="BN2" s="180"/>
+      <c r="BO2" s="180"/>
+      <c r="BP2" s="180"/>
+      <c r="BQ2" s="180"/>
+      <c r="BR2" s="180"/>
+      <c r="BS2" s="180"/>
+      <c r="BT2" s="180"/>
+      <c r="BU2" s="180"/>
+      <c r="BV2" s="180"/>
+      <c r="BW2" s="180"/>
+      <c r="BX2" s="182"/>
+      <c r="BY2" s="182"/>
+      <c r="BZ2" s="182"/>
+      <c r="CA2" s="182"/>
+      <c r="CB2" s="182"/>
+      <c r="CC2" s="182"/>
+      <c r="CD2" s="182"/>
+      <c r="CE2" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="186"/>
-      <c r="CG2" s="186"/>
-      <c r="CH2" s="186"/>
-      <c r="CI2" s="186"/>
-      <c r="CJ2" s="186"/>
-      <c r="CK2" s="186"/>
-      <c r="CL2" s="186"/>
-      <c r="CM2" s="186"/>
-      <c r="CN2" s="186"/>
-      <c r="CO2" s="186"/>
-      <c r="CP2" s="186"/>
-      <c r="CQ2" s="186"/>
-      <c r="CR2" s="186"/>
-      <c r="CS2" s="186"/>
+      <c r="CF2" s="184"/>
+      <c r="CG2" s="184"/>
+      <c r="CH2" s="184"/>
+      <c r="CI2" s="184"/>
+      <c r="CJ2" s="184"/>
+      <c r="CK2" s="184"/>
+      <c r="CL2" s="184"/>
+      <c r="CM2" s="184"/>
+      <c r="CN2" s="184"/>
+      <c r="CO2" s="184"/>
+      <c r="CP2" s="184"/>
+      <c r="CQ2" s="184"/>
+      <c r="CR2" s="184"/>
+      <c r="CS2" s="184"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3604,618 +3629,632 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="178" t="s">
+    <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="176" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="178"/>
+      <c r="D4" s="179" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="181" t="s">
+      <c r="E4" s="179" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="181" t="s">
+      <c r="F4" s="179" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="181" t="s">
+      <c r="G4" s="179" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="181" t="s">
+      <c r="H4" s="179" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="181" t="s">
+      <c r="I4" s="179" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="181" t="s">
+      <c r="J4" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="179" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="187" t="s">
+      <c r="L4" s="185" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="187" t="s">
+      <c r="M4" s="185" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="187" t="s">
+      <c r="N4" s="185" t="s">
         <v>151</v>
       </c>
-      <c r="O4" s="187" t="s">
+      <c r="O4" s="185" t="s">
         <v>153</v>
       </c>
-      <c r="P4" s="187" t="s">
+      <c r="P4" s="185" t="s">
         <v>154</v>
       </c>
-      <c r="Q4" s="187" t="s">
+      <c r="Q4" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="R4" s="187" t="s">
+      <c r="R4" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="S4" s="187" t="s">
+      <c r="S4" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="187" t="s">
+      <c r="T4" s="185" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="187" t="s">
+      <c r="U4" s="185" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="187" t="s">
+      <c r="V4" s="185" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="188" t="s">
+      <c r="W4" s="186" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="188" t="s">
+      <c r="X4" s="186" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="188" t="s">
+      <c r="Y4" s="186" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="188" t="s">
+      <c r="Z4" s="186" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="188" t="s">
+      <c r="AA4" s="186" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="189" t="s">
+      <c r="AB4" s="187" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="189" t="s">
+      <c r="AC4" s="187" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="189" t="s">
+      <c r="AD4" s="187" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="189" t="s">
+      <c r="AE4" s="187" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="189" t="s">
+      <c r="AF4" s="187" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="189" t="s">
+      <c r="AG4" s="187" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="189" t="s">
+      <c r="AH4" s="187" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="189" t="s">
+      <c r="AI4" s="187" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="189" t="s">
+      <c r="AJ4" s="187" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="189" t="s">
+      <c r="AK4" s="187" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" s="189" t="s">
+      <c r="AL4" s="187" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" s="189" t="s">
+      <c r="AM4" s="187" t="s">
         <v>177</v>
       </c>
-      <c r="AN4" s="189" t="s">
+      <c r="AN4" s="187" t="s">
         <v>178</v>
       </c>
-      <c r="AO4" s="189" t="s">
+      <c r="AO4" s="187" t="s">
         <v>179</v>
       </c>
-      <c r="AP4" s="189" t="s">
+      <c r="AP4" s="187" t="s">
         <v>180</v>
       </c>
-      <c r="AQ4" s="189"/>
-      <c r="AR4" s="192"/>
-      <c r="AS4" s="192"/>
-      <c r="AT4" s="192"/>
-      <c r="AU4" s="176"/>
-      <c r="AV4" s="179"/>
-      <c r="AW4" s="179"/>
-      <c r="AX4" s="195"/>
-      <c r="AY4" s="197"/>
-      <c r="AZ4" s="197"/>
-      <c r="BA4" s="197"/>
-      <c r="BB4" s="197"/>
-      <c r="BC4" s="197"/>
-      <c r="BD4" s="197"/>
-      <c r="BE4" s="197"/>
-      <c r="BF4" s="198"/>
-      <c r="BG4" s="198"/>
-      <c r="BT4" s="179"/>
-      <c r="BW4" s="179"/>
-      <c r="CT4" s="179"/>
-    </row>
-    <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="178"/>
-      <c r="B5" s="180" t="s">
+      <c r="AQ4" s="187" t="s">
+        <v>183</v>
+      </c>
+      <c r="AR4" s="187" t="s">
+        <v>183</v>
+      </c>
+      <c r="AS4" s="187" t="s">
+        <v>183</v>
+      </c>
+      <c r="AT4" s="187" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU4" s="193" t="s">
+        <v>182</v>
+      </c>
+      <c r="AV4" s="177" t="s">
+        <v>184</v>
+      </c>
+      <c r="AW4" s="177" t="s">
+        <v>184</v>
+      </c>
+      <c r="AX4" s="190"/>
+      <c r="AY4" s="192"/>
+      <c r="AZ4" s="192"/>
+      <c r="BA4" s="192"/>
+      <c r="BB4" s="192"/>
+      <c r="BC4" s="192"/>
+      <c r="BD4" s="192"/>
+      <c r="BE4" s="192"/>
+      <c r="BF4" s="195"/>
+      <c r="BG4" s="195"/>
+      <c r="BT4" s="177"/>
+      <c r="BW4" s="177"/>
+      <c r="CT4" s="177"/>
+    </row>
+    <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="176"/>
+      <c r="B5" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="188"/>
-      <c r="X5" s="188"/>
-      <c r="Y5" s="188"/>
-      <c r="Z5" s="188"/>
-      <c r="AA5" s="188"/>
-      <c r="AB5" s="190"/>
-      <c r="AC5" s="190"/>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="190"/>
-      <c r="AH5" s="190"/>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="190"/>
-      <c r="AK5" s="190"/>
-      <c r="AL5" s="190"/>
-      <c r="AM5" s="190"/>
-      <c r="AN5" s="190"/>
-      <c r="AO5" s="190"/>
-      <c r="AP5" s="190"/>
-      <c r="AQ5" s="190"/>
-      <c r="AR5" s="193"/>
-      <c r="AS5" s="193"/>
-      <c r="AT5" s="193"/>
-      <c r="AU5" s="176"/>
-      <c r="AV5" s="179"/>
-      <c r="AW5" s="179"/>
-      <c r="AX5" s="196"/>
-      <c r="AY5" s="197"/>
-      <c r="AZ5" s="197"/>
-      <c r="BA5" s="197"/>
-      <c r="BB5" s="197"/>
-      <c r="BC5" s="197"/>
-      <c r="BD5" s="197"/>
-      <c r="BE5" s="197"/>
-      <c r="BF5" s="199"/>
-      <c r="BG5" s="199"/>
-      <c r="BT5" s="179"/>
-      <c r="BW5" s="179"/>
-      <c r="CT5" s="179"/>
-    </row>
-    <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="178"/>
-      <c r="B6" s="180" t="s">
+      <c r="C5" s="178"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
+      <c r="G5" s="179"/>
+      <c r="H5" s="179"/>
+      <c r="I5" s="179"/>
+      <c r="J5" s="179"/>
+      <c r="K5" s="179"/>
+      <c r="L5" s="185"/>
+      <c r="M5" s="185"/>
+      <c r="N5" s="185"/>
+      <c r="O5" s="185"/>
+      <c r="P5" s="185"/>
+      <c r="Q5" s="185"/>
+      <c r="R5" s="185"/>
+      <c r="S5" s="185"/>
+      <c r="T5" s="185"/>
+      <c r="U5" s="185"/>
+      <c r="V5" s="185"/>
+      <c r="W5" s="186"/>
+      <c r="X5" s="186"/>
+      <c r="Y5" s="186"/>
+      <c r="Z5" s="186"/>
+      <c r="AA5" s="186"/>
+      <c r="AB5" s="188"/>
+      <c r="AC5" s="188"/>
+      <c r="AD5" s="188"/>
+      <c r="AE5" s="188"/>
+      <c r="AF5" s="188"/>
+      <c r="AG5" s="188"/>
+      <c r="AH5" s="188"/>
+      <c r="AI5" s="188"/>
+      <c r="AJ5" s="188"/>
+      <c r="AK5" s="188"/>
+      <c r="AL5" s="188"/>
+      <c r="AM5" s="188"/>
+      <c r="AN5" s="188"/>
+      <c r="AO5" s="188"/>
+      <c r="AP5" s="188"/>
+      <c r="AQ5" s="188"/>
+      <c r="AR5" s="188"/>
+      <c r="AS5" s="188"/>
+      <c r="AT5" s="188"/>
+      <c r="AU5" s="194"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="AX5" s="191"/>
+      <c r="AY5" s="192"/>
+      <c r="AZ5" s="192"/>
+      <c r="BA5" s="192"/>
+      <c r="BB5" s="192"/>
+      <c r="BC5" s="192"/>
+      <c r="BD5" s="192"/>
+      <c r="BE5" s="192"/>
+      <c r="BF5" s="196"/>
+      <c r="BG5" s="196"/>
+      <c r="BT5" s="177"/>
+      <c r="BW5" s="177"/>
+      <c r="CT5" s="177"/>
+    </row>
+    <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="176"/>
+      <c r="B6" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="181"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="181"/>
-      <c r="J6" s="181"/>
-      <c r="K6" s="181"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
-      <c r="X6" s="188"/>
-      <c r="Y6" s="188"/>
-      <c r="Z6" s="188"/>
-      <c r="AA6" s="188"/>
-      <c r="AB6" s="190"/>
-      <c r="AC6" s="190"/>
-      <c r="AD6" s="190"/>
-      <c r="AE6" s="190"/>
-      <c r="AF6" s="190"/>
-      <c r="AG6" s="190"/>
-      <c r="AH6" s="190"/>
-      <c r="AI6" s="190"/>
-      <c r="AJ6" s="190"/>
-      <c r="AK6" s="190"/>
-      <c r="AL6" s="190"/>
-      <c r="AM6" s="190"/>
-      <c r="AN6" s="190"/>
-      <c r="AO6" s="190"/>
-      <c r="AP6" s="190"/>
-      <c r="AQ6" s="190"/>
-      <c r="AR6" s="193"/>
-      <c r="AS6" s="193"/>
-      <c r="AT6" s="193"/>
-      <c r="AU6" s="176"/>
-      <c r="AV6" s="179"/>
-      <c r="AW6" s="179"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="197"/>
-      <c r="AZ6" s="197"/>
-      <c r="BA6" s="197"/>
-      <c r="BB6" s="197"/>
-      <c r="BC6" s="197"/>
-      <c r="BD6" s="197"/>
-      <c r="BE6" s="197"/>
-      <c r="BF6" s="199"/>
-      <c r="BG6" s="199"/>
-      <c r="BT6" s="179"/>
-      <c r="BW6" s="179"/>
-      <c r="CT6" s="179"/>
-    </row>
-    <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="178"/>
-      <c r="B7" s="180" t="s">
+      <c r="C6" s="178"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
+      <c r="G6" s="179"/>
+      <c r="H6" s="179"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="179"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="185"/>
+      <c r="M6" s="185"/>
+      <c r="N6" s="185"/>
+      <c r="O6" s="185"/>
+      <c r="P6" s="185"/>
+      <c r="Q6" s="185"/>
+      <c r="R6" s="185"/>
+      <c r="S6" s="185"/>
+      <c r="T6" s="185"/>
+      <c r="U6" s="185"/>
+      <c r="V6" s="185"/>
+      <c r="W6" s="186"/>
+      <c r="X6" s="186"/>
+      <c r="Y6" s="186"/>
+      <c r="Z6" s="186"/>
+      <c r="AA6" s="186"/>
+      <c r="AB6" s="188"/>
+      <c r="AC6" s="188"/>
+      <c r="AD6" s="188"/>
+      <c r="AE6" s="188"/>
+      <c r="AF6" s="188"/>
+      <c r="AG6" s="188"/>
+      <c r="AH6" s="188"/>
+      <c r="AI6" s="188"/>
+      <c r="AJ6" s="188"/>
+      <c r="AK6" s="188"/>
+      <c r="AL6" s="188"/>
+      <c r="AM6" s="188"/>
+      <c r="AN6" s="188"/>
+      <c r="AO6" s="188"/>
+      <c r="AP6" s="188"/>
+      <c r="AQ6" s="188"/>
+      <c r="AR6" s="188"/>
+      <c r="AS6" s="188"/>
+      <c r="AT6" s="188"/>
+      <c r="AU6" s="194"/>
+      <c r="AV6" s="177"/>
+      <c r="AW6" s="177"/>
+      <c r="AX6" s="191"/>
+      <c r="AY6" s="192"/>
+      <c r="AZ6" s="192"/>
+      <c r="BA6" s="192"/>
+      <c r="BB6" s="192"/>
+      <c r="BC6" s="192"/>
+      <c r="BD6" s="192"/>
+      <c r="BE6" s="192"/>
+      <c r="BF6" s="196"/>
+      <c r="BG6" s="196"/>
+      <c r="BT6" s="177"/>
+      <c r="BW6" s="177"/>
+      <c r="CT6" s="177"/>
+    </row>
+    <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="176"/>
+      <c r="B7" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="181"/>
-      <c r="E7" s="181"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="181"/>
-      <c r="H7" s="181"/>
-      <c r="I7" s="181"/>
-      <c r="J7" s="181"/>
-      <c r="K7" s="181"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="188"/>
-      <c r="X7" s="188"/>
-      <c r="Y7" s="188"/>
-      <c r="Z7" s="188"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="190"/>
-      <c r="AC7" s="190"/>
-      <c r="AD7" s="190"/>
-      <c r="AE7" s="190"/>
-      <c r="AF7" s="190"/>
-      <c r="AG7" s="190"/>
-      <c r="AH7" s="190"/>
-      <c r="AI7" s="190"/>
-      <c r="AJ7" s="190"/>
-      <c r="AK7" s="190"/>
-      <c r="AL7" s="190"/>
-      <c r="AM7" s="190"/>
-      <c r="AN7" s="190"/>
-      <c r="AO7" s="190"/>
-      <c r="AP7" s="190"/>
-      <c r="AQ7" s="190"/>
-      <c r="AR7" s="193"/>
-      <c r="AS7" s="193"/>
-      <c r="AT7" s="193"/>
-      <c r="AU7" s="177"/>
-      <c r="AV7" s="179"/>
-      <c r="AW7" s="179"/>
-      <c r="AX7" s="196"/>
-      <c r="AY7" s="197"/>
-      <c r="AZ7" s="197"/>
-      <c r="BA7" s="197"/>
-      <c r="BB7" s="197"/>
-      <c r="BC7" s="197"/>
-      <c r="BD7" s="197"/>
-      <c r="BE7" s="197"/>
-      <c r="BF7" s="199"/>
-      <c r="BG7" s="199"/>
-      <c r="BT7" s="179"/>
-      <c r="BW7" s="179"/>
-      <c r="CT7" s="179"/>
-    </row>
-    <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="178" t="s">
+      <c r="C7" s="178"/>
+      <c r="D7" s="179"/>
+      <c r="E7" s="179"/>
+      <c r="F7" s="179"/>
+      <c r="G7" s="179"/>
+      <c r="H7" s="179"/>
+      <c r="I7" s="179"/>
+      <c r="J7" s="179"/>
+      <c r="K7" s="179"/>
+      <c r="L7" s="185"/>
+      <c r="M7" s="185"/>
+      <c r="N7" s="185"/>
+      <c r="O7" s="185"/>
+      <c r="P7" s="185"/>
+      <c r="Q7" s="185"/>
+      <c r="R7" s="185"/>
+      <c r="S7" s="185"/>
+      <c r="T7" s="185"/>
+      <c r="U7" s="185"/>
+      <c r="V7" s="185"/>
+      <c r="W7" s="186"/>
+      <c r="X7" s="186"/>
+      <c r="Y7" s="186"/>
+      <c r="Z7" s="186"/>
+      <c r="AA7" s="186"/>
+      <c r="AB7" s="188"/>
+      <c r="AC7" s="188"/>
+      <c r="AD7" s="188"/>
+      <c r="AE7" s="188"/>
+      <c r="AF7" s="188"/>
+      <c r="AG7" s="188"/>
+      <c r="AH7" s="188"/>
+      <c r="AI7" s="188"/>
+      <c r="AJ7" s="188"/>
+      <c r="AK7" s="188"/>
+      <c r="AL7" s="188"/>
+      <c r="AM7" s="188"/>
+      <c r="AN7" s="188"/>
+      <c r="AO7" s="188"/>
+      <c r="AP7" s="188"/>
+      <c r="AQ7" s="188"/>
+      <c r="AR7" s="188"/>
+      <c r="AS7" s="188"/>
+      <c r="AT7" s="188"/>
+      <c r="AU7" s="194"/>
+      <c r="AV7" s="177"/>
+      <c r="AW7" s="177"/>
+      <c r="AX7" s="191"/>
+      <c r="AY7" s="192"/>
+      <c r="AZ7" s="192"/>
+      <c r="BA7" s="192"/>
+      <c r="BB7" s="192"/>
+      <c r="BC7" s="192"/>
+      <c r="BD7" s="192"/>
+      <c r="BE7" s="192"/>
+      <c r="BF7" s="196"/>
+      <c r="BG7" s="196"/>
+      <c r="BT7" s="177"/>
+      <c r="BW7" s="177"/>
+      <c r="CT7" s="177"/>
+    </row>
+    <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="176" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="180" t="s">
+      <c r="B8" s="178" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="187"/>
-      <c r="M8" s="187"/>
-      <c r="N8" s="187"/>
-      <c r="O8" s="187"/>
-      <c r="P8" s="187"/>
-      <c r="Q8" s="187"/>
-      <c r="R8" s="187"/>
-      <c r="S8" s="187"/>
-      <c r="T8" s="187"/>
-      <c r="U8" s="187"/>
-      <c r="V8" s="187"/>
-      <c r="W8" s="188"/>
-      <c r="X8" s="188"/>
-      <c r="Y8" s="188"/>
-      <c r="Z8" s="188"/>
-      <c r="AA8" s="188"/>
-      <c r="AB8" s="190"/>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="190"/>
-      <c r="AG8" s="190"/>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="190"/>
-      <c r="AL8" s="190"/>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="190"/>
-      <c r="AQ8" s="190"/>
-      <c r="AR8" s="193"/>
-      <c r="AS8" s="193"/>
-      <c r="AT8" s="193"/>
-      <c r="AU8" s="177"/>
-      <c r="AV8" s="179"/>
-      <c r="AW8" s="179"/>
-      <c r="AX8" s="196"/>
-      <c r="AY8" s="197"/>
-      <c r="AZ8" s="197"/>
-      <c r="BA8" s="197"/>
-      <c r="BB8" s="197"/>
-      <c r="BC8" s="197"/>
-      <c r="BD8" s="197"/>
-      <c r="BE8" s="197"/>
-      <c r="BF8" s="199"/>
-      <c r="BG8" s="199"/>
-      <c r="BT8" s="179"/>
-      <c r="BW8" s="179"/>
-      <c r="CT8" s="179"/>
-    </row>
-    <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="178"/>
-      <c r="B9" s="180" t="s">
+      <c r="C8" s="178"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="179"/>
+      <c r="H8" s="179"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="179"/>
+      <c r="K8" s="179"/>
+      <c r="L8" s="185"/>
+      <c r="M8" s="185"/>
+      <c r="N8" s="185"/>
+      <c r="O8" s="185"/>
+      <c r="P8" s="185"/>
+      <c r="Q8" s="185"/>
+      <c r="R8" s="185"/>
+      <c r="S8" s="185"/>
+      <c r="T8" s="185"/>
+      <c r="U8" s="185"/>
+      <c r="V8" s="185"/>
+      <c r="W8" s="186"/>
+      <c r="X8" s="186"/>
+      <c r="Y8" s="186"/>
+      <c r="Z8" s="186"/>
+      <c r="AA8" s="186"/>
+      <c r="AB8" s="188"/>
+      <c r="AC8" s="188"/>
+      <c r="AD8" s="188"/>
+      <c r="AE8" s="188"/>
+      <c r="AF8" s="188"/>
+      <c r="AG8" s="188"/>
+      <c r="AH8" s="188"/>
+      <c r="AI8" s="188"/>
+      <c r="AJ8" s="188"/>
+      <c r="AK8" s="188"/>
+      <c r="AL8" s="188"/>
+      <c r="AM8" s="188"/>
+      <c r="AN8" s="188"/>
+      <c r="AO8" s="188"/>
+      <c r="AP8" s="188"/>
+      <c r="AQ8" s="188"/>
+      <c r="AR8" s="188"/>
+      <c r="AS8" s="188"/>
+      <c r="AT8" s="188"/>
+      <c r="AU8" s="194"/>
+      <c r="AV8" s="177"/>
+      <c r="AW8" s="177"/>
+      <c r="AX8" s="191"/>
+      <c r="AY8" s="192"/>
+      <c r="AZ8" s="192"/>
+      <c r="BA8" s="192"/>
+      <c r="BB8" s="192"/>
+      <c r="BC8" s="192"/>
+      <c r="BD8" s="192"/>
+      <c r="BE8" s="192"/>
+      <c r="BF8" s="196"/>
+      <c r="BG8" s="196"/>
+      <c r="BT8" s="177"/>
+      <c r="BW8" s="177"/>
+      <c r="CT8" s="177"/>
+    </row>
+    <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="176"/>
+      <c r="B9" s="178" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="180"/>
-      <c r="D9" s="181"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="187"/>
-      <c r="M9" s="187"/>
-      <c r="N9" s="187"/>
-      <c r="O9" s="187"/>
-      <c r="P9" s="187"/>
-      <c r="Q9" s="187"/>
-      <c r="R9" s="187"/>
-      <c r="S9" s="187"/>
-      <c r="T9" s="187"/>
-      <c r="U9" s="187"/>
-      <c r="V9" s="187"/>
-      <c r="W9" s="188"/>
-      <c r="X9" s="188"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="188"/>
-      <c r="AA9" s="188"/>
-      <c r="AB9" s="190"/>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="190"/>
-      <c r="AG9" s="190"/>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="190"/>
-      <c r="AL9" s="190"/>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="190"/>
-      <c r="AQ9" s="190"/>
-      <c r="AR9" s="193"/>
-      <c r="AS9" s="193"/>
-      <c r="AT9" s="193"/>
-      <c r="AU9" s="177"/>
-      <c r="AV9" s="179"/>
-      <c r="AW9" s="179"/>
-      <c r="AX9" s="196"/>
-      <c r="AY9" s="197"/>
-      <c r="AZ9" s="197"/>
-      <c r="BA9" s="197"/>
-      <c r="BB9" s="197"/>
-      <c r="BC9" s="197"/>
-      <c r="BD9" s="197"/>
-      <c r="BE9" s="197"/>
-      <c r="BF9" s="199"/>
-      <c r="BG9" s="199"/>
-      <c r="BT9" s="179"/>
-      <c r="BW9" s="179"/>
-      <c r="CT9" s="179"/>
-    </row>
-    <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="178"/>
-      <c r="B10" s="180" t="s">
+      <c r="C9" s="178"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="179"/>
+      <c r="K9" s="179"/>
+      <c r="L9" s="185"/>
+      <c r="M9" s="185"/>
+      <c r="N9" s="185"/>
+      <c r="O9" s="185"/>
+      <c r="P9" s="185"/>
+      <c r="Q9" s="185"/>
+      <c r="R9" s="185"/>
+      <c r="S9" s="185"/>
+      <c r="T9" s="185"/>
+      <c r="U9" s="185"/>
+      <c r="V9" s="185"/>
+      <c r="W9" s="186"/>
+      <c r="X9" s="186"/>
+      <c r="Y9" s="186"/>
+      <c r="Z9" s="186"/>
+      <c r="AA9" s="186"/>
+      <c r="AB9" s="188"/>
+      <c r="AC9" s="188"/>
+      <c r="AD9" s="188"/>
+      <c r="AE9" s="188"/>
+      <c r="AF9" s="188"/>
+      <c r="AG9" s="188"/>
+      <c r="AH9" s="188"/>
+      <c r="AI9" s="188"/>
+      <c r="AJ9" s="188"/>
+      <c r="AK9" s="188"/>
+      <c r="AL9" s="188"/>
+      <c r="AM9" s="188"/>
+      <c r="AN9" s="188"/>
+      <c r="AO9" s="188"/>
+      <c r="AP9" s="188"/>
+      <c r="AQ9" s="188"/>
+      <c r="AR9" s="188"/>
+      <c r="AS9" s="188"/>
+      <c r="AT9" s="188"/>
+      <c r="AU9" s="194"/>
+      <c r="AV9" s="177"/>
+      <c r="AW9" s="177"/>
+      <c r="AX9" s="191"/>
+      <c r="AY9" s="192"/>
+      <c r="AZ9" s="192"/>
+      <c r="BA9" s="192"/>
+      <c r="BB9" s="192"/>
+      <c r="BC9" s="192"/>
+      <c r="BD9" s="192"/>
+      <c r="BE9" s="192"/>
+      <c r="BF9" s="196"/>
+      <c r="BG9" s="196"/>
+      <c r="BT9" s="177"/>
+      <c r="BW9" s="177"/>
+      <c r="CT9" s="177"/>
+    </row>
+    <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="176"/>
+      <c r="B10" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="187"/>
-      <c r="M10" s="187"/>
-      <c r="N10" s="187"/>
-      <c r="O10" s="187"/>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="U10" s="187"/>
-      <c r="V10" s="187"/>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AB10" s="190"/>
-      <c r="AC10" s="190"/>
-      <c r="AD10" s="190"/>
-      <c r="AE10" s="190"/>
-      <c r="AF10" s="190"/>
-      <c r="AG10" s="190"/>
-      <c r="AH10" s="190"/>
-      <c r="AI10" s="190"/>
-      <c r="AJ10" s="190"/>
-      <c r="AK10" s="190"/>
-      <c r="AL10" s="190"/>
-      <c r="AM10" s="190"/>
-      <c r="AN10" s="190"/>
-      <c r="AO10" s="190"/>
-      <c r="AP10" s="190"/>
-      <c r="AQ10" s="190"/>
-      <c r="AR10" s="193"/>
-      <c r="AS10" s="193"/>
-      <c r="AT10" s="193"/>
-      <c r="AU10" s="177"/>
-      <c r="AV10" s="179"/>
-      <c r="AW10" s="179"/>
-      <c r="AX10" s="196"/>
-      <c r="AY10" s="197"/>
-      <c r="AZ10" s="197"/>
-      <c r="BA10" s="197"/>
-      <c r="BB10" s="197"/>
-      <c r="BC10" s="197"/>
-      <c r="BD10" s="197"/>
-      <c r="BE10" s="197"/>
-      <c r="BF10" s="199"/>
-      <c r="BG10" s="199"/>
-      <c r="BT10" s="179"/>
-      <c r="BW10" s="179"/>
-      <c r="CT10" s="179"/>
-    </row>
-    <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="178"/>
-      <c r="B11" s="180" t="s">
+      <c r="C10" s="178"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="179"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="179"/>
+      <c r="K10" s="179"/>
+      <c r="L10" s="185"/>
+      <c r="M10" s="185"/>
+      <c r="N10" s="185"/>
+      <c r="O10" s="185"/>
+      <c r="P10" s="185"/>
+      <c r="Q10" s="185"/>
+      <c r="R10" s="185"/>
+      <c r="S10" s="185"/>
+      <c r="T10" s="185"/>
+      <c r="U10" s="185"/>
+      <c r="V10" s="185"/>
+      <c r="W10" s="186"/>
+      <c r="X10" s="186"/>
+      <c r="Y10" s="186"/>
+      <c r="Z10" s="186"/>
+      <c r="AA10" s="186"/>
+      <c r="AB10" s="188"/>
+      <c r="AC10" s="188"/>
+      <c r="AD10" s="188"/>
+      <c r="AE10" s="188"/>
+      <c r="AF10" s="188"/>
+      <c r="AG10" s="188"/>
+      <c r="AH10" s="188"/>
+      <c r="AI10" s="188"/>
+      <c r="AJ10" s="188"/>
+      <c r="AK10" s="188"/>
+      <c r="AL10" s="188"/>
+      <c r="AM10" s="188"/>
+      <c r="AN10" s="188"/>
+      <c r="AO10" s="188"/>
+      <c r="AP10" s="188"/>
+      <c r="AQ10" s="188"/>
+      <c r="AR10" s="188"/>
+      <c r="AS10" s="188"/>
+      <c r="AT10" s="188"/>
+      <c r="AU10" s="194"/>
+      <c r="AV10" s="177"/>
+      <c r="AW10" s="177"/>
+      <c r="AX10" s="191"/>
+      <c r="AY10" s="192"/>
+      <c r="AZ10" s="192"/>
+      <c r="BA10" s="192"/>
+      <c r="BB10" s="192"/>
+      <c r="BC10" s="192"/>
+      <c r="BD10" s="192"/>
+      <c r="BE10" s="192"/>
+      <c r="BF10" s="196"/>
+      <c r="BG10" s="196"/>
+      <c r="BT10" s="177"/>
+      <c r="BW10" s="177"/>
+      <c r="CT10" s="177"/>
+    </row>
+    <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="176"/>
+      <c r="B11" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="181"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="181"/>
-      <c r="H11" s="181"/>
-      <c r="I11" s="181"/>
-      <c r="J11" s="181"/>
-      <c r="K11" s="181"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
-      <c r="X11" s="188"/>
-      <c r="Y11" s="188"/>
-      <c r="Z11" s="188"/>
-      <c r="AA11" s="188"/>
-      <c r="AB11" s="191"/>
-      <c r="AC11" s="191"/>
-      <c r="AD11" s="191"/>
-      <c r="AE11" s="191"/>
-      <c r="AF11" s="191"/>
-      <c r="AG11" s="191"/>
-      <c r="AH11" s="191"/>
-      <c r="AI11" s="191"/>
-      <c r="AJ11" s="191"/>
-      <c r="AK11" s="191"/>
-      <c r="AL11" s="191"/>
-      <c r="AM11" s="191"/>
-      <c r="AN11" s="191"/>
-      <c r="AO11" s="191"/>
-      <c r="AP11" s="191"/>
-      <c r="AQ11" s="191"/>
-      <c r="AR11" s="194"/>
-      <c r="AS11" s="194"/>
-      <c r="AT11" s="194"/>
-      <c r="AU11" s="177"/>
-      <c r="AV11" s="179"/>
-      <c r="AW11" s="179"/>
-      <c r="AX11" s="196"/>
-      <c r="AY11" s="197"/>
-      <c r="AZ11" s="197"/>
-      <c r="BA11" s="197"/>
-      <c r="BB11" s="197"/>
-      <c r="BC11" s="197"/>
-      <c r="BD11" s="197"/>
-      <c r="BE11" s="197"/>
-      <c r="BF11" s="199"/>
-      <c r="BG11" s="199"/>
-      <c r="BT11" s="179"/>
-      <c r="BW11" s="179"/>
-      <c r="CT11" s="179"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="179"/>
+      <c r="E11" s="179"/>
+      <c r="F11" s="179"/>
+      <c r="G11" s="179"/>
+      <c r="H11" s="179"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="179"/>
+      <c r="K11" s="179"/>
+      <c r="L11" s="185"/>
+      <c r="M11" s="185"/>
+      <c r="N11" s="185"/>
+      <c r="O11" s="185"/>
+      <c r="P11" s="185"/>
+      <c r="Q11" s="185"/>
+      <c r="R11" s="185"/>
+      <c r="S11" s="185"/>
+      <c r="T11" s="185"/>
+      <c r="U11" s="185"/>
+      <c r="V11" s="185"/>
+      <c r="W11" s="186"/>
+      <c r="X11" s="186"/>
+      <c r="Y11" s="186"/>
+      <c r="Z11" s="186"/>
+      <c r="AA11" s="186"/>
+      <c r="AB11" s="189"/>
+      <c r="AC11" s="189"/>
+      <c r="AD11" s="189"/>
+      <c r="AE11" s="189"/>
+      <c r="AF11" s="189"/>
+      <c r="AG11" s="189"/>
+      <c r="AH11" s="189"/>
+      <c r="AI11" s="189"/>
+      <c r="AJ11" s="189"/>
+      <c r="AK11" s="189"/>
+      <c r="AL11" s="189"/>
+      <c r="AM11" s="189"/>
+      <c r="AN11" s="189"/>
+      <c r="AO11" s="189"/>
+      <c r="AP11" s="189"/>
+      <c r="AQ11" s="189"/>
+      <c r="AR11" s="189"/>
+      <c r="AS11" s="189"/>
+      <c r="AT11" s="189"/>
+      <c r="AU11" s="194"/>
+      <c r="AV11" s="177"/>
+      <c r="AW11" s="177"/>
+      <c r="AX11" s="191"/>
+      <c r="AY11" s="192"/>
+      <c r="AZ11" s="192"/>
+      <c r="BA11" s="192"/>
+      <c r="BB11" s="192"/>
+      <c r="BC11" s="192"/>
+      <c r="BD11" s="192"/>
+      <c r="BE11" s="192"/>
+      <c r="BF11" s="196"/>
+      <c r="BG11" s="196"/>
+      <c r="BT11" s="177"/>
+      <c r="BW11" s="177"/>
+      <c r="CT11" s="177"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="74">
     <mergeCell ref="BG4:BG11"/>
     <mergeCell ref="BB4:BB11"/>
     <mergeCell ref="BC4:BC11"/>
@@ -4227,6 +4266,7 @@
     <mergeCell ref="AY4:AY11"/>
     <mergeCell ref="AZ4:AZ11"/>
     <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AU4:AU11"/>
     <mergeCell ref="AO4:AO11"/>
     <mergeCell ref="AP4:AP11"/>
     <mergeCell ref="AQ4:AQ11"/>
@@ -5810,13 +5850,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="212" t="s">
+      <c r="A4" s="209" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="210" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="214"/>
+      <c r="C4" s="211"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5921,9 +5961,9 @@
       <c r="DA4" s="62"/>
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="201"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="201"/>
+      <c r="A5" s="198"/>
+      <c r="B5" s="208"/>
+      <c r="C5" s="198"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -6028,11 +6068,11 @@
       <c r="DA5" s="64"/>
     </row>
     <row r="6" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="201"/>
+      <c r="A6" s="198"/>
       <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="201"/>
+      <c r="C6" s="198"/>
       <c r="D6" s="66"/>
       <c r="E6" s="61"/>
       <c r="F6" s="61"/>
@@ -6137,11 +6177,11 @@
       <c r="DA6" s="64"/>
     </row>
     <row r="7" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="201"/>
+      <c r="A7" s="198"/>
       <c r="B7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="201"/>
+      <c r="C7" s="198"/>
       <c r="D7" s="66"/>
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
@@ -6246,11 +6286,11 @@
       <c r="DA7" s="64"/>
     </row>
     <row r="8" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201"/>
+      <c r="A8" s="198"/>
       <c r="B8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="201"/>
+      <c r="C8" s="198"/>
       <c r="D8" s="66"/>
       <c r="E8" s="61"/>
       <c r="F8" s="61"/>
@@ -6355,11 +6395,11 @@
       <c r="DA8" s="64"/>
     </row>
     <row r="9" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+      <c r="A9" s="198"/>
       <c r="B9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="201"/>
+      <c r="C9" s="198"/>
       <c r="D9" s="66"/>
       <c r="E9" s="61"/>
       <c r="F9" s="61"/>
@@ -6464,11 +6504,11 @@
       <c r="DA9" s="64"/>
     </row>
     <row r="10" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+      <c r="A10" s="198"/>
       <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="198"/>
       <c r="D10" s="66"/>
       <c r="E10" s="61"/>
       <c r="F10" s="61"/>
@@ -6573,11 +6613,11 @@
       <c r="DA10" s="64"/>
     </row>
     <row r="11" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
+      <c r="A11" s="198"/>
       <c r="B11" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="198"/>
       <c r="D11" s="66"/>
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
@@ -6682,9 +6722,9 @@
       <c r="DA11" s="64"/>
     </row>
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="201"/>
+      <c r="A12" s="198"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="202"/>
+      <c r="C12" s="199"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6789,10 +6829,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="215" t="s">
+      <c r="A13" s="212" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="213" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -6901,8 +6941,8 @@
       <c r="DB13" s="83"/>
     </row>
     <row r="14" spans="1:106" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="201"/>
-      <c r="B14" s="207"/>
+      <c r="A14" s="198"/>
+      <c r="B14" s="204"/>
       <c r="C14" s="84"/>
       <c r="D14" s="76"/>
       <c r="E14" s="77"/>
@@ -7023,7 +7063,7 @@
       <c r="DB14" s="83"/>
     </row>
     <row r="15" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="201"/>
+      <c r="A15" s="198"/>
       <c r="B15" s="87" t="s">
         <v>32</v>
       </c>
@@ -7133,7 +7173,7 @@
       <c r="DB15" s="83"/>
     </row>
     <row r="16" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="198"/>
       <c r="B16" s="88" t="s">
         <v>33</v>
       </c>
@@ -7243,7 +7283,7 @@
       <c r="DB16" s="83"/>
     </row>
     <row r="17" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="198"/>
       <c r="B17" s="88" t="s">
         <v>34</v>
       </c>
@@ -7355,7 +7395,7 @@
       <c r="DB17" s="83"/>
     </row>
     <row r="18" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
+      <c r="A18" s="198"/>
       <c r="B18" s="88" t="s">
         <v>35</v>
       </c>
@@ -7465,7 +7505,7 @@
       <c r="DB18" s="83"/>
     </row>
     <row r="19" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
+      <c r="A19" s="198"/>
       <c r="B19" s="88" t="s">
         <v>36</v>
       </c>
@@ -7575,7 +7615,7 @@
       <c r="DB19" s="83"/>
     </row>
     <row r="20" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="201"/>
+      <c r="A20" s="198"/>
       <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
@@ -7685,7 +7725,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="202"/>
+      <c r="A21" s="199"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7796,7 +7836,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="207" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7906,7 +7946,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="211"/>
+      <c r="B23" s="208"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -8013,13 +8053,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="203" t="s">
+      <c r="A24" s="200" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="205">
+      <c r="C24" s="202">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8127,11 +8167,11 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="204"/>
+      <c r="A25" s="201"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="201"/>
+      <c r="C25" s="198"/>
       <c r="D25" s="104"/>
       <c r="E25" s="98"/>
       <c r="F25" s="98"/>
@@ -8237,11 +8277,11 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="204"/>
+      <c r="A26" s="201"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="201"/>
+      <c r="C26" s="198"/>
       <c r="D26" s="104"/>
       <c r="E26" s="98"/>
       <c r="F26" s="98"/>
@@ -8347,11 +8387,11 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="204"/>
+      <c r="A27" s="201"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="201"/>
+      <c r="C27" s="198"/>
       <c r="D27" s="104"/>
       <c r="E27" s="98"/>
       <c r="F27" s="98"/>
@@ -8457,11 +8497,11 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="204"/>
+      <c r="A28" s="201"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="201"/>
+      <c r="C28" s="198"/>
       <c r="D28" s="104"/>
       <c r="E28" s="98"/>
       <c r="F28" s="98"/>
@@ -8567,11 +8607,11 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="204"/>
+      <c r="A29" s="201"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="201"/>
+      <c r="C29" s="198"/>
       <c r="D29" s="104"/>
       <c r="E29" s="98"/>
       <c r="F29" s="98"/>
@@ -8677,11 +8717,11 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="204"/>
+      <c r="A30" s="201"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="201"/>
+      <c r="C30" s="198"/>
       <c r="D30" s="104"/>
       <c r="E30" s="98"/>
       <c r="F30" s="98"/>
@@ -8787,11 +8827,11 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="204"/>
+      <c r="A31" s="201"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="201"/>
+      <c r="C31" s="198"/>
       <c r="D31" s="104"/>
       <c r="E31" s="98"/>
       <c r="F31" s="98"/>
@@ -8897,11 +8937,11 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="204"/>
+      <c r="A32" s="201"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="201"/>
+      <c r="C32" s="198"/>
       <c r="D32" s="104"/>
       <c r="E32" s="98"/>
       <c r="F32" s="98"/>
@@ -9007,11 +9047,11 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="204"/>
+      <c r="A33" s="201"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="201"/>
+      <c r="C33" s="198"/>
       <c r="D33" s="104"/>
       <c r="E33" s="98"/>
       <c r="F33" s="98"/>
@@ -9117,11 +9157,11 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="204"/>
+      <c r="A34" s="201"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="201"/>
+      <c r="C34" s="198"/>
       <c r="D34" s="104"/>
       <c r="E34" s="98"/>
       <c r="F34" s="98"/>
@@ -9227,11 +9267,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="204"/>
+      <c r="A35" s="201"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="202"/>
+      <c r="C35" s="199"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9337,11 +9377,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="204"/>
+      <c r="A36" s="201"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="205">
+      <c r="C36" s="202">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9449,11 +9489,11 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="204"/>
+      <c r="A37" s="201"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="201"/>
+      <c r="C37" s="198"/>
       <c r="D37" s="104"/>
       <c r="E37" s="98"/>
       <c r="F37" s="98"/>
@@ -9559,11 +9599,11 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="204"/>
+      <c r="A38" s="201"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="201"/>
+      <c r="C38" s="198"/>
       <c r="D38" s="104"/>
       <c r="E38" s="98"/>
       <c r="F38" s="98"/>
@@ -9669,11 +9709,11 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="204"/>
+      <c r="A39" s="201"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="201"/>
+      <c r="C39" s="198"/>
       <c r="D39" s="104"/>
       <c r="E39" s="98"/>
       <c r="F39" s="98"/>
@@ -9779,11 +9819,11 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="204"/>
+      <c r="A40" s="201"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="201"/>
+      <c r="C40" s="198"/>
       <c r="D40" s="104"/>
       <c r="E40" s="98"/>
       <c r="F40" s="98"/>
@@ -9889,11 +9929,11 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="204"/>
+      <c r="A41" s="201"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="201"/>
+      <c r="C41" s="198"/>
       <c r="D41" s="104"/>
       <c r="E41" s="98"/>
       <c r="F41" s="98"/>
@@ -9999,11 +10039,11 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="204"/>
+      <c r="A42" s="201"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="201"/>
+      <c r="C42" s="198"/>
       <c r="D42" s="104"/>
       <c r="E42" s="98"/>
       <c r="F42" s="98"/>
@@ -10109,11 +10149,11 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="204"/>
+      <c r="A43" s="201"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="201"/>
+      <c r="C43" s="198"/>
       <c r="D43" s="104"/>
       <c r="E43" s="98"/>
       <c r="F43" s="98"/>
@@ -10219,11 +10259,11 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="204"/>
+      <c r="A44" s="201"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="201"/>
+      <c r="C44" s="198"/>
       <c r="D44" s="104"/>
       <c r="E44" s="98"/>
       <c r="F44" s="98"/>
@@ -10329,11 +10369,11 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="204"/>
+      <c r="A45" s="201"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="198"/>
       <c r="D45" s="104"/>
       <c r="E45" s="98"/>
       <c r="F45" s="98"/>
@@ -10439,11 +10479,11 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="204"/>
+      <c r="A46" s="201"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="201"/>
+      <c r="C46" s="198"/>
       <c r="D46" s="104"/>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
@@ -10549,11 +10589,11 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="204"/>
+      <c r="A47" s="201"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="201"/>
+      <c r="C47" s="198"/>
       <c r="D47" s="104"/>
       <c r="E47" s="98"/>
       <c r="F47" s="98"/>
@@ -10667,11 +10707,11 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="204"/>
+      <c r="A48" s="201"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="201"/>
+      <c r="C48" s="198"/>
       <c r="D48" s="104"/>
       <c r="E48" s="98"/>
       <c r="F48" s="98"/>
@@ -10780,7 +10820,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="203" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -10890,7 +10930,7 @@
     </row>
     <row r="50" spans="1:106" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="116"/>
-      <c r="B50" s="207"/>
+      <c r="B50" s="204"/>
       <c r="C50" s="116"/>
       <c r="D50" s="112"/>
       <c r="E50" s="113"/>
@@ -14321,7 +14361,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="208" t="s">
+      <c r="A81" s="205" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -14433,7 +14473,7 @@
       <c r="DB81" s="129"/>
     </row>
     <row r="82" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="201"/>
+      <c r="A82" s="198"/>
       <c r="B82" s="130" t="s">
         <v>100</v>
       </c>
@@ -14543,7 +14583,7 @@
       <c r="DB82" s="129"/>
     </row>
     <row r="83" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="201"/>
+      <c r="A83" s="198"/>
       <c r="B83" s="130" t="s">
         <v>101</v>
       </c>
@@ -14653,7 +14693,7 @@
       <c r="DB83" s="129"/>
     </row>
     <row r="84" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="201"/>
+      <c r="A84" s="198"/>
       <c r="B84" s="130" t="s">
         <v>102</v>
       </c>
@@ -14763,7 +14803,7 @@
       <c r="DB84" s="129"/>
     </row>
     <row r="85" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="201"/>
+      <c r="A85" s="198"/>
       <c r="B85" s="130" t="s">
         <v>103</v>
       </c>
@@ -14873,7 +14913,7 @@
       <c r="DB85" s="129"/>
     </row>
     <row r="86" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="201"/>
+      <c r="A86" s="198"/>
       <c r="B86" s="130" t="s">
         <v>104</v>
       </c>
@@ -14983,7 +15023,7 @@
       <c r="DB86" s="129"/>
     </row>
     <row r="87" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="201"/>
+      <c r="A87" s="198"/>
       <c r="B87" s="130" t="s">
         <v>105</v>
       </c>
@@ -15095,7 +15135,7 @@
       <c r="DB87" s="129"/>
     </row>
     <row r="88" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="201"/>
+      <c r="A88" s="198"/>
       <c r="B88" s="130" t="s">
         <v>106</v>
       </c>
@@ -15205,7 +15245,7 @@
       <c r="DB88" s="129"/>
     </row>
     <row r="89" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="201"/>
+      <c r="A89" s="198"/>
       <c r="B89" s="130" t="s">
         <v>107</v>
       </c>
@@ -15315,7 +15355,7 @@
       <c r="DB89" s="129"/>
     </row>
     <row r="90" spans="1:106" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="201"/>
+      <c r="A90" s="198"/>
       <c r="B90" s="130" t="s">
         <v>108</v>
       </c>
@@ -15425,11 +15465,11 @@
       <c r="DB90" s="129"/>
     </row>
     <row r="91" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="201"/>
+      <c r="A91" s="198"/>
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="209"/>
+      <c r="C91" s="206"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15535,11 +15575,11 @@
       <c r="DB91" s="129"/>
     </row>
     <row r="92" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="201"/>
+      <c r="A92" s="198"/>
       <c r="B92" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="198"/>
       <c r="D92" s="124"/>
       <c r="E92" s="125"/>
       <c r="F92" s="125"/>
@@ -15645,11 +15685,11 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="202"/>
+      <c r="A93" s="199"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="C93" s="201"/>
+      <c r="C93" s="198"/>
       <c r="D93" s="124"/>
       <c r="E93" s="125"/>
       <c r="F93" s="125"/>
@@ -15873,7 +15913,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="200" t="s">
+      <c r="A95" s="197" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -15985,7 +16025,7 @@
       <c r="DB95" s="141"/>
     </row>
     <row r="96" spans="1:106" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="201"/>
+      <c r="A96" s="198"/>
       <c r="B96" s="142" t="s">
         <v>114</v>
       </c>
@@ -16095,7 +16135,7 @@
       <c r="DB96" s="141"/>
     </row>
     <row r="97" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="201"/>
+      <c r="A97" s="198"/>
       <c r="B97" s="145" t="s">
         <v>115</v>
       </c>
@@ -16205,7 +16245,7 @@
       <c r="DB97" s="141"/>
     </row>
     <row r="98" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="201"/>
+      <c r="A98" s="198"/>
       <c r="B98" s="145" t="s">
         <v>116</v>
       </c>
@@ -16315,7 +16355,7 @@
       <c r="DB98" s="141"/>
     </row>
     <row r="99" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="201"/>
+      <c r="A99" s="198"/>
       <c r="B99" s="145" t="s">
         <v>117</v>
       </c>
@@ -16425,7 +16465,7 @@
       <c r="DB99" s="141"/>
     </row>
     <row r="100" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="201"/>
+      <c r="A100" s="198"/>
       <c r="B100" s="145" t="s">
         <v>118</v>
       </c>
@@ -16535,7 +16575,7 @@
       <c r="DB100" s="141"/>
     </row>
     <row r="101" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="201"/>
+      <c r="A101" s="198"/>
       <c r="B101" s="145" t="s">
         <v>119</v>
       </c>
@@ -16645,7 +16685,7 @@
       <c r="DB101" s="141"/>
     </row>
     <row r="102" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="201"/>
+      <c r="A102" s="198"/>
       <c r="B102" s="145" t="s">
         <v>120</v>
       </c>
@@ -16755,7 +16795,7 @@
       <c r="DB102" s="141"/>
     </row>
     <row r="103" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="201"/>
+      <c r="A103" s="198"/>
       <c r="B103" s="145" t="s">
         <v>121</v>
       </c>
@@ -16867,7 +16907,7 @@
       <c r="DB103" s="141"/>
     </row>
     <row r="104" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="201"/>
+      <c r="A104" s="198"/>
       <c r="B104" s="145" t="s">
         <v>122</v>
       </c>
@@ -16977,7 +17017,7 @@
       <c r="DB104" s="141"/>
     </row>
     <row r="105" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="201"/>
+      <c r="A105" s="198"/>
       <c r="B105" s="148" t="s">
         <v>123</v>
       </c>
@@ -17095,7 +17135,7 @@
       <c r="DB105" s="141"/>
     </row>
     <row r="106" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="201"/>
+      <c r="A106" s="198"/>
       <c r="B106" s="149" t="s">
         <v>125</v>
       </c>
@@ -17205,7 +17245,7 @@
       <c r="DB106" s="141"/>
     </row>
     <row r="107" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="201"/>
+      <c r="A107" s="198"/>
       <c r="B107" s="150" t="s">
         <v>126</v>
       </c>
@@ -17315,7 +17355,7 @@
       <c r="DB107" s="141"/>
     </row>
     <row r="108" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="201"/>
+      <c r="A108" s="198"/>
       <c r="B108" s="145" t="s">
         <v>127</v>
       </c>
@@ -17425,7 +17465,7 @@
       <c r="DB108" s="141"/>
     </row>
     <row r="109" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="201"/>
+      <c r="A109" s="198"/>
       <c r="B109" s="145" t="s">
         <v>128</v>
       </c>
@@ -17535,7 +17575,7 @@
       <c r="DB109" s="141"/>
     </row>
     <row r="110" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="201"/>
+      <c r="A110" s="198"/>
       <c r="B110" s="145" t="s">
         <v>129</v>
       </c>
@@ -17645,7 +17685,7 @@
       <c r="DB110" s="141"/>
     </row>
     <row r="111" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="201"/>
+      <c r="A111" s="198"/>
       <c r="B111" s="145" t="s">
         <v>130</v>
       </c>
@@ -17755,7 +17795,7 @@
       <c r="DB111" s="141"/>
     </row>
     <row r="112" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="201"/>
+      <c r="A112" s="198"/>
       <c r="B112" s="145" t="s">
         <v>131</v>
       </c>
@@ -17865,7 +17905,7 @@
       <c r="DB112" s="141"/>
     </row>
     <row r="113" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="201"/>
+      <c r="A113" s="198"/>
       <c r="B113" s="145" t="s">
         <v>132</v>
       </c>
@@ -17975,7 +18015,7 @@
       <c r="DB113" s="141"/>
     </row>
     <row r="114" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="201"/>
+      <c r="A114" s="198"/>
       <c r="B114" s="145" t="s">
         <v>133</v>
       </c>
@@ -18085,7 +18125,7 @@
       <c r="DB114" s="141"/>
     </row>
     <row r="115" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="201"/>
+      <c r="A115" s="198"/>
       <c r="B115" s="145" t="s">
         <v>134</v>
       </c>
@@ -18195,7 +18235,7 @@
       <c r="DB115" s="141"/>
     </row>
     <row r="116" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="201"/>
+      <c r="A116" s="198"/>
       <c r="B116" s="151" t="s">
         <v>135</v>
       </c>
@@ -18321,7 +18361,7 @@
       <c r="DB116" s="141"/>
     </row>
     <row r="117" spans="1:106" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="201"/>
+      <c r="A117" s="198"/>
       <c r="B117" s="148" t="s">
         <v>136</v>
       </c>
@@ -18431,7 +18471,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="202"/>
+      <c r="A118" s="199"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
Adiciona acompanhamento do dia 16-09
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7A2D30-9BDF-470C-B3CD-0E4ABFF8A4E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -27,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="186">
   <si>
     <t>S</t>
   </si>
@@ -765,11 +764,14 @@
   <si>
     <t>Nossa Sra Aparecida</t>
   </si>
+  <si>
+    <t>Modelagem do banco de dados do projeto Linx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2311,17 +2313,38 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2338,47 +2361,40 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2389,36 +2405,22 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2915,11 +2917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AS4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AY4" sqref="AY4:AY11"/>
@@ -3231,110 +3233,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="180" t="s">
+      <c r="D2" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
-      <c r="M2" s="180"/>
-      <c r="N2" s="180"/>
-      <c r="O2" s="180"/>
-      <c r="P2" s="180"/>
-      <c r="Q2" s="180"/>
-      <c r="R2" s="180" t="s">
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+      <c r="Q2" s="187"/>
+      <c r="R2" s="187" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="180"/>
-      <c r="T2" s="180"/>
-      <c r="U2" s="180"/>
-      <c r="V2" s="180"/>
-      <c r="W2" s="180"/>
-      <c r="X2" s="180"/>
-      <c r="Y2" s="180"/>
-      <c r="Z2" s="180"/>
-      <c r="AA2" s="180"/>
-      <c r="AB2" s="180"/>
-      <c r="AC2" s="180"/>
-      <c r="AD2" s="180"/>
-      <c r="AE2" s="180"/>
-      <c r="AF2" s="180"/>
-      <c r="AG2" s="180"/>
-      <c r="AH2" s="180"/>
-      <c r="AI2" s="180"/>
-      <c r="AJ2" s="180"/>
-      <c r="AK2" s="180"/>
-      <c r="AL2" s="180"/>
-      <c r="AM2" s="180" t="s">
+      <c r="S2" s="187"/>
+      <c r="T2" s="187"/>
+      <c r="U2" s="187"/>
+      <c r="V2" s="187"/>
+      <c r="W2" s="187"/>
+      <c r="X2" s="187"/>
+      <c r="Y2" s="187"/>
+      <c r="Z2" s="187"/>
+      <c r="AA2" s="187"/>
+      <c r="AB2" s="187"/>
+      <c r="AC2" s="187"/>
+      <c r="AD2" s="187"/>
+      <c r="AE2" s="187"/>
+      <c r="AF2" s="187"/>
+      <c r="AG2" s="187"/>
+      <c r="AH2" s="187"/>
+      <c r="AI2" s="187"/>
+      <c r="AJ2" s="187"/>
+      <c r="AK2" s="187"/>
+      <c r="AL2" s="187"/>
+      <c r="AM2" s="187" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="180"/>
-      <c r="AO2" s="180"/>
-      <c r="AP2" s="180"/>
-      <c r="AQ2" s="180"/>
-      <c r="AR2" s="180"/>
-      <c r="AS2" s="180"/>
-      <c r="AT2" s="180"/>
-      <c r="AU2" s="180"/>
-      <c r="AV2" s="180"/>
-      <c r="AW2" s="180"/>
-      <c r="AX2" s="181"/>
-      <c r="AY2" s="181"/>
-      <c r="AZ2" s="181"/>
-      <c r="BA2" s="181"/>
-      <c r="BB2" s="181"/>
-      <c r="BC2" s="181"/>
-      <c r="BD2" s="181"/>
-      <c r="BE2" s="181"/>
-      <c r="BF2" s="181"/>
-      <c r="BG2" s="181"/>
-      <c r="BH2" s="181"/>
-      <c r="BI2" s="181"/>
-      <c r="BJ2" s="180" t="s">
+      <c r="AN2" s="187"/>
+      <c r="AO2" s="187"/>
+      <c r="AP2" s="187"/>
+      <c r="AQ2" s="187"/>
+      <c r="AR2" s="187"/>
+      <c r="AS2" s="187"/>
+      <c r="AT2" s="187"/>
+      <c r="AU2" s="187"/>
+      <c r="AV2" s="187"/>
+      <c r="AW2" s="187"/>
+      <c r="AX2" s="188"/>
+      <c r="AY2" s="188"/>
+      <c r="AZ2" s="188"/>
+      <c r="BA2" s="188"/>
+      <c r="BB2" s="188"/>
+      <c r="BC2" s="188"/>
+      <c r="BD2" s="188"/>
+      <c r="BE2" s="188"/>
+      <c r="BF2" s="188"/>
+      <c r="BG2" s="188"/>
+      <c r="BH2" s="188"/>
+      <c r="BI2" s="188"/>
+      <c r="BJ2" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="BK2" s="180"/>
-      <c r="BL2" s="180"/>
-      <c r="BM2" s="180"/>
-      <c r="BN2" s="180"/>
-      <c r="BO2" s="180"/>
-      <c r="BP2" s="180"/>
-      <c r="BQ2" s="180"/>
-      <c r="BR2" s="180"/>
-      <c r="BS2" s="180"/>
-      <c r="BT2" s="180"/>
-      <c r="BU2" s="180"/>
-      <c r="BV2" s="180"/>
-      <c r="BW2" s="180"/>
-      <c r="BX2" s="182"/>
-      <c r="BY2" s="182"/>
-      <c r="BZ2" s="182"/>
-      <c r="CA2" s="182"/>
-      <c r="CB2" s="182"/>
-      <c r="CC2" s="182"/>
-      <c r="CD2" s="182"/>
-      <c r="CE2" s="183" t="s">
+      <c r="BK2" s="187"/>
+      <c r="BL2" s="187"/>
+      <c r="BM2" s="187"/>
+      <c r="BN2" s="187"/>
+      <c r="BO2" s="187"/>
+      <c r="BP2" s="187"/>
+      <c r="BQ2" s="187"/>
+      <c r="BR2" s="187"/>
+      <c r="BS2" s="187"/>
+      <c r="BT2" s="187"/>
+      <c r="BU2" s="187"/>
+      <c r="BV2" s="187"/>
+      <c r="BW2" s="187"/>
+      <c r="BX2" s="189"/>
+      <c r="BY2" s="189"/>
+      <c r="BZ2" s="189"/>
+      <c r="CA2" s="189"/>
+      <c r="CB2" s="189"/>
+      <c r="CC2" s="189"/>
+      <c r="CD2" s="189"/>
+      <c r="CE2" s="190" t="s">
         <v>8</v>
       </c>
-      <c r="CF2" s="184"/>
-      <c r="CG2" s="184"/>
-      <c r="CH2" s="184"/>
-      <c r="CI2" s="184"/>
-      <c r="CJ2" s="184"/>
-      <c r="CK2" s="184"/>
-      <c r="CL2" s="184"/>
-      <c r="CM2" s="184"/>
-      <c r="CN2" s="184"/>
-      <c r="CO2" s="184"/>
-      <c r="CP2" s="184"/>
-      <c r="CQ2" s="184"/>
-      <c r="CR2" s="184"/>
-      <c r="CS2" s="184"/>
+      <c r="CF2" s="191"/>
+      <c r="CG2" s="191"/>
+      <c r="CH2" s="191"/>
+      <c r="CI2" s="191"/>
+      <c r="CJ2" s="191"/>
+      <c r="CK2" s="191"/>
+      <c r="CL2" s="191"/>
+      <c r="CM2" s="191"/>
+      <c r="CN2" s="191"/>
+      <c r="CO2" s="191"/>
+      <c r="CP2" s="191"/>
+      <c r="CQ2" s="191"/>
+      <c r="CR2" s="191"/>
+      <c r="CS2" s="191"/>
       <c r="CT2" s="170"/>
     </row>
     <row r="3" spans="1:98" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -3630,35 +3632,35 @@
       </c>
     </row>
     <row r="4" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="193" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="194" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="D4" s="179" t="s">
+      <c r="C4" s="194"/>
+      <c r="D4" s="192" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="179" t="s">
+      <c r="E4" s="192" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="179" t="s">
+      <c r="F4" s="192" t="s">
         <v>145</v>
       </c>
-      <c r="G4" s="179" t="s">
+      <c r="G4" s="192" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="179" t="s">
+      <c r="H4" s="192" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="179" t="s">
+      <c r="I4" s="192" t="s">
         <v>147</v>
       </c>
-      <c r="J4" s="179" t="s">
+      <c r="J4" s="192" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="179" t="s">
+      <c r="K4" s="192" t="s">
         <v>149</v>
       </c>
       <c r="L4" s="185" t="s">
@@ -3694,115 +3696,117 @@
       <c r="V4" s="185" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="186" t="s">
+      <c r="W4" s="184" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="186" t="s">
+      <c r="X4" s="184" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="186" t="s">
+      <c r="Y4" s="184" t="s">
         <v>163</v>
       </c>
-      <c r="Z4" s="186" t="s">
+      <c r="Z4" s="184" t="s">
         <v>164</v>
       </c>
-      <c r="AA4" s="186" t="s">
+      <c r="AA4" s="184" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" s="187" t="s">
+      <c r="AB4" s="179" t="s">
         <v>166</v>
       </c>
-      <c r="AC4" s="187" t="s">
+      <c r="AC4" s="179" t="s">
         <v>167</v>
       </c>
-      <c r="AD4" s="187" t="s">
+      <c r="AD4" s="179" t="s">
         <v>168</v>
       </c>
-      <c r="AE4" s="187" t="s">
+      <c r="AE4" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="AF4" s="187" t="s">
+      <c r="AF4" s="179" t="s">
         <v>170</v>
       </c>
-      <c r="AG4" s="187" t="s">
+      <c r="AG4" s="179" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="187" t="s">
+      <c r="AH4" s="179" t="s">
         <v>172</v>
       </c>
-      <c r="AI4" s="187" t="s">
+      <c r="AI4" s="179" t="s">
         <v>174</v>
       </c>
-      <c r="AJ4" s="187" t="s">
+      <c r="AJ4" s="179" t="s">
         <v>173</v>
       </c>
-      <c r="AK4" s="187" t="s">
+      <c r="AK4" s="179" t="s">
         <v>175</v>
       </c>
-      <c r="AL4" s="187" t="s">
+      <c r="AL4" s="179" t="s">
         <v>176</v>
       </c>
-      <c r="AM4" s="187" t="s">
+      <c r="AM4" s="179" t="s">
         <v>177</v>
       </c>
-      <c r="AN4" s="187" t="s">
+      <c r="AN4" s="179" t="s">
         <v>178</v>
       </c>
-      <c r="AO4" s="187" t="s">
+      <c r="AO4" s="179" t="s">
         <v>179</v>
       </c>
-      <c r="AP4" s="187" t="s">
+      <c r="AP4" s="179" t="s">
         <v>180</v>
       </c>
-      <c r="AQ4" s="187" t="s">
+      <c r="AQ4" s="179" t="s">
         <v>183</v>
       </c>
-      <c r="AR4" s="187" t="s">
+      <c r="AR4" s="179" t="s">
         <v>183</v>
       </c>
-      <c r="AS4" s="187" t="s">
+      <c r="AS4" s="179" t="s">
         <v>183</v>
       </c>
-      <c r="AT4" s="187" t="s">
+      <c r="AT4" s="179" t="s">
         <v>181</v>
       </c>
-      <c r="AU4" s="193" t="s">
+      <c r="AU4" s="182" t="s">
         <v>182</v>
       </c>
-      <c r="AV4" s="177" t="s">
+      <c r="AV4" s="186" t="s">
         <v>184</v>
       </c>
-      <c r="AW4" s="177" t="s">
+      <c r="AW4" s="186" t="s">
         <v>184</v>
       </c>
-      <c r="AX4" s="190"/>
-      <c r="AY4" s="192"/>
-      <c r="AZ4" s="192"/>
-      <c r="BA4" s="192"/>
-      <c r="BB4" s="192"/>
-      <c r="BC4" s="192"/>
-      <c r="BD4" s="192"/>
-      <c r="BE4" s="192"/>
-      <c r="BF4" s="195"/>
-      <c r="BG4" s="195"/>
-      <c r="BT4" s="177"/>
-      <c r="BW4" s="177"/>
-      <c r="CT4" s="177"/>
+      <c r="AX4" s="212" t="s">
+        <v>185</v>
+      </c>
+      <c r="AY4" s="178"/>
+      <c r="AZ4" s="178"/>
+      <c r="BA4" s="178"/>
+      <c r="BB4" s="178"/>
+      <c r="BC4" s="178"/>
+      <c r="BD4" s="178"/>
+      <c r="BE4" s="178"/>
+      <c r="BF4" s="176"/>
+      <c r="BG4" s="176"/>
+      <c r="BT4" s="186"/>
+      <c r="BW4" s="186"/>
+      <c r="CT4" s="186"/>
     </row>
     <row r="5" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="176"/>
-      <c r="B5" s="178" t="s">
+      <c r="A5" s="193"/>
+      <c r="B5" s="194" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="178"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
-      <c r="G5" s="179"/>
-      <c r="H5" s="179"/>
-      <c r="I5" s="179"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="179"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="192"/>
+      <c r="F5" s="192"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="192"/>
+      <c r="K5" s="192"/>
       <c r="L5" s="185"/>
       <c r="M5" s="185"/>
       <c r="N5" s="185"/>
@@ -3814,61 +3818,61 @@
       <c r="T5" s="185"/>
       <c r="U5" s="185"/>
       <c r="V5" s="185"/>
-      <c r="W5" s="186"/>
-      <c r="X5" s="186"/>
-      <c r="Y5" s="186"/>
-      <c r="Z5" s="186"/>
-      <c r="AA5" s="186"/>
-      <c r="AB5" s="188"/>
-      <c r="AC5" s="188"/>
-      <c r="AD5" s="188"/>
-      <c r="AE5" s="188"/>
-      <c r="AF5" s="188"/>
-      <c r="AG5" s="188"/>
-      <c r="AH5" s="188"/>
-      <c r="AI5" s="188"/>
-      <c r="AJ5" s="188"/>
-      <c r="AK5" s="188"/>
-      <c r="AL5" s="188"/>
-      <c r="AM5" s="188"/>
-      <c r="AN5" s="188"/>
-      <c r="AO5" s="188"/>
-      <c r="AP5" s="188"/>
-      <c r="AQ5" s="188"/>
-      <c r="AR5" s="188"/>
-      <c r="AS5" s="188"/>
-      <c r="AT5" s="188"/>
-      <c r="AU5" s="194"/>
-      <c r="AV5" s="177"/>
-      <c r="AW5" s="177"/>
-      <c r="AX5" s="191"/>
-      <c r="AY5" s="192"/>
-      <c r="AZ5" s="192"/>
-      <c r="BA5" s="192"/>
-      <c r="BB5" s="192"/>
-      <c r="BC5" s="192"/>
-      <c r="BD5" s="192"/>
-      <c r="BE5" s="192"/>
-      <c r="BF5" s="196"/>
-      <c r="BG5" s="196"/>
-      <c r="BT5" s="177"/>
-      <c r="BW5" s="177"/>
-      <c r="CT5" s="177"/>
+      <c r="W5" s="184"/>
+      <c r="X5" s="184"/>
+      <c r="Y5" s="184"/>
+      <c r="Z5" s="184"/>
+      <c r="AA5" s="184"/>
+      <c r="AB5" s="180"/>
+      <c r="AC5" s="180"/>
+      <c r="AD5" s="180"/>
+      <c r="AE5" s="180"/>
+      <c r="AF5" s="180"/>
+      <c r="AG5" s="180"/>
+      <c r="AH5" s="180"/>
+      <c r="AI5" s="180"/>
+      <c r="AJ5" s="180"/>
+      <c r="AK5" s="180"/>
+      <c r="AL5" s="180"/>
+      <c r="AM5" s="180"/>
+      <c r="AN5" s="180"/>
+      <c r="AO5" s="180"/>
+      <c r="AP5" s="180"/>
+      <c r="AQ5" s="180"/>
+      <c r="AR5" s="180"/>
+      <c r="AS5" s="180"/>
+      <c r="AT5" s="180"/>
+      <c r="AU5" s="183"/>
+      <c r="AV5" s="186"/>
+      <c r="AW5" s="186"/>
+      <c r="AX5" s="213"/>
+      <c r="AY5" s="178"/>
+      <c r="AZ5" s="178"/>
+      <c r="BA5" s="178"/>
+      <c r="BB5" s="178"/>
+      <c r="BC5" s="178"/>
+      <c r="BD5" s="178"/>
+      <c r="BE5" s="178"/>
+      <c r="BF5" s="177"/>
+      <c r="BG5" s="177"/>
+      <c r="BT5" s="186"/>
+      <c r="BW5" s="186"/>
+      <c r="CT5" s="186"/>
     </row>
     <row r="6" spans="1:98" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="176"/>
-      <c r="B6" s="178" t="s">
+      <c r="A6" s="193"/>
+      <c r="B6" s="194" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
-      <c r="G6" s="179"/>
-      <c r="H6" s="179"/>
-      <c r="I6" s="179"/>
-      <c r="J6" s="179"/>
-      <c r="K6" s="179"/>
+      <c r="C6" s="194"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="192"/>
       <c r="L6" s="185"/>
       <c r="M6" s="185"/>
       <c r="N6" s="185"/>
@@ -3880,61 +3884,61 @@
       <c r="T6" s="185"/>
       <c r="U6" s="185"/>
       <c r="V6" s="185"/>
-      <c r="W6" s="186"/>
-      <c r="X6" s="186"/>
-      <c r="Y6" s="186"/>
-      <c r="Z6" s="186"/>
-      <c r="AA6" s="186"/>
-      <c r="AB6" s="188"/>
-      <c r="AC6" s="188"/>
-      <c r="AD6" s="188"/>
-      <c r="AE6" s="188"/>
-      <c r="AF6" s="188"/>
-      <c r="AG6" s="188"/>
-      <c r="AH6" s="188"/>
-      <c r="AI6" s="188"/>
-      <c r="AJ6" s="188"/>
-      <c r="AK6" s="188"/>
-      <c r="AL6" s="188"/>
-      <c r="AM6" s="188"/>
-      <c r="AN6" s="188"/>
-      <c r="AO6" s="188"/>
-      <c r="AP6" s="188"/>
-      <c r="AQ6" s="188"/>
-      <c r="AR6" s="188"/>
-      <c r="AS6" s="188"/>
-      <c r="AT6" s="188"/>
-      <c r="AU6" s="194"/>
-      <c r="AV6" s="177"/>
-      <c r="AW6" s="177"/>
-      <c r="AX6" s="191"/>
-      <c r="AY6" s="192"/>
-      <c r="AZ6" s="192"/>
-      <c r="BA6" s="192"/>
-      <c r="BB6" s="192"/>
-      <c r="BC6" s="192"/>
-      <c r="BD6" s="192"/>
-      <c r="BE6" s="192"/>
-      <c r="BF6" s="196"/>
-      <c r="BG6" s="196"/>
-      <c r="BT6" s="177"/>
-      <c r="BW6" s="177"/>
-      <c r="CT6" s="177"/>
+      <c r="W6" s="184"/>
+      <c r="X6" s="184"/>
+      <c r="Y6" s="184"/>
+      <c r="Z6" s="184"/>
+      <c r="AA6" s="184"/>
+      <c r="AB6" s="180"/>
+      <c r="AC6" s="180"/>
+      <c r="AD6" s="180"/>
+      <c r="AE6" s="180"/>
+      <c r="AF6" s="180"/>
+      <c r="AG6" s="180"/>
+      <c r="AH6" s="180"/>
+      <c r="AI6" s="180"/>
+      <c r="AJ6" s="180"/>
+      <c r="AK6" s="180"/>
+      <c r="AL6" s="180"/>
+      <c r="AM6" s="180"/>
+      <c r="AN6" s="180"/>
+      <c r="AO6" s="180"/>
+      <c r="AP6" s="180"/>
+      <c r="AQ6" s="180"/>
+      <c r="AR6" s="180"/>
+      <c r="AS6" s="180"/>
+      <c r="AT6" s="180"/>
+      <c r="AU6" s="183"/>
+      <c r="AV6" s="186"/>
+      <c r="AW6" s="186"/>
+      <c r="AX6" s="213"/>
+      <c r="AY6" s="178"/>
+      <c r="AZ6" s="178"/>
+      <c r="BA6" s="178"/>
+      <c r="BB6" s="178"/>
+      <c r="BC6" s="178"/>
+      <c r="BD6" s="178"/>
+      <c r="BE6" s="178"/>
+      <c r="BF6" s="177"/>
+      <c r="BG6" s="177"/>
+      <c r="BT6" s="186"/>
+      <c r="BW6" s="186"/>
+      <c r="CT6" s="186"/>
     </row>
     <row r="7" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="176"/>
-      <c r="B7" s="178" t="s">
+      <c r="A7" s="193"/>
+      <c r="B7" s="194" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="179"/>
-      <c r="E7" s="179"/>
-      <c r="F7" s="179"/>
-      <c r="G7" s="179"/>
-      <c r="H7" s="179"/>
-      <c r="I7" s="179"/>
-      <c r="J7" s="179"/>
-      <c r="K7" s="179"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="192"/>
+      <c r="F7" s="192"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="192"/>
+      <c r="J7" s="192"/>
+      <c r="K7" s="192"/>
       <c r="L7" s="185"/>
       <c r="M7" s="185"/>
       <c r="N7" s="185"/>
@@ -3946,63 +3950,63 @@
       <c r="T7" s="185"/>
       <c r="U7" s="185"/>
       <c r="V7" s="185"/>
-      <c r="W7" s="186"/>
-      <c r="X7" s="186"/>
-      <c r="Y7" s="186"/>
-      <c r="Z7" s="186"/>
-      <c r="AA7" s="186"/>
-      <c r="AB7" s="188"/>
-      <c r="AC7" s="188"/>
-      <c r="AD7" s="188"/>
-      <c r="AE7" s="188"/>
-      <c r="AF7" s="188"/>
-      <c r="AG7" s="188"/>
-      <c r="AH7" s="188"/>
-      <c r="AI7" s="188"/>
-      <c r="AJ7" s="188"/>
-      <c r="AK7" s="188"/>
-      <c r="AL7" s="188"/>
-      <c r="AM7" s="188"/>
-      <c r="AN7" s="188"/>
-      <c r="AO7" s="188"/>
-      <c r="AP7" s="188"/>
-      <c r="AQ7" s="188"/>
-      <c r="AR7" s="188"/>
-      <c r="AS7" s="188"/>
-      <c r="AT7" s="188"/>
-      <c r="AU7" s="194"/>
-      <c r="AV7" s="177"/>
-      <c r="AW7" s="177"/>
-      <c r="AX7" s="191"/>
-      <c r="AY7" s="192"/>
-      <c r="AZ7" s="192"/>
-      <c r="BA7" s="192"/>
-      <c r="BB7" s="192"/>
-      <c r="BC7" s="192"/>
-      <c r="BD7" s="192"/>
-      <c r="BE7" s="192"/>
-      <c r="BF7" s="196"/>
-      <c r="BG7" s="196"/>
-      <c r="BT7" s="177"/>
-      <c r="BW7" s="177"/>
-      <c r="CT7" s="177"/>
+      <c r="W7" s="184"/>
+      <c r="X7" s="184"/>
+      <c r="Y7" s="184"/>
+      <c r="Z7" s="184"/>
+      <c r="AA7" s="184"/>
+      <c r="AB7" s="180"/>
+      <c r="AC7" s="180"/>
+      <c r="AD7" s="180"/>
+      <c r="AE7" s="180"/>
+      <c r="AF7" s="180"/>
+      <c r="AG7" s="180"/>
+      <c r="AH7" s="180"/>
+      <c r="AI7" s="180"/>
+      <c r="AJ7" s="180"/>
+      <c r="AK7" s="180"/>
+      <c r="AL7" s="180"/>
+      <c r="AM7" s="180"/>
+      <c r="AN7" s="180"/>
+      <c r="AO7" s="180"/>
+      <c r="AP7" s="180"/>
+      <c r="AQ7" s="180"/>
+      <c r="AR7" s="180"/>
+      <c r="AS7" s="180"/>
+      <c r="AT7" s="180"/>
+      <c r="AU7" s="183"/>
+      <c r="AV7" s="186"/>
+      <c r="AW7" s="186"/>
+      <c r="AX7" s="213"/>
+      <c r="AY7" s="178"/>
+      <c r="AZ7" s="178"/>
+      <c r="BA7" s="178"/>
+      <c r="BB7" s="178"/>
+      <c r="BC7" s="178"/>
+      <c r="BD7" s="178"/>
+      <c r="BE7" s="178"/>
+      <c r="BF7" s="177"/>
+      <c r="BG7" s="177"/>
+      <c r="BT7" s="186"/>
+      <c r="BW7" s="186"/>
+      <c r="CT7" s="186"/>
     </row>
     <row r="8" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="193" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="178" t="s">
+      <c r="B8" s="194" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="178"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="179"/>
-      <c r="H8" s="179"/>
-      <c r="I8" s="179"/>
-      <c r="J8" s="179"/>
-      <c r="K8" s="179"/>
+      <c r="C8" s="194"/>
+      <c r="D8" s="192"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="192"/>
+      <c r="G8" s="192"/>
+      <c r="H8" s="192"/>
+      <c r="I8" s="192"/>
+      <c r="J8" s="192"/>
+      <c r="K8" s="192"/>
       <c r="L8" s="185"/>
       <c r="M8" s="185"/>
       <c r="N8" s="185"/>
@@ -4014,61 +4018,61 @@
       <c r="T8" s="185"/>
       <c r="U8" s="185"/>
       <c r="V8" s="185"/>
-      <c r="W8" s="186"/>
-      <c r="X8" s="186"/>
-      <c r="Y8" s="186"/>
-      <c r="Z8" s="186"/>
-      <c r="AA8" s="186"/>
-      <c r="AB8" s="188"/>
-      <c r="AC8" s="188"/>
-      <c r="AD8" s="188"/>
-      <c r="AE8" s="188"/>
-      <c r="AF8" s="188"/>
-      <c r="AG8" s="188"/>
-      <c r="AH8" s="188"/>
-      <c r="AI8" s="188"/>
-      <c r="AJ8" s="188"/>
-      <c r="AK8" s="188"/>
-      <c r="AL8" s="188"/>
-      <c r="AM8" s="188"/>
-      <c r="AN8" s="188"/>
-      <c r="AO8" s="188"/>
-      <c r="AP8" s="188"/>
-      <c r="AQ8" s="188"/>
-      <c r="AR8" s="188"/>
-      <c r="AS8" s="188"/>
-      <c r="AT8" s="188"/>
-      <c r="AU8" s="194"/>
-      <c r="AV8" s="177"/>
-      <c r="AW8" s="177"/>
-      <c r="AX8" s="191"/>
-      <c r="AY8" s="192"/>
-      <c r="AZ8" s="192"/>
-      <c r="BA8" s="192"/>
-      <c r="BB8" s="192"/>
-      <c r="BC8" s="192"/>
-      <c r="BD8" s="192"/>
-      <c r="BE8" s="192"/>
-      <c r="BF8" s="196"/>
-      <c r="BG8" s="196"/>
-      <c r="BT8" s="177"/>
-      <c r="BW8" s="177"/>
-      <c r="CT8" s="177"/>
+      <c r="W8" s="184"/>
+      <c r="X8" s="184"/>
+      <c r="Y8" s="184"/>
+      <c r="Z8" s="184"/>
+      <c r="AA8" s="184"/>
+      <c r="AB8" s="180"/>
+      <c r="AC8" s="180"/>
+      <c r="AD8" s="180"/>
+      <c r="AE8" s="180"/>
+      <c r="AF8" s="180"/>
+      <c r="AG8" s="180"/>
+      <c r="AH8" s="180"/>
+      <c r="AI8" s="180"/>
+      <c r="AJ8" s="180"/>
+      <c r="AK8" s="180"/>
+      <c r="AL8" s="180"/>
+      <c r="AM8" s="180"/>
+      <c r="AN8" s="180"/>
+      <c r="AO8" s="180"/>
+      <c r="AP8" s="180"/>
+      <c r="AQ8" s="180"/>
+      <c r="AR8" s="180"/>
+      <c r="AS8" s="180"/>
+      <c r="AT8" s="180"/>
+      <c r="AU8" s="183"/>
+      <c r="AV8" s="186"/>
+      <c r="AW8" s="186"/>
+      <c r="AX8" s="213"/>
+      <c r="AY8" s="178"/>
+      <c r="AZ8" s="178"/>
+      <c r="BA8" s="178"/>
+      <c r="BB8" s="178"/>
+      <c r="BC8" s="178"/>
+      <c r="BD8" s="178"/>
+      <c r="BE8" s="178"/>
+      <c r="BF8" s="177"/>
+      <c r="BG8" s="177"/>
+      <c r="BT8" s="186"/>
+      <c r="BW8" s="186"/>
+      <c r="CT8" s="186"/>
     </row>
     <row r="9" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="176"/>
-      <c r="B9" s="178" t="s">
+      <c r="A9" s="193"/>
+      <c r="B9" s="194" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="178"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="179"/>
-      <c r="H9" s="179"/>
-      <c r="I9" s="179"/>
-      <c r="J9" s="179"/>
-      <c r="K9" s="179"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="192"/>
+      <c r="E9" s="192"/>
+      <c r="F9" s="192"/>
+      <c r="G9" s="192"/>
+      <c r="H9" s="192"/>
+      <c r="I9" s="192"/>
+      <c r="J9" s="192"/>
+      <c r="K9" s="192"/>
       <c r="L9" s="185"/>
       <c r="M9" s="185"/>
       <c r="N9" s="185"/>
@@ -4080,61 +4084,61 @@
       <c r="T9" s="185"/>
       <c r="U9" s="185"/>
       <c r="V9" s="185"/>
-      <c r="W9" s="186"/>
-      <c r="X9" s="186"/>
-      <c r="Y9" s="186"/>
-      <c r="Z9" s="186"/>
-      <c r="AA9" s="186"/>
-      <c r="AB9" s="188"/>
-      <c r="AC9" s="188"/>
-      <c r="AD9" s="188"/>
-      <c r="AE9" s="188"/>
-      <c r="AF9" s="188"/>
-      <c r="AG9" s="188"/>
-      <c r="AH9" s="188"/>
-      <c r="AI9" s="188"/>
-      <c r="AJ9" s="188"/>
-      <c r="AK9" s="188"/>
-      <c r="AL9" s="188"/>
-      <c r="AM9" s="188"/>
-      <c r="AN9" s="188"/>
-      <c r="AO9" s="188"/>
-      <c r="AP9" s="188"/>
-      <c r="AQ9" s="188"/>
-      <c r="AR9" s="188"/>
-      <c r="AS9" s="188"/>
-      <c r="AT9" s="188"/>
-      <c r="AU9" s="194"/>
-      <c r="AV9" s="177"/>
-      <c r="AW9" s="177"/>
-      <c r="AX9" s="191"/>
-      <c r="AY9" s="192"/>
-      <c r="AZ9" s="192"/>
-      <c r="BA9" s="192"/>
-      <c r="BB9" s="192"/>
-      <c r="BC9" s="192"/>
-      <c r="BD9" s="192"/>
-      <c r="BE9" s="192"/>
-      <c r="BF9" s="196"/>
-      <c r="BG9" s="196"/>
-      <c r="BT9" s="177"/>
-      <c r="BW9" s="177"/>
-      <c r="CT9" s="177"/>
+      <c r="W9" s="184"/>
+      <c r="X9" s="184"/>
+      <c r="Y9" s="184"/>
+      <c r="Z9" s="184"/>
+      <c r="AA9" s="184"/>
+      <c r="AB9" s="180"/>
+      <c r="AC9" s="180"/>
+      <c r="AD9" s="180"/>
+      <c r="AE9" s="180"/>
+      <c r="AF9" s="180"/>
+      <c r="AG9" s="180"/>
+      <c r="AH9" s="180"/>
+      <c r="AI9" s="180"/>
+      <c r="AJ9" s="180"/>
+      <c r="AK9" s="180"/>
+      <c r="AL9" s="180"/>
+      <c r="AM9" s="180"/>
+      <c r="AN9" s="180"/>
+      <c r="AO9" s="180"/>
+      <c r="AP9" s="180"/>
+      <c r="AQ9" s="180"/>
+      <c r="AR9" s="180"/>
+      <c r="AS9" s="180"/>
+      <c r="AT9" s="180"/>
+      <c r="AU9" s="183"/>
+      <c r="AV9" s="186"/>
+      <c r="AW9" s="186"/>
+      <c r="AX9" s="213"/>
+      <c r="AY9" s="178"/>
+      <c r="AZ9" s="178"/>
+      <c r="BA9" s="178"/>
+      <c r="BB9" s="178"/>
+      <c r="BC9" s="178"/>
+      <c r="BD9" s="178"/>
+      <c r="BE9" s="178"/>
+      <c r="BF9" s="177"/>
+      <c r="BG9" s="177"/>
+      <c r="BT9" s="186"/>
+      <c r="BW9" s="186"/>
+      <c r="CT9" s="186"/>
     </row>
     <row r="10" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="176"/>
-      <c r="B10" s="178" t="s">
+      <c r="A10" s="193"/>
+      <c r="B10" s="194" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="178"/>
-      <c r="D10" s="179"/>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
-      <c r="G10" s="179"/>
-      <c r="H10" s="179"/>
-      <c r="I10" s="179"/>
-      <c r="J10" s="179"/>
-      <c r="K10" s="179"/>
+      <c r="C10" s="194"/>
+      <c r="D10" s="192"/>
+      <c r="E10" s="192"/>
+      <c r="F10" s="192"/>
+      <c r="G10" s="192"/>
+      <c r="H10" s="192"/>
+      <c r="I10" s="192"/>
+      <c r="J10" s="192"/>
+      <c r="K10" s="192"/>
       <c r="L10" s="185"/>
       <c r="M10" s="185"/>
       <c r="N10" s="185"/>
@@ -4146,61 +4150,61 @@
       <c r="T10" s="185"/>
       <c r="U10" s="185"/>
       <c r="V10" s="185"/>
-      <c r="W10" s="186"/>
-      <c r="X10" s="186"/>
-      <c r="Y10" s="186"/>
-      <c r="Z10" s="186"/>
-      <c r="AA10" s="186"/>
-      <c r="AB10" s="188"/>
-      <c r="AC10" s="188"/>
-      <c r="AD10" s="188"/>
-      <c r="AE10" s="188"/>
-      <c r="AF10" s="188"/>
-      <c r="AG10" s="188"/>
-      <c r="AH10" s="188"/>
-      <c r="AI10" s="188"/>
-      <c r="AJ10" s="188"/>
-      <c r="AK10" s="188"/>
-      <c r="AL10" s="188"/>
-      <c r="AM10" s="188"/>
-      <c r="AN10" s="188"/>
-      <c r="AO10" s="188"/>
-      <c r="AP10" s="188"/>
-      <c r="AQ10" s="188"/>
-      <c r="AR10" s="188"/>
-      <c r="AS10" s="188"/>
-      <c r="AT10" s="188"/>
-      <c r="AU10" s="194"/>
-      <c r="AV10" s="177"/>
-      <c r="AW10" s="177"/>
-      <c r="AX10" s="191"/>
-      <c r="AY10" s="192"/>
-      <c r="AZ10" s="192"/>
-      <c r="BA10" s="192"/>
-      <c r="BB10" s="192"/>
-      <c r="BC10" s="192"/>
-      <c r="BD10" s="192"/>
-      <c r="BE10" s="192"/>
-      <c r="BF10" s="196"/>
-      <c r="BG10" s="196"/>
-      <c r="BT10" s="177"/>
-      <c r="BW10" s="177"/>
-      <c r="CT10" s="177"/>
+      <c r="W10" s="184"/>
+      <c r="X10" s="184"/>
+      <c r="Y10" s="184"/>
+      <c r="Z10" s="184"/>
+      <c r="AA10" s="184"/>
+      <c r="AB10" s="180"/>
+      <c r="AC10" s="180"/>
+      <c r="AD10" s="180"/>
+      <c r="AE10" s="180"/>
+      <c r="AF10" s="180"/>
+      <c r="AG10" s="180"/>
+      <c r="AH10" s="180"/>
+      <c r="AI10" s="180"/>
+      <c r="AJ10" s="180"/>
+      <c r="AK10" s="180"/>
+      <c r="AL10" s="180"/>
+      <c r="AM10" s="180"/>
+      <c r="AN10" s="180"/>
+      <c r="AO10" s="180"/>
+      <c r="AP10" s="180"/>
+      <c r="AQ10" s="180"/>
+      <c r="AR10" s="180"/>
+      <c r="AS10" s="180"/>
+      <c r="AT10" s="180"/>
+      <c r="AU10" s="183"/>
+      <c r="AV10" s="186"/>
+      <c r="AW10" s="186"/>
+      <c r="AX10" s="213"/>
+      <c r="AY10" s="178"/>
+      <c r="AZ10" s="178"/>
+      <c r="BA10" s="178"/>
+      <c r="BB10" s="178"/>
+      <c r="BC10" s="178"/>
+      <c r="BD10" s="178"/>
+      <c r="BE10" s="178"/>
+      <c r="BF10" s="177"/>
+      <c r="BG10" s="177"/>
+      <c r="BT10" s="186"/>
+      <c r="BW10" s="186"/>
+      <c r="CT10" s="186"/>
     </row>
     <row r="11" spans="1:98" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="176"/>
-      <c r="B11" s="178" t="s">
+      <c r="A11" s="193"/>
+      <c r="B11" s="194" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="179"/>
-      <c r="E11" s="179"/>
-      <c r="F11" s="179"/>
-      <c r="G11" s="179"/>
-      <c r="H11" s="179"/>
-      <c r="I11" s="179"/>
-      <c r="J11" s="179"/>
-      <c r="K11" s="179"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="192"/>
+      <c r="E11" s="192"/>
+      <c r="F11" s="192"/>
+      <c r="G11" s="192"/>
+      <c r="H11" s="192"/>
+      <c r="I11" s="192"/>
+      <c r="J11" s="192"/>
+      <c r="K11" s="192"/>
       <c r="L11" s="185"/>
       <c r="M11" s="185"/>
       <c r="N11" s="185"/>
@@ -4212,91 +4216,65 @@
       <c r="T11" s="185"/>
       <c r="U11" s="185"/>
       <c r="V11" s="185"/>
-      <c r="W11" s="186"/>
-      <c r="X11" s="186"/>
-      <c r="Y11" s="186"/>
-      <c r="Z11" s="186"/>
-      <c r="AA11" s="186"/>
-      <c r="AB11" s="189"/>
-      <c r="AC11" s="189"/>
-      <c r="AD11" s="189"/>
-      <c r="AE11" s="189"/>
-      <c r="AF11" s="189"/>
-      <c r="AG11" s="189"/>
-      <c r="AH11" s="189"/>
-      <c r="AI11" s="189"/>
-      <c r="AJ11" s="189"/>
-      <c r="AK11" s="189"/>
-      <c r="AL11" s="189"/>
-      <c r="AM11" s="189"/>
-      <c r="AN11" s="189"/>
-      <c r="AO11" s="189"/>
-      <c r="AP11" s="189"/>
-      <c r="AQ11" s="189"/>
-      <c r="AR11" s="189"/>
-      <c r="AS11" s="189"/>
-      <c r="AT11" s="189"/>
-      <c r="AU11" s="194"/>
-      <c r="AV11" s="177"/>
-      <c r="AW11" s="177"/>
-      <c r="AX11" s="191"/>
-      <c r="AY11" s="192"/>
-      <c r="AZ11" s="192"/>
-      <c r="BA11" s="192"/>
-      <c r="BB11" s="192"/>
-      <c r="BC11" s="192"/>
-      <c r="BD11" s="192"/>
-      <c r="BE11" s="192"/>
-      <c r="BF11" s="196"/>
-      <c r="BG11" s="196"/>
-      <c r="BT11" s="177"/>
-      <c r="BW11" s="177"/>
-      <c r="CT11" s="177"/>
+      <c r="W11" s="184"/>
+      <c r="X11" s="184"/>
+      <c r="Y11" s="184"/>
+      <c r="Z11" s="184"/>
+      <c r="AA11" s="184"/>
+      <c r="AB11" s="181"/>
+      <c r="AC11" s="181"/>
+      <c r="AD11" s="181"/>
+      <c r="AE11" s="181"/>
+      <c r="AF11" s="181"/>
+      <c r="AG11" s="181"/>
+      <c r="AH11" s="181"/>
+      <c r="AI11" s="181"/>
+      <c r="AJ11" s="181"/>
+      <c r="AK11" s="181"/>
+      <c r="AL11" s="181"/>
+      <c r="AM11" s="181"/>
+      <c r="AN11" s="181"/>
+      <c r="AO11" s="181"/>
+      <c r="AP11" s="181"/>
+      <c r="AQ11" s="181"/>
+      <c r="AR11" s="181"/>
+      <c r="AS11" s="181"/>
+      <c r="AT11" s="181"/>
+      <c r="AU11" s="183"/>
+      <c r="AV11" s="186"/>
+      <c r="AW11" s="186"/>
+      <c r="AX11" s="213"/>
+      <c r="AY11" s="178"/>
+      <c r="AZ11" s="178"/>
+      <c r="BA11" s="178"/>
+      <c r="BB11" s="178"/>
+      <c r="BC11" s="178"/>
+      <c r="BD11" s="178"/>
+      <c r="BE11" s="178"/>
+      <c r="BF11" s="177"/>
+      <c r="BG11" s="177"/>
+      <c r="BT11" s="186"/>
+      <c r="BW11" s="186"/>
+      <c r="CT11" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="BG4:BG11"/>
-    <mergeCell ref="BB4:BB11"/>
-    <mergeCell ref="BC4:BC11"/>
-    <mergeCell ref="BD4:BD11"/>
-    <mergeCell ref="BE4:BE11"/>
-    <mergeCell ref="BF4:BF11"/>
-    <mergeCell ref="AT4:AT11"/>
-    <mergeCell ref="AX4:AX11"/>
-    <mergeCell ref="AY4:AY11"/>
-    <mergeCell ref="AZ4:AZ11"/>
-    <mergeCell ref="BA4:BA11"/>
-    <mergeCell ref="AU4:AU11"/>
-    <mergeCell ref="AO4:AO11"/>
-    <mergeCell ref="AP4:AP11"/>
-    <mergeCell ref="AQ4:AQ11"/>
-    <mergeCell ref="AR4:AR11"/>
-    <mergeCell ref="AS4:AS11"/>
-    <mergeCell ref="AJ4:AJ11"/>
-    <mergeCell ref="AK4:AK11"/>
-    <mergeCell ref="AL4:AL11"/>
-    <mergeCell ref="AM4:AM11"/>
-    <mergeCell ref="AN4:AN11"/>
-    <mergeCell ref="AE4:AE11"/>
-    <mergeCell ref="AF4:AF11"/>
-    <mergeCell ref="AG4:AG11"/>
-    <mergeCell ref="AH4:AH11"/>
-    <mergeCell ref="AI4:AI11"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="AA4:AA11"/>
-    <mergeCell ref="AB4:AB11"/>
-    <mergeCell ref="AC4:AC11"/>
-    <mergeCell ref="AD4:AD11"/>
-    <mergeCell ref="U4:U11"/>
-    <mergeCell ref="V4:V11"/>
-    <mergeCell ref="W4:W11"/>
-    <mergeCell ref="X4:X11"/>
-    <mergeCell ref="Y4:Y11"/>
-    <mergeCell ref="P4:P11"/>
-    <mergeCell ref="Q4:Q11"/>
-    <mergeCell ref="R4:R11"/>
-    <mergeCell ref="S4:S11"/>
-    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="AV4:AV11"/>
+    <mergeCell ref="AW4:AW11"/>
+    <mergeCell ref="BT4:BT11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="J4:J11"/>
     <mergeCell ref="CT4:CT11"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
@@ -4313,22 +4291,48 @@
     <mergeCell ref="M4:M11"/>
     <mergeCell ref="N4:N11"/>
     <mergeCell ref="O4:O11"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="AV4:AV11"/>
-    <mergeCell ref="AW4:AW11"/>
-    <mergeCell ref="BT4:BT11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="J4:J11"/>
+    <mergeCell ref="P4:P11"/>
+    <mergeCell ref="Q4:Q11"/>
+    <mergeCell ref="R4:R11"/>
+    <mergeCell ref="S4:S11"/>
+    <mergeCell ref="T4:T11"/>
+    <mergeCell ref="U4:U11"/>
+    <mergeCell ref="V4:V11"/>
+    <mergeCell ref="W4:W11"/>
+    <mergeCell ref="X4:X11"/>
+    <mergeCell ref="Y4:Y11"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="AA4:AA11"/>
+    <mergeCell ref="AB4:AB11"/>
+    <mergeCell ref="AC4:AC11"/>
+    <mergeCell ref="AD4:AD11"/>
+    <mergeCell ref="AE4:AE11"/>
+    <mergeCell ref="AF4:AF11"/>
+    <mergeCell ref="AG4:AG11"/>
+    <mergeCell ref="AH4:AH11"/>
+    <mergeCell ref="AI4:AI11"/>
+    <mergeCell ref="AJ4:AJ11"/>
+    <mergeCell ref="AK4:AK11"/>
+    <mergeCell ref="AL4:AL11"/>
+    <mergeCell ref="AM4:AM11"/>
+    <mergeCell ref="AN4:AN11"/>
+    <mergeCell ref="AO4:AO11"/>
+    <mergeCell ref="AP4:AP11"/>
+    <mergeCell ref="AQ4:AQ11"/>
+    <mergeCell ref="AR4:AR11"/>
+    <mergeCell ref="AS4:AS11"/>
+    <mergeCell ref="AT4:AT11"/>
+    <mergeCell ref="AX4:AX11"/>
+    <mergeCell ref="AY4:AY11"/>
+    <mergeCell ref="AZ4:AZ11"/>
+    <mergeCell ref="BA4:BA11"/>
+    <mergeCell ref="AU4:AU11"/>
+    <mergeCell ref="BG4:BG11"/>
+    <mergeCell ref="BB4:BB11"/>
+    <mergeCell ref="BC4:BC11"/>
+    <mergeCell ref="BD4:BD11"/>
+    <mergeCell ref="BE4:BE11"/>
+    <mergeCell ref="BF4:BF11"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4338,7 +4342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -5186,7 +5190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5850,13 +5854,13 @@
       </c>
     </row>
     <row r="4" spans="1:106" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="209" t="s">
+      <c r="A4" s="197" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="210" t="s">
+      <c r="B4" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="211"/>
+      <c r="C4" s="200"/>
       <c r="D4" s="57"/>
       <c r="E4" s="58"/>
       <c r="F4" s="58"/>
@@ -5962,7 +5966,7 @@
     </row>
     <row r="5" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="198"/>
-      <c r="B5" s="208"/>
+      <c r="B5" s="196"/>
       <c r="C5" s="198"/>
       <c r="D5" s="63"/>
       <c r="E5" s="60"/>
@@ -6724,7 +6728,7 @@
     <row r="12" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="198"/>
       <c r="B12" s="71"/>
-      <c r="C12" s="199"/>
+      <c r="C12" s="201"/>
       <c r="D12" s="72"/>
       <c r="E12" s="73"/>
       <c r="F12" s="73"/>
@@ -6829,10 +6833,10 @@
       <c r="DA12" s="64"/>
     </row>
     <row r="13" spans="1:106" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="212" t="s">
+      <c r="A13" s="202" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="213" t="s">
+      <c r="B13" s="203" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="75"/>
@@ -7725,7 +7729,7 @@
       <c r="DB20" s="83"/>
     </row>
     <row r="21" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="199"/>
+      <c r="A21" s="201"/>
       <c r="B21" s="91" t="s">
         <v>38</v>
       </c>
@@ -7836,7 +7840,7 @@
     </row>
     <row r="22" spans="1:106" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="93"/>
-      <c r="B22" s="207" t="s">
+      <c r="B22" s="195" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="94"/>
@@ -7946,7 +7950,7 @@
     </row>
     <row r="23" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="93"/>
-      <c r="B23" s="208"/>
+      <c r="B23" s="196"/>
       <c r="C23" s="100"/>
       <c r="D23" s="95"/>
       <c r="E23" s="96"/>
@@ -8053,13 +8057,13 @@
       <c r="DB23" s="99"/>
     </row>
     <row r="24" spans="1:106" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="200" t="s">
+      <c r="A24" s="206" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="202">
+      <c r="C24" s="208">
         <v>0.1</v>
       </c>
       <c r="D24" s="95"/>
@@ -8167,7 +8171,7 @@
       <c r="DB24" s="99"/>
     </row>
     <row r="25" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="201"/>
+      <c r="A25" s="207"/>
       <c r="B25" s="103" t="s">
         <v>42</v>
       </c>
@@ -8277,7 +8281,7 @@
       <c r="DB25" s="99"/>
     </row>
     <row r="26" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="201"/>
+      <c r="A26" s="207"/>
       <c r="B26" s="103" t="s">
         <v>43</v>
       </c>
@@ -8387,7 +8391,7 @@
       <c r="DB26" s="99"/>
     </row>
     <row r="27" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="201"/>
+      <c r="A27" s="207"/>
       <c r="B27" s="103" t="s">
         <v>44</v>
       </c>
@@ -8497,7 +8501,7 @@
       <c r="DB27" s="99"/>
     </row>
     <row r="28" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="201"/>
+      <c r="A28" s="207"/>
       <c r="B28" s="103" t="s">
         <v>45</v>
       </c>
@@ -8607,7 +8611,7 @@
       <c r="DB28" s="99"/>
     </row>
     <row r="29" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="201"/>
+      <c r="A29" s="207"/>
       <c r="B29" s="103" t="s">
         <v>46</v>
       </c>
@@ -8717,7 +8721,7 @@
       <c r="DB29" s="99"/>
     </row>
     <row r="30" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="201"/>
+      <c r="A30" s="207"/>
       <c r="B30" s="103" t="s">
         <v>47</v>
       </c>
@@ -8827,7 +8831,7 @@
       <c r="DB30" s="99"/>
     </row>
     <row r="31" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="201"/>
+      <c r="A31" s="207"/>
       <c r="B31" s="103" t="s">
         <v>48</v>
       </c>
@@ -8937,7 +8941,7 @@
       <c r="DB31" s="99"/>
     </row>
     <row r="32" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="201"/>
+      <c r="A32" s="207"/>
       <c r="B32" s="103" t="s">
         <v>49</v>
       </c>
@@ -9047,7 +9051,7 @@
       <c r="DB32" s="99"/>
     </row>
     <row r="33" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="201"/>
+      <c r="A33" s="207"/>
       <c r="B33" s="103" t="s">
         <v>50</v>
       </c>
@@ -9157,7 +9161,7 @@
       <c r="DB33" s="99"/>
     </row>
     <row r="34" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="201"/>
+      <c r="A34" s="207"/>
       <c r="B34" s="105" t="s">
         <v>51</v>
       </c>
@@ -9267,11 +9271,11 @@
       <c r="DB34" s="99"/>
     </row>
     <row r="35" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="201"/>
+      <c r="A35" s="207"/>
       <c r="B35" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="199"/>
+      <c r="C35" s="201"/>
       <c r="D35" s="104"/>
       <c r="E35" s="98"/>
       <c r="F35" s="98"/>
@@ -9377,11 +9381,11 @@
       <c r="DB35" s="99"/>
     </row>
     <row r="36" spans="1:106" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="201"/>
+      <c r="A36" s="207"/>
       <c r="B36" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="202">
+      <c r="C36" s="208">
         <v>0.1</v>
       </c>
       <c r="D36" s="104"/>
@@ -9489,7 +9493,7 @@
       <c r="DB36" s="99"/>
     </row>
     <row r="37" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="201"/>
+      <c r="A37" s="207"/>
       <c r="B37" s="103" t="s">
         <v>42</v>
       </c>
@@ -9599,7 +9603,7 @@
       <c r="DB37" s="99"/>
     </row>
     <row r="38" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="201"/>
+      <c r="A38" s="207"/>
       <c r="B38" s="103" t="s">
         <v>54</v>
       </c>
@@ -9709,7 +9713,7 @@
       <c r="DB38" s="99"/>
     </row>
     <row r="39" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="201"/>
+      <c r="A39" s="207"/>
       <c r="B39" s="103" t="s">
         <v>55</v>
       </c>
@@ -9819,7 +9823,7 @@
       <c r="DB39" s="99"/>
     </row>
     <row r="40" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="201"/>
+      <c r="A40" s="207"/>
       <c r="B40" s="103" t="s">
         <v>56</v>
       </c>
@@ -9929,7 +9933,7 @@
       <c r="DB40" s="99"/>
     </row>
     <row r="41" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="201"/>
+      <c r="A41" s="207"/>
       <c r="B41" s="103" t="s">
         <v>57</v>
       </c>
@@ -10039,7 +10043,7 @@
       <c r="DB41" s="99"/>
     </row>
     <row r="42" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="201"/>
+      <c r="A42" s="207"/>
       <c r="B42" s="103" t="s">
         <v>58</v>
       </c>
@@ -10149,7 +10153,7 @@
       <c r="DB42" s="99"/>
     </row>
     <row r="43" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="201"/>
+      <c r="A43" s="207"/>
       <c r="B43" s="103" t="s">
         <v>59</v>
       </c>
@@ -10259,7 +10263,7 @@
       <c r="DB43" s="99"/>
     </row>
     <row r="44" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="201"/>
+      <c r="A44" s="207"/>
       <c r="B44" s="103" t="s">
         <v>60</v>
       </c>
@@ -10369,7 +10373,7 @@
       <c r="DB44" s="99"/>
     </row>
     <row r="45" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="201"/>
+      <c r="A45" s="207"/>
       <c r="B45" s="103" t="s">
         <v>61</v>
       </c>
@@ -10479,7 +10483,7 @@
       <c r="DB45" s="99"/>
     </row>
     <row r="46" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="201"/>
+      <c r="A46" s="207"/>
       <c r="B46" s="103" t="s">
         <v>62</v>
       </c>
@@ -10589,7 +10593,7 @@
       <c r="DB46" s="99"/>
     </row>
     <row r="47" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="201"/>
+      <c r="A47" s="207"/>
       <c r="B47" s="108" t="s">
         <v>63</v>
       </c>
@@ -10707,7 +10711,7 @@
       <c r="DB47" s="99"/>
     </row>
     <row r="48" spans="1:106" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="201"/>
+      <c r="A48" s="207"/>
       <c r="B48" s="110" t="s">
         <v>64</v>
       </c>
@@ -10820,7 +10824,7 @@
     </row>
     <row r="49" spans="1:106" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="111"/>
-      <c r="B49" s="203" t="s">
+      <c r="B49" s="209" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="111"/>
@@ -14361,7 +14365,7 @@
       <c r="DB80" s="115"/>
     </row>
     <row r="81" spans="1:106" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="205" t="s">
+      <c r="A81" s="210" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="122" t="s">
@@ -15469,7 +15473,7 @@
       <c r="B91" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="C91" s="206"/>
+      <c r="C91" s="211"/>
       <c r="D91" s="124"/>
       <c r="E91" s="125"/>
       <c r="F91" s="125"/>
@@ -15685,7 +15689,7 @@
       <c r="DB92" s="129"/>
     </row>
     <row r="93" spans="1:106" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="199"/>
+      <c r="A93" s="201"/>
       <c r="B93" s="134" t="s">
         <v>111</v>
       </c>
@@ -15913,7 +15917,7 @@
       <c r="DB94" s="129"/>
     </row>
     <row r="95" spans="1:106" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="197" t="s">
+      <c r="A95" s="205" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="137" t="s">
@@ -18471,7 +18475,7 @@
       <c r="DB117" s="141"/>
     </row>
     <row r="118" spans="1:106" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="199"/>
+      <c r="A118" s="201"/>
       <c r="B118" s="154" t="s">
         <v>137</v>
       </c>
@@ -25842,12 +25846,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A4:A12"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A95:A118"/>
     <mergeCell ref="A24:A48"/>
     <mergeCell ref="C24:C35"/>
@@ -25855,6 +25853,12 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A81:A93"/>
     <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adiciona acompanhamento dos dias 17 e 18-10
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
+++ b/Cronograma/CodeXp_acompanhamento_turma_B_manha.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39893838843\Downloads\2s2019-t3-mentoria\Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Cursos\senai_desenvolvimento\2s2019\2s2019-t3-mentoria\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2A3F3-145D-40AE-8409-40853C16095B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dailies" sheetId="2" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Saulo Santos</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -88,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="188">
   <si>
     <t>S</t>
   </si>
@@ -762,16 +763,23 @@
     <t>Não foi possível realizar acompanhamento devido às atividades do SAEP</t>
   </si>
   <si>
-    <t>Nossa Sra Aparecida</t>
+    <t>Modelagem do banco de dados do projeto Linx</t>
   </si>
   <si>
-    <t>Modelagem do banco de dados do projeto Linx</t>
+    <t>Dia dos Professores</t>
+  </si>
+  <si>
+    <t>Alinhamento da modelagem e scripts do banco de dados projeto Linx</t>
+  </si>
+  <si>
+    <t>Instalação do ambiente EF.
+CategoriaController</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1970,7 +1978,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2313,38 +2321,17 @@
     <xf numFmtId="0" fontId="16" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2361,40 +2348,44 @@
     <xf numFmtId="0" fontId="18" fillId="22" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2405,22 +2396,36 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2917,14 +2922,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AS4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AT4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AY4" sqref="AY4:AY11"/>
+      <selection pane="bottomRight" activeCell="BA4" sqref="BA4:BA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3233,110 +3238,110 @@
       <c r="C2" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="187" t="s">
+      <c r="D2" s="180" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="187"/>
-      <c r="F2" s="187"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="187"/>
-      <c r="I2" s="187"/>
-      <c r="J2" s="187"/>
-      <c r="K2" s="187"/>
-      <c r="L2" s="187"/>
-      <c r="M2" s="187"/>
-      <c r="N2" s="187"/>
-      <c r="O2" s="187"/>
-      <c r="P2" s="187"/>
-      <c r="Q2" s="187"/>
-      <c r="R2" s="187" t="s">
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
+      <c r="N2" s="180"/>
+      <c r="O2" s="180"/>
+      <c r="P2" s="180"/>
+      <c r="Q2" s="180"/>
+      <c r="R2" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="187"/>
-      <c r="T2" s="187"/>
-      <c r="U2" s="187"/>
-      <c r="V2" s="187"/>
-      <c r="W2" s="187"/>
-      <c r="X2" s="187"/>
-      <c r="Y2" s="187"/>
-      <c r="Z2" s="187"/>
-      <c r="AA2" s="187"/>
-      <c r="AB2" s="187"/>
-      <c r="AC2" s="187"/>
-      <c r="AD2" s="187"/>
-      <c r="AE2" s="187"/>
-      <c r="AF2" s="187"/>
-      <c r="AG2" s="187"/>
-      <c r="AH2" s="187"/>
-      <c r="AI2" s="187"/>
-      <c r="AJ2" s="187"/>
-      <c r="AK2" s="187"/>
-      <c r="AL2" s="187"/>
-      <c r="AM2" s="187" t="s">
+      <c r="S2" s="180"/>
+      <c r="T2" s="180"/>
+      <c r="U2" s="180"/>
+      <c r="V2" s="180"/>
+      <c r="W2" s="180"/>
+      <c r="X2" s="180"/>
+      <c r="Y2" s="180"/>
+      <c r="Z2" s="180"/>
+      <c r="AA2" s="180"/>
+      <c r="AB2" s="180"/>
+      <c r="AC2" s="180"/>
+      <c r="AD2" s="180"/>
+      <c r="AE2" s="180"/>
+      <c r="AF2" s="180"/>
+      <c r="AG2" s="180"/>
+      <c r="AH2" s="180"/>
+      <c r="AI2" s="180"/>
+      <c r="AJ2" s="180"/>
+      <c r="AK2" s="180"/>
+      <c r="AL2" s="180"/>
+      <c r="AM2" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" s="187"/>
-      <c r="AO2" s="187"/>
-      <c r="AP2" s="187"/>
-      <c r="AQ2" s="187"/>
-      <c r="AR2" s="187"/>
-      <c r="AS2" s="187"/>
-      <c r="AT2" s="187"/>
-      <c r="AU2" s="187"/>
-      <c r="AV2" s="187"/>
-      <c r="AW2" s="187"/>
-      <c r="AX2" s="188"/>
-      <c r="AY2" s="188"/>
-      <c r="AZ2" s="188"/>
-      <c r="BA2" s="188"/>
-      <c r="BB2" s="188"/>
-      <c r="BC2" s="188"/>
-      <c r="BD2" s="188"/>
-      <c r="BE2" s="188"/>
-      <c r="BF2" s="188"